<commit_message>
viz y tablas update
</commit_message>
<xml_diff>
--- a/Data/Base_fichas_indicadores.xlsx
+++ b/Data/Base_fichas_indicadores.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\DESCA-app\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Trabajo\DESCA\DESCA-app\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1167F29F-BBDA-4956-B4B5-1A5DBC6BC95C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BASE_FICHAS" sheetId="4" r:id="rId1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1976" uniqueCount="719">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1976" uniqueCount="722">
   <si>
     <t>id</t>
   </si>
@@ -2181,12 +2182,21 @@
   </si>
   <si>
     <t>Cantidad de NNA</t>
+  </si>
+  <si>
+    <t>SEXO_POB</t>
+  </si>
+  <si>
+    <t>EDAD_POB</t>
+  </si>
+  <si>
+    <t>ASCENDENCIA_POB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.000&quot;&quot;;\-#,##0.000&quot;&quot;"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -2403,10 +2413,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Excel Built-in Normal" xfId="3"/>
+    <cellStyle name="Excel Built-in Normal" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal_DISEÑO" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal_DISEÑO" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2717,42 +2727,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AI140"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="P1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E111" sqref="E111"/>
-      <selection pane="bottomLeft" activeCell="I142" sqref="I142"/>
+      <selection pane="bottomLeft" activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="13" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" style="13" customWidth="1"/>
-    <col min="4" max="4" width="37.7109375" style="13" customWidth="1"/>
-    <col min="5" max="5" width="94.7109375" style="13" customWidth="1"/>
-    <col min="6" max="6" width="157.28515625" style="13" customWidth="1"/>
-    <col min="7" max="7" width="255.7109375" style="13" customWidth="1"/>
-    <col min="8" max="8" width="181.140625" style="13" customWidth="1"/>
-    <col min="9" max="9" width="59.42578125" style="13" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" style="13" customWidth="1"/>
-    <col min="11" max="11" width="20.42578125" style="13" customWidth="1"/>
-    <col min="12" max="12" width="20.5703125" style="13" customWidth="1"/>
-    <col min="13" max="14" width="255.7109375" style="13" customWidth="1"/>
-    <col min="15" max="15" width="230.140625" style="13" customWidth="1"/>
-    <col min="16" max="16" width="98.7109375" style="13" customWidth="1"/>
-    <col min="17" max="17" width="19.140625" style="13" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="37.6640625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="94.6640625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="157.33203125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="255.6640625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="181.109375" style="13" customWidth="1"/>
+    <col min="9" max="9" width="59.44140625" style="13" customWidth="1"/>
+    <col min="10" max="10" width="16.109375" style="13" customWidth="1"/>
+    <col min="11" max="11" width="20.44140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="20.5546875" style="13" customWidth="1"/>
+    <col min="13" max="14" width="255.6640625" style="13" customWidth="1"/>
+    <col min="15" max="15" width="230.109375" style="13" customWidth="1"/>
+    <col min="16" max="16" width="98.6640625" style="13" customWidth="1"/>
+    <col min="17" max="17" width="19.109375" style="13" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.88671875" style="13" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="22" max="26" width="9.42578125" style="13" customWidth="1"/>
-    <col min="27" max="29" width="9.140625" style="13"/>
-    <col min="30" max="30" width="55.140625" style="13" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="13"/>
+    <col min="21" max="21" width="15.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="26" width="9.44140625" style="13" customWidth="1"/>
+    <col min="27" max="29" width="9.109375" style="13"/>
+    <col min="30" max="30" width="55.109375" style="13" customWidth="1"/>
+    <col min="31" max="16384" width="9.109375" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -2811,13 +2821,13 @@
         <v>693</v>
       </c>
       <c r="S1" s="35" t="s">
-        <v>696</v>
+        <v>719</v>
       </c>
       <c r="T1" s="35" t="s">
-        <v>697</v>
+        <v>720</v>
       </c>
       <c r="U1" s="35" t="s">
-        <v>698</v>
+        <v>721</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="6" customFormat="1">
@@ -12089,7 +12099,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -12097,11 +12107,11 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="17.25" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="17.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="255.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="27.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="255.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1">

</xml_diff>

<commit_message>
Act base fichas indicadores
</commit_message>
<xml_diff>
--- a/Data/Base_fichas_indicadores.xlsx
+++ b/Data/Base_fichas_indicadores.xlsx
@@ -1,23 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Trabajo\DESCA\DESCA-app\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\DESCA-app\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1167F29F-BBDA-4956-B4B5-1A5DBC6BC95C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="BASE_FICHAS" sheetId="4" r:id="rId1"/>
     <sheet name="REF_COLUMNAS" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BASE_FICHAS!$A$1:$AI$128</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BASE_FICHAS!$A$1:$AI$136</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
@@ -2196,7 +2195,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.000&quot;&quot;;\-#,##0.000&quot;&quot;"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -2413,10 +2412,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Excel Built-in Normal" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Excel Built-in Normal" xfId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal_DISEÑO" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal_DISEÑO" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2727,42 +2726,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AI140"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="P1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E111" sqref="E111"/>
-      <selection pane="bottomLeft" activeCell="S2" sqref="S2"/>
+      <selection pane="bottomLeft" activeCell="Y10" sqref="Y10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="13" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" style="13" customWidth="1"/>
-    <col min="4" max="4" width="37.6640625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="94.6640625" style="13" customWidth="1"/>
-    <col min="6" max="6" width="157.33203125" style="13" customWidth="1"/>
-    <col min="7" max="7" width="255.6640625" style="13" customWidth="1"/>
-    <col min="8" max="8" width="181.109375" style="13" customWidth="1"/>
-    <col min="9" max="9" width="59.44140625" style="13" customWidth="1"/>
-    <col min="10" max="10" width="16.109375" style="13" customWidth="1"/>
-    <col min="11" max="11" width="20.44140625" style="13" customWidth="1"/>
-    <col min="12" max="12" width="20.5546875" style="13" customWidth="1"/>
-    <col min="13" max="14" width="255.6640625" style="13" customWidth="1"/>
-    <col min="15" max="15" width="230.109375" style="13" customWidth="1"/>
-    <col min="16" max="16" width="98.6640625" style="13" customWidth="1"/>
-    <col min="17" max="17" width="19.109375" style="13" customWidth="1"/>
-    <col min="18" max="18" width="12.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" style="13" customWidth="1"/>
+    <col min="4" max="4" width="37.7109375" style="13" customWidth="1"/>
+    <col min="5" max="5" width="94.7109375" style="13" customWidth="1"/>
+    <col min="6" max="6" width="157.28515625" style="13" customWidth="1"/>
+    <col min="7" max="7" width="255.7109375" style="13" customWidth="1"/>
+    <col min="8" max="8" width="181.140625" style="13" customWidth="1"/>
+    <col min="9" max="9" width="59.42578125" style="13" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" style="13" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" style="13" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" style="13" customWidth="1"/>
+    <col min="13" max="14" width="255.7109375" style="13" customWidth="1"/>
+    <col min="15" max="15" width="230.140625" style="13" customWidth="1"/>
+    <col min="16" max="16" width="98.7109375" style="13" customWidth="1"/>
+    <col min="17" max="17" width="19.140625" style="13" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.85546875" style="13" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="22" max="26" width="9.44140625" style="13" customWidth="1"/>
-    <col min="27" max="29" width="9.109375" style="13"/>
-    <col min="30" max="30" width="55.109375" style="13" customWidth="1"/>
-    <col min="31" max="16384" width="9.109375" style="13"/>
+    <col min="21" max="21" width="15.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="26" width="9.42578125" style="13" customWidth="1"/>
+    <col min="27" max="29" width="9.140625" style="13"/>
+    <col min="30" max="30" width="55.140625" style="13" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -2880,16 +2879,16 @@
         <v>0</v>
       </c>
       <c r="R2" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S2" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T2" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U2" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:21" s="6" customFormat="1">
@@ -2939,7 +2938,7 @@
         <v>17</v>
       </c>
       <c r="Q3" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R3" s="6">
         <v>0</v>
@@ -3001,7 +3000,7 @@
         <v>17</v>
       </c>
       <c r="Q4" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R4" s="6">
         <v>0</v>
@@ -3063,7 +3062,7 @@
         <v>17</v>
       </c>
       <c r="Q5" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5" s="6">
         <v>0</v>
@@ -3875,16 +3874,16 @@
         <v>1</v>
       </c>
       <c r="R18" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S18" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T18" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U18" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:35">
@@ -5238,7 +5237,7 @@
         <v>17</v>
       </c>
       <c r="Q37" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R37" s="6">
         <v>0</v>
@@ -5300,7 +5299,7 @@
         <v>17</v>
       </c>
       <c r="Q38" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R38" s="6">
         <v>0</v>
@@ -5362,7 +5361,7 @@
         <v>17</v>
       </c>
       <c r="Q39" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R39" s="6">
         <v>0</v>
@@ -5424,7 +5423,7 @@
         <v>17</v>
       </c>
       <c r="Q40" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R40" s="6">
         <v>0</v>
@@ -6621,7 +6620,7 @@
         <v>17</v>
       </c>
       <c r="Q56" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R56" s="6">
         <v>0</v>
@@ -6683,7 +6682,7 @@
         <v>17</v>
       </c>
       <c r="Q57" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R57" s="6">
         <v>0</v>
@@ -6745,7 +6744,7 @@
         <v>17</v>
       </c>
       <c r="Q58" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R58" s="6">
         <v>0</v>
@@ -6807,7 +6806,7 @@
         <v>17</v>
       </c>
       <c r="Q59" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R59" s="6">
         <v>0</v>
@@ -8355,7 +8354,7 @@
         <v>17</v>
       </c>
       <c r="Q83" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R83" s="6">
         <v>0</v>
@@ -8418,7 +8417,7 @@
         <v>17</v>
       </c>
       <c r="Q84" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R84" s="6">
         <v>0</v>
@@ -8495,7 +8494,7 @@
         <v>17</v>
       </c>
       <c r="Q85" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R85" s="6">
         <v>0</v>
@@ -8571,7 +8570,7 @@
         <v>17</v>
       </c>
       <c r="Q86" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R86" s="6">
         <v>0</v>
@@ -12099,7 +12098,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -12107,11 +12106,11 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="17.25" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="17.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="27.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="255.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="11.44140625" style="1"/>
+    <col min="1" max="1" width="27.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="255.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1">

</xml_diff>

<commit_message>
graficos poblacion + update tablas y viz
</commit_message>
<xml_diff>
--- a/Data/Base_fichas_indicadores.xlsx
+++ b/Data/Base_fichas_indicadores.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\DESCA-app\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Trabajo\DESCA\DESCA-app\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F55FF2A-303C-4F74-8723-C06AE9E5BCE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BASE_FICHAS" sheetId="4" r:id="rId1"/>
@@ -2195,7 +2196,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.000&quot;&quot;;\-#,##0.000&quot;&quot;"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -2412,10 +2413,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Excel Built-in Normal" xfId="3"/>
+    <cellStyle name="Excel Built-in Normal" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal_DISEÑO" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal_DISEÑO" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2726,42 +2727,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AI140"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="P1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E111" sqref="E111"/>
-      <selection pane="bottomLeft" activeCell="Y10" sqref="Y10"/>
+      <selection pane="bottomLeft" activeCell="Q36" sqref="Q36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="13" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" style="13" customWidth="1"/>
-    <col min="4" max="4" width="37.7109375" style="13" customWidth="1"/>
-    <col min="5" max="5" width="94.7109375" style="13" customWidth="1"/>
-    <col min="6" max="6" width="157.28515625" style="13" customWidth="1"/>
-    <col min="7" max="7" width="255.7109375" style="13" customWidth="1"/>
-    <col min="8" max="8" width="181.140625" style="13" customWidth="1"/>
-    <col min="9" max="9" width="59.42578125" style="13" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" style="13" customWidth="1"/>
-    <col min="11" max="11" width="20.42578125" style="13" customWidth="1"/>
-    <col min="12" max="12" width="20.5703125" style="13" customWidth="1"/>
-    <col min="13" max="14" width="255.7109375" style="13" customWidth="1"/>
-    <col min="15" max="15" width="230.140625" style="13" customWidth="1"/>
-    <col min="16" max="16" width="98.7109375" style="13" customWidth="1"/>
-    <col min="17" max="17" width="19.140625" style="13" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="37.6640625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="94.6640625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="157.33203125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="255.6640625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="181.109375" style="13" customWidth="1"/>
+    <col min="9" max="9" width="59.44140625" style="13" customWidth="1"/>
+    <col min="10" max="10" width="16.109375" style="13" customWidth="1"/>
+    <col min="11" max="11" width="20.44140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="20.5546875" style="13" customWidth="1"/>
+    <col min="13" max="14" width="255.6640625" style="13" customWidth="1"/>
+    <col min="15" max="15" width="230.109375" style="13" customWidth="1"/>
+    <col min="16" max="16" width="98.6640625" style="13" customWidth="1"/>
+    <col min="17" max="17" width="19.109375" style="13" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.88671875" style="13" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="22" max="26" width="9.42578125" style="13" customWidth="1"/>
-    <col min="27" max="29" width="9.140625" style="13"/>
-    <col min="30" max="30" width="55.140625" style="13" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="13"/>
+    <col min="21" max="21" width="15.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="26" width="9.44140625" style="13" customWidth="1"/>
+    <col min="27" max="29" width="9.109375" style="13"/>
+    <col min="30" max="30" width="55.109375" style="13" customWidth="1"/>
+    <col min="31" max="16384" width="9.109375" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -2876,7 +2877,7 @@
         <v>17</v>
       </c>
       <c r="Q2" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R2" s="6">
         <v>0</v>
@@ -4145,7 +4146,7 @@
         <v>510</v>
       </c>
       <c r="Q22" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R22" s="6">
         <v>0</v>
@@ -5110,7 +5111,7 @@
         <v>17</v>
       </c>
       <c r="Q35" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R35" s="6">
         <v>0</v>
@@ -11879,7 +11880,7 @@
         <v>0</v>
       </c>
       <c r="T134" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U134" s="6">
         <v>0</v>
@@ -12098,7 +12099,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -12106,11 +12107,11 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="17.25" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="17.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="255.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="27.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="255.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1">

</xml_diff>

<commit_message>
Act Bases Mirador y Fichas
</commit_message>
<xml_diff>
--- a/Data/Base_fichas_indicadores.xlsx
+++ b/Data/Base_fichas_indicadores.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Trabajo\DESCA\DESCA-app\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\DESCA-app\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F55FF2A-303C-4F74-8723-C06AE9E5BCE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="BASE_FICHAS" sheetId="4" r:id="rId1"/>
@@ -969,9 +968,6 @@
     <t>Para cada año calcular: (Cantidad de nacidos vivos -o niños y niñas- inmunizados según tipo de vacuna / Total de nacidos vivos -o niños y niñas-)*100</t>
   </si>
   <si>
-    <t>Porcentaje de nacidos vivos o niños inmunizados según tipo de vacuna y dosis (estimación OMS - UNICEF)</t>
-  </si>
-  <si>
     <t>No es un gasto soportable en vivienda aquel cuya erogación tiene como consecuencia que una persona se ubique debajo de la línea de pobreza monetaria.</t>
   </si>
   <si>
@@ -2191,12 +2187,15 @@
   </si>
   <si>
     <t>ASCENDENCIA_POB</t>
+  </si>
+  <si>
+    <t>Porcentaje de niños y niñas inmunizados según tipo de vacuna y dosis (estimación OMS - UNICEF)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.000&quot;&quot;;\-#,##0.000&quot;&quot;"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -2413,10 +2412,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Excel Built-in Normal" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Excel Built-in Normal" xfId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal_DISEÑO" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal_DISEÑO" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2727,107 +2726,107 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AI140"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="P1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="D1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E111" sqref="E111"/>
-      <selection pane="bottomLeft" activeCell="Q36" sqref="Q36"/>
+      <selection pane="bottomLeft" activeCell="F91" sqref="F91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="13" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" style="13" customWidth="1"/>
-    <col min="4" max="4" width="37.6640625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="94.6640625" style="13" customWidth="1"/>
-    <col min="6" max="6" width="157.33203125" style="13" customWidth="1"/>
-    <col min="7" max="7" width="255.6640625" style="13" customWidth="1"/>
-    <col min="8" max="8" width="181.109375" style="13" customWidth="1"/>
-    <col min="9" max="9" width="59.44140625" style="13" customWidth="1"/>
-    <col min="10" max="10" width="16.109375" style="13" customWidth="1"/>
-    <col min="11" max="11" width="20.44140625" style="13" customWidth="1"/>
-    <col min="12" max="12" width="20.5546875" style="13" customWidth="1"/>
-    <col min="13" max="14" width="255.6640625" style="13" customWidth="1"/>
-    <col min="15" max="15" width="230.109375" style="13" customWidth="1"/>
-    <col min="16" max="16" width="98.6640625" style="13" customWidth="1"/>
-    <col min="17" max="17" width="19.109375" style="13" customWidth="1"/>
-    <col min="18" max="18" width="12.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" style="13" customWidth="1"/>
+    <col min="4" max="4" width="37.7109375" style="13" customWidth="1"/>
+    <col min="5" max="5" width="94.7109375" style="13" customWidth="1"/>
+    <col min="6" max="6" width="157.28515625" style="13" customWidth="1"/>
+    <col min="7" max="7" width="255.7109375" style="13" customWidth="1"/>
+    <col min="8" max="8" width="181.140625" style="13" customWidth="1"/>
+    <col min="9" max="9" width="59.42578125" style="13" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" style="13" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" style="13" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" style="13" customWidth="1"/>
+    <col min="13" max="14" width="255.7109375" style="13" customWidth="1"/>
+    <col min="15" max="15" width="230.140625" style="13" customWidth="1"/>
+    <col min="16" max="16" width="98.7109375" style="13" customWidth="1"/>
+    <col min="17" max="17" width="19.140625" style="13" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.85546875" style="13" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="22" max="26" width="9.44140625" style="13" customWidth="1"/>
-    <col min="27" max="29" width="9.109375" style="13"/>
-    <col min="30" max="30" width="55.109375" style="13" customWidth="1"/>
-    <col min="31" max="16384" width="9.109375" style="13"/>
+    <col min="21" max="21" width="15.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="26" width="9.42578125" style="13" customWidth="1"/>
+    <col min="27" max="29" width="9.140625" style="13"/>
+    <col min="30" max="30" width="55.140625" style="13" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="26" t="s">
+        <v>348</v>
+      </c>
+      <c r="B1" s="26" t="s">
         <v>349</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="C1" s="26" t="s">
         <v>350</v>
       </c>
-      <c r="C1" s="26" t="s">
-        <v>351</v>
-      </c>
       <c r="D1" s="26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F1" s="26" t="s">
+        <v>352</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>362</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>363</v>
-      </c>
       <c r="Q1" s="26" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="R1" s="13" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="S1" s="35" t="s">
+        <v>718</v>
+      </c>
+      <c r="T1" s="35" t="s">
         <v>719</v>
       </c>
-      <c r="T1" s="35" t="s">
+      <c r="U1" s="35" t="s">
         <v>720</v>
-      </c>
-      <c r="U1" s="35" t="s">
-        <v>721</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="6" customFormat="1">
@@ -2844,13 +2843,13 @@
         <v>104</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="F2" s="31" t="s">
         <v>80</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>114</v>
@@ -2862,16 +2861,16 @@
         <v>6</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="P2" s="6" t="s">
         <v>17</v>
@@ -2906,13 +2905,13 @@
         <v>104</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="F3" s="31" t="s">
         <v>81</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>113</v>
@@ -2924,16 +2923,16 @@
         <v>6</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>17</v>
@@ -2968,13 +2967,13 @@
         <v>104</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="F4" s="31" t="s">
         <v>82</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>116</v>
@@ -2986,16 +2985,16 @@
         <v>6</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="L4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="P4" s="6" t="s">
         <v>17</v>
@@ -3030,13 +3029,13 @@
         <v>104</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>76</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>112</v>
@@ -3054,10 +3053,10 @@
         <v>8</v>
       </c>
       <c r="M5" s="6" t="s">
+        <v>526</v>
+      </c>
+      <c r="N5" s="6" t="s">
         <v>527</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>528</v>
       </c>
       <c r="P5" s="6" t="s">
         <v>17</v>
@@ -3092,16 +3091,16 @@
         <v>104</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>79</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>5</v>
@@ -3116,10 +3115,10 @@
         <v>8</v>
       </c>
       <c r="M6" s="6" t="s">
+        <v>524</v>
+      </c>
+      <c r="N6" s="6" t="s">
         <v>525</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>526</v>
       </c>
       <c r="P6" s="6" t="s">
         <v>25</v>
@@ -3154,16 +3153,16 @@
         <v>104</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>78</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>5</v>
@@ -3178,10 +3177,10 @@
         <v>8</v>
       </c>
       <c r="M7" s="6" t="s">
+        <v>524</v>
+      </c>
+      <c r="N7" s="6" t="s">
         <v>525</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>526</v>
       </c>
       <c r="P7" s="6" t="s">
         <v>25</v>
@@ -3216,13 +3215,13 @@
         <v>104</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>83</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>115</v>
@@ -3240,10 +3239,10 @@
         <v>8</v>
       </c>
       <c r="M8" s="6" t="s">
+        <v>524</v>
+      </c>
+      <c r="N8" s="6" t="s">
         <v>525</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>526</v>
       </c>
       <c r="P8" s="6" t="s">
         <v>25</v>
@@ -3278,13 +3277,13 @@
         <v>104</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>84</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>30</v>
@@ -3302,10 +3301,10 @@
         <v>8</v>
       </c>
       <c r="M9" s="6" t="s">
+        <v>524</v>
+      </c>
+      <c r="N9" s="6" t="s">
         <v>525</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>526</v>
       </c>
       <c r="P9" s="6" t="s">
         <v>85</v>
@@ -3340,13 +3339,13 @@
         <v>104</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>88</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>86</v>
@@ -3364,10 +3363,10 @@
         <v>8</v>
       </c>
       <c r="M10" s="6" t="s">
+        <v>524</v>
+      </c>
+      <c r="N10" s="6" t="s">
         <v>525</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>526</v>
       </c>
       <c r="P10" s="6" t="s">
         <v>85</v>
@@ -3402,13 +3401,13 @@
         <v>104</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>89</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>90</v>
@@ -3426,10 +3425,10 @@
         <v>8</v>
       </c>
       <c r="M11" s="6" t="s">
+        <v>524</v>
+      </c>
+      <c r="N11" s="6" t="s">
         <v>525</v>
-      </c>
-      <c r="N11" s="6" t="s">
-        <v>526</v>
       </c>
       <c r="P11" s="6" t="s">
         <v>85</v>
@@ -3464,16 +3463,16 @@
         <v>104</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>33</v>
@@ -3488,13 +3487,13 @@
         <v>8</v>
       </c>
       <c r="M12" s="6" t="s">
+        <v>524</v>
+      </c>
+      <c r="N12" s="6" t="s">
         <v>525</v>
       </c>
-      <c r="N12" s="6" t="s">
-        <v>526</v>
-      </c>
       <c r="P12" s="6" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="Q12" s="6">
         <v>0</v>
@@ -3526,13 +3525,13 @@
         <v>104</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>92</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>299</v>
@@ -3550,7 +3549,7 @@
         <v>8</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="N13" s="6" t="s">
         <v>13</v>
@@ -3588,13 +3587,13 @@
         <v>104</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>97</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>28</v>
@@ -3612,10 +3611,10 @@
         <v>300</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="P14" s="6" t="s">
         <v>96</v>
@@ -3650,16 +3649,16 @@
         <v>307</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>309</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>5</v>
@@ -3712,16 +3711,16 @@
         <v>307</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>308</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I16" s="7" t="s">
         <v>5</v>
@@ -3774,16 +3773,16 @@
         <v>307</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>306</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="I17" s="7" t="s">
         <v>5</v>
@@ -3836,13 +3835,13 @@
         <v>3</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F18" s="13" t="s">
         <v>4</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H18" s="14" t="s">
         <v>139</v>
@@ -3869,7 +3868,7 @@
         <v>10</v>
       </c>
       <c r="P18" s="13" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="Q18" s="6">
         <v>1</v>
@@ -3901,13 +3900,13 @@
         <v>3</v>
       </c>
       <c r="E19" s="30" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F19" s="13" t="s">
         <v>100</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H19" s="14" t="s">
         <v>140</v>
@@ -3934,7 +3933,7 @@
         <v>11</v>
       </c>
       <c r="P19" s="13" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="Q19" s="6">
         <v>1</v>
@@ -3966,13 +3965,13 @@
         <v>3</v>
       </c>
       <c r="E20" s="30" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F20" s="13" t="s">
         <v>102</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="H20" s="14" t="s">
         <v>141</v>
@@ -3999,7 +3998,7 @@
         <v>11</v>
       </c>
       <c r="P20" s="13" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="Q20" s="6">
         <v>0</v>
@@ -4031,13 +4030,13 @@
         <v>3</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F21" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H21" s="13" t="s">
         <v>148</v>
@@ -4064,7 +4063,7 @@
         <v>10</v>
       </c>
       <c r="P21" s="13" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="Q21" s="6">
         <v>0</v>
@@ -4110,13 +4109,13 @@
         <v>3</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H22" s="13" t="s">
         <v>149</v>
@@ -4143,7 +4142,7 @@
         <v>10</v>
       </c>
       <c r="P22" s="13" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="Q22" s="6">
         <v>0</v>
@@ -4189,13 +4188,13 @@
         <v>3</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="F23" s="13" t="s">
         <v>20</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H23" s="13" t="s">
         <v>150</v>
@@ -4222,7 +4221,7 @@
         <v>10</v>
       </c>
       <c r="P23" s="13" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="Q23" s="6">
         <v>0</v>
@@ -4254,13 +4253,13 @@
         <v>3</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="F24" s="15" t="s">
         <v>301</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H24" s="15" t="s">
         <v>302</v>
@@ -4287,7 +4286,7 @@
         <v>234</v>
       </c>
       <c r="P24" s="13" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="Q24" s="6">
         <v>0</v>
@@ -4333,13 +4332,13 @@
         <v>3</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F25" s="15" t="s">
         <v>236</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H25" s="15" t="s">
         <v>235</v>
@@ -4366,7 +4365,7 @@
         <v>234</v>
       </c>
       <c r="P25" s="13" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="Q25" s="6">
         <v>1</v>
@@ -4412,13 +4411,13 @@
         <v>12</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>98</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H26" s="6" t="s">
         <v>142</v>
@@ -4436,16 +4435,16 @@
         <v>8</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="N26" s="6" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="O26" s="6" t="s">
         <v>14</v>
       </c>
       <c r="P26" s="6" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="Q26" s="6">
         <v>0</v>
@@ -4477,13 +4476,13 @@
         <v>12</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>73</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H27" s="6" t="s">
         <v>143</v>
@@ -4501,16 +4500,16 @@
         <v>8</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="N27" s="6" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="O27" s="6" t="s">
         <v>14</v>
       </c>
       <c r="P27" s="6" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="Q27" s="6">
         <v>0</v>
@@ -4556,13 +4555,13 @@
         <v>12</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>99</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="H28" s="6" t="s">
         <v>151</v>
@@ -4580,16 +4579,16 @@
         <v>8</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="N28" s="6" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="O28" s="6" t="s">
         <v>14</v>
       </c>
       <c r="P28" s="6" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="Q28" s="6">
         <v>0</v>
@@ -4635,16 +4634,16 @@
         <v>12</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F29" s="13" t="s">
         <v>101</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="I29" s="13" t="s">
         <v>5</v>
@@ -4659,16 +4658,16 @@
         <v>8</v>
       </c>
       <c r="M29" s="13" t="s">
+        <v>524</v>
+      </c>
+      <c r="N29" s="13" t="s">
         <v>525</v>
-      </c>
-      <c r="N29" s="13" t="s">
-        <v>526</v>
       </c>
       <c r="O29" s="13" t="s">
         <v>21</v>
       </c>
       <c r="P29" s="13" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="Q29" s="6">
         <v>0</v>
@@ -4700,16 +4699,16 @@
         <v>12</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F30" s="13" t="s">
         <v>103</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="I30" s="13" t="s">
         <v>5</v>
@@ -4724,16 +4723,16 @@
         <v>8</v>
       </c>
       <c r="M30" s="13" t="s">
+        <v>524</v>
+      </c>
+      <c r="N30" s="13" t="s">
         <v>525</v>
-      </c>
-      <c r="N30" s="13" t="s">
-        <v>526</v>
       </c>
       <c r="O30" s="13" t="s">
         <v>21</v>
       </c>
       <c r="P30" s="13" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="Q30" s="6">
         <v>0</v>
@@ -4779,13 +4778,13 @@
         <v>15</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>108</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H31" s="13" t="s">
         <v>144</v>
@@ -4803,10 +4802,10 @@
         <v>16</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="N31" s="6" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="O31" s="16"/>
       <c r="P31" s="13" t="s">
@@ -4856,13 +4855,13 @@
         <v>15</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>109</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="H32" s="13" t="s">
         <v>145</v>
@@ -4880,10 +4879,10 @@
         <v>16</v>
       </c>
       <c r="M32" s="6" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="N32" s="6" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="O32" s="16"/>
       <c r="P32" s="13" t="s">
@@ -4933,13 +4932,13 @@
         <v>15</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>107</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="H33" s="13" t="s">
         <v>146</v>
@@ -4957,10 +4956,10 @@
         <v>16</v>
       </c>
       <c r="M33" s="6" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="O33" s="16"/>
       <c r="P33" s="13" t="s">
@@ -4996,13 +4995,13 @@
         <v>15</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>110</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="H34" s="13" t="s">
         <v>147</v>
@@ -5020,10 +5019,10 @@
         <v>16</v>
       </c>
       <c r="M34" s="6" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="N34" s="6" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="O34" s="6" t="s">
         <v>105</v>
@@ -5075,13 +5074,13 @@
         <v>15</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>22</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H35" s="6" t="s">
         <v>152</v>
@@ -5140,13 +5139,13 @@
         <v>3</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F36" s="13" t="s">
         <v>74</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="H36" s="13" t="s">
         <v>153</v>
@@ -5173,7 +5172,7 @@
         <v>75</v>
       </c>
       <c r="P36" s="13" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="Q36" s="6">
         <v>0</v>
@@ -5205,13 +5204,13 @@
         <v>104</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F37" s="31" t="s">
         <v>118</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H37" s="6" t="s">
         <v>119</v>
@@ -5223,16 +5222,16 @@
         <v>6</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="L37" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M37" s="6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="P37" s="6" t="s">
         <v>17</v>
@@ -5267,13 +5266,13 @@
         <v>104</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F38" s="31" t="s">
         <v>120</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H38" s="6" t="s">
         <v>121</v>
@@ -5291,10 +5290,10 @@
         <v>8</v>
       </c>
       <c r="M38" s="6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="N38" s="6" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="P38" s="6" t="s">
         <v>17</v>
@@ -5329,16 +5328,16 @@
         <v>104</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F39" s="31" t="s">
         <v>122</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="I39" s="6" t="s">
         <v>5</v>
@@ -5347,16 +5346,16 @@
         <v>6</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="L39" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M39" s="6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="N39" s="6" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="P39" s="6" t="s">
         <v>17</v>
@@ -5391,13 +5390,13 @@
         <v>104</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>123</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="H40" s="6" t="s">
         <v>124</v>
@@ -5415,10 +5414,10 @@
         <v>8</v>
       </c>
       <c r="M40" s="6" t="s">
+        <v>526</v>
+      </c>
+      <c r="N40" s="6" t="s">
         <v>527</v>
-      </c>
-      <c r="N40" s="6" t="s">
-        <v>528</v>
       </c>
       <c r="P40" s="6" t="s">
         <v>17</v>
@@ -5453,19 +5452,19 @@
         <v>104</v>
       </c>
       <c r="E41" s="30" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F41" s="24" t="s">
+        <v>321</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>454</v>
+      </c>
+      <c r="H41" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="G41" s="6" t="s">
-        <v>455</v>
-      </c>
-      <c r="H41" s="6" t="s">
+      <c r="I41" s="6" t="s">
         <v>323</v>
-      </c>
-      <c r="I41" s="6" t="s">
-        <v>324</v>
       </c>
       <c r="J41" s="6" t="s">
         <v>6</v>
@@ -5477,14 +5476,14 @@
         <v>8</v>
       </c>
       <c r="M41" s="24" t="s">
+        <v>324</v>
+      </c>
+      <c r="N41" s="6" t="s">
         <v>325</v>
-      </c>
-      <c r="N41" s="6" t="s">
-        <v>326</v>
       </c>
       <c r="O41" s="6"/>
       <c r="P41" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="Q41" s="6">
         <v>0</v>
@@ -5530,38 +5529,38 @@
         <v>104</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="F42" s="24" t="s">
+        <v>327</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>455</v>
+      </c>
+      <c r="H42" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="G42" s="6" t="s">
-        <v>456</v>
-      </c>
-      <c r="H42" s="6" t="s">
-        <v>329</v>
-      </c>
       <c r="I42" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J42" s="6" t="s">
         <v>6</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="L42" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M42" s="24" t="s">
+        <v>330</v>
+      </c>
+      <c r="N42" s="6" t="s">
         <v>331</v>
-      </c>
-      <c r="N42" s="6" t="s">
-        <v>332</v>
       </c>
       <c r="O42" s="25"/>
       <c r="P42" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="Q42" s="6">
         <v>0</v>
@@ -5607,38 +5606,38 @@
         <v>104</v>
       </c>
       <c r="E43" s="30" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F43" s="24" t="s">
+        <v>332</v>
+      </c>
+      <c r="G43" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="G43" s="6" t="s">
+      <c r="H43" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="H43" s="6" t="s">
-        <v>335</v>
-      </c>
       <c r="I43" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="J43" s="6" t="s">
         <v>6</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="L43" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M43" s="24" t="s">
+        <v>336</v>
+      </c>
+      <c r="N43" s="6" t="s">
         <v>337</v>
-      </c>
-      <c r="N43" s="6" t="s">
-        <v>338</v>
       </c>
       <c r="O43" s="25"/>
       <c r="P43" s="6" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="Q43" s="6">
         <v>0</v>
@@ -5684,13 +5683,13 @@
         <v>36</v>
       </c>
       <c r="E44" s="30" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F44" s="13" t="s">
         <v>37</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="H44" s="13" t="s">
         <v>38</v>
@@ -5717,7 +5716,7 @@
         <v>40</v>
       </c>
       <c r="P44" s="13" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="Q44" s="6">
         <v>1</v>
@@ -5763,13 +5762,13 @@
         <v>41</v>
       </c>
       <c r="E45" s="32" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F45" s="13" t="s">
         <v>42</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="H45" s="13" t="s">
         <v>154</v>
@@ -5796,7 +5795,7 @@
         <v>43</v>
       </c>
       <c r="P45" s="13" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="Q45" s="6">
         <v>0</v>
@@ -5842,13 +5841,13 @@
         <v>41</v>
       </c>
       <c r="E46" s="32" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F46" s="13" t="s">
         <v>44</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H46" s="13" t="s">
         <v>155</v>
@@ -5875,7 +5874,7 @@
         <v>45</v>
       </c>
       <c r="P46" s="13" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="Q46" s="6">
         <v>0</v>
@@ -5921,13 +5920,13 @@
         <v>41</v>
       </c>
       <c r="E47" s="32" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="H47" s="6" t="s">
         <v>189</v>
@@ -5951,10 +5950,10 @@
         <v>195</v>
       </c>
       <c r="O47" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="P47" s="6" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="Q47" s="6">
         <v>1</v>
@@ -5986,13 +5985,13 @@
         <v>41</v>
       </c>
       <c r="E48" s="32" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>161</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="H48" s="13" t="s">
         <v>162</v>
@@ -6019,7 +6018,7 @@
         <v>163</v>
       </c>
       <c r="P48" s="13" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="Q48" s="6">
         <v>0</v>
@@ -6051,16 +6050,16 @@
         <v>46</v>
       </c>
       <c r="E49" s="32" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="H49" s="27" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="I49" s="6" t="s">
         <v>5</v>
@@ -6081,10 +6080,10 @@
         <v>195</v>
       </c>
       <c r="O49" s="7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="P49" s="6" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="Q49" s="6">
         <v>0</v>
@@ -6116,16 +6115,16 @@
         <v>46</v>
       </c>
       <c r="E50" s="32" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H50" s="27" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="I50" s="6" t="s">
         <v>5</v>
@@ -6146,10 +6145,10 @@
         <v>195</v>
       </c>
       <c r="O50" s="7" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="P50" s="13" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="Q50" s="6">
         <v>0</v>
@@ -6195,16 +6194,16 @@
         <v>46</v>
       </c>
       <c r="E51" s="32" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="H51" s="27" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="I51" s="6" t="s">
         <v>5</v>
@@ -6225,10 +6224,10 @@
         <v>195</v>
       </c>
       <c r="O51" s="7" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="P51" s="13" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="Q51" s="6">
         <v>0</v>
@@ -6274,16 +6273,16 @@
         <v>46</v>
       </c>
       <c r="E52" s="32" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F52" s="28" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H52" s="27" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="I52" s="6" t="s">
         <v>5</v>
@@ -6304,10 +6303,10 @@
         <v>195</v>
       </c>
       <c r="O52" s="7" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="P52" s="13" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="Q52" s="6">
         <v>0</v>
@@ -6353,16 +6352,16 @@
         <v>47</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="F53" s="28" t="s">
+        <v>683</v>
+      </c>
+      <c r="G53" s="28" t="s">
         <v>684</v>
       </c>
-      <c r="G53" s="28" t="s">
-        <v>685</v>
-      </c>
       <c r="H53" s="34" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="I53" s="6" t="s">
         <v>5</v>
@@ -6383,10 +6382,10 @@
         <v>195</v>
       </c>
       <c r="O53" s="7" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="P53" s="13" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="Q53" s="6">
         <v>1</v>
@@ -6432,13 +6431,13 @@
         <v>47</v>
       </c>
       <c r="E54" s="32" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="F54" s="13" t="s">
         <v>48</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H54" s="13" t="s">
         <v>156</v>
@@ -6465,7 +6464,7 @@
         <v>49</v>
       </c>
       <c r="P54" s="13" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="Q54" s="6">
         <v>0</v>
@@ -6511,13 +6510,13 @@
         <v>50</v>
       </c>
       <c r="E55" s="32" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F55" s="13" t="s">
         <v>51</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H55" s="13" t="s">
         <v>157</v>
@@ -6542,7 +6541,7 @@
       </c>
       <c r="O55" s="13"/>
       <c r="P55" s="13" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="Q55" s="6">
         <v>1</v>
@@ -6588,13 +6587,13 @@
         <v>104</v>
       </c>
       <c r="E56" s="32" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F56" s="31" t="s">
         <v>125</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H56" s="6" t="s">
         <v>126</v>
@@ -6606,16 +6605,16 @@
         <v>6</v>
       </c>
       <c r="K56" s="6" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="L56" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M56" s="6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="N56" s="6" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="P56" s="6" t="s">
         <v>17</v>
@@ -6650,13 +6649,13 @@
         <v>104</v>
       </c>
       <c r="E57" s="30" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F57" s="31" t="s">
         <v>127</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="H57" s="6" t="s">
         <v>128</v>
@@ -6674,10 +6673,10 @@
         <v>8</v>
       </c>
       <c r="M57" s="6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="N57" s="6" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="P57" s="6" t="s">
         <v>17</v>
@@ -6712,16 +6711,16 @@
         <v>104</v>
       </c>
       <c r="E58" s="30" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F58" s="31" t="s">
         <v>129</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="I58" s="6" t="s">
         <v>5</v>
@@ -6730,16 +6729,16 @@
         <v>6</v>
       </c>
       <c r="K58" s="6" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="L58" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M58" s="6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="N58" s="6" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="P58" s="6" t="s">
         <v>17</v>
@@ -6774,13 +6773,13 @@
         <v>104</v>
       </c>
       <c r="E59" s="30" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>130</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="H59" s="6" t="s">
         <v>131</v>
@@ -6798,10 +6797,10 @@
         <v>8</v>
       </c>
       <c r="M59" s="6" t="s">
+        <v>526</v>
+      </c>
+      <c r="N59" s="6" t="s">
         <v>527</v>
-      </c>
-      <c r="N59" s="6" t="s">
-        <v>528</v>
       </c>
       <c r="P59" s="6" t="s">
         <v>17</v>
@@ -6836,13 +6835,13 @@
         <v>104</v>
       </c>
       <c r="E60" s="30" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>171</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="H60" s="6" t="s">
         <v>170</v>
@@ -6860,10 +6859,10 @@
         <v>8</v>
       </c>
       <c r="M60" s="6" t="s">
+        <v>528</v>
+      </c>
+      <c r="N60" s="6" t="s">
         <v>529</v>
-      </c>
-      <c r="N60" s="6" t="s">
-        <v>530</v>
       </c>
       <c r="P60" s="6" t="s">
         <v>17</v>
@@ -6898,13 +6897,13 @@
         <v>104</v>
       </c>
       <c r="E61" s="30" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>172</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H61" s="6" t="s">
         <v>173</v>
@@ -6922,10 +6921,10 @@
         <v>8</v>
       </c>
       <c r="M61" s="6" t="s">
+        <v>528</v>
+      </c>
+      <c r="N61" s="6" t="s">
         <v>529</v>
-      </c>
-      <c r="N61" s="6" t="s">
-        <v>530</v>
       </c>
       <c r="P61" s="6" t="s">
         <v>17</v>
@@ -6960,13 +6959,13 @@
         <v>104</v>
       </c>
       <c r="E62" s="30" t="s">
+        <v>678</v>
+      </c>
+      <c r="F62" s="5" t="s">
         <v>679</v>
       </c>
-      <c r="F62" s="5" t="s">
-        <v>680</v>
-      </c>
       <c r="G62" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H62" s="6" t="s">
         <v>174</v>
@@ -6984,10 +6983,10 @@
         <v>8</v>
       </c>
       <c r="M62" s="6" t="s">
+        <v>528</v>
+      </c>
+      <c r="N62" s="6" t="s">
         <v>529</v>
-      </c>
-      <c r="N62" s="6" t="s">
-        <v>530</v>
       </c>
       <c r="P62" s="6" t="s">
         <v>17</v>
@@ -7022,13 +7021,13 @@
         <v>3</v>
       </c>
       <c r="E63" s="30" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F63" s="6" t="s">
         <v>53</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="H63" s="6" t="s">
         <v>158</v>
@@ -7040,7 +7039,7 @@
         <v>6</v>
       </c>
       <c r="K63" s="6" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="L63" s="6" t="s">
         <v>8</v>
@@ -7087,13 +7086,13 @@
         <v>3</v>
       </c>
       <c r="E64" s="30" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F64" s="6" t="s">
         <v>304</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="H64" s="6" t="s">
         <v>159</v>
@@ -7120,7 +7119,7 @@
         <v>54</v>
       </c>
       <c r="P64" s="13" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="Q64" s="6">
         <v>1</v>
@@ -7152,16 +7151,16 @@
         <v>3</v>
       </c>
       <c r="E65" s="30" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="F65" s="6" t="s">
         <v>55</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="I65" s="6" t="s">
         <v>5</v>
@@ -7185,7 +7184,7 @@
         <v>54</v>
       </c>
       <c r="P65" s="13" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="Q65" s="6">
         <v>0</v>
@@ -7223,10 +7222,10 @@
         <v>56</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I66" s="6" t="s">
         <v>5</v>
@@ -7250,7 +7249,7 @@
         <v>54</v>
       </c>
       <c r="P66" s="13" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="Q66" s="6">
         <v>1</v>
@@ -7282,16 +7281,16 @@
         <v>3</v>
       </c>
       <c r="E67" s="30" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="F67" s="6" t="s">
         <v>57</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="I67" s="6" t="s">
         <v>5</v>
@@ -7347,16 +7346,16 @@
         <v>3</v>
       </c>
       <c r="E68" s="30" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F68" s="6" t="s">
         <v>58</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H68" s="6" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="I68" s="6" t="s">
         <v>5</v>
@@ -7412,13 +7411,13 @@
         <v>3</v>
       </c>
       <c r="E69" s="30" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F69" s="6" t="s">
         <v>303</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="H69" s="6" t="s">
         <v>159</v>
@@ -7445,7 +7444,7 @@
         <v>54</v>
       </c>
       <c r="P69" s="13" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="Q69" s="6">
         <v>0</v>
@@ -7477,16 +7476,16 @@
         <v>59</v>
       </c>
       <c r="E70" s="30" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F70" s="6" t="s">
         <v>60</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="H70" s="6" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="I70" s="6" t="s">
         <v>5</v>
@@ -7542,16 +7541,16 @@
         <v>59</v>
       </c>
       <c r="E71" s="30" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>164</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H71" s="6" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="I71" s="6" t="s">
         <v>5</v>
@@ -7607,16 +7606,16 @@
         <v>59</v>
       </c>
       <c r="E72" s="30" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="F72" s="6" t="s">
         <v>62</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I72" s="6" t="s">
         <v>5</v>
@@ -7672,16 +7671,16 @@
         <v>59</v>
       </c>
       <c r="E73" s="30" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F73" s="6" t="s">
         <v>63</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="I73" s="6" t="s">
         <v>5</v>
@@ -7737,16 +7736,16 @@
         <v>59</v>
       </c>
       <c r="E74" s="30" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="F74" s="6" t="s">
         <v>165</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H74" s="6" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I74" s="6" t="s">
         <v>5</v>
@@ -7802,16 +7801,16 @@
         <v>59</v>
       </c>
       <c r="E75" s="30" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F75" s="6" t="s">
         <v>166</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H75" s="6" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I75" s="6" t="s">
         <v>5</v>
@@ -7867,16 +7866,16 @@
         <v>59</v>
       </c>
       <c r="E76" s="30" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F76" s="6" t="s">
         <v>167</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H76" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="I76" s="6" t="s">
         <v>5</v>
@@ -7932,16 +7931,16 @@
         <v>59</v>
       </c>
       <c r="E77" s="30" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F77" s="6" t="s">
         <v>168</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H77" s="6" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I77" s="6" t="s">
         <v>5</v>
@@ -7997,16 +7996,16 @@
         <v>59</v>
       </c>
       <c r="E78" s="30" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F78" s="6" t="s">
         <v>64</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H78" s="6" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I78" s="6" t="s">
         <v>5</v>
@@ -8062,16 +8061,16 @@
         <v>59</v>
       </c>
       <c r="E79" s="30" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="F79" s="6" t="s">
         <v>65</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H79" s="6" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I79" s="6" t="s">
         <v>5</v>
@@ -8127,16 +8126,16 @@
         <v>59</v>
       </c>
       <c r="E80" s="30" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="F80" s="6" t="s">
         <v>66</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="H80" s="6" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="I80" s="6" t="s">
         <v>5</v>
@@ -8192,16 +8191,16 @@
         <v>59</v>
       </c>
       <c r="E81" s="30" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="F81" s="6" t="s">
         <v>67</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H81" s="6" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I81" s="6" t="s">
         <v>5</v>
@@ -8257,13 +8256,13 @@
         <v>59</v>
       </c>
       <c r="E82" s="30" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F82" s="6" t="s">
         <v>68</v>
       </c>
       <c r="G82" s="6" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="H82" s="6" t="s">
         <v>160</v>
@@ -8322,13 +8321,13 @@
         <v>104</v>
       </c>
       <c r="E83" s="30" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F83" s="31" t="s">
         <v>132</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H83" s="6" t="s">
         <v>133</v>
@@ -8340,16 +8339,16 @@
         <v>6</v>
       </c>
       <c r="K83" s="6" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="L83" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M83" s="6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="N83" s="6" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="P83" s="6" t="s">
         <v>17</v>
@@ -8384,13 +8383,13 @@
         <v>104</v>
       </c>
       <c r="E84" s="30" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F84" s="31" t="s">
         <v>134</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H84" s="6" t="s">
         <v>135</v>
@@ -8408,10 +8407,10 @@
         <v>8</v>
       </c>
       <c r="M84" s="6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="N84" s="6" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="O84" s="6"/>
       <c r="P84" s="6" t="s">
@@ -8461,16 +8460,16 @@
         <v>104</v>
       </c>
       <c r="E85" s="30" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F85" s="31" t="s">
         <v>136</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H85" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="I85" s="6" t="s">
         <v>5</v>
@@ -8479,16 +8478,16 @@
         <v>6</v>
       </c>
       <c r="K85" s="6" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="L85" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M85" s="6" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="N85" s="6" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="O85" s="6"/>
       <c r="P85" s="6" t="s">
@@ -8538,13 +8537,13 @@
         <v>104</v>
       </c>
       <c r="E86" s="30" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F86" s="6" t="s">
         <v>137</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="H86" s="6" t="s">
         <v>138</v>
@@ -8562,10 +8561,10 @@
         <v>8</v>
       </c>
       <c r="M86" s="6" t="s">
+        <v>526</v>
+      </c>
+      <c r="N86" s="6" t="s">
         <v>527</v>
-      </c>
-      <c r="N86" s="6" t="s">
-        <v>528</v>
       </c>
       <c r="P86" s="6" t="s">
         <v>17</v>
@@ -8600,16 +8599,16 @@
         <v>104</v>
       </c>
       <c r="E87" s="30" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="F87" s="19" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="I87" s="7" t="s">
         <v>238</v>
@@ -8677,16 +8676,16 @@
         <v>104</v>
       </c>
       <c r="E88" s="32" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F88" s="19" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="H88" s="7" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="I88" s="7" t="s">
         <v>243</v>
@@ -8739,16 +8738,16 @@
         <v>104</v>
       </c>
       <c r="E89" s="30" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F89" s="19" t="s">
         <v>245</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="H89" s="7" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="I89" s="7" t="s">
         <v>238</v>
@@ -8816,16 +8815,16 @@
         <v>104</v>
       </c>
       <c r="E90" s="30" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="F90" s="20" t="s">
         <v>248</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="H90" s="7" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="I90" s="7" t="s">
         <v>243</v>
@@ -8893,13 +8892,13 @@
         <v>307</v>
       </c>
       <c r="E91" s="30" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>314</v>
+        <v>721</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="H91" s="2" t="s">
         <v>313</v>
@@ -8967,16 +8966,16 @@
         <v>2</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F92" s="6" t="s">
         <v>190</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H92" s="6" t="s">
         <v>191</v>
@@ -9001,7 +9000,7 @@
       </c>
       <c r="O92" s="6"/>
       <c r="P92" s="6" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="Q92" s="6">
         <v>1</v>
@@ -9044,7 +9043,7 @@
         <v>2</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E93" s="30" t="s">
         <v>71</v>
@@ -9053,10 +9052,10 @@
         <v>71</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H93" s="6" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I93" s="6" t="s">
         <v>192</v>
@@ -9078,7 +9077,7 @@
       </c>
       <c r="O93" s="6"/>
       <c r="P93" s="6" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="Q93" s="6">
         <v>1</v>
@@ -9121,19 +9120,19 @@
         <v>2</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E94" s="30" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>295</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="I94" s="11" t="s">
         <v>296</v>
@@ -9198,10 +9197,10 @@
         <v>2</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E95" s="30" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F95" s="12" t="s">
         <v>197</v>
@@ -9210,7 +9209,7 @@
         <v>198</v>
       </c>
       <c r="H95" s="11" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="I95" s="11" t="s">
         <v>199</v>
@@ -9260,10 +9259,10 @@
         <v>2</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E96" s="30" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="F96" s="12" t="s">
         <v>231</v>
@@ -9272,7 +9271,7 @@
         <v>203</v>
       </c>
       <c r="H96" s="11" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="I96" s="11" t="s">
         <v>199</v>
@@ -9322,19 +9321,19 @@
         <v>2</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E97" s="30" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F97" s="12" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G97" s="6" t="s">
         <v>204</v>
       </c>
       <c r="H97" s="11" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="I97" s="11" t="s">
         <v>199</v>
@@ -9384,10 +9383,10 @@
         <v>2</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E98" s="30" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="F98" s="12" t="s">
         <v>232</v>
@@ -9396,7 +9395,7 @@
         <v>205</v>
       </c>
       <c r="H98" s="11" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="I98" s="11" t="s">
         <v>206</v>
@@ -9446,10 +9445,10 @@
         <v>2</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E99" s="30" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F99" s="12" t="s">
         <v>207</v>
@@ -9458,7 +9457,7 @@
         <v>208</v>
       </c>
       <c r="H99" s="11" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="I99" s="11" t="s">
         <v>209</v>
@@ -9508,10 +9507,10 @@
         <v>2</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E100" s="30" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F100" s="12" t="s">
         <v>225</v>
@@ -9520,7 +9519,7 @@
         <v>214</v>
       </c>
       <c r="H100" s="11" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="I100" s="11" t="s">
         <v>215</v>
@@ -9570,10 +9569,10 @@
         <v>2</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E101" s="30" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="F101" s="12" t="s">
         <v>226</v>
@@ -9582,7 +9581,7 @@
         <v>217</v>
       </c>
       <c r="H101" s="11" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="I101" s="11" t="s">
         <v>215</v>
@@ -9632,10 +9631,10 @@
         <v>2</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E102" s="30" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="F102" s="12" t="s">
         <v>227</v>
@@ -9644,7 +9643,7 @@
         <v>218</v>
       </c>
       <c r="H102" s="11" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="I102" s="11" t="s">
         <v>215</v>
@@ -9694,10 +9693,10 @@
         <v>2</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E103" s="30" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="F103" s="12" t="s">
         <v>228</v>
@@ -9706,7 +9705,7 @@
         <v>219</v>
       </c>
       <c r="H103" s="11" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="I103" s="11" t="s">
         <v>215</v>
@@ -9771,10 +9770,10 @@
         <v>2</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E104" s="30" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="F104" s="12" t="s">
         <v>229</v>
@@ -9783,7 +9782,7 @@
         <v>220</v>
       </c>
       <c r="H104" s="11" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="I104" s="11" t="s">
         <v>215</v>
@@ -9848,10 +9847,10 @@
         <v>2</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="E105" s="30" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="F105" s="12" t="s">
         <v>230</v>
@@ -9860,7 +9859,7 @@
         <v>221</v>
       </c>
       <c r="H105" s="11" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="I105" s="11" t="s">
         <v>215</v>
@@ -9928,13 +9927,13 @@
         <v>3</v>
       </c>
       <c r="E106" s="30" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="F106" s="21" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="G106" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H106" s="7" t="s">
         <v>260</v>
@@ -9990,13 +9989,13 @@
         <v>3</v>
       </c>
       <c r="E107" s="30" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="F107" s="8" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H107" s="7" t="s">
         <v>262</v>
@@ -10052,13 +10051,13 @@
         <v>3</v>
       </c>
       <c r="E108" s="30" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="F108" s="8" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="G108" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H108" s="7" t="s">
         <v>264</v>
@@ -10114,13 +10113,13 @@
         <v>3</v>
       </c>
       <c r="E109" s="30" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="F109" s="8" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="G109" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H109" s="7" t="s">
         <v>270</v>
@@ -10191,13 +10190,13 @@
         <v>3</v>
       </c>
       <c r="E110" s="30" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="F110" s="22" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="G110" s="6" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="H110" s="7" t="s">
         <v>266</v>
@@ -10253,13 +10252,13 @@
         <v>3</v>
       </c>
       <c r="E111" s="30" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="F111" s="22" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="G111" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="H111" s="7" t="s">
         <v>268</v>
@@ -10330,13 +10329,13 @@
         <v>3</v>
       </c>
       <c r="E112" s="30" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="F112" s="7" t="s">
         <v>249</v>
       </c>
       <c r="G112" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H112" s="7" t="s">
         <v>250</v>
@@ -10392,13 +10391,13 @@
         <v>3</v>
       </c>
       <c r="E113" s="30" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="F113" s="7" t="s">
         <v>252</v>
       </c>
       <c r="G113" s="6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H113" s="7" t="s">
         <v>253</v>
@@ -10454,13 +10453,13 @@
         <v>3</v>
       </c>
       <c r="E114" s="30" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="F114" s="7" t="s">
         <v>254</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H114" s="7" t="s">
         <v>255</v>
@@ -10516,13 +10515,13 @@
         <v>15</v>
       </c>
       <c r="E115" s="30" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F115" s="21" t="s">
         <v>256</v>
       </c>
       <c r="G115" s="6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="H115" s="7" t="s">
         <v>257</v>
@@ -10578,16 +10577,16 @@
         <v>15</v>
       </c>
       <c r="E116" s="30" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F116" s="8" t="s">
         <v>273</v>
       </c>
       <c r="G116" s="6" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="H116" s="7" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="I116" s="7" t="s">
         <v>5</v>
@@ -10655,16 +10654,16 @@
         <v>15</v>
       </c>
       <c r="E117" s="30" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="F117" s="2" t="s">
         <v>298</v>
       </c>
       <c r="G117" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H117" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="I117" s="11" t="s">
         <v>5</v>
@@ -10732,7 +10731,7 @@
         <v>15</v>
       </c>
       <c r="E118" s="30" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="F118" s="12" t="s">
         <v>210</v>
@@ -10741,7 +10740,7 @@
         <v>222</v>
       </c>
       <c r="H118" s="11" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="I118" s="11" t="s">
         <v>211</v>
@@ -10794,7 +10793,7 @@
         <v>15</v>
       </c>
       <c r="E119" s="30" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="F119" s="12" t="s">
         <v>212</v>
@@ -10803,7 +10802,7 @@
         <v>223</v>
       </c>
       <c r="H119" s="11" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="I119" s="11" t="s">
         <v>211</v>
@@ -10856,7 +10855,7 @@
         <v>15</v>
       </c>
       <c r="E120" s="30" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F120" s="12" t="s">
         <v>213</v>
@@ -10865,7 +10864,7 @@
         <v>224</v>
       </c>
       <c r="H120" s="11" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="I120" s="11" t="s">
         <v>211</v>
@@ -10918,16 +10917,16 @@
         <v>15</v>
       </c>
       <c r="E121" s="30" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="F121" s="7" t="s">
         <v>272</v>
       </c>
       <c r="G121" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H121" s="7" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="I121" s="7" t="s">
         <v>5</v>
@@ -10992,16 +10991,16 @@
         <v>2</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E122" s="30" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F122" s="33" t="s">
         <v>274</v>
       </c>
       <c r="G122" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H122" s="23" t="s">
         <v>275</v>
@@ -11052,13 +11051,13 @@
         <v>2</v>
       </c>
       <c r="D123" s="6" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E123" s="30" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="F123" s="33" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G123" s="6" t="s">
         <v>279</v>
@@ -11112,10 +11111,10 @@
         <v>2</v>
       </c>
       <c r="D124" s="6" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E124" s="30" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="F124" s="33" t="s">
         <v>281</v>
@@ -11172,10 +11171,10 @@
         <v>2</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E125" s="30" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="F125" s="33" t="s">
         <v>284</v>
@@ -11247,19 +11246,19 @@
         <v>2</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E126" s="30" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="F126" s="33" t="s">
         <v>287</v>
       </c>
       <c r="G126" s="6" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="H126" s="23" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I126" s="23"/>
       <c r="J126" s="7" t="s">
@@ -11322,10 +11321,10 @@
         <v>2</v>
       </c>
       <c r="D127" s="6" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E127" s="30" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="F127" s="33" t="s">
         <v>288</v>
@@ -11396,10 +11395,10 @@
         <v>2</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E128" s="32" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="F128" s="33" t="s">
         <v>292</v>
@@ -11476,15 +11475,15 @@
         <v>3</v>
       </c>
       <c r="E129" s="32" t="s">
+        <v>701</v>
+      </c>
+      <c r="F129" s="33" t="s">
         <v>702</v>
-      </c>
-      <c r="F129" s="33" t="s">
-        <v>703</v>
       </c>
       <c r="G129" s="36"/>
       <c r="H129" s="37"/>
       <c r="I129" s="23" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="J129" s="7" t="s">
         <v>6</v>
@@ -11549,15 +11548,15 @@
         <v>3</v>
       </c>
       <c r="E130" s="32" t="s">
+        <v>703</v>
+      </c>
+      <c r="F130" s="33" t="s">
         <v>704</v>
-      </c>
-      <c r="F130" s="33" t="s">
-        <v>705</v>
       </c>
       <c r="G130" s="36"/>
       <c r="H130" s="37"/>
       <c r="I130" s="23" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="J130" s="7" t="s">
         <v>6</v>
@@ -11622,15 +11621,15 @@
         <v>3</v>
       </c>
       <c r="E131" s="32" t="s">
+        <v>705</v>
+      </c>
+      <c r="F131" s="33" t="s">
         <v>706</v>
-      </c>
-      <c r="F131" s="33" t="s">
-        <v>707</v>
       </c>
       <c r="G131" s="36"/>
       <c r="H131" s="37"/>
       <c r="I131" s="23" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="J131" s="7" t="s">
         <v>6</v>
@@ -11695,10 +11694,10 @@
         <v>3</v>
       </c>
       <c r="E132" s="32" t="s">
+        <v>707</v>
+      </c>
+      <c r="F132" s="33" t="s">
         <v>708</v>
-      </c>
-      <c r="F132" s="33" t="s">
-        <v>709</v>
       </c>
       <c r="G132" s="36"/>
       <c r="H132" s="37"/>
@@ -11768,10 +11767,10 @@
         <v>3</v>
       </c>
       <c r="E133" s="32" t="s">
+        <v>709</v>
+      </c>
+      <c r="F133" s="33" t="s">
         <v>710</v>
-      </c>
-      <c r="F133" s="33" t="s">
-        <v>711</v>
       </c>
       <c r="G133" s="36"/>
       <c r="H133" s="37"/>
@@ -11841,10 +11840,10 @@
         <v>3</v>
       </c>
       <c r="E134" s="32" t="s">
+        <v>711</v>
+      </c>
+      <c r="F134" s="33" t="s">
         <v>712</v>
-      </c>
-      <c r="F134" s="33" t="s">
-        <v>713</v>
       </c>
       <c r="G134" s="36"/>
       <c r="H134" s="37"/>
@@ -11914,10 +11913,10 @@
         <v>3</v>
       </c>
       <c r="E135" s="32" t="s">
+        <v>713</v>
+      </c>
+      <c r="F135" s="33" t="s">
         <v>714</v>
-      </c>
-      <c r="F135" s="33" t="s">
-        <v>715</v>
       </c>
       <c r="G135" s="36"/>
       <c r="H135" s="37"/>
@@ -11987,10 +11986,10 @@
         <v>3</v>
       </c>
       <c r="E136" s="32" t="s">
+        <v>715</v>
+      </c>
+      <c r="F136" s="33" t="s">
         <v>716</v>
-      </c>
-      <c r="F136" s="33" t="s">
-        <v>717</v>
       </c>
       <c r="G136" s="36"/>
       <c r="H136" s="37"/>
@@ -12099,7 +12098,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -12107,11 +12106,11 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="17.25" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="17.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="27.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="255.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="11.44140625" style="1"/>
+    <col min="1" max="1" width="27.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="255.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1">
@@ -12124,7 +12123,7 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
       <c r="A2" s="26" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>175</v>
@@ -12132,7 +12131,7 @@
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1">
       <c r="A3" s="26" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>177</v>
@@ -12140,7 +12139,7 @@
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1">
       <c r="A4" s="26" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>176</v>
@@ -12148,7 +12147,7 @@
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1">
       <c r="A5" s="26" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>178</v>
@@ -12156,15 +12155,15 @@
     </row>
     <row r="6" spans="1:2" ht="17.25" customHeight="1">
       <c r="A6" s="26" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>179</v>
@@ -12172,7 +12171,7 @@
     </row>
     <row r="8" spans="1:2" ht="17.25" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>180</v>
@@ -12180,7 +12179,7 @@
     </row>
     <row r="9" spans="1:2" ht="17.25" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>181</v>
@@ -12188,7 +12187,7 @@
     </row>
     <row r="10" spans="1:2" ht="17.25" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>182</v>
@@ -12196,7 +12195,7 @@
     </row>
     <row r="11" spans="1:2" ht="17.25" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>183</v>
@@ -12204,7 +12203,7 @@
     </row>
     <row r="12" spans="1:2" ht="17.25" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>184</v>
@@ -12212,7 +12211,7 @@
     </row>
     <row r="13" spans="1:2" ht="17.25" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>185</v>
@@ -12220,7 +12219,7 @@
     </row>
     <row r="14" spans="1:2" ht="17.25" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>186</v>
@@ -12228,7 +12227,7 @@
     </row>
     <row r="15" spans="1:2" ht="17.25" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>187</v>
@@ -12236,7 +12235,7 @@
     </row>
     <row r="16" spans="1:2" ht="17.25" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>188</v>
@@ -12244,42 +12243,42 @@
     </row>
     <row r="17" spans="1:2" ht="17.25" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="17.25" customHeight="1">
       <c r="A18" s="1" t="s">
+        <v>692</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>693</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>694</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="17.25" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="17.25" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="17.25" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="17.25" customHeight="1">

</xml_diff>

<commit_message>
Definición y forma de cálculo de indicadores de NNA-seguridad social
</commit_message>
<xml_diff>
--- a/Data/Base_fichas_indicadores.xlsx
+++ b/Data/Base_fichas_indicadores.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\DESCA-app\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shari\Dropbox\UMAD\DESCA\NUEVO REPOSITORIO\DESCA-app\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8B6CF7-94F4-4CCE-9B68-FBB4CEFC63D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BASE_FICHAS" sheetId="4" r:id="rId1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1976" uniqueCount="722">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1992" uniqueCount="738">
   <si>
     <t>id</t>
   </si>
@@ -2190,12 +2191,60 @@
   </si>
   <si>
     <t>Porcentaje de niños y niñas inmunizados según tipo de vacuna y dosis (estimación OMS - UNICEF)</t>
+  </si>
+  <si>
+    <t>El indicador mide la cantidad de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares en los que alguno de sus integrantes es beneficiario de Asignaciones Familiares contributivas.</t>
+  </si>
+  <si>
+    <t>Para cada año calcular: Cantidad de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares en los que alguno de sus integrantes es beneficiario de Asignaciones Familiares contributivas.</t>
+  </si>
+  <si>
+    <t>El indicador mide la cantidad de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares en los que alguno de sus integrantes es beneficiario de Asignaciones Familiares - Plan de Equidad.</t>
+  </si>
+  <si>
+    <t>Para cada año calcular: Cantidad de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares en los que alguno de sus integrantes es beneficiario de Asignaciones Familiares - Plan de Equidad</t>
+  </si>
+  <si>
+    <t>El indicador mide la cantidad de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares en los que alguno de sus integrantes es beneficiario de Tarjeta Uruguay Social.</t>
+  </si>
+  <si>
+    <t>Para cada año calcular: Cantidad de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares en los que alguno de sus integrantes es beneficiario de Tarjeta Uruguay Social</t>
+  </si>
+  <si>
+    <t>El indicador mide el porcentaje de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares en los que ningún integrante percibe Asignaciones Familaires - Plan de Equidad en el total de hogares pobres</t>
+  </si>
+  <si>
+    <t>Para cada año calcular: (Cantidad de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares en los que ninguno de sus integrantes es beneficiario de Asignaciones Familiares - Plan de Equidad/Cantidad de niños, niñas y adolescentes que residen en hogares pobres)*100</t>
+  </si>
+  <si>
+    <t>El indicador mide el porcentaje de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares en los que ningún integrante percibe Tarjeta Uruguay Social en el total de hogares pobres</t>
+  </si>
+  <si>
+    <t>Para cada año calcular: (Cantidad de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares en los que ninguno de sus integrantes es beneficiario de Tarjeta Uruguay Social/Cantidad de niños, niñas y adolescentes que residen en hogares pobres)*100</t>
+  </si>
+  <si>
+    <t>El indicador mide el porcentaje de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares en los que ningún integrante percibe Asignaciones Familaires - Plan de Equidad ni Tarjeta Uruguay Social en el total de hogares pobres</t>
+  </si>
+  <si>
+    <t>Para cada año calcular: (Cantidad de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares en los que ninguno de sus integrantes es beneficiario de Asignaciones Familiares - Plan de Equidad ni Tarjeta Uruguay Social/Cantidad de niños, niñas y adolescentes que residen en hogares pobres)*100</t>
+  </si>
+  <si>
+    <t>El indicador mide el porcentaje de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares cuyo jefe/a y/o cónyuge están desocupados sin seguro de desempleo</t>
+  </si>
+  <si>
+    <t>Para cada año calcular: (Cantidad de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares cuyo jefe/a y/o cónyuge están desocupados sin seguro de desempleo/Cantidad de niños, niñas y adolescentes)*100</t>
+  </si>
+  <si>
+    <t>El indicador mide el porcentaje de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares cuyo jefe/a y/o cónyuge están ocupados y no aportan a la seguridad social</t>
+  </si>
+  <si>
+    <t>Para cada año calcular: (Cantidad de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares cuyo jefe/a y/o cónyuge están ocupados y no aportan a la seguridad social/Cantidad de niños, niñas y adolescentes)*100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.000&quot;&quot;;\-#,##0.000&quot;&quot;"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -2276,18 +2325,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -2305,7 +2348,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2404,18 +2447,12 @@
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Excel Built-in Normal" xfId="3"/>
+    <cellStyle name="Excel Built-in Normal" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal_DISEÑO" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal_DISEÑO" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2726,42 +2763,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AI140"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="D1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="G1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E111" sqref="E111"/>
-      <selection pane="bottomLeft" activeCell="F91" sqref="F91"/>
+      <selection pane="bottomLeft" activeCell="G123" sqref="G123"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.1796875" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="13" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" style="13" customWidth="1"/>
-    <col min="4" max="4" width="37.7109375" style="13" customWidth="1"/>
-    <col min="5" max="5" width="94.7109375" style="13" customWidth="1"/>
-    <col min="6" max="6" width="157.28515625" style="13" customWidth="1"/>
-    <col min="7" max="7" width="255.7109375" style="13" customWidth="1"/>
-    <col min="8" max="8" width="181.140625" style="13" customWidth="1"/>
-    <col min="9" max="9" width="59.42578125" style="13" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" style="13" customWidth="1"/>
-    <col min="11" max="11" width="20.42578125" style="13" customWidth="1"/>
-    <col min="12" max="12" width="20.5703125" style="13" customWidth="1"/>
-    <col min="13" max="14" width="255.7109375" style="13" customWidth="1"/>
-    <col min="15" max="15" width="230.140625" style="13" customWidth="1"/>
-    <col min="16" max="16" width="98.7109375" style="13" customWidth="1"/>
-    <col min="17" max="17" width="19.140625" style="13" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.7265625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="37.7265625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="94.7265625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="157.26953125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="255.7265625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="181.1796875" style="13" customWidth="1"/>
+    <col min="9" max="9" width="59.453125" style="13" customWidth="1"/>
+    <col min="10" max="10" width="16.1796875" style="13" customWidth="1"/>
+    <col min="11" max="11" width="20.453125" style="13" customWidth="1"/>
+    <col min="12" max="12" width="20.54296875" style="13" customWidth="1"/>
+    <col min="13" max="14" width="255.7265625" style="13" customWidth="1"/>
+    <col min="15" max="15" width="230.1796875" style="13" customWidth="1"/>
+    <col min="16" max="16" width="98.7265625" style="13" customWidth="1"/>
+    <col min="17" max="17" width="19.1796875" style="13" customWidth="1"/>
+    <col min="18" max="18" width="12.7265625" style="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.81640625" style="13" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="22" max="26" width="9.42578125" style="13" customWidth="1"/>
-    <col min="27" max="29" width="9.140625" style="13"/>
-    <col min="30" max="30" width="55.140625" style="13" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="13"/>
+    <col min="21" max="21" width="15.54296875" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="26" width="9.453125" style="13" customWidth="1"/>
+    <col min="27" max="29" width="9.1796875" style="13"/>
+    <col min="30" max="30" width="55.1796875" style="13" customWidth="1"/>
+    <col min="31" max="16384" width="9.1796875" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -11480,8 +11517,12 @@
       <c r="F129" s="33" t="s">
         <v>702</v>
       </c>
-      <c r="G129" s="36"/>
-      <c r="H129" s="37"/>
+      <c r="G129" s="6" t="s">
+        <v>722</v>
+      </c>
+      <c r="H129" s="7" t="s">
+        <v>723</v>
+      </c>
       <c r="I129" s="23" t="s">
         <v>717</v>
       </c>
@@ -11553,8 +11594,12 @@
       <c r="F130" s="33" t="s">
         <v>704</v>
       </c>
-      <c r="G130" s="36"/>
-      <c r="H130" s="37"/>
+      <c r="G130" s="6" t="s">
+        <v>724</v>
+      </c>
+      <c r="H130" s="7" t="s">
+        <v>725</v>
+      </c>
       <c r="I130" s="23" t="s">
         <v>717</v>
       </c>
@@ -11626,8 +11671,12 @@
       <c r="F131" s="33" t="s">
         <v>706</v>
       </c>
-      <c r="G131" s="36"/>
-      <c r="H131" s="37"/>
+      <c r="G131" s="6" t="s">
+        <v>726</v>
+      </c>
+      <c r="H131" s="7" t="s">
+        <v>727</v>
+      </c>
       <c r="I131" s="23" t="s">
         <v>717</v>
       </c>
@@ -11699,8 +11748,12 @@
       <c r="F132" s="33" t="s">
         <v>708</v>
       </c>
-      <c r="G132" s="36"/>
-      <c r="H132" s="37"/>
+      <c r="G132" s="6" t="s">
+        <v>728</v>
+      </c>
+      <c r="H132" s="7" t="s">
+        <v>729</v>
+      </c>
       <c r="I132" s="23" t="s">
         <v>5</v>
       </c>
@@ -11772,8 +11825,12 @@
       <c r="F133" s="33" t="s">
         <v>710</v>
       </c>
-      <c r="G133" s="36"/>
-      <c r="H133" s="37"/>
+      <c r="G133" s="6" t="s">
+        <v>730</v>
+      </c>
+      <c r="H133" s="7" t="s">
+        <v>731</v>
+      </c>
       <c r="I133" s="23" t="s">
         <v>5</v>
       </c>
@@ -11845,8 +11902,12 @@
       <c r="F134" s="33" t="s">
         <v>712</v>
       </c>
-      <c r="G134" s="36"/>
-      <c r="H134" s="37"/>
+      <c r="G134" s="6" t="s">
+        <v>732</v>
+      </c>
+      <c r="H134" s="7" t="s">
+        <v>733</v>
+      </c>
       <c r="I134" s="23" t="s">
         <v>5</v>
       </c>
@@ -11918,8 +11979,12 @@
       <c r="F135" s="33" t="s">
         <v>714</v>
       </c>
-      <c r="G135" s="36"/>
-      <c r="H135" s="37"/>
+      <c r="G135" s="6" t="s">
+        <v>734</v>
+      </c>
+      <c r="H135" s="7" t="s">
+        <v>735</v>
+      </c>
       <c r="I135" s="23" t="s">
         <v>5</v>
       </c>
@@ -11991,8 +12056,12 @@
       <c r="F136" s="33" t="s">
         <v>716</v>
       </c>
-      <c r="G136" s="36"/>
-      <c r="H136" s="37"/>
+      <c r="G136" s="6" t="s">
+        <v>736</v>
+      </c>
+      <c r="H136" s="7" t="s">
+        <v>737</v>
+      </c>
       <c r="I136" s="23" t="s">
         <v>5</v>
       </c>
@@ -12098,7 +12167,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -12106,11 +12175,11 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="17.25" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="17.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="255.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="27.54296875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="255.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1">

</xml_diff>

<commit_message>
Act base mirador, fichas, gráficas y tablas.
</commit_message>
<xml_diff>
--- a/Data/Base_fichas_indicadores.xlsx
+++ b/Data/Base_fichas_indicadores.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Trabajo\DESCA\DESCA-app\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\DESCA-app\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F55FF2A-303C-4F74-8723-C06AE9E5BCE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="BASE_FICHAS" sheetId="4" r:id="rId1"/>
@@ -2196,7 +2195,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.000&quot;&quot;;\-#,##0.000&quot;&quot;"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -2413,10 +2412,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Excel Built-in Normal" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Excel Built-in Normal" xfId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Normal_DISEÑO" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Normal 2" xfId="2"/>
+    <cellStyle name="Normal_DISEÑO" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2727,42 +2726,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Hoja1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja1" filterMode="1"/>
   <dimension ref="A1:AI140"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="P1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E111" sqref="E111"/>
-      <selection pane="bottomLeft" activeCell="Q36" sqref="Q36"/>
+      <selection pane="bottomLeft" activeCell="U66" sqref="U66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="13" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" style="13" customWidth="1"/>
-    <col min="4" max="4" width="37.6640625" style="13" customWidth="1"/>
-    <col min="5" max="5" width="94.6640625" style="13" customWidth="1"/>
-    <col min="6" max="6" width="157.33203125" style="13" customWidth="1"/>
-    <col min="7" max="7" width="255.6640625" style="13" customWidth="1"/>
-    <col min="8" max="8" width="181.109375" style="13" customWidth="1"/>
-    <col min="9" max="9" width="59.44140625" style="13" customWidth="1"/>
-    <col min="10" max="10" width="16.109375" style="13" customWidth="1"/>
-    <col min="11" max="11" width="20.44140625" style="13" customWidth="1"/>
-    <col min="12" max="12" width="20.5546875" style="13" customWidth="1"/>
-    <col min="13" max="14" width="255.6640625" style="13" customWidth="1"/>
-    <col min="15" max="15" width="230.109375" style="13" customWidth="1"/>
-    <col min="16" max="16" width="98.6640625" style="13" customWidth="1"/>
-    <col min="17" max="17" width="19.109375" style="13" customWidth="1"/>
-    <col min="18" max="18" width="12.6640625" style="13" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" style="13" customWidth="1"/>
+    <col min="4" max="4" width="37.7109375" style="13" customWidth="1"/>
+    <col min="5" max="5" width="94.7109375" style="13" customWidth="1"/>
+    <col min="6" max="6" width="157.28515625" style="13" customWidth="1"/>
+    <col min="7" max="7" width="255.7109375" style="13" customWidth="1"/>
+    <col min="8" max="8" width="181.140625" style="13" customWidth="1"/>
+    <col min="9" max="9" width="59.42578125" style="13" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" style="13" customWidth="1"/>
+    <col min="11" max="11" width="20.42578125" style="13" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" style="13" customWidth="1"/>
+    <col min="13" max="14" width="255.7109375" style="13" customWidth="1"/>
+    <col min="15" max="15" width="230.140625" style="13" customWidth="1"/>
+    <col min="16" max="16" width="98.7109375" style="13" customWidth="1"/>
+    <col min="17" max="17" width="19.140625" style="13" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.85546875" style="13" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.5546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="22" max="26" width="9.44140625" style="13" customWidth="1"/>
-    <col min="27" max="29" width="9.109375" style="13"/>
-    <col min="30" max="30" width="55.109375" style="13" customWidth="1"/>
-    <col min="31" max="16384" width="9.109375" style="13"/>
+    <col min="21" max="21" width="15.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="26" width="9.42578125" style="13" customWidth="1"/>
+    <col min="27" max="29" width="9.140625" style="13"/>
+    <col min="30" max="30" width="55.140625" style="13" customWidth="1"/>
+    <col min="31" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -2830,7 +2829,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="6" customFormat="1">
+    <row r="2" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A2" s="6">
         <v>120101</v>
       </c>
@@ -2892,7 +2891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="6" customFormat="1">
+    <row r="3" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A3" s="6">
         <v>120102</v>
       </c>
@@ -2954,7 +2953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="6" customFormat="1">
+    <row r="4" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A4" s="6">
         <v>120103</v>
       </c>
@@ -3016,7 +3015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="6" customFormat="1">
+    <row r="5" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A5" s="6">
         <v>120104</v>
       </c>
@@ -3078,7 +3077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21" s="6" customFormat="1">
+    <row r="6" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A6" s="6">
         <v>120105</v>
       </c>
@@ -3140,7 +3139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="6" customFormat="1">
+    <row r="7" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A7" s="6">
         <v>120106</v>
       </c>
@@ -3202,7 +3201,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="6" customFormat="1">
+    <row r="8" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A8" s="6">
         <v>120107</v>
       </c>
@@ -3264,7 +3263,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="6" customFormat="1">
+    <row r="9" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A9" s="6">
         <v>120108</v>
       </c>
@@ -3326,7 +3325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="6" customFormat="1">
+    <row r="10" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A10" s="6">
         <v>120109</v>
       </c>
@@ -3388,7 +3387,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="6" customFormat="1">
+    <row r="11" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A11" s="6">
         <v>120110</v>
       </c>
@@ -3450,7 +3449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:21" s="6" customFormat="1">
+    <row r="12" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A12" s="6">
         <v>120111</v>
       </c>
@@ -3512,7 +3511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:21" s="6" customFormat="1">
+    <row r="13" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A13" s="6">
         <v>120112</v>
       </c>
@@ -3574,7 +3573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="6" customFormat="1">
+    <row r="14" spans="1:21" s="6" customFormat="1" hidden="1">
       <c r="A14" s="6">
         <v>120113</v>
       </c>
@@ -3636,7 +3635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:21" s="7" customFormat="1">
+    <row r="15" spans="1:21" s="7" customFormat="1" hidden="1">
       <c r="A15" s="6">
         <v>120114</v>
       </c>
@@ -3698,7 +3697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:21" s="7" customFormat="1">
+    <row r="16" spans="1:21" s="7" customFormat="1" hidden="1">
       <c r="A16" s="6">
         <v>120115</v>
       </c>
@@ -3760,7 +3759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:35" s="7" customFormat="1">
+    <row r="17" spans="1:35" s="7" customFormat="1" hidden="1">
       <c r="A17" s="6">
         <v>120116</v>
       </c>
@@ -3822,7 +3821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:35">
+    <row r="18" spans="1:35" hidden="1">
       <c r="A18" s="13">
         <v>130101</v>
       </c>
@@ -3878,16 +3877,16 @@
         <v>1</v>
       </c>
       <c r="S18" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T18" s="6">
         <v>1</v>
       </c>
       <c r="U18" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:35" hidden="1">
       <c r="A19" s="13">
         <v>130102</v>
       </c>
@@ -3952,7 +3951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:35">
+    <row r="20" spans="1:35" hidden="1">
       <c r="A20" s="13">
         <v>130103</v>
       </c>
@@ -4017,7 +4016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:35" s="6" customFormat="1">
+    <row r="21" spans="1:35" s="6" customFormat="1" hidden="1">
       <c r="A21" s="14">
         <v>130104</v>
       </c>
@@ -4096,7 +4095,7 @@
       <c r="AH21" s="13"/>
       <c r="AI21" s="13"/>
     </row>
-    <row r="22" spans="1:35" s="6" customFormat="1">
+    <row r="22" spans="1:35" s="6" customFormat="1" hidden="1">
       <c r="A22" s="14">
         <v>130105</v>
       </c>
@@ -4175,7 +4174,7 @@
       <c r="AH22" s="13"/>
       <c r="AI22" s="13"/>
     </row>
-    <row r="23" spans="1:35">
+    <row r="23" spans="1:35" hidden="1">
       <c r="A23" s="14">
         <v>130106</v>
       </c>
@@ -4240,7 +4239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:35">
+    <row r="24" spans="1:35" hidden="1">
       <c r="A24" s="15">
         <v>130107</v>
       </c>
@@ -4319,7 +4318,7 @@
       <c r="AH24" s="15"/>
       <c r="AI24" s="15"/>
     </row>
-    <row r="25" spans="1:35">
+    <row r="25" spans="1:35" hidden="1">
       <c r="A25" s="15">
         <v>130108</v>
       </c>
@@ -4398,7 +4397,7 @@
       <c r="AH25" s="15"/>
       <c r="AI25" s="15"/>
     </row>
-    <row r="26" spans="1:35" s="6" customFormat="1">
+    <row r="26" spans="1:35" s="6" customFormat="1" hidden="1">
       <c r="A26" s="6">
         <v>130201</v>
       </c>
@@ -4463,7 +4462,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:35">
+    <row r="27" spans="1:35" hidden="1">
       <c r="A27" s="6">
         <v>130202</v>
       </c>
@@ -4542,7 +4541,7 @@
       <c r="AH27" s="6"/>
       <c r="AI27" s="6"/>
     </row>
-    <row r="28" spans="1:35">
+    <row r="28" spans="1:35" hidden="1">
       <c r="A28" s="6">
         <v>130203</v>
       </c>
@@ -4621,7 +4620,7 @@
       <c r="AH28" s="6"/>
       <c r="AI28" s="6"/>
     </row>
-    <row r="29" spans="1:35">
+    <row r="29" spans="1:35" hidden="1">
       <c r="A29" s="6">
         <v>130204</v>
       </c>
@@ -4686,7 +4685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:35" s="15" customFormat="1">
+    <row r="30" spans="1:35" s="15" customFormat="1" hidden="1">
       <c r="A30" s="6">
         <v>130205</v>
       </c>
@@ -4765,7 +4764,7 @@
       <c r="AH30" s="13"/>
       <c r="AI30" s="13"/>
     </row>
-    <row r="31" spans="1:35" s="15" customFormat="1">
+    <row r="31" spans="1:35" s="15" customFormat="1" hidden="1">
       <c r="A31" s="6">
         <v>130301</v>
       </c>
@@ -4842,7 +4841,7 @@
       <c r="AH31" s="13"/>
       <c r="AI31" s="13"/>
     </row>
-    <row r="32" spans="1:35" s="6" customFormat="1">
+    <row r="32" spans="1:35" s="6" customFormat="1" hidden="1">
       <c r="A32" s="6">
         <v>130302</v>
       </c>
@@ -4919,7 +4918,7 @@
       <c r="AH32" s="13"/>
       <c r="AI32" s="13"/>
     </row>
-    <row r="33" spans="1:35">
+    <row r="33" spans="1:35" hidden="1">
       <c r="A33" s="6">
         <v>130303</v>
       </c>
@@ -4982,7 +4981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:35">
+    <row r="34" spans="1:35" hidden="1">
       <c r="A34" s="6">
         <v>130304</v>
       </c>
@@ -5061,7 +5060,7 @@
       <c r="AH34" s="6"/>
       <c r="AI34" s="6"/>
     </row>
-    <row r="35" spans="1:35" s="6" customFormat="1">
+    <row r="35" spans="1:35" s="6" customFormat="1" hidden="1">
       <c r="A35" s="6">
         <v>130305</v>
       </c>
@@ -5126,7 +5125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:35">
+    <row r="36" spans="1:35" hidden="1">
       <c r="A36" s="6">
         <v>130306</v>
       </c>
@@ -5179,7 +5178,7 @@
         <v>0</v>
       </c>
       <c r="R36" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S36" s="6">
         <v>0</v>
@@ -5188,10 +5187,10 @@
         <v>0</v>
       </c>
       <c r="U36" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:35" s="6" customFormat="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:35" s="6" customFormat="1" hidden="1">
       <c r="A37" s="6">
         <v>220101</v>
       </c>
@@ -5253,7 +5252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:35" s="6" customFormat="1">
+    <row r="38" spans="1:35" s="6" customFormat="1" hidden="1">
       <c r="A38" s="6">
         <v>220102</v>
       </c>
@@ -5315,7 +5314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:35" s="6" customFormat="1">
+    <row r="39" spans="1:35" s="6" customFormat="1" hidden="1">
       <c r="A39" s="6">
         <v>220103</v>
       </c>
@@ -5377,7 +5376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:35" s="6" customFormat="1">
+    <row r="40" spans="1:35" s="6" customFormat="1" hidden="1">
       <c r="A40" s="6">
         <v>220104</v>
       </c>
@@ -5439,7 +5438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:35">
+    <row r="41" spans="1:35" hidden="1">
       <c r="A41" s="6">
         <v>220105</v>
       </c>
@@ -5516,7 +5515,7 @@
       <c r="AH41" s="6"/>
       <c r="AI41" s="6"/>
     </row>
-    <row r="42" spans="1:35">
+    <row r="42" spans="1:35" hidden="1">
       <c r="A42" s="6">
         <v>220106</v>
       </c>
@@ -5593,7 +5592,7 @@
       <c r="AH42" s="25"/>
       <c r="AI42" s="25"/>
     </row>
-    <row r="43" spans="1:35">
+    <row r="43" spans="1:35" hidden="1">
       <c r="A43" s="6">
         <v>220107</v>
       </c>
@@ -5670,7 +5669,7 @@
       <c r="AH43" s="25"/>
       <c r="AI43" s="25"/>
     </row>
-    <row r="44" spans="1:35" s="6" customFormat="1">
+    <row r="44" spans="1:35" s="6" customFormat="1" hidden="1">
       <c r="A44" s="17">
         <v>230101</v>
       </c>
@@ -5749,7 +5748,7 @@
       <c r="AH44" s="13"/>
       <c r="AI44" s="13"/>
     </row>
-    <row r="45" spans="1:35" s="6" customFormat="1" ht="16.5" customHeight="1">
+    <row r="45" spans="1:35" s="6" customFormat="1" ht="16.5" hidden="1" customHeight="1">
       <c r="A45" s="17">
         <v>230201</v>
       </c>
@@ -5828,7 +5827,7 @@
       <c r="AH45" s="13"/>
       <c r="AI45" s="13"/>
     </row>
-    <row r="46" spans="1:35" s="6" customFormat="1">
+    <row r="46" spans="1:35" s="6" customFormat="1" hidden="1">
       <c r="A46" s="17">
         <v>230202</v>
       </c>
@@ -5907,7 +5906,7 @@
       <c r="AH46" s="13"/>
       <c r="AI46" s="13"/>
     </row>
-    <row r="47" spans="1:35" s="6" customFormat="1">
+    <row r="47" spans="1:35" s="6" customFormat="1" hidden="1">
       <c r="A47" s="10">
         <v>230203</v>
       </c>
@@ -5972,7 +5971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:35" s="6" customFormat="1">
+    <row r="48" spans="1:35" s="6" customFormat="1" hidden="1">
       <c r="A48" s="10">
         <v>230204</v>
       </c>
@@ -6037,7 +6036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:35" s="6" customFormat="1">
+    <row r="49" spans="1:35" s="6" customFormat="1" hidden="1">
       <c r="A49" s="6">
         <v>230301</v>
       </c>
@@ -6087,13 +6086,13 @@
         <v>513</v>
       </c>
       <c r="Q49" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R49" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S49" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T49" s="6">
         <v>0</v>
@@ -6102,7 +6101,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:35">
+    <row r="50" spans="1:35" hidden="1">
       <c r="A50" s="6">
         <v>230302</v>
       </c>
@@ -6181,7 +6180,7 @@
       <c r="AH50" s="6"/>
       <c r="AI50" s="6"/>
     </row>
-    <row r="51" spans="1:35">
+    <row r="51" spans="1:35" hidden="1">
       <c r="A51" s="6">
         <v>230303</v>
       </c>
@@ -6260,7 +6259,7 @@
       <c r="AH51" s="6"/>
       <c r="AI51" s="6"/>
     </row>
-    <row r="52" spans="1:35">
+    <row r="52" spans="1:35" hidden="1">
       <c r="A52" s="6">
         <v>230304</v>
       </c>
@@ -6339,7 +6338,7 @@
       <c r="AH52" s="6"/>
       <c r="AI52" s="6"/>
     </row>
-    <row r="53" spans="1:35">
+    <row r="53" spans="1:35" hidden="1">
       <c r="A53" s="6">
         <v>230401</v>
       </c>
@@ -6418,7 +6417,7 @@
       <c r="AH53" s="6"/>
       <c r="AI53" s="6"/>
     </row>
-    <row r="54" spans="1:35" s="6" customFormat="1">
+    <row r="54" spans="1:35" s="6" customFormat="1" hidden="1">
       <c r="A54" s="17">
         <v>230402</v>
       </c>
@@ -6497,7 +6496,7 @@
       <c r="AH54" s="13"/>
       <c r="AI54" s="13"/>
     </row>
-    <row r="55" spans="1:35" s="6" customFormat="1">
+    <row r="55" spans="1:35" s="6" customFormat="1" hidden="1">
       <c r="A55" s="17">
         <v>230501</v>
       </c>
@@ -6574,7 +6573,7 @@
       <c r="AH55" s="13"/>
       <c r="AI55" s="13"/>
     </row>
-    <row r="56" spans="1:35" s="6" customFormat="1">
+    <row r="56" spans="1:35" s="6" customFormat="1" hidden="1">
       <c r="A56" s="6">
         <v>320101</v>
       </c>
@@ -6636,7 +6635,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:35" s="6" customFormat="1">
+    <row r="57" spans="1:35" s="6" customFormat="1" hidden="1">
       <c r="A57" s="6">
         <v>320102</v>
       </c>
@@ -6698,7 +6697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:35" s="6" customFormat="1">
+    <row r="58" spans="1:35" s="6" customFormat="1" hidden="1">
       <c r="A58" s="6">
         <v>320103</v>
       </c>
@@ -6760,7 +6759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:35" s="6" customFormat="1">
+    <row r="59" spans="1:35" s="6" customFormat="1" hidden="1">
       <c r="A59" s="6">
         <v>320104</v>
       </c>
@@ -6822,7 +6821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:35" s="6" customFormat="1">
+    <row r="60" spans="1:35" s="6" customFormat="1" hidden="1">
       <c r="A60" s="6">
         <v>320105</v>
       </c>
@@ -6884,7 +6883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:35" s="6" customFormat="1">
+    <row r="61" spans="1:35" s="6" customFormat="1" hidden="1">
       <c r="A61" s="6">
         <v>320106</v>
       </c>
@@ -6946,7 +6945,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:35" s="6" customFormat="1">
+    <row r="62" spans="1:35" s="6" customFormat="1" hidden="1">
       <c r="A62" s="6">
         <v>320107</v>
       </c>
@@ -7135,7 +7134,7 @@
         <v>0</v>
       </c>
       <c r="U64" s="6">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="1:21" s="6" customFormat="1">
@@ -7256,7 +7255,7 @@
         <v>1</v>
       </c>
       <c r="R66" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S66" s="6">
         <v>0</v>
@@ -7265,7 +7264,7 @@
         <v>0</v>
       </c>
       <c r="U66" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:21" s="6" customFormat="1">
@@ -8308,7 +8307,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:35" s="6" customFormat="1">
+    <row r="83" spans="1:35" s="6" customFormat="1" hidden="1">
       <c r="A83" s="6">
         <v>420101</v>
       </c>
@@ -8370,7 +8369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:35" s="7" customFormat="1">
+    <row r="84" spans="1:35" s="7" customFormat="1" hidden="1">
       <c r="A84" s="6">
         <v>420102</v>
       </c>
@@ -8447,7 +8446,7 @@
       <c r="AH84" s="6"/>
       <c r="AI84" s="6"/>
     </row>
-    <row r="85" spans="1:35" s="7" customFormat="1">
+    <row r="85" spans="1:35" s="7" customFormat="1" hidden="1">
       <c r="A85" s="6">
         <v>420103</v>
       </c>
@@ -8524,7 +8523,7 @@
       <c r="AH85" s="6"/>
       <c r="AI85" s="6"/>
     </row>
-    <row r="86" spans="1:35" s="6" customFormat="1">
+    <row r="86" spans="1:35" s="6" customFormat="1" hidden="1">
       <c r="A86" s="6">
         <v>420104</v>
       </c>
@@ -8586,7 +8585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:35" s="7" customFormat="1">
+    <row r="87" spans="1:35" s="7" customFormat="1" hidden="1">
       <c r="A87" s="6">
         <v>420105</v>
       </c>
@@ -8663,7 +8662,7 @@
       <c r="AH87" s="6"/>
       <c r="AI87" s="6"/>
     </row>
-    <row r="88" spans="1:35" s="6" customFormat="1">
+    <row r="88" spans="1:35" s="6" customFormat="1" hidden="1">
       <c r="A88" s="6">
         <v>420106</v>
       </c>
@@ -8725,7 +8724,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:35" s="6" customFormat="1">
+    <row r="89" spans="1:35" s="6" customFormat="1" hidden="1">
       <c r="A89" s="6">
         <v>420107</v>
       </c>
@@ -8802,7 +8801,7 @@
       <c r="AH89" s="7"/>
       <c r="AI89" s="7"/>
     </row>
-    <row r="90" spans="1:35" s="11" customFormat="1">
+    <row r="90" spans="1:35" s="11" customFormat="1" hidden="1">
       <c r="A90" s="6">
         <v>420108</v>
       </c>
@@ -8879,7 +8878,7 @@
       <c r="AH90" s="7"/>
       <c r="AI90" s="7"/>
     </row>
-    <row r="91" spans="1:35" s="11" customFormat="1">
+    <row r="91" spans="1:35" s="11" customFormat="1" hidden="1">
       <c r="A91" s="6">
         <v>420109</v>
       </c>
@@ -8956,7 +8955,7 @@
       <c r="AH91" s="7"/>
       <c r="AI91" s="7"/>
     </row>
-    <row r="92" spans="1:35" s="7" customFormat="1">
+    <row r="92" spans="1:35" s="7" customFormat="1" hidden="1">
       <c r="A92" s="6">
         <v>430101</v>
       </c>
@@ -9033,7 +9032,7 @@
       <c r="AH92" s="6"/>
       <c r="AI92" s="6"/>
     </row>
-    <row r="93" spans="1:35" s="11" customFormat="1">
+    <row r="93" spans="1:35" s="11" customFormat="1" hidden="1">
       <c r="A93" s="6">
         <v>430102</v>
       </c>
@@ -9110,7 +9109,7 @@
       <c r="AH93" s="6"/>
       <c r="AI93" s="6"/>
     </row>
-    <row r="94" spans="1:35" s="6" customFormat="1">
+    <row r="94" spans="1:35" s="6" customFormat="1" hidden="1">
       <c r="A94" s="6">
         <v>430103</v>
       </c>
@@ -9187,7 +9186,7 @@
       <c r="AH94" s="11"/>
       <c r="AI94" s="11"/>
     </row>
-    <row r="95" spans="1:35" s="11" customFormat="1">
+    <row r="95" spans="1:35" s="11" customFormat="1" hidden="1">
       <c r="A95" s="6">
         <v>430104</v>
       </c>
@@ -9237,7 +9236,7 @@
         <v>1</v>
       </c>
       <c r="R95" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S95" s="6">
         <v>0</v>
@@ -9249,7 +9248,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:35" s="11" customFormat="1">
+    <row r="96" spans="1:35" s="11" customFormat="1" hidden="1">
       <c r="A96" s="6">
         <v>430105</v>
       </c>
@@ -9311,7 +9310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:35" s="11" customFormat="1">
+    <row r="97" spans="1:35" s="11" customFormat="1" hidden="1">
       <c r="A97" s="6">
         <v>430106</v>
       </c>
@@ -9373,7 +9372,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:35" s="11" customFormat="1">
+    <row r="98" spans="1:35" s="11" customFormat="1" hidden="1">
       <c r="A98" s="6">
         <v>430107</v>
       </c>
@@ -9435,7 +9434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:35" s="11" customFormat="1">
+    <row r="99" spans="1:35" s="11" customFormat="1" hidden="1">
       <c r="A99" s="6">
         <v>430108</v>
       </c>
@@ -9485,7 +9484,7 @@
         <v>0</v>
       </c>
       <c r="R99" s="6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S99" s="6">
         <v>0</v>
@@ -9497,7 +9496,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:35" s="11" customFormat="1">
+    <row r="100" spans="1:35" s="11" customFormat="1" hidden="1">
       <c r="A100" s="6">
         <v>430109</v>
       </c>
@@ -9559,7 +9558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:35" s="11" customFormat="1">
+    <row r="101" spans="1:35" s="11" customFormat="1" hidden="1">
       <c r="A101" s="6">
         <v>430110</v>
       </c>
@@ -9621,7 +9620,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:35" s="11" customFormat="1">
+    <row r="102" spans="1:35" s="11" customFormat="1" hidden="1">
       <c r="A102" s="6">
         <v>430111</v>
       </c>
@@ -9683,7 +9682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:35" s="7" customFormat="1">
+    <row r="103" spans="1:35" s="7" customFormat="1" hidden="1">
       <c r="A103" s="6">
         <v>430112</v>
       </c>
@@ -9760,7 +9759,7 @@
       <c r="AH103" s="11"/>
       <c r="AI103" s="11"/>
     </row>
-    <row r="104" spans="1:35" s="7" customFormat="1">
+    <row r="104" spans="1:35" s="7" customFormat="1" hidden="1">
       <c r="A104" s="6">
         <v>430113</v>
       </c>
@@ -9837,7 +9836,7 @@
       <c r="AH104" s="11"/>
       <c r="AI104" s="11"/>
     </row>
-    <row r="105" spans="1:35" s="7" customFormat="1">
+    <row r="105" spans="1:35" s="7" customFormat="1" hidden="1">
       <c r="A105" s="6">
         <v>430114</v>
       </c>
@@ -9914,7 +9913,7 @@
       <c r="AH105" s="11"/>
       <c r="AI105" s="11"/>
     </row>
-    <row r="106" spans="1:35" s="7" customFormat="1">
+    <row r="106" spans="1:35" s="7" customFormat="1" hidden="1">
       <c r="A106" s="6">
         <v>430201</v>
       </c>
@@ -9976,7 +9975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:35" s="7" customFormat="1">
+    <row r="107" spans="1:35" s="7" customFormat="1" hidden="1">
       <c r="A107" s="6">
         <v>430202</v>
       </c>
@@ -10038,7 +10037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:35" s="7" customFormat="1">
+    <row r="108" spans="1:35" s="7" customFormat="1" hidden="1">
       <c r="A108" s="6">
         <v>430203</v>
       </c>
@@ -10100,7 +10099,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:35" s="23" customFormat="1">
+    <row r="109" spans="1:35" s="23" customFormat="1" hidden="1">
       <c r="A109" s="6">
         <v>430204</v>
       </c>
@@ -10177,7 +10176,7 @@
       <c r="AH109" s="7"/>
       <c r="AI109" s="7"/>
     </row>
-    <row r="110" spans="1:35" s="7" customFormat="1">
+    <row r="110" spans="1:35" s="7" customFormat="1" hidden="1">
       <c r="A110" s="6">
         <v>430205</v>
       </c>
@@ -10239,7 +10238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:35" s="23" customFormat="1">
+    <row r="111" spans="1:35" s="23" customFormat="1" hidden="1">
       <c r="A111" s="6">
         <v>430206</v>
       </c>
@@ -10316,7 +10315,7 @@
       <c r="AH111" s="7"/>
       <c r="AI111" s="7"/>
     </row>
-    <row r="112" spans="1:35" s="7" customFormat="1">
+    <row r="112" spans="1:35" s="7" customFormat="1" hidden="1">
       <c r="A112" s="6">
         <v>430207</v>
       </c>
@@ -10378,7 +10377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:35" s="7" customFormat="1">
+    <row r="113" spans="1:35" s="7" customFormat="1" hidden="1">
       <c r="A113" s="6">
         <v>430208</v>
       </c>
@@ -10440,7 +10439,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:35" s="7" customFormat="1">
+    <row r="114" spans="1:35" s="7" customFormat="1" hidden="1">
       <c r="A114" s="6">
         <v>430209</v>
       </c>
@@ -10502,7 +10501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:35" s="7" customFormat="1">
+    <row r="115" spans="1:35" s="7" customFormat="1" hidden="1">
       <c r="A115" s="29">
         <v>430301</v>
       </c>
@@ -10564,7 +10563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:35" s="23" customFormat="1">
+    <row r="116" spans="1:35" s="23" customFormat="1" hidden="1">
       <c r="A116" s="29">
         <v>430302</v>
       </c>
@@ -10641,7 +10640,7 @@
       <c r="AH116" s="7"/>
       <c r="AI116" s="7"/>
     </row>
-    <row r="117" spans="1:35" s="25" customFormat="1">
+    <row r="117" spans="1:35" s="25" customFormat="1" hidden="1">
       <c r="A117" s="29">
         <v>430303</v>
       </c>
@@ -10718,7 +10717,7 @@
       <c r="AH117" s="11"/>
       <c r="AI117" s="11"/>
     </row>
-    <row r="118" spans="1:35" s="11" customFormat="1">
+    <row r="118" spans="1:35" s="11" customFormat="1" hidden="1">
       <c r="A118" s="29">
         <v>430304</v>
       </c>
@@ -10780,7 +10779,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:35" s="11" customFormat="1">
+    <row r="119" spans="1:35" s="11" customFormat="1" hidden="1">
       <c r="A119" s="29">
         <v>430305</v>
       </c>
@@ -10842,7 +10841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:35" s="11" customFormat="1">
+    <row r="120" spans="1:35" s="11" customFormat="1" hidden="1">
       <c r="A120" s="29">
         <v>430306</v>
       </c>
@@ -10904,7 +10903,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:35" s="23" customFormat="1">
+    <row r="121" spans="1:35" s="23" customFormat="1" hidden="1">
       <c r="A121" s="29">
         <v>430307</v>
       </c>
@@ -10981,7 +10980,7 @@
       <c r="AH121" s="7"/>
       <c r="AI121" s="7"/>
     </row>
-    <row r="122" spans="1:35" s="23" customFormat="1">
+    <row r="122" spans="1:35" s="23" customFormat="1" hidden="1">
       <c r="A122" s="7">
         <v>430401</v>
       </c>
@@ -11041,7 +11040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:35" s="23" customFormat="1">
+    <row r="123" spans="1:35" s="23" customFormat="1" hidden="1">
       <c r="A123" s="7">
         <v>430402</v>
       </c>
@@ -11101,7 +11100,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:35" s="23" customFormat="1">
+    <row r="124" spans="1:35" s="23" customFormat="1" hidden="1">
       <c r="A124" s="7">
         <v>430403</v>
       </c>
@@ -11161,7 +11160,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:35" s="11" customFormat="1">
+    <row r="125" spans="1:35" s="11" customFormat="1" hidden="1">
       <c r="A125" s="7">
         <v>430404</v>
       </c>
@@ -11236,7 +11235,7 @@
       <c r="AH125" s="23"/>
       <c r="AI125" s="23"/>
     </row>
-    <row r="126" spans="1:35" s="11" customFormat="1">
+    <row r="126" spans="1:35" s="11" customFormat="1" hidden="1">
       <c r="A126" s="7">
         <v>430405</v>
       </c>
@@ -11311,7 +11310,7 @@
       <c r="AH126" s="23"/>
       <c r="AI126" s="23"/>
     </row>
-    <row r="127" spans="1:35" s="7" customFormat="1">
+    <row r="127" spans="1:35" s="7" customFormat="1" hidden="1">
       <c r="A127" s="7">
         <v>430406</v>
       </c>
@@ -11385,7 +11384,7 @@
       <c r="AH127" s="23"/>
       <c r="AI127" s="23"/>
     </row>
-    <row r="128" spans="1:35">
+    <row r="128" spans="1:35" hidden="1">
       <c r="A128" s="7">
         <v>430407</v>
       </c>
@@ -12092,6 +12091,18 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <autoFilter ref="A1:AI136">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Seguridad Social"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="2">
+      <filters>
+        <filter val="Resultados"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -12099,7 +12110,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -12107,11 +12118,11 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="17.25" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="17.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="27.5546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="255.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="11.44140625" style="1"/>
+    <col min="1" max="1" width="27.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="255.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1">

</xml_diff>

<commit_message>
Act base Mirador y Base fichas. Elimino fichas técnicas viejas en html.
</commit_message>
<xml_diff>
--- a/Data/Base_fichas_indicadores.xlsx
+++ b/Data/Base_fichas_indicadores.xlsx
@@ -749,12 +749,6 @@
     <t>2014-2020</t>
   </si>
   <si>
-    <t>SINADI - MSP</t>
-  </si>
-  <si>
-    <t>UMAD con base en SINADI - MSP</t>
-  </si>
-  <si>
     <t>Promedio de camas de cuidados moderados</t>
   </si>
   <si>
@@ -1121,24 +1115,6 @@
     <t>DIMENSIÓN</t>
   </si>
   <si>
-    <t>El indicador mide el promedio anual de consultas urgentes y no urgentes, en consultorio y en domicilio, por usuario.</t>
-  </si>
-  <si>
-    <t>El indicador mide el promedio anual de consultas no urgentes, en consultorio y en domicilio, por usuario.</t>
-  </si>
-  <si>
-    <t>El indicador mide el promedio anual de consultas urgentes, en consultorio y en domicilio, por usuario.</t>
-  </si>
-  <si>
-    <t>El indicador mide el promedio anual de radiologías indicadas por usuario (en todas las modalidades de atención).</t>
-  </si>
-  <si>
-    <t>El indicador mide el promedio anual de recetas de medicamentos indicadas por usuario (en consultas urgentes, no urgentes e internación).</t>
-  </si>
-  <si>
-    <t>El indicador mide la razón de las consultas médicas no urgentes sobre las consultas médicas urgentes y busca reflejar el control periódico, la prevención y detección temprana de las afecciones de salud.</t>
-  </si>
-  <si>
     <t>El indicador del índice de satisfacción global con la institución de salud de los usuarios según tipo de institución prestadora de salud del SNIS se construye a partir de las respuestas obtenidas en la siguiente pregunta de la Encuesta de Satisfacción de PNA: Teniendo en cuenta todos los aspectos evaluados ¿Cuán satisfecho se encuentra con (Institución)?</t>
   </si>
   <si>
@@ -1325,15 +1301,6 @@
     <t>El indicador refleja la distribución porcentual de personas según institución prestadora en la cual tienen derecho vigente.</t>
   </si>
   <si>
-    <t>El indicador mide el promedio anual de cirugías por 1000 usuarios.</t>
-  </si>
-  <si>
-    <t>El indicador mide el promedio anual de cirugías coordinadas por 1000 usuarios.</t>
-  </si>
-  <si>
-    <t>El indicador mide el promedio anual de cirugías urgentes por 1000 usuarios.</t>
-  </si>
-  <si>
     <t>El indicador mide la cantidad anual de defunciones registradas en el año en relación a la población del país proyectada según censo 1996.</t>
   </si>
   <si>
@@ -1346,9 +1313,6 @@
     <t>El indicador de esperanza de vida al nacer representa la duración media de la vida de hombres y mujeres, que integran una cohorte hipotética de nacimientos, sometidos en todas las edades a los riesgos de mortalidad del período en estudio. .</t>
   </si>
   <si>
-    <t>El indicador mide el porcentaje partos registrados en el período anual considerado que requirieron la realización de cesárea.</t>
-  </si>
-  <si>
     <t>El indicador mide el ratio entre cantidad de estudiantes y docentes en la educación primaria privada.</t>
   </si>
   <si>
@@ -1415,12 +1379,6 @@
     <t>El indicador mide el porcentaje de cobertura de vacunación en nacidos vivos o niños y niñas (de acuerdo al esquema de vacunación). Las vacunas consideradas son: primera dosis contra tuberculosis (BCG); primera y tercera dosis contra difteria, tétanos y tosferina (DTP1 y DTP2); tercera dosis contra hepatitis B (HepB3); tercera dosis contra Haemophilus influenzae tipo b (Hib3); primera y tercera dosis contra poliomielitis (IPV1 y Pol3); primera y segunda dosis contra el sarampión (MCV1 y MCV2); tercera dosis antineumocócica (PcV3) y primera dosis contra la rubéola (RCV1).</t>
   </si>
   <si>
-    <t>El indicador mide el porcentaje de mujeres con partos registrados en el período anual considerado, cuyo embarazo fue captado en el primer trimestre.</t>
-  </si>
-  <si>
-    <t>El indicador mide el promedio anual de exámenes de laboratorio indicados por usuario (en consultas urgentes, no urgentes e internación).</t>
-  </si>
-  <si>
     <t>Para cada año calcular: Porcentaje de usuarios según tipo de institución prestadora de salud del SNIS que en la Encuesta de Satisfacción de PNA respondieron que son Muy fácil y Fácil a la pregunta: Los trámites y gestiones que debe realizar en su Institución para consultar médico de medicina general o especialista, ¿le resultan fáciles o difíciles?</t>
   </si>
   <si>
@@ -2190,6 +2148,48 @@
   </si>
   <si>
     <t>ASCENDENCIA_POB</t>
+  </si>
+  <si>
+    <t>SINADI - MSP (*2020 datos preliminares)</t>
+  </si>
+  <si>
+    <t>UMAD con base en SINADI - MSP (*2020 datos preliminares)</t>
+  </si>
+  <si>
+    <t>El indicador mide el promedio anual de consultas urgentes y no urgentes, en consultorio y en domicilio, por usuario. El Total SNIS es el promedio ponderado por cantidad de afiliados de cada tipo de prestador.</t>
+  </si>
+  <si>
+    <t>El indicador mide el promedio anual de consultas no urgentes, en consultorio y en domicilio, por usuario. El Total SNIS es el promedio ponderado por cantidad de afiliados de cada tipo de prestador.</t>
+  </si>
+  <si>
+    <t>El indicador mide el promedio anual de consultas urgentes, en consultorio y en domicilio, por usuario. El Total SNIS es el promedio ponderado por cantidad de afiliados de cada tipo de prestador.</t>
+  </si>
+  <si>
+    <t>El indicador mide el promedio anual de recetas de medicamentos indicadas por usuario (en consultas urgentes, no urgentes e internación). El Total SNIS es el promedio ponderado por cantidad de afiliados de cada tipo de prestador.</t>
+  </si>
+  <si>
+    <t>El indicador mide el promedio anual de exámenes de laboratorio indicados por usuario (en consultas urgentes, no urgentes e internación). El Total SNIS es el promedio ponderado por cantidad de afiliados de cada tipo de prestador.</t>
+  </si>
+  <si>
+    <t>El indicador mide el promedio anual de radiologías indicadas por usuario (en todas las modalidades de atención). El Total SNIS es el promedio ponderado por cantidad de afiliados de cada tipo de prestador.</t>
+  </si>
+  <si>
+    <t>El indicador mide el promedio anual de cirugías por 1000 usuarios. El Total SNIS es el promedio ponderado por cantidad de afiliados de cada tipo de prestador.</t>
+  </si>
+  <si>
+    <t>El indicador mide el promedio anual de cirugías coordinadas por 1000 usuarios. El Total SNIS es el promedio ponderado por cantidad de afiliados de cada tipo de prestador.</t>
+  </si>
+  <si>
+    <t>El indicador mide el promedio anual de cirugías urgentes por 1000 usuarios. El Total SNIS es el promedio ponderado por cantidad de afiliados de cada tipo de prestador.</t>
+  </si>
+  <si>
+    <t>El indicador mide la razón de las consultas médicas no urgentes sobre las consultas médicas urgentes y busca reflejar el control periódico, la prevención y detección temprana de las afecciones de salud. El Total SNIS es el promedio ponderado por cantidad de afiliados de cada tipo de prestador.</t>
+  </si>
+  <si>
+    <t>El indicador mide el porcentaje de mujeres con partos registrados en el período anual considerado, cuyo embarazo fue captado en el primer trimestre. El Total SNIS es el promedio ponderado por cantidad de afiliados de cada tipo de prestador.</t>
+  </si>
+  <si>
+    <t>El indicador mide el porcentaje partos registrados en el período anual considerado que requirieron la realización de cesárea. El Total SNIS es el promedio ponderado por cantidad de afiliados de cada tipo de prestador.</t>
   </si>
 </sst>
 </file>
@@ -2730,10 +2730,10 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AI140"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="J1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E111" sqref="E111"/>
-      <selection pane="bottomLeft" activeCell="U66" sqref="U66"/>
+      <selection pane="bottomLeft" activeCell="M99" sqref="M99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2766,67 +2766,67 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="26" t="s">
+        <v>347</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>348</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>349</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>350</v>
-      </c>
-      <c r="C1" s="26" t="s">
+      <c r="D1" s="26" t="s">
+        <v>362</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>517</v>
+      </c>
+      <c r="F1" s="26" t="s">
         <v>351</v>
       </c>
-      <c r="D1" s="26" t="s">
-        <v>364</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>531</v>
-      </c>
-      <c r="F1" s="26" t="s">
+      <c r="G1" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>360</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>361</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>363</v>
-      </c>
       <c r="Q1" s="26" t="s">
-        <v>688</v>
+        <v>674</v>
       </c>
       <c r="R1" s="13" t="s">
-        <v>693</v>
+        <v>679</v>
       </c>
       <c r="S1" s="35" t="s">
-        <v>719</v>
+        <v>705</v>
       </c>
       <c r="T1" s="35" t="s">
-        <v>720</v>
+        <v>706</v>
       </c>
       <c r="U1" s="35" t="s">
-        <v>721</v>
+        <v>707</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="6" customFormat="1">
@@ -2843,13 +2843,13 @@
         <v>104</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>532</v>
+        <v>518</v>
       </c>
       <c r="F2" s="31" t="s">
         <v>80</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>374</v>
+        <v>366</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>114</v>
@@ -2861,16 +2861,16 @@
         <v>6</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>691</v>
+        <v>677</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>689</v>
+        <v>675</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>692</v>
+        <v>678</v>
       </c>
       <c r="P2" s="6" t="s">
         <v>17</v>
@@ -2905,13 +2905,13 @@
         <v>104</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>533</v>
+        <v>519</v>
       </c>
       <c r="F3" s="31" t="s">
         <v>81</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>375</v>
+        <v>367</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>113</v>
@@ -2923,16 +2923,16 @@
         <v>6</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>690</v>
+        <v>676</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>689</v>
+        <v>675</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>692</v>
+        <v>678</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>17</v>
@@ -2967,13 +2967,13 @@
         <v>104</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>534</v>
+        <v>520</v>
       </c>
       <c r="F4" s="31" t="s">
         <v>82</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>376</v>
+        <v>368</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>116</v>
@@ -2985,16 +2985,16 @@
         <v>6</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>690</v>
+        <v>676</v>
       </c>
       <c r="L4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>689</v>
+        <v>675</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>692</v>
+        <v>678</v>
       </c>
       <c r="P4" s="6" t="s">
         <v>17</v>
@@ -3029,13 +3029,13 @@
         <v>104</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>535</v>
+        <v>521</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>76</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>446</v>
+        <v>434</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>112</v>
@@ -3053,10 +3053,10 @@
         <v>8</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>527</v>
+        <v>513</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>528</v>
+        <v>514</v>
       </c>
       <c r="P5" s="6" t="s">
         <v>17</v>
@@ -3091,16 +3091,16 @@
         <v>104</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>536</v>
+        <v>522</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>79</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>377</v>
+        <v>369</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>467</v>
+        <v>453</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>5</v>
@@ -3115,10 +3115,10 @@
         <v>8</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>525</v>
+        <v>511</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>526</v>
+        <v>512</v>
       </c>
       <c r="P6" s="6" t="s">
         <v>25</v>
@@ -3153,16 +3153,16 @@
         <v>104</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>537</v>
+        <v>523</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>78</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>378</v>
+        <v>370</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>445</v>
+        <v>433</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>5</v>
@@ -3177,10 +3177,10 @@
         <v>8</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>525</v>
+        <v>511</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>526</v>
+        <v>512</v>
       </c>
       <c r="P7" s="6" t="s">
         <v>25</v>
@@ -3215,13 +3215,13 @@
         <v>104</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>538</v>
+        <v>524</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>83</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>379</v>
+        <v>371</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>115</v>
@@ -3239,10 +3239,10 @@
         <v>8</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>525</v>
+        <v>511</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>526</v>
+        <v>512</v>
       </c>
       <c r="P8" s="6" t="s">
         <v>25</v>
@@ -3277,13 +3277,13 @@
         <v>104</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>539</v>
+        <v>525</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>84</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>30</v>
@@ -3301,10 +3301,10 @@
         <v>8</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>525</v>
+        <v>511</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>526</v>
+        <v>512</v>
       </c>
       <c r="P9" s="6" t="s">
         <v>85</v>
@@ -3339,13 +3339,13 @@
         <v>104</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>540</v>
+        <v>526</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>88</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>381</v>
+        <v>373</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>86</v>
@@ -3363,10 +3363,10 @@
         <v>8</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>525</v>
+        <v>511</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>526</v>
+        <v>512</v>
       </c>
       <c r="P10" s="6" t="s">
         <v>85</v>
@@ -3401,13 +3401,13 @@
         <v>104</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>541</v>
+        <v>527</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>89</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>382</v>
+        <v>374</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>90</v>
@@ -3425,10 +3425,10 @@
         <v>8</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>525</v>
+        <v>511</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>526</v>
+        <v>512</v>
       </c>
       <c r="P11" s="6" t="s">
         <v>85</v>
@@ -3463,16 +3463,16 @@
         <v>104</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>542</v>
+        <v>528</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>438</v>
+        <v>427</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>468</v>
+        <v>454</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>33</v>
@@ -3487,13 +3487,13 @@
         <v>8</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>525</v>
+        <v>511</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>526</v>
+        <v>512</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>520</v>
+        <v>506</v>
       </c>
       <c r="Q12" s="6">
         <v>0</v>
@@ -3525,16 +3525,16 @@
         <v>104</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>543</v>
+        <v>529</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>92</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>449</v>
+        <v>437</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="I13" s="6" t="s">
         <v>94</v>
@@ -3549,7 +3549,7 @@
         <v>8</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>521</v>
+        <v>507</v>
       </c>
       <c r="N13" s="6" t="s">
         <v>13</v>
@@ -3587,13 +3587,13 @@
         <v>104</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>544</v>
+        <v>530</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>97</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>383</v>
+        <v>375</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>28</v>
@@ -3608,13 +3608,13 @@
         <v>95</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>524</v>
+        <v>510</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>522</v>
+        <v>508</v>
       </c>
       <c r="P14" s="6" t="s">
         <v>96</v>
@@ -3643,22 +3643,22 @@
         <v>1</v>
       </c>
       <c r="C15" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="E15" s="30" t="s">
+        <v>531</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>307</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="E15" s="30" t="s">
-        <v>545</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>309</v>
-      </c>
       <c r="G15" s="6" t="s">
-        <v>450</v>
+        <v>438</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>469</v>
+        <v>455</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>5</v>
@@ -3667,7 +3667,7 @@
         <v>6</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="L15" s="7" t="s">
         <v>8</v>
@@ -3705,22 +3705,22 @@
         <v>1</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>546</v>
+        <v>532</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>451</v>
+        <v>439</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>470</v>
+        <v>456</v>
       </c>
       <c r="I16" s="7" t="s">
         <v>5</v>
@@ -3729,7 +3729,7 @@
         <v>6</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="L16" s="7" t="s">
         <v>8</v>
@@ -3767,22 +3767,22 @@
         <v>1</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>547</v>
+        <v>533</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>441</v>
+        <v>429</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>471</v>
+        <v>457</v>
       </c>
       <c r="I17" s="7" t="s">
         <v>5</v>
@@ -3791,7 +3791,7 @@
         <v>6</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="L17" s="7" t="s">
         <v>8</v>
@@ -3835,13 +3835,13 @@
         <v>3</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>548</v>
+        <v>534</v>
       </c>
       <c r="F18" s="13" t="s">
         <v>4</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>384</v>
+        <v>376</v>
       </c>
       <c r="H18" s="14" t="s">
         <v>139</v>
@@ -3868,7 +3868,7 @@
         <v>10</v>
       </c>
       <c r="P18" s="13" t="s">
-        <v>515</v>
+        <v>501</v>
       </c>
       <c r="Q18" s="6">
         <v>1</v>
@@ -3900,13 +3900,13 @@
         <v>3</v>
       </c>
       <c r="E19" s="30" t="s">
-        <v>549</v>
+        <v>535</v>
       </c>
       <c r="F19" s="13" t="s">
         <v>100</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>385</v>
+        <v>377</v>
       </c>
       <c r="H19" s="14" t="s">
         <v>140</v>
@@ -3933,7 +3933,7 @@
         <v>11</v>
       </c>
       <c r="P19" s="13" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="Q19" s="6">
         <v>1</v>
@@ -3965,13 +3965,13 @@
         <v>3</v>
       </c>
       <c r="E20" s="30" t="s">
-        <v>550</v>
+        <v>536</v>
       </c>
       <c r="F20" s="13" t="s">
         <v>102</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>386</v>
+        <v>378</v>
       </c>
       <c r="H20" s="14" t="s">
         <v>141</v>
@@ -3998,7 +3998,7 @@
         <v>11</v>
       </c>
       <c r="P20" s="13" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="Q20" s="6">
         <v>0</v>
@@ -4030,13 +4030,13 @@
         <v>3</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>551</v>
+        <v>537</v>
       </c>
       <c r="F21" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="H21" s="13" t="s">
         <v>148</v>
@@ -4063,7 +4063,7 @@
         <v>10</v>
       </c>
       <c r="P21" s="13" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="Q21" s="6">
         <v>0</v>
@@ -4109,13 +4109,13 @@
         <v>3</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>552</v>
+        <v>538</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>388</v>
+        <v>380</v>
       </c>
       <c r="H22" s="13" t="s">
         <v>149</v>
@@ -4142,7 +4142,7 @@
         <v>10</v>
       </c>
       <c r="P22" s="13" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="Q22" s="6">
         <v>0</v>
@@ -4188,13 +4188,13 @@
         <v>3</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>553</v>
+        <v>539</v>
       </c>
       <c r="F23" s="13" t="s">
         <v>20</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>389</v>
+        <v>381</v>
       </c>
       <c r="H23" s="13" t="s">
         <v>150</v>
@@ -4221,7 +4221,7 @@
         <v>10</v>
       </c>
       <c r="P23" s="13" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="Q23" s="6">
         <v>0</v>
@@ -4253,16 +4253,16 @@
         <v>3</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>554</v>
+        <v>540</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>390</v>
+        <v>382</v>
       </c>
       <c r="H24" s="15" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="I24" s="15" t="s">
         <v>5</v>
@@ -4286,7 +4286,7 @@
         <v>234</v>
       </c>
       <c r="P24" s="13" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="Q24" s="6">
         <v>0</v>
@@ -4332,13 +4332,13 @@
         <v>3</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>555</v>
+        <v>541</v>
       </c>
       <c r="F25" s="15" t="s">
         <v>236</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="H25" s="15" t="s">
         <v>235</v>
@@ -4365,7 +4365,7 @@
         <v>234</v>
       </c>
       <c r="P25" s="13" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="Q25" s="6">
         <v>1</v>
@@ -4411,13 +4411,13 @@
         <v>12</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>556</v>
+        <v>542</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>98</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="H26" s="6" t="s">
         <v>142</v>
@@ -4435,16 +4435,16 @@
         <v>8</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>521</v>
+        <v>507</v>
       </c>
       <c r="N26" s="6" t="s">
-        <v>523</v>
+        <v>509</v>
       </c>
       <c r="O26" s="6" t="s">
         <v>14</v>
       </c>
       <c r="P26" s="6" t="s">
-        <v>661</v>
+        <v>647</v>
       </c>
       <c r="Q26" s="6">
         <v>0</v>
@@ -4476,13 +4476,13 @@
         <v>12</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>557</v>
+        <v>543</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>73</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="H27" s="6" t="s">
         <v>143</v>
@@ -4500,16 +4500,16 @@
         <v>8</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>521</v>
+        <v>507</v>
       </c>
       <c r="N27" s="6" t="s">
-        <v>523</v>
+        <v>509</v>
       </c>
       <c r="O27" s="6" t="s">
         <v>14</v>
       </c>
       <c r="P27" s="6" t="s">
-        <v>661</v>
+        <v>647</v>
       </c>
       <c r="Q27" s="6">
         <v>0</v>
@@ -4555,13 +4555,13 @@
         <v>12</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>558</v>
+        <v>544</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>99</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>452</v>
+        <v>440</v>
       </c>
       <c r="H28" s="6" t="s">
         <v>151</v>
@@ -4579,16 +4579,16 @@
         <v>8</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>521</v>
+        <v>507</v>
       </c>
       <c r="N28" s="6" t="s">
-        <v>523</v>
+        <v>509</v>
       </c>
       <c r="O28" s="6" t="s">
         <v>14</v>
       </c>
       <c r="P28" s="6" t="s">
-        <v>518</v>
+        <v>504</v>
       </c>
       <c r="Q28" s="6">
         <v>0</v>
@@ -4634,16 +4634,16 @@
         <v>12</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>559</v>
+        <v>545</v>
       </c>
       <c r="F29" s="13" t="s">
         <v>101</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>394</v>
+        <v>386</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>372</v>
+        <v>364</v>
       </c>
       <c r="I29" s="13" t="s">
         <v>5</v>
@@ -4658,16 +4658,16 @@
         <v>8</v>
       </c>
       <c r="M29" s="13" t="s">
-        <v>525</v>
+        <v>511</v>
       </c>
       <c r="N29" s="13" t="s">
-        <v>526</v>
+        <v>512</v>
       </c>
       <c r="O29" s="13" t="s">
         <v>21</v>
       </c>
       <c r="P29" s="13" t="s">
-        <v>517</v>
+        <v>503</v>
       </c>
       <c r="Q29" s="6">
         <v>0</v>
@@ -4699,16 +4699,16 @@
         <v>12</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>560</v>
+        <v>546</v>
       </c>
       <c r="F30" s="13" t="s">
         <v>103</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>373</v>
+        <v>365</v>
       </c>
       <c r="I30" s="13" t="s">
         <v>5</v>
@@ -4723,16 +4723,16 @@
         <v>8</v>
       </c>
       <c r="M30" s="13" t="s">
-        <v>525</v>
+        <v>511</v>
       </c>
       <c r="N30" s="13" t="s">
-        <v>526</v>
+        <v>512</v>
       </c>
       <c r="O30" s="13" t="s">
         <v>21</v>
       </c>
       <c r="P30" s="13" t="s">
-        <v>517</v>
+        <v>503</v>
       </c>
       <c r="Q30" s="6">
         <v>0</v>
@@ -4778,13 +4778,13 @@
         <v>15</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>561</v>
+        <v>547</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>108</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="H31" s="13" t="s">
         <v>144</v>
@@ -4802,10 +4802,10 @@
         <v>16</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>521</v>
+        <v>507</v>
       </c>
       <c r="N31" s="6" t="s">
-        <v>523</v>
+        <v>509</v>
       </c>
       <c r="O31" s="16"/>
       <c r="P31" s="13" t="s">
@@ -4855,13 +4855,13 @@
         <v>15</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>562</v>
+        <v>548</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>109</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>397</v>
+        <v>389</v>
       </c>
       <c r="H32" s="13" t="s">
         <v>145</v>
@@ -4879,10 +4879,10 @@
         <v>16</v>
       </c>
       <c r="M32" s="6" t="s">
-        <v>521</v>
+        <v>507</v>
       </c>
       <c r="N32" s="6" t="s">
-        <v>523</v>
+        <v>509</v>
       </c>
       <c r="O32" s="16"/>
       <c r="P32" s="13" t="s">
@@ -4932,13 +4932,13 @@
         <v>15</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>563</v>
+        <v>549</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>107</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>453</v>
+        <v>441</v>
       </c>
       <c r="H33" s="13" t="s">
         <v>146</v>
@@ -4956,10 +4956,10 @@
         <v>16</v>
       </c>
       <c r="M33" s="6" t="s">
-        <v>521</v>
+        <v>507</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>523</v>
+        <v>509</v>
       </c>
       <c r="O33" s="16"/>
       <c r="P33" s="13" t="s">
@@ -4995,13 +4995,13 @@
         <v>15</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>564</v>
+        <v>550</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>110</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>519</v>
+        <v>505</v>
       </c>
       <c r="H34" s="13" t="s">
         <v>147</v>
@@ -5019,10 +5019,10 @@
         <v>16</v>
       </c>
       <c r="M34" s="6" t="s">
-        <v>521</v>
+        <v>507</v>
       </c>
       <c r="N34" s="6" t="s">
-        <v>523</v>
+        <v>509</v>
       </c>
       <c r="O34" s="6" t="s">
         <v>105</v>
@@ -5074,13 +5074,13 @@
         <v>15</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>565</v>
+        <v>551</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>22</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>454</v>
+        <v>442</v>
       </c>
       <c r="H35" s="6" t="s">
         <v>152</v>
@@ -5139,13 +5139,13 @@
         <v>3</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>566</v>
+        <v>552</v>
       </c>
       <c r="F36" s="13" t="s">
         <v>74</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>398</v>
+        <v>390</v>
       </c>
       <c r="H36" s="13" t="s">
         <v>153</v>
@@ -5172,7 +5172,7 @@
         <v>75</v>
       </c>
       <c r="P36" s="13" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="Q36" s="6">
         <v>0</v>
@@ -5204,13 +5204,13 @@
         <v>104</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>567</v>
+        <v>553</v>
       </c>
       <c r="F37" s="31" t="s">
         <v>118</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>399</v>
+        <v>391</v>
       </c>
       <c r="H37" s="6" t="s">
         <v>119</v>
@@ -5222,16 +5222,16 @@
         <v>6</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>691</v>
+        <v>677</v>
       </c>
       <c r="L37" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M37" s="6" t="s">
-        <v>689</v>
+        <v>675</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>692</v>
+        <v>678</v>
       </c>
       <c r="P37" s="6" t="s">
         <v>17</v>
@@ -5266,13 +5266,13 @@
         <v>104</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>568</v>
+        <v>554</v>
       </c>
       <c r="F38" s="31" t="s">
         <v>120</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>400</v>
+        <v>392</v>
       </c>
       <c r="H38" s="6" t="s">
         <v>121</v>
@@ -5290,10 +5290,10 @@
         <v>8</v>
       </c>
       <c r="M38" s="6" t="s">
-        <v>689</v>
+        <v>675</v>
       </c>
       <c r="N38" s="6" t="s">
-        <v>692</v>
+        <v>678</v>
       </c>
       <c r="P38" s="6" t="s">
         <v>17</v>
@@ -5328,16 +5328,16 @@
         <v>104</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>569</v>
+        <v>555</v>
       </c>
       <c r="F39" s="31" t="s">
         <v>122</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>401</v>
+        <v>393</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>444</v>
+        <v>432</v>
       </c>
       <c r="I39" s="6" t="s">
         <v>5</v>
@@ -5346,16 +5346,16 @@
         <v>6</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>690</v>
+        <v>676</v>
       </c>
       <c r="L39" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M39" s="6" t="s">
-        <v>689</v>
+        <v>675</v>
       </c>
       <c r="N39" s="6" t="s">
-        <v>692</v>
+        <v>678</v>
       </c>
       <c r="P39" s="6" t="s">
         <v>17</v>
@@ -5390,13 +5390,13 @@
         <v>104</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>570</v>
+        <v>556</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>123</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>687</v>
+        <v>673</v>
       </c>
       <c r="H40" s="6" t="s">
         <v>124</v>
@@ -5414,10 +5414,10 @@
         <v>8</v>
       </c>
       <c r="M40" s="6" t="s">
-        <v>527</v>
+        <v>513</v>
       </c>
       <c r="N40" s="6" t="s">
-        <v>528</v>
+        <v>514</v>
       </c>
       <c r="P40" s="6" t="s">
         <v>17</v>
@@ -5452,19 +5452,19 @@
         <v>104</v>
       </c>
       <c r="E41" s="30" t="s">
-        <v>571</v>
+        <v>557</v>
       </c>
       <c r="F41" s="24" t="s">
+        <v>320</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>443</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>321</v>
+      </c>
+      <c r="I41" s="6" t="s">
         <v>322</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>455</v>
-      </c>
-      <c r="H41" s="6" t="s">
-        <v>323</v>
-      </c>
-      <c r="I41" s="6" t="s">
-        <v>324</v>
       </c>
       <c r="J41" s="6" t="s">
         <v>6</v>
@@ -5476,14 +5476,14 @@
         <v>8</v>
       </c>
       <c r="M41" s="24" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="N41" s="6" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="O41" s="6"/>
       <c r="P41" s="6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="Q41" s="6">
         <v>0</v>
@@ -5529,38 +5529,38 @@
         <v>104</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>572</v>
+        <v>558</v>
       </c>
       <c r="F42" s="24" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>456</v>
+        <v>444</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="J42" s="6" t="s">
         <v>6</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="L42" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M42" s="24" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="N42" s="6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="O42" s="25"/>
       <c r="P42" s="6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="Q42" s="6">
         <v>0</v>
@@ -5606,38 +5606,38 @@
         <v>104</v>
       </c>
       <c r="E43" s="30" t="s">
-        <v>573</v>
+        <v>559</v>
       </c>
       <c r="F43" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>332</v>
+      </c>
+      <c r="H43" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="G43" s="6" t="s">
-        <v>334</v>
-      </c>
-      <c r="H43" s="6" t="s">
-        <v>335</v>
-      </c>
       <c r="I43" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="J43" s="6" t="s">
         <v>6</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="L43" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M43" s="24" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="N43" s="6" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="O43" s="25"/>
       <c r="P43" s="6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="Q43" s="6">
         <v>0</v>
@@ -5683,13 +5683,13 @@
         <v>36</v>
       </c>
       <c r="E44" s="30" t="s">
-        <v>574</v>
+        <v>560</v>
       </c>
       <c r="F44" s="13" t="s">
         <v>37</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="H44" s="13" t="s">
         <v>38</v>
@@ -5716,7 +5716,7 @@
         <v>40</v>
       </c>
       <c r="P44" s="13" t="s">
-        <v>510</v>
+        <v>496</v>
       </c>
       <c r="Q44" s="6">
         <v>1</v>
@@ -5762,13 +5762,13 @@
         <v>41</v>
       </c>
       <c r="E45" s="32" t="s">
-        <v>575</v>
+        <v>561</v>
       </c>
       <c r="F45" s="13" t="s">
         <v>42</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>457</v>
+        <v>445</v>
       </c>
       <c r="H45" s="13" t="s">
         <v>154</v>
@@ -5795,7 +5795,7 @@
         <v>43</v>
       </c>
       <c r="P45" s="13" t="s">
-        <v>511</v>
+        <v>497</v>
       </c>
       <c r="Q45" s="6">
         <v>0</v>
@@ -5841,13 +5841,13 @@
         <v>41</v>
       </c>
       <c r="E46" s="32" t="s">
-        <v>576</v>
+        <v>562</v>
       </c>
       <c r="F46" s="13" t="s">
         <v>44</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="H46" s="13" t="s">
         <v>155</v>
@@ -5874,7 +5874,7 @@
         <v>45</v>
       </c>
       <c r="P46" s="13" t="s">
-        <v>511</v>
+        <v>497</v>
       </c>
       <c r="Q46" s="6">
         <v>0</v>
@@ -5920,13 +5920,13 @@
         <v>41</v>
       </c>
       <c r="E47" s="32" t="s">
-        <v>577</v>
+        <v>563</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="H47" s="6" t="s">
         <v>189</v>
@@ -5950,10 +5950,10 @@
         <v>195</v>
       </c>
       <c r="O47" s="7" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="P47" s="6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="Q47" s="6">
         <v>1</v>
@@ -5985,13 +5985,13 @@
         <v>41</v>
       </c>
       <c r="E48" s="32" t="s">
-        <v>578</v>
+        <v>564</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>161</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>458</v>
+        <v>446</v>
       </c>
       <c r="H48" s="13" t="s">
         <v>162</v>
@@ -6018,7 +6018,7 @@
         <v>163</v>
       </c>
       <c r="P48" s="13" t="s">
-        <v>512</v>
+        <v>498</v>
       </c>
       <c r="Q48" s="6">
         <v>0</v>
@@ -6050,16 +6050,16 @@
         <v>46</v>
       </c>
       <c r="E49" s="32" t="s">
-        <v>579</v>
+        <v>565</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>660</v>
+        <v>646</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>459</v>
+        <v>447</v>
       </c>
       <c r="H49" s="27" t="s">
-        <v>646</v>
+        <v>632</v>
       </c>
       <c r="I49" s="6" t="s">
         <v>5</v>
@@ -6080,10 +6080,10 @@
         <v>195</v>
       </c>
       <c r="O49" s="7" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="P49" s="6" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="Q49" s="6">
         <v>1</v>
@@ -6115,16 +6115,16 @@
         <v>46</v>
       </c>
       <c r="E50" s="32" t="s">
-        <v>580</v>
+        <v>566</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>682</v>
+        <v>668</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="H50" s="27" t="s">
-        <v>472</v>
+        <v>458</v>
       </c>
       <c r="I50" s="6" t="s">
         <v>5</v>
@@ -6145,10 +6145,10 @@
         <v>195</v>
       </c>
       <c r="O50" s="7" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="P50" s="13" t="s">
-        <v>662</v>
+        <v>648</v>
       </c>
       <c r="Q50" s="6">
         <v>0</v>
@@ -6194,16 +6194,16 @@
         <v>46</v>
       </c>
       <c r="E51" s="32" t="s">
-        <v>581</v>
+        <v>567</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H51" s="27" t="s">
-        <v>473</v>
+        <v>459</v>
       </c>
       <c r="I51" s="6" t="s">
         <v>5</v>
@@ -6224,10 +6224,10 @@
         <v>195</v>
       </c>
       <c r="O51" s="7" t="s">
-        <v>647</v>
+        <v>633</v>
       </c>
       <c r="P51" s="13" t="s">
-        <v>662</v>
+        <v>648</v>
       </c>
       <c r="Q51" s="6">
         <v>0</v>
@@ -6273,16 +6273,16 @@
         <v>46</v>
       </c>
       <c r="E52" s="32" t="s">
-        <v>582</v>
+        <v>568</v>
       </c>
       <c r="F52" s="28" t="s">
-        <v>683</v>
+        <v>669</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="H52" s="27" t="s">
-        <v>474</v>
+        <v>460</v>
       </c>
       <c r="I52" s="6" t="s">
         <v>5</v>
@@ -6303,10 +6303,10 @@
         <v>195</v>
       </c>
       <c r="O52" s="7" t="s">
-        <v>648</v>
+        <v>634</v>
       </c>
       <c r="P52" s="13" t="s">
-        <v>663</v>
+        <v>649</v>
       </c>
       <c r="Q52" s="6">
         <v>0</v>
@@ -6352,16 +6352,16 @@
         <v>47</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>678</v>
+        <v>664</v>
       </c>
       <c r="F53" s="28" t="s">
-        <v>684</v>
+        <v>670</v>
       </c>
       <c r="G53" s="28" t="s">
-        <v>685</v>
+        <v>671</v>
       </c>
       <c r="H53" s="34" t="s">
-        <v>681</v>
+        <v>667</v>
       </c>
       <c r="I53" s="6" t="s">
         <v>5</v>
@@ -6382,10 +6382,10 @@
         <v>195</v>
       </c>
       <c r="O53" s="7" t="s">
-        <v>686</v>
+        <v>672</v>
       </c>
       <c r="P53" s="13" t="s">
-        <v>511</v>
+        <v>497</v>
       </c>
       <c r="Q53" s="6">
         <v>1</v>
@@ -6431,13 +6431,13 @@
         <v>47</v>
       </c>
       <c r="E54" s="32" t="s">
-        <v>583</v>
+        <v>569</v>
       </c>
       <c r="F54" s="13" t="s">
         <v>48</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="H54" s="13" t="s">
         <v>156</v>
@@ -6464,7 +6464,7 @@
         <v>49</v>
       </c>
       <c r="P54" s="13" t="s">
-        <v>512</v>
+        <v>498</v>
       </c>
       <c r="Q54" s="6">
         <v>0</v>
@@ -6510,13 +6510,13 @@
         <v>50</v>
       </c>
       <c r="E55" s="32" t="s">
-        <v>584</v>
+        <v>570</v>
       </c>
       <c r="F55" s="13" t="s">
         <v>51</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="H55" s="13" t="s">
         <v>157</v>
@@ -6541,7 +6541,7 @@
       </c>
       <c r="O55" s="13"/>
       <c r="P55" s="13" t="s">
-        <v>514</v>
+        <v>500</v>
       </c>
       <c r="Q55" s="6">
         <v>1</v>
@@ -6587,13 +6587,13 @@
         <v>104</v>
       </c>
       <c r="E56" s="32" t="s">
-        <v>585</v>
+        <v>571</v>
       </c>
       <c r="F56" s="31" t="s">
         <v>125</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="H56" s="6" t="s">
         <v>126</v>
@@ -6605,16 +6605,16 @@
         <v>6</v>
       </c>
       <c r="K56" s="6" t="s">
-        <v>691</v>
+        <v>677</v>
       </c>
       <c r="L56" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M56" s="6" t="s">
-        <v>689</v>
+        <v>675</v>
       </c>
       <c r="N56" s="6" t="s">
-        <v>692</v>
+        <v>678</v>
       </c>
       <c r="P56" s="6" t="s">
         <v>17</v>
@@ -6649,13 +6649,13 @@
         <v>104</v>
       </c>
       <c r="E57" s="30" t="s">
-        <v>586</v>
+        <v>572</v>
       </c>
       <c r="F57" s="31" t="s">
         <v>127</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="H57" s="6" t="s">
         <v>128</v>
@@ -6673,10 +6673,10 @@
         <v>8</v>
       </c>
       <c r="M57" s="6" t="s">
-        <v>689</v>
+        <v>675</v>
       </c>
       <c r="N57" s="6" t="s">
-        <v>692</v>
+        <v>678</v>
       </c>
       <c r="P57" s="6" t="s">
         <v>17</v>
@@ -6711,16 +6711,16 @@
         <v>104</v>
       </c>
       <c r="E58" s="30" t="s">
-        <v>587</v>
+        <v>573</v>
       </c>
       <c r="F58" s="31" t="s">
         <v>129</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>408</v>
+        <v>400</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>443</v>
+        <v>431</v>
       </c>
       <c r="I58" s="6" t="s">
         <v>5</v>
@@ -6729,16 +6729,16 @@
         <v>6</v>
       </c>
       <c r="K58" s="6" t="s">
-        <v>690</v>
+        <v>676</v>
       </c>
       <c r="L58" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M58" s="6" t="s">
-        <v>689</v>
+        <v>675</v>
       </c>
       <c r="N58" s="6" t="s">
-        <v>692</v>
+        <v>678</v>
       </c>
       <c r="P58" s="6" t="s">
         <v>17</v>
@@ -6773,13 +6773,13 @@
         <v>104</v>
       </c>
       <c r="E59" s="30" t="s">
-        <v>588</v>
+        <v>574</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>130</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>447</v>
+        <v>435</v>
       </c>
       <c r="H59" s="6" t="s">
         <v>131</v>
@@ -6797,10 +6797,10 @@
         <v>8</v>
       </c>
       <c r="M59" s="6" t="s">
-        <v>527</v>
+        <v>513</v>
       </c>
       <c r="N59" s="6" t="s">
-        <v>528</v>
+        <v>514</v>
       </c>
       <c r="P59" s="6" t="s">
         <v>17</v>
@@ -6835,13 +6835,13 @@
         <v>104</v>
       </c>
       <c r="E60" s="30" t="s">
-        <v>589</v>
+        <v>575</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>171</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>409</v>
+        <v>401</v>
       </c>
       <c r="H60" s="6" t="s">
         <v>170</v>
@@ -6859,10 +6859,10 @@
         <v>8</v>
       </c>
       <c r="M60" s="6" t="s">
-        <v>529</v>
+        <v>515</v>
       </c>
       <c r="N60" s="6" t="s">
-        <v>530</v>
+        <v>516</v>
       </c>
       <c r="P60" s="6" t="s">
         <v>17</v>
@@ -6897,13 +6897,13 @@
         <v>104</v>
       </c>
       <c r="E61" s="30" t="s">
-        <v>590</v>
+        <v>576</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>172</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>410</v>
+        <v>402</v>
       </c>
       <c r="H61" s="6" t="s">
         <v>173</v>
@@ -6921,10 +6921,10 @@
         <v>8</v>
       </c>
       <c r="M61" s="6" t="s">
-        <v>529</v>
+        <v>515</v>
       </c>
       <c r="N61" s="6" t="s">
-        <v>530</v>
+        <v>516</v>
       </c>
       <c r="P61" s="6" t="s">
         <v>17</v>
@@ -6959,13 +6959,13 @@
         <v>104</v>
       </c>
       <c r="E62" s="30" t="s">
-        <v>679</v>
+        <v>665</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>680</v>
+        <v>666</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="H62" s="6" t="s">
         <v>174</v>
@@ -6983,10 +6983,10 @@
         <v>8</v>
       </c>
       <c r="M62" s="6" t="s">
-        <v>529</v>
+        <v>515</v>
       </c>
       <c r="N62" s="6" t="s">
-        <v>530</v>
+        <v>516</v>
       </c>
       <c r="P62" s="6" t="s">
         <v>17</v>
@@ -7021,13 +7021,13 @@
         <v>3</v>
       </c>
       <c r="E63" s="30" t="s">
-        <v>591</v>
+        <v>577</v>
       </c>
       <c r="F63" s="6" t="s">
         <v>53</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>412</v>
+        <v>404</v>
       </c>
       <c r="H63" s="6" t="s">
         <v>158</v>
@@ -7039,7 +7039,7 @@
         <v>6</v>
       </c>
       <c r="K63" s="6" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="L63" s="6" t="s">
         <v>8</v>
@@ -7086,13 +7086,13 @@
         <v>3</v>
       </c>
       <c r="E64" s="30" t="s">
-        <v>592</v>
+        <v>578</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="H64" s="6" t="s">
         <v>159</v>
@@ -7119,7 +7119,7 @@
         <v>54</v>
       </c>
       <c r="P64" s="13" t="s">
-        <v>515</v>
+        <v>501</v>
       </c>
       <c r="Q64" s="6">
         <v>1</v>
@@ -7151,16 +7151,16 @@
         <v>3</v>
       </c>
       <c r="E65" s="30" t="s">
-        <v>594</v>
+        <v>580</v>
       </c>
       <c r="F65" s="6" t="s">
         <v>55</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>414</v>
+        <v>406</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>476</v>
+        <v>462</v>
       </c>
       <c r="I65" s="6" t="s">
         <v>5</v>
@@ -7184,7 +7184,7 @@
         <v>54</v>
       </c>
       <c r="P65" s="13" t="s">
-        <v>515</v>
+        <v>501</v>
       </c>
       <c r="Q65" s="6">
         <v>0</v>
@@ -7222,10 +7222,10 @@
         <v>56</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>415</v>
+        <v>407</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>475</v>
+        <v>461</v>
       </c>
       <c r="I66" s="6" t="s">
         <v>5</v>
@@ -7249,7 +7249,7 @@
         <v>54</v>
       </c>
       <c r="P66" s="13" t="s">
-        <v>515</v>
+        <v>501</v>
       </c>
       <c r="Q66" s="6">
         <v>1</v>
@@ -7281,16 +7281,16 @@
         <v>3</v>
       </c>
       <c r="E67" s="30" t="s">
-        <v>595</v>
+        <v>581</v>
       </c>
       <c r="F67" s="6" t="s">
         <v>57</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>416</v>
+        <v>408</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>477</v>
+        <v>463</v>
       </c>
       <c r="I67" s="6" t="s">
         <v>5</v>
@@ -7346,16 +7346,16 @@
         <v>3</v>
       </c>
       <c r="E68" s="30" t="s">
-        <v>596</v>
+        <v>582</v>
       </c>
       <c r="F68" s="6" t="s">
         <v>58</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>460</v>
+        <v>448</v>
       </c>
       <c r="H68" s="6" t="s">
-        <v>478</v>
+        <v>464</v>
       </c>
       <c r="I68" s="6" t="s">
         <v>5</v>
@@ -7411,13 +7411,13 @@
         <v>3</v>
       </c>
       <c r="E69" s="30" t="s">
-        <v>593</v>
+        <v>579</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="H69" s="6" t="s">
         <v>159</v>
@@ -7444,7 +7444,7 @@
         <v>54</v>
       </c>
       <c r="P69" s="13" t="s">
-        <v>515</v>
+        <v>501</v>
       </c>
       <c r="Q69" s="6">
         <v>0</v>
@@ -7476,16 +7476,16 @@
         <v>59</v>
       </c>
       <c r="E70" s="30" t="s">
-        <v>597</v>
+        <v>583</v>
       </c>
       <c r="F70" s="6" t="s">
         <v>60</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>417</v>
+        <v>409</v>
       </c>
       <c r="H70" s="6" t="s">
-        <v>479</v>
+        <v>465</v>
       </c>
       <c r="I70" s="6" t="s">
         <v>5</v>
@@ -7541,16 +7541,16 @@
         <v>59</v>
       </c>
       <c r="E71" s="30" t="s">
-        <v>598</v>
+        <v>584</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>164</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="H71" s="6" t="s">
-        <v>480</v>
+        <v>466</v>
       </c>
       <c r="I71" s="6" t="s">
         <v>5</v>
@@ -7606,16 +7606,16 @@
         <v>59</v>
       </c>
       <c r="E72" s="30" t="s">
-        <v>599</v>
+        <v>585</v>
       </c>
       <c r="F72" s="6" t="s">
         <v>62</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>419</v>
+        <v>411</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>481</v>
+        <v>467</v>
       </c>
       <c r="I72" s="6" t="s">
         <v>5</v>
@@ -7671,16 +7671,16 @@
         <v>59</v>
       </c>
       <c r="E73" s="30" t="s">
-        <v>600</v>
+        <v>586</v>
       </c>
       <c r="F73" s="6" t="s">
         <v>63</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>420</v>
+        <v>412</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>482</v>
+        <v>468</v>
       </c>
       <c r="I73" s="6" t="s">
         <v>5</v>
@@ -7736,16 +7736,16 @@
         <v>59</v>
       </c>
       <c r="E74" s="30" t="s">
-        <v>601</v>
+        <v>587</v>
       </c>
       <c r="F74" s="6" t="s">
         <v>165</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>421</v>
+        <v>413</v>
       </c>
       <c r="H74" s="6" t="s">
-        <v>483</v>
+        <v>469</v>
       </c>
       <c r="I74" s="6" t="s">
         <v>5</v>
@@ -7801,16 +7801,16 @@
         <v>59</v>
       </c>
       <c r="E75" s="30" t="s">
-        <v>602</v>
+        <v>588</v>
       </c>
       <c r="F75" s="6" t="s">
         <v>166</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>422</v>
+        <v>414</v>
       </c>
       <c r="H75" s="6" t="s">
-        <v>484</v>
+        <v>470</v>
       </c>
       <c r="I75" s="6" t="s">
         <v>5</v>
@@ -7866,16 +7866,16 @@
         <v>59</v>
       </c>
       <c r="E76" s="30" t="s">
-        <v>603</v>
+        <v>589</v>
       </c>
       <c r="F76" s="6" t="s">
         <v>167</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>423</v>
+        <v>415</v>
       </c>
       <c r="H76" s="6" t="s">
-        <v>485</v>
+        <v>471</v>
       </c>
       <c r="I76" s="6" t="s">
         <v>5</v>
@@ -7931,16 +7931,16 @@
         <v>59</v>
       </c>
       <c r="E77" s="30" t="s">
-        <v>604</v>
+        <v>590</v>
       </c>
       <c r="F77" s="6" t="s">
         <v>168</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>424</v>
+        <v>416</v>
       </c>
       <c r="H77" s="6" t="s">
-        <v>486</v>
+        <v>472</v>
       </c>
       <c r="I77" s="6" t="s">
         <v>5</v>
@@ -7996,16 +7996,16 @@
         <v>59</v>
       </c>
       <c r="E78" s="30" t="s">
-        <v>605</v>
+        <v>591</v>
       </c>
       <c r="F78" s="6" t="s">
         <v>64</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>425</v>
+        <v>417</v>
       </c>
       <c r="H78" s="6" t="s">
-        <v>487</v>
+        <v>473</v>
       </c>
       <c r="I78" s="6" t="s">
         <v>5</v>
@@ -8061,16 +8061,16 @@
         <v>59</v>
       </c>
       <c r="E79" s="30" t="s">
-        <v>606</v>
+        <v>592</v>
       </c>
       <c r="F79" s="6" t="s">
         <v>65</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>426</v>
+        <v>418</v>
       </c>
       <c r="H79" s="6" t="s">
-        <v>488</v>
+        <v>474</v>
       </c>
       <c r="I79" s="6" t="s">
         <v>5</v>
@@ -8126,16 +8126,16 @@
         <v>59</v>
       </c>
       <c r="E80" s="30" t="s">
-        <v>607</v>
+        <v>593</v>
       </c>
       <c r="F80" s="6" t="s">
         <v>66</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>427</v>
+        <v>419</v>
       </c>
       <c r="H80" s="6" t="s">
-        <v>489</v>
+        <v>475</v>
       </c>
       <c r="I80" s="6" t="s">
         <v>5</v>
@@ -8191,16 +8191,16 @@
         <v>59</v>
       </c>
       <c r="E81" s="30" t="s">
-        <v>608</v>
+        <v>594</v>
       </c>
       <c r="F81" s="6" t="s">
         <v>67</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>428</v>
+        <v>420</v>
       </c>
       <c r="H81" s="6" t="s">
-        <v>490</v>
+        <v>476</v>
       </c>
       <c r="I81" s="6" t="s">
         <v>5</v>
@@ -8256,13 +8256,13 @@
         <v>59</v>
       </c>
       <c r="E82" s="30" t="s">
-        <v>609</v>
+        <v>595</v>
       </c>
       <c r="F82" s="6" t="s">
         <v>68</v>
       </c>
       <c r="G82" s="6" t="s">
-        <v>461</v>
+        <v>449</v>
       </c>
       <c r="H82" s="6" t="s">
         <v>160</v>
@@ -8321,13 +8321,13 @@
         <v>104</v>
       </c>
       <c r="E83" s="30" t="s">
-        <v>610</v>
+        <v>596</v>
       </c>
       <c r="F83" s="31" t="s">
         <v>132</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>429</v>
+        <v>421</v>
       </c>
       <c r="H83" s="6" t="s">
         <v>133</v>
@@ -8339,16 +8339,16 @@
         <v>6</v>
       </c>
       <c r="K83" s="6" t="s">
-        <v>691</v>
+        <v>677</v>
       </c>
       <c r="L83" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M83" s="6" t="s">
-        <v>689</v>
+        <v>675</v>
       </c>
       <c r="N83" s="6" t="s">
-        <v>692</v>
+        <v>678</v>
       </c>
       <c r="P83" s="6" t="s">
         <v>17</v>
@@ -8383,13 +8383,13 @@
         <v>104</v>
       </c>
       <c r="E84" s="30" t="s">
-        <v>611</v>
+        <v>597</v>
       </c>
       <c r="F84" s="31" t="s">
         <v>134</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>430</v>
+        <v>422</v>
       </c>
       <c r="H84" s="6" t="s">
         <v>135</v>
@@ -8407,10 +8407,10 @@
         <v>8</v>
       </c>
       <c r="M84" s="6" t="s">
-        <v>689</v>
+        <v>675</v>
       </c>
       <c r="N84" s="6" t="s">
-        <v>692</v>
+        <v>678</v>
       </c>
       <c r="O84" s="6"/>
       <c r="P84" s="6" t="s">
@@ -8460,16 +8460,16 @@
         <v>104</v>
       </c>
       <c r="E85" s="30" t="s">
-        <v>612</v>
+        <v>598</v>
       </c>
       <c r="F85" s="31" t="s">
         <v>136</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>431</v>
+        <v>423</v>
       </c>
       <c r="H85" s="6" t="s">
-        <v>442</v>
+        <v>430</v>
       </c>
       <c r="I85" s="6" t="s">
         <v>5</v>
@@ -8478,16 +8478,16 @@
         <v>6</v>
       </c>
       <c r="K85" s="6" t="s">
-        <v>690</v>
+        <v>676</v>
       </c>
       <c r="L85" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M85" s="6" t="s">
-        <v>689</v>
+        <v>675</v>
       </c>
       <c r="N85" s="6" t="s">
-        <v>692</v>
+        <v>678</v>
       </c>
       <c r="O85" s="6"/>
       <c r="P85" s="6" t="s">
@@ -8537,13 +8537,13 @@
         <v>104</v>
       </c>
       <c r="E86" s="30" t="s">
-        <v>613</v>
+        <v>599</v>
       </c>
       <c r="F86" s="6" t="s">
         <v>137</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>448</v>
+        <v>436</v>
       </c>
       <c r="H86" s="6" t="s">
         <v>138</v>
@@ -8561,10 +8561,10 @@
         <v>8</v>
       </c>
       <c r="M86" s="6" t="s">
-        <v>527</v>
+        <v>513</v>
       </c>
       <c r="N86" s="6" t="s">
-        <v>528</v>
+        <v>514</v>
       </c>
       <c r="P86" s="6" t="s">
         <v>17</v>
@@ -8599,16 +8599,16 @@
         <v>104</v>
       </c>
       <c r="E87" s="30" t="s">
-        <v>614</v>
+        <v>600</v>
       </c>
       <c r="F87" s="19" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>664</v>
+        <v>650</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>674</v>
+        <v>660</v>
       </c>
       <c r="I87" s="7" t="s">
         <v>238</v>
@@ -8623,10 +8623,10 @@
         <v>8</v>
       </c>
       <c r="M87" s="7" t="s">
-        <v>241</v>
+        <v>708</v>
       </c>
       <c r="N87" s="7" t="s">
-        <v>242</v>
+        <v>709</v>
       </c>
       <c r="O87" s="6"/>
       <c r="P87" s="6" t="s">
@@ -8676,34 +8676,34 @@
         <v>104</v>
       </c>
       <c r="E88" s="32" t="s">
-        <v>615</v>
+        <v>601</v>
       </c>
       <c r="F88" s="19" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>665</v>
+        <v>651</v>
       </c>
       <c r="H88" s="7" t="s">
-        <v>675</v>
+        <v>661</v>
       </c>
       <c r="I88" s="7" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J88" s="7" t="s">
         <v>239</v>
       </c>
       <c r="K88" s="6" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="L88" s="7" t="s">
         <v>8</v>
       </c>
       <c r="M88" s="7" t="s">
-        <v>241</v>
+        <v>708</v>
       </c>
       <c r="N88" s="7" t="s">
-        <v>242</v>
+        <v>709</v>
       </c>
       <c r="P88" s="6" t="s">
         <v>17</v>
@@ -8738,16 +8738,16 @@
         <v>104</v>
       </c>
       <c r="E89" s="30" t="s">
-        <v>616</v>
+        <v>602</v>
       </c>
       <c r="F89" s="19" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>666</v>
+        <v>652</v>
       </c>
       <c r="H89" s="7" t="s">
-        <v>676</v>
+        <v>662</v>
       </c>
       <c r="I89" s="7" t="s">
         <v>238</v>
@@ -8756,20 +8756,20 @@
         <v>239</v>
       </c>
       <c r="K89" s="7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="L89" s="7" t="s">
         <v>8</v>
       </c>
       <c r="M89" s="7" t="s">
-        <v>241</v>
+        <v>708</v>
       </c>
       <c r="N89" s="7" t="s">
-        <v>242</v>
+        <v>709</v>
       </c>
       <c r="O89" s="7"/>
       <c r="P89" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q89" s="6">
         <v>0</v>
@@ -8815,38 +8815,38 @@
         <v>104</v>
       </c>
       <c r="E90" s="30" t="s">
-        <v>617</v>
+        <v>603</v>
       </c>
       <c r="F90" s="20" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>667</v>
+        <v>653</v>
       </c>
       <c r="H90" s="7" t="s">
-        <v>677</v>
+        <v>663</v>
       </c>
       <c r="I90" s="7" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J90" s="7" t="s">
         <v>239</v>
       </c>
       <c r="K90" s="7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="L90" s="7" t="s">
         <v>8</v>
       </c>
       <c r="M90" s="7" t="s">
-        <v>241</v>
+        <v>708</v>
       </c>
       <c r="N90" s="7" t="s">
-        <v>242</v>
+        <v>709</v>
       </c>
       <c r="O90" s="7"/>
       <c r="P90" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q90" s="6">
         <v>0</v>
@@ -8886,22 +8886,22 @@
         <v>70</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D91" s="7" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="E91" s="30" t="s">
-        <v>618</v>
+        <v>604</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>462</v>
+        <v>450</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="I91" s="7" t="s">
         <v>5</v>
@@ -8916,14 +8916,14 @@
         <v>8</v>
       </c>
       <c r="M91" s="9" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="N91" s="7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="O91" s="7"/>
       <c r="P91" s="7" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="Q91" s="6">
         <v>0</v>
@@ -8966,16 +8966,16 @@
         <v>2</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>649</v>
+        <v>635</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>645</v>
+        <v>631</v>
       </c>
       <c r="F92" s="6" t="s">
         <v>190</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="H92" s="6" t="s">
         <v>191</v>
@@ -9000,7 +9000,7 @@
       </c>
       <c r="O92" s="6"/>
       <c r="P92" s="6" t="s">
-        <v>515</v>
+        <v>501</v>
       </c>
       <c r="Q92" s="6">
         <v>1</v>
@@ -9043,7 +9043,7 @@
         <v>2</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>649</v>
+        <v>635</v>
       </c>
       <c r="E93" s="30" t="s">
         <v>71</v>
@@ -9052,10 +9052,10 @@
         <v>71</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>439</v>
+        <v>428</v>
       </c>
       <c r="H93" s="6" t="s">
-        <v>491</v>
+        <v>477</v>
       </c>
       <c r="I93" s="6" t="s">
         <v>192</v>
@@ -9077,7 +9077,7 @@
       </c>
       <c r="O93" s="6"/>
       <c r="P93" s="6" t="s">
-        <v>516</v>
+        <v>502</v>
       </c>
       <c r="Q93" s="6">
         <v>1</v>
@@ -9120,28 +9120,28 @@
         <v>2</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>649</v>
+        <v>635</v>
       </c>
       <c r="E94" s="30" t="s">
-        <v>643</v>
+        <v>629</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>436</v>
+        <v>425</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>508</v>
+        <v>494</v>
       </c>
       <c r="I94" s="11" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="J94" s="11" t="s">
         <v>6</v>
       </c>
       <c r="K94" s="11" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="L94" s="11" t="s">
         <v>8</v>
@@ -9197,10 +9197,10 @@
         <v>2</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>649</v>
+        <v>635</v>
       </c>
       <c r="E95" s="30" t="s">
-        <v>619</v>
+        <v>605</v>
       </c>
       <c r="F95" s="12" t="s">
         <v>197</v>
@@ -9209,7 +9209,7 @@
         <v>198</v>
       </c>
       <c r="H95" s="11" t="s">
-        <v>492</v>
+        <v>478</v>
       </c>
       <c r="I95" s="11" t="s">
         <v>199</v>
@@ -9259,10 +9259,10 @@
         <v>2</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>649</v>
+        <v>635</v>
       </c>
       <c r="E96" s="30" t="s">
-        <v>620</v>
+        <v>606</v>
       </c>
       <c r="F96" s="12" t="s">
         <v>231</v>
@@ -9271,7 +9271,7 @@
         <v>203</v>
       </c>
       <c r="H96" s="11" t="s">
-        <v>493</v>
+        <v>479</v>
       </c>
       <c r="I96" s="11" t="s">
         <v>199</v>
@@ -9321,19 +9321,19 @@
         <v>2</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>649</v>
+        <v>635</v>
       </c>
       <c r="E97" s="30" t="s">
-        <v>621</v>
+        <v>607</v>
       </c>
       <c r="F97" s="12" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G97" s="6" t="s">
         <v>204</v>
       </c>
       <c r="H97" s="11" t="s">
-        <v>494</v>
+        <v>480</v>
       </c>
       <c r="I97" s="11" t="s">
         <v>199</v>
@@ -9383,10 +9383,10 @@
         <v>2</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>649</v>
+        <v>635</v>
       </c>
       <c r="E98" s="30" t="s">
-        <v>622</v>
+        <v>608</v>
       </c>
       <c r="F98" s="12" t="s">
         <v>232</v>
@@ -9395,7 +9395,7 @@
         <v>205</v>
       </c>
       <c r="H98" s="11" t="s">
-        <v>495</v>
+        <v>481</v>
       </c>
       <c r="I98" s="11" t="s">
         <v>206</v>
@@ -9445,10 +9445,10 @@
         <v>2</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>649</v>
+        <v>635</v>
       </c>
       <c r="E99" s="30" t="s">
-        <v>623</v>
+        <v>609</v>
       </c>
       <c r="F99" s="12" t="s">
         <v>207</v>
@@ -9457,7 +9457,7 @@
         <v>208</v>
       </c>
       <c r="H99" s="11" t="s">
-        <v>496</v>
+        <v>482</v>
       </c>
       <c r="I99" s="11" t="s">
         <v>209</v>
@@ -9507,10 +9507,10 @@
         <v>2</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>649</v>
+        <v>635</v>
       </c>
       <c r="E100" s="30" t="s">
-        <v>627</v>
+        <v>613</v>
       </c>
       <c r="F100" s="12" t="s">
         <v>225</v>
@@ -9519,7 +9519,7 @@
         <v>214</v>
       </c>
       <c r="H100" s="11" t="s">
-        <v>500</v>
+        <v>486</v>
       </c>
       <c r="I100" s="11" t="s">
         <v>215</v>
@@ -9569,10 +9569,10 @@
         <v>2</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>649</v>
+        <v>635</v>
       </c>
       <c r="E101" s="30" t="s">
-        <v>628</v>
+        <v>614</v>
       </c>
       <c r="F101" s="12" t="s">
         <v>226</v>
@@ -9581,7 +9581,7 @@
         <v>217</v>
       </c>
       <c r="H101" s="11" t="s">
-        <v>501</v>
+        <v>487</v>
       </c>
       <c r="I101" s="11" t="s">
         <v>215</v>
@@ -9631,10 +9631,10 @@
         <v>2</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>649</v>
+        <v>635</v>
       </c>
       <c r="E102" s="30" t="s">
-        <v>629</v>
+        <v>615</v>
       </c>
       <c r="F102" s="12" t="s">
         <v>227</v>
@@ -9643,7 +9643,7 @@
         <v>218</v>
       </c>
       <c r="H102" s="11" t="s">
-        <v>502</v>
+        <v>488</v>
       </c>
       <c r="I102" s="11" t="s">
         <v>215</v>
@@ -9693,10 +9693,10 @@
         <v>2</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>649</v>
+        <v>635</v>
       </c>
       <c r="E103" s="30" t="s">
-        <v>630</v>
+        <v>616</v>
       </c>
       <c r="F103" s="12" t="s">
         <v>228</v>
@@ -9705,7 +9705,7 @@
         <v>219</v>
       </c>
       <c r="H103" s="11" t="s">
-        <v>503</v>
+        <v>489</v>
       </c>
       <c r="I103" s="11" t="s">
         <v>215</v>
@@ -9770,10 +9770,10 @@
         <v>2</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>649</v>
+        <v>635</v>
       </c>
       <c r="E104" s="30" t="s">
-        <v>631</v>
+        <v>617</v>
       </c>
       <c r="F104" s="12" t="s">
         <v>229</v>
@@ -9782,7 +9782,7 @@
         <v>220</v>
       </c>
       <c r="H104" s="11" t="s">
-        <v>504</v>
+        <v>490</v>
       </c>
       <c r="I104" s="11" t="s">
         <v>215</v>
@@ -9847,10 +9847,10 @@
         <v>2</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>649</v>
+        <v>635</v>
       </c>
       <c r="E105" s="30" t="s">
-        <v>632</v>
+        <v>618</v>
       </c>
       <c r="F105" s="12" t="s">
         <v>230</v>
@@ -9859,7 +9859,7 @@
         <v>221</v>
       </c>
       <c r="H105" s="11" t="s">
-        <v>505</v>
+        <v>491</v>
       </c>
       <c r="I105" s="11" t="s">
         <v>215</v>
@@ -9927,37 +9927,37 @@
         <v>3</v>
       </c>
       <c r="E106" s="30" t="s">
+        <v>640</v>
+      </c>
+      <c r="F106" s="21" t="s">
         <v>654</v>
       </c>
-      <c r="F106" s="21" t="s">
-        <v>668</v>
-      </c>
       <c r="G106" s="6" t="s">
-        <v>365</v>
+        <v>710</v>
       </c>
       <c r="H106" s="7" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="I106" s="7" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="J106" s="7" t="s">
         <v>239</v>
       </c>
       <c r="K106" s="7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="L106" s="7" t="s">
         <v>8</v>
       </c>
       <c r="M106" s="7" t="s">
-        <v>241</v>
+        <v>708</v>
       </c>
       <c r="N106" s="7" t="s">
-        <v>242</v>
+        <v>709</v>
       </c>
       <c r="P106" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q106" s="6">
         <v>0</v>
@@ -9989,37 +9989,37 @@
         <v>3</v>
       </c>
       <c r="E107" s="30" t="s">
+        <v>641</v>
+      </c>
+      <c r="F107" s="8" t="s">
         <v>655</v>
       </c>
-      <c r="F107" s="8" t="s">
-        <v>669</v>
-      </c>
       <c r="G107" s="6" t="s">
-        <v>366</v>
+        <v>711</v>
       </c>
       <c r="H107" s="7" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="I107" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="J107" s="7" t="s">
         <v>239</v>
       </c>
       <c r="K107" s="7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="L107" s="7" t="s">
         <v>8</v>
       </c>
       <c r="M107" s="7" t="s">
-        <v>241</v>
+        <v>708</v>
       </c>
       <c r="N107" s="7" t="s">
-        <v>242</v>
+        <v>709</v>
       </c>
       <c r="P107" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q107" s="6">
         <v>0</v>
@@ -10051,37 +10051,37 @@
         <v>3</v>
       </c>
       <c r="E108" s="30" t="s">
+        <v>642</v>
+      </c>
+      <c r="F108" s="8" t="s">
         <v>656</v>
       </c>
-      <c r="F108" s="8" t="s">
-        <v>670</v>
-      </c>
       <c r="G108" s="6" t="s">
-        <v>367</v>
+        <v>712</v>
       </c>
       <c r="H108" s="7" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="I108" s="7" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="J108" s="7" t="s">
         <v>239</v>
       </c>
       <c r="K108" s="7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="L108" s="7" t="s">
         <v>8</v>
       </c>
       <c r="M108" s="7" t="s">
-        <v>241</v>
+        <v>708</v>
       </c>
       <c r="N108" s="7" t="s">
-        <v>242</v>
+        <v>709</v>
       </c>
       <c r="P108" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q108" s="6">
         <v>0</v>
@@ -10113,38 +10113,38 @@
         <v>3</v>
       </c>
       <c r="E109" s="30" t="s">
-        <v>659</v>
+        <v>645</v>
       </c>
       <c r="F109" s="8" t="s">
-        <v>671</v>
+        <v>657</v>
       </c>
       <c r="G109" s="6" t="s">
-        <v>369</v>
+        <v>713</v>
       </c>
       <c r="H109" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="I109" s="7" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="J109" s="7" t="s">
         <v>239</v>
       </c>
       <c r="K109" s="7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="L109" s="7" t="s">
         <v>8</v>
       </c>
       <c r="M109" s="7" t="s">
-        <v>241</v>
+        <v>708</v>
       </c>
       <c r="N109" s="7" t="s">
-        <v>242</v>
+        <v>709</v>
       </c>
       <c r="O109" s="7"/>
       <c r="P109" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q109" s="6">
         <v>0</v>
@@ -10190,37 +10190,37 @@
         <v>3</v>
       </c>
       <c r="E110" s="30" t="s">
-        <v>657</v>
+        <v>643</v>
       </c>
       <c r="F110" s="22" t="s">
-        <v>672</v>
+        <v>658</v>
       </c>
       <c r="G110" s="6" t="s">
-        <v>464</v>
+        <v>714</v>
       </c>
       <c r="H110" s="7" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="I110" s="7" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="J110" s="7" t="s">
         <v>239</v>
       </c>
       <c r="K110" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="L110" s="7" t="s">
         <v>8</v>
       </c>
       <c r="M110" s="7" t="s">
-        <v>241</v>
+        <v>708</v>
       </c>
       <c r="N110" s="7" t="s">
-        <v>242</v>
+        <v>709</v>
       </c>
       <c r="P110" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q110" s="6">
         <v>0</v>
@@ -10252,38 +10252,38 @@
         <v>3</v>
       </c>
       <c r="E111" s="30" t="s">
-        <v>658</v>
+        <v>644</v>
       </c>
       <c r="F111" s="22" t="s">
-        <v>673</v>
+        <v>659</v>
       </c>
       <c r="G111" s="6" t="s">
-        <v>368</v>
+        <v>715</v>
       </c>
       <c r="H111" s="7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="I111" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="J111" s="7" t="s">
         <v>239</v>
       </c>
       <c r="K111" s="7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="L111" s="7" t="s">
         <v>8</v>
       </c>
       <c r="M111" s="7" t="s">
-        <v>241</v>
+        <v>708</v>
       </c>
       <c r="N111" s="7" t="s">
-        <v>242</v>
+        <v>709</v>
       </c>
       <c r="O111" s="7"/>
       <c r="P111" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q111" s="6">
         <v>0</v>
@@ -10329,37 +10329,37 @@
         <v>3</v>
       </c>
       <c r="E112" s="30" t="s">
-        <v>651</v>
+        <v>637</v>
       </c>
       <c r="F112" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="G112" s="6" t="s">
+        <v>716</v>
+      </c>
+      <c r="H112" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="I112" s="7" t="s">
         <v>249</v>
-      </c>
-      <c r="G112" s="6" t="s">
-        <v>433</v>
-      </c>
-      <c r="H112" s="7" t="s">
-        <v>250</v>
-      </c>
-      <c r="I112" s="7" t="s">
-        <v>251</v>
       </c>
       <c r="J112" s="7" t="s">
         <v>239</v>
       </c>
       <c r="K112" s="7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="L112" s="7" t="s">
         <v>8</v>
       </c>
       <c r="M112" s="7" t="s">
-        <v>241</v>
+        <v>708</v>
       </c>
       <c r="N112" s="7" t="s">
-        <v>242</v>
+        <v>709</v>
       </c>
       <c r="P112" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q112" s="6">
         <v>0</v>
@@ -10391,37 +10391,37 @@
         <v>3</v>
       </c>
       <c r="E113" s="30" t="s">
-        <v>652</v>
+        <v>638</v>
       </c>
       <c r="F113" s="7" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="G113" s="6" t="s">
-        <v>434</v>
+        <v>717</v>
       </c>
       <c r="H113" s="7" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="I113" s="7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="J113" s="7" t="s">
         <v>239</v>
       </c>
       <c r="K113" s="7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="L113" s="7" t="s">
         <v>8</v>
       </c>
       <c r="M113" s="7" t="s">
-        <v>241</v>
+        <v>708</v>
       </c>
       <c r="N113" s="7" t="s">
-        <v>242</v>
+        <v>709</v>
       </c>
       <c r="P113" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q113" s="6">
         <v>0</v>
@@ -10453,37 +10453,37 @@
         <v>3</v>
       </c>
       <c r="E114" s="30" t="s">
-        <v>653</v>
+        <v>639</v>
       </c>
       <c r="F114" s="7" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>435</v>
+        <v>718</v>
       </c>
       <c r="H114" s="7" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="I114" s="7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="J114" s="7" t="s">
         <v>239</v>
       </c>
       <c r="K114" s="7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="L114" s="7" t="s">
         <v>8</v>
       </c>
       <c r="M114" s="7" t="s">
-        <v>241</v>
+        <v>708</v>
       </c>
       <c r="N114" s="7" t="s">
-        <v>242</v>
+        <v>709</v>
       </c>
       <c r="P114" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q114" s="6">
         <v>0</v>
@@ -10515,37 +10515,37 @@
         <v>15</v>
       </c>
       <c r="E115" s="30" t="s">
-        <v>633</v>
+        <v>619</v>
       </c>
       <c r="F115" s="21" t="s">
+        <v>254</v>
+      </c>
+      <c r="G115" s="6" t="s">
+        <v>719</v>
+      </c>
+      <c r="H115" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="I115" s="7" t="s">
         <v>256</v>
-      </c>
-      <c r="G115" s="6" t="s">
-        <v>370</v>
-      </c>
-      <c r="H115" s="7" t="s">
-        <v>257</v>
-      </c>
-      <c r="I115" s="7" t="s">
-        <v>258</v>
       </c>
       <c r="J115" s="7" t="s">
         <v>239</v>
       </c>
       <c r="K115" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="L115" s="7" t="s">
         <v>8</v>
       </c>
       <c r="M115" s="7" t="s">
-        <v>241</v>
+        <v>708</v>
       </c>
       <c r="N115" s="7" t="s">
-        <v>242</v>
+        <v>709</v>
       </c>
       <c r="P115" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q115" s="6">
         <v>1</v>
@@ -10577,16 +10577,16 @@
         <v>15</v>
       </c>
       <c r="E116" s="30" t="s">
-        <v>635</v>
+        <v>621</v>
       </c>
       <c r="F116" s="8" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="G116" s="6" t="s">
-        <v>463</v>
+        <v>720</v>
       </c>
       <c r="H116" s="7" t="s">
-        <v>507</v>
+        <v>493</v>
       </c>
       <c r="I116" s="7" t="s">
         <v>5</v>
@@ -10595,20 +10595,20 @@
         <v>239</v>
       </c>
       <c r="K116" s="7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="L116" s="7" t="s">
         <v>8</v>
       </c>
       <c r="M116" s="7" t="s">
-        <v>241</v>
+        <v>708</v>
       </c>
       <c r="N116" s="7" t="s">
-        <v>242</v>
+        <v>709</v>
       </c>
       <c r="O116" s="7"/>
       <c r="P116" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q116" s="6">
         <v>0</v>
@@ -10654,16 +10654,16 @@
         <v>15</v>
       </c>
       <c r="E117" s="30" t="s">
-        <v>644</v>
+        <v>630</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="G117" s="6" t="s">
-        <v>437</v>
+        <v>426</v>
       </c>
       <c r="H117" s="2" t="s">
-        <v>509</v>
+        <v>495</v>
       </c>
       <c r="I117" s="11" t="s">
         <v>5</v>
@@ -10672,7 +10672,7 @@
         <v>6</v>
       </c>
       <c r="K117" s="11" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="L117" s="11" t="s">
         <v>8</v>
@@ -10731,7 +10731,7 @@
         <v>15</v>
       </c>
       <c r="E118" s="30" t="s">
-        <v>624</v>
+        <v>610</v>
       </c>
       <c r="F118" s="12" t="s">
         <v>210</v>
@@ -10740,7 +10740,7 @@
         <v>222</v>
       </c>
       <c r="H118" s="11" t="s">
-        <v>497</v>
+        <v>483</v>
       </c>
       <c r="I118" s="11" t="s">
         <v>211</v>
@@ -10793,7 +10793,7 @@
         <v>15</v>
       </c>
       <c r="E119" s="30" t="s">
-        <v>625</v>
+        <v>611</v>
       </c>
       <c r="F119" s="12" t="s">
         <v>212</v>
@@ -10802,7 +10802,7 @@
         <v>223</v>
       </c>
       <c r="H119" s="11" t="s">
-        <v>498</v>
+        <v>484</v>
       </c>
       <c r="I119" s="11" t="s">
         <v>211</v>
@@ -10855,7 +10855,7 @@
         <v>15</v>
       </c>
       <c r="E120" s="30" t="s">
-        <v>626</v>
+        <v>612</v>
       </c>
       <c r="F120" s="12" t="s">
         <v>213</v>
@@ -10864,7 +10864,7 @@
         <v>224</v>
       </c>
       <c r="H120" s="11" t="s">
-        <v>499</v>
+        <v>485</v>
       </c>
       <c r="I120" s="11" t="s">
         <v>211</v>
@@ -10917,16 +10917,16 @@
         <v>15</v>
       </c>
       <c r="E121" s="30" t="s">
-        <v>634</v>
+        <v>620</v>
       </c>
       <c r="F121" s="7" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="G121" s="6" t="s">
-        <v>440</v>
+        <v>721</v>
       </c>
       <c r="H121" s="7" t="s">
-        <v>506</v>
+        <v>492</v>
       </c>
       <c r="I121" s="7" t="s">
         <v>5</v>
@@ -10935,20 +10935,20 @@
         <v>239</v>
       </c>
       <c r="K121" s="7" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="L121" s="7" t="s">
         <v>8</v>
       </c>
       <c r="M121" s="7" t="s">
-        <v>241</v>
+        <v>708</v>
       </c>
       <c r="N121" s="7" t="s">
-        <v>242</v>
+        <v>709</v>
       </c>
       <c r="O121" s="7"/>
       <c r="P121" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q121" s="6">
         <v>0</v>
@@ -10991,38 +10991,38 @@
         <v>2</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>650</v>
+        <v>636</v>
       </c>
       <c r="E122" s="30" t="s">
-        <v>636</v>
+        <v>622</v>
       </c>
       <c r="F122" s="33" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="G122" s="6" t="s">
-        <v>371</v>
+        <v>363</v>
       </c>
       <c r="H122" s="23" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="J122" s="7" t="s">
         <v>239</v>
       </c>
       <c r="K122" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="L122" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="M122" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="N122" s="7" t="s">
         <v>276</v>
-      </c>
-      <c r="L122" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="M122" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="N122" s="7" t="s">
-        <v>278</v>
       </c>
       <c r="O122" s="7"/>
       <c r="P122" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q122" s="6">
         <v>0</v>
@@ -11051,38 +11051,38 @@
         <v>2</v>
       </c>
       <c r="D123" s="6" t="s">
-        <v>650</v>
+        <v>636</v>
       </c>
       <c r="E123" s="30" t="s">
-        <v>637</v>
+        <v>623</v>
       </c>
       <c r="F123" s="33" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="G123" s="6" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="H123" s="23" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="J123" s="7" t="s">
         <v>239</v>
       </c>
       <c r="K123" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="L123" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="M123" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="N123" s="7" t="s">
         <v>276</v>
-      </c>
-      <c r="L123" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="M123" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="N123" s="7" t="s">
-        <v>278</v>
       </c>
       <c r="O123" s="7"/>
       <c r="P123" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q123" s="6">
         <v>0</v>
@@ -11111,38 +11111,38 @@
         <v>2</v>
       </c>
       <c r="D124" s="6" t="s">
-        <v>650</v>
+        <v>636</v>
       </c>
       <c r="E124" s="30" t="s">
-        <v>638</v>
+        <v>624</v>
       </c>
       <c r="F124" s="33" t="s">
+        <v>279</v>
+      </c>
+      <c r="G124" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="H124" s="23" t="s">
         <v>281</v>
-      </c>
-      <c r="G124" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="H124" s="23" t="s">
-        <v>283</v>
       </c>
       <c r="J124" s="7" t="s">
         <v>239</v>
       </c>
       <c r="K124" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="L124" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="M124" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="N124" s="7" t="s">
         <v>276</v>
-      </c>
-      <c r="L124" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="M124" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="N124" s="7" t="s">
-        <v>278</v>
       </c>
       <c r="O124" s="7"/>
       <c r="P124" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q124" s="6">
         <v>0</v>
@@ -11171,39 +11171,39 @@
         <v>2</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>650</v>
+        <v>636</v>
       </c>
       <c r="E125" s="30" t="s">
-        <v>639</v>
+        <v>625</v>
       </c>
       <c r="F125" s="33" t="s">
+        <v>282</v>
+      </c>
+      <c r="G125" s="6" t="s">
+        <v>283</v>
+      </c>
+      <c r="H125" s="23" t="s">
         <v>284</v>
-      </c>
-      <c r="G125" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="H125" s="23" t="s">
-        <v>286</v>
       </c>
       <c r="I125" s="23"/>
       <c r="J125" s="7" t="s">
         <v>239</v>
       </c>
       <c r="K125" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="L125" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="M125" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="N125" s="7" t="s">
         <v>276</v>
-      </c>
-      <c r="L125" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="M125" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="N125" s="7" t="s">
-        <v>278</v>
       </c>
       <c r="O125" s="7"/>
       <c r="P125" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q125" s="6">
         <v>0</v>
@@ -11246,39 +11246,39 @@
         <v>2</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>650</v>
+        <v>636</v>
       </c>
       <c r="E126" s="30" t="s">
-        <v>640</v>
+        <v>626</v>
       </c>
       <c r="F126" s="33" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="G126" s="6" t="s">
-        <v>466</v>
+        <v>452</v>
       </c>
       <c r="H126" s="23" t="s">
-        <v>465</v>
+        <v>451</v>
       </c>
       <c r="I126" s="23"/>
       <c r="J126" s="7" t="s">
         <v>239</v>
       </c>
       <c r="K126" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="L126" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="M126" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="N126" s="7" t="s">
         <v>276</v>
-      </c>
-      <c r="L126" s="7" t="s">
-        <v>300</v>
-      </c>
-      <c r="M126" s="7" t="s">
-        <v>277</v>
-      </c>
-      <c r="N126" s="7" t="s">
-        <v>278</v>
       </c>
       <c r="O126" s="7"/>
       <c r="P126" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q126" s="6">
         <v>0</v>
@@ -11321,38 +11321,38 @@
         <v>2</v>
       </c>
       <c r="D127" s="6" t="s">
-        <v>650</v>
+        <v>636</v>
       </c>
       <c r="E127" s="30" t="s">
-        <v>641</v>
+        <v>627</v>
       </c>
       <c r="F127" s="33" t="s">
+        <v>286</v>
+      </c>
+      <c r="G127" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="H127" s="23" t="s">
         <v>288</v>
-      </c>
-      <c r="G127" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="H127" s="23" t="s">
-        <v>290</v>
       </c>
       <c r="I127" s="23"/>
       <c r="J127" s="7" t="s">
         <v>239</v>
       </c>
       <c r="K127" s="7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="L127" s="7" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="M127" s="7" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="N127" s="7" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="P127" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q127" s="6">
         <v>0</v>
@@ -11395,19 +11395,19 @@
         <v>2</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>650</v>
+        <v>636</v>
       </c>
       <c r="E128" s="32" t="s">
-        <v>642</v>
+        <v>628</v>
       </c>
       <c r="F128" s="33" t="s">
+        <v>290</v>
+      </c>
+      <c r="G128" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="H128" s="7" t="s">
         <v>292</v>
-      </c>
-      <c r="G128" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="H128" s="7" t="s">
-        <v>294</v>
       </c>
       <c r="I128" s="23" t="s">
         <v>5</v>
@@ -11419,17 +11419,17 @@
         <v>2017</v>
       </c>
       <c r="L128" s="7" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="M128" s="7" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="N128" s="7" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="O128" s="7"/>
       <c r="P128" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="Q128" s="6">
         <v>0</v>
@@ -11475,15 +11475,15 @@
         <v>3</v>
       </c>
       <c r="E129" s="32" t="s">
-        <v>702</v>
+        <v>688</v>
       </c>
       <c r="F129" s="33" t="s">
-        <v>703</v>
+        <v>689</v>
       </c>
       <c r="G129" s="36"/>
       <c r="H129" s="37"/>
       <c r="I129" s="23" t="s">
-        <v>718</v>
+        <v>704</v>
       </c>
       <c r="J129" s="7" t="s">
         <v>6</v>
@@ -11548,15 +11548,15 @@
         <v>3</v>
       </c>
       <c r="E130" s="32" t="s">
-        <v>704</v>
+        <v>690</v>
       </c>
       <c r="F130" s="33" t="s">
-        <v>705</v>
+        <v>691</v>
       </c>
       <c r="G130" s="36"/>
       <c r="H130" s="37"/>
       <c r="I130" s="23" t="s">
-        <v>718</v>
+        <v>704</v>
       </c>
       <c r="J130" s="7" t="s">
         <v>6</v>
@@ -11621,15 +11621,15 @@
         <v>3</v>
       </c>
       <c r="E131" s="32" t="s">
-        <v>706</v>
+        <v>692</v>
       </c>
       <c r="F131" s="33" t="s">
-        <v>707</v>
+        <v>693</v>
       </c>
       <c r="G131" s="36"/>
       <c r="H131" s="37"/>
       <c r="I131" s="23" t="s">
-        <v>718</v>
+        <v>704</v>
       </c>
       <c r="J131" s="7" t="s">
         <v>6</v>
@@ -11694,10 +11694,10 @@
         <v>3</v>
       </c>
       <c r="E132" s="32" t="s">
-        <v>708</v>
+        <v>694</v>
       </c>
       <c r="F132" s="33" t="s">
-        <v>709</v>
+        <v>695</v>
       </c>
       <c r="G132" s="36"/>
       <c r="H132" s="37"/>
@@ -11767,10 +11767,10 @@
         <v>3</v>
       </c>
       <c r="E133" s="32" t="s">
-        <v>710</v>
+        <v>696</v>
       </c>
       <c r="F133" s="33" t="s">
-        <v>711</v>
+        <v>697</v>
       </c>
       <c r="G133" s="36"/>
       <c r="H133" s="37"/>
@@ -11840,10 +11840,10 @@
         <v>3</v>
       </c>
       <c r="E134" s="32" t="s">
-        <v>712</v>
+        <v>698</v>
       </c>
       <c r="F134" s="33" t="s">
-        <v>713</v>
+        <v>699</v>
       </c>
       <c r="G134" s="36"/>
       <c r="H134" s="37"/>
@@ -11913,10 +11913,10 @@
         <v>3</v>
       </c>
       <c r="E135" s="32" t="s">
-        <v>714</v>
+        <v>700</v>
       </c>
       <c r="F135" s="33" t="s">
-        <v>715</v>
+        <v>701</v>
       </c>
       <c r="G135" s="36"/>
       <c r="H135" s="37"/>
@@ -11986,10 +11986,10 @@
         <v>3</v>
       </c>
       <c r="E136" s="32" t="s">
-        <v>716</v>
+        <v>702</v>
       </c>
       <c r="F136" s="33" t="s">
-        <v>717</v>
+        <v>703</v>
       </c>
       <c r="G136" s="36"/>
       <c r="H136" s="37"/>
@@ -12123,7 +12123,7 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
       <c r="A2" s="26" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>175</v>
@@ -12131,7 +12131,7 @@
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1">
       <c r="A3" s="26" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>177</v>
@@ -12139,7 +12139,7 @@
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1">
       <c r="A4" s="26" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>176</v>
@@ -12147,7 +12147,7 @@
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1">
       <c r="A5" s="26" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>178</v>
@@ -12155,15 +12155,15 @@
     </row>
     <row r="6" spans="1:2" ht="17.25" customHeight="1">
       <c r="A6" s="26" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>179</v>
@@ -12171,7 +12171,7 @@
     </row>
     <row r="8" spans="1:2" ht="17.25" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>180</v>
@@ -12179,7 +12179,7 @@
     </row>
     <row r="9" spans="1:2" ht="17.25" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>181</v>
@@ -12187,7 +12187,7 @@
     </row>
     <row r="10" spans="1:2" ht="17.25" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>182</v>
@@ -12195,7 +12195,7 @@
     </row>
     <row r="11" spans="1:2" ht="17.25" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>183</v>
@@ -12203,7 +12203,7 @@
     </row>
     <row r="12" spans="1:2" ht="17.25" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>184</v>
@@ -12211,7 +12211,7 @@
     </row>
     <row r="13" spans="1:2" ht="17.25" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>185</v>
@@ -12219,7 +12219,7 @@
     </row>
     <row r="14" spans="1:2" ht="17.25" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>186</v>
@@ -12227,7 +12227,7 @@
     </row>
     <row r="15" spans="1:2" ht="17.25" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>187</v>
@@ -12235,7 +12235,7 @@
     </row>
     <row r="16" spans="1:2" ht="17.25" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>188</v>
@@ -12243,42 +12243,42 @@
     </row>
     <row r="17" spans="1:2" ht="17.25" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>688</v>
+        <v>674</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>695</v>
+        <v>681</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="17.25" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>693</v>
+        <v>679</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>694</v>
+        <v>680</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="17.25" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>696</v>
+        <v>682</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>699</v>
+        <v>685</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="17.25" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>697</v>
+        <v>683</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>700</v>
+        <v>686</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="17.25" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>698</v>
+        <v>684</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>701</v>
+        <v>687</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="17.25" customHeight="1">

</xml_diff>

<commit_message>
Act bases (SINADI-MSP datos 2020).
</commit_message>
<xml_diff>
--- a/Data/Base_fichas_indicadores.xlsx
+++ b/Data/Base_fichas_indicadores.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1976" uniqueCount="722">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1992" uniqueCount="738">
   <si>
     <t>id</t>
   </si>
@@ -2190,6 +2190,54 @@
   </si>
   <si>
     <t>El indicador mide el porcentaje partos registrados en el período anual considerado que requirieron la realización de cesárea. El Total SNIS es el promedio ponderado por cantidad de afiliados de cada tipo de prestador.</t>
+  </si>
+  <si>
+    <t>El indicador mide la cantidad de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares en los que alguno de sus integrantes es beneficiario de Asignaciones Familiares contributivas.</t>
+  </si>
+  <si>
+    <t>Para cada año calcular: Cantidad de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares en los que alguno de sus integrantes es beneficiario de Asignaciones Familiares contributivas.</t>
+  </si>
+  <si>
+    <t>El indicador mide la cantidad de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares en los que alguno de sus integrantes es beneficiario de Asignaciones Familiares - Plan de Equidad.</t>
+  </si>
+  <si>
+    <t>Para cada año calcular: Cantidad de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares en los que alguno de sus integrantes es beneficiario de Asignaciones Familiares - Plan de Equidad</t>
+  </si>
+  <si>
+    <t>El indicador mide la cantidad de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares en los que alguno de sus integrantes es beneficiario de Tarjeta Uruguay Social.</t>
+  </si>
+  <si>
+    <t>Para cada año calcular: Cantidad de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares en los que alguno de sus integrantes es beneficiario de Tarjeta Uruguay Social</t>
+  </si>
+  <si>
+    <t>El indicador mide el porcentaje de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares en los que ningún integrante percibe Asignaciones Familaires - Plan de Equidad en el total de hogares pobres</t>
+  </si>
+  <si>
+    <t>Para cada año calcular: (Cantidad de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares en los que ninguno de sus integrantes es beneficiario de Asignaciones Familiares - Plan de Equidad/Cantidad de niños, niñas y adolescentes que residen en hogares pobres)*100</t>
+  </si>
+  <si>
+    <t>El indicador mide el porcentaje de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares en los que ningún integrante percibe Tarjeta Uruguay Social en el total de hogares pobres</t>
+  </si>
+  <si>
+    <t>Para cada año calcular: (Cantidad de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares en los que ninguno de sus integrantes es beneficiario de Tarjeta Uruguay Social/Cantidad de niños, niñas y adolescentes que residen en hogares pobres)*100</t>
+  </si>
+  <si>
+    <t>El indicador mide el porcentaje de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares en los que ningún integrante percibe Asignaciones Familaires - Plan de Equidad ni Tarjeta Uruguay Social en el total de hogares pobres</t>
+  </si>
+  <si>
+    <t>Para cada año calcular: (Cantidad de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares en los que ninguno de sus integrantes es beneficiario de Asignaciones Familiares - Plan de Equidad ni Tarjeta Uruguay Social/Cantidad de niños, niñas y adolescentes que residen en hogares pobres)*100</t>
+  </si>
+  <si>
+    <t>El indicador mide el porcentaje de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares cuyo jefe/a y/o cónyuge están desocupados sin seguro de desempleo</t>
+  </si>
+  <si>
+    <t>Para cada año calcular: (Cantidad de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares cuyo jefe/a y/o cónyuge están desocupados sin seguro de desempleo/Cantidad de niños, niñas y adolescentes)*100</t>
+  </si>
+  <si>
+    <t>El indicador mide el porcentaje de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares cuyo jefe/a y/o cónyuge están ocupados y no aportan a la seguridad social</t>
+  </si>
+  <si>
+    <t>Para cada año calcular: (Cantidad de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares cuyo jefe/a y/o cónyuge están ocupados y no aportan a la seguridad social/Cantidad de niños, niñas y adolescentes)*100</t>
   </si>
 </sst>
 </file>
@@ -2200,11 +2248,18 @@
     <numFmt numFmtId="164" formatCode="#,##0.000&quot;&quot;;\-#,##0.000&quot;&quot;"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -2276,18 +2331,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -2301,113 +2350,110 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2730,10 +2776,10 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AI140"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="J1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E111" sqref="E111"/>
-      <selection pane="bottomLeft" activeCell="M99" sqref="M99"/>
+      <selection pane="bottomLeft" activeCell="A129" sqref="A129:P136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -11477,11 +11523,15 @@
       <c r="E129" s="32" t="s">
         <v>688</v>
       </c>
-      <c r="F129" s="33" t="s">
+      <c r="F129" s="36" t="s">
         <v>689</v>
       </c>
-      <c r="G129" s="36"/>
-      <c r="H129" s="37"/>
+      <c r="G129" s="6" t="s">
+        <v>722</v>
+      </c>
+      <c r="H129" s="7" t="s">
+        <v>723</v>
+      </c>
       <c r="I129" s="23" t="s">
         <v>704</v>
       </c>
@@ -11550,11 +11600,15 @@
       <c r="E130" s="32" t="s">
         <v>690</v>
       </c>
-      <c r="F130" s="33" t="s">
+      <c r="F130" s="36" t="s">
         <v>691</v>
       </c>
-      <c r="G130" s="36"/>
-      <c r="H130" s="37"/>
+      <c r="G130" s="6" t="s">
+        <v>724</v>
+      </c>
+      <c r="H130" s="7" t="s">
+        <v>725</v>
+      </c>
       <c r="I130" s="23" t="s">
         <v>704</v>
       </c>
@@ -11623,11 +11677,15 @@
       <c r="E131" s="32" t="s">
         <v>692</v>
       </c>
-      <c r="F131" s="33" t="s">
+      <c r="F131" s="36" t="s">
         <v>693</v>
       </c>
-      <c r="G131" s="36"/>
-      <c r="H131" s="37"/>
+      <c r="G131" s="6" t="s">
+        <v>726</v>
+      </c>
+      <c r="H131" s="7" t="s">
+        <v>727</v>
+      </c>
       <c r="I131" s="23" t="s">
         <v>704</v>
       </c>
@@ -11696,11 +11754,15 @@
       <c r="E132" s="32" t="s">
         <v>694</v>
       </c>
-      <c r="F132" s="33" t="s">
+      <c r="F132" s="36" t="s">
         <v>695</v>
       </c>
-      <c r="G132" s="36"/>
-      <c r="H132" s="37"/>
+      <c r="G132" s="6" t="s">
+        <v>728</v>
+      </c>
+      <c r="H132" s="7" t="s">
+        <v>729</v>
+      </c>
       <c r="I132" s="23" t="s">
         <v>5</v>
       </c>
@@ -11769,11 +11831,15 @@
       <c r="E133" s="32" t="s">
         <v>696</v>
       </c>
-      <c r="F133" s="33" t="s">
+      <c r="F133" s="36" t="s">
         <v>697</v>
       </c>
-      <c r="G133" s="36"/>
-      <c r="H133" s="37"/>
+      <c r="G133" s="6" t="s">
+        <v>730</v>
+      </c>
+      <c r="H133" s="7" t="s">
+        <v>731</v>
+      </c>
       <c r="I133" s="23" t="s">
         <v>5</v>
       </c>
@@ -11842,11 +11908,15 @@
       <c r="E134" s="32" t="s">
         <v>698</v>
       </c>
-      <c r="F134" s="33" t="s">
+      <c r="F134" s="36" t="s">
         <v>699</v>
       </c>
-      <c r="G134" s="36"/>
-      <c r="H134" s="37"/>
+      <c r="G134" s="6" t="s">
+        <v>732</v>
+      </c>
+      <c r="H134" s="7" t="s">
+        <v>733</v>
+      </c>
       <c r="I134" s="23" t="s">
         <v>5</v>
       </c>
@@ -11915,11 +11985,15 @@
       <c r="E135" s="32" t="s">
         <v>700</v>
       </c>
-      <c r="F135" s="33" t="s">
+      <c r="F135" s="36" t="s">
         <v>701</v>
       </c>
-      <c r="G135" s="36"/>
-      <c r="H135" s="37"/>
+      <c r="G135" s="6" t="s">
+        <v>734</v>
+      </c>
+      <c r="H135" s="7" t="s">
+        <v>735</v>
+      </c>
       <c r="I135" s="23" t="s">
         <v>5</v>
       </c>
@@ -11988,11 +12062,15 @@
       <c r="E136" s="32" t="s">
         <v>702</v>
       </c>
-      <c r="F136" s="33" t="s">
+      <c r="F136" s="36" t="s">
         <v>703</v>
       </c>
-      <c r="G136" s="36"/>
-      <c r="H136" s="37"/>
+      <c r="G136" s="6" t="s">
+        <v>736</v>
+      </c>
+      <c r="H136" s="7" t="s">
+        <v>737</v>
+      </c>
       <c r="I136" s="23" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Cambio nomindicador Cobertura Vacunacion
</commit_message>
<xml_diff>
--- a/Data/Base_fichas_indicadores.xlsx
+++ b/Data/Base_fichas_indicadores.xlsx
@@ -959,12 +959,6 @@
     <t>WHO and UNICEF estimates of immunization coverage (2019 revision)</t>
   </si>
   <si>
-    <t>Para cada año calcular: (Cantidad de nacidos vivos -o niños y niñas- inmunizados según tipo de vacuna / Total de nacidos vivos -o niños y niñas-)*100</t>
-  </si>
-  <si>
-    <t>Porcentaje de nacidos vivos o niños inmunizados según tipo de vacuna y dosis (estimación OMS - UNICEF)</t>
-  </si>
-  <si>
     <t>No es un gasto soportable en vivienda aquel cuya erogación tiene como consecuencia que una persona se ubique debajo de la línea de pobreza monetaria.</t>
   </si>
   <si>
@@ -2238,6 +2232,12 @@
   </si>
   <si>
     <t>Para cada año calcular: (Cantidad de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares cuyo jefe/a y/o cónyuge están ocupados y no aportan a la seguridad social/Cantidad de niños, niñas y adolescentes)*100</t>
+  </si>
+  <si>
+    <t>Porcentaje de niños y niñas inmunizados según tipo de vacuna y dosis (estimación OMS - UNICEF)</t>
+  </si>
+  <si>
+    <t>Para cada año calcular: (Cantidad de niños y niñas inmunizados según tipo de vacuna / Total de niños y niñas)*100</t>
   </si>
 </sst>
 </file>
@@ -2776,10 +2776,10 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AI140"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="D1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E111" sqref="E111"/>
-      <selection pane="bottomLeft" activeCell="A129" sqref="A129:P136"/>
+      <selection pane="bottomLeft" activeCell="F91" sqref="F91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2812,67 +2812,67 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="26" t="s">
+        <v>345</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1" s="26" t="s">
         <v>347</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>348</v>
-      </c>
-      <c r="C1" s="26" t="s">
+      <c r="D1" s="26" t="s">
+        <v>360</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>515</v>
+      </c>
+      <c r="F1" s="26" t="s">
         <v>349</v>
       </c>
-      <c r="D1" s="26" t="s">
-        <v>362</v>
-      </c>
-      <c r="E1" s="30" t="s">
-        <v>517</v>
-      </c>
-      <c r="F1" s="26" t="s">
+      <c r="G1" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>356</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>359</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>361</v>
-      </c>
       <c r="Q1" s="26" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="R1" s="13" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="S1" s="35" t="s">
+        <v>703</v>
+      </c>
+      <c r="T1" s="35" t="s">
+        <v>704</v>
+      </c>
+      <c r="U1" s="35" t="s">
         <v>705</v>
-      </c>
-      <c r="T1" s="35" t="s">
-        <v>706</v>
-      </c>
-      <c r="U1" s="35" t="s">
-        <v>707</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="6" customFormat="1">
@@ -2889,13 +2889,13 @@
         <v>104</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="F2" s="31" t="s">
         <v>80</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>114</v>
@@ -2907,16 +2907,16 @@
         <v>6</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="P2" s="6" t="s">
         <v>17</v>
@@ -2951,13 +2951,13 @@
         <v>104</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F3" s="31" t="s">
         <v>81</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>113</v>
@@ -2969,16 +2969,16 @@
         <v>6</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>17</v>
@@ -3013,13 +3013,13 @@
         <v>104</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="F4" s="31" t="s">
         <v>82</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>116</v>
@@ -3031,16 +3031,16 @@
         <v>6</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="L4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="P4" s="6" t="s">
         <v>17</v>
@@ -3075,13 +3075,13 @@
         <v>104</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>76</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>112</v>
@@ -3099,10 +3099,10 @@
         <v>8</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="N5" s="6" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="P5" s="6" t="s">
         <v>17</v>
@@ -3137,16 +3137,16 @@
         <v>104</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>79</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>5</v>
@@ -3161,10 +3161,10 @@
         <v>8</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="P6" s="6" t="s">
         <v>25</v>
@@ -3199,16 +3199,16 @@
         <v>104</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>78</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>5</v>
@@ -3223,10 +3223,10 @@
         <v>8</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="N7" s="6" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="P7" s="6" t="s">
         <v>25</v>
@@ -3261,13 +3261,13 @@
         <v>104</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>83</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>115</v>
@@ -3285,10 +3285,10 @@
         <v>8</v>
       </c>
       <c r="M8" s="6" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="N8" s="6" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="P8" s="6" t="s">
         <v>25</v>
@@ -3323,13 +3323,13 @@
         <v>104</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>84</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>30</v>
@@ -3347,10 +3347,10 @@
         <v>8</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="P9" s="6" t="s">
         <v>85</v>
@@ -3385,13 +3385,13 @@
         <v>104</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>88</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>86</v>
@@ -3409,10 +3409,10 @@
         <v>8</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="N10" s="6" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="P10" s="6" t="s">
         <v>85</v>
@@ -3447,13 +3447,13 @@
         <v>104</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>89</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>90</v>
@@ -3471,10 +3471,10 @@
         <v>8</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="N11" s="6" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="P11" s="6" t="s">
         <v>85</v>
@@ -3509,16 +3509,16 @@
         <v>104</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>454</v>
+        <v>452</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>33</v>
@@ -3533,13 +3533,13 @@
         <v>8</v>
       </c>
       <c r="M12" s="6" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="N12" s="6" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="P12" s="6" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="Q12" s="6">
         <v>0</v>
@@ -3571,13 +3571,13 @@
         <v>104</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>92</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>297</v>
@@ -3595,7 +3595,7 @@
         <v>8</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="N13" s="6" t="s">
         <v>13</v>
@@ -3633,13 +3633,13 @@
         <v>104</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>97</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>28</v>
@@ -3657,10 +3657,10 @@
         <v>298</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="P14" s="6" t="s">
         <v>96</v>
@@ -3695,16 +3695,16 @@
         <v>305</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>307</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>455</v>
+        <v>453</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>5</v>
@@ -3757,16 +3757,16 @@
         <v>305</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>306</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>456</v>
+        <v>454</v>
       </c>
       <c r="I16" s="7" t="s">
         <v>5</v>
@@ -3819,16 +3819,16 @@
         <v>305</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>304</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="I17" s="7" t="s">
         <v>5</v>
@@ -3881,13 +3881,13 @@
         <v>3</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="F18" s="13" t="s">
         <v>4</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="H18" s="14" t="s">
         <v>139</v>
@@ -3914,7 +3914,7 @@
         <v>10</v>
       </c>
       <c r="P18" s="13" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="Q18" s="6">
         <v>1</v>
@@ -3946,13 +3946,13 @@
         <v>3</v>
       </c>
       <c r="E19" s="30" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="F19" s="13" t="s">
         <v>100</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="H19" s="14" t="s">
         <v>140</v>
@@ -3979,7 +3979,7 @@
         <v>11</v>
       </c>
       <c r="P19" s="13" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="Q19" s="6">
         <v>1</v>
@@ -4011,13 +4011,13 @@
         <v>3</v>
       </c>
       <c r="E20" s="30" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="F20" s="13" t="s">
         <v>102</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="H20" s="14" t="s">
         <v>141</v>
@@ -4044,7 +4044,7 @@
         <v>11</v>
       </c>
       <c r="P20" s="13" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="Q20" s="6">
         <v>0</v>
@@ -4076,13 +4076,13 @@
         <v>3</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="F21" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="H21" s="13" t="s">
         <v>148</v>
@@ -4109,7 +4109,7 @@
         <v>10</v>
       </c>
       <c r="P21" s="13" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="Q21" s="6">
         <v>0</v>
@@ -4155,13 +4155,13 @@
         <v>3</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="H22" s="13" t="s">
         <v>149</v>
@@ -4188,7 +4188,7 @@
         <v>10</v>
       </c>
       <c r="P22" s="13" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="Q22" s="6">
         <v>0</v>
@@ -4234,13 +4234,13 @@
         <v>3</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="F23" s="13" t="s">
         <v>20</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H23" s="13" t="s">
         <v>150</v>
@@ -4267,7 +4267,7 @@
         <v>10</v>
       </c>
       <c r="P23" s="13" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="Q23" s="6">
         <v>0</v>
@@ -4299,13 +4299,13 @@
         <v>3</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="F24" s="15" t="s">
         <v>299</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H24" s="15" t="s">
         <v>300</v>
@@ -4332,7 +4332,7 @@
         <v>234</v>
       </c>
       <c r="P24" s="13" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="Q24" s="6">
         <v>0</v>
@@ -4378,13 +4378,13 @@
         <v>3</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="F25" s="15" t="s">
         <v>236</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H25" s="15" t="s">
         <v>235</v>
@@ -4411,7 +4411,7 @@
         <v>234</v>
       </c>
       <c r="P25" s="13" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="Q25" s="6">
         <v>1</v>
@@ -4457,13 +4457,13 @@
         <v>12</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>98</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="H26" s="6" t="s">
         <v>142</v>
@@ -4481,16 +4481,16 @@
         <v>8</v>
       </c>
       <c r="M26" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="N26" s="6" t="s">
         <v>507</v>
-      </c>
-      <c r="N26" s="6" t="s">
-        <v>509</v>
       </c>
       <c r="O26" s="6" t="s">
         <v>14</v>
       </c>
       <c r="P26" s="6" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="Q26" s="6">
         <v>0</v>
@@ -4522,13 +4522,13 @@
         <v>12</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>73</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H27" s="6" t="s">
         <v>143</v>
@@ -4546,16 +4546,16 @@
         <v>8</v>
       </c>
       <c r="M27" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="N27" s="6" t="s">
         <v>507</v>
-      </c>
-      <c r="N27" s="6" t="s">
-        <v>509</v>
       </c>
       <c r="O27" s="6" t="s">
         <v>14</v>
       </c>
       <c r="P27" s="6" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="Q27" s="6">
         <v>0</v>
@@ -4601,13 +4601,13 @@
         <v>12</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>99</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H28" s="6" t="s">
         <v>151</v>
@@ -4625,16 +4625,16 @@
         <v>8</v>
       </c>
       <c r="M28" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="N28" s="6" t="s">
         <v>507</v>
-      </c>
-      <c r="N28" s="6" t="s">
-        <v>509</v>
       </c>
       <c r="O28" s="6" t="s">
         <v>14</v>
       </c>
       <c r="P28" s="6" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="Q28" s="6">
         <v>0</v>
@@ -4680,16 +4680,16 @@
         <v>12</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="F29" s="13" t="s">
         <v>101</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="I29" s="13" t="s">
         <v>5</v>
@@ -4704,16 +4704,16 @@
         <v>8</v>
       </c>
       <c r="M29" s="13" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="N29" s="13" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="O29" s="13" t="s">
         <v>21</v>
       </c>
       <c r="P29" s="13" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="Q29" s="6">
         <v>0</v>
@@ -4745,16 +4745,16 @@
         <v>12</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="F30" s="13" t="s">
         <v>103</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="I30" s="13" t="s">
         <v>5</v>
@@ -4769,16 +4769,16 @@
         <v>8</v>
       </c>
       <c r="M30" s="13" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="N30" s="13" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="O30" s="13" t="s">
         <v>21</v>
       </c>
       <c r="P30" s="13" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="Q30" s="6">
         <v>0</v>
@@ -4824,13 +4824,13 @@
         <v>15</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>108</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="H31" s="13" t="s">
         <v>144</v>
@@ -4848,10 +4848,10 @@
         <v>16</v>
       </c>
       <c r="M31" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="N31" s="6" t="s">
         <v>507</v>
-      </c>
-      <c r="N31" s="6" t="s">
-        <v>509</v>
       </c>
       <c r="O31" s="16"/>
       <c r="P31" s="13" t="s">
@@ -4901,13 +4901,13 @@
         <v>15</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>109</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="H32" s="13" t="s">
         <v>145</v>
@@ -4925,10 +4925,10 @@
         <v>16</v>
       </c>
       <c r="M32" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="N32" s="6" t="s">
         <v>507</v>
-      </c>
-      <c r="N32" s="6" t="s">
-        <v>509</v>
       </c>
       <c r="O32" s="16"/>
       <c r="P32" s="13" t="s">
@@ -4978,13 +4978,13 @@
         <v>15</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>107</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="H33" s="13" t="s">
         <v>146</v>
@@ -5002,10 +5002,10 @@
         <v>16</v>
       </c>
       <c r="M33" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="N33" s="6" t="s">
         <v>507</v>
-      </c>
-      <c r="N33" s="6" t="s">
-        <v>509</v>
       </c>
       <c r="O33" s="16"/>
       <c r="P33" s="13" t="s">
@@ -5041,13 +5041,13 @@
         <v>15</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>110</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="H34" s="13" t="s">
         <v>147</v>
@@ -5065,10 +5065,10 @@
         <v>16</v>
       </c>
       <c r="M34" s="6" t="s">
+        <v>505</v>
+      </c>
+      <c r="N34" s="6" t="s">
         <v>507</v>
-      </c>
-      <c r="N34" s="6" t="s">
-        <v>509</v>
       </c>
       <c r="O34" s="6" t="s">
         <v>105</v>
@@ -5120,13 +5120,13 @@
         <v>15</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>22</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="H35" s="6" t="s">
         <v>152</v>
@@ -5185,13 +5185,13 @@
         <v>3</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="F36" s="13" t="s">
         <v>74</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="H36" s="13" t="s">
         <v>153</v>
@@ -5218,7 +5218,7 @@
         <v>75</v>
       </c>
       <c r="P36" s="13" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="Q36" s="6">
         <v>0</v>
@@ -5250,13 +5250,13 @@
         <v>104</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="F37" s="31" t="s">
         <v>118</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="H37" s="6" t="s">
         <v>119</v>
@@ -5268,16 +5268,16 @@
         <v>6</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="L37" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M37" s="6" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="P37" s="6" t="s">
         <v>17</v>
@@ -5312,13 +5312,13 @@
         <v>104</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="F38" s="31" t="s">
         <v>120</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H38" s="6" t="s">
         <v>121</v>
@@ -5336,10 +5336,10 @@
         <v>8</v>
       </c>
       <c r="M38" s="6" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="N38" s="6" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="P38" s="6" t="s">
         <v>17</v>
@@ -5374,16 +5374,16 @@
         <v>104</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="F39" s="31" t="s">
         <v>122</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="I39" s="6" t="s">
         <v>5</v>
@@ -5392,16 +5392,16 @@
         <v>6</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="L39" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M39" s="6" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="N39" s="6" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="P39" s="6" t="s">
         <v>17</v>
@@ -5436,13 +5436,13 @@
         <v>104</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>123</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="H40" s="6" t="s">
         <v>124</v>
@@ -5460,10 +5460,10 @@
         <v>8</v>
       </c>
       <c r="M40" s="6" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="N40" s="6" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="P40" s="6" t="s">
         <v>17</v>
@@ -5498,19 +5498,19 @@
         <v>104</v>
       </c>
       <c r="E41" s="30" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="F41" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>441</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="I41" s="6" t="s">
         <v>320</v>
-      </c>
-      <c r="G41" s="6" t="s">
-        <v>443</v>
-      </c>
-      <c r="H41" s="6" t="s">
-        <v>321</v>
-      </c>
-      <c r="I41" s="6" t="s">
-        <v>322</v>
       </c>
       <c r="J41" s="6" t="s">
         <v>6</v>
@@ -5522,14 +5522,14 @@
         <v>8</v>
       </c>
       <c r="M41" s="24" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="N41" s="6" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="O41" s="6"/>
       <c r="P41" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="Q41" s="6">
         <v>0</v>
@@ -5575,38 +5575,38 @@
         <v>104</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="F42" s="24" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="J42" s="6" t="s">
         <v>6</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="L42" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M42" s="24" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="N42" s="6" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="O42" s="25"/>
       <c r="P42" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="Q42" s="6">
         <v>0</v>
@@ -5652,38 +5652,38 @@
         <v>104</v>
       </c>
       <c r="E43" s="30" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="F43" s="24" t="s">
+        <v>329</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="H43" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="G43" s="6" t="s">
-        <v>332</v>
-      </c>
-      <c r="H43" s="6" t="s">
-        <v>333</v>
-      </c>
       <c r="I43" s="6" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="J43" s="6" t="s">
         <v>6</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="L43" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M43" s="24" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="N43" s="6" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="O43" s="25"/>
       <c r="P43" s="6" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="Q43" s="6">
         <v>0</v>
@@ -5729,13 +5729,13 @@
         <v>36</v>
       </c>
       <c r="E44" s="30" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="F44" s="13" t="s">
         <v>37</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="H44" s="13" t="s">
         <v>38</v>
@@ -5762,7 +5762,7 @@
         <v>40</v>
       </c>
       <c r="P44" s="13" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="Q44" s="6">
         <v>1</v>
@@ -5808,13 +5808,13 @@
         <v>41</v>
       </c>
       <c r="E45" s="32" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="F45" s="13" t="s">
         <v>42</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>445</v>
+        <v>443</v>
       </c>
       <c r="H45" s="13" t="s">
         <v>154</v>
@@ -5841,7 +5841,7 @@
         <v>43</v>
       </c>
       <c r="P45" s="13" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="Q45" s="6">
         <v>0</v>
@@ -5887,13 +5887,13 @@
         <v>41</v>
       </c>
       <c r="E46" s="32" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="F46" s="13" t="s">
         <v>44</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="H46" s="13" t="s">
         <v>155</v>
@@ -5920,7 +5920,7 @@
         <v>45</v>
       </c>
       <c r="P46" s="13" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="Q46" s="6">
         <v>0</v>
@@ -5966,13 +5966,13 @@
         <v>41</v>
       </c>
       <c r="E47" s="32" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="H47" s="6" t="s">
         <v>189</v>
@@ -5996,10 +5996,10 @@
         <v>195</v>
       </c>
       <c r="O47" s="7" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="P47" s="6" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="Q47" s="6">
         <v>1</v>
@@ -6031,13 +6031,13 @@
         <v>41</v>
       </c>
       <c r="E48" s="32" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>161</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>446</v>
+        <v>444</v>
       </c>
       <c r="H48" s="13" t="s">
         <v>162</v>
@@ -6064,7 +6064,7 @@
         <v>163</v>
       </c>
       <c r="P48" s="13" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="Q48" s="6">
         <v>0</v>
@@ -6096,16 +6096,16 @@
         <v>46</v>
       </c>
       <c r="E49" s="32" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>447</v>
+        <v>445</v>
       </c>
       <c r="H49" s="27" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="I49" s="6" t="s">
         <v>5</v>
@@ -6126,10 +6126,10 @@
         <v>195</v>
       </c>
       <c r="O49" s="7" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="P49" s="6" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="Q49" s="6">
         <v>1</v>
@@ -6161,16 +6161,16 @@
         <v>46</v>
       </c>
       <c r="E50" s="32" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="H50" s="27" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="I50" s="6" t="s">
         <v>5</v>
@@ -6191,10 +6191,10 @@
         <v>195</v>
       </c>
       <c r="O50" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="P50" s="13" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="Q50" s="6">
         <v>0</v>
@@ -6240,16 +6240,16 @@
         <v>46</v>
       </c>
       <c r="E51" s="32" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="H51" s="27" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="I51" s="6" t="s">
         <v>5</v>
@@ -6270,10 +6270,10 @@
         <v>195</v>
       </c>
       <c r="O51" s="7" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="P51" s="13" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="Q51" s="6">
         <v>0</v>
@@ -6319,16 +6319,16 @@
         <v>46</v>
       </c>
       <c r="E52" s="32" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="F52" s="28" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="H52" s="27" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="I52" s="6" t="s">
         <v>5</v>
@@ -6349,10 +6349,10 @@
         <v>195</v>
       </c>
       <c r="O52" s="7" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="P52" s="13" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="Q52" s="6">
         <v>0</v>
@@ -6398,16 +6398,16 @@
         <v>47</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="F53" s="28" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="G53" s="28" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="H53" s="34" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="I53" s="6" t="s">
         <v>5</v>
@@ -6428,10 +6428,10 @@
         <v>195</v>
       </c>
       <c r="O53" s="7" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="P53" s="13" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="Q53" s="6">
         <v>1</v>
@@ -6477,13 +6477,13 @@
         <v>47</v>
       </c>
       <c r="E54" s="32" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="F54" s="13" t="s">
         <v>48</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="H54" s="13" t="s">
         <v>156</v>
@@ -6510,7 +6510,7 @@
         <v>49</v>
       </c>
       <c r="P54" s="13" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="Q54" s="6">
         <v>0</v>
@@ -6556,13 +6556,13 @@
         <v>50</v>
       </c>
       <c r="E55" s="32" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="F55" s="13" t="s">
         <v>51</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="H55" s="13" t="s">
         <v>157</v>
@@ -6587,7 +6587,7 @@
       </c>
       <c r="O55" s="13"/>
       <c r="P55" s="13" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="Q55" s="6">
         <v>1</v>
@@ -6633,13 +6633,13 @@
         <v>104</v>
       </c>
       <c r="E56" s="32" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="F56" s="31" t="s">
         <v>125</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="H56" s="6" t="s">
         <v>126</v>
@@ -6651,16 +6651,16 @@
         <v>6</v>
       </c>
       <c r="K56" s="6" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="L56" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M56" s="6" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="N56" s="6" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="P56" s="6" t="s">
         <v>17</v>
@@ -6695,13 +6695,13 @@
         <v>104</v>
       </c>
       <c r="E57" s="30" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="F57" s="31" t="s">
         <v>127</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="H57" s="6" t="s">
         <v>128</v>
@@ -6719,10 +6719,10 @@
         <v>8</v>
       </c>
       <c r="M57" s="6" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="N57" s="6" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="P57" s="6" t="s">
         <v>17</v>
@@ -6757,16 +6757,16 @@
         <v>104</v>
       </c>
       <c r="E58" s="30" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="F58" s="31" t="s">
         <v>129</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="I58" s="6" t="s">
         <v>5</v>
@@ -6775,16 +6775,16 @@
         <v>6</v>
       </c>
       <c r="K58" s="6" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="L58" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M58" s="6" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="N58" s="6" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="P58" s="6" t="s">
         <v>17</v>
@@ -6819,13 +6819,13 @@
         <v>104</v>
       </c>
       <c r="E59" s="30" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>130</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="H59" s="6" t="s">
         <v>131</v>
@@ -6843,10 +6843,10 @@
         <v>8</v>
       </c>
       <c r="M59" s="6" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="N59" s="6" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="P59" s="6" t="s">
         <v>17</v>
@@ -6881,13 +6881,13 @@
         <v>104</v>
       </c>
       <c r="E60" s="30" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>171</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H60" s="6" t="s">
         <v>170</v>
@@ -6905,10 +6905,10 @@
         <v>8</v>
       </c>
       <c r="M60" s="6" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="N60" s="6" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="P60" s="6" t="s">
         <v>17</v>
@@ -6943,13 +6943,13 @@
         <v>104</v>
       </c>
       <c r="E61" s="30" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>172</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H61" s="6" t="s">
         <v>173</v>
@@ -6967,10 +6967,10 @@
         <v>8</v>
       </c>
       <c r="M61" s="6" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="N61" s="6" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="P61" s="6" t="s">
         <v>17</v>
@@ -7005,13 +7005,13 @@
         <v>104</v>
       </c>
       <c r="E62" s="30" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H62" s="6" t="s">
         <v>174</v>
@@ -7029,10 +7029,10 @@
         <v>8</v>
       </c>
       <c r="M62" s="6" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="N62" s="6" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="P62" s="6" t="s">
         <v>17</v>
@@ -7067,13 +7067,13 @@
         <v>3</v>
       </c>
       <c r="E63" s="30" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="F63" s="6" t="s">
         <v>53</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="H63" s="6" t="s">
         <v>158</v>
@@ -7085,7 +7085,7 @@
         <v>6</v>
       </c>
       <c r="K63" s="6" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="L63" s="6" t="s">
         <v>8</v>
@@ -7132,13 +7132,13 @@
         <v>3</v>
       </c>
       <c r="E64" s="30" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="F64" s="6" t="s">
         <v>302</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H64" s="6" t="s">
         <v>159</v>
@@ -7165,7 +7165,7 @@
         <v>54</v>
       </c>
       <c r="P64" s="13" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="Q64" s="6">
         <v>1</v>
@@ -7197,16 +7197,16 @@
         <v>3</v>
       </c>
       <c r="E65" s="30" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="F65" s="6" t="s">
         <v>55</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="I65" s="6" t="s">
         <v>5</v>
@@ -7230,7 +7230,7 @@
         <v>54</v>
       </c>
       <c r="P65" s="13" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="Q65" s="6">
         <v>0</v>
@@ -7268,10 +7268,10 @@
         <v>56</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="I66" s="6" t="s">
         <v>5</v>
@@ -7295,7 +7295,7 @@
         <v>54</v>
       </c>
       <c r="P66" s="13" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="Q66" s="6">
         <v>1</v>
@@ -7327,16 +7327,16 @@
         <v>3</v>
       </c>
       <c r="E67" s="30" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="F67" s="6" t="s">
         <v>57</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="I67" s="6" t="s">
         <v>5</v>
@@ -7392,16 +7392,16 @@
         <v>3</v>
       </c>
       <c r="E68" s="30" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="F68" s="6" t="s">
         <v>58</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="H68" s="6" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="I68" s="6" t="s">
         <v>5</v>
@@ -7457,13 +7457,13 @@
         <v>3</v>
       </c>
       <c r="E69" s="30" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="F69" s="6" t="s">
         <v>301</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H69" s="6" t="s">
         <v>159</v>
@@ -7490,7 +7490,7 @@
         <v>54</v>
       </c>
       <c r="P69" s="13" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="Q69" s="6">
         <v>0</v>
@@ -7522,16 +7522,16 @@
         <v>59</v>
       </c>
       <c r="E70" s="30" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="F70" s="6" t="s">
         <v>60</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="H70" s="6" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I70" s="6" t="s">
         <v>5</v>
@@ -7587,16 +7587,16 @@
         <v>59</v>
       </c>
       <c r="E71" s="30" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>164</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="H71" s="6" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="I71" s="6" t="s">
         <v>5</v>
@@ -7652,16 +7652,16 @@
         <v>59</v>
       </c>
       <c r="E72" s="30" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="F72" s="6" t="s">
         <v>62</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="I72" s="6" t="s">
         <v>5</v>
@@ -7717,16 +7717,16 @@
         <v>59</v>
       </c>
       <c r="E73" s="30" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="F73" s="6" t="s">
         <v>63</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="I73" s="6" t="s">
         <v>5</v>
@@ -7782,16 +7782,16 @@
         <v>59</v>
       </c>
       <c r="E74" s="30" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F74" s="6" t="s">
         <v>165</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H74" s="6" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="I74" s="6" t="s">
         <v>5</v>
@@ -7847,16 +7847,16 @@
         <v>59</v>
       </c>
       <c r="E75" s="30" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="F75" s="6" t="s">
         <v>166</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="H75" s="6" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="I75" s="6" t="s">
         <v>5</v>
@@ -7912,16 +7912,16 @@
         <v>59</v>
       </c>
       <c r="E76" s="30" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="F76" s="6" t="s">
         <v>167</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="H76" s="6" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="I76" s="6" t="s">
         <v>5</v>
@@ -7977,16 +7977,16 @@
         <v>59</v>
       </c>
       <c r="E77" s="30" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="F77" s="6" t="s">
         <v>168</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="H77" s="6" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="I77" s="6" t="s">
         <v>5</v>
@@ -8042,16 +8042,16 @@
         <v>59</v>
       </c>
       <c r="E78" s="30" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="F78" s="6" t="s">
         <v>64</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="H78" s="6" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="I78" s="6" t="s">
         <v>5</v>
@@ -8107,16 +8107,16 @@
         <v>59</v>
       </c>
       <c r="E79" s="30" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="F79" s="6" t="s">
         <v>65</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="H79" s="6" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="I79" s="6" t="s">
         <v>5</v>
@@ -8172,16 +8172,16 @@
         <v>59</v>
       </c>
       <c r="E80" s="30" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="F80" s="6" t="s">
         <v>66</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="H80" s="6" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="I80" s="6" t="s">
         <v>5</v>
@@ -8237,16 +8237,16 @@
         <v>59</v>
       </c>
       <c r="E81" s="30" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="F81" s="6" t="s">
         <v>67</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="H81" s="6" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="I81" s="6" t="s">
         <v>5</v>
@@ -8302,13 +8302,13 @@
         <v>59</v>
       </c>
       <c r="E82" s="30" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="F82" s="6" t="s">
         <v>68</v>
       </c>
       <c r="G82" s="6" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="H82" s="6" t="s">
         <v>160</v>
@@ -8367,13 +8367,13 @@
         <v>104</v>
       </c>
       <c r="E83" s="30" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="F83" s="31" t="s">
         <v>132</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="H83" s="6" t="s">
         <v>133</v>
@@ -8385,16 +8385,16 @@
         <v>6</v>
       </c>
       <c r="K83" s="6" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="L83" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M83" s="6" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="N83" s="6" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="P83" s="6" t="s">
         <v>17</v>
@@ -8429,13 +8429,13 @@
         <v>104</v>
       </c>
       <c r="E84" s="30" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="F84" s="31" t="s">
         <v>134</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="H84" s="6" t="s">
         <v>135</v>
@@ -8453,10 +8453,10 @@
         <v>8</v>
       </c>
       <c r="M84" s="6" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="N84" s="6" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="O84" s="6"/>
       <c r="P84" s="6" t="s">
@@ -8506,16 +8506,16 @@
         <v>104</v>
       </c>
       <c r="E85" s="30" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="F85" s="31" t="s">
         <v>136</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="H85" s="6" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="I85" s="6" t="s">
         <v>5</v>
@@ -8524,16 +8524,16 @@
         <v>6</v>
       </c>
       <c r="K85" s="6" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="L85" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M85" s="6" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="N85" s="6" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="O85" s="6"/>
       <c r="P85" s="6" t="s">
@@ -8583,13 +8583,13 @@
         <v>104</v>
       </c>
       <c r="E86" s="30" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="F86" s="6" t="s">
         <v>137</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="H86" s="6" t="s">
         <v>138</v>
@@ -8607,10 +8607,10 @@
         <v>8</v>
       </c>
       <c r="M86" s="6" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="N86" s="6" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="P86" s="6" t="s">
         <v>17</v>
@@ -8645,16 +8645,16 @@
         <v>104</v>
       </c>
       <c r="E87" s="30" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="F87" s="19" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="I87" s="7" t="s">
         <v>238</v>
@@ -8669,10 +8669,10 @@
         <v>8</v>
       </c>
       <c r="M87" s="7" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="N87" s="7" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="O87" s="6"/>
       <c r="P87" s="6" t="s">
@@ -8722,16 +8722,16 @@
         <v>104</v>
       </c>
       <c r="E88" s="32" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="F88" s="19" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="H88" s="7" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="I88" s="7" t="s">
         <v>241</v>
@@ -8746,10 +8746,10 @@
         <v>8</v>
       </c>
       <c r="M88" s="7" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="N88" s="7" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="P88" s="6" t="s">
         <v>17</v>
@@ -8784,16 +8784,16 @@
         <v>104</v>
       </c>
       <c r="E89" s="30" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="F89" s="19" t="s">
         <v>243</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="H89" s="7" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="I89" s="7" t="s">
         <v>238</v>
@@ -8808,10 +8808,10 @@
         <v>8</v>
       </c>
       <c r="M89" s="7" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="N89" s="7" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="O89" s="7"/>
       <c r="P89" s="7" t="s">
@@ -8861,16 +8861,16 @@
         <v>104</v>
       </c>
       <c r="E90" s="30" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="F90" s="20" t="s">
         <v>246</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="H90" s="7" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="I90" s="7" t="s">
         <v>241</v>
@@ -8885,10 +8885,10 @@
         <v>8</v>
       </c>
       <c r="M90" s="7" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="N90" s="7" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="O90" s="7"/>
       <c r="P90" s="7" t="s">
@@ -8938,16 +8938,16 @@
         <v>305</v>
       </c>
       <c r="E91" s="30" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>312</v>
+        <v>736</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>311</v>
+        <v>737</v>
       </c>
       <c r="I91" s="7" t="s">
         <v>5</v>
@@ -9012,16 +9012,16 @@
         <v>2</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="F92" s="6" t="s">
         <v>190</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="H92" s="6" t="s">
         <v>191</v>
@@ -9046,7 +9046,7 @@
       </c>
       <c r="O92" s="6"/>
       <c r="P92" s="6" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="Q92" s="6">
         <v>1</v>
@@ -9089,7 +9089,7 @@
         <v>2</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E93" s="30" t="s">
         <v>71</v>
@@ -9098,10 +9098,10 @@
         <v>71</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="H93" s="6" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="I93" s="6" t="s">
         <v>192</v>
@@ -9123,7 +9123,7 @@
       </c>
       <c r="O93" s="6"/>
       <c r="P93" s="6" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="Q93" s="6">
         <v>1</v>
@@ -9166,19 +9166,19 @@
         <v>2</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E94" s="30" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>293</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="I94" s="11" t="s">
         <v>294</v>
@@ -9243,10 +9243,10 @@
         <v>2</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E95" s="30" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="F95" s="12" t="s">
         <v>197</v>
@@ -9255,7 +9255,7 @@
         <v>198</v>
       </c>
       <c r="H95" s="11" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="I95" s="11" t="s">
         <v>199</v>
@@ -9305,10 +9305,10 @@
         <v>2</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E96" s="30" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="F96" s="12" t="s">
         <v>231</v>
@@ -9317,7 +9317,7 @@
         <v>203</v>
       </c>
       <c r="H96" s="11" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="I96" s="11" t="s">
         <v>199</v>
@@ -9367,19 +9367,19 @@
         <v>2</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E97" s="30" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="F97" s="12" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="G97" s="6" t="s">
         <v>204</v>
       </c>
       <c r="H97" s="11" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="I97" s="11" t="s">
         <v>199</v>
@@ -9429,10 +9429,10 @@
         <v>2</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E98" s="30" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="F98" s="12" t="s">
         <v>232</v>
@@ -9441,7 +9441,7 @@
         <v>205</v>
       </c>
       <c r="H98" s="11" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="I98" s="11" t="s">
         <v>206</v>
@@ -9491,10 +9491,10 @@
         <v>2</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E99" s="30" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="F99" s="12" t="s">
         <v>207</v>
@@ -9503,7 +9503,7 @@
         <v>208</v>
       </c>
       <c r="H99" s="11" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="I99" s="11" t="s">
         <v>209</v>
@@ -9553,10 +9553,10 @@
         <v>2</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E100" s="30" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="F100" s="12" t="s">
         <v>225</v>
@@ -9565,7 +9565,7 @@
         <v>214</v>
       </c>
       <c r="H100" s="11" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="I100" s="11" t="s">
         <v>215</v>
@@ -9615,10 +9615,10 @@
         <v>2</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E101" s="30" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="F101" s="12" t="s">
         <v>226</v>
@@ -9627,7 +9627,7 @@
         <v>217</v>
       </c>
       <c r="H101" s="11" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="I101" s="11" t="s">
         <v>215</v>
@@ -9677,10 +9677,10 @@
         <v>2</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E102" s="30" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="F102" s="12" t="s">
         <v>227</v>
@@ -9689,7 +9689,7 @@
         <v>218</v>
       </c>
       <c r="H102" s="11" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="I102" s="11" t="s">
         <v>215</v>
@@ -9739,10 +9739,10 @@
         <v>2</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E103" s="30" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="F103" s="12" t="s">
         <v>228</v>
@@ -9751,7 +9751,7 @@
         <v>219</v>
       </c>
       <c r="H103" s="11" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="I103" s="11" t="s">
         <v>215</v>
@@ -9816,10 +9816,10 @@
         <v>2</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E104" s="30" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="F104" s="12" t="s">
         <v>229</v>
@@ -9828,7 +9828,7 @@
         <v>220</v>
       </c>
       <c r="H104" s="11" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="I104" s="11" t="s">
         <v>215</v>
@@ -9893,10 +9893,10 @@
         <v>2</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="E105" s="30" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="F105" s="12" t="s">
         <v>230</v>
@@ -9905,7 +9905,7 @@
         <v>221</v>
       </c>
       <c r="H105" s="11" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="I105" s="11" t="s">
         <v>215</v>
@@ -9973,13 +9973,13 @@
         <v>3</v>
       </c>
       <c r="E106" s="30" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="F106" s="21" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="G106" s="6" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="H106" s="7" t="s">
         <v>258</v>
@@ -9997,10 +9997,10 @@
         <v>8</v>
       </c>
       <c r="M106" s="7" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="N106" s="7" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="P106" s="7" t="s">
         <v>245</v>
@@ -10035,13 +10035,13 @@
         <v>3</v>
       </c>
       <c r="E107" s="30" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="F107" s="8" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="H107" s="7" t="s">
         <v>260</v>
@@ -10059,10 +10059,10 @@
         <v>8</v>
       </c>
       <c r="M107" s="7" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="N107" s="7" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="P107" s="7" t="s">
         <v>245</v>
@@ -10097,13 +10097,13 @@
         <v>3</v>
       </c>
       <c r="E108" s="30" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="F108" s="8" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="G108" s="6" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="H108" s="7" t="s">
         <v>262</v>
@@ -10121,10 +10121,10 @@
         <v>8</v>
       </c>
       <c r="M108" s="7" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="N108" s="7" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="P108" s="7" t="s">
         <v>245</v>
@@ -10159,13 +10159,13 @@
         <v>3</v>
       </c>
       <c r="E109" s="30" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="F109" s="8" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="G109" s="6" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="H109" s="7" t="s">
         <v>268</v>
@@ -10183,10 +10183,10 @@
         <v>8</v>
       </c>
       <c r="M109" s="7" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="N109" s="7" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="O109" s="7"/>
       <c r="P109" s="7" t="s">
@@ -10236,13 +10236,13 @@
         <v>3</v>
       </c>
       <c r="E110" s="30" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="F110" s="22" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="G110" s="6" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="H110" s="7" t="s">
         <v>264</v>
@@ -10260,10 +10260,10 @@
         <v>8</v>
       </c>
       <c r="M110" s="7" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="N110" s="7" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="P110" s="7" t="s">
         <v>245</v>
@@ -10298,13 +10298,13 @@
         <v>3</v>
       </c>
       <c r="E111" s="30" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="F111" s="22" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="G111" s="6" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="H111" s="7" t="s">
         <v>266</v>
@@ -10322,10 +10322,10 @@
         <v>8</v>
       </c>
       <c r="M111" s="7" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="N111" s="7" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="O111" s="7"/>
       <c r="P111" s="7" t="s">
@@ -10375,13 +10375,13 @@
         <v>3</v>
       </c>
       <c r="E112" s="30" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="F112" s="7" t="s">
         <v>247</v>
       </c>
       <c r="G112" s="6" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="H112" s="7" t="s">
         <v>248</v>
@@ -10399,10 +10399,10 @@
         <v>8</v>
       </c>
       <c r="M112" s="7" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="N112" s="7" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="P112" s="7" t="s">
         <v>245</v>
@@ -10437,13 +10437,13 @@
         <v>3</v>
       </c>
       <c r="E113" s="30" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="F113" s="7" t="s">
         <v>250</v>
       </c>
       <c r="G113" s="6" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="H113" s="7" t="s">
         <v>251</v>
@@ -10461,10 +10461,10 @@
         <v>8</v>
       </c>
       <c r="M113" s="7" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="N113" s="7" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="P113" s="7" t="s">
         <v>245</v>
@@ -10499,13 +10499,13 @@
         <v>3</v>
       </c>
       <c r="E114" s="30" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="F114" s="7" t="s">
         <v>252</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="H114" s="7" t="s">
         <v>253</v>
@@ -10523,10 +10523,10 @@
         <v>8</v>
       </c>
       <c r="M114" s="7" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="N114" s="7" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="P114" s="7" t="s">
         <v>245</v>
@@ -10561,13 +10561,13 @@
         <v>15</v>
       </c>
       <c r="E115" s="30" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="F115" s="21" t="s">
         <v>254</v>
       </c>
       <c r="G115" s="6" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="H115" s="7" t="s">
         <v>255</v>
@@ -10585,10 +10585,10 @@
         <v>8</v>
       </c>
       <c r="M115" s="7" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="N115" s="7" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="P115" s="7" t="s">
         <v>245</v>
@@ -10623,16 +10623,16 @@
         <v>15</v>
       </c>
       <c r="E116" s="30" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="F116" s="8" t="s">
         <v>271</v>
       </c>
       <c r="G116" s="6" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="H116" s="7" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="I116" s="7" t="s">
         <v>5</v>
@@ -10647,10 +10647,10 @@
         <v>8</v>
       </c>
       <c r="M116" s="7" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="N116" s="7" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="O116" s="7"/>
       <c r="P116" s="7" t="s">
@@ -10700,16 +10700,16 @@
         <v>15</v>
       </c>
       <c r="E117" s="30" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="F117" s="2" t="s">
         <v>296</v>
       </c>
       <c r="G117" s="6" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="H117" s="2" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="I117" s="11" t="s">
         <v>5</v>
@@ -10777,7 +10777,7 @@
         <v>15</v>
       </c>
       <c r="E118" s="30" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="F118" s="12" t="s">
         <v>210</v>
@@ -10786,7 +10786,7 @@
         <v>222</v>
       </c>
       <c r="H118" s="11" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="I118" s="11" t="s">
         <v>211</v>
@@ -10839,7 +10839,7 @@
         <v>15</v>
       </c>
       <c r="E119" s="30" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="F119" s="12" t="s">
         <v>212</v>
@@ -10848,7 +10848,7 @@
         <v>223</v>
       </c>
       <c r="H119" s="11" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="I119" s="11" t="s">
         <v>211</v>
@@ -10901,7 +10901,7 @@
         <v>15</v>
       </c>
       <c r="E120" s="30" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="F120" s="12" t="s">
         <v>213</v>
@@ -10910,7 +10910,7 @@
         <v>224</v>
       </c>
       <c r="H120" s="11" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="I120" s="11" t="s">
         <v>211</v>
@@ -10963,16 +10963,16 @@
         <v>15</v>
       </c>
       <c r="E121" s="30" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="F121" s="7" t="s">
         <v>270</v>
       </c>
       <c r="G121" s="6" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="H121" s="7" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="I121" s="7" t="s">
         <v>5</v>
@@ -10987,10 +10987,10 @@
         <v>8</v>
       </c>
       <c r="M121" s="7" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="N121" s="7" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="O121" s="7"/>
       <c r="P121" s="7" t="s">
@@ -11037,16 +11037,16 @@
         <v>2</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="E122" s="30" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="F122" s="33" t="s">
         <v>272</v>
       </c>
       <c r="G122" s="6" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="H122" s="23" t="s">
         <v>273</v>
@@ -11097,13 +11097,13 @@
         <v>2</v>
       </c>
       <c r="D123" s="6" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="E123" s="30" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="F123" s="33" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="G123" s="6" t="s">
         <v>277</v>
@@ -11157,10 +11157,10 @@
         <v>2</v>
       </c>
       <c r="D124" s="6" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="E124" s="30" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="F124" s="33" t="s">
         <v>279</v>
@@ -11217,10 +11217,10 @@
         <v>2</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="E125" s="30" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="F125" s="33" t="s">
         <v>282</v>
@@ -11292,19 +11292,19 @@
         <v>2</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="E126" s="30" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="F126" s="33" t="s">
         <v>285</v>
       </c>
       <c r="G126" s="6" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="H126" s="23" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="I126" s="23"/>
       <c r="J126" s="7" t="s">
@@ -11367,10 +11367,10 @@
         <v>2</v>
       </c>
       <c r="D127" s="6" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="E127" s="30" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="F127" s="33" t="s">
         <v>286</v>
@@ -11441,10 +11441,10 @@
         <v>2</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="E128" s="32" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F128" s="33" t="s">
         <v>290</v>
@@ -11521,19 +11521,19 @@
         <v>3</v>
       </c>
       <c r="E129" s="32" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="F129" s="36" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="G129" s="6" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="H129" s="7" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="I129" s="23" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="J129" s="7" t="s">
         <v>6</v>
@@ -11598,19 +11598,19 @@
         <v>3</v>
       </c>
       <c r="E130" s="32" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="F130" s="36" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="G130" s="6" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="H130" s="7" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="I130" s="23" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="J130" s="7" t="s">
         <v>6</v>
@@ -11675,19 +11675,19 @@
         <v>3</v>
       </c>
       <c r="E131" s="32" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="F131" s="36" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="G131" s="6" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H131" s="7" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="I131" s="23" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="J131" s="7" t="s">
         <v>6</v>
@@ -11752,16 +11752,16 @@
         <v>3</v>
       </c>
       <c r="E132" s="32" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="F132" s="36" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="G132" s="6" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="H132" s="7" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="I132" s="23" t="s">
         <v>5</v>
@@ -11829,16 +11829,16 @@
         <v>3</v>
       </c>
       <c r="E133" s="32" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="F133" s="36" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="G133" s="6" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="H133" s="7" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="I133" s="23" t="s">
         <v>5</v>
@@ -11906,16 +11906,16 @@
         <v>3</v>
       </c>
       <c r="E134" s="32" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="F134" s="36" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="G134" s="6" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="H134" s="7" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="I134" s="23" t="s">
         <v>5</v>
@@ -11983,16 +11983,16 @@
         <v>3</v>
       </c>
       <c r="E135" s="32" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="F135" s="36" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="G135" s="6" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="H135" s="7" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="I135" s="23" t="s">
         <v>5</v>
@@ -12060,16 +12060,16 @@
         <v>3</v>
       </c>
       <c r="E136" s="32" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="F136" s="36" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="G136" s="6" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="H136" s="7" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="I136" s="23" t="s">
         <v>5</v>
@@ -12201,7 +12201,7 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
       <c r="A2" s="26" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>175</v>
@@ -12209,7 +12209,7 @@
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1">
       <c r="A3" s="26" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>177</v>
@@ -12217,7 +12217,7 @@
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1">
       <c r="A4" s="26" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>176</v>
@@ -12225,7 +12225,7 @@
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1">
       <c r="A5" s="26" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>178</v>
@@ -12233,15 +12233,15 @@
     </row>
     <row r="6" spans="1:2" ht="17.25" customHeight="1">
       <c r="A6" s="26" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>179</v>
@@ -12249,7 +12249,7 @@
     </row>
     <row r="8" spans="1:2" ht="17.25" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>180</v>
@@ -12257,7 +12257,7 @@
     </row>
     <row r="9" spans="1:2" ht="17.25" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>181</v>
@@ -12265,7 +12265,7 @@
     </row>
     <row r="10" spans="1:2" ht="17.25" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>182</v>
@@ -12273,7 +12273,7 @@
     </row>
     <row r="11" spans="1:2" ht="17.25" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>183</v>
@@ -12281,7 +12281,7 @@
     </row>
     <row r="12" spans="1:2" ht="17.25" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>184</v>
@@ -12289,7 +12289,7 @@
     </row>
     <row r="13" spans="1:2" ht="17.25" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>185</v>
@@ -12297,7 +12297,7 @@
     </row>
     <row r="14" spans="1:2" ht="17.25" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>186</v>
@@ -12305,7 +12305,7 @@
     </row>
     <row r="15" spans="1:2" ht="17.25" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>187</v>
@@ -12313,7 +12313,7 @@
     </row>
     <row r="16" spans="1:2" ht="17.25" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>188</v>
@@ -12321,42 +12321,42 @@
     </row>
     <row r="17" spans="1:2" ht="17.25" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="17.25" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="17.25" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="17.25" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="17.25" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="17.25" customHeight="1">

</xml_diff>

<commit_message>
Mod nomindicador Cobertura de salud
</commit_message>
<xml_diff>
--- a/Data/Base_fichas_indicadores.xlsx
+++ b/Data/Base_fichas_indicadores.xlsx
@@ -1286,9 +1286,6 @@
     <t>El indicador mide el peso del gasto público en salud en el total de gasto público social (GPS) EL GPS se compone del gasto en salud; salud; seguridad y asistencia social; salud, medio ambiente, agua y saneamiento; y cultura y deporte					.</t>
   </si>
   <si>
-    <t>El indicador refleja la distribución porcentual de personas según institución prestadora en la cual tienen derecho vigente.</t>
-  </si>
-  <si>
     <t>El indicador mide la cantidad anual de defunciones registradas en el año en relación a la población del país proyectada según censo 1996.</t>
   </si>
   <si>
@@ -2241,6 +2238,9 @@
   </si>
   <si>
     <t>Distribución porcentual de personas según institución prestadora en la cual tienen cobertura vigente</t>
+  </si>
+  <si>
+    <t>El indicador refleja la distribución porcentual de personas según institución prestadora integral de salud en la cual tienen cobertura (derecho vigente según la pregunta específica de la ECH).</t>
   </si>
 </sst>
 </file>
@@ -2779,10 +2779,10 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AI140"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="G1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E111" sqref="E111"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="G107" sqref="G106:G107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2793,12 +2793,12 @@
     <col min="4" max="4" width="37.7109375" style="13" customWidth="1"/>
     <col min="5" max="5" width="94.7109375" style="13" customWidth="1"/>
     <col min="6" max="6" width="157.28515625" style="13" customWidth="1"/>
-    <col min="7" max="7" width="255.7109375" style="13" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="181.140625" style="13" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="59.42578125" style="13" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" style="13" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="255.7109375" style="13" customWidth="1"/>
+    <col min="8" max="8" width="181.140625" style="13" customWidth="1"/>
+    <col min="9" max="9" width="59.42578125" style="13" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" style="13" customWidth="1"/>
     <col min="11" max="11" width="20.42578125" style="13" customWidth="1"/>
-    <col min="12" max="12" width="20.5703125" style="13" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" style="13" customWidth="1"/>
     <col min="13" max="14" width="255.7109375" style="13" customWidth="1"/>
     <col min="15" max="15" width="230.140625" style="13" customWidth="1"/>
     <col min="16" max="16" width="98.7109375" style="13" customWidth="1"/>
@@ -2827,7 +2827,7 @@
         <v>358</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F1" s="26" t="s">
         <v>347</v>
@@ -2863,19 +2863,19 @@
         <v>357</v>
       </c>
       <c r="Q1" s="26" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="R1" s="13" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="S1" s="35" t="s">
+        <v>700</v>
+      </c>
+      <c r="T1" s="35" t="s">
         <v>701</v>
       </c>
-      <c r="T1" s="35" t="s">
+      <c r="U1" s="35" t="s">
         <v>702</v>
-      </c>
-      <c r="U1" s="35" t="s">
-        <v>703</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="6" customFormat="1">
@@ -2892,7 +2892,7 @@
         <v>104</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F2" s="31" t="s">
         <v>80</v>
@@ -2910,16 +2910,16 @@
         <v>6</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="P2" s="6" t="s">
         <v>17</v>
@@ -2954,7 +2954,7 @@
         <v>104</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F3" s="31" t="s">
         <v>81</v>
@@ -2972,16 +2972,16 @@
         <v>6</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>17</v>
@@ -3016,7 +3016,7 @@
         <v>104</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F4" s="31" t="s">
         <v>82</v>
@@ -3034,16 +3034,16 @@
         <v>6</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="L4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="P4" s="6" t="s">
         <v>17</v>
@@ -3078,13 +3078,13 @@
         <v>104</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>76</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>112</v>
@@ -3102,10 +3102,10 @@
         <v>8</v>
       </c>
       <c r="M5" s="6" t="s">
+        <v>508</v>
+      </c>
+      <c r="N5" s="6" t="s">
         <v>509</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>510</v>
       </c>
       <c r="P5" s="6" t="s">
         <v>17</v>
@@ -3140,7 +3140,7 @@
         <v>104</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>79</v>
@@ -3149,7 +3149,7 @@
         <v>365</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>5</v>
@@ -3164,10 +3164,10 @@
         <v>8</v>
       </c>
       <c r="M6" s="6" t="s">
+        <v>506</v>
+      </c>
+      <c r="N6" s="6" t="s">
         <v>507</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>508</v>
       </c>
       <c r="P6" s="6" t="s">
         <v>25</v>
@@ -3202,7 +3202,7 @@
         <v>104</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>78</v>
@@ -3211,7 +3211,7 @@
         <v>366</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>5</v>
@@ -3226,10 +3226,10 @@
         <v>8</v>
       </c>
       <c r="M7" s="6" t="s">
+        <v>506</v>
+      </c>
+      <c r="N7" s="6" t="s">
         <v>507</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>508</v>
       </c>
       <c r="P7" s="6" t="s">
         <v>25</v>
@@ -3264,7 +3264,7 @@
         <v>104</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>83</v>
@@ -3288,10 +3288,10 @@
         <v>8</v>
       </c>
       <c r="M8" s="6" t="s">
+        <v>506</v>
+      </c>
+      <c r="N8" s="6" t="s">
         <v>507</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>508</v>
       </c>
       <c r="P8" s="6" t="s">
         <v>25</v>
@@ -3326,7 +3326,7 @@
         <v>104</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>84</v>
@@ -3350,10 +3350,10 @@
         <v>8</v>
       </c>
       <c r="M9" s="6" t="s">
+        <v>506</v>
+      </c>
+      <c r="N9" s="6" t="s">
         <v>507</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>508</v>
       </c>
       <c r="P9" s="6" t="s">
         <v>85</v>
@@ -3388,7 +3388,7 @@
         <v>104</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>88</v>
@@ -3412,10 +3412,10 @@
         <v>8</v>
       </c>
       <c r="M10" s="6" t="s">
+        <v>506</v>
+      </c>
+      <c r="N10" s="6" t="s">
         <v>507</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>508</v>
       </c>
       <c r="P10" s="6" t="s">
         <v>85</v>
@@ -3450,7 +3450,7 @@
         <v>104</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>89</v>
@@ -3474,10 +3474,10 @@
         <v>8</v>
       </c>
       <c r="M11" s="6" t="s">
+        <v>506</v>
+      </c>
+      <c r="N11" s="6" t="s">
         <v>507</v>
-      </c>
-      <c r="N11" s="6" t="s">
-        <v>508</v>
       </c>
       <c r="P11" s="6" t="s">
         <v>85</v>
@@ -3512,16 +3512,16 @@
         <v>104</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>315</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>33</v>
@@ -3536,13 +3536,13 @@
         <v>8</v>
       </c>
       <c r="M12" s="6" t="s">
+        <v>506</v>
+      </c>
+      <c r="N12" s="6" t="s">
         <v>507</v>
       </c>
-      <c r="N12" s="6" t="s">
-        <v>508</v>
-      </c>
       <c r="P12" s="6" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="Q12" s="6">
         <v>0</v>
@@ -3574,13 +3574,13 @@
         <v>104</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>92</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>295</v>
@@ -3598,7 +3598,7 @@
         <v>8</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N13" s="6" t="s">
         <v>13</v>
@@ -3636,7 +3636,7 @@
         <v>104</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>97</v>
@@ -3660,10 +3660,10 @@
         <v>296</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="P14" s="6" t="s">
         <v>96</v>
@@ -3698,16 +3698,16 @@
         <v>303</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>305</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>5</v>
@@ -3760,16 +3760,16 @@
         <v>303</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>304</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="I16" s="7" t="s">
         <v>5</v>
@@ -3822,16 +3822,16 @@
         <v>303</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>302</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I17" s="7" t="s">
         <v>5</v>
@@ -3884,7 +3884,7 @@
         <v>3</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F18" s="13" t="s">
         <v>4</v>
@@ -3917,7 +3917,7 @@
         <v>10</v>
       </c>
       <c r="P18" s="13" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="Q18" s="6">
         <v>1</v>
@@ -3949,7 +3949,7 @@
         <v>3</v>
       </c>
       <c r="E19" s="30" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F19" s="13" t="s">
         <v>100</v>
@@ -3982,7 +3982,7 @@
         <v>11</v>
       </c>
       <c r="P19" s="13" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="Q19" s="6">
         <v>1</v>
@@ -4014,7 +4014,7 @@
         <v>3</v>
       </c>
       <c r="E20" s="30" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="F20" s="13" t="s">
         <v>102</v>
@@ -4047,7 +4047,7 @@
         <v>11</v>
       </c>
       <c r="P20" s="13" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="Q20" s="6">
         <v>0</v>
@@ -4079,7 +4079,7 @@
         <v>3</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="F21" s="13" t="s">
         <v>18</v>
@@ -4112,7 +4112,7 @@
         <v>10</v>
       </c>
       <c r="P21" s="13" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="Q21" s="6">
         <v>0</v>
@@ -4158,7 +4158,7 @@
         <v>3</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>19</v>
@@ -4191,7 +4191,7 @@
         <v>10</v>
       </c>
       <c r="P22" s="13" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="Q22" s="6">
         <v>0</v>
@@ -4237,7 +4237,7 @@
         <v>3</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F23" s="13" t="s">
         <v>20</v>
@@ -4270,7 +4270,7 @@
         <v>10</v>
       </c>
       <c r="P23" s="13" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="Q23" s="6">
         <v>0</v>
@@ -4302,7 +4302,7 @@
         <v>3</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="F24" s="15" t="s">
         <v>297</v>
@@ -4335,7 +4335,7 @@
         <v>233</v>
       </c>
       <c r="P24" s="13" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="Q24" s="6">
         <v>0</v>
@@ -4381,7 +4381,7 @@
         <v>3</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F25" s="15" t="s">
         <v>235</v>
@@ -4414,7 +4414,7 @@
         <v>233</v>
       </c>
       <c r="P25" s="13" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="Q25" s="6">
         <v>1</v>
@@ -4460,7 +4460,7 @@
         <v>12</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>98</v>
@@ -4484,16 +4484,16 @@
         <v>8</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N26" s="6" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="O26" s="6" t="s">
         <v>14</v>
       </c>
       <c r="P26" s="6" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="Q26" s="6">
         <v>0</v>
@@ -4525,7 +4525,7 @@
         <v>12</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>73</v>
@@ -4549,16 +4549,16 @@
         <v>8</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N27" s="6" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="O27" s="6" t="s">
         <v>14</v>
       </c>
       <c r="P27" s="6" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="Q27" s="6">
         <v>0</v>
@@ -4604,13 +4604,13 @@
         <v>12</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>99</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="H28" s="6" t="s">
         <v>151</v>
@@ -4628,16 +4628,16 @@
         <v>8</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N28" s="6" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="O28" s="6" t="s">
         <v>14</v>
       </c>
       <c r="P28" s="6" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="Q28" s="6">
         <v>0</v>
@@ -4683,7 +4683,7 @@
         <v>12</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F29" s="13" t="s">
         <v>101</v>
@@ -4707,16 +4707,16 @@
         <v>8</v>
       </c>
       <c r="M29" s="13" t="s">
+        <v>506</v>
+      </c>
+      <c r="N29" s="13" t="s">
         <v>507</v>
-      </c>
-      <c r="N29" s="13" t="s">
-        <v>508</v>
       </c>
       <c r="O29" s="13" t="s">
         <v>21</v>
       </c>
       <c r="P29" s="13" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="Q29" s="6">
         <v>0</v>
@@ -4748,7 +4748,7 @@
         <v>12</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F30" s="13" t="s">
         <v>103</v>
@@ -4772,16 +4772,16 @@
         <v>8</v>
       </c>
       <c r="M30" s="13" t="s">
+        <v>506</v>
+      </c>
+      <c r="N30" s="13" t="s">
         <v>507</v>
-      </c>
-      <c r="N30" s="13" t="s">
-        <v>508</v>
       </c>
       <c r="O30" s="13" t="s">
         <v>21</v>
       </c>
       <c r="P30" s="13" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="Q30" s="6">
         <v>0</v>
@@ -4827,7 +4827,7 @@
         <v>15</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>108</v>
@@ -4851,10 +4851,10 @@
         <v>16</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N31" s="6" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="O31" s="16"/>
       <c r="P31" s="13" t="s">
@@ -4904,7 +4904,7 @@
         <v>15</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>109</v>
@@ -4928,10 +4928,10 @@
         <v>16</v>
       </c>
       <c r="M32" s="6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N32" s="6" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="O32" s="16"/>
       <c r="P32" s="13" t="s">
@@ -4981,13 +4981,13 @@
         <v>15</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>107</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="H33" s="13" t="s">
         <v>146</v>
@@ -5005,10 +5005,10 @@
         <v>16</v>
       </c>
       <c r="M33" s="6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="O33" s="16"/>
       <c r="P33" s="13" t="s">
@@ -5044,13 +5044,13 @@
         <v>15</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>110</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="H34" s="13" t="s">
         <v>147</v>
@@ -5068,10 +5068,10 @@
         <v>16</v>
       </c>
       <c r="M34" s="6" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="N34" s="6" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="O34" s="6" t="s">
         <v>105</v>
@@ -5123,13 +5123,13 @@
         <v>15</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>22</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H35" s="6" t="s">
         <v>152</v>
@@ -5188,7 +5188,7 @@
         <v>3</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F36" s="13" t="s">
         <v>74</v>
@@ -5221,7 +5221,7 @@
         <v>75</v>
       </c>
       <c r="P36" s="13" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="Q36" s="6">
         <v>0</v>
@@ -5253,7 +5253,7 @@
         <v>104</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F37" s="31" t="s">
         <v>118</v>
@@ -5271,16 +5271,16 @@
         <v>6</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="L37" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M37" s="6" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="P37" s="6" t="s">
         <v>17</v>
@@ -5315,7 +5315,7 @@
         <v>104</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F38" s="31" t="s">
         <v>120</v>
@@ -5339,10 +5339,10 @@
         <v>8</v>
       </c>
       <c r="M38" s="6" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="N38" s="6" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="P38" s="6" t="s">
         <v>17</v>
@@ -5377,7 +5377,7 @@
         <v>104</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F39" s="31" t="s">
         <v>122</v>
@@ -5386,7 +5386,7 @@
         <v>389</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="I39" s="6" t="s">
         <v>5</v>
@@ -5395,16 +5395,16 @@
         <v>6</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="L39" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M39" s="6" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="N39" s="6" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="P39" s="6" t="s">
         <v>17</v>
@@ -5439,13 +5439,13 @@
         <v>104</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>123</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="H40" s="6" t="s">
         <v>124</v>
@@ -5463,10 +5463,10 @@
         <v>8</v>
       </c>
       <c r="M40" s="6" t="s">
+        <v>508</v>
+      </c>
+      <c r="N40" s="6" t="s">
         <v>509</v>
-      </c>
-      <c r="N40" s="6" t="s">
-        <v>510</v>
       </c>
       <c r="P40" s="6" t="s">
         <v>17</v>
@@ -5501,13 +5501,13 @@
         <v>104</v>
       </c>
       <c r="E41" s="30" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="F41" s="24" t="s">
         <v>316</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="H41" s="6" t="s">
         <v>317</v>
@@ -5578,13 +5578,13 @@
         <v>104</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="F42" s="24" t="s">
         <v>322</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="H42" s="6" t="s">
         <v>323</v>
@@ -5655,7 +5655,7 @@
         <v>104</v>
       </c>
       <c r="E43" s="30" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F43" s="24" t="s">
         <v>327</v>
@@ -5732,7 +5732,7 @@
         <v>36</v>
       </c>
       <c r="E44" s="30" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F44" s="13" t="s">
         <v>37</v>
@@ -5765,7 +5765,7 @@
         <v>40</v>
       </c>
       <c r="P44" s="13" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="Q44" s="6">
         <v>1</v>
@@ -5811,13 +5811,13 @@
         <v>41</v>
       </c>
       <c r="E45" s="32" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F45" s="13" t="s">
         <v>42</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="H45" s="13" t="s">
         <v>154</v>
@@ -5844,7 +5844,7 @@
         <v>43</v>
       </c>
       <c r="P45" s="13" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="Q45" s="6">
         <v>0</v>
@@ -5890,7 +5890,7 @@
         <v>41</v>
       </c>
       <c r="E46" s="32" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F46" s="13" t="s">
         <v>44</v>
@@ -5923,7 +5923,7 @@
         <v>45</v>
       </c>
       <c r="P46" s="13" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="Q46" s="6">
         <v>0</v>
@@ -5969,7 +5969,7 @@
         <v>41</v>
       </c>
       <c r="E47" s="32" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>313</v>
@@ -6034,13 +6034,13 @@
         <v>41</v>
       </c>
       <c r="E48" s="32" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>161</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="H48" s="13" t="s">
         <v>162</v>
@@ -6067,7 +6067,7 @@
         <v>163</v>
       </c>
       <c r="P48" s="13" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="Q48" s="6">
         <v>0</v>
@@ -6099,16 +6099,16 @@
         <v>46</v>
       </c>
       <c r="E49" s="32" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="H49" s="27" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="I49" s="6" t="s">
         <v>5</v>
@@ -6132,7 +6132,7 @@
         <v>309</v>
       </c>
       <c r="P49" s="6" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="Q49" s="6">
         <v>1</v>
@@ -6164,16 +6164,16 @@
         <v>46</v>
       </c>
       <c r="E50" s="32" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="G50" s="6" t="s">
         <v>340</v>
       </c>
       <c r="H50" s="27" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="I50" s="6" t="s">
         <v>5</v>
@@ -6197,7 +6197,7 @@
         <v>341</v>
       </c>
       <c r="P50" s="13" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="Q50" s="6">
         <v>0</v>
@@ -6243,7 +6243,7 @@
         <v>46</v>
       </c>
       <c r="E51" s="32" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>339</v>
@@ -6252,7 +6252,7 @@
         <v>338</v>
       </c>
       <c r="H51" s="27" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I51" s="6" t="s">
         <v>5</v>
@@ -6273,10 +6273,10 @@
         <v>194</v>
       </c>
       <c r="O51" s="7" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="P51" s="13" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="Q51" s="6">
         <v>0</v>
@@ -6322,16 +6322,16 @@
         <v>46</v>
       </c>
       <c r="E52" s="32" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F52" s="28" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="G52" s="6" t="s">
         <v>337</v>
       </c>
       <c r="H52" s="27" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="I52" s="6" t="s">
         <v>5</v>
@@ -6352,10 +6352,10 @@
         <v>194</v>
       </c>
       <c r="O52" s="7" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="P52" s="13" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="Q52" s="6">
         <v>0</v>
@@ -6401,16 +6401,16 @@
         <v>47</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="F53" s="28" t="s">
+        <v>665</v>
+      </c>
+      <c r="G53" s="28" t="s">
         <v>666</v>
       </c>
-      <c r="G53" s="28" t="s">
-        <v>667</v>
-      </c>
       <c r="H53" s="34" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="I53" s="6" t="s">
         <v>5</v>
@@ -6431,10 +6431,10 @@
         <v>194</v>
       </c>
       <c r="O53" s="7" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="P53" s="13" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="Q53" s="6">
         <v>1</v>
@@ -6480,7 +6480,7 @@
         <v>47</v>
       </c>
       <c r="E54" s="32" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F54" s="13" t="s">
         <v>48</v>
@@ -6513,7 +6513,7 @@
         <v>49</v>
       </c>
       <c r="P54" s="13" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="Q54" s="6">
         <v>0</v>
@@ -6559,7 +6559,7 @@
         <v>50</v>
       </c>
       <c r="E55" s="32" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="F55" s="13" t="s">
         <v>51</v>
@@ -6590,7 +6590,7 @@
       </c>
       <c r="O55" s="13"/>
       <c r="P55" s="13" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="Q55" s="6">
         <v>1</v>
@@ -6636,7 +6636,7 @@
         <v>104</v>
       </c>
       <c r="E56" s="32" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F56" s="31" t="s">
         <v>125</v>
@@ -6654,16 +6654,16 @@
         <v>6</v>
       </c>
       <c r="K56" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="L56" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M56" s="6" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="N56" s="6" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="P56" s="6" t="s">
         <v>17</v>
@@ -6698,7 +6698,7 @@
         <v>104</v>
       </c>
       <c r="E57" s="30" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F57" s="31" t="s">
         <v>127</v>
@@ -6722,10 +6722,10 @@
         <v>8</v>
       </c>
       <c r="M57" s="6" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="N57" s="6" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="P57" s="6" t="s">
         <v>17</v>
@@ -6760,7 +6760,7 @@
         <v>104</v>
       </c>
       <c r="E58" s="30" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F58" s="31" t="s">
         <v>129</v>
@@ -6769,7 +6769,7 @@
         <v>396</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="I58" s="6" t="s">
         <v>5</v>
@@ -6778,16 +6778,16 @@
         <v>6</v>
       </c>
       <c r="K58" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="L58" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M58" s="6" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="N58" s="6" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="P58" s="6" t="s">
         <v>17</v>
@@ -6822,13 +6822,13 @@
         <v>104</v>
       </c>
       <c r="E59" s="30" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>130</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H59" s="6" t="s">
         <v>131</v>
@@ -6846,10 +6846,10 @@
         <v>8</v>
       </c>
       <c r="M59" s="6" t="s">
+        <v>508</v>
+      </c>
+      <c r="N59" s="6" t="s">
         <v>509</v>
-      </c>
-      <c r="N59" s="6" t="s">
-        <v>510</v>
       </c>
       <c r="P59" s="6" t="s">
         <v>17</v>
@@ -6884,7 +6884,7 @@
         <v>104</v>
       </c>
       <c r="E60" s="30" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>171</v>
@@ -6908,10 +6908,10 @@
         <v>8</v>
       </c>
       <c r="M60" s="6" t="s">
+        <v>510</v>
+      </c>
+      <c r="N60" s="6" t="s">
         <v>511</v>
-      </c>
-      <c r="N60" s="6" t="s">
-        <v>512</v>
       </c>
       <c r="P60" s="6" t="s">
         <v>17</v>
@@ -6946,7 +6946,7 @@
         <v>104</v>
       </c>
       <c r="E61" s="30" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>172</v>
@@ -6970,10 +6970,10 @@
         <v>8</v>
       </c>
       <c r="M61" s="6" t="s">
+        <v>510</v>
+      </c>
+      <c r="N61" s="6" t="s">
         <v>511</v>
-      </c>
-      <c r="N61" s="6" t="s">
-        <v>512</v>
       </c>
       <c r="P61" s="6" t="s">
         <v>17</v>
@@ -7008,10 +7008,10 @@
         <v>104</v>
       </c>
       <c r="E62" s="30" t="s">
+        <v>660</v>
+      </c>
+      <c r="F62" s="5" t="s">
         <v>661</v>
-      </c>
-      <c r="F62" s="5" t="s">
-        <v>662</v>
       </c>
       <c r="G62" s="6" t="s">
         <v>399</v>
@@ -7032,10 +7032,10 @@
         <v>8</v>
       </c>
       <c r="M62" s="6" t="s">
+        <v>510</v>
+      </c>
+      <c r="N62" s="6" t="s">
         <v>511</v>
-      </c>
-      <c r="N62" s="6" t="s">
-        <v>512</v>
       </c>
       <c r="P62" s="6" t="s">
         <v>17</v>
@@ -7070,7 +7070,7 @@
         <v>3</v>
       </c>
       <c r="E63" s="30" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F63" s="6" t="s">
         <v>53</v>
@@ -7135,7 +7135,7 @@
         <v>3</v>
       </c>
       <c r="E64" s="30" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F64" s="6" t="s">
         <v>300</v>
@@ -7168,7 +7168,7 @@
         <v>54</v>
       </c>
       <c r="P64" s="13" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="Q64" s="6">
         <v>1</v>
@@ -7200,7 +7200,7 @@
         <v>3</v>
       </c>
       <c r="E65" s="30" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F65" s="6" t="s">
         <v>55</v>
@@ -7209,7 +7209,7 @@
         <v>402</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="I65" s="6" t="s">
         <v>5</v>
@@ -7233,7 +7233,7 @@
         <v>54</v>
       </c>
       <c r="P65" s="13" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="Q65" s="6">
         <v>0</v>
@@ -7274,7 +7274,7 @@
         <v>403</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="I66" s="6" t="s">
         <v>5</v>
@@ -7298,7 +7298,7 @@
         <v>54</v>
       </c>
       <c r="P66" s="13" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="Q66" s="6">
         <v>1</v>
@@ -7330,7 +7330,7 @@
         <v>3</v>
       </c>
       <c r="E67" s="30" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="F67" s="6" t="s">
         <v>57</v>
@@ -7339,7 +7339,7 @@
         <v>404</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="I67" s="6" t="s">
         <v>5</v>
@@ -7395,16 +7395,16 @@
         <v>3</v>
       </c>
       <c r="E68" s="30" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F68" s="6" t="s">
         <v>58</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="H68" s="6" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="I68" s="6" t="s">
         <v>5</v>
@@ -7460,7 +7460,7 @@
         <v>3</v>
       </c>
       <c r="E69" s="30" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="F69" s="6" t="s">
         <v>299</v>
@@ -7493,7 +7493,7 @@
         <v>54</v>
       </c>
       <c r="P69" s="13" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="Q69" s="6">
         <v>0</v>
@@ -7525,7 +7525,7 @@
         <v>59</v>
       </c>
       <c r="E70" s="30" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F70" s="6" t="s">
         <v>60</v>
@@ -7534,7 +7534,7 @@
         <v>405</v>
       </c>
       <c r="H70" s="6" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="I70" s="6" t="s">
         <v>5</v>
@@ -7590,7 +7590,7 @@
         <v>59</v>
       </c>
       <c r="E71" s="30" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>164</v>
@@ -7599,7 +7599,7 @@
         <v>406</v>
       </c>
       <c r="H71" s="6" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I71" s="6" t="s">
         <v>5</v>
@@ -7655,7 +7655,7 @@
         <v>59</v>
       </c>
       <c r="E72" s="30" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="F72" s="6" t="s">
         <v>62</v>
@@ -7664,7 +7664,7 @@
         <v>407</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="I72" s="6" t="s">
         <v>5</v>
@@ -7720,7 +7720,7 @@
         <v>59</v>
       </c>
       <c r="E73" s="30" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="F73" s="6" t="s">
         <v>63</v>
@@ -7729,7 +7729,7 @@
         <v>408</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I73" s="6" t="s">
         <v>5</v>
@@ -7785,7 +7785,7 @@
         <v>59</v>
       </c>
       <c r="E74" s="30" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="F74" s="6" t="s">
         <v>165</v>
@@ -7794,7 +7794,7 @@
         <v>409</v>
       </c>
       <c r="H74" s="6" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I74" s="6" t="s">
         <v>5</v>
@@ -7850,7 +7850,7 @@
         <v>59</v>
       </c>
       <c r="E75" s="30" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F75" s="6" t="s">
         <v>166</v>
@@ -7859,7 +7859,7 @@
         <v>410</v>
       </c>
       <c r="H75" s="6" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I75" s="6" t="s">
         <v>5</v>
@@ -7915,7 +7915,7 @@
         <v>59</v>
       </c>
       <c r="E76" s="30" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F76" s="6" t="s">
         <v>167</v>
@@ -7924,7 +7924,7 @@
         <v>411</v>
       </c>
       <c r="H76" s="6" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I76" s="6" t="s">
         <v>5</v>
@@ -7980,7 +7980,7 @@
         <v>59</v>
       </c>
       <c r="E77" s="30" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F77" s="6" t="s">
         <v>168</v>
@@ -7989,7 +7989,7 @@
         <v>412</v>
       </c>
       <c r="H77" s="6" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="I77" s="6" t="s">
         <v>5</v>
@@ -8045,7 +8045,7 @@
         <v>59</v>
       </c>
       <c r="E78" s="30" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="F78" s="6" t="s">
         <v>64</v>
@@ -8054,7 +8054,7 @@
         <v>413</v>
       </c>
       <c r="H78" s="6" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="I78" s="6" t="s">
         <v>5</v>
@@ -8110,7 +8110,7 @@
         <v>59</v>
       </c>
       <c r="E79" s="30" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F79" s="6" t="s">
         <v>65</v>
@@ -8119,7 +8119,7 @@
         <v>414</v>
       </c>
       <c r="H79" s="6" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I79" s="6" t="s">
         <v>5</v>
@@ -8175,7 +8175,7 @@
         <v>59</v>
       </c>
       <c r="E80" s="30" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="F80" s="6" t="s">
         <v>66</v>
@@ -8184,7 +8184,7 @@
         <v>415</v>
       </c>
       <c r="H80" s="6" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="I80" s="6" t="s">
         <v>5</v>
@@ -8240,7 +8240,7 @@
         <v>59</v>
       </c>
       <c r="E81" s="30" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="F81" s="6" t="s">
         <v>67</v>
@@ -8249,7 +8249,7 @@
         <v>416</v>
       </c>
       <c r="H81" s="6" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="I81" s="6" t="s">
         <v>5</v>
@@ -8305,13 +8305,13 @@
         <v>59</v>
       </c>
       <c r="E82" s="30" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="F82" s="6" t="s">
         <v>68</v>
       </c>
       <c r="G82" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="H82" s="6" t="s">
         <v>160</v>
@@ -8370,7 +8370,7 @@
         <v>104</v>
       </c>
       <c r="E83" s="30" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="F83" s="31" t="s">
         <v>132</v>
@@ -8388,16 +8388,16 @@
         <v>6</v>
       </c>
       <c r="K83" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="L83" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M83" s="6" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="N83" s="6" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="P83" s="6" t="s">
         <v>17</v>
@@ -8432,7 +8432,7 @@
         <v>104</v>
       </c>
       <c r="E84" s="30" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="F84" s="31" t="s">
         <v>134</v>
@@ -8456,10 +8456,10 @@
         <v>8</v>
       </c>
       <c r="M84" s="6" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="N84" s="6" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="O84" s="6"/>
       <c r="P84" s="6" t="s">
@@ -8509,7 +8509,7 @@
         <v>104</v>
       </c>
       <c r="E85" s="30" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="F85" s="31" t="s">
         <v>136</v>
@@ -8518,7 +8518,7 @@
         <v>419</v>
       </c>
       <c r="H85" s="6" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I85" s="6" t="s">
         <v>5</v>
@@ -8527,16 +8527,16 @@
         <v>6</v>
       </c>
       <c r="K85" s="6" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="L85" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M85" s="6" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="N85" s="6" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="O85" s="6"/>
       <c r="P85" s="6" t="s">
@@ -8586,13 +8586,13 @@
         <v>104</v>
       </c>
       <c r="E86" s="30" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="F86" s="6" t="s">
         <v>137</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H86" s="6" t="s">
         <v>138</v>
@@ -8610,10 +8610,10 @@
         <v>8</v>
       </c>
       <c r="M86" s="6" t="s">
+        <v>508</v>
+      </c>
+      <c r="N86" s="6" t="s">
         <v>509</v>
-      </c>
-      <c r="N86" s="6" t="s">
-        <v>510</v>
       </c>
       <c r="P86" s="6" t="s">
         <v>17</v>
@@ -8648,16 +8648,16 @@
         <v>104</v>
       </c>
       <c r="E87" s="30" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F87" s="19" t="s">
         <v>333</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="I87" s="7" t="s">
         <v>237</v>
@@ -8672,10 +8672,10 @@
         <v>8</v>
       </c>
       <c r="M87" s="7" t="s">
+        <v>703</v>
+      </c>
+      <c r="N87" s="7" t="s">
         <v>704</v>
-      </c>
-      <c r="N87" s="7" t="s">
-        <v>705</v>
       </c>
       <c r="O87" s="6"/>
       <c r="P87" s="6" t="s">
@@ -8725,16 +8725,16 @@
         <v>104</v>
       </c>
       <c r="E88" s="32" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="F88" s="19" t="s">
         <v>334</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="H88" s="7" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="I88" s="7" t="s">
         <v>240</v>
@@ -8749,10 +8749,10 @@
         <v>8</v>
       </c>
       <c r="M88" s="7" t="s">
+        <v>703</v>
+      </c>
+      <c r="N88" s="7" t="s">
         <v>704</v>
-      </c>
-      <c r="N88" s="7" t="s">
-        <v>705</v>
       </c>
       <c r="P88" s="6" t="s">
         <v>17</v>
@@ -8787,16 +8787,16 @@
         <v>104</v>
       </c>
       <c r="E89" s="30" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="F89" s="19" t="s">
         <v>242</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="H89" s="7" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="I89" s="7" t="s">
         <v>237</v>
@@ -8811,10 +8811,10 @@
         <v>8</v>
       </c>
       <c r="M89" s="7" t="s">
+        <v>703</v>
+      </c>
+      <c r="N89" s="7" t="s">
         <v>704</v>
-      </c>
-      <c r="N89" s="7" t="s">
-        <v>705</v>
       </c>
       <c r="O89" s="7"/>
       <c r="P89" s="7" t="s">
@@ -8864,16 +8864,16 @@
         <v>104</v>
       </c>
       <c r="E90" s="30" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="F90" s="20" t="s">
         <v>245</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="H90" s="7" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="I90" s="7" t="s">
         <v>240</v>
@@ -8888,10 +8888,10 @@
         <v>8</v>
       </c>
       <c r="M90" s="7" t="s">
+        <v>703</v>
+      </c>
+      <c r="N90" s="7" t="s">
         <v>704</v>
-      </c>
-      <c r="N90" s="7" t="s">
-        <v>705</v>
       </c>
       <c r="O90" s="7"/>
       <c r="P90" s="7" t="s">
@@ -8941,16 +8941,16 @@
         <v>303</v>
       </c>
       <c r="E91" s="30" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="F91" s="2" t="s">
+        <v>733</v>
+      </c>
+      <c r="G91" s="6" t="s">
+        <v>445</v>
+      </c>
+      <c r="H91" s="2" t="s">
         <v>734</v>
-      </c>
-      <c r="G91" s="6" t="s">
-        <v>446</v>
-      </c>
-      <c r="H91" s="2" t="s">
-        <v>735</v>
       </c>
       <c r="I91" s="7" t="s">
         <v>5</v>
@@ -9015,16 +9015,16 @@
         <v>2</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="F92" s="6" t="s">
+        <v>737</v>
+      </c>
+      <c r="G92" s="6" t="s">
         <v>738</v>
-      </c>
-      <c r="G92" s="6" t="s">
-        <v>420</v>
       </c>
       <c r="H92" s="6" t="s">
         <v>190</v>
@@ -9049,7 +9049,7 @@
       </c>
       <c r="O92" s="6"/>
       <c r="P92" s="6" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="Q92" s="6">
         <v>1</v>
@@ -9092,7 +9092,7 @@
         <v>2</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E93" s="30" t="s">
         <v>71</v>
@@ -9101,10 +9101,10 @@
         <v>71</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H93" s="6" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="I93" s="6" t="s">
         <v>191</v>
@@ -9126,7 +9126,7 @@
       </c>
       <c r="O93" s="6"/>
       <c r="P93" s="6" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="Q93" s="6">
         <v>1</v>
@@ -9169,19 +9169,19 @@
         <v>2</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E94" s="30" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>292</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="I94" s="11" t="s">
         <v>293</v>
@@ -9190,7 +9190,7 @@
         <v>6</v>
       </c>
       <c r="K94" s="11" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="L94" s="11" t="s">
         <v>8</v>
@@ -9246,10 +9246,10 @@
         <v>2</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E95" s="30" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="F95" s="12" t="s">
         <v>196</v>
@@ -9258,7 +9258,7 @@
         <v>197</v>
       </c>
       <c r="H95" s="11" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="I95" s="11" t="s">
         <v>198</v>
@@ -9267,7 +9267,7 @@
         <v>6</v>
       </c>
       <c r="K95" s="11" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="L95" s="11" t="s">
         <v>8</v>
@@ -9308,10 +9308,10 @@
         <v>2</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E96" s="30" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F96" s="12" t="s">
         <v>230</v>
@@ -9320,7 +9320,7 @@
         <v>202</v>
       </c>
       <c r="H96" s="11" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I96" s="11" t="s">
         <v>198</v>
@@ -9329,7 +9329,7 @@
         <v>6</v>
       </c>
       <c r="K96" s="11" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="L96" s="11" t="s">
         <v>8</v>
@@ -9370,10 +9370,10 @@
         <v>2</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E97" s="30" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="F97" s="12" t="s">
         <v>335</v>
@@ -9382,7 +9382,7 @@
         <v>203</v>
       </c>
       <c r="H97" s="11" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="I97" s="11" t="s">
         <v>198</v>
@@ -9391,7 +9391,7 @@
         <v>6</v>
       </c>
       <c r="K97" s="11" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="L97" s="11" t="s">
         <v>8</v>
@@ -9432,10 +9432,10 @@
         <v>2</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E98" s="30" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F98" s="12" t="s">
         <v>231</v>
@@ -9444,7 +9444,7 @@
         <v>204</v>
       </c>
       <c r="H98" s="11" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="I98" s="11" t="s">
         <v>205</v>
@@ -9453,7 +9453,7 @@
         <v>6</v>
       </c>
       <c r="K98" s="11" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="L98" s="11" t="s">
         <v>8</v>
@@ -9494,10 +9494,10 @@
         <v>2</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E99" s="30" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="F99" s="12" t="s">
         <v>206</v>
@@ -9506,7 +9506,7 @@
         <v>207</v>
       </c>
       <c r="H99" s="11" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="I99" s="11" t="s">
         <v>208</v>
@@ -9515,7 +9515,7 @@
         <v>6</v>
       </c>
       <c r="K99" s="11" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="L99" s="11" t="s">
         <v>8</v>
@@ -9556,10 +9556,10 @@
         <v>2</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E100" s="30" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="F100" s="12" t="s">
         <v>224</v>
@@ -9568,7 +9568,7 @@
         <v>213</v>
       </c>
       <c r="H100" s="11" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="I100" s="11" t="s">
         <v>214</v>
@@ -9577,7 +9577,7 @@
         <v>6</v>
       </c>
       <c r="K100" s="11" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="L100" s="11" t="s">
         <v>8</v>
@@ -9618,10 +9618,10 @@
         <v>2</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E101" s="30" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="F101" s="12" t="s">
         <v>225</v>
@@ -9630,7 +9630,7 @@
         <v>216</v>
       </c>
       <c r="H101" s="11" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I101" s="11" t="s">
         <v>214</v>
@@ -9639,7 +9639,7 @@
         <v>6</v>
       </c>
       <c r="K101" s="11" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="L101" s="11" t="s">
         <v>8</v>
@@ -9680,10 +9680,10 @@
         <v>2</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E102" s="30" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="F102" s="12" t="s">
         <v>226</v>
@@ -9692,7 +9692,7 @@
         <v>217</v>
       </c>
       <c r="H102" s="11" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="I102" s="11" t="s">
         <v>214</v>
@@ -9701,7 +9701,7 @@
         <v>6</v>
       </c>
       <c r="K102" s="11" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="L102" s="11" t="s">
         <v>8</v>
@@ -9742,10 +9742,10 @@
         <v>2</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E103" s="30" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="F103" s="12" t="s">
         <v>227</v>
@@ -9754,7 +9754,7 @@
         <v>218</v>
       </c>
       <c r="H103" s="11" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="I103" s="11" t="s">
         <v>214</v>
@@ -9763,7 +9763,7 @@
         <v>6</v>
       </c>
       <c r="K103" s="11" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="L103" s="11" t="s">
         <v>8</v>
@@ -9819,10 +9819,10 @@
         <v>2</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E104" s="30" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F104" s="12" t="s">
         <v>228</v>
@@ -9831,7 +9831,7 @@
         <v>219</v>
       </c>
       <c r="H104" s="11" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="I104" s="11" t="s">
         <v>214</v>
@@ -9840,7 +9840,7 @@
         <v>6</v>
       </c>
       <c r="K104" s="11" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="L104" s="11" t="s">
         <v>8</v>
@@ -9896,10 +9896,10 @@
         <v>2</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="E105" s="30" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="F105" s="12" t="s">
         <v>229</v>
@@ -9908,7 +9908,7 @@
         <v>220</v>
       </c>
       <c r="H105" s="11" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="I105" s="11" t="s">
         <v>214</v>
@@ -9917,7 +9917,7 @@
         <v>6</v>
       </c>
       <c r="K105" s="11" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="L105" s="11" t="s">
         <v>8</v>
@@ -9976,13 +9976,13 @@
         <v>3</v>
       </c>
       <c r="E106" s="30" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="F106" s="21" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="G106" s="6" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="H106" s="7" t="s">
         <v>257</v>
@@ -10000,10 +10000,10 @@
         <v>8</v>
       </c>
       <c r="M106" s="7" t="s">
+        <v>703</v>
+      </c>
+      <c r="N106" s="7" t="s">
         <v>704</v>
-      </c>
-      <c r="N106" s="7" t="s">
-        <v>705</v>
       </c>
       <c r="P106" s="7" t="s">
         <v>244</v>
@@ -10038,13 +10038,13 @@
         <v>3</v>
       </c>
       <c r="E107" s="30" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="F107" s="8" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="H107" s="7" t="s">
         <v>259</v>
@@ -10062,10 +10062,10 @@
         <v>8</v>
       </c>
       <c r="M107" s="7" t="s">
+        <v>703</v>
+      </c>
+      <c r="N107" s="7" t="s">
         <v>704</v>
-      </c>
-      <c r="N107" s="7" t="s">
-        <v>705</v>
       </c>
       <c r="P107" s="7" t="s">
         <v>244</v>
@@ -10100,13 +10100,13 @@
         <v>3</v>
       </c>
       <c r="E108" s="30" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="F108" s="8" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="G108" s="6" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H108" s="7" t="s">
         <v>261</v>
@@ -10124,10 +10124,10 @@
         <v>8</v>
       </c>
       <c r="M108" s="7" t="s">
+        <v>703</v>
+      </c>
+      <c r="N108" s="7" t="s">
         <v>704</v>
-      </c>
-      <c r="N108" s="7" t="s">
-        <v>705</v>
       </c>
       <c r="P108" s="7" t="s">
         <v>244</v>
@@ -10162,13 +10162,13 @@
         <v>3</v>
       </c>
       <c r="E109" s="30" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="F109" s="8" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="G109" s="6" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="H109" s="7" t="s">
         <v>267</v>
@@ -10186,10 +10186,10 @@
         <v>8</v>
       </c>
       <c r="M109" s="7" t="s">
+        <v>703</v>
+      </c>
+      <c r="N109" s="7" t="s">
         <v>704</v>
-      </c>
-      <c r="N109" s="7" t="s">
-        <v>705</v>
       </c>
       <c r="O109" s="7"/>
       <c r="P109" s="7" t="s">
@@ -10239,13 +10239,13 @@
         <v>3</v>
       </c>
       <c r="E110" s="30" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="F110" s="22" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="G110" s="6" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="H110" s="7" t="s">
         <v>263</v>
@@ -10263,10 +10263,10 @@
         <v>8</v>
       </c>
       <c r="M110" s="7" t="s">
+        <v>703</v>
+      </c>
+      <c r="N110" s="7" t="s">
         <v>704</v>
-      </c>
-      <c r="N110" s="7" t="s">
-        <v>705</v>
       </c>
       <c r="P110" s="7" t="s">
         <v>244</v>
@@ -10301,13 +10301,13 @@
         <v>3</v>
       </c>
       <c r="E111" s="30" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="F111" s="22" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="G111" s="6" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="H111" s="7" t="s">
         <v>265</v>
@@ -10325,10 +10325,10 @@
         <v>8</v>
       </c>
       <c r="M111" s="7" t="s">
+        <v>703</v>
+      </c>
+      <c r="N111" s="7" t="s">
         <v>704</v>
-      </c>
-      <c r="N111" s="7" t="s">
-        <v>705</v>
       </c>
       <c r="O111" s="7"/>
       <c r="P111" s="7" t="s">
@@ -10378,13 +10378,13 @@
         <v>3</v>
       </c>
       <c r="E112" s="30" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="F112" s="7" t="s">
         <v>246</v>
       </c>
       <c r="G112" s="6" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="H112" s="7" t="s">
         <v>247</v>
@@ -10402,10 +10402,10 @@
         <v>8</v>
       </c>
       <c r="M112" s="7" t="s">
+        <v>703</v>
+      </c>
+      <c r="N112" s="7" t="s">
         <v>704</v>
-      </c>
-      <c r="N112" s="7" t="s">
-        <v>705</v>
       </c>
       <c r="P112" s="7" t="s">
         <v>244</v>
@@ -10440,13 +10440,13 @@
         <v>3</v>
       </c>
       <c r="E113" s="30" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="F113" s="7" t="s">
         <v>249</v>
       </c>
       <c r="G113" s="6" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="H113" s="7" t="s">
         <v>250</v>
@@ -10464,10 +10464,10 @@
         <v>8</v>
       </c>
       <c r="M113" s="7" t="s">
+        <v>703</v>
+      </c>
+      <c r="N113" s="7" t="s">
         <v>704</v>
-      </c>
-      <c r="N113" s="7" t="s">
-        <v>705</v>
       </c>
       <c r="P113" s="7" t="s">
         <v>244</v>
@@ -10502,13 +10502,13 @@
         <v>3</v>
       </c>
       <c r="E114" s="30" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F114" s="7" t="s">
         <v>251</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="H114" s="7" t="s">
         <v>252</v>
@@ -10526,10 +10526,10 @@
         <v>8</v>
       </c>
       <c r="M114" s="7" t="s">
+        <v>703</v>
+      </c>
+      <c r="N114" s="7" t="s">
         <v>704</v>
-      </c>
-      <c r="N114" s="7" t="s">
-        <v>705</v>
       </c>
       <c r="P114" s="7" t="s">
         <v>244</v>
@@ -10564,13 +10564,13 @@
         <v>15</v>
       </c>
       <c r="E115" s="30" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F115" s="21" t="s">
         <v>253</v>
       </c>
       <c r="G115" s="6" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="H115" s="7" t="s">
         <v>254</v>
@@ -10588,10 +10588,10 @@
         <v>8</v>
       </c>
       <c r="M115" s="7" t="s">
+        <v>703</v>
+      </c>
+      <c r="N115" s="7" t="s">
         <v>704</v>
-      </c>
-      <c r="N115" s="7" t="s">
-        <v>705</v>
       </c>
       <c r="P115" s="7" t="s">
         <v>244</v>
@@ -10626,16 +10626,16 @@
         <v>15</v>
       </c>
       <c r="E116" s="30" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="F116" s="8" t="s">
         <v>270</v>
       </c>
       <c r="G116" s="6" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="H116" s="7" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="I116" s="7" t="s">
         <v>5</v>
@@ -10650,10 +10650,10 @@
         <v>8</v>
       </c>
       <c r="M116" s="7" t="s">
+        <v>703</v>
+      </c>
+      <c r="N116" s="7" t="s">
         <v>704</v>
-      </c>
-      <c r="N116" s="7" t="s">
-        <v>705</v>
       </c>
       <c r="O116" s="7"/>
       <c r="P116" s="7" t="s">
@@ -10703,16 +10703,16 @@
         <v>15</v>
       </c>
       <c r="E117" s="30" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="F117" s="2" t="s">
         <v>294</v>
       </c>
       <c r="G117" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H117" s="2" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I117" s="11" t="s">
         <v>5</v>
@@ -10721,7 +10721,7 @@
         <v>6</v>
       </c>
       <c r="K117" s="11" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="L117" s="11" t="s">
         <v>8</v>
@@ -10780,7 +10780,7 @@
         <v>15</v>
       </c>
       <c r="E118" s="30" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="F118" s="12" t="s">
         <v>209</v>
@@ -10789,7 +10789,7 @@
         <v>221</v>
       </c>
       <c r="H118" s="11" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="I118" s="11" t="s">
         <v>210</v>
@@ -10798,7 +10798,7 @@
         <v>6</v>
       </c>
       <c r="K118" s="11" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="L118" s="11" t="s">
         <v>8</v>
@@ -10842,7 +10842,7 @@
         <v>15</v>
       </c>
       <c r="E119" s="30" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="F119" s="12" t="s">
         <v>211</v>
@@ -10851,7 +10851,7 @@
         <v>222</v>
       </c>
       <c r="H119" s="11" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="I119" s="11" t="s">
         <v>210</v>
@@ -10860,7 +10860,7 @@
         <v>6</v>
       </c>
       <c r="K119" s="11" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="L119" s="11" t="s">
         <v>8</v>
@@ -10904,7 +10904,7 @@
         <v>15</v>
       </c>
       <c r="E120" s="30" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="F120" s="12" t="s">
         <v>212</v>
@@ -10913,7 +10913,7 @@
         <v>223</v>
       </c>
       <c r="H120" s="11" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I120" s="11" t="s">
         <v>210</v>
@@ -10922,7 +10922,7 @@
         <v>6</v>
       </c>
       <c r="K120" s="11" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="L120" s="11" t="s">
         <v>8</v>
@@ -10966,16 +10966,16 @@
         <v>15</v>
       </c>
       <c r="E121" s="30" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F121" s="7" t="s">
         <v>269</v>
       </c>
       <c r="G121" s="6" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="H121" s="7" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="I121" s="7" t="s">
         <v>5</v>
@@ -10990,10 +10990,10 @@
         <v>8</v>
       </c>
       <c r="M121" s="7" t="s">
+        <v>703</v>
+      </c>
+      <c r="N121" s="7" t="s">
         <v>704</v>
-      </c>
-      <c r="N121" s="7" t="s">
-        <v>705</v>
       </c>
       <c r="O121" s="7"/>
       <c r="P121" s="7" t="s">
@@ -11040,10 +11040,10 @@
         <v>2</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E122" s="30" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F122" s="33" t="s">
         <v>271</v>
@@ -11100,10 +11100,10 @@
         <v>2</v>
       </c>
       <c r="D123" s="6" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E123" s="30" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F123" s="33" t="s">
         <v>336</v>
@@ -11160,10 +11160,10 @@
         <v>2</v>
       </c>
       <c r="D124" s="6" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E124" s="30" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="F124" s="33" t="s">
         <v>278</v>
@@ -11220,10 +11220,10 @@
         <v>2</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E125" s="30" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F125" s="33" t="s">
         <v>281</v>
@@ -11295,19 +11295,19 @@
         <v>2</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E126" s="30" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="F126" s="33" t="s">
         <v>284</v>
       </c>
       <c r="G126" s="6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="H126" s="23" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="I126" s="23"/>
       <c r="J126" s="7" t="s">
@@ -11370,10 +11370,10 @@
         <v>2</v>
       </c>
       <c r="D127" s="6" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E127" s="30" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="F127" s="33" t="s">
         <v>285</v>
@@ -11444,10 +11444,10 @@
         <v>2</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E128" s="32" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="F128" s="33" t="s">
         <v>289</v>
@@ -11524,19 +11524,19 @@
         <v>3</v>
       </c>
       <c r="E129" s="32" t="s">
+        <v>683</v>
+      </c>
+      <c r="F129" s="36" t="s">
         <v>684</v>
       </c>
-      <c r="F129" s="36" t="s">
-        <v>685</v>
-      </c>
       <c r="G129" s="6" t="s">
+        <v>717</v>
+      </c>
+      <c r="H129" s="7" t="s">
         <v>718</v>
       </c>
-      <c r="H129" s="7" t="s">
-        <v>719</v>
-      </c>
       <c r="I129" s="23" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="J129" s="7" t="s">
         <v>6</v>
@@ -11601,19 +11601,19 @@
         <v>3</v>
       </c>
       <c r="E130" s="32" t="s">
+        <v>685</v>
+      </c>
+      <c r="F130" s="36" t="s">
         <v>686</v>
       </c>
-      <c r="F130" s="36" t="s">
-        <v>687</v>
-      </c>
       <c r="G130" s="6" t="s">
+        <v>719</v>
+      </c>
+      <c r="H130" s="7" t="s">
         <v>720</v>
       </c>
-      <c r="H130" s="7" t="s">
-        <v>721</v>
-      </c>
       <c r="I130" s="23" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="J130" s="7" t="s">
         <v>6</v>
@@ -11678,19 +11678,19 @@
         <v>3</v>
       </c>
       <c r="E131" s="32" t="s">
+        <v>687</v>
+      </c>
+      <c r="F131" s="36" t="s">
         <v>688</v>
       </c>
-      <c r="F131" s="36" t="s">
-        <v>689</v>
-      </c>
       <c r="G131" s="6" t="s">
+        <v>721</v>
+      </c>
+      <c r="H131" s="7" t="s">
         <v>722</v>
       </c>
-      <c r="H131" s="7" t="s">
-        <v>723</v>
-      </c>
       <c r="I131" s="23" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="J131" s="7" t="s">
         <v>6</v>
@@ -11755,16 +11755,16 @@
         <v>3</v>
       </c>
       <c r="E132" s="32" t="s">
+        <v>689</v>
+      </c>
+      <c r="F132" s="36" t="s">
         <v>690</v>
       </c>
-      <c r="F132" s="36" t="s">
-        <v>691</v>
-      </c>
       <c r="G132" s="6" t="s">
+        <v>723</v>
+      </c>
+      <c r="H132" s="7" t="s">
         <v>724</v>
-      </c>
-      <c r="H132" s="7" t="s">
-        <v>725</v>
       </c>
       <c r="I132" s="23" t="s">
         <v>5</v>
@@ -11832,16 +11832,16 @@
         <v>3</v>
       </c>
       <c r="E133" s="32" t="s">
+        <v>691</v>
+      </c>
+      <c r="F133" s="36" t="s">
         <v>692</v>
       </c>
-      <c r="F133" s="36" t="s">
-        <v>693</v>
-      </c>
       <c r="G133" s="6" t="s">
+        <v>725</v>
+      </c>
+      <c r="H133" s="7" t="s">
         <v>726</v>
-      </c>
-      <c r="H133" s="7" t="s">
-        <v>727</v>
       </c>
       <c r="I133" s="23" t="s">
         <v>5</v>
@@ -11909,16 +11909,16 @@
         <v>3</v>
       </c>
       <c r="E134" s="32" t="s">
+        <v>693</v>
+      </c>
+      <c r="F134" s="36" t="s">
         <v>694</v>
       </c>
-      <c r="F134" s="36" t="s">
-        <v>695</v>
-      </c>
       <c r="G134" s="6" t="s">
+        <v>727</v>
+      </c>
+      <c r="H134" s="7" t="s">
         <v>728</v>
-      </c>
-      <c r="H134" s="7" t="s">
-        <v>729</v>
       </c>
       <c r="I134" s="23" t="s">
         <v>5</v>
@@ -11986,16 +11986,16 @@
         <v>3</v>
       </c>
       <c r="E135" s="32" t="s">
+        <v>695</v>
+      </c>
+      <c r="F135" s="36" t="s">
         <v>696</v>
       </c>
-      <c r="F135" s="36" t="s">
-        <v>697</v>
-      </c>
       <c r="G135" s="6" t="s">
+        <v>729</v>
+      </c>
+      <c r="H135" s="7" t="s">
         <v>730</v>
-      </c>
-      <c r="H135" s="7" t="s">
-        <v>731</v>
       </c>
       <c r="I135" s="23" t="s">
         <v>5</v>
@@ -12063,16 +12063,16 @@
         <v>3</v>
       </c>
       <c r="E136" s="32" t="s">
+        <v>697</v>
+      </c>
+      <c r="F136" s="36" t="s">
         <v>698</v>
       </c>
-      <c r="F136" s="36" t="s">
-        <v>699</v>
-      </c>
       <c r="G136" s="6" t="s">
+        <v>731</v>
+      </c>
+      <c r="H136" s="7" t="s">
         <v>732</v>
-      </c>
-      <c r="H136" s="7" t="s">
-        <v>733</v>
       </c>
       <c r="I136" s="23" t="s">
         <v>5</v>
@@ -12324,42 +12324,42 @@
     </row>
     <row r="17" spans="1:2" ht="17.25" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="17.25" customHeight="1">
       <c r="A18" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>675</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>676</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="17.25" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="17.25" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="17.25" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="17.25" customHeight="1">

</xml_diff>

<commit_message>
Corrección dato iq salud SINADI
</commit_message>
<xml_diff>
--- a/Data/Base_fichas_indicadores.xlsx
+++ b/Data/Base_fichas_indicadores.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1992" uniqueCount="739">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1992" uniqueCount="741">
   <si>
     <t>id</t>
   </si>
@@ -2141,9 +2141,6 @@
     <t>UMAD con base en SINADI - MSP (*2020 datos preliminares)</t>
   </si>
   <si>
-    <t>El indicador mide el promedio anual de consultas urgentes y no urgentes, en consultorio y en domicilio, por usuario. El Total SNIS es el promedio ponderado por cantidad de afiliados de cada tipo de prestador.</t>
-  </si>
-  <si>
     <t>El indicador mide el promedio anual de consultas no urgentes, en consultorio y en domicilio, por usuario. El Total SNIS es el promedio ponderado por cantidad de afiliados de cada tipo de prestador.</t>
   </si>
   <si>
@@ -2241,6 +2238,15 @@
   </si>
   <si>
     <t>El indicador refleja la distribución porcentual de personas según institución prestadora integral de salud en la cual tienen cobertura (derecho vigente según la pregunta específica de la ECH).</t>
+  </si>
+  <si>
+    <t>El indicador mide el promedio anual de consultas urgentes y no urgentes, en consultorio y en domicilio, por usuario. El Total SNIS es el promedio ponderado por cantidad de afiliados de cada tipo de prestador. Los datos de 2020 incluyen las consultas por telemedicina.</t>
+  </si>
+  <si>
+    <t>Observatorio Territorio Uruguay - OPP a partir de estimaciones de INE.</t>
+  </si>
+  <si>
+    <t>UMAD con base en Observatorio Territorio Uruguay - OPP a partir de estimaciones de INE.</t>
   </si>
 </sst>
 </file>
@@ -2780,9 +2786,9 @@
   <dimension ref="A1:AI140"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="G1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E111" sqref="E111"/>
-      <selection pane="bottomLeft" activeCell="G107" sqref="G106:G107"/>
+      <selection pane="bottomLeft" activeCell="G92" sqref="G92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -8944,13 +8950,13 @@
         <v>599</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="G91" s="6" t="s">
         <v>445</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="I91" s="7" t="s">
         <v>5</v>
@@ -9021,10 +9027,10 @@
         <v>626</v>
       </c>
       <c r="F92" s="6" t="s">
+        <v>736</v>
+      </c>
+      <c r="G92" s="6" t="s">
         <v>737</v>
-      </c>
-      <c r="G92" s="6" t="s">
-        <v>738</v>
       </c>
       <c r="H92" s="6" t="s">
         <v>190</v>
@@ -9119,10 +9125,10 @@
         <v>8</v>
       </c>
       <c r="M93" s="7" t="s">
-        <v>193</v>
+        <v>739</v>
       </c>
       <c r="N93" s="6" t="s">
-        <v>195</v>
+        <v>740</v>
       </c>
       <c r="O93" s="6"/>
       <c r="P93" s="6" t="s">
@@ -9190,7 +9196,7 @@
         <v>6</v>
       </c>
       <c r="K94" s="11" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="L94" s="11" t="s">
         <v>8</v>
@@ -9267,7 +9273,7 @@
         <v>6</v>
       </c>
       <c r="K95" s="11" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="L95" s="11" t="s">
         <v>8</v>
@@ -9329,7 +9335,7 @@
         <v>6</v>
       </c>
       <c r="K96" s="11" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="L96" s="11" t="s">
         <v>8</v>
@@ -9391,7 +9397,7 @@
         <v>6</v>
       </c>
       <c r="K97" s="11" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="L97" s="11" t="s">
         <v>8</v>
@@ -9453,7 +9459,7 @@
         <v>6</v>
       </c>
       <c r="K98" s="11" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="L98" s="11" t="s">
         <v>8</v>
@@ -9515,7 +9521,7 @@
         <v>6</v>
       </c>
       <c r="K99" s="11" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="L99" s="11" t="s">
         <v>8</v>
@@ -9577,7 +9583,7 @@
         <v>6</v>
       </c>
       <c r="K100" s="11" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="L100" s="11" t="s">
         <v>8</v>
@@ -9639,7 +9645,7 @@
         <v>6</v>
       </c>
       <c r="K101" s="11" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="L101" s="11" t="s">
         <v>8</v>
@@ -9701,7 +9707,7 @@
         <v>6</v>
       </c>
       <c r="K102" s="11" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="L102" s="11" t="s">
         <v>8</v>
@@ -9763,7 +9769,7 @@
         <v>6</v>
       </c>
       <c r="K103" s="11" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="L103" s="11" t="s">
         <v>8</v>
@@ -9840,7 +9846,7 @@
         <v>6</v>
       </c>
       <c r="K104" s="11" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="L104" s="11" t="s">
         <v>8</v>
@@ -9917,7 +9923,7 @@
         <v>6</v>
       </c>
       <c r="K105" s="11" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="L105" s="11" t="s">
         <v>8</v>
@@ -9982,7 +9988,7 @@
         <v>649</v>
       </c>
       <c r="G106" s="6" t="s">
-        <v>705</v>
+        <v>738</v>
       </c>
       <c r="H106" s="7" t="s">
         <v>257</v>
@@ -10044,7 +10050,7 @@
         <v>650</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="H107" s="7" t="s">
         <v>259</v>
@@ -10106,7 +10112,7 @@
         <v>651</v>
       </c>
       <c r="G108" s="6" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="H108" s="7" t="s">
         <v>261</v>
@@ -10168,7 +10174,7 @@
         <v>652</v>
       </c>
       <c r="G109" s="6" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="H109" s="7" t="s">
         <v>267</v>
@@ -10245,7 +10251,7 @@
         <v>653</v>
       </c>
       <c r="G110" s="6" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="H110" s="7" t="s">
         <v>263</v>
@@ -10307,7 +10313,7 @@
         <v>654</v>
       </c>
       <c r="G111" s="6" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="H111" s="7" t="s">
         <v>265</v>
@@ -10384,7 +10390,7 @@
         <v>246</v>
       </c>
       <c r="G112" s="6" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="H112" s="7" t="s">
         <v>247</v>
@@ -10446,7 +10452,7 @@
         <v>249</v>
       </c>
       <c r="G113" s="6" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="H113" s="7" t="s">
         <v>250</v>
@@ -10508,7 +10514,7 @@
         <v>251</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="H114" s="7" t="s">
         <v>252</v>
@@ -10570,7 +10576,7 @@
         <v>253</v>
       </c>
       <c r="G115" s="6" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="H115" s="7" t="s">
         <v>254</v>
@@ -10632,7 +10638,7 @@
         <v>270</v>
       </c>
       <c r="G116" s="6" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="H116" s="7" t="s">
         <v>488</v>
@@ -10721,7 +10727,7 @@
         <v>6</v>
       </c>
       <c r="K117" s="11" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="L117" s="11" t="s">
         <v>8</v>
@@ -10798,7 +10804,7 @@
         <v>6</v>
       </c>
       <c r="K118" s="11" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="L118" s="11" t="s">
         <v>8</v>
@@ -10860,7 +10866,7 @@
         <v>6</v>
       </c>
       <c r="K119" s="11" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="L119" s="11" t="s">
         <v>8</v>
@@ -10922,7 +10928,7 @@
         <v>6</v>
       </c>
       <c r="K120" s="11" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="L120" s="11" t="s">
         <v>8</v>
@@ -10972,7 +10978,7 @@
         <v>269</v>
       </c>
       <c r="G121" s="6" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="H121" s="7" t="s">
         <v>487</v>
@@ -11530,10 +11536,10 @@
         <v>684</v>
       </c>
       <c r="G129" s="6" t="s">
+        <v>716</v>
+      </c>
+      <c r="H129" s="7" t="s">
         <v>717</v>
-      </c>
-      <c r="H129" s="7" t="s">
-        <v>718</v>
       </c>
       <c r="I129" s="23" t="s">
         <v>699</v>
@@ -11607,10 +11613,10 @@
         <v>686</v>
       </c>
       <c r="G130" s="6" t="s">
+        <v>718</v>
+      </c>
+      <c r="H130" s="7" t="s">
         <v>719</v>
-      </c>
-      <c r="H130" s="7" t="s">
-        <v>720</v>
       </c>
       <c r="I130" s="23" t="s">
         <v>699</v>
@@ -11684,10 +11690,10 @@
         <v>688</v>
       </c>
       <c r="G131" s="6" t="s">
+        <v>720</v>
+      </c>
+      <c r="H131" s="7" t="s">
         <v>721</v>
-      </c>
-      <c r="H131" s="7" t="s">
-        <v>722</v>
       </c>
       <c r="I131" s="23" t="s">
         <v>699</v>
@@ -11761,10 +11767,10 @@
         <v>690</v>
       </c>
       <c r="G132" s="6" t="s">
+        <v>722</v>
+      </c>
+      <c r="H132" s="7" t="s">
         <v>723</v>
-      </c>
-      <c r="H132" s="7" t="s">
-        <v>724</v>
       </c>
       <c r="I132" s="23" t="s">
         <v>5</v>
@@ -11838,10 +11844,10 @@
         <v>692</v>
       </c>
       <c r="G133" s="6" t="s">
+        <v>724</v>
+      </c>
+      <c r="H133" s="7" t="s">
         <v>725</v>
-      </c>
-      <c r="H133" s="7" t="s">
-        <v>726</v>
       </c>
       <c r="I133" s="23" t="s">
         <v>5</v>
@@ -11915,10 +11921,10 @@
         <v>694</v>
       </c>
       <c r="G134" s="6" t="s">
+        <v>726</v>
+      </c>
+      <c r="H134" s="7" t="s">
         <v>727</v>
-      </c>
-      <c r="H134" s="7" t="s">
-        <v>728</v>
       </c>
       <c r="I134" s="23" t="s">
         <v>5</v>
@@ -11992,10 +11998,10 @@
         <v>696</v>
       </c>
       <c r="G135" s="6" t="s">
+        <v>728</v>
+      </c>
+      <c r="H135" s="7" t="s">
         <v>729</v>
-      </c>
-      <c r="H135" s="7" t="s">
-        <v>730</v>
       </c>
       <c r="I135" s="23" t="s">
         <v>5</v>
@@ -12069,10 +12075,10 @@
         <v>698</v>
       </c>
       <c r="G136" s="6" t="s">
+        <v>730</v>
+      </c>
+      <c r="H136" s="7" t="s">
         <v>731</v>
-      </c>
-      <c r="H136" s="7" t="s">
-        <v>732</v>
       </c>
       <c r="I136" s="23" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
cambios nombre distribucion institucion prestadora
</commit_message>
<xml_diff>
--- a/Data/Base_fichas_indicadores.xlsx
+++ b/Data/Base_fichas_indicadores.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\DESCA-app\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marti\Dropbox\Trabajo\DESCA\DESCA-app\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89D923C-3B06-4231-A7A7-CD1AC685F8F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
+    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BASE_FICHAS" sheetId="4" r:id="rId1"/>
@@ -2234,12 +2235,6 @@
     <t>2000-2020</t>
   </si>
   <si>
-    <t>Distribución porcentual de personas según institución prestadora en la cual tienen cobertura vigente</t>
-  </si>
-  <si>
-    <t>El indicador refleja la distribución porcentual de personas según institución prestadora integral de salud en la cual tienen cobertura (derecho vigente según la pregunta específica de la ECH).</t>
-  </si>
-  <si>
     <t>El indicador mide el promedio anual de consultas urgentes y no urgentes, en consultorio y en domicilio, por usuario. El Total SNIS es el promedio ponderado por cantidad de afiliados de cada tipo de prestador. Los datos de 2020 incluyen las consultas por telemedicina.</t>
   </si>
   <si>
@@ -2247,12 +2242,18 @@
   </si>
   <si>
     <t>UMAD con base en Observatorio Territorio Uruguay - OPP a partir de estimaciones de INE.</t>
+  </si>
+  <si>
+    <t>Distribución porcentual de personas según institución prestadora en la cual declaran tener cobertura vigente</t>
+  </si>
+  <si>
+    <t>El indicador refleja la distribución porcentual de personas según institución prestadora integral de salud en la cual declaran tener cobertura (derecho vigente según la pregunta específica de la ECH).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.000&quot;&quot;;\-#,##0.000&quot;&quot;"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -2467,10 +2468,10 @@
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Excel Built-in Normal" xfId="3"/>
+    <cellStyle name="Excel Built-in Normal" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Normal_DISEÑO" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal_DISEÑO" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2781,42 +2782,42 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AI140"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" topLeftCell="G1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E111" sqref="E111"/>
-      <selection pane="bottomLeft" activeCell="G92" sqref="G92"/>
+      <selection pane="bottomLeft" activeCell="G93" sqref="G93"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="19.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" style="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="13" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" style="13" customWidth="1"/>
-    <col min="4" max="4" width="37.7109375" style="13" customWidth="1"/>
-    <col min="5" max="5" width="94.7109375" style="13" customWidth="1"/>
-    <col min="6" max="6" width="157.28515625" style="13" customWidth="1"/>
-    <col min="7" max="7" width="255.7109375" style="13" customWidth="1"/>
-    <col min="8" max="8" width="181.140625" style="13" customWidth="1"/>
-    <col min="9" max="9" width="59.42578125" style="13" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" style="13" customWidth="1"/>
-    <col min="11" max="11" width="20.42578125" style="13" customWidth="1"/>
-    <col min="12" max="12" width="20.5703125" style="13" customWidth="1"/>
-    <col min="13" max="14" width="255.7109375" style="13" customWidth="1"/>
-    <col min="15" max="15" width="230.140625" style="13" customWidth="1"/>
-    <col min="16" max="16" width="98.7109375" style="13" customWidth="1"/>
-    <col min="17" max="17" width="19.140625" style="13" customWidth="1"/>
-    <col min="18" max="18" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="6.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="37.6640625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="94.6640625" style="13" customWidth="1"/>
+    <col min="6" max="6" width="157.33203125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="255.6640625" style="13" customWidth="1"/>
+    <col min="8" max="8" width="181.109375" style="13" customWidth="1"/>
+    <col min="9" max="9" width="59.44140625" style="13" customWidth="1"/>
+    <col min="10" max="10" width="16.109375" style="13" customWidth="1"/>
+    <col min="11" max="11" width="20.44140625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="20.5546875" style="13" customWidth="1"/>
+    <col min="13" max="14" width="255.6640625" style="13" customWidth="1"/>
+    <col min="15" max="15" width="230.109375" style="13" customWidth="1"/>
+    <col min="16" max="16" width="98.6640625" style="13" customWidth="1"/>
+    <col min="17" max="17" width="19.109375" style="13" customWidth="1"/>
+    <col min="18" max="18" width="12.6640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.88671875" style="13" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="22" max="26" width="9.42578125" style="13" customWidth="1"/>
-    <col min="27" max="29" width="9.140625" style="13"/>
-    <col min="30" max="30" width="55.140625" style="13" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="13"/>
+    <col min="21" max="21" width="15.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="26" width="9.44140625" style="13" customWidth="1"/>
+    <col min="27" max="29" width="9.109375" style="13"/>
+    <col min="30" max="30" width="55.109375" style="13" customWidth="1"/>
+    <col min="31" max="16384" width="9.109375" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -9027,10 +9028,10 @@
         <v>626</v>
       </c>
       <c r="F92" s="6" t="s">
-        <v>736</v>
+        <v>739</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>737</v>
+        <v>740</v>
       </c>
       <c r="H92" s="6" t="s">
         <v>190</v>
@@ -9125,10 +9126,10 @@
         <v>8</v>
       </c>
       <c r="M93" s="7" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="N93" s="6" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="O93" s="6"/>
       <c r="P93" s="6" t="s">
@@ -9988,7 +9989,7 @@
         <v>649</v>
       </c>
       <c r="G106" s="6" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="H106" s="7" t="s">
         <v>257</v>
@@ -12185,7 +12186,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:B25"/>
   <sheetViews>
@@ -12193,11 +12194,11 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="17.25" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="17.25" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="255.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="27.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="255.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.44140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1">

</xml_diff>

<commit_message>
Act Base Mirador y Fichas
</commit_message>
<xml_diff>
--- a/Data/Base_fichas_indicadores.xlsx
+++ b/Data/Base_fichas_indicadores.xlsx
@@ -923,9 +923,6 @@
     <t>Para cada año calcular: (Cantidad de personas de 21 a 23 años que no culminaron la educación media básica / Cantidad de población de 21 a 23 años)*100</t>
   </si>
   <si>
-    <t>Porcentaje de inactivos mayores de 60 años que no perciben jubilaciones ni pensiones</t>
-  </si>
-  <si>
     <t>Porcentaje de mayores de 65 años que no perciben jubilaciones ni pensiones</t>
   </si>
   <si>
@@ -1712,9 +1709,6 @@
     <t>Mayores de 65 años sin pensión ni jubilación</t>
   </si>
   <si>
-    <t>Inactivos mayores de 60 años sin pensión ni jubilación</t>
-  </si>
-  <si>
     <t>Población activa que no aporta a la seguridad social</t>
   </si>
   <si>
@@ -2207,9 +2201,6 @@
     <t>El indicador mide el porcentaje de personas residiendo en viviendas con tenencia insegura. Esta situación es aqeulla en que las personas residen en viviendas de las cuales son propietarios del inmueble (ya pago o en proceso) pero no del terreno; son ocupantes gratuitos (en préstamo), en relación de dependencia o sin permiso del propietario.</t>
   </si>
   <si>
-    <t>El indicador mide el porcentaje de mayores de 60 años inactivos que no perciben jubilaciones ni pensiones.</t>
-  </si>
-  <si>
     <t>El indicador mide el porcentaje de mayores de 65 años que no perciben jubilaciones ni pensiones.</t>
   </si>
   <si>
@@ -2253,6 +2244,15 @@
   </si>
   <si>
     <t xml:space="preserve">El indicador mide el porcentaje de niños, niñas y adolescentes (hasta 17 años de edad) que residen en hogares cuyo jefe/a y/o cónyuge están desocupados y no perciben seguro de desempleo, sobre el total de NNA que residen en hogares cuyo jefe/a y/o cónyuge están desempleados. </t>
+  </si>
+  <si>
+    <t>Mayores de 60 años sin pensión ni jubilación y que no participan del mercado de trabajo</t>
+  </si>
+  <si>
+    <t>Porcentaje de mayores de 60 años que no perciben jubilaciones ni pensiones y que no participan del mercado de trabajo</t>
+  </si>
+  <si>
+    <t>El indicador mide el porcentaje de mayores de 60 años inactivos (que no participan del mercado de trabajo) que no perciben jubilaciones ni pensiones.</t>
   </si>
 </sst>
 </file>
@@ -2781,10 +2781,10 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AI140"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="G1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E111" sqref="E111"/>
-      <selection pane="bottomLeft" activeCell="G130" sqref="G130"/>
+      <selection pane="bottomLeft" activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -2817,67 +2817,67 @@
   <sheetData>
     <row r="1" spans="1:21">
       <c r="A1" s="26" t="s">
+        <v>341</v>
+      </c>
+      <c r="B1" s="26" t="s">
         <v>342</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="C1" s="26" t="s">
         <v>343</v>
       </c>
-      <c r="C1" s="26" t="s">
-        <v>344</v>
-      </c>
       <c r="D1" s="26" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="F1" s="26" t="s">
+        <v>345</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>348</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>350</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>351</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>352</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>353</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>354</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>355</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>356</v>
-      </c>
       <c r="Q1" s="26" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="R1" s="13" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="S1" s="34" t="s">
+        <v>684</v>
+      </c>
+      <c r="T1" s="34" t="s">
+        <v>685</v>
+      </c>
+      <c r="U1" s="34" t="s">
         <v>686</v>
-      </c>
-      <c r="T1" s="34" t="s">
-        <v>687</v>
-      </c>
-      <c r="U1" s="34" t="s">
-        <v>688</v>
       </c>
     </row>
     <row r="2" spans="1:21" s="6" customFormat="1">
@@ -2894,13 +2894,13 @@
         <v>104</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="F2" s="31" t="s">
         <v>80</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>114</v>
@@ -2912,16 +2912,16 @@
         <v>6</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="L2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="P2" s="6" t="s">
         <v>17</v>
@@ -2956,13 +2956,13 @@
         <v>104</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="F3" s="31" t="s">
         <v>81</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H3" s="6" t="s">
         <v>113</v>
@@ -2974,16 +2974,16 @@
         <v>6</v>
       </c>
       <c r="K3" s="6" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="L3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="P3" s="6" t="s">
         <v>17</v>
@@ -3018,13 +3018,13 @@
         <v>104</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="F4" s="31" t="s">
         <v>82</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>116</v>
@@ -3036,16 +3036,16 @@
         <v>6</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="L4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="P4" s="6" t="s">
         <v>17</v>
@@ -3080,13 +3080,13 @@
         <v>104</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>76</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="H5" s="6" t="s">
         <v>112</v>
@@ -3104,10 +3104,10 @@
         <v>8</v>
       </c>
       <c r="M5" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="N5" s="6" t="s">
         <v>496</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>497</v>
       </c>
       <c r="P5" s="6" t="s">
         <v>17</v>
@@ -3142,16 +3142,16 @@
         <v>104</v>
       </c>
       <c r="E6" s="30" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>79</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="I6" s="6" t="s">
         <v>5</v>
@@ -3166,10 +3166,10 @@
         <v>8</v>
       </c>
       <c r="M6" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="N6" s="6" t="s">
         <v>494</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>495</v>
       </c>
       <c r="P6" s="6" t="s">
         <v>25</v>
@@ -3204,16 +3204,16 @@
         <v>104</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>78</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I7" s="6" t="s">
         <v>5</v>
@@ -3228,10 +3228,10 @@
         <v>8</v>
       </c>
       <c r="M7" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="N7" s="6" t="s">
         <v>494</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>495</v>
       </c>
       <c r="P7" s="6" t="s">
         <v>25</v>
@@ -3266,13 +3266,13 @@
         <v>104</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>83</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="H8" s="6" t="s">
         <v>115</v>
@@ -3290,10 +3290,10 @@
         <v>8</v>
       </c>
       <c r="M8" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="N8" s="6" t="s">
         <v>494</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>495</v>
       </c>
       <c r="P8" s="6" t="s">
         <v>25</v>
@@ -3328,13 +3328,13 @@
         <v>104</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>84</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H9" s="6" t="s">
         <v>30</v>
@@ -3352,10 +3352,10 @@
         <v>8</v>
       </c>
       <c r="M9" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="N9" s="6" t="s">
         <v>494</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>495</v>
       </c>
       <c r="P9" s="6" t="s">
         <v>85</v>
@@ -3390,13 +3390,13 @@
         <v>104</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>88</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H10" s="6" t="s">
         <v>86</v>
@@ -3414,10 +3414,10 @@
         <v>8</v>
       </c>
       <c r="M10" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="N10" s="6" t="s">
         <v>494</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>495</v>
       </c>
       <c r="P10" s="6" t="s">
         <v>85</v>
@@ -3452,13 +3452,13 @@
         <v>104</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>89</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>90</v>
@@ -3476,10 +3476,10 @@
         <v>8</v>
       </c>
       <c r="M11" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="N11" s="6" t="s">
         <v>494</v>
-      </c>
-      <c r="N11" s="6" t="s">
-        <v>495</v>
       </c>
       <c r="P11" s="6" t="s">
         <v>85</v>
@@ -3514,16 +3514,16 @@
         <v>104</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="I12" s="6" t="s">
         <v>33</v>
@@ -3538,13 +3538,13 @@
         <v>8</v>
       </c>
       <c r="M12" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="N12" s="6" t="s">
         <v>494</v>
       </c>
-      <c r="N12" s="6" t="s">
-        <v>495</v>
-      </c>
       <c r="P12" s="6" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="Q12" s="6">
         <v>0</v>
@@ -3576,13 +3576,13 @@
         <v>104</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>92</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>295</v>
@@ -3600,7 +3600,7 @@
         <v>8</v>
       </c>
       <c r="M13" s="6" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N13" s="6" t="s">
         <v>13</v>
@@ -3638,13 +3638,13 @@
         <v>104</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>97</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H14" s="6" t="s">
         <v>28</v>
@@ -3662,10 +3662,10 @@
         <v>296</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="P14" s="6" t="s">
         <v>96</v>
@@ -3694,22 +3694,22 @@
         <v>1</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>5</v>
@@ -3718,7 +3718,7 @@
         <v>6</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="L15" s="7" t="s">
         <v>8</v>
@@ -3756,22 +3756,22 @@
         <v>1</v>
       </c>
       <c r="C16" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>514</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="E16" s="30" t="s">
-        <v>515</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>304</v>
-      </c>
       <c r="G16" s="6" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="I16" s="7" t="s">
         <v>5</v>
@@ -3780,7 +3780,7 @@
         <v>6</v>
       </c>
       <c r="K16" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="L16" s="7" t="s">
         <v>8</v>
@@ -3818,22 +3818,22 @@
         <v>1</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="I17" s="7" t="s">
         <v>5</v>
@@ -3842,7 +3842,7 @@
         <v>6</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="L17" s="7" t="s">
         <v>8</v>
@@ -3886,13 +3886,13 @@
         <v>3</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F18" s="13" t="s">
         <v>4</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="H18" s="14" t="s">
         <v>139</v>
@@ -3919,7 +3919,7 @@
         <v>10</v>
       </c>
       <c r="P18" s="13" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="Q18" s="6">
         <v>1</v>
@@ -3951,13 +3951,13 @@
         <v>3</v>
       </c>
       <c r="E19" s="30" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F19" s="13" t="s">
         <v>100</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H19" s="14" t="s">
         <v>140</v>
@@ -3984,7 +3984,7 @@
         <v>11</v>
       </c>
       <c r="P19" s="13" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="Q19" s="6">
         <v>1</v>
@@ -4016,13 +4016,13 @@
         <v>3</v>
       </c>
       <c r="E20" s="30" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="F20" s="13" t="s">
         <v>102</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="H20" s="14" t="s">
         <v>141</v>
@@ -4049,7 +4049,7 @@
         <v>11</v>
       </c>
       <c r="P20" s="13" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="Q20" s="6">
         <v>0</v>
@@ -4081,13 +4081,13 @@
         <v>3</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F21" s="13" t="s">
         <v>18</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H21" s="13" t="s">
         <v>148</v>
@@ -4114,7 +4114,7 @@
         <v>10</v>
       </c>
       <c r="P21" s="13" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="Q21" s="6">
         <v>0</v>
@@ -4160,13 +4160,13 @@
         <v>3</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="F22" s="4" t="s">
         <v>19</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="H22" s="13" t="s">
         <v>149</v>
@@ -4193,7 +4193,7 @@
         <v>10</v>
       </c>
       <c r="P22" s="13" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="Q22" s="6">
         <v>0</v>
@@ -4239,13 +4239,13 @@
         <v>3</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F23" s="13" t="s">
         <v>20</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="H23" s="13" t="s">
         <v>150</v>
@@ -4272,7 +4272,7 @@
         <v>10</v>
       </c>
       <c r="P23" s="13" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="Q23" s="6">
         <v>0</v>
@@ -4304,13 +4304,13 @@
         <v>3</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="F24" s="15" t="s">
         <v>297</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H24" s="15" t="s">
         <v>298</v>
@@ -4337,7 +4337,7 @@
         <v>233</v>
       </c>
       <c r="P24" s="13" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="Q24" s="6">
         <v>0</v>
@@ -4383,13 +4383,13 @@
         <v>3</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="F25" s="15" t="s">
         <v>235</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H25" s="15" t="s">
         <v>234</v>
@@ -4416,7 +4416,7 @@
         <v>233</v>
       </c>
       <c r="P25" s="13" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="Q25" s="6">
         <v>1</v>
@@ -4462,13 +4462,13 @@
         <v>12</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>98</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H26" s="6" t="s">
         <v>142</v>
@@ -4486,16 +4486,16 @@
         <v>8</v>
       </c>
       <c r="M26" s="6" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N26" s="6" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="O26" s="6" t="s">
         <v>14</v>
       </c>
       <c r="P26" s="6" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="Q26" s="6">
         <v>0</v>
@@ -4527,13 +4527,13 @@
         <v>12</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>73</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H27" s="6" t="s">
         <v>143</v>
@@ -4551,16 +4551,16 @@
         <v>8</v>
       </c>
       <c r="M27" s="6" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N27" s="6" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="O27" s="6" t="s">
         <v>14</v>
       </c>
       <c r="P27" s="6" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="Q27" s="6">
         <v>0</v>
@@ -4606,13 +4606,13 @@
         <v>12</v>
       </c>
       <c r="E28" s="30" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>99</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H28" s="6" t="s">
         <v>151</v>
@@ -4630,16 +4630,16 @@
         <v>8</v>
       </c>
       <c r="M28" s="6" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N28" s="6" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="O28" s="6" t="s">
         <v>14</v>
       </c>
       <c r="P28" s="6" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="Q28" s="6">
         <v>0</v>
@@ -4685,16 +4685,16 @@
         <v>12</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F29" s="13" t="s">
         <v>101</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="I29" s="13" t="s">
         <v>5</v>
@@ -4709,16 +4709,16 @@
         <v>8</v>
       </c>
       <c r="M29" s="13" t="s">
+        <v>493</v>
+      </c>
+      <c r="N29" s="13" t="s">
         <v>494</v>
-      </c>
-      <c r="N29" s="13" t="s">
-        <v>495</v>
       </c>
       <c r="O29" s="13" t="s">
         <v>21</v>
       </c>
       <c r="P29" s="13" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="Q29" s="6">
         <v>0</v>
@@ -4750,16 +4750,16 @@
         <v>12</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="F30" s="13" t="s">
         <v>103</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="I30" s="13" t="s">
         <v>5</v>
@@ -4774,16 +4774,16 @@
         <v>8</v>
       </c>
       <c r="M30" s="13" t="s">
+        <v>493</v>
+      </c>
+      <c r="N30" s="13" t="s">
         <v>494</v>
-      </c>
-      <c r="N30" s="13" t="s">
-        <v>495</v>
       </c>
       <c r="O30" s="13" t="s">
         <v>21</v>
       </c>
       <c r="P30" s="13" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="Q30" s="6">
         <v>0</v>
@@ -4829,13 +4829,13 @@
         <v>15</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F31" s="2" t="s">
         <v>108</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H31" s="13" t="s">
         <v>144</v>
@@ -4853,10 +4853,10 @@
         <v>16</v>
       </c>
       <c r="M31" s="6" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N31" s="6" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="O31" s="16"/>
       <c r="P31" s="13" t="s">
@@ -4906,13 +4906,13 @@
         <v>15</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>109</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H32" s="13" t="s">
         <v>145</v>
@@ -4930,10 +4930,10 @@
         <v>16</v>
       </c>
       <c r="M32" s="6" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N32" s="6" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="O32" s="16"/>
       <c r="P32" s="13" t="s">
@@ -4983,13 +4983,13 @@
         <v>15</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="F33" s="2" t="s">
         <v>107</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="H33" s="13" t="s">
         <v>146</v>
@@ -5007,10 +5007,10 @@
         <v>16</v>
       </c>
       <c r="M33" s="6" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="O33" s="16"/>
       <c r="P33" s="13" t="s">
@@ -5046,13 +5046,13 @@
         <v>15</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>110</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="H34" s="13" t="s">
         <v>147</v>
@@ -5070,10 +5070,10 @@
         <v>16</v>
       </c>
       <c r="M34" s="6" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="N34" s="6" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="O34" s="6" t="s">
         <v>105</v>
@@ -5125,13 +5125,13 @@
         <v>15</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>22</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H35" s="6" t="s">
         <v>152</v>
@@ -5190,13 +5190,13 @@
         <v>3</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="F36" s="13" t="s">
         <v>74</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="H36" s="13" t="s">
         <v>153</v>
@@ -5223,7 +5223,7 @@
         <v>75</v>
       </c>
       <c r="P36" s="13" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="Q36" s="6">
         <v>0</v>
@@ -5255,13 +5255,13 @@
         <v>104</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="F37" s="31" t="s">
         <v>118</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H37" s="6" t="s">
         <v>119</v>
@@ -5273,16 +5273,16 @@
         <v>6</v>
       </c>
       <c r="K37" s="6" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="L37" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M37" s="6" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="N37" s="6" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="P37" s="6" t="s">
         <v>17</v>
@@ -5317,13 +5317,13 @@
         <v>104</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="F38" s="31" t="s">
         <v>120</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="H38" s="6" t="s">
         <v>121</v>
@@ -5341,10 +5341,10 @@
         <v>8</v>
       </c>
       <c r="M38" s="6" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="N38" s="6" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="P38" s="6" t="s">
         <v>17</v>
@@ -5379,16 +5379,16 @@
         <v>104</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F39" s="31" t="s">
         <v>122</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="I39" s="6" t="s">
         <v>5</v>
@@ -5397,16 +5397,16 @@
         <v>6</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="L39" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M39" s="6" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="N39" s="6" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="P39" s="6" t="s">
         <v>17</v>
@@ -5441,13 +5441,13 @@
         <v>104</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>123</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="H40" s="6" t="s">
         <v>124</v>
@@ -5465,10 +5465,10 @@
         <v>8</v>
       </c>
       <c r="M40" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="N40" s="6" t="s">
         <v>496</v>
-      </c>
-      <c r="N40" s="6" t="s">
-        <v>497</v>
       </c>
       <c r="P40" s="6" t="s">
         <v>17</v>
@@ -5503,19 +5503,19 @@
         <v>104</v>
       </c>
       <c r="E41" s="30" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="F41" s="24" t="s">
+        <v>315</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>425</v>
+      </c>
+      <c r="H41" s="6" t="s">
         <v>316</v>
       </c>
-      <c r="G41" s="6" t="s">
-        <v>426</v>
-      </c>
-      <c r="H41" s="6" t="s">
+      <c r="I41" s="6" t="s">
         <v>317</v>
-      </c>
-      <c r="I41" s="6" t="s">
-        <v>318</v>
       </c>
       <c r="J41" s="6" t="s">
         <v>6</v>
@@ -5527,14 +5527,14 @@
         <v>8</v>
       </c>
       <c r="M41" s="24" t="s">
+        <v>318</v>
+      </c>
+      <c r="N41" s="6" t="s">
         <v>319</v>
-      </c>
-      <c r="N41" s="6" t="s">
-        <v>320</v>
       </c>
       <c r="O41" s="6"/>
       <c r="P41" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Q41" s="6">
         <v>0</v>
@@ -5580,38 +5580,38 @@
         <v>104</v>
       </c>
       <c r="E42" s="30" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F42" s="24" t="s">
+        <v>321</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>426</v>
+      </c>
+      <c r="H42" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="G42" s="6" t="s">
-        <v>427</v>
-      </c>
-      <c r="H42" s="6" t="s">
-        <v>323</v>
-      </c>
       <c r="I42" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J42" s="6" t="s">
         <v>6</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="L42" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M42" s="24" t="s">
+        <v>324</v>
+      </c>
+      <c r="N42" s="6" t="s">
         <v>325</v>
-      </c>
-      <c r="N42" s="6" t="s">
-        <v>326</v>
       </c>
       <c r="O42" s="25"/>
       <c r="P42" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Q42" s="6">
         <v>0</v>
@@ -5657,38 +5657,38 @@
         <v>104</v>
       </c>
       <c r="E43" s="30" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="F43" s="24" t="s">
+        <v>326</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>727</v>
+      </c>
+      <c r="H43" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="G43" s="6" t="s">
-        <v>730</v>
-      </c>
-      <c r="H43" s="6" t="s">
-        <v>328</v>
-      </c>
       <c r="I43" s="6" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="J43" s="6" t="s">
         <v>6</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="L43" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M43" s="24" t="s">
+        <v>329</v>
+      </c>
+      <c r="N43" s="6" t="s">
         <v>330</v>
-      </c>
-      <c r="N43" s="6" t="s">
-        <v>331</v>
       </c>
       <c r="O43" s="25"/>
       <c r="P43" s="6" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="Q43" s="6">
         <v>0</v>
@@ -5734,13 +5734,13 @@
         <v>36</v>
       </c>
       <c r="E44" s="30" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="F44" s="13" t="s">
         <v>37</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="H44" s="13" t="s">
         <v>38</v>
@@ -5767,7 +5767,7 @@
         <v>40</v>
       </c>
       <c r="P44" s="13" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="Q44" s="6">
         <v>1</v>
@@ -5813,13 +5813,13 @@
         <v>41</v>
       </c>
       <c r="E45" s="32" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="F45" s="13" t="s">
         <v>42</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H45" s="13" t="s">
         <v>154</v>
@@ -5846,7 +5846,7 @@
         <v>43</v>
       </c>
       <c r="P45" s="13" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="Q45" s="6">
         <v>0</v>
@@ -5892,13 +5892,13 @@
         <v>41</v>
       </c>
       <c r="E46" s="32" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F46" s="13" t="s">
         <v>44</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H46" s="13" t="s">
         <v>155</v>
@@ -5925,7 +5925,7 @@
         <v>45</v>
       </c>
       <c r="P46" s="13" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="Q46" s="6">
         <v>0</v>
@@ -5971,13 +5971,13 @@
         <v>41</v>
       </c>
       <c r="E47" s="32" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H47" s="6" t="s">
         <v>189</v>
@@ -6001,10 +6001,10 @@
         <v>194</v>
       </c>
       <c r="O47" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="P47" s="6" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Q47" s="6">
         <v>1</v>
@@ -6036,13 +6036,13 @@
         <v>41</v>
       </c>
       <c r="E48" s="32" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>161</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H48" s="13" t="s">
         <v>162</v>
@@ -6069,7 +6069,7 @@
         <v>163</v>
       </c>
       <c r="P48" s="13" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="Q48" s="6">
         <v>0</v>
@@ -6101,16 +6101,16 @@
         <v>46</v>
       </c>
       <c r="E49" s="32" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H49" s="27" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="I49" s="6" t="s">
         <v>5</v>
@@ -6131,10 +6131,10 @@
         <v>194</v>
       </c>
       <c r="O49" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="P49" s="6" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="Q49" s="6">
         <v>1</v>
@@ -6166,16 +6166,16 @@
         <v>46</v>
       </c>
       <c r="E50" s="32" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H50" s="27" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="I50" s="6" t="s">
         <v>5</v>
@@ -6196,10 +6196,10 @@
         <v>194</v>
       </c>
       <c r="O50" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="P50" s="13" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="Q50" s="6">
         <v>0</v>
@@ -6245,16 +6245,16 @@
         <v>46</v>
       </c>
       <c r="E51" s="32" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H51" s="27" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="I51" s="6" t="s">
         <v>5</v>
@@ -6275,10 +6275,10 @@
         <v>194</v>
       </c>
       <c r="O51" s="7" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="P51" s="13" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="Q51" s="6">
         <v>0</v>
@@ -6324,16 +6324,16 @@
         <v>46</v>
       </c>
       <c r="E52" s="32" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F52" s="28" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H52" s="27" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="I52" s="6" t="s">
         <v>5</v>
@@ -6354,10 +6354,10 @@
         <v>194</v>
       </c>
       <c r="O52" s="7" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="P52" s="13" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="Q52" s="6">
         <v>0</v>
@@ -6403,16 +6403,16 @@
         <v>47</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="F53" s="28" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="G53" s="28" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="H53" s="27" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="I53" s="6" t="s">
         <v>5</v>
@@ -6433,10 +6433,10 @@
         <v>194</v>
       </c>
       <c r="O53" s="7" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="P53" s="13" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="Q53" s="6">
         <v>1</v>
@@ -6482,13 +6482,13 @@
         <v>47</v>
       </c>
       <c r="E54" s="32" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F54" s="13" t="s">
         <v>48</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H54" s="13" t="s">
         <v>156</v>
@@ -6515,7 +6515,7 @@
         <v>49</v>
       </c>
       <c r="P54" s="13" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="Q54" s="6">
         <v>0</v>
@@ -6561,13 +6561,13 @@
         <v>50</v>
       </c>
       <c r="E55" s="32" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="F55" s="13" t="s">
         <v>51</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H55" s="13" t="s">
         <v>157</v>
@@ -6592,7 +6592,7 @@
       </c>
       <c r="O55" s="13"/>
       <c r="P55" s="13" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="Q55" s="6">
         <v>1</v>
@@ -6638,13 +6638,13 @@
         <v>104</v>
       </c>
       <c r="E56" s="32" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="F56" s="31" t="s">
         <v>125</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="H56" s="6" t="s">
         <v>126</v>
@@ -6656,16 +6656,16 @@
         <v>6</v>
       </c>
       <c r="K56" s="6" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="L56" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M56" s="6" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="N56" s="6" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="P56" s="6" t="s">
         <v>17</v>
@@ -6700,13 +6700,13 @@
         <v>104</v>
       </c>
       <c r="E57" s="30" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F57" s="31" t="s">
         <v>127</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="H57" s="6" t="s">
         <v>128</v>
@@ -6724,10 +6724,10 @@
         <v>8</v>
       </c>
       <c r="M57" s="6" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="N57" s="6" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="P57" s="6" t="s">
         <v>17</v>
@@ -6762,16 +6762,16 @@
         <v>104</v>
       </c>
       <c r="E58" s="30" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F58" s="31" t="s">
         <v>129</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="I58" s="6" t="s">
         <v>5</v>
@@ -6780,16 +6780,16 @@
         <v>6</v>
       </c>
       <c r="K58" s="6" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="L58" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M58" s="6" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="N58" s="6" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="P58" s="6" t="s">
         <v>17</v>
@@ -6824,13 +6824,13 @@
         <v>104</v>
       </c>
       <c r="E59" s="30" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>130</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="H59" s="6" t="s">
         <v>131</v>
@@ -6848,10 +6848,10 @@
         <v>8</v>
       </c>
       <c r="M59" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="N59" s="6" t="s">
         <v>496</v>
-      </c>
-      <c r="N59" s="6" t="s">
-        <v>497</v>
       </c>
       <c r="P59" s="6" t="s">
         <v>17</v>
@@ -6886,13 +6886,13 @@
         <v>104</v>
       </c>
       <c r="E60" s="30" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F60" s="5" t="s">
         <v>171</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="H60" s="6" t="s">
         <v>170</v>
@@ -6910,10 +6910,10 @@
         <v>8</v>
       </c>
       <c r="M60" s="6" t="s">
+        <v>497</v>
+      </c>
+      <c r="N60" s="6" t="s">
         <v>498</v>
-      </c>
-      <c r="N60" s="6" t="s">
-        <v>499</v>
       </c>
       <c r="P60" s="6" t="s">
         <v>17</v>
@@ -6948,13 +6948,13 @@
         <v>104</v>
       </c>
       <c r="E61" s="30" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F61" s="5" t="s">
         <v>172</v>
       </c>
       <c r="G61" s="6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="H61" s="6" t="s">
         <v>173</v>
@@ -6972,10 +6972,10 @@
         <v>8</v>
       </c>
       <c r="M61" s="6" t="s">
+        <v>497</v>
+      </c>
+      <c r="N61" s="6" t="s">
         <v>498</v>
-      </c>
-      <c r="N61" s="6" t="s">
-        <v>499</v>
       </c>
       <c r="P61" s="6" t="s">
         <v>17</v>
@@ -7010,13 +7010,13 @@
         <v>104</v>
       </c>
       <c r="E62" s="30" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="H62" s="6" t="s">
         <v>174</v>
@@ -7034,10 +7034,10 @@
         <v>8</v>
       </c>
       <c r="M62" s="6" t="s">
+        <v>497</v>
+      </c>
+      <c r="N62" s="6" t="s">
         <v>498</v>
-      </c>
-      <c r="N62" s="6" t="s">
-        <v>499</v>
       </c>
       <c r="P62" s="6" t="s">
         <v>17</v>
@@ -7072,13 +7072,13 @@
         <v>3</v>
       </c>
       <c r="E63" s="30" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F63" s="6" t="s">
         <v>53</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="H63" s="6" t="s">
         <v>158</v>
@@ -7090,7 +7090,7 @@
         <v>6</v>
       </c>
       <c r="K63" s="6" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="L63" s="6" t="s">
         <v>8</v>
@@ -7137,13 +7137,13 @@
         <v>3</v>
       </c>
       <c r="E64" s="30" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F64" s="6" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G64" s="6" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="H64" s="6" t="s">
         <v>159</v>
@@ -7170,7 +7170,7 @@
         <v>54</v>
       </c>
       <c r="P64" s="13" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="Q64" s="6">
         <v>0</v>
@@ -7202,16 +7202,16 @@
         <v>3</v>
       </c>
       <c r="E65" s="30" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="F65" s="6" t="s">
         <v>55</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="I65" s="6" t="s">
         <v>5</v>
@@ -7235,7 +7235,7 @@
         <v>54</v>
       </c>
       <c r="P65" s="13" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="Q65" s="6">
         <v>0</v>
@@ -7273,10 +7273,10 @@
         <v>56</v>
       </c>
       <c r="G66" s="6" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="H66" s="6" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="I66" s="6" t="s">
         <v>5</v>
@@ -7300,7 +7300,7 @@
         <v>54</v>
       </c>
       <c r="P66" s="13" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="Q66" s="6">
         <v>1</v>
@@ -7332,16 +7332,16 @@
         <v>3</v>
       </c>
       <c r="E67" s="30" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="F67" s="6" t="s">
         <v>57</v>
       </c>
       <c r="G67" s="6" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I67" s="6" t="s">
         <v>5</v>
@@ -7397,16 +7397,16 @@
         <v>3</v>
       </c>
       <c r="E68" s="30" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="F68" s="6" t="s">
         <v>58</v>
       </c>
       <c r="G68" s="6" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H68" s="6" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="I68" s="6" t="s">
         <v>5</v>
@@ -7462,16 +7462,16 @@
         <v>3</v>
       </c>
       <c r="E69" s="30" t="s">
-        <v>562</v>
+        <v>740</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>299</v>
+        <v>741</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>727</v>
+        <v>742</v>
       </c>
       <c r="H69" s="6" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="I69" s="6" t="s">
         <v>5</v>
@@ -7495,7 +7495,7 @@
         <v>54</v>
       </c>
       <c r="P69" s="13" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="Q69" s="6">
         <v>1</v>
@@ -7527,16 +7527,16 @@
         <v>59</v>
       </c>
       <c r="E70" s="30" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="F70" s="6" t="s">
         <v>60</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="H70" s="6" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="I70" s="6" t="s">
         <v>5</v>
@@ -7592,16 +7592,16 @@
         <v>59</v>
       </c>
       <c r="E71" s="30" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>164</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="H71" s="6" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="I71" s="6" t="s">
         <v>5</v>
@@ -7657,16 +7657,16 @@
         <v>59</v>
       </c>
       <c r="E72" s="30" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="F72" s="6" t="s">
         <v>62</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="I72" s="6" t="s">
         <v>5</v>
@@ -7722,16 +7722,16 @@
         <v>59</v>
       </c>
       <c r="E73" s="30" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="F73" s="6" t="s">
         <v>63</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I73" s="6" t="s">
         <v>5</v>
@@ -7787,16 +7787,16 @@
         <v>59</v>
       </c>
       <c r="E74" s="30" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="F74" s="6" t="s">
         <v>165</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="H74" s="6" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="I74" s="6" t="s">
         <v>5</v>
@@ -7852,16 +7852,16 @@
         <v>59</v>
       </c>
       <c r="E75" s="30" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="F75" s="6" t="s">
         <v>166</v>
       </c>
       <c r="G75" s="6" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H75" s="6" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I75" s="6" t="s">
         <v>5</v>
@@ -7917,16 +7917,16 @@
         <v>59</v>
       </c>
       <c r="E76" s="30" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="F76" s="6" t="s">
         <v>167</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="H76" s="6" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="I76" s="6" t="s">
         <v>5</v>
@@ -7982,16 +7982,16 @@
         <v>59</v>
       </c>
       <c r="E77" s="30" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="F77" s="6" t="s">
         <v>168</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="H77" s="6" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I77" s="6" t="s">
         <v>5</v>
@@ -8047,16 +8047,16 @@
         <v>59</v>
       </c>
       <c r="E78" s="30" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="F78" s="6" t="s">
         <v>64</v>
       </c>
       <c r="G78" s="6" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="H78" s="6" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="I78" s="6" t="s">
         <v>5</v>
@@ -8112,16 +8112,16 @@
         <v>59</v>
       </c>
       <c r="E79" s="30" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="F79" s="6" t="s">
         <v>65</v>
       </c>
       <c r="G79" s="6" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H79" s="6" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="I79" s="6" t="s">
         <v>5</v>
@@ -8177,16 +8177,16 @@
         <v>59</v>
       </c>
       <c r="E80" s="30" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="F80" s="6" t="s">
         <v>66</v>
       </c>
       <c r="G80" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="H80" s="6" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="I80" s="6" t="s">
         <v>5</v>
@@ -8242,16 +8242,16 @@
         <v>59</v>
       </c>
       <c r="E81" s="30" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="F81" s="6" t="s">
         <v>67</v>
       </c>
       <c r="G81" s="6" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="H81" s="6" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="I81" s="6" t="s">
         <v>5</v>
@@ -8307,13 +8307,13 @@
         <v>59</v>
       </c>
       <c r="E82" s="30" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="F82" s="6" t="s">
         <v>68</v>
       </c>
       <c r="G82" s="6" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="H82" s="6" t="s">
         <v>160</v>
@@ -8372,13 +8372,13 @@
         <v>104</v>
       </c>
       <c r="E83" s="30" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="F83" s="31" t="s">
         <v>132</v>
       </c>
       <c r="G83" s="6" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="H83" s="6" t="s">
         <v>133</v>
@@ -8390,16 +8390,16 @@
         <v>6</v>
       </c>
       <c r="K83" s="6" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="L83" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M83" s="6" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="N83" s="6" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="P83" s="6" t="s">
         <v>17</v>
@@ -8434,13 +8434,13 @@
         <v>104</v>
       </c>
       <c r="E84" s="30" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="F84" s="31" t="s">
         <v>134</v>
       </c>
       <c r="G84" s="6" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="H84" s="6" t="s">
         <v>135</v>
@@ -8458,10 +8458,10 @@
         <v>8</v>
       </c>
       <c r="M84" s="6" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="N84" s="6" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="O84" s="6"/>
       <c r="P84" s="6" t="s">
@@ -8511,16 +8511,16 @@
         <v>104</v>
       </c>
       <c r="E85" s="30" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="F85" s="31" t="s">
         <v>136</v>
       </c>
       <c r="G85" s="6" t="s">
-        <v>740</v>
+        <v>737</v>
       </c>
       <c r="H85" s="6" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I85" s="6" t="s">
         <v>5</v>
@@ -8529,16 +8529,16 @@
         <v>6</v>
       </c>
       <c r="K85" s="6" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="L85" s="6" t="s">
         <v>8</v>
       </c>
       <c r="M85" s="6" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="N85" s="6" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="O85" s="6"/>
       <c r="P85" s="6" t="s">
@@ -8588,13 +8588,13 @@
         <v>104</v>
       </c>
       <c r="E86" s="30" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="F86" s="6" t="s">
         <v>137</v>
       </c>
       <c r="G86" s="6" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="H86" s="6" t="s">
         <v>138</v>
@@ -8612,10 +8612,10 @@
         <v>8</v>
       </c>
       <c r="M86" s="6" t="s">
+        <v>495</v>
+      </c>
+      <c r="N86" s="6" t="s">
         <v>496</v>
-      </c>
-      <c r="N86" s="6" t="s">
-        <v>497</v>
       </c>
       <c r="P86" s="6" t="s">
         <v>17</v>
@@ -8650,16 +8650,16 @@
         <v>104</v>
       </c>
       <c r="E87" s="30" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="F87" s="19" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="G87" s="6" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="H87" s="7" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="I87" s="7" t="s">
         <v>237</v>
@@ -8674,10 +8674,10 @@
         <v>8</v>
       </c>
       <c r="M87" s="7" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="N87" s="7" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="O87" s="6"/>
       <c r="P87" s="6" t="s">
@@ -8727,16 +8727,16 @@
         <v>104</v>
       </c>
       <c r="E88" s="32" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="F88" s="19" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G88" s="6" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="H88" s="7" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="I88" s="7" t="s">
         <v>240</v>
@@ -8751,10 +8751,10 @@
         <v>8</v>
       </c>
       <c r="M88" s="7" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="N88" s="7" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="P88" s="6" t="s">
         <v>17</v>
@@ -8789,16 +8789,16 @@
         <v>104</v>
       </c>
       <c r="E89" s="30" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="F89" s="19" t="s">
         <v>242</v>
       </c>
       <c r="G89" s="6" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="H89" s="7" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="I89" s="7" t="s">
         <v>237</v>
@@ -8813,10 +8813,10 @@
         <v>8</v>
       </c>
       <c r="M89" s="7" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="N89" s="7" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="O89" s="7"/>
       <c r="P89" s="7" t="s">
@@ -8866,16 +8866,16 @@
         <v>104</v>
       </c>
       <c r="E90" s="30" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="F90" s="20" t="s">
         <v>245</v>
       </c>
       <c r="G90" s="6" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="H90" s="7" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="I90" s="7" t="s">
         <v>240</v>
@@ -8890,10 +8890,10 @@
         <v>8</v>
       </c>
       <c r="M90" s="7" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="N90" s="7" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="O90" s="7"/>
       <c r="P90" s="7" t="s">
@@ -8937,22 +8937,22 @@
         <v>70</v>
       </c>
       <c r="C91" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D91" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E91" s="30" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="G91" s="6" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="H91" s="2" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="I91" s="7" t="s">
         <v>5</v>
@@ -8967,14 +8967,14 @@
         <v>8</v>
       </c>
       <c r="M91" s="9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="N91" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="O91" s="7"/>
       <c r="P91" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="Q91" s="6">
         <v>0</v>
@@ -9017,16 +9017,16 @@
         <v>2</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="F92" s="6" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="G92" s="6" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="H92" s="6" t="s">
         <v>190</v>
@@ -9051,7 +9051,7 @@
       </c>
       <c r="O92" s="6"/>
       <c r="P92" s="6" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="Q92" s="6">
         <v>1</v>
@@ -9094,7 +9094,7 @@
         <v>2</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E93" s="30" t="s">
         <v>71</v>
@@ -9103,10 +9103,10 @@
         <v>71</v>
       </c>
       <c r="G93" s="6" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="H93" s="6" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="I93" s="6" t="s">
         <v>191</v>
@@ -9121,14 +9121,14 @@
         <v>8</v>
       </c>
       <c r="M93" s="7" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="N93" s="6" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="O93" s="6"/>
       <c r="P93" s="6" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="Q93" s="6">
         <v>1</v>
@@ -9171,19 +9171,19 @@
         <v>2</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E94" s="30" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="F94" s="2" t="s">
         <v>292</v>
       </c>
       <c r="G94" s="6" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="H94" s="2" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="I94" s="11" t="s">
         <v>293</v>
@@ -9192,7 +9192,7 @@
         <v>6</v>
       </c>
       <c r="K94" s="11" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="L94" s="11" t="s">
         <v>8</v>
@@ -9248,10 +9248,10 @@
         <v>2</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E95" s="30" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="F95" s="12" t="s">
         <v>196</v>
@@ -9260,7 +9260,7 @@
         <v>197</v>
       </c>
       <c r="H95" s="11" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="I95" s="11" t="s">
         <v>198</v>
@@ -9269,7 +9269,7 @@
         <v>6</v>
       </c>
       <c r="K95" s="11" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="L95" s="11" t="s">
         <v>8</v>
@@ -9310,10 +9310,10 @@
         <v>2</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E96" s="30" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="F96" s="12" t="s">
         <v>230</v>
@@ -9322,7 +9322,7 @@
         <v>202</v>
       </c>
       <c r="H96" s="11" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I96" s="11" t="s">
         <v>198</v>
@@ -9331,7 +9331,7 @@
         <v>6</v>
       </c>
       <c r="K96" s="11" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="L96" s="11" t="s">
         <v>8</v>
@@ -9372,19 +9372,19 @@
         <v>2</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E97" s="30" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="F97" s="12" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="G97" s="6" t="s">
         <v>203</v>
       </c>
       <c r="H97" s="11" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="I97" s="11" t="s">
         <v>198</v>
@@ -9393,7 +9393,7 @@
         <v>6</v>
       </c>
       <c r="K97" s="11" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="L97" s="11" t="s">
         <v>8</v>
@@ -9434,10 +9434,10 @@
         <v>2</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E98" s="30" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="F98" s="12" t="s">
         <v>231</v>
@@ -9446,7 +9446,7 @@
         <v>204</v>
       </c>
       <c r="H98" s="11" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="I98" s="11" t="s">
         <v>205</v>
@@ -9455,7 +9455,7 @@
         <v>6</v>
       </c>
       <c r="K98" s="11" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="L98" s="11" t="s">
         <v>8</v>
@@ -9496,10 +9496,10 @@
         <v>2</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E99" s="30" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="F99" s="12" t="s">
         <v>206</v>
@@ -9508,7 +9508,7 @@
         <v>207</v>
       </c>
       <c r="H99" s="11" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I99" s="11" t="s">
         <v>208</v>
@@ -9517,7 +9517,7 @@
         <v>6</v>
       </c>
       <c r="K99" s="11" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="L99" s="11" t="s">
         <v>8</v>
@@ -9558,10 +9558,10 @@
         <v>2</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E100" s="30" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="F100" s="12" t="s">
         <v>224</v>
@@ -9570,7 +9570,7 @@
         <v>213</v>
       </c>
       <c r="H100" s="11" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="I100" s="11" t="s">
         <v>214</v>
@@ -9579,7 +9579,7 @@
         <v>6</v>
       </c>
       <c r="K100" s="11" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="L100" s="11" t="s">
         <v>8</v>
@@ -9620,10 +9620,10 @@
         <v>2</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E101" s="30" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="F101" s="12" t="s">
         <v>225</v>
@@ -9632,7 +9632,7 @@
         <v>216</v>
       </c>
       <c r="H101" s="11" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I101" s="11" t="s">
         <v>214</v>
@@ -9641,7 +9641,7 @@
         <v>6</v>
       </c>
       <c r="K101" s="11" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="L101" s="11" t="s">
         <v>8</v>
@@ -9682,10 +9682,10 @@
         <v>2</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E102" s="30" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="F102" s="12" t="s">
         <v>226</v>
@@ -9694,7 +9694,7 @@
         <v>217</v>
       </c>
       <c r="H102" s="11" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="I102" s="11" t="s">
         <v>214</v>
@@ -9703,7 +9703,7 @@
         <v>6</v>
       </c>
       <c r="K102" s="11" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="L102" s="11" t="s">
         <v>8</v>
@@ -9744,10 +9744,10 @@
         <v>2</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E103" s="30" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="F103" s="12" t="s">
         <v>227</v>
@@ -9756,7 +9756,7 @@
         <v>218</v>
       </c>
       <c r="H103" s="11" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="I103" s="11" t="s">
         <v>214</v>
@@ -9765,7 +9765,7 @@
         <v>6</v>
       </c>
       <c r="K103" s="11" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="L103" s="11" t="s">
         <v>8</v>
@@ -9821,10 +9821,10 @@
         <v>2</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E104" s="30" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="F104" s="12" t="s">
         <v>228</v>
@@ -9833,7 +9833,7 @@
         <v>219</v>
       </c>
       <c r="H104" s="11" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="I104" s="11" t="s">
         <v>214</v>
@@ -9842,7 +9842,7 @@
         <v>6</v>
       </c>
       <c r="K104" s="11" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="L104" s="11" t="s">
         <v>8</v>
@@ -9898,10 +9898,10 @@
         <v>2</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="E105" s="30" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="F105" s="12" t="s">
         <v>229</v>
@@ -9910,7 +9910,7 @@
         <v>220</v>
       </c>
       <c r="H105" s="11" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="I105" s="11" t="s">
         <v>214</v>
@@ -9919,7 +9919,7 @@
         <v>6</v>
       </c>
       <c r="K105" s="11" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="L105" s="11" t="s">
         <v>8</v>
@@ -9978,13 +9978,13 @@
         <v>3</v>
       </c>
       <c r="E106" s="30" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="F106" s="21" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="G106" s="6" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="H106" s="7" t="s">
         <v>257</v>
@@ -10002,10 +10002,10 @@
         <v>8</v>
       </c>
       <c r="M106" s="7" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="N106" s="7" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="P106" s="7" t="s">
         <v>244</v>
@@ -10040,13 +10040,13 @@
         <v>3</v>
       </c>
       <c r="E107" s="30" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="F107" s="8" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="G107" s="6" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="H107" s="7" t="s">
         <v>259</v>
@@ -10064,10 +10064,10 @@
         <v>8</v>
       </c>
       <c r="M107" s="7" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="N107" s="7" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="P107" s="7" t="s">
         <v>244</v>
@@ -10102,13 +10102,13 @@
         <v>3</v>
       </c>
       <c r="E108" s="30" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="F108" s="8" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="G108" s="6" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="H108" s="7" t="s">
         <v>261</v>
@@ -10126,10 +10126,10 @@
         <v>8</v>
       </c>
       <c r="M108" s="7" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="N108" s="7" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="P108" s="7" t="s">
         <v>244</v>
@@ -10164,13 +10164,13 @@
         <v>3</v>
       </c>
       <c r="E109" s="30" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="F109" s="8" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="G109" s="6" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="H109" s="7" t="s">
         <v>267</v>
@@ -10188,10 +10188,10 @@
         <v>8</v>
       </c>
       <c r="M109" s="7" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="N109" s="7" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="O109" s="7"/>
       <c r="P109" s="7" t="s">
@@ -10241,13 +10241,13 @@
         <v>3</v>
       </c>
       <c r="E110" s="30" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="F110" s="22" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="G110" s="6" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="H110" s="7" t="s">
         <v>263</v>
@@ -10265,10 +10265,10 @@
         <v>8</v>
       </c>
       <c r="M110" s="7" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="N110" s="7" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="P110" s="7" t="s">
         <v>244</v>
@@ -10303,13 +10303,13 @@
         <v>3</v>
       </c>
       <c r="E111" s="30" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="F111" s="22" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="G111" s="6" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="H111" s="7" t="s">
         <v>265</v>
@@ -10327,10 +10327,10 @@
         <v>8</v>
       </c>
       <c r="M111" s="7" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="N111" s="7" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="O111" s="7"/>
       <c r="P111" s="7" t="s">
@@ -10380,13 +10380,13 @@
         <v>3</v>
       </c>
       <c r="E112" s="30" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="F112" s="7" t="s">
         <v>246</v>
       </c>
       <c r="G112" s="6" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="H112" s="7" t="s">
         <v>247</v>
@@ -10404,10 +10404,10 @@
         <v>8</v>
       </c>
       <c r="M112" s="7" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="N112" s="7" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="P112" s="7" t="s">
         <v>244</v>
@@ -10442,13 +10442,13 @@
         <v>3</v>
       </c>
       <c r="E113" s="30" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="F113" s="7" t="s">
         <v>249</v>
       </c>
       <c r="G113" s="6" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="H113" s="7" t="s">
         <v>250</v>
@@ -10466,10 +10466,10 @@
         <v>8</v>
       </c>
       <c r="M113" s="7" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="N113" s="7" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="P113" s="7" t="s">
         <v>244</v>
@@ -10504,13 +10504,13 @@
         <v>3</v>
       </c>
       <c r="E114" s="30" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="F114" s="7" t="s">
         <v>251</v>
       </c>
       <c r="G114" s="6" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="H114" s="7" t="s">
         <v>252</v>
@@ -10528,10 +10528,10 @@
         <v>8</v>
       </c>
       <c r="M114" s="7" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="N114" s="7" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="P114" s="7" t="s">
         <v>244</v>
@@ -10566,13 +10566,13 @@
         <v>15</v>
       </c>
       <c r="E115" s="30" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="F115" s="21" t="s">
         <v>253</v>
       </c>
       <c r="G115" s="6" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="H115" s="7" t="s">
         <v>254</v>
@@ -10590,10 +10590,10 @@
         <v>8</v>
       </c>
       <c r="M115" s="7" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="N115" s="7" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="P115" s="7" t="s">
         <v>244</v>
@@ -10628,16 +10628,16 @@
         <v>15</v>
       </c>
       <c r="E116" s="30" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="F116" s="8" t="s">
         <v>270</v>
       </c>
       <c r="G116" s="6" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="H116" s="7" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="I116" s="7" t="s">
         <v>5</v>
@@ -10652,10 +10652,10 @@
         <v>8</v>
       </c>
       <c r="M116" s="7" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="N116" s="7" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="O116" s="7"/>
       <c r="P116" s="7" t="s">
@@ -10705,16 +10705,16 @@
         <v>15</v>
       </c>
       <c r="E117" s="30" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="F117" s="2" t="s">
         <v>294</v>
       </c>
       <c r="G117" s="6" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="H117" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="I117" s="11" t="s">
         <v>5</v>
@@ -10723,7 +10723,7 @@
         <v>6</v>
       </c>
       <c r="K117" s="11" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="L117" s="11" t="s">
         <v>8</v>
@@ -10782,7 +10782,7 @@
         <v>15</v>
       </c>
       <c r="E118" s="30" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="F118" s="12" t="s">
         <v>209</v>
@@ -10791,7 +10791,7 @@
         <v>221</v>
       </c>
       <c r="H118" s="11" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I118" s="11" t="s">
         <v>210</v>
@@ -10800,7 +10800,7 @@
         <v>6</v>
       </c>
       <c r="K118" s="11" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="L118" s="11" t="s">
         <v>8</v>
@@ -10844,7 +10844,7 @@
         <v>15</v>
       </c>
       <c r="E119" s="30" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="F119" s="12" t="s">
         <v>211</v>
@@ -10853,7 +10853,7 @@
         <v>222</v>
       </c>
       <c r="H119" s="11" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I119" s="11" t="s">
         <v>210</v>
@@ -10862,7 +10862,7 @@
         <v>6</v>
       </c>
       <c r="K119" s="11" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="L119" s="11" t="s">
         <v>8</v>
@@ -10906,7 +10906,7 @@
         <v>15</v>
       </c>
       <c r="E120" s="30" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="F120" s="12" t="s">
         <v>212</v>
@@ -10915,7 +10915,7 @@
         <v>223</v>
       </c>
       <c r="H120" s="11" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="I120" s="11" t="s">
         <v>210</v>
@@ -10924,7 +10924,7 @@
         <v>6</v>
       </c>
       <c r="K120" s="11" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="L120" s="11" t="s">
         <v>8</v>
@@ -10968,16 +10968,16 @@
         <v>15</v>
       </c>
       <c r="E121" s="30" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="F121" s="7" t="s">
         <v>269</v>
       </c>
       <c r="G121" s="6" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="H121" s="7" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="I121" s="7" t="s">
         <v>5</v>
@@ -10992,10 +10992,10 @@
         <v>8</v>
       </c>
       <c r="M121" s="7" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="N121" s="7" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="O121" s="7"/>
       <c r="P121" s="7" t="s">
@@ -11042,16 +11042,16 @@
         <v>2</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="E122" s="30" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="F122" s="33" t="s">
         <v>271</v>
       </c>
       <c r="G122" s="6" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H122" s="23" t="s">
         <v>272</v>
@@ -11102,13 +11102,13 @@
         <v>2</v>
       </c>
       <c r="D123" s="6" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="E123" s="30" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="F123" s="33" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G123" s="6" t="s">
         <v>276</v>
@@ -11162,10 +11162,10 @@
         <v>2</v>
       </c>
       <c r="D124" s="6" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="E124" s="30" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="F124" s="33" t="s">
         <v>278</v>
@@ -11222,10 +11222,10 @@
         <v>2</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="E125" s="30" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="F125" s="33" t="s">
         <v>281</v>
@@ -11297,19 +11297,19 @@
         <v>2</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="E126" s="30" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="F126" s="33" t="s">
         <v>284</v>
       </c>
       <c r="G126" s="6" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H126" s="23" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="I126" s="23"/>
       <c r="J126" s="7" t="s">
@@ -11372,10 +11372,10 @@
         <v>2</v>
       </c>
       <c r="D127" s="6" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="E127" s="30" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="F127" s="33" t="s">
         <v>285</v>
@@ -11446,10 +11446,10 @@
         <v>2</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="E128" s="32" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="F128" s="33" t="s">
         <v>289</v>
@@ -11526,19 +11526,19 @@
         <v>3</v>
       </c>
       <c r="E129" s="32" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="F129" s="35" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="G129" s="6" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="H129" s="7" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="I129" s="23" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="J129" s="7" t="s">
         <v>6</v>
@@ -11603,19 +11603,19 @@
         <v>3</v>
       </c>
       <c r="E130" s="32" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="F130" s="35" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="G130" s="6" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="H130" s="7" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="I130" s="23" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="J130" s="7" t="s">
         <v>6</v>
@@ -11680,19 +11680,19 @@
         <v>3</v>
       </c>
       <c r="E131" s="32" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="F131" s="35" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="G131" s="6" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="H131" s="7" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="I131" s="23" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="J131" s="7" t="s">
         <v>6</v>
@@ -11757,16 +11757,16 @@
         <v>3</v>
       </c>
       <c r="E132" s="32" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="F132" s="35" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="G132" s="6" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="H132" s="7" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="I132" s="23" t="s">
         <v>5</v>
@@ -11834,16 +11834,16 @@
         <v>3</v>
       </c>
       <c r="E133" s="32" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="F133" s="35" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="G133" s="6" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="H133" s="7" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="I133" s="23" t="s">
         <v>5</v>
@@ -11911,16 +11911,16 @@
         <v>3</v>
       </c>
       <c r="E134" s="32" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="F134" s="35" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="G134" s="6" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="H134" s="7" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="I134" s="23" t="s">
         <v>5</v>
@@ -11988,16 +11988,16 @@
         <v>3</v>
       </c>
       <c r="E135" s="32" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="F135" s="35" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="G135" s="6" t="s">
-        <v>742</v>
+        <v>739</v>
       </c>
       <c r="H135" s="7" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="I135" s="23" t="s">
         <v>5</v>
@@ -12065,16 +12065,16 @@
         <v>3</v>
       </c>
       <c r="E136" s="32" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="F136" s="35" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="G136" s="6" t="s">
-        <v>741</v>
+        <v>738</v>
       </c>
       <c r="H136" s="7" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="I136" s="23" t="s">
         <v>5</v>
@@ -12206,7 +12206,7 @@
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1">
       <c r="A2" s="26" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>175</v>
@@ -12214,7 +12214,7 @@
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1">
       <c r="A3" s="26" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>177</v>
@@ -12222,7 +12222,7 @@
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1">
       <c r="A4" s="26" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>176</v>
@@ -12230,7 +12230,7 @@
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1">
       <c r="A5" s="26" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>178</v>
@@ -12238,15 +12238,15 @@
     </row>
     <row r="6" spans="1:2" ht="17.25" customHeight="1">
       <c r="A6" s="26" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>179</v>
@@ -12254,7 +12254,7 @@
     </row>
     <row r="8" spans="1:2" ht="17.25" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>180</v>
@@ -12262,7 +12262,7 @@
     </row>
     <row r="9" spans="1:2" ht="17.25" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>181</v>
@@ -12270,7 +12270,7 @@
     </row>
     <row r="10" spans="1:2" ht="17.25" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>182</v>
@@ -12278,7 +12278,7 @@
     </row>
     <row r="11" spans="1:2" ht="17.25" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>183</v>
@@ -12286,7 +12286,7 @@
     </row>
     <row r="12" spans="1:2" ht="17.25" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>184</v>
@@ -12294,7 +12294,7 @@
     </row>
     <row r="13" spans="1:2" ht="17.25" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>185</v>
@@ -12302,7 +12302,7 @@
     </row>
     <row r="14" spans="1:2" ht="17.25" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>186</v>
@@ -12310,7 +12310,7 @@
     </row>
     <row r="15" spans="1:2" ht="17.25" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>187</v>
@@ -12318,7 +12318,7 @@
     </row>
     <row r="16" spans="1:2" ht="17.25" customHeight="1">
       <c r="A16" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>188</v>
@@ -12326,42 +12326,42 @@
     </row>
     <row r="17" spans="1:2" ht="17.25" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="17.25" customHeight="1">
       <c r="A18" s="1" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="17.25" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="17.25" customHeight="1">
       <c r="A20" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="17.25" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="17.25" customHeight="1">

</xml_diff>

<commit_message>
Corr. nom indicador 530207
</commit_message>
<xml_diff>
--- a/Data/Base_fichas_indicadores.xlsx
+++ b/Data/Base_fichas_indicadores.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\DESCA-app-mainRESPALDO 01.9.2022\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\DESCA-app\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -3377,9 +3377,6 @@
     <t>Poseer ingresos por debajo de la línea de pobreza</t>
   </si>
   <si>
-    <t>Ingresos insuficientes (inferiores al salario mínimo nacional de línea de pobreza)</t>
-  </si>
-  <si>
     <t>Porcentaje de ocupados con salario por debajo del Salario Mínimo Nacional</t>
   </si>
   <si>
@@ -4085,6 +4082,9 @@
   </si>
   <si>
     <t xml:space="preserve">Porcentaje de convenios colectivos que incorporan cláusulas no salariales,: </t>
+  </si>
+  <si>
+    <t>Ingresos insuficientes (inferiores al salario mínimo nacional)</t>
   </si>
 </sst>
 </file>
@@ -4663,9 +4663,9 @@
   <dimension ref="A1:AK269"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A151" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E111" sqref="E111"/>
-      <selection pane="bottomLeft" activeCell="A162" sqref="A162"/>
+      <selection pane="bottomLeft" activeCell="F153" sqref="F153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4766,7 +4766,7 @@
         <v>675</v>
       </c>
       <c r="W1" s="13" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="2" spans="1:37" s="6" customFormat="1">
@@ -7156,10 +7156,10 @@
         <v>8</v>
       </c>
       <c r="N35" s="6" t="s">
+        <v>1339</v>
+      </c>
+      <c r="O35" s="6" t="s">
         <v>1340</v>
-      </c>
-      <c r="O35" s="6" t="s">
-        <v>1341</v>
       </c>
       <c r="P35" s="6" t="s">
         <v>23</v>
@@ -7339,7 +7339,7 @@
         <v>792</v>
       </c>
       <c r="G38" s="51" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="H38" s="6" t="s">
         <v>377</v>
@@ -7405,7 +7405,7 @@
         <v>795</v>
       </c>
       <c r="G39" s="51" t="s">
-        <v>1288</v>
+        <v>1287</v>
       </c>
       <c r="H39" s="6" t="s">
         <v>722</v>
@@ -9205,10 +9205,10 @@
         <v>8</v>
       </c>
       <c r="N63" s="6" t="s">
+        <v>1339</v>
+      </c>
+      <c r="O63" s="6" t="s">
         <v>1340</v>
-      </c>
-      <c r="O63" s="6" t="s">
-        <v>1341</v>
       </c>
       <c r="P63" s="6" t="s">
         <v>54</v>
@@ -9258,7 +9258,7 @@
         <v>714</v>
       </c>
       <c r="I64" s="6" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="J64" s="6" t="s">
         <v>5</v>
@@ -9273,10 +9273,10 @@
         <v>8</v>
       </c>
       <c r="N64" s="6" t="s">
+        <v>1339</v>
+      </c>
+      <c r="O64" s="6" t="s">
         <v>1340</v>
-      </c>
-      <c r="O64" s="6" t="s">
-        <v>1341</v>
       </c>
       <c r="P64" s="6" t="s">
         <v>54</v>
@@ -9342,10 +9342,10 @@
         <v>8</v>
       </c>
       <c r="N65" s="6" t="s">
+        <v>1339</v>
+      </c>
+      <c r="O65" s="6" t="s">
         <v>1340</v>
-      </c>
-      <c r="O65" s="6" t="s">
-        <v>1341</v>
       </c>
       <c r="P65" s="6" t="s">
         <v>54</v>
@@ -9410,10 +9410,10 @@
         <v>8</v>
       </c>
       <c r="N66" s="6" t="s">
+        <v>1339</v>
+      </c>
+      <c r="O66" s="6" t="s">
         <v>1340</v>
-      </c>
-      <c r="O66" s="6" t="s">
-        <v>1341</v>
       </c>
       <c r="P66" s="6" t="s">
         <v>54</v>
@@ -9478,10 +9478,10 @@
         <v>8</v>
       </c>
       <c r="N67" s="6" t="s">
+        <v>1339</v>
+      </c>
+      <c r="O67" s="6" t="s">
         <v>1340</v>
-      </c>
-      <c r="O67" s="6" t="s">
-        <v>1341</v>
       </c>
       <c r="P67" s="6" t="s">
         <v>54</v>
@@ -9547,10 +9547,10 @@
         <v>8</v>
       </c>
       <c r="N68" s="6" t="s">
+        <v>1339</v>
+      </c>
+      <c r="O68" s="6" t="s">
         <v>1340</v>
-      </c>
-      <c r="O68" s="6" t="s">
-        <v>1341</v>
       </c>
       <c r="P68" s="6" t="s">
         <v>54</v>
@@ -9611,16 +9611,16 @@
         <v>6</v>
       </c>
       <c r="L69" s="7" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="M69" s="7" t="s">
         <v>8</v>
       </c>
       <c r="N69" s="6" t="s">
+        <v>1339</v>
+      </c>
+      <c r="O69" s="6" t="s">
         <v>1340</v>
-      </c>
-      <c r="O69" s="6" t="s">
-        <v>1341</v>
       </c>
       <c r="P69" s="7"/>
       <c r="Q69" s="7" t="s">
@@ -10248,7 +10248,7 @@
         <v>730</v>
       </c>
       <c r="I77" s="6" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="J77" s="6" t="s">
         <v>5</v>
@@ -10332,10 +10332,10 @@
         <v>8</v>
       </c>
       <c r="N78" s="6" t="s">
+        <v>1339</v>
+      </c>
+      <c r="O78" s="6" t="s">
         <v>1340</v>
-      </c>
-      <c r="O78" s="6" t="s">
-        <v>1341</v>
       </c>
       <c r="P78" s="6" t="s">
         <v>61</v>
@@ -10401,10 +10401,10 @@
         <v>8</v>
       </c>
       <c r="N79" s="6" t="s">
+        <v>1339</v>
+      </c>
+      <c r="O79" s="6" t="s">
         <v>1340</v>
-      </c>
-      <c r="O79" s="6" t="s">
-        <v>1341</v>
       </c>
       <c r="P79" s="6" t="s">
         <v>61</v>
@@ -10470,10 +10470,10 @@
         <v>8</v>
       </c>
       <c r="N80" s="6" t="s">
+        <v>1339</v>
+      </c>
+      <c r="O80" s="6" t="s">
         <v>1340</v>
-      </c>
-      <c r="O80" s="6" t="s">
-        <v>1341</v>
       </c>
       <c r="P80" s="6" t="s">
         <v>61</v>
@@ -10539,10 +10539,10 @@
         <v>8</v>
       </c>
       <c r="N81" s="6" t="s">
+        <v>1339</v>
+      </c>
+      <c r="O81" s="6" t="s">
         <v>1340</v>
-      </c>
-      <c r="O81" s="6" t="s">
-        <v>1341</v>
       </c>
       <c r="P81" s="6" t="s">
         <v>61</v>
@@ -10608,10 +10608,10 @@
         <v>8</v>
       </c>
       <c r="N82" s="6" t="s">
+        <v>1339</v>
+      </c>
+      <c r="O82" s="6" t="s">
         <v>1340</v>
-      </c>
-      <c r="O82" s="6" t="s">
-        <v>1341</v>
       </c>
       <c r="P82" s="6" t="s">
         <v>61</v>
@@ -10677,10 +10677,10 @@
         <v>8</v>
       </c>
       <c r="N83" s="6" t="s">
+        <v>1339</v>
+      </c>
+      <c r="O83" s="6" t="s">
         <v>1340</v>
-      </c>
-      <c r="O83" s="6" t="s">
-        <v>1341</v>
       </c>
       <c r="P83" s="6" t="s">
         <v>61</v>
@@ -10747,10 +10747,10 @@
         <v>8</v>
       </c>
       <c r="N84" s="6" t="s">
+        <v>1339</v>
+      </c>
+      <c r="O84" s="6" t="s">
         <v>1340</v>
-      </c>
-      <c r="O84" s="6" t="s">
-        <v>1341</v>
       </c>
       <c r="P84" s="6" t="s">
         <v>61</v>
@@ -10829,10 +10829,10 @@
         <v>8</v>
       </c>
       <c r="N85" s="6" t="s">
+        <v>1339</v>
+      </c>
+      <c r="O85" s="6" t="s">
         <v>1340</v>
-      </c>
-      <c r="O85" s="6" t="s">
-        <v>1341</v>
       </c>
       <c r="P85" s="6" t="s">
         <v>61</v>
@@ -10910,10 +10910,10 @@
         <v>8</v>
       </c>
       <c r="N86" s="6" t="s">
+        <v>1339</v>
+      </c>
+      <c r="O86" s="6" t="s">
         <v>1340</v>
-      </c>
-      <c r="O86" s="6" t="s">
-        <v>1341</v>
       </c>
       <c r="P86" s="6" t="s">
         <v>61</v>
@@ -10980,10 +10980,10 @@
         <v>8</v>
       </c>
       <c r="N87" s="6" t="s">
+        <v>1339</v>
+      </c>
+      <c r="O87" s="6" t="s">
         <v>1340</v>
-      </c>
-      <c r="O87" s="6" t="s">
-        <v>1341</v>
       </c>
       <c r="P87" s="6" t="s">
         <v>61</v>
@@ -11061,10 +11061,10 @@
         <v>8</v>
       </c>
       <c r="N88" s="6" t="s">
+        <v>1339</v>
+      </c>
+      <c r="O88" s="6" t="s">
         <v>1340</v>
-      </c>
-      <c r="O88" s="6" t="s">
-        <v>1341</v>
       </c>
       <c r="P88" s="6" t="s">
         <v>61</v>
@@ -11130,10 +11130,10 @@
         <v>8</v>
       </c>
       <c r="N89" s="6" t="s">
+        <v>1339</v>
+      </c>
+      <c r="O89" s="6" t="s">
         <v>1340</v>
-      </c>
-      <c r="O89" s="6" t="s">
-        <v>1341</v>
       </c>
       <c r="P89" s="6" t="s">
         <v>61</v>
@@ -11200,10 +11200,10 @@
         <v>8</v>
       </c>
       <c r="N90" s="6" t="s">
+        <v>1339</v>
+      </c>
+      <c r="O90" s="6" t="s">
         <v>1340</v>
-      </c>
-      <c r="O90" s="6" t="s">
-        <v>1341</v>
       </c>
       <c r="P90" s="6" t="s">
         <v>61</v>
@@ -15296,7 +15296,7 @@
         <v>1098</v>
       </c>
       <c r="H143" s="52" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="I143" s="6" t="s">
         <v>1099</v>
@@ -15494,7 +15494,7 @@
         <v>1104</v>
       </c>
       <c r="H146" s="7" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="I146" s="6" t="s">
         <v>1105</v>
@@ -15559,7 +15559,7 @@
         <v>1088</v>
       </c>
       <c r="H147" s="7" t="s">
-        <v>1297</v>
+        <v>1296</v>
       </c>
       <c r="I147" s="6" t="s">
         <v>1089</v>
@@ -15624,7 +15624,7 @@
         <v>1090</v>
       </c>
       <c r="H148" s="7" t="s">
-        <v>1300</v>
+        <v>1299</v>
       </c>
       <c r="I148" s="6" t="s">
         <v>1091</v>
@@ -15692,7 +15692,7 @@
         <v>1092</v>
       </c>
       <c r="H149" s="7" t="s">
-        <v>1301</v>
+        <v>1300</v>
       </c>
       <c r="I149" s="6" t="s">
         <v>1093</v>
@@ -15757,7 +15757,7 @@
         <v>1094</v>
       </c>
       <c r="H150" s="7" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="I150" s="6" t="s">
         <v>1095</v>
@@ -15822,7 +15822,7 @@
         <v>1096</v>
       </c>
       <c r="H151" s="7" t="s">
-        <v>1302</v>
+        <v>1301</v>
       </c>
       <c r="I151" s="6" t="s">
         <v>1097</v>
@@ -15887,7 +15887,7 @@
         <v>1106</v>
       </c>
       <c r="H152" s="7" t="s">
-        <v>1303</v>
+        <v>1302</v>
       </c>
       <c r="I152" s="6" t="s">
         <v>1107</v>
@@ -15949,16 +15949,16 @@
         <v>15</v>
       </c>
       <c r="F153" s="7" t="s">
+        <v>1342</v>
+      </c>
+      <c r="G153" s="7" t="s">
         <v>1109</v>
       </c>
-      <c r="G153" s="7" t="s">
+      <c r="H153" s="7" t="s">
+        <v>1303</v>
+      </c>
+      <c r="I153" s="6" t="s">
         <v>1110</v>
-      </c>
-      <c r="H153" s="7" t="s">
-        <v>1304</v>
-      </c>
-      <c r="I153" s="6" t="s">
-        <v>1111</v>
       </c>
       <c r="J153" s="6" t="s">
         <v>5</v>
@@ -15973,13 +15973,13 @@
         <v>8</v>
       </c>
       <c r="N153" s="6" t="s">
+        <v>1111</v>
+      </c>
+      <c r="O153" s="6" t="s">
         <v>1112</v>
       </c>
-      <c r="O153" s="6" t="s">
+      <c r="P153" s="7" t="s">
         <v>1113</v>
-      </c>
-      <c r="P153" s="7" t="s">
-        <v>1114</v>
       </c>
       <c r="Q153" s="6" t="s">
         <v>470</v>
@@ -16017,16 +16017,16 @@
         <v>15</v>
       </c>
       <c r="F154" s="7" t="s">
+        <v>1114</v>
+      </c>
+      <c r="G154" s="7" t="s">
+        <v>1305</v>
+      </c>
+      <c r="H154" s="7" t="s">
+        <v>1304</v>
+      </c>
+      <c r="I154" s="6" t="s">
         <v>1115</v>
-      </c>
-      <c r="G154" s="7" t="s">
-        <v>1306</v>
-      </c>
-      <c r="H154" s="7" t="s">
-        <v>1305</v>
-      </c>
-      <c r="I154" s="6" t="s">
-        <v>1116</v>
       </c>
       <c r="J154" s="6" t="s">
         <v>5</v>
@@ -16082,16 +16082,16 @@
         <v>15</v>
       </c>
       <c r="F155" s="7" t="s">
+        <v>1116</v>
+      </c>
+      <c r="G155" s="4" t="s">
         <v>1117</v>
       </c>
-      <c r="G155" s="4" t="s">
+      <c r="H155" s="7" t="s">
         <v>1118</v>
       </c>
-      <c r="H155" s="7" t="s">
+      <c r="I155" s="6" t="s">
         <v>1119</v>
-      </c>
-      <c r="I155" s="6" t="s">
-        <v>1120</v>
       </c>
       <c r="J155" s="6" t="s">
         <v>5</v>
@@ -16112,7 +16112,7 @@
         <v>187</v>
       </c>
       <c r="P155" s="6" t="s">
-        <v>1121</v>
+        <v>1120</v>
       </c>
       <c r="Q155" s="7" t="s">
         <v>475</v>
@@ -16150,16 +16150,16 @@
         <v>15</v>
       </c>
       <c r="F156" s="7" t="s">
+        <v>1121</v>
+      </c>
+      <c r="G156" s="7" t="s">
+        <v>1121</v>
+      </c>
+      <c r="H156" s="7" t="s">
         <v>1122</v>
       </c>
-      <c r="G156" s="7" t="s">
-        <v>1122</v>
-      </c>
-      <c r="H156" s="7" t="s">
+      <c r="I156" s="7" t="s">
         <v>1123</v>
-      </c>
-      <c r="I156" s="7" t="s">
-        <v>1124</v>
       </c>
       <c r="J156" s="7" t="s">
         <v>5</v>
@@ -16168,16 +16168,16 @@
         <v>231</v>
       </c>
       <c r="L156" s="7" t="s">
-        <v>1125</v>
+        <v>1124</v>
       </c>
       <c r="M156" s="7" t="s">
         <v>8</v>
       </c>
       <c r="N156" s="7" t="s">
+        <v>1125</v>
+      </c>
+      <c r="O156" s="7" t="s">
         <v>1126</v>
-      </c>
-      <c r="O156" s="7" t="s">
-        <v>1127</v>
       </c>
       <c r="Q156" s="7" t="s">
         <v>17</v>
@@ -16215,16 +16215,16 @@
         <v>15</v>
       </c>
       <c r="F157" s="7" t="s">
+        <v>1127</v>
+      </c>
+      <c r="G157" s="7" t="s">
+        <v>1127</v>
+      </c>
+      <c r="H157" s="7" t="s">
         <v>1128</v>
       </c>
-      <c r="G157" s="7" t="s">
-        <v>1128</v>
-      </c>
-      <c r="H157" s="7" t="s">
+      <c r="I157" s="7" t="s">
         <v>1129</v>
-      </c>
-      <c r="I157" s="7" t="s">
-        <v>1130</v>
       </c>
       <c r="J157" s="7" t="s">
         <v>5</v>
@@ -16233,16 +16233,16 @@
         <v>231</v>
       </c>
       <c r="L157" s="7" t="s">
-        <v>1131</v>
+        <v>1130</v>
       </c>
       <c r="M157" s="7" t="s">
         <v>8</v>
       </c>
       <c r="N157" s="7" t="s">
+        <v>1131</v>
+      </c>
+      <c r="O157" s="7" t="s">
         <v>1132</v>
-      </c>
-      <c r="O157" s="7" t="s">
-        <v>1133</v>
       </c>
       <c r="Q157" s="7" t="s">
         <v>17</v>
@@ -16280,19 +16280,19 @@
         <v>15</v>
       </c>
       <c r="F158" s="7" t="s">
+        <v>1133</v>
+      </c>
+      <c r="G158" s="7" t="s">
         <v>1134</v>
       </c>
-      <c r="G158" s="7" t="s">
+      <c r="H158" s="7" t="s">
         <v>1135</v>
       </c>
-      <c r="H158" s="7" t="s">
+      <c r="I158" s="7" t="s">
         <v>1136</v>
       </c>
-      <c r="I158" s="7" t="s">
+      <c r="J158" s="7" t="s">
         <v>1137</v>
-      </c>
-      <c r="J158" s="7" t="s">
-        <v>1138</v>
       </c>
       <c r="K158" s="7" t="s">
         <v>231</v>
@@ -16346,16 +16346,16 @@
         <v>15</v>
       </c>
       <c r="F159" s="40" t="s">
+        <v>1138</v>
+      </c>
+      <c r="G159" s="40" t="s">
+        <v>1341</v>
+      </c>
+      <c r="H159" s="40" t="s">
         <v>1139</v>
       </c>
-      <c r="G159" s="40" t="s">
-        <v>1342</v>
-      </c>
-      <c r="H159" s="40" t="s">
+      <c r="I159" s="40" t="s">
         <v>1140</v>
-      </c>
-      <c r="I159" s="40" t="s">
-        <v>1141</v>
       </c>
       <c r="J159" s="40" t="s">
         <v>5</v>
@@ -16364,20 +16364,20 @@
         <v>6</v>
       </c>
       <c r="L159" s="40" t="s">
+        <v>1141</v>
+      </c>
+      <c r="M159" s="44" t="s">
         <v>1142</v>
       </c>
-      <c r="M159" s="44" t="s">
+      <c r="N159" s="40" t="s">
         <v>1143</v>
       </c>
-      <c r="N159" s="40" t="s">
+      <c r="O159" s="40" t="s">
         <v>1144</v>
-      </c>
-      <c r="O159" s="40" t="s">
-        <v>1145</v>
       </c>
       <c r="P159" s="40"/>
       <c r="Q159" s="40" t="s">
-        <v>1146</v>
+        <v>1145</v>
       </c>
       <c r="R159" s="44">
         <v>0</v>
@@ -16412,10 +16412,10 @@
         <v>104</v>
       </c>
       <c r="F160" s="37" t="s">
-        <v>1289</v>
+        <v>1288</v>
       </c>
       <c r="G160" s="3" t="s">
-        <v>1294</v>
+        <v>1293</v>
       </c>
       <c r="H160" s="6" t="s">
         <v>790</v>
@@ -16478,10 +16478,10 @@
         <v>104</v>
       </c>
       <c r="F161" s="37" t="s">
-        <v>1290</v>
+        <v>1289</v>
       </c>
       <c r="G161" s="3" t="s">
-        <v>1293</v>
+        <v>1292</v>
       </c>
       <c r="H161" s="6" t="s">
         <v>793</v>
@@ -16544,10 +16544,10 @@
         <v>104</v>
       </c>
       <c r="F162" s="37" t="s">
+        <v>1290</v>
+      </c>
+      <c r="G162" s="3" t="s">
         <v>1291</v>
-      </c>
-      <c r="G162" s="3" t="s">
-        <v>1292</v>
       </c>
       <c r="H162" s="6" t="s">
         <v>796</v>
@@ -17261,10 +17261,10 @@
         <v>3</v>
       </c>
       <c r="F173" s="7" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="G173" s="7" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="H173" s="6" t="s">
         <v>798</v>
@@ -17329,10 +17329,10 @@
         <v>3</v>
       </c>
       <c r="F174" s="7" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="G174" s="7" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="H174" s="6" t="s">
         <v>378</v>
@@ -17397,10 +17397,10 @@
         <v>3</v>
       </c>
       <c r="F175" s="36" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="G175" s="6" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="H175" s="6" t="s">
         <v>419</v>
@@ -18697,19 +18697,19 @@
         <v>2</v>
       </c>
       <c r="E194" s="7" t="s">
+        <v>1146</v>
+      </c>
+      <c r="F194" s="6" t="s">
         <v>1147</v>
       </c>
-      <c r="F194" s="6" t="s">
+      <c r="G194" s="6" t="s">
         <v>1148</v>
       </c>
-      <c r="G194" s="6" t="s">
+      <c r="H194" s="7" t="s">
         <v>1149</v>
       </c>
-      <c r="H194" s="7" t="s">
+      <c r="I194" s="7" t="s">
         <v>1150</v>
-      </c>
-      <c r="I194" s="7" t="s">
-        <v>1151</v>
       </c>
       <c r="J194" s="6" t="s">
         <v>5</v>
@@ -18765,19 +18765,19 @@
         <v>2</v>
       </c>
       <c r="E195" s="7" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F195" s="6" t="s">
+        <v>1151</v>
+      </c>
+      <c r="G195" s="6" t="s">
         <v>1152</v>
       </c>
-      <c r="G195" s="6" t="s">
+      <c r="H195" s="7" t="s">
         <v>1153</v>
       </c>
-      <c r="H195" s="7" t="s">
+      <c r="I195" s="46" t="s">
         <v>1154</v>
-      </c>
-      <c r="I195" s="46" t="s">
-        <v>1155</v>
       </c>
       <c r="J195" s="7" t="s">
         <v>979</v>
@@ -18833,19 +18833,19 @@
         <v>2</v>
       </c>
       <c r="E196" s="7" t="s">
-        <v>1147</v>
+        <v>1146</v>
       </c>
       <c r="F196" s="6" t="s">
+        <v>1155</v>
+      </c>
+      <c r="G196" s="6" t="s">
+        <v>1155</v>
+      </c>
+      <c r="H196" s="7" t="s">
         <v>1156</v>
       </c>
-      <c r="G196" s="6" t="s">
-        <v>1156</v>
-      </c>
-      <c r="H196" s="7" t="s">
+      <c r="I196" s="7" t="s">
         <v>1157</v>
-      </c>
-      <c r="I196" s="7" t="s">
-        <v>1158</v>
       </c>
       <c r="J196" s="7" t="s">
         <v>806</v>
@@ -18866,7 +18866,7 @@
         <v>909</v>
       </c>
       <c r="Q196" s="7" t="s">
-        <v>1159</v>
+        <v>1158</v>
       </c>
       <c r="R196" s="44">
         <v>0</v>
@@ -19395,7 +19395,7 @@
         <v>912</v>
       </c>
       <c r="G204" s="7" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="H204" s="7" t="s">
         <v>913</v>
@@ -19464,7 +19464,7 @@
         <v>919</v>
       </c>
       <c r="G205" s="7" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="H205" s="7" t="s">
         <v>920</v>
@@ -19533,7 +19533,7 @@
         <v>922</v>
       </c>
       <c r="G206" s="7" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="H206" s="7" t="s">
         <v>923</v>
@@ -19602,7 +19602,7 @@
         <v>925</v>
       </c>
       <c r="G207" s="7" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="H207" s="7" t="s">
         <v>926</v>
@@ -19742,10 +19742,10 @@
         <v>3</v>
       </c>
       <c r="F209" s="7" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="G209" s="7" t="s">
-        <v>1317</v>
+        <v>1316</v>
       </c>
       <c r="H209" s="7" t="s">
         <v>1048</v>
@@ -19810,10 +19810,10 @@
         <v>3</v>
       </c>
       <c r="F210" s="7" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="G210" s="7" t="s">
-        <v>1318</v>
+        <v>1317</v>
       </c>
       <c r="H210" s="7" t="s">
         <v>1051</v>
@@ -19878,10 +19878,10 @@
         <v>3</v>
       </c>
       <c r="F211" s="7" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="G211" s="7" t="s">
-        <v>1319</v>
+        <v>1318</v>
       </c>
       <c r="H211" s="7" t="s">
         <v>1053</v>
@@ -19946,10 +19946,10 @@
         <v>3</v>
       </c>
       <c r="F212" s="7" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="G212" s="7" t="s">
-        <v>1320</v>
+        <v>1319</v>
       </c>
       <c r="H212" s="7" t="s">
         <v>1055</v>
@@ -20014,10 +20014,10 @@
         <v>3</v>
       </c>
       <c r="F213" s="7" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="G213" s="7" t="s">
-        <v>1321</v>
+        <v>1320</v>
       </c>
       <c r="H213" s="7" t="s">
         <v>1057</v>
@@ -20082,10 +20082,10 @@
         <v>3</v>
       </c>
       <c r="F214" s="7" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="G214" s="7" t="s">
-        <v>1322</v>
+        <v>1321</v>
       </c>
       <c r="H214" s="7" t="s">
         <v>1059</v>
@@ -20150,10 +20150,10 @@
         <v>3</v>
       </c>
       <c r="F215" s="7" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="G215" s="7" t="s">
-        <v>1323</v>
+        <v>1322</v>
       </c>
       <c r="H215" s="7" t="s">
         <v>1061</v>
@@ -20218,10 +20218,10 @@
         <v>3</v>
       </c>
       <c r="F216" s="7" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="G216" s="7" t="s">
-        <v>1324</v>
+        <v>1323</v>
       </c>
       <c r="H216" s="7" t="s">
         <v>1063</v>
@@ -20286,10 +20286,10 @@
         <v>3</v>
       </c>
       <c r="F217" s="7" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="G217" s="7" t="s">
-        <v>1325</v>
+        <v>1324</v>
       </c>
       <c r="H217" s="7" t="s">
         <v>1065</v>
@@ -20345,7 +20345,7 @@
         <v>1</v>
       </c>
       <c r="C218" s="7" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="D218" s="7" t="s">
         <v>2</v>
@@ -20372,7 +20372,7 @@
         <v>6</v>
       </c>
       <c r="L218" s="7" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="M218" s="7" t="s">
         <v>940</v>
@@ -20417,7 +20417,7 @@
         <v>1</v>
       </c>
       <c r="C219" s="7" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="D219" s="7" t="s">
         <v>2</v>
@@ -20444,7 +20444,7 @@
         <v>6</v>
       </c>
       <c r="L219" s="7" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="M219" s="7" t="s">
         <v>940</v>
@@ -20489,7 +20489,7 @@
         <v>35</v>
       </c>
       <c r="C220" s="7" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="D220" s="7" t="s">
         <v>2</v>
@@ -20498,16 +20498,16 @@
         <v>36</v>
       </c>
       <c r="F220" s="7" t="s">
+        <v>1165</v>
+      </c>
+      <c r="G220" s="7" t="s">
         <v>1166</v>
       </c>
-      <c r="G220" s="7" t="s">
+      <c r="H220" s="6" t="s">
         <v>1167</v>
       </c>
-      <c r="H220" s="6" t="s">
+      <c r="I220" s="6" t="s">
         <v>1168</v>
-      </c>
-      <c r="I220" s="6" t="s">
-        <v>1169</v>
       </c>
       <c r="J220" s="6" t="s">
         <v>5</v>
@@ -20516,7 +20516,7 @@
         <v>6</v>
       </c>
       <c r="L220" s="7" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="M220" s="7" t="s">
         <v>940</v>
@@ -20560,7 +20560,7 @@
         <v>35</v>
       </c>
       <c r="C221" s="7" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="D221" s="7" t="s">
         <v>2</v>
@@ -20569,16 +20569,16 @@
         <v>41</v>
       </c>
       <c r="F221" s="7" t="s">
+        <v>1169</v>
+      </c>
+      <c r="G221" s="7" t="s">
         <v>1170</v>
-      </c>
-      <c r="G221" s="7" t="s">
-        <v>1171</v>
       </c>
       <c r="H221" s="6" t="s">
         <v>419</v>
       </c>
       <c r="I221" s="6" t="s">
-        <v>1172</v>
+        <v>1171</v>
       </c>
       <c r="J221" s="6" t="s">
         <v>5</v>
@@ -20587,7 +20587,7 @@
         <v>6</v>
       </c>
       <c r="L221" s="7" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="M221" s="7" t="s">
         <v>940</v>
@@ -20631,7 +20631,7 @@
         <v>35</v>
       </c>
       <c r="C222" s="7" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="D222" s="7" t="s">
         <v>2</v>
@@ -20640,16 +20640,16 @@
         <v>41</v>
       </c>
       <c r="F222" s="7" t="s">
+        <v>1172</v>
+      </c>
+      <c r="G222" s="7" t="s">
         <v>1173</v>
-      </c>
-      <c r="G222" s="7" t="s">
-        <v>1174</v>
       </c>
       <c r="H222" s="6" t="s">
         <v>378</v>
       </c>
       <c r="I222" s="6" t="s">
-        <v>1175</v>
+        <v>1174</v>
       </c>
       <c r="J222" s="6" t="s">
         <v>5</v>
@@ -20658,7 +20658,7 @@
         <v>6</v>
       </c>
       <c r="L222" s="7" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="M222" s="7" t="s">
         <v>940</v>
@@ -20702,7 +20702,7 @@
         <v>35</v>
       </c>
       <c r="C223" s="7" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="D223" s="7" t="s">
         <v>2</v>
@@ -20711,16 +20711,16 @@
         <v>41</v>
       </c>
       <c r="F223" s="7" t="s">
+        <v>1175</v>
+      </c>
+      <c r="G223" s="7" t="s">
         <v>1176</v>
-      </c>
-      <c r="G223" s="7" t="s">
-        <v>1177</v>
       </c>
       <c r="H223" s="6" t="s">
         <v>304</v>
       </c>
       <c r="I223" s="6" t="s">
-        <v>1178</v>
+        <v>1177</v>
       </c>
       <c r="J223" s="6" t="s">
         <v>5</v>
@@ -20729,7 +20729,7 @@
         <v>6</v>
       </c>
       <c r="L223" s="7" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="M223" s="7" t="s">
         <v>940</v>
@@ -20773,7 +20773,7 @@
         <v>35</v>
       </c>
       <c r="C224" s="7" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="D224" s="7" t="s">
         <v>2</v>
@@ -20782,16 +20782,16 @@
         <v>41</v>
       </c>
       <c r="F224" s="7" t="s">
+        <v>1178</v>
+      </c>
+      <c r="G224" s="7" t="s">
         <v>1179</v>
-      </c>
-      <c r="G224" s="7" t="s">
-        <v>1180</v>
       </c>
       <c r="H224" s="6" t="s">
         <v>420</v>
       </c>
       <c r="I224" s="6" t="s">
-        <v>1181</v>
+        <v>1180</v>
       </c>
       <c r="J224" s="6" t="s">
         <v>5</v>
@@ -20800,7 +20800,7 @@
         <v>6</v>
       </c>
       <c r="L224" s="7" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="M224" s="7" t="s">
         <v>940</v>
@@ -20850,7 +20850,7 @@
         <v>35</v>
       </c>
       <c r="C225" s="7" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="D225" s="7" t="s">
         <v>2</v>
@@ -20859,16 +20859,16 @@
         <v>46</v>
       </c>
       <c r="F225" s="7" t="s">
+        <v>1181</v>
+      </c>
+      <c r="G225" s="7" t="s">
         <v>1182</v>
-      </c>
-      <c r="G225" s="7" t="s">
-        <v>1183</v>
       </c>
       <c r="H225" s="6" t="s">
         <v>421</v>
       </c>
       <c r="I225" s="27" t="s">
-        <v>1184</v>
+        <v>1183</v>
       </c>
       <c r="J225" s="6" t="s">
         <v>5</v>
@@ -20877,7 +20877,7 @@
         <v>6</v>
       </c>
       <c r="L225" s="7" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="M225" s="7" t="s">
         <v>940</v>
@@ -20927,7 +20927,7 @@
         <v>35</v>
       </c>
       <c r="C226" s="7" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="D226" s="7" t="s">
         <v>2</v>
@@ -20936,16 +20936,16 @@
         <v>47</v>
       </c>
       <c r="F226" s="6" t="s">
+        <v>1184</v>
+      </c>
+      <c r="G226" s="7" t="s">
         <v>1185</v>
-      </c>
-      <c r="G226" s="7" t="s">
-        <v>1186</v>
       </c>
       <c r="H226" s="6" t="s">
         <v>641</v>
       </c>
       <c r="I226" s="27" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="J226" s="6" t="s">
         <v>5</v>
@@ -20954,7 +20954,7 @@
         <v>6</v>
       </c>
       <c r="L226" s="7" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="M226" s="7" t="s">
         <v>940</v>
@@ -21004,7 +21004,7 @@
         <v>35</v>
       </c>
       <c r="C227" s="7" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="D227" s="7" t="s">
         <v>2</v>
@@ -21013,16 +21013,16 @@
         <v>47</v>
       </c>
       <c r="F227" s="7" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G227" s="7" t="s">
         <v>1188</v>
-      </c>
-      <c r="G227" s="7" t="s">
-        <v>1189</v>
       </c>
       <c r="H227" s="6" t="s">
         <v>379</v>
       </c>
       <c r="I227" s="6" t="s">
-        <v>1190</v>
+        <v>1189</v>
       </c>
       <c r="J227" s="6" t="s">
         <v>5</v>
@@ -21031,7 +21031,7 @@
         <v>6</v>
       </c>
       <c r="L227" s="7" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="M227" s="7" t="s">
         <v>940</v>
@@ -21081,7 +21081,7 @@
         <v>52</v>
       </c>
       <c r="C228" s="7" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="D228" s="7" t="s">
         <v>2</v>
@@ -21108,7 +21108,7 @@
         <v>6</v>
       </c>
       <c r="L228" s="7" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="M228" s="7" t="s">
         <v>940</v>
@@ -21155,7 +21155,7 @@
         <v>52</v>
       </c>
       <c r="C229" s="7" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="D229" s="7" t="s">
         <v>2</v>
@@ -21167,13 +21167,13 @@
         <v>996</v>
       </c>
       <c r="G229" s="7" t="s">
-        <v>1328</v>
+        <v>1327</v>
       </c>
       <c r="H229" s="6" t="s">
         <v>714</v>
       </c>
       <c r="I229" s="6" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="J229" s="6" t="s">
         <v>5</v>
@@ -21182,7 +21182,7 @@
         <v>6</v>
       </c>
       <c r="L229" s="7" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="M229" s="7" t="s">
         <v>940</v>
@@ -21232,7 +21232,7 @@
         <v>52</v>
       </c>
       <c r="C230" s="7" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="D230" s="7" t="s">
         <v>2</v>
@@ -21244,7 +21244,7 @@
         <v>997</v>
       </c>
       <c r="G230" s="7" t="s">
-        <v>1329</v>
+        <v>1328</v>
       </c>
       <c r="H230" s="6" t="s">
         <v>384</v>
@@ -21259,7 +21259,7 @@
         <v>6</v>
       </c>
       <c r="L230" s="7" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="M230" s="7" t="s">
         <v>940</v>
@@ -21309,7 +21309,7 @@
         <v>52</v>
       </c>
       <c r="C231" s="7" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="D231" s="7" t="s">
         <v>2</v>
@@ -21321,13 +21321,13 @@
         <v>999</v>
       </c>
       <c r="G231" s="7" t="s">
-        <v>1330</v>
+        <v>1329</v>
       </c>
       <c r="H231" s="6" t="s">
         <v>714</v>
       </c>
       <c r="I231" s="6" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="J231" s="6" t="s">
         <v>5</v>
@@ -21336,7 +21336,7 @@
         <v>6</v>
       </c>
       <c r="L231" s="7" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="M231" s="7" t="s">
         <v>940</v>
@@ -21386,7 +21386,7 @@
         <v>70</v>
       </c>
       <c r="C232" s="7" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="D232" s="7" t="s">
         <v>2</v>
@@ -21413,7 +21413,7 @@
         <v>6</v>
       </c>
       <c r="L232" s="7" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="M232" s="7" t="s">
         <v>940</v>
@@ -21463,7 +21463,7 @@
         <v>1000</v>
       </c>
       <c r="C233" s="7" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="D233" s="7" t="s">
         <v>2</v>
@@ -21478,7 +21478,7 @@
         <v>1074</v>
       </c>
       <c r="H233" s="7" t="s">
-        <v>1295</v>
+        <v>1294</v>
       </c>
       <c r="I233" s="6" t="s">
         <v>1075</v>
@@ -21490,7 +21490,7 @@
         <v>6</v>
       </c>
       <c r="L233" s="7" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="M233" s="7" t="s">
         <v>940</v>
@@ -21531,7 +21531,7 @@
         <v>1000</v>
       </c>
       <c r="C234" s="7" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="D234" s="7" t="s">
         <v>2</v>
@@ -21546,7 +21546,7 @@
         <v>1076</v>
       </c>
       <c r="H234" s="7" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="I234" s="6" t="s">
         <v>1078</v>
@@ -21558,7 +21558,7 @@
         <v>6</v>
       </c>
       <c r="L234" s="7" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="M234" s="7" t="s">
         <v>940</v>
@@ -21599,7 +21599,7 @@
         <v>1000</v>
       </c>
       <c r="C235" s="7" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="D235" s="7" t="s">
         <v>2</v>
@@ -21626,7 +21626,7 @@
         <v>6</v>
       </c>
       <c r="L235" s="7" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="M235" s="7" t="s">
         <v>940</v>
@@ -21667,7 +21667,7 @@
         <v>1000</v>
       </c>
       <c r="C236" s="7" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="D236" s="7" t="s">
         <v>2</v>
@@ -21682,7 +21682,7 @@
         <v>1081</v>
       </c>
       <c r="H236" s="7" t="s">
-        <v>1296</v>
+        <v>1295</v>
       </c>
       <c r="I236" s="6" t="s">
         <v>1082</v>
@@ -21694,7 +21694,7 @@
         <v>6</v>
       </c>
       <c r="L236" s="7" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="M236" s="7" t="s">
         <v>940</v>
@@ -21735,7 +21735,7 @@
         <v>1000</v>
       </c>
       <c r="C237" s="7" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="D237" s="7" t="s">
         <v>2</v>
@@ -21750,7 +21750,7 @@
         <v>1083</v>
       </c>
       <c r="H237" s="7" t="s">
-        <v>1298</v>
+        <v>1297</v>
       </c>
       <c r="I237" s="6" t="s">
         <v>1084</v>
@@ -21762,7 +21762,7 @@
         <v>6</v>
       </c>
       <c r="L237" s="7" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="M237" s="7" t="s">
         <v>940</v>
@@ -21803,7 +21803,7 @@
         <v>1000</v>
       </c>
       <c r="C238" s="7" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="D238" s="7" t="s">
         <v>2</v>
@@ -21815,10 +21815,10 @@
         <v>1085</v>
       </c>
       <c r="G238" s="7" t="s">
-        <v>1326</v>
+        <v>1325</v>
       </c>
       <c r="H238" s="6" t="s">
-        <v>1299</v>
+        <v>1298</v>
       </c>
       <c r="I238" s="6" t="s">
         <v>1086</v>
@@ -21830,7 +21830,7 @@
         <v>6</v>
       </c>
       <c r="L238" s="7" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="M238" s="7" t="s">
         <v>940</v>
@@ -22090,16 +22090,16 @@
         <v>47</v>
       </c>
       <c r="F242" s="41" t="s">
+        <v>1159</v>
+      </c>
+      <c r="G242" s="41" t="s">
         <v>1160</v>
       </c>
-      <c r="G242" s="41" t="s">
+      <c r="H242" s="40" t="s">
         <v>1161</v>
       </c>
-      <c r="H242" s="40" t="s">
+      <c r="I242" s="41" t="s">
         <v>1162</v>
-      </c>
-      <c r="I242" s="41" t="s">
-        <v>1163</v>
       </c>
       <c r="J242" s="40" t="s">
         <v>5</v>
@@ -22114,10 +22114,10 @@
         <v>8</v>
       </c>
       <c r="N242" s="41" t="s">
+        <v>1163</v>
+      </c>
+      <c r="O242" s="40" t="s">
         <v>1164</v>
-      </c>
-      <c r="O242" s="40" t="s">
-        <v>1165</v>
       </c>
       <c r="P242" s="40"/>
       <c r="Q242" s="40" t="s">
@@ -22386,7 +22386,7 @@
         <v>1072</v>
       </c>
       <c r="H246" s="42" t="s">
-        <v>1338</v>
+        <v>1337</v>
       </c>
       <c r="I246" s="42" t="s">
         <v>1073</v>
@@ -22441,25 +22441,25 @@
         <v>884</v>
       </c>
       <c r="D247" s="40" t="s">
+        <v>1190</v>
+      </c>
+      <c r="E247" s="40" t="s">
+        <v>1190</v>
+      </c>
+      <c r="F247" s="7" t="s">
         <v>1191</v>
       </c>
-      <c r="E247" s="40" t="s">
+      <c r="G247" s="6" t="s">
         <v>1191</v>
       </c>
-      <c r="F247" s="7" t="s">
+      <c r="H247" s="6" t="s">
         <v>1192</v>
       </c>
-      <c r="G247" s="6" t="s">
-        <v>1192</v>
-      </c>
-      <c r="H247" s="6" t="s">
+      <c r="I247" s="6" t="s">
         <v>1193</v>
       </c>
-      <c r="I247" s="6" t="s">
+      <c r="J247" s="6" t="s">
         <v>1194</v>
-      </c>
-      <c r="J247" s="6" t="s">
-        <v>1195</v>
       </c>
       <c r="K247" s="6" t="s">
         <v>6</v>
@@ -22508,22 +22508,22 @@
         <v>911</v>
       </c>
       <c r="D248" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="E248" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F248" s="7" t="s">
+        <v>1195</v>
+      </c>
+      <c r="G248" s="7" t="s">
         <v>1196</v>
       </c>
-      <c r="G248" s="7" t="s">
+      <c r="H248" s="7" t="s">
         <v>1197</v>
       </c>
-      <c r="H248" s="7" t="s">
+      <c r="I248" s="7" t="s">
         <v>1198</v>
-      </c>
-      <c r="I248" s="7" t="s">
-        <v>1199</v>
       </c>
       <c r="J248" s="7" t="s">
         <v>5</v>
@@ -22544,7 +22544,7 @@
         <v>917</v>
       </c>
       <c r="Q248" s="7" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="R248" s="7">
         <v>0</v>
@@ -22574,22 +22574,22 @@
         <v>911</v>
       </c>
       <c r="D249" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="E249" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F249" s="7" t="s">
+        <v>1200</v>
+      </c>
+      <c r="G249" s="7" t="s">
         <v>1201</v>
       </c>
-      <c r="G249" s="7" t="s">
+      <c r="H249" s="7" t="s">
         <v>1202</v>
       </c>
-      <c r="H249" s="7" t="s">
+      <c r="I249" s="7" t="s">
         <v>1203</v>
-      </c>
-      <c r="I249" s="7" t="s">
-        <v>1204</v>
       </c>
       <c r="J249" s="7" t="s">
         <v>5</v>
@@ -22610,7 +22610,7 @@
         <v>917</v>
       </c>
       <c r="Q249" s="7" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="R249" s="7">
         <v>0</v>
@@ -22640,22 +22640,22 @@
         <v>911</v>
       </c>
       <c r="D250" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="E250" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F250" s="7" t="s">
+        <v>1204</v>
+      </c>
+      <c r="G250" s="7" t="s">
         <v>1205</v>
       </c>
-      <c r="G250" s="7" t="s">
+      <c r="H250" s="7" t="s">
         <v>1206</v>
       </c>
-      <c r="H250" s="7" t="s">
+      <c r="I250" s="7" t="s">
         <v>1207</v>
-      </c>
-      <c r="I250" s="7" t="s">
-        <v>1208</v>
       </c>
       <c r="J250" s="7" t="s">
         <v>5</v>
@@ -22676,7 +22676,7 @@
         <v>917</v>
       </c>
       <c r="Q250" s="7" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="R250" s="7">
         <v>0</v>
@@ -22706,22 +22706,22 @@
         <v>911</v>
       </c>
       <c r="D251" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="E251" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F251" s="7" t="s">
+        <v>1208</v>
+      </c>
+      <c r="G251" s="7" t="s">
         <v>1209</v>
       </c>
-      <c r="G251" s="7" t="s">
+      <c r="H251" s="7" t="s">
         <v>1210</v>
       </c>
-      <c r="H251" s="7" t="s">
+      <c r="I251" s="7" t="s">
         <v>1211</v>
-      </c>
-      <c r="I251" s="7" t="s">
-        <v>1212</v>
       </c>
       <c r="J251" s="7" t="s">
         <v>5</v>
@@ -22742,7 +22742,7 @@
         <v>917</v>
       </c>
       <c r="Q251" s="7" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="R251" s="7">
         <v>0</v>
@@ -22773,22 +22773,22 @@
         <v>911</v>
       </c>
       <c r="D252" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="E252" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F252" s="7" t="s">
+        <v>1212</v>
+      </c>
+      <c r="G252" s="7" t="s">
         <v>1213</v>
       </c>
-      <c r="G252" s="7" t="s">
+      <c r="H252" s="7" t="s">
         <v>1214</v>
       </c>
-      <c r="H252" s="7" t="s">
+      <c r="I252" s="7" t="s">
         <v>1215</v>
-      </c>
-      <c r="I252" s="7" t="s">
-        <v>1216</v>
       </c>
       <c r="J252" s="7" t="s">
         <v>5</v>
@@ -22810,7 +22810,7 @@
       </c>
       <c r="P252" s="7"/>
       <c r="Q252" s="7" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="R252" s="7">
         <v>0</v>
@@ -22845,22 +22845,22 @@
         <v>911</v>
       </c>
       <c r="D253" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="E253" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F253" s="7" t="s">
+        <v>1216</v>
+      </c>
+      <c r="G253" s="7" t="s">
         <v>1217</v>
       </c>
-      <c r="G253" s="7" t="s">
+      <c r="H253" s="7" t="s">
         <v>1218</v>
       </c>
-      <c r="H253" s="7" t="s">
+      <c r="I253" s="7" t="s">
         <v>1219</v>
-      </c>
-      <c r="I253" s="7" t="s">
-        <v>1220</v>
       </c>
       <c r="J253" s="7" t="s">
         <v>5</v>
@@ -22881,7 +22881,7 @@
         <v>917</v>
       </c>
       <c r="Q253" s="7" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="R253" s="7">
         <v>0</v>
@@ -22918,22 +22918,22 @@
         <v>911</v>
       </c>
       <c r="D254" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="E254" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F254" s="7" t="s">
+        <v>1220</v>
+      </c>
+      <c r="G254" s="7" t="s">
         <v>1221</v>
       </c>
-      <c r="G254" s="7" t="s">
+      <c r="H254" s="7" t="s">
         <v>1222</v>
       </c>
-      <c r="H254" s="7" t="s">
+      <c r="I254" s="7" t="s">
         <v>1223</v>
-      </c>
-      <c r="I254" s="7" t="s">
-        <v>1224</v>
       </c>
       <c r="J254" s="7" t="s">
         <v>5</v>
@@ -22954,7 +22954,7 @@
         <v>917</v>
       </c>
       <c r="Q254" s="7" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="R254" s="7">
         <v>0</v>
@@ -22992,22 +22992,22 @@
         <v>911</v>
       </c>
       <c r="D255" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="E255" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F255" s="7" t="s">
+        <v>1224</v>
+      </c>
+      <c r="G255" s="7" t="s">
         <v>1225</v>
       </c>
-      <c r="G255" s="7" t="s">
+      <c r="H255" s="7" t="s">
         <v>1226</v>
       </c>
-      <c r="H255" s="7" t="s">
+      <c r="I255" s="7" t="s">
         <v>1227</v>
-      </c>
-      <c r="I255" s="7" t="s">
-        <v>1228</v>
       </c>
       <c r="J255" s="7" t="s">
         <v>5</v>
@@ -23029,7 +23029,7 @@
       </c>
       <c r="P255" s="7"/>
       <c r="Q255" s="7" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="R255" s="7">
         <v>0</v>
@@ -23066,22 +23066,22 @@
         <v>911</v>
       </c>
       <c r="D256" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="E256" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F256" s="7" t="s">
+        <v>1228</v>
+      </c>
+      <c r="G256" s="7" t="s">
         <v>1229</v>
       </c>
-      <c r="G256" s="7" t="s">
+      <c r="H256" s="7" t="s">
         <v>1230</v>
       </c>
-      <c r="H256" s="7" t="s">
+      <c r="I256" s="7" t="s">
         <v>1231</v>
-      </c>
-      <c r="I256" s="7" t="s">
-        <v>1232</v>
       </c>
       <c r="J256" s="7" t="s">
         <v>5</v>
@@ -23103,7 +23103,7 @@
       </c>
       <c r="P256" s="7"/>
       <c r="Q256" s="7" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="R256" s="7">
         <v>0</v>
@@ -23140,22 +23140,22 @@
         <v>911</v>
       </c>
       <c r="D257" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="E257" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F257" s="7" t="s">
+        <v>1232</v>
+      </c>
+      <c r="G257" s="7" t="s">
         <v>1233</v>
       </c>
-      <c r="G257" s="7" t="s">
+      <c r="H257" s="7" t="s">
         <v>1234</v>
       </c>
-      <c r="H257" s="7" t="s">
+      <c r="I257" s="7" t="s">
         <v>1235</v>
-      </c>
-      <c r="I257" s="7" t="s">
-        <v>1236</v>
       </c>
       <c r="J257" s="7" t="s">
         <v>5</v>
@@ -23177,7 +23177,7 @@
       </c>
       <c r="P257" s="7"/>
       <c r="Q257" s="7" t="s">
-        <v>1200</v>
+        <v>1199</v>
       </c>
       <c r="R257" s="7">
         <v>0</v>
@@ -23214,22 +23214,22 @@
         <v>911</v>
       </c>
       <c r="D258" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="E258" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F258" s="7" t="s">
+        <v>1236</v>
+      </c>
+      <c r="G258" s="7" t="s">
+        <v>1236</v>
+      </c>
+      <c r="H258" s="7" t="s">
         <v>1237</v>
       </c>
-      <c r="G258" s="7" t="s">
-        <v>1237</v>
-      </c>
-      <c r="H258" s="7" t="s">
+      <c r="I258" s="45" t="s">
         <v>1238</v>
-      </c>
-      <c r="I258" s="45" t="s">
-        <v>1239</v>
       </c>
       <c r="J258" s="7" t="s">
         <v>979</v>
@@ -23288,22 +23288,22 @@
         <v>911</v>
       </c>
       <c r="D259" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="E259" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F259" s="7" t="s">
+        <v>1239</v>
+      </c>
+      <c r="G259" s="7" t="s">
+        <v>1239</v>
+      </c>
+      <c r="H259" s="7" t="s">
         <v>1240</v>
       </c>
-      <c r="G259" s="7" t="s">
-        <v>1240</v>
-      </c>
-      <c r="H259" s="7" t="s">
-        <v>1241</v>
-      </c>
       <c r="I259" s="45" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="J259" s="7" t="s">
         <v>979</v>
@@ -23362,22 +23362,22 @@
         <v>911</v>
       </c>
       <c r="D260" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="E260" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F260" s="7" t="s">
+        <v>1241</v>
+      </c>
+      <c r="G260" s="7" t="s">
+        <v>1241</v>
+      </c>
+      <c r="H260" s="7" t="s">
         <v>1242</v>
       </c>
-      <c r="G260" s="7" t="s">
-        <v>1242</v>
-      </c>
-      <c r="H260" s="7" t="s">
-        <v>1243</v>
-      </c>
       <c r="I260" s="45" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="J260" s="7" t="s">
         <v>979</v>
@@ -23436,22 +23436,22 @@
         <v>911</v>
       </c>
       <c r="D261" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="E261" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F261" s="7" t="s">
+        <v>1243</v>
+      </c>
+      <c r="G261" s="7" t="s">
+        <v>1243</v>
+      </c>
+      <c r="H261" s="7" t="s">
         <v>1244</v>
       </c>
-      <c r="G261" s="7" t="s">
-        <v>1244</v>
-      </c>
-      <c r="H261" s="7" t="s">
-        <v>1245</v>
-      </c>
       <c r="I261" s="45" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="J261" s="7" t="s">
         <v>979</v>
@@ -23510,22 +23510,22 @@
         <v>911</v>
       </c>
       <c r="D262" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="E262" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F262" s="7" t="s">
+        <v>1245</v>
+      </c>
+      <c r="G262" s="7" t="s">
+        <v>1245</v>
+      </c>
+      <c r="H262" s="7" t="s">
         <v>1246</v>
       </c>
-      <c r="G262" s="7" t="s">
-        <v>1246</v>
-      </c>
-      <c r="H262" s="7" t="s">
-        <v>1247</v>
-      </c>
       <c r="I262" s="45" t="s">
-        <v>1239</v>
+        <v>1238</v>
       </c>
       <c r="J262" s="7" t="s">
         <v>979</v>
@@ -23581,25 +23581,25 @@
       </c>
       <c r="B263" s="7"/>
       <c r="C263" s="7" t="s">
-        <v>1335</v>
+        <v>1334</v>
       </c>
       <c r="D263" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="E263" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F263" s="7" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="G263" s="7" t="s">
-        <v>1327</v>
+        <v>1326</v>
       </c>
       <c r="H263" s="7" t="s">
+        <v>1277</v>
+      </c>
+      <c r="I263" s="6" t="s">
         <v>1278</v>
-      </c>
-      <c r="I263" s="6" t="s">
-        <v>1279</v>
       </c>
       <c r="J263" s="7" t="s">
         <v>979</v>
@@ -23608,7 +23608,7 @@
         <v>6</v>
       </c>
       <c r="L263" s="7" t="s">
-        <v>1339</v>
+        <v>1338</v>
       </c>
       <c r="M263" s="6" t="s">
         <v>8</v>
@@ -23652,22 +23652,22 @@
         <v>875</v>
       </c>
       <c r="D264" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="E264" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F264" s="40" t="s">
+        <v>1247</v>
+      </c>
+      <c r="G264" s="41" t="s">
         <v>1248</v>
       </c>
-      <c r="G264" s="41" t="s">
+      <c r="H264" s="40" t="s">
         <v>1249</v>
       </c>
-      <c r="H264" s="40" t="s">
+      <c r="I264" s="41" t="s">
         <v>1250</v>
-      </c>
-      <c r="I264" s="41" t="s">
-        <v>1251</v>
       </c>
       <c r="J264" s="40" t="s">
         <v>806</v>
@@ -23676,16 +23676,16 @@
         <v>231</v>
       </c>
       <c r="L264" s="40" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="M264" s="40" t="s">
         <v>8</v>
       </c>
       <c r="N264" s="41" t="s">
+        <v>1252</v>
+      </c>
+      <c r="O264" s="40" t="s">
         <v>1253</v>
-      </c>
-      <c r="O264" s="40" t="s">
-        <v>1254</v>
       </c>
       <c r="P264" s="40"/>
       <c r="Q264" s="40" t="s">
@@ -23726,22 +23726,22 @@
         <v>875</v>
       </c>
       <c r="D265" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="E265" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F265" s="41" t="s">
+        <v>1254</v>
+      </c>
+      <c r="G265" s="41" t="s">
+        <v>1254</v>
+      </c>
+      <c r="H265" s="47" t="s">
         <v>1255</v>
       </c>
-      <c r="G265" s="41" t="s">
-        <v>1255</v>
-      </c>
-      <c r="H265" s="47" t="s">
+      <c r="I265" s="41" t="s">
         <v>1256</v>
-      </c>
-      <c r="I265" s="41" t="s">
-        <v>1257</v>
       </c>
       <c r="J265" s="41" t="s">
         <v>1050</v>
@@ -23750,16 +23750,16 @@
         <v>231</v>
       </c>
       <c r="L265" s="40" t="s">
-        <v>1252</v>
+        <v>1251</v>
       </c>
       <c r="M265" s="40" t="s">
         <v>8</v>
       </c>
       <c r="N265" s="41" t="s">
+        <v>1257</v>
+      </c>
+      <c r="O265" s="40" t="s">
         <v>1258</v>
-      </c>
-      <c r="O265" s="40" t="s">
-        <v>1259</v>
       </c>
       <c r="P265" s="40"/>
       <c r="Q265" s="40" t="s">
@@ -23800,22 +23800,22 @@
         <v>875</v>
       </c>
       <c r="D266" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="E266" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F266" s="40" t="s">
+        <v>1259</v>
+      </c>
+      <c r="G266" s="41" t="s">
         <v>1260</v>
       </c>
-      <c r="G266" s="41" t="s">
+      <c r="H266" s="47" t="s">
         <v>1261</v>
       </c>
-      <c r="H266" s="47" t="s">
+      <c r="I266" s="41" t="s">
         <v>1262</v>
-      </c>
-      <c r="I266" s="41" t="s">
-        <v>1263</v>
       </c>
       <c r="J266" s="40" t="s">
         <v>806</v>
@@ -23830,10 +23830,10 @@
         <v>8</v>
       </c>
       <c r="N266" s="41" t="s">
+        <v>1263</v>
+      </c>
+      <c r="O266" s="40" t="s">
         <v>1264</v>
-      </c>
-      <c r="O266" s="40" t="s">
-        <v>1265</v>
       </c>
       <c r="P266" s="40"/>
       <c r="Q266" s="40" t="s">
@@ -23874,22 +23874,22 @@
         <v>875</v>
       </c>
       <c r="D267" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="E267" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F267" s="41" t="s">
+        <v>1265</v>
+      </c>
+      <c r="G267" s="41" t="s">
+        <v>1265</v>
+      </c>
+      <c r="H267" s="47" t="s">
         <v>1266</v>
       </c>
-      <c r="G267" s="41" t="s">
-        <v>1266</v>
-      </c>
-      <c r="H267" s="47" t="s">
+      <c r="I267" s="41" t="s">
         <v>1267</v>
-      </c>
-      <c r="I267" s="41" t="s">
-        <v>1268</v>
       </c>
       <c r="J267" s="40" t="s">
         <v>979</v>
@@ -23904,10 +23904,10 @@
         <v>8</v>
       </c>
       <c r="N267" s="40" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="O267" s="40" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="P267" s="40"/>
       <c r="Q267" s="40" t="s">
@@ -23948,22 +23948,22 @@
         <v>875</v>
       </c>
       <c r="D268" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="E268" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F268" s="40" t="s">
+        <v>1268</v>
+      </c>
+      <c r="G268" s="41" t="s">
         <v>1269</v>
       </c>
-      <c r="G268" s="41" t="s">
+      <c r="H268" s="47" t="s">
         <v>1270</v>
       </c>
-      <c r="H268" s="47" t="s">
+      <c r="I268" s="41" t="s">
         <v>1271</v>
-      </c>
-      <c r="I268" s="41" t="s">
-        <v>1272</v>
       </c>
       <c r="J268" s="40" t="s">
         <v>806</v>
@@ -23978,14 +23978,14 @@
         <v>8</v>
       </c>
       <c r="N268" s="41" t="s">
+        <v>1272</v>
+      </c>
+      <c r="O268" s="40" t="s">
         <v>1273</v>
-      </c>
-      <c r="O268" s="40" t="s">
-        <v>1274</v>
       </c>
       <c r="P268" s="40"/>
       <c r="Q268" s="40" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="R268" s="7">
         <v>0</v>
@@ -24022,22 +24022,22 @@
         <v>875</v>
       </c>
       <c r="D269" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="E269" s="40" t="s">
-        <v>1191</v>
+        <v>1190</v>
       </c>
       <c r="F269" s="41" t="s">
+        <v>1275</v>
+      </c>
+      <c r="G269" s="41" t="s">
+        <v>1275</v>
+      </c>
+      <c r="H269" s="47" t="s">
+        <v>1266</v>
+      </c>
+      <c r="I269" s="41" t="s">
         <v>1276</v>
-      </c>
-      <c r="G269" s="41" t="s">
-        <v>1276</v>
-      </c>
-      <c r="H269" s="47" t="s">
-        <v>1267</v>
-      </c>
-      <c r="I269" s="41" t="s">
-        <v>1277</v>
       </c>
       <c r="J269" s="40" t="s">
         <v>979</v>
@@ -24052,14 +24052,14 @@
         <v>8</v>
       </c>
       <c r="N269" s="40" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="O269" s="40" t="s">
-        <v>1265</v>
+        <v>1264</v>
       </c>
       <c r="P269" s="40"/>
       <c r="Q269" s="40" t="s">
-        <v>1275</v>
+        <v>1274</v>
       </c>
       <c r="R269" s="7">
         <v>0</v>
@@ -24129,7 +24129,7 @@
         <v>333</v>
       </c>
       <c r="B2" s="53" t="s">
-        <v>1336</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1">
@@ -24145,7 +24145,7 @@
         <v>732</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1331</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1">
@@ -24161,7 +24161,7 @@
         <v>336</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1334</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" customHeight="1">
@@ -24169,7 +24169,7 @@
         <v>337</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1333</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="17.25" customHeight="1">
@@ -24241,7 +24241,7 @@
         <v>346</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1337</v>
+        <v>1336</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="17.25" customHeight="1">
@@ -24294,10 +24294,10 @@
     </row>
     <row r="23" spans="1:2" ht="17.25" customHeight="1">
       <c r="A23" s="13" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>1332</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="17.25" customHeight="1">

</xml_diff>

<commit_message>
Act. trabajo 2020 y 2021
</commit_message>
<xml_diff>
--- a/Data/Base_fichas_indicadores.xlsx
+++ b/Data/Base_fichas_indicadores.xlsx
@@ -3404,12 +3404,6 @@
     <t>Porcentaje de personas ocupadas a tiempo completo que perciben ingresos por debajo de la línea de pobreza</t>
   </si>
   <si>
-    <t>El indicador mide el procentaje de personas ocupadas con al menos 40 horas de trabajo semanales que perciben ingresos por debajo de la línea de pobreza.</t>
-  </si>
-  <si>
-    <t>Para cada año calcular: (Cantidad de personas ocupadas con al menos 40 horas semanales con ingreso por debajo de la línea de pobreza / Cantidad de personas ocupadas con al menos 40 horas semanales) *100</t>
-  </si>
-  <si>
     <t>Percibir ingresos por debajo de la línea de pobreza</t>
   </si>
   <si>
@@ -4085,6 +4079,12 @@
   </si>
   <si>
     <t>Ingresos insuficientes (inferiores al salario mínimo nacional)</t>
+  </si>
+  <si>
+    <t>Para cada año calcular: ((Cantidad de personas ocupadas que trabajan más de 40 horas semanales con ingresos inferiores a la LP / Cantidad de personas ocupadas que trabajan más de 40 horas semanaless)) * 100</t>
+  </si>
+  <si>
+    <t>El indicador mide el porcentaje de ocupados que trabajan más de 40 horas semanales y perciben un salario inferior a la línea de pobreza individual.</t>
   </si>
 </sst>
 </file>
@@ -4201,7 +4201,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4341,6 +4341,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -4663,9 +4666,9 @@
   <dimension ref="A1:AK269"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A127" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A250" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E111" sqref="E111"/>
-      <selection pane="bottomLeft" activeCell="F153" sqref="F153"/>
+      <selection pane="bottomLeft" activeCell="C284" sqref="C284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4687,12 +4690,13 @@
     <col min="15" max="15" width="130.42578125" style="13" customWidth="1"/>
     <col min="16" max="16" width="230.140625" style="13" customWidth="1"/>
     <col min="17" max="17" width="98.7109375" style="13" customWidth="1"/>
-    <col min="18" max="18" width="19.140625" style="13" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="7" style="13" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="23" max="27" width="9.42578125" style="13" customWidth="1"/>
+    <col min="18" max="18" width="15.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="16.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="27" width="9.42578125" style="13" customWidth="1"/>
     <col min="28" max="30" width="9.140625" style="13"/>
     <col min="31" max="31" width="55.140625" style="13" customWidth="1"/>
     <col min="32" max="16384" width="9.140625" style="13"/>
@@ -4766,7 +4770,7 @@
         <v>675</v>
       </c>
       <c r="W1" s="13" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="2" spans="1:37" s="6" customFormat="1">
@@ -7156,10 +7160,10 @@
         <v>8</v>
       </c>
       <c r="N35" s="6" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="O35" s="6" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="P35" s="6" t="s">
         <v>23</v>
@@ -7339,7 +7343,7 @@
         <v>792</v>
       </c>
       <c r="G38" s="51" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="H38" s="6" t="s">
         <v>377</v>
@@ -7405,7 +7409,7 @@
         <v>795</v>
       </c>
       <c r="G39" s="51" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="H39" s="6" t="s">
         <v>722</v>
@@ -9205,10 +9209,10 @@
         <v>8</v>
       </c>
       <c r="N63" s="6" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="O63" s="6" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="P63" s="6" t="s">
         <v>54</v>
@@ -9258,7 +9262,7 @@
         <v>714</v>
       </c>
       <c r="I64" s="6" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
       <c r="J64" s="6" t="s">
         <v>5</v>
@@ -9273,10 +9277,10 @@
         <v>8</v>
       </c>
       <c r="N64" s="6" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="O64" s="6" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="P64" s="6" t="s">
         <v>54</v>
@@ -9342,10 +9346,10 @@
         <v>8</v>
       </c>
       <c r="N65" s="6" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="O65" s="6" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="P65" s="6" t="s">
         <v>54</v>
@@ -9410,10 +9414,10 @@
         <v>8</v>
       </c>
       <c r="N66" s="6" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="O66" s="6" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="P66" s="6" t="s">
         <v>54</v>
@@ -9478,10 +9482,10 @@
         <v>8</v>
       </c>
       <c r="N67" s="6" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="O67" s="6" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="P67" s="6" t="s">
         <v>54</v>
@@ -9547,10 +9551,10 @@
         <v>8</v>
       </c>
       <c r="N68" s="6" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="O68" s="6" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="P68" s="6" t="s">
         <v>54</v>
@@ -9611,16 +9615,16 @@
         <v>6</v>
       </c>
       <c r="L69" s="7" t="s">
-        <v>1279</v>
+        <v>1277</v>
       </c>
       <c r="M69" s="7" t="s">
         <v>8</v>
       </c>
       <c r="N69" s="6" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="O69" s="6" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="P69" s="7"/>
       <c r="Q69" s="7" t="s">
@@ -10248,7 +10252,7 @@
         <v>730</v>
       </c>
       <c r="I77" s="6" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
       <c r="J77" s="6" t="s">
         <v>5</v>
@@ -10332,10 +10336,10 @@
         <v>8</v>
       </c>
       <c r="N78" s="6" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="O78" s="6" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="P78" s="6" t="s">
         <v>61</v>
@@ -10401,10 +10405,10 @@
         <v>8</v>
       </c>
       <c r="N79" s="6" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="O79" s="6" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="P79" s="6" t="s">
         <v>61</v>
@@ -10470,10 +10474,10 @@
         <v>8</v>
       </c>
       <c r="N80" s="6" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="O80" s="6" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="P80" s="6" t="s">
         <v>61</v>
@@ -10539,10 +10543,10 @@
         <v>8</v>
       </c>
       <c r="N81" s="6" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="O81" s="6" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="P81" s="6" t="s">
         <v>61</v>
@@ -10608,10 +10612,10 @@
         <v>8</v>
       </c>
       <c r="N82" s="6" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="O82" s="6" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="P82" s="6" t="s">
         <v>61</v>
@@ -10677,10 +10681,10 @@
         <v>8</v>
       </c>
       <c r="N83" s="6" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="O83" s="6" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="P83" s="6" t="s">
         <v>61</v>
@@ -10747,10 +10751,10 @@
         <v>8</v>
       </c>
       <c r="N84" s="6" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="O84" s="6" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="P84" s="6" t="s">
         <v>61</v>
@@ -10829,10 +10833,10 @@
         <v>8</v>
       </c>
       <c r="N85" s="6" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="O85" s="6" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="P85" s="6" t="s">
         <v>61</v>
@@ -10910,10 +10914,10 @@
         <v>8</v>
       </c>
       <c r="N86" s="6" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="O86" s="6" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="P86" s="6" t="s">
         <v>61</v>
@@ -10980,10 +10984,10 @@
         <v>8</v>
       </c>
       <c r="N87" s="6" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="O87" s="6" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="P87" s="6" t="s">
         <v>61</v>
@@ -11061,10 +11065,10 @@
         <v>8</v>
       </c>
       <c r="N88" s="6" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="O88" s="6" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="P88" s="6" t="s">
         <v>61</v>
@@ -11130,10 +11134,10 @@
         <v>8</v>
       </c>
       <c r="N89" s="6" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="O89" s="6" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="P89" s="6" t="s">
         <v>61</v>
@@ -11200,10 +11204,10 @@
         <v>8</v>
       </c>
       <c r="N90" s="6" t="s">
-        <v>1339</v>
+        <v>1337</v>
       </c>
       <c r="O90" s="6" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="P90" s="6" t="s">
         <v>61</v>
@@ -15296,7 +15300,7 @@
         <v>1098</v>
       </c>
       <c r="H143" s="52" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="I143" s="6" t="s">
         <v>1099</v>
@@ -15494,7 +15498,7 @@
         <v>1104</v>
       </c>
       <c r="H146" s="7" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="I146" s="6" t="s">
         <v>1105</v>
@@ -15559,7 +15563,7 @@
         <v>1088</v>
       </c>
       <c r="H147" s="7" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="I147" s="6" t="s">
         <v>1089</v>
@@ -15624,7 +15628,7 @@
         <v>1090</v>
       </c>
       <c r="H148" s="7" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
       <c r="I148" s="6" t="s">
         <v>1091</v>
@@ -15692,7 +15696,7 @@
         <v>1092</v>
       </c>
       <c r="H149" s="7" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
       <c r="I149" s="6" t="s">
         <v>1093</v>
@@ -15757,7 +15761,7 @@
         <v>1094</v>
       </c>
       <c r="H150" s="7" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="I150" s="6" t="s">
         <v>1095</v>
@@ -15822,7 +15826,7 @@
         <v>1096</v>
       </c>
       <c r="H151" s="7" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="I151" s="6" t="s">
         <v>1097</v>
@@ -15867,7 +15871,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:23" s="7" customFormat="1">
+    <row r="152" spans="1:23" s="7" customFormat="1" ht="16.5" customHeight="1">
       <c r="A152" s="10">
         <v>530206</v>
       </c>
@@ -15887,7 +15891,7 @@
         <v>1106</v>
       </c>
       <c r="H152" s="7" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="I152" s="6" t="s">
         <v>1107</v>
@@ -15949,13 +15953,13 @@
         <v>15</v>
       </c>
       <c r="F153" s="7" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
       <c r="G153" s="7" t="s">
         <v>1109</v>
       </c>
       <c r="H153" s="7" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="I153" s="6" t="s">
         <v>1110</v>
@@ -16020,10 +16024,10 @@
         <v>1114</v>
       </c>
       <c r="G154" s="7" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="H154" s="7" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="I154" s="6" t="s">
         <v>1115</v>
@@ -16068,71 +16072,71 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:23" s="7" customFormat="1">
-      <c r="A155" s="10">
+    <row r="155" spans="1:23" s="54" customFormat="1">
+      <c r="A155" s="54">
         <v>530209</v>
       </c>
-      <c r="B155" s="7" t="s">
+      <c r="B155" s="44" t="s">
         <v>1000</v>
       </c>
-      <c r="D155" s="7" t="s">
+      <c r="D155" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="E155" s="7" t="s">
+      <c r="E155" s="54" t="s">
         <v>15</v>
       </c>
-      <c r="F155" s="7" t="s">
+      <c r="F155" s="54" t="s">
         <v>1116</v>
       </c>
-      <c r="G155" s="4" t="s">
+      <c r="G155" s="44" t="s">
         <v>1117</v>
       </c>
-      <c r="H155" s="7" t="s">
+      <c r="H155" s="44" t="s">
+        <v>1342</v>
+      </c>
+      <c r="I155" s="13" t="s">
+        <v>1341</v>
+      </c>
+      <c r="J155" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="K155" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="L155" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="M155" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="N155" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="O155" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="P155" s="6" t="s">
         <v>1118</v>
       </c>
-      <c r="I155" s="6" t="s">
-        <v>1119</v>
-      </c>
-      <c r="J155" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="K155" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="L155" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="M155" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="N155" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="O155" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="P155" s="6" t="s">
-        <v>1120</v>
-      </c>
-      <c r="Q155" s="7" t="s">
-        <v>475</v>
-      </c>
-      <c r="R155" s="44">
-        <v>0</v>
-      </c>
-      <c r="S155" s="44">
-        <v>0</v>
-      </c>
-      <c r="T155" s="44">
-        <v>0</v>
-      </c>
-      <c r="U155" s="44">
-        <v>0</v>
-      </c>
-      <c r="V155" s="44">
-        <v>0</v>
-      </c>
-      <c r="W155" s="6">
+      <c r="Q155" s="13" t="s">
+        <v>470</v>
+      </c>
+      <c r="R155" s="54">
+        <v>0</v>
+      </c>
+      <c r="S155" s="54">
+        <v>0</v>
+      </c>
+      <c r="T155" s="54">
+        <v>0</v>
+      </c>
+      <c r="U155" s="54">
+        <v>0</v>
+      </c>
+      <c r="V155" s="54">
+        <v>0</v>
+      </c>
+      <c r="W155" s="54">
         <v>0</v>
       </c>
     </row>
@@ -16150,16 +16154,16 @@
         <v>15</v>
       </c>
       <c r="F156" s="7" t="s">
+        <v>1119</v>
+      </c>
+      <c r="G156" s="7" t="s">
+        <v>1119</v>
+      </c>
+      <c r="H156" s="7" t="s">
+        <v>1120</v>
+      </c>
+      <c r="I156" s="7" t="s">
         <v>1121</v>
-      </c>
-      <c r="G156" s="7" t="s">
-        <v>1121</v>
-      </c>
-      <c r="H156" s="7" t="s">
-        <v>1122</v>
-      </c>
-      <c r="I156" s="7" t="s">
-        <v>1123</v>
       </c>
       <c r="J156" s="7" t="s">
         <v>5</v>
@@ -16168,16 +16172,16 @@
         <v>231</v>
       </c>
       <c r="L156" s="7" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="M156" s="7" t="s">
         <v>8</v>
       </c>
       <c r="N156" s="7" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="O156" s="7" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="Q156" s="7" t="s">
         <v>17</v>
@@ -16215,16 +16219,16 @@
         <v>15</v>
       </c>
       <c r="F157" s="7" t="s">
+        <v>1125</v>
+      </c>
+      <c r="G157" s="7" t="s">
+        <v>1125</v>
+      </c>
+      <c r="H157" s="7" t="s">
+        <v>1126</v>
+      </c>
+      <c r="I157" s="7" t="s">
         <v>1127</v>
-      </c>
-      <c r="G157" s="7" t="s">
-        <v>1127</v>
-      </c>
-      <c r="H157" s="7" t="s">
-        <v>1128</v>
-      </c>
-      <c r="I157" s="7" t="s">
-        <v>1129</v>
       </c>
       <c r="J157" s="7" t="s">
         <v>5</v>
@@ -16233,16 +16237,16 @@
         <v>231</v>
       </c>
       <c r="L157" s="7" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="M157" s="7" t="s">
         <v>8</v>
       </c>
       <c r="N157" s="7" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="O157" s="7" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="Q157" s="7" t="s">
         <v>17</v>
@@ -16280,19 +16284,19 @@
         <v>15</v>
       </c>
       <c r="F158" s="7" t="s">
+        <v>1131</v>
+      </c>
+      <c r="G158" s="7" t="s">
+        <v>1132</v>
+      </c>
+      <c r="H158" s="7" t="s">
         <v>1133</v>
       </c>
-      <c r="G158" s="7" t="s">
+      <c r="I158" s="7" t="s">
         <v>1134</v>
       </c>
-      <c r="H158" s="7" t="s">
+      <c r="J158" s="7" t="s">
         <v>1135</v>
-      </c>
-      <c r="I158" s="7" t="s">
-        <v>1136</v>
-      </c>
-      <c r="J158" s="7" t="s">
-        <v>1137</v>
       </c>
       <c r="K158" s="7" t="s">
         <v>231</v>
@@ -16346,16 +16350,16 @@
         <v>15</v>
       </c>
       <c r="F159" s="40" t="s">
+        <v>1136</v>
+      </c>
+      <c r="G159" s="40" t="s">
+        <v>1339</v>
+      </c>
+      <c r="H159" s="40" t="s">
+        <v>1137</v>
+      </c>
+      <c r="I159" s="40" t="s">
         <v>1138</v>
-      </c>
-      <c r="G159" s="40" t="s">
-        <v>1341</v>
-      </c>
-      <c r="H159" s="40" t="s">
-        <v>1139</v>
-      </c>
-      <c r="I159" s="40" t="s">
-        <v>1140</v>
       </c>
       <c r="J159" s="40" t="s">
         <v>5</v>
@@ -16364,20 +16368,20 @@
         <v>6</v>
       </c>
       <c r="L159" s="40" t="s">
+        <v>1139</v>
+      </c>
+      <c r="M159" s="44" t="s">
+        <v>1140</v>
+      </c>
+      <c r="N159" s="40" t="s">
         <v>1141</v>
       </c>
-      <c r="M159" s="44" t="s">
+      <c r="O159" s="40" t="s">
         <v>1142</v>
-      </c>
-      <c r="N159" s="40" t="s">
-        <v>1143</v>
-      </c>
-      <c r="O159" s="40" t="s">
-        <v>1144</v>
       </c>
       <c r="P159" s="40"/>
       <c r="Q159" s="40" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="R159" s="44">
         <v>0</v>
@@ -16412,10 +16416,10 @@
         <v>104</v>
       </c>
       <c r="F160" s="37" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="G160" s="3" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="H160" s="6" t="s">
         <v>790</v>
@@ -16478,10 +16482,10 @@
         <v>104</v>
       </c>
       <c r="F161" s="37" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="G161" s="3" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="H161" s="6" t="s">
         <v>793</v>
@@ -16544,10 +16548,10 @@
         <v>104</v>
       </c>
       <c r="F162" s="37" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="G162" s="3" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="H162" s="6" t="s">
         <v>796</v>
@@ -17261,10 +17265,10 @@
         <v>3</v>
       </c>
       <c r="F173" s="7" t="s">
+        <v>1278</v>
+      </c>
+      <c r="G173" s="7" t="s">
         <v>1280</v>
-      </c>
-      <c r="G173" s="7" t="s">
-        <v>1282</v>
       </c>
       <c r="H173" s="6" t="s">
         <v>798</v>
@@ -17329,10 +17333,10 @@
         <v>3</v>
       </c>
       <c r="F174" s="7" t="s">
+        <v>1279</v>
+      </c>
+      <c r="G174" s="7" t="s">
         <v>1281</v>
-      </c>
-      <c r="G174" s="7" t="s">
-        <v>1283</v>
       </c>
       <c r="H174" s="6" t="s">
         <v>378</v>
@@ -17397,10 +17401,10 @@
         <v>3</v>
       </c>
       <c r="F175" s="36" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="G175" s="6" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="H175" s="6" t="s">
         <v>419</v>
@@ -18697,19 +18701,19 @@
         <v>2</v>
       </c>
       <c r="E194" s="7" t="s">
+        <v>1144</v>
+      </c>
+      <c r="F194" s="6" t="s">
+        <v>1145</v>
+      </c>
+      <c r="G194" s="6" t="s">
         <v>1146</v>
       </c>
-      <c r="F194" s="6" t="s">
+      <c r="H194" s="7" t="s">
         <v>1147</v>
       </c>
-      <c r="G194" s="6" t="s">
+      <c r="I194" s="7" t="s">
         <v>1148</v>
-      </c>
-      <c r="H194" s="7" t="s">
-        <v>1149</v>
-      </c>
-      <c r="I194" s="7" t="s">
-        <v>1150</v>
       </c>
       <c r="J194" s="6" t="s">
         <v>5</v>
@@ -18765,19 +18769,19 @@
         <v>2</v>
       </c>
       <c r="E195" s="7" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="F195" s="6" t="s">
+        <v>1149</v>
+      </c>
+      <c r="G195" s="6" t="s">
+        <v>1150</v>
+      </c>
+      <c r="H195" s="7" t="s">
         <v>1151</v>
       </c>
-      <c r="G195" s="6" t="s">
+      <c r="I195" s="46" t="s">
         <v>1152</v>
-      </c>
-      <c r="H195" s="7" t="s">
-        <v>1153</v>
-      </c>
-      <c r="I195" s="46" t="s">
-        <v>1154</v>
       </c>
       <c r="J195" s="7" t="s">
         <v>979</v>
@@ -18833,19 +18837,19 @@
         <v>2</v>
       </c>
       <c r="E196" s="7" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="F196" s="6" t="s">
+        <v>1153</v>
+      </c>
+      <c r="G196" s="6" t="s">
+        <v>1153</v>
+      </c>
+      <c r="H196" s="7" t="s">
+        <v>1154</v>
+      </c>
+      <c r="I196" s="7" t="s">
         <v>1155</v>
-      </c>
-      <c r="G196" s="6" t="s">
-        <v>1155</v>
-      </c>
-      <c r="H196" s="7" t="s">
-        <v>1156</v>
-      </c>
-      <c r="I196" s="7" t="s">
-        <v>1157</v>
       </c>
       <c r="J196" s="7" t="s">
         <v>806</v>
@@ -18866,7 +18870,7 @@
         <v>909</v>
       </c>
       <c r="Q196" s="7" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="R196" s="44">
         <v>0</v>
@@ -19395,7 +19399,7 @@
         <v>912</v>
       </c>
       <c r="G204" s="7" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="H204" s="7" t="s">
         <v>913</v>
@@ -19464,7 +19468,7 @@
         <v>919</v>
       </c>
       <c r="G205" s="7" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="H205" s="7" t="s">
         <v>920</v>
@@ -19533,7 +19537,7 @@
         <v>922</v>
       </c>
       <c r="G206" s="7" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
       <c r="H206" s="7" t="s">
         <v>923</v>
@@ -19602,7 +19606,7 @@
         <v>925</v>
       </c>
       <c r="G207" s="7" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
       <c r="H207" s="7" t="s">
         <v>926</v>
@@ -19742,10 +19746,10 @@
         <v>3</v>
       </c>
       <c r="F209" s="7" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="G209" s="7" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="H209" s="7" t="s">
         <v>1048</v>
@@ -19810,10 +19814,10 @@
         <v>3</v>
       </c>
       <c r="F210" s="7" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="G210" s="7" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="H210" s="7" t="s">
         <v>1051</v>
@@ -19878,10 +19882,10 @@
         <v>3</v>
       </c>
       <c r="F211" s="7" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="G211" s="7" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="H211" s="7" t="s">
         <v>1053</v>
@@ -19946,10 +19950,10 @@
         <v>3</v>
       </c>
       <c r="F212" s="7" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="G212" s="7" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="H212" s="7" t="s">
         <v>1055</v>
@@ -20014,10 +20018,10 @@
         <v>3</v>
       </c>
       <c r="F213" s="7" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="G213" s="7" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="H213" s="7" t="s">
         <v>1057</v>
@@ -20082,10 +20086,10 @@
         <v>3</v>
       </c>
       <c r="F214" s="7" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="G214" s="7" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="H214" s="7" t="s">
         <v>1059</v>
@@ -20150,10 +20154,10 @@
         <v>3</v>
       </c>
       <c r="F215" s="7" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
       <c r="G215" s="7" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
       <c r="H215" s="7" t="s">
         <v>1061</v>
@@ -20218,10 +20222,10 @@
         <v>3</v>
       </c>
       <c r="F216" s="7" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="G216" s="7" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="H216" s="7" t="s">
         <v>1063</v>
@@ -20286,10 +20290,10 @@
         <v>3</v>
       </c>
       <c r="F217" s="7" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="G217" s="7" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="H217" s="7" t="s">
         <v>1065</v>
@@ -20345,7 +20349,7 @@
         <v>1</v>
       </c>
       <c r="C218" s="7" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="D218" s="7" t="s">
         <v>2</v>
@@ -20372,7 +20376,7 @@
         <v>6</v>
       </c>
       <c r="L218" s="7" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="M218" s="7" t="s">
         <v>940</v>
@@ -20417,7 +20421,7 @@
         <v>1</v>
       </c>
       <c r="C219" s="7" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="D219" s="7" t="s">
         <v>2</v>
@@ -20444,7 +20448,7 @@
         <v>6</v>
       </c>
       <c r="L219" s="7" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="M219" s="7" t="s">
         <v>940</v>
@@ -20489,7 +20493,7 @@
         <v>35</v>
       </c>
       <c r="C220" s="7" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="D220" s="7" t="s">
         <v>2</v>
@@ -20498,16 +20502,16 @@
         <v>36</v>
       </c>
       <c r="F220" s="7" t="s">
+        <v>1163</v>
+      </c>
+      <c r="G220" s="7" t="s">
+        <v>1164</v>
+      </c>
+      <c r="H220" s="6" t="s">
         <v>1165</v>
       </c>
-      <c r="G220" s="7" t="s">
+      <c r="I220" s="6" t="s">
         <v>1166</v>
-      </c>
-      <c r="H220" s="6" t="s">
-        <v>1167</v>
-      </c>
-      <c r="I220" s="6" t="s">
-        <v>1168</v>
       </c>
       <c r="J220" s="6" t="s">
         <v>5</v>
@@ -20516,7 +20520,7 @@
         <v>6</v>
       </c>
       <c r="L220" s="7" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="M220" s="7" t="s">
         <v>940</v>
@@ -20560,7 +20564,7 @@
         <v>35</v>
       </c>
       <c r="C221" s="7" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="D221" s="7" t="s">
         <v>2</v>
@@ -20569,16 +20573,16 @@
         <v>41</v>
       </c>
       <c r="F221" s="7" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="G221" s="7" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="H221" s="6" t="s">
         <v>419</v>
       </c>
       <c r="I221" s="6" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="J221" s="6" t="s">
         <v>5</v>
@@ -20587,7 +20591,7 @@
         <v>6</v>
       </c>
       <c r="L221" s="7" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="M221" s="7" t="s">
         <v>940</v>
@@ -20631,7 +20635,7 @@
         <v>35</v>
       </c>
       <c r="C222" s="7" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="D222" s="7" t="s">
         <v>2</v>
@@ -20640,16 +20644,16 @@
         <v>41</v>
       </c>
       <c r="F222" s="7" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="G222" s="7" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="H222" s="6" t="s">
         <v>378</v>
       </c>
       <c r="I222" s="6" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="J222" s="6" t="s">
         <v>5</v>
@@ -20658,7 +20662,7 @@
         <v>6</v>
       </c>
       <c r="L222" s="7" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="M222" s="7" t="s">
         <v>940</v>
@@ -20702,7 +20706,7 @@
         <v>35</v>
       </c>
       <c r="C223" s="7" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="D223" s="7" t="s">
         <v>2</v>
@@ -20711,16 +20715,16 @@
         <v>41</v>
       </c>
       <c r="F223" s="7" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="G223" s="7" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="H223" s="6" t="s">
         <v>304</v>
       </c>
       <c r="I223" s="6" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="J223" s="6" t="s">
         <v>5</v>
@@ -20729,7 +20733,7 @@
         <v>6</v>
       </c>
       <c r="L223" s="7" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="M223" s="7" t="s">
         <v>940</v>
@@ -20773,7 +20777,7 @@
         <v>35</v>
       </c>
       <c r="C224" s="7" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="D224" s="7" t="s">
         <v>2</v>
@@ -20782,16 +20786,16 @@
         <v>41</v>
       </c>
       <c r="F224" s="7" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="G224" s="7" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="H224" s="6" t="s">
         <v>420</v>
       </c>
       <c r="I224" s="6" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="J224" s="6" t="s">
         <v>5</v>
@@ -20800,7 +20804,7 @@
         <v>6</v>
       </c>
       <c r="L224" s="7" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="M224" s="7" t="s">
         <v>940</v>
@@ -20850,7 +20854,7 @@
         <v>35</v>
       </c>
       <c r="C225" s="7" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="D225" s="7" t="s">
         <v>2</v>
@@ -20859,16 +20863,16 @@
         <v>46</v>
       </c>
       <c r="F225" s="7" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="G225" s="7" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="H225" s="6" t="s">
         <v>421</v>
       </c>
       <c r="I225" s="27" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="J225" s="6" t="s">
         <v>5</v>
@@ -20877,7 +20881,7 @@
         <v>6</v>
       </c>
       <c r="L225" s="7" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="M225" s="7" t="s">
         <v>940</v>
@@ -20927,7 +20931,7 @@
         <v>35</v>
       </c>
       <c r="C226" s="7" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="D226" s="7" t="s">
         <v>2</v>
@@ -20936,16 +20940,16 @@
         <v>47</v>
       </c>
       <c r="F226" s="6" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="G226" s="7" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="H226" s="6" t="s">
         <v>641</v>
       </c>
       <c r="I226" s="27" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="J226" s="6" t="s">
         <v>5</v>
@@ -20954,7 +20958,7 @@
         <v>6</v>
       </c>
       <c r="L226" s="7" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="M226" s="7" t="s">
         <v>940</v>
@@ -21004,7 +21008,7 @@
         <v>35</v>
       </c>
       <c r="C227" s="7" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="D227" s="7" t="s">
         <v>2</v>
@@ -21013,16 +21017,16 @@
         <v>47</v>
       </c>
       <c r="F227" s="7" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="G227" s="7" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="H227" s="6" t="s">
         <v>379</v>
       </c>
       <c r="I227" s="6" t="s">
-        <v>1189</v>
+        <v>1187</v>
       </c>
       <c r="J227" s="6" t="s">
         <v>5</v>
@@ -21031,7 +21035,7 @@
         <v>6</v>
       </c>
       <c r="L227" s="7" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="M227" s="7" t="s">
         <v>940</v>
@@ -21081,7 +21085,7 @@
         <v>52</v>
       </c>
       <c r="C228" s="7" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="D228" s="7" t="s">
         <v>2</v>
@@ -21108,7 +21112,7 @@
         <v>6</v>
       </c>
       <c r="L228" s="7" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="M228" s="7" t="s">
         <v>940</v>
@@ -21155,7 +21159,7 @@
         <v>52</v>
       </c>
       <c r="C229" s="7" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="D229" s="7" t="s">
         <v>2</v>
@@ -21167,13 +21171,13 @@
         <v>996</v>
       </c>
       <c r="G229" s="7" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="H229" s="6" t="s">
         <v>714</v>
       </c>
       <c r="I229" s="6" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
       <c r="J229" s="6" t="s">
         <v>5</v>
@@ -21182,7 +21186,7 @@
         <v>6</v>
       </c>
       <c r="L229" s="7" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="M229" s="7" t="s">
         <v>940</v>
@@ -21232,7 +21236,7 @@
         <v>52</v>
       </c>
       <c r="C230" s="7" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="D230" s="7" t="s">
         <v>2</v>
@@ -21244,7 +21248,7 @@
         <v>997</v>
       </c>
       <c r="G230" s="7" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
       <c r="H230" s="6" t="s">
         <v>384</v>
@@ -21259,7 +21263,7 @@
         <v>6</v>
       </c>
       <c r="L230" s="7" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="M230" s="7" t="s">
         <v>940</v>
@@ -21309,7 +21313,7 @@
         <v>52</v>
       </c>
       <c r="C231" s="7" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="D231" s="7" t="s">
         <v>2</v>
@@ -21321,13 +21325,13 @@
         <v>999</v>
       </c>
       <c r="G231" s="7" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
       <c r="H231" s="6" t="s">
         <v>714</v>
       </c>
       <c r="I231" s="6" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
       <c r="J231" s="6" t="s">
         <v>5</v>
@@ -21336,7 +21340,7 @@
         <v>6</v>
       </c>
       <c r="L231" s="7" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="M231" s="7" t="s">
         <v>940</v>
@@ -21386,7 +21390,7 @@
         <v>70</v>
       </c>
       <c r="C232" s="7" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="D232" s="7" t="s">
         <v>2</v>
@@ -21413,7 +21417,7 @@
         <v>6</v>
       </c>
       <c r="L232" s="7" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="M232" s="7" t="s">
         <v>940</v>
@@ -21463,7 +21467,7 @@
         <v>1000</v>
       </c>
       <c r="C233" s="7" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="D233" s="7" t="s">
         <v>2</v>
@@ -21478,7 +21482,7 @@
         <v>1074</v>
       </c>
       <c r="H233" s="7" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="I233" s="6" t="s">
         <v>1075</v>
@@ -21490,7 +21494,7 @@
         <v>6</v>
       </c>
       <c r="L233" s="7" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="M233" s="7" t="s">
         <v>940</v>
@@ -21531,7 +21535,7 @@
         <v>1000</v>
       </c>
       <c r="C234" s="7" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="D234" s="7" t="s">
         <v>2</v>
@@ -21546,7 +21550,7 @@
         <v>1076</v>
       </c>
       <c r="H234" s="7" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="I234" s="6" t="s">
         <v>1078</v>
@@ -21558,7 +21562,7 @@
         <v>6</v>
       </c>
       <c r="L234" s="7" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="M234" s="7" t="s">
         <v>940</v>
@@ -21599,7 +21603,7 @@
         <v>1000</v>
       </c>
       <c r="C235" s="7" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="D235" s="7" t="s">
         <v>2</v>
@@ -21626,7 +21630,7 @@
         <v>6</v>
       </c>
       <c r="L235" s="7" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="M235" s="7" t="s">
         <v>940</v>
@@ -21667,7 +21671,7 @@
         <v>1000</v>
       </c>
       <c r="C236" s="7" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="D236" s="7" t="s">
         <v>2</v>
@@ -21682,7 +21686,7 @@
         <v>1081</v>
       </c>
       <c r="H236" s="7" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="I236" s="6" t="s">
         <v>1082</v>
@@ -21694,7 +21698,7 @@
         <v>6</v>
       </c>
       <c r="L236" s="7" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="M236" s="7" t="s">
         <v>940</v>
@@ -21735,7 +21739,7 @@
         <v>1000</v>
       </c>
       <c r="C237" s="7" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="D237" s="7" t="s">
         <v>2</v>
@@ -21750,7 +21754,7 @@
         <v>1083</v>
       </c>
       <c r="H237" s="7" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="I237" s="6" t="s">
         <v>1084</v>
@@ -21762,7 +21766,7 @@
         <v>6</v>
       </c>
       <c r="L237" s="7" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="M237" s="7" t="s">
         <v>940</v>
@@ -21803,7 +21807,7 @@
         <v>1000</v>
       </c>
       <c r="C238" s="7" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="D238" s="7" t="s">
         <v>2</v>
@@ -21815,10 +21819,10 @@
         <v>1085</v>
       </c>
       <c r="G238" s="7" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
       <c r="H238" s="6" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="I238" s="6" t="s">
         <v>1086</v>
@@ -21830,7 +21834,7 @@
         <v>6</v>
       </c>
       <c r="L238" s="7" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="M238" s="7" t="s">
         <v>940</v>
@@ -22090,16 +22094,16 @@
         <v>47</v>
       </c>
       <c r="F242" s="41" t="s">
+        <v>1157</v>
+      </c>
+      <c r="G242" s="41" t="s">
+        <v>1158</v>
+      </c>
+      <c r="H242" s="40" t="s">
         <v>1159</v>
       </c>
-      <c r="G242" s="41" t="s">
+      <c r="I242" s="41" t="s">
         <v>1160</v>
-      </c>
-      <c r="H242" s="40" t="s">
-        <v>1161</v>
-      </c>
-      <c r="I242" s="41" t="s">
-        <v>1162</v>
       </c>
       <c r="J242" s="40" t="s">
         <v>5</v>
@@ -22114,10 +22118,10 @@
         <v>8</v>
       </c>
       <c r="N242" s="41" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="O242" s="40" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="P242" s="40"/>
       <c r="Q242" s="40" t="s">
@@ -22386,7 +22390,7 @@
         <v>1072</v>
       </c>
       <c r="H246" s="42" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="I246" s="42" t="s">
         <v>1073</v>
@@ -22441,25 +22445,25 @@
         <v>884</v>
       </c>
       <c r="D247" s="40" t="s">
+        <v>1188</v>
+      </c>
+      <c r="E247" s="40" t="s">
+        <v>1188</v>
+      </c>
+      <c r="F247" s="7" t="s">
+        <v>1189</v>
+      </c>
+      <c r="G247" s="6" t="s">
+        <v>1189</v>
+      </c>
+      <c r="H247" s="6" t="s">
         <v>1190</v>
       </c>
-      <c r="E247" s="40" t="s">
-        <v>1190</v>
-      </c>
-      <c r="F247" s="7" t="s">
+      <c r="I247" s="6" t="s">
         <v>1191</v>
       </c>
-      <c r="G247" s="6" t="s">
-        <v>1191</v>
-      </c>
-      <c r="H247" s="6" t="s">
+      <c r="J247" s="6" t="s">
         <v>1192</v>
-      </c>
-      <c r="I247" s="6" t="s">
-        <v>1193</v>
-      </c>
-      <c r="J247" s="6" t="s">
-        <v>1194</v>
       </c>
       <c r="K247" s="6" t="s">
         <v>6</v>
@@ -22508,22 +22512,22 @@
         <v>911</v>
       </c>
       <c r="D248" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="E248" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="F248" s="7" t="s">
+        <v>1193</v>
+      </c>
+      <c r="G248" s="7" t="s">
+        <v>1194</v>
+      </c>
+      <c r="H248" s="7" t="s">
         <v>1195</v>
       </c>
-      <c r="G248" s="7" t="s">
+      <c r="I248" s="7" t="s">
         <v>1196</v>
-      </c>
-      <c r="H248" s="7" t="s">
-        <v>1197</v>
-      </c>
-      <c r="I248" s="7" t="s">
-        <v>1198</v>
       </c>
       <c r="J248" s="7" t="s">
         <v>5</v>
@@ -22544,7 +22548,7 @@
         <v>917</v>
       </c>
       <c r="Q248" s="7" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="R248" s="7">
         <v>0</v>
@@ -22574,22 +22578,22 @@
         <v>911</v>
       </c>
       <c r="D249" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="E249" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="F249" s="7" t="s">
+        <v>1198</v>
+      </c>
+      <c r="G249" s="7" t="s">
+        <v>1199</v>
+      </c>
+      <c r="H249" s="7" t="s">
         <v>1200</v>
       </c>
-      <c r="G249" s="7" t="s">
+      <c r="I249" s="7" t="s">
         <v>1201</v>
-      </c>
-      <c r="H249" s="7" t="s">
-        <v>1202</v>
-      </c>
-      <c r="I249" s="7" t="s">
-        <v>1203</v>
       </c>
       <c r="J249" s="7" t="s">
         <v>5</v>
@@ -22610,7 +22614,7 @@
         <v>917</v>
       </c>
       <c r="Q249" s="7" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="R249" s="7">
         <v>0</v>
@@ -22640,22 +22644,22 @@
         <v>911</v>
       </c>
       <c r="D250" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="E250" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="F250" s="7" t="s">
+        <v>1202</v>
+      </c>
+      <c r="G250" s="7" t="s">
+        <v>1203</v>
+      </c>
+      <c r="H250" s="7" t="s">
         <v>1204</v>
       </c>
-      <c r="G250" s="7" t="s">
+      <c r="I250" s="7" t="s">
         <v>1205</v>
-      </c>
-      <c r="H250" s="7" t="s">
-        <v>1206</v>
-      </c>
-      <c r="I250" s="7" t="s">
-        <v>1207</v>
       </c>
       <c r="J250" s="7" t="s">
         <v>5</v>
@@ -22676,7 +22680,7 @@
         <v>917</v>
       </c>
       <c r="Q250" s="7" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="R250" s="7">
         <v>0</v>
@@ -22706,22 +22710,22 @@
         <v>911</v>
       </c>
       <c r="D251" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="E251" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="F251" s="7" t="s">
+        <v>1206</v>
+      </c>
+      <c r="G251" s="7" t="s">
+        <v>1207</v>
+      </c>
+      <c r="H251" s="7" t="s">
         <v>1208</v>
       </c>
-      <c r="G251" s="7" t="s">
+      <c r="I251" s="7" t="s">
         <v>1209</v>
-      </c>
-      <c r="H251" s="7" t="s">
-        <v>1210</v>
-      </c>
-      <c r="I251" s="7" t="s">
-        <v>1211</v>
       </c>
       <c r="J251" s="7" t="s">
         <v>5</v>
@@ -22742,7 +22746,7 @@
         <v>917</v>
       </c>
       <c r="Q251" s="7" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="R251" s="7">
         <v>0</v>
@@ -22773,22 +22777,22 @@
         <v>911</v>
       </c>
       <c r="D252" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="E252" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="F252" s="7" t="s">
+        <v>1210</v>
+      </c>
+      <c r="G252" s="7" t="s">
+        <v>1211</v>
+      </c>
+      <c r="H252" s="7" t="s">
         <v>1212</v>
       </c>
-      <c r="G252" s="7" t="s">
+      <c r="I252" s="7" t="s">
         <v>1213</v>
-      </c>
-      <c r="H252" s="7" t="s">
-        <v>1214</v>
-      </c>
-      <c r="I252" s="7" t="s">
-        <v>1215</v>
       </c>
       <c r="J252" s="7" t="s">
         <v>5</v>
@@ -22810,7 +22814,7 @@
       </c>
       <c r="P252" s="7"/>
       <c r="Q252" s="7" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="R252" s="7">
         <v>0</v>
@@ -22845,22 +22849,22 @@
         <v>911</v>
       </c>
       <c r="D253" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="E253" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="F253" s="7" t="s">
+        <v>1214</v>
+      </c>
+      <c r="G253" s="7" t="s">
+        <v>1215</v>
+      </c>
+      <c r="H253" s="7" t="s">
         <v>1216</v>
       </c>
-      <c r="G253" s="7" t="s">
+      <c r="I253" s="7" t="s">
         <v>1217</v>
-      </c>
-      <c r="H253" s="7" t="s">
-        <v>1218</v>
-      </c>
-      <c r="I253" s="7" t="s">
-        <v>1219</v>
       </c>
       <c r="J253" s="7" t="s">
         <v>5</v>
@@ -22881,7 +22885,7 @@
         <v>917</v>
       </c>
       <c r="Q253" s="7" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="R253" s="7">
         <v>0</v>
@@ -22918,22 +22922,22 @@
         <v>911</v>
       </c>
       <c r="D254" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="E254" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="F254" s="7" t="s">
+        <v>1218</v>
+      </c>
+      <c r="G254" s="7" t="s">
+        <v>1219</v>
+      </c>
+      <c r="H254" s="7" t="s">
         <v>1220</v>
       </c>
-      <c r="G254" s="7" t="s">
+      <c r="I254" s="7" t="s">
         <v>1221</v>
-      </c>
-      <c r="H254" s="7" t="s">
-        <v>1222</v>
-      </c>
-      <c r="I254" s="7" t="s">
-        <v>1223</v>
       </c>
       <c r="J254" s="7" t="s">
         <v>5</v>
@@ -22954,7 +22958,7 @@
         <v>917</v>
       </c>
       <c r="Q254" s="7" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="R254" s="7">
         <v>0</v>
@@ -22992,22 +22996,22 @@
         <v>911</v>
       </c>
       <c r="D255" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="E255" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="F255" s="7" t="s">
+        <v>1222</v>
+      </c>
+      <c r="G255" s="7" t="s">
+        <v>1223</v>
+      </c>
+      <c r="H255" s="7" t="s">
         <v>1224</v>
       </c>
-      <c r="G255" s="7" t="s">
+      <c r="I255" s="7" t="s">
         <v>1225</v>
-      </c>
-      <c r="H255" s="7" t="s">
-        <v>1226</v>
-      </c>
-      <c r="I255" s="7" t="s">
-        <v>1227</v>
       </c>
       <c r="J255" s="7" t="s">
         <v>5</v>
@@ -23029,7 +23033,7 @@
       </c>
       <c r="P255" s="7"/>
       <c r="Q255" s="7" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="R255" s="7">
         <v>0</v>
@@ -23066,22 +23070,22 @@
         <v>911</v>
       </c>
       <c r="D256" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="E256" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="F256" s="7" t="s">
+        <v>1226</v>
+      </c>
+      <c r="G256" s="7" t="s">
+        <v>1227</v>
+      </c>
+      <c r="H256" s="7" t="s">
         <v>1228</v>
       </c>
-      <c r="G256" s="7" t="s">
+      <c r="I256" s="7" t="s">
         <v>1229</v>
-      </c>
-      <c r="H256" s="7" t="s">
-        <v>1230</v>
-      </c>
-      <c r="I256" s="7" t="s">
-        <v>1231</v>
       </c>
       <c r="J256" s="7" t="s">
         <v>5</v>
@@ -23103,7 +23107,7 @@
       </c>
       <c r="P256" s="7"/>
       <c r="Q256" s="7" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="R256" s="7">
         <v>0</v>
@@ -23140,22 +23144,22 @@
         <v>911</v>
       </c>
       <c r="D257" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="E257" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="F257" s="7" t="s">
+        <v>1230</v>
+      </c>
+      <c r="G257" s="7" t="s">
+        <v>1231</v>
+      </c>
+      <c r="H257" s="7" t="s">
         <v>1232</v>
       </c>
-      <c r="G257" s="7" t="s">
+      <c r="I257" s="7" t="s">
         <v>1233</v>
-      </c>
-      <c r="H257" s="7" t="s">
-        <v>1234</v>
-      </c>
-      <c r="I257" s="7" t="s">
-        <v>1235</v>
       </c>
       <c r="J257" s="7" t="s">
         <v>5</v>
@@ -23177,7 +23181,7 @@
       </c>
       <c r="P257" s="7"/>
       <c r="Q257" s="7" t="s">
-        <v>1199</v>
+        <v>1197</v>
       </c>
       <c r="R257" s="7">
         <v>0</v>
@@ -23214,22 +23218,22 @@
         <v>911</v>
       </c>
       <c r="D258" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="E258" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="F258" s="7" t="s">
+        <v>1234</v>
+      </c>
+      <c r="G258" s="7" t="s">
+        <v>1234</v>
+      </c>
+      <c r="H258" s="7" t="s">
+        <v>1235</v>
+      </c>
+      <c r="I258" s="45" t="s">
         <v>1236</v>
-      </c>
-      <c r="G258" s="7" t="s">
-        <v>1236</v>
-      </c>
-      <c r="H258" s="7" t="s">
-        <v>1237</v>
-      </c>
-      <c r="I258" s="45" t="s">
-        <v>1238</v>
       </c>
       <c r="J258" s="7" t="s">
         <v>979</v>
@@ -23288,22 +23292,22 @@
         <v>911</v>
       </c>
       <c r="D259" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="E259" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="F259" s="7" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="G259" s="7" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="H259" s="7" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="I259" s="45" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="J259" s="7" t="s">
         <v>979</v>
@@ -23362,22 +23366,22 @@
         <v>911</v>
       </c>
       <c r="D260" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="E260" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="F260" s="7" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="G260" s="7" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="H260" s="7" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="I260" s="45" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="J260" s="7" t="s">
         <v>979</v>
@@ -23436,22 +23440,22 @@
         <v>911</v>
       </c>
       <c r="D261" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="E261" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="F261" s="7" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="G261" s="7" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="H261" s="7" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="I261" s="45" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="J261" s="7" t="s">
         <v>979</v>
@@ -23510,22 +23514,22 @@
         <v>911</v>
       </c>
       <c r="D262" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="E262" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="F262" s="7" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="G262" s="7" t="s">
-        <v>1245</v>
+        <v>1243</v>
       </c>
       <c r="H262" s="7" t="s">
-        <v>1246</v>
+        <v>1244</v>
       </c>
       <c r="I262" s="45" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="J262" s="7" t="s">
         <v>979</v>
@@ -23581,25 +23585,25 @@
       </c>
       <c r="B263" s="7"/>
       <c r="C263" s="7" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
       <c r="D263" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="E263" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="F263" s="7" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="G263" s="7" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="H263" s="7" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="I263" s="6" t="s">
-        <v>1278</v>
+        <v>1276</v>
       </c>
       <c r="J263" s="7" t="s">
         <v>979</v>
@@ -23608,7 +23612,7 @@
         <v>6</v>
       </c>
       <c r="L263" s="7" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="M263" s="6" t="s">
         <v>8</v>
@@ -23652,22 +23656,22 @@
         <v>875</v>
       </c>
       <c r="D264" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="E264" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="F264" s="40" t="s">
+        <v>1245</v>
+      </c>
+      <c r="G264" s="41" t="s">
+        <v>1246</v>
+      </c>
+      <c r="H264" s="40" t="s">
         <v>1247</v>
       </c>
-      <c r="G264" s="41" t="s">
+      <c r="I264" s="41" t="s">
         <v>1248</v>
-      </c>
-      <c r="H264" s="40" t="s">
-        <v>1249</v>
-      </c>
-      <c r="I264" s="41" t="s">
-        <v>1250</v>
       </c>
       <c r="J264" s="40" t="s">
         <v>806</v>
@@ -23676,16 +23680,16 @@
         <v>231</v>
       </c>
       <c r="L264" s="40" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="M264" s="40" t="s">
         <v>8</v>
       </c>
       <c r="N264" s="41" t="s">
-        <v>1252</v>
+        <v>1250</v>
       </c>
       <c r="O264" s="40" t="s">
-        <v>1253</v>
+        <v>1251</v>
       </c>
       <c r="P264" s="40"/>
       <c r="Q264" s="40" t="s">
@@ -23726,22 +23730,22 @@
         <v>875</v>
       </c>
       <c r="D265" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="E265" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="F265" s="41" t="s">
+        <v>1252</v>
+      </c>
+      <c r="G265" s="41" t="s">
+        <v>1252</v>
+      </c>
+      <c r="H265" s="47" t="s">
+        <v>1253</v>
+      </c>
+      <c r="I265" s="41" t="s">
         <v>1254</v>
-      </c>
-      <c r="G265" s="41" t="s">
-        <v>1254</v>
-      </c>
-      <c r="H265" s="47" t="s">
-        <v>1255</v>
-      </c>
-      <c r="I265" s="41" t="s">
-        <v>1256</v>
       </c>
       <c r="J265" s="41" t="s">
         <v>1050</v>
@@ -23750,16 +23754,16 @@
         <v>231</v>
       </c>
       <c r="L265" s="40" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="M265" s="40" t="s">
         <v>8</v>
       </c>
       <c r="N265" s="41" t="s">
-        <v>1257</v>
+        <v>1255</v>
       </c>
       <c r="O265" s="40" t="s">
-        <v>1258</v>
+        <v>1256</v>
       </c>
       <c r="P265" s="40"/>
       <c r="Q265" s="40" t="s">
@@ -23800,22 +23804,22 @@
         <v>875</v>
       </c>
       <c r="D266" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="E266" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="F266" s="40" t="s">
+        <v>1257</v>
+      </c>
+      <c r="G266" s="41" t="s">
+        <v>1258</v>
+      </c>
+      <c r="H266" s="47" t="s">
         <v>1259</v>
       </c>
-      <c r="G266" s="41" t="s">
+      <c r="I266" s="41" t="s">
         <v>1260</v>
-      </c>
-      <c r="H266" s="47" t="s">
-        <v>1261</v>
-      </c>
-      <c r="I266" s="41" t="s">
-        <v>1262</v>
       </c>
       <c r="J266" s="40" t="s">
         <v>806</v>
@@ -23830,10 +23834,10 @@
         <v>8</v>
       </c>
       <c r="N266" s="41" t="s">
-        <v>1263</v>
+        <v>1261</v>
       </c>
       <c r="O266" s="40" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="P266" s="40"/>
       <c r="Q266" s="40" t="s">
@@ -23874,22 +23878,22 @@
         <v>875</v>
       </c>
       <c r="D267" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="E267" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="F267" s="41" t="s">
+        <v>1263</v>
+      </c>
+      <c r="G267" s="41" t="s">
+        <v>1263</v>
+      </c>
+      <c r="H267" s="47" t="s">
+        <v>1264</v>
+      </c>
+      <c r="I267" s="41" t="s">
         <v>1265</v>
-      </c>
-      <c r="G267" s="41" t="s">
-        <v>1265</v>
-      </c>
-      <c r="H267" s="47" t="s">
-        <v>1266</v>
-      </c>
-      <c r="I267" s="41" t="s">
-        <v>1267</v>
       </c>
       <c r="J267" s="40" t="s">
         <v>979</v>
@@ -23904,10 +23908,10 @@
         <v>8</v>
       </c>
       <c r="N267" s="40" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="O267" s="40" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="P267" s="40"/>
       <c r="Q267" s="40" t="s">
@@ -23948,22 +23952,22 @@
         <v>875</v>
       </c>
       <c r="D268" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="E268" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="F268" s="40" t="s">
+        <v>1266</v>
+      </c>
+      <c r="G268" s="41" t="s">
+        <v>1267</v>
+      </c>
+      <c r="H268" s="47" t="s">
         <v>1268</v>
       </c>
-      <c r="G268" s="41" t="s">
+      <c r="I268" s="41" t="s">
         <v>1269</v>
-      </c>
-      <c r="H268" s="47" t="s">
-        <v>1270</v>
-      </c>
-      <c r="I268" s="41" t="s">
-        <v>1271</v>
       </c>
       <c r="J268" s="40" t="s">
         <v>806</v>
@@ -23978,14 +23982,14 @@
         <v>8</v>
       </c>
       <c r="N268" s="41" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="O268" s="40" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="P268" s="40"/>
       <c r="Q268" s="40" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="R268" s="7">
         <v>0</v>
@@ -24022,22 +24026,22 @@
         <v>875</v>
       </c>
       <c r="D269" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="E269" s="40" t="s">
-        <v>1190</v>
+        <v>1188</v>
       </c>
       <c r="F269" s="41" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="G269" s="41" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="H269" s="47" t="s">
-        <v>1266</v>
+        <v>1264</v>
       </c>
       <c r="I269" s="41" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="J269" s="40" t="s">
         <v>979</v>
@@ -24052,14 +24056,14 @@
         <v>8</v>
       </c>
       <c r="N269" s="40" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="O269" s="40" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="P269" s="40"/>
       <c r="Q269" s="40" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="R269" s="7">
         <v>0</v>
@@ -24129,7 +24133,7 @@
         <v>333</v>
       </c>
       <c r="B2" s="53" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1">
@@ -24145,7 +24149,7 @@
         <v>732</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1">
@@ -24161,7 +24165,7 @@
         <v>336</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" customHeight="1">
@@ -24169,7 +24173,7 @@
         <v>337</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="17.25" customHeight="1">
@@ -24241,7 +24245,7 @@
         <v>346</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="17.25" customHeight="1">
@@ -24294,10 +24298,10 @@
     </row>
     <row r="23" spans="1:2" ht="17.25" customHeight="1">
       <c r="A23" s="13" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="17.25" customHeight="1">

</xml_diff>

<commit_message>
Act trabajo 2020 2021
</commit_message>
<xml_diff>
--- a/Data/Base_fichas_indicadores.xlsx
+++ b/Data/Base_fichas_indicadores.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3908" uniqueCount="1343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3908" uniqueCount="1341">
   <si>
     <t>id</t>
   </si>
@@ -3381,12 +3381,6 @@
   </si>
   <si>
     <t>Para cada año calcular: (Cantidad de personas ocupadas que perciben ingresos por hora en la ocupación principal por debajo del Salario Mínimo Nacional correspondiente al mes de relevamiento de la encuesta / Cantidad de personas ocupadas) *100</t>
-  </si>
-  <si>
-    <t>Instituto de Economía, Universidad de la República (2020) Encuesta Continua de Hogares Compatibilizada 1981-2018 Versión 12 DOI: http://doiorg/1047426/ECHINE y Series de Salario Mínimo Nacional (INE)</t>
-  </si>
-  <si>
-    <t>UMAD con base en Instituto de Economía, Universidad de la República (2020) Encuesta Continua de Hogares Compatibilizada 1981-2018 Versión 12 DOI: http://doiorg/1047426/ECHINE y Series de Salario Mínimo Nacional (INE)</t>
   </si>
   <si>
     <t>Poseer ingresos laborales por debajo del Salario Mïnimo Nacional</t>
@@ -4666,9 +4660,9 @@
   <dimension ref="A1:AK269"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A250" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A136" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E111" sqref="E111"/>
-      <selection pane="bottomLeft" activeCell="C284" sqref="C284"/>
+      <selection pane="bottomLeft" activeCell="Q159" sqref="Q159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4770,7 +4764,7 @@
         <v>675</v>
       </c>
       <c r="W1" s="13" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
     </row>
     <row r="2" spans="1:37" s="6" customFormat="1">
@@ -7160,10 +7154,10 @@
         <v>8</v>
       </c>
       <c r="N35" s="6" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="O35" s="6" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="P35" s="6" t="s">
         <v>23</v>
@@ -7343,7 +7337,7 @@
         <v>792</v>
       </c>
       <c r="G38" s="51" t="s">
-        <v>1284</v>
+        <v>1282</v>
       </c>
       <c r="H38" s="6" t="s">
         <v>377</v>
@@ -7409,7 +7403,7 @@
         <v>795</v>
       </c>
       <c r="G39" s="51" t="s">
-        <v>1285</v>
+        <v>1283</v>
       </c>
       <c r="H39" s="6" t="s">
         <v>722</v>
@@ -9209,10 +9203,10 @@
         <v>8</v>
       </c>
       <c r="N63" s="6" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="O63" s="6" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="P63" s="6" t="s">
         <v>54</v>
@@ -9262,7 +9256,7 @@
         <v>714</v>
       </c>
       <c r="I64" s="6" t="s">
-        <v>1305</v>
+        <v>1303</v>
       </c>
       <c r="J64" s="6" t="s">
         <v>5</v>
@@ -9277,10 +9271,10 @@
         <v>8</v>
       </c>
       <c r="N64" s="6" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="O64" s="6" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="P64" s="6" t="s">
         <v>54</v>
@@ -9346,10 +9340,10 @@
         <v>8</v>
       </c>
       <c r="N65" s="6" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="O65" s="6" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="P65" s="6" t="s">
         <v>54</v>
@@ -9414,10 +9408,10 @@
         <v>8</v>
       </c>
       <c r="N66" s="6" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="O66" s="6" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="P66" s="6" t="s">
         <v>54</v>
@@ -9482,10 +9476,10 @@
         <v>8</v>
       </c>
       <c r="N67" s="6" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="O67" s="6" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="P67" s="6" t="s">
         <v>54</v>
@@ -9551,10 +9545,10 @@
         <v>8</v>
       </c>
       <c r="N68" s="6" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="O68" s="6" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="P68" s="6" t="s">
         <v>54</v>
@@ -9615,16 +9609,16 @@
         <v>6</v>
       </c>
       <c r="L69" s="7" t="s">
-        <v>1277</v>
+        <v>1275</v>
       </c>
       <c r="M69" s="7" t="s">
         <v>8</v>
       </c>
       <c r="N69" s="6" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="O69" s="6" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="P69" s="7"/>
       <c r="Q69" s="7" t="s">
@@ -10252,7 +10246,7 @@
         <v>730</v>
       </c>
       <c r="I77" s="6" t="s">
-        <v>1306</v>
+        <v>1304</v>
       </c>
       <c r="J77" s="6" t="s">
         <v>5</v>
@@ -10336,10 +10330,10 @@
         <v>8</v>
       </c>
       <c r="N78" s="6" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="O78" s="6" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="P78" s="6" t="s">
         <v>61</v>
@@ -10405,10 +10399,10 @@
         <v>8</v>
       </c>
       <c r="N79" s="6" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="O79" s="6" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="P79" s="6" t="s">
         <v>61</v>
@@ -10474,10 +10468,10 @@
         <v>8</v>
       </c>
       <c r="N80" s="6" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="O80" s="6" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="P80" s="6" t="s">
         <v>61</v>
@@ -10543,10 +10537,10 @@
         <v>8</v>
       </c>
       <c r="N81" s="6" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="O81" s="6" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="P81" s="6" t="s">
         <v>61</v>
@@ -10612,10 +10606,10 @@
         <v>8</v>
       </c>
       <c r="N82" s="6" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="O82" s="6" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="P82" s="6" t="s">
         <v>61</v>
@@ -10681,10 +10675,10 @@
         <v>8</v>
       </c>
       <c r="N83" s="6" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="O83" s="6" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="P83" s="6" t="s">
         <v>61</v>
@@ -10751,10 +10745,10 @@
         <v>8</v>
       </c>
       <c r="N84" s="6" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="O84" s="6" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="P84" s="6" t="s">
         <v>61</v>
@@ -10833,10 +10827,10 @@
         <v>8</v>
       </c>
       <c r="N85" s="6" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="O85" s="6" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="P85" s="6" t="s">
         <v>61</v>
@@ -10914,10 +10908,10 @@
         <v>8</v>
       </c>
       <c r="N86" s="6" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="O86" s="6" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="P86" s="6" t="s">
         <v>61</v>
@@ -10984,10 +10978,10 @@
         <v>8</v>
       </c>
       <c r="N87" s="6" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="O87" s="6" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="P87" s="6" t="s">
         <v>61</v>
@@ -11065,10 +11059,10 @@
         <v>8</v>
       </c>
       <c r="N88" s="6" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="O88" s="6" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="P88" s="6" t="s">
         <v>61</v>
@@ -11134,10 +11128,10 @@
         <v>8</v>
       </c>
       <c r="N89" s="6" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="O89" s="6" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="P89" s="6" t="s">
         <v>61</v>
@@ -11204,10 +11198,10 @@
         <v>8</v>
       </c>
       <c r="N90" s="6" t="s">
-        <v>1337</v>
+        <v>1335</v>
       </c>
       <c r="O90" s="6" t="s">
-        <v>1338</v>
+        <v>1336</v>
       </c>
       <c r="P90" s="6" t="s">
         <v>61</v>
@@ -15300,7 +15294,7 @@
         <v>1098</v>
       </c>
       <c r="H143" s="52" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="I143" s="6" t="s">
         <v>1099</v>
@@ -15312,19 +15306,19 @@
         <v>6</v>
       </c>
       <c r="L143" s="6" t="s">
-        <v>7</v>
+        <v>966</v>
       </c>
       <c r="M143" s="6" t="s">
         <v>8</v>
       </c>
       <c r="N143" s="6" t="s">
-        <v>9</v>
+        <v>1335</v>
       </c>
       <c r="O143" s="6" t="s">
-        <v>187</v>
+        <v>1336</v>
       </c>
       <c r="Q143" s="6" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="R143" s="44">
         <v>0</v>
@@ -15378,19 +15372,19 @@
         <v>6</v>
       </c>
       <c r="L144" s="6" t="s">
-        <v>7</v>
+        <v>966</v>
       </c>
       <c r="M144" s="6" t="s">
         <v>8</v>
       </c>
       <c r="N144" s="6" t="s">
-        <v>9</v>
+        <v>1335</v>
       </c>
       <c r="O144" s="6" t="s">
-        <v>187</v>
+        <v>1336</v>
       </c>
       <c r="Q144" s="6" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="R144" s="44">
         <v>0</v>
@@ -15444,19 +15438,19 @@
         <v>6</v>
       </c>
       <c r="L145" s="6" t="s">
-        <v>7</v>
+        <v>966</v>
       </c>
       <c r="M145" s="6" t="s">
         <v>8</v>
       </c>
       <c r="N145" s="6" t="s">
-        <v>9</v>
+        <v>1335</v>
       </c>
       <c r="O145" s="6" t="s">
-        <v>187</v>
+        <v>1336</v>
       </c>
       <c r="Q145" s="6" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="R145" s="44">
         <v>0</v>
@@ -15498,7 +15492,7 @@
         <v>1104</v>
       </c>
       <c r="H146" s="7" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="I146" s="6" t="s">
         <v>1105</v>
@@ -15510,19 +15504,19 @@
         <v>6</v>
       </c>
       <c r="L146" s="6" t="s">
-        <v>7</v>
+        <v>966</v>
       </c>
       <c r="M146" s="6" t="s">
         <v>8</v>
       </c>
       <c r="N146" s="6" t="s">
-        <v>9</v>
+        <v>1335</v>
       </c>
       <c r="O146" s="6" t="s">
-        <v>187</v>
+        <v>1336</v>
       </c>
       <c r="Q146" s="6" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="R146" s="44">
         <v>0</v>
@@ -15563,7 +15557,7 @@
         <v>1088</v>
       </c>
       <c r="H147" s="7" t="s">
-        <v>1294</v>
+        <v>1292</v>
       </c>
       <c r="I147" s="6" t="s">
         <v>1089</v>
@@ -15575,19 +15569,19 @@
         <v>6</v>
       </c>
       <c r="L147" s="6" t="s">
-        <v>7</v>
+        <v>966</v>
       </c>
       <c r="M147" s="6" t="s">
         <v>8</v>
       </c>
       <c r="N147" s="6" t="s">
-        <v>9</v>
+        <v>1335</v>
       </c>
       <c r="O147" s="6" t="s">
-        <v>187</v>
+        <v>1336</v>
       </c>
       <c r="Q147" s="6" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="R147" s="44">
         <v>0</v>
@@ -15628,7 +15622,7 @@
         <v>1090</v>
       </c>
       <c r="H148" s="7" t="s">
-        <v>1297</v>
+        <v>1295</v>
       </c>
       <c r="I148" s="6" t="s">
         <v>1091</v>
@@ -15640,22 +15634,22 @@
         <v>6</v>
       </c>
       <c r="L148" s="6" t="s">
-        <v>7</v>
+        <v>966</v>
       </c>
       <c r="M148" s="6" t="s">
         <v>8</v>
       </c>
       <c r="N148" s="6" t="s">
-        <v>9</v>
+        <v>1335</v>
       </c>
       <c r="O148" s="6" t="s">
-        <v>187</v>
+        <v>1336</v>
       </c>
       <c r="P148" s="6" t="s">
         <v>54</v>
       </c>
       <c r="Q148" s="6" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="R148" s="44">
         <v>0</v>
@@ -15696,7 +15690,7 @@
         <v>1092</v>
       </c>
       <c r="H149" s="7" t="s">
-        <v>1298</v>
+        <v>1296</v>
       </c>
       <c r="I149" s="6" t="s">
         <v>1093</v>
@@ -15708,19 +15702,19 @@
         <v>6</v>
       </c>
       <c r="L149" s="6" t="s">
-        <v>7</v>
+        <v>966</v>
       </c>
       <c r="M149" s="6" t="s">
         <v>8</v>
       </c>
       <c r="N149" s="6" t="s">
-        <v>9</v>
+        <v>1335</v>
       </c>
       <c r="O149" s="6" t="s">
-        <v>187</v>
+        <v>1336</v>
       </c>
       <c r="Q149" s="6" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="R149" s="44">
         <v>0</v>
@@ -15761,7 +15755,7 @@
         <v>1094</v>
       </c>
       <c r="H150" s="7" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="I150" s="6" t="s">
         <v>1095</v>
@@ -15773,19 +15767,19 @@
         <v>6</v>
       </c>
       <c r="L150" s="6" t="s">
-        <v>7</v>
+        <v>966</v>
       </c>
       <c r="M150" s="6" t="s">
         <v>8</v>
       </c>
       <c r="N150" s="6" t="s">
-        <v>9</v>
+        <v>1335</v>
       </c>
       <c r="O150" s="6" t="s">
-        <v>187</v>
+        <v>1336</v>
       </c>
       <c r="Q150" s="6" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="R150" s="44">
         <v>0</v>
@@ -15826,7 +15820,7 @@
         <v>1096</v>
       </c>
       <c r="H151" s="7" t="s">
-        <v>1299</v>
+        <v>1297</v>
       </c>
       <c r="I151" s="6" t="s">
         <v>1097</v>
@@ -15838,19 +15832,19 @@
         <v>6</v>
       </c>
       <c r="L151" s="6" t="s">
-        <v>7</v>
+        <v>966</v>
       </c>
       <c r="M151" s="6" t="s">
         <v>8</v>
       </c>
       <c r="N151" s="6" t="s">
-        <v>9</v>
+        <v>1335</v>
       </c>
       <c r="O151" s="6" t="s">
-        <v>187</v>
+        <v>1336</v>
       </c>
       <c r="Q151" s="6" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="R151" s="44">
         <v>0</v>
@@ -15891,7 +15885,7 @@
         <v>1106</v>
       </c>
       <c r="H152" s="7" t="s">
-        <v>1300</v>
+        <v>1298</v>
       </c>
       <c r="I152" s="6" t="s">
         <v>1107</v>
@@ -15903,22 +15897,22 @@
         <v>6</v>
       </c>
       <c r="L152" s="6" t="s">
-        <v>7</v>
+        <v>966</v>
       </c>
       <c r="M152" s="6" t="s">
         <v>8</v>
       </c>
       <c r="N152" s="6" t="s">
-        <v>9</v>
+        <v>1335</v>
       </c>
       <c r="O152" s="6" t="s">
-        <v>187</v>
+        <v>1336</v>
       </c>
       <c r="P152" s="7" t="s">
         <v>1108</v>
       </c>
       <c r="Q152" s="6" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="R152" s="44">
         <v>0</v>
@@ -15953,13 +15947,13 @@
         <v>15</v>
       </c>
       <c r="F153" s="7" t="s">
-        <v>1340</v>
+        <v>1338</v>
       </c>
       <c r="G153" s="7" t="s">
         <v>1109</v>
       </c>
       <c r="H153" s="7" t="s">
-        <v>1301</v>
+        <v>1299</v>
       </c>
       <c r="I153" s="6" t="s">
         <v>1110</v>
@@ -15971,22 +15965,22 @@
         <v>6</v>
       </c>
       <c r="L153" s="6" t="s">
-        <v>7</v>
+        <v>966</v>
       </c>
       <c r="M153" s="6" t="s">
         <v>8</v>
       </c>
       <c r="N153" s="6" t="s">
+        <v>1335</v>
+      </c>
+      <c r="O153" s="6" t="s">
+        <v>1336</v>
+      </c>
+      <c r="P153" s="7" t="s">
         <v>1111</v>
       </c>
-      <c r="O153" s="6" t="s">
-        <v>1112</v>
-      </c>
-      <c r="P153" s="7" t="s">
-        <v>1113</v>
-      </c>
       <c r="Q153" s="6" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="R153" s="44">
         <v>0</v>
@@ -16021,16 +16015,16 @@
         <v>15</v>
       </c>
       <c r="F154" s="7" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="G154" s="7" t="s">
-        <v>1303</v>
+        <v>1301</v>
       </c>
       <c r="H154" s="7" t="s">
-        <v>1302</v>
+        <v>1300</v>
       </c>
       <c r="I154" s="6" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="J154" s="6" t="s">
         <v>5</v>
@@ -16039,19 +16033,19 @@
         <v>6</v>
       </c>
       <c r="L154" s="6" t="s">
-        <v>7</v>
+        <v>966</v>
       </c>
       <c r="M154" s="6" t="s">
         <v>8</v>
       </c>
       <c r="N154" s="6" t="s">
-        <v>9</v>
+        <v>1335</v>
       </c>
       <c r="O154" s="6" t="s">
-        <v>187</v>
+        <v>1336</v>
       </c>
       <c r="Q154" s="6" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="R154" s="44">
         <v>0</v>
@@ -16086,16 +16080,16 @@
         <v>15</v>
       </c>
       <c r="F155" s="54" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="G155" s="44" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="H155" s="44" t="s">
-        <v>1342</v>
+        <v>1340</v>
       </c>
       <c r="I155" s="13" t="s">
-        <v>1341</v>
+        <v>1339</v>
       </c>
       <c r="J155" s="14" t="s">
         <v>5</v>
@@ -16103,23 +16097,23 @@
       <c r="K155" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="L155" s="14" t="s">
-        <v>7</v>
+      <c r="L155" s="6" t="s">
+        <v>966</v>
       </c>
       <c r="M155" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="N155" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="O155" s="13" t="s">
-        <v>187</v>
+      <c r="N155" s="6" t="s">
+        <v>1335</v>
+      </c>
+      <c r="O155" s="6" t="s">
+        <v>1336</v>
       </c>
       <c r="P155" s="6" t="s">
-        <v>1118</v>
-      </c>
-      <c r="Q155" s="13" t="s">
-        <v>470</v>
+        <v>1116</v>
+      </c>
+      <c r="Q155" s="6" t="s">
+        <v>475</v>
       </c>
       <c r="R155" s="54">
         <v>0</v>
@@ -16154,16 +16148,16 @@
         <v>15</v>
       </c>
       <c r="F156" s="7" t="s">
+        <v>1117</v>
+      </c>
+      <c r="G156" s="7" t="s">
+        <v>1117</v>
+      </c>
+      <c r="H156" s="7" t="s">
+        <v>1118</v>
+      </c>
+      <c r="I156" s="7" t="s">
         <v>1119</v>
-      </c>
-      <c r="G156" s="7" t="s">
-        <v>1119</v>
-      </c>
-      <c r="H156" s="7" t="s">
-        <v>1120</v>
-      </c>
-      <c r="I156" s="7" t="s">
-        <v>1121</v>
       </c>
       <c r="J156" s="7" t="s">
         <v>5</v>
@@ -16172,16 +16166,16 @@
         <v>231</v>
       </c>
       <c r="L156" s="7" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="M156" s="7" t="s">
         <v>8</v>
       </c>
       <c r="N156" s="7" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="O156" s="7" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="Q156" s="7" t="s">
         <v>17</v>
@@ -16219,16 +16213,16 @@
         <v>15</v>
       </c>
       <c r="F157" s="7" t="s">
+        <v>1123</v>
+      </c>
+      <c r="G157" s="7" t="s">
+        <v>1123</v>
+      </c>
+      <c r="H157" s="7" t="s">
+        <v>1124</v>
+      </c>
+      <c r="I157" s="7" t="s">
         <v>1125</v>
-      </c>
-      <c r="G157" s="7" t="s">
-        <v>1125</v>
-      </c>
-      <c r="H157" s="7" t="s">
-        <v>1126</v>
-      </c>
-      <c r="I157" s="7" t="s">
-        <v>1127</v>
       </c>
       <c r="J157" s="7" t="s">
         <v>5</v>
@@ -16237,16 +16231,16 @@
         <v>231</v>
       </c>
       <c r="L157" s="7" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="M157" s="7" t="s">
         <v>8</v>
       </c>
       <c r="N157" s="7" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="O157" s="7" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="Q157" s="7" t="s">
         <v>17</v>
@@ -16284,19 +16278,19 @@
         <v>15</v>
       </c>
       <c r="F158" s="7" t="s">
+        <v>1129</v>
+      </c>
+      <c r="G158" s="7" t="s">
+        <v>1130</v>
+      </c>
+      <c r="H158" s="7" t="s">
         <v>1131</v>
       </c>
-      <c r="G158" s="7" t="s">
+      <c r="I158" s="7" t="s">
         <v>1132</v>
       </c>
-      <c r="H158" s="7" t="s">
+      <c r="J158" s="7" t="s">
         <v>1133</v>
-      </c>
-      <c r="I158" s="7" t="s">
-        <v>1134</v>
-      </c>
-      <c r="J158" s="7" t="s">
-        <v>1135</v>
       </c>
       <c r="K158" s="7" t="s">
         <v>231</v>
@@ -16350,16 +16344,16 @@
         <v>15</v>
       </c>
       <c r="F159" s="40" t="s">
+        <v>1134</v>
+      </c>
+      <c r="G159" s="40" t="s">
+        <v>1337</v>
+      </c>
+      <c r="H159" s="40" t="s">
+        <v>1135</v>
+      </c>
+      <c r="I159" s="40" t="s">
         <v>1136</v>
-      </c>
-      <c r="G159" s="40" t="s">
-        <v>1339</v>
-      </c>
-      <c r="H159" s="40" t="s">
-        <v>1137</v>
-      </c>
-      <c r="I159" s="40" t="s">
-        <v>1138</v>
       </c>
       <c r="J159" s="40" t="s">
         <v>5</v>
@@ -16368,20 +16362,20 @@
         <v>6</v>
       </c>
       <c r="L159" s="40" t="s">
+        <v>1137</v>
+      </c>
+      <c r="M159" s="44" t="s">
+        <v>1138</v>
+      </c>
+      <c r="N159" s="40" t="s">
         <v>1139</v>
       </c>
-      <c r="M159" s="44" t="s">
+      <c r="O159" s="40" t="s">
         <v>1140</v>
-      </c>
-      <c r="N159" s="40" t="s">
-        <v>1141</v>
-      </c>
-      <c r="O159" s="40" t="s">
-        <v>1142</v>
       </c>
       <c r="P159" s="40"/>
       <c r="Q159" s="40" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="R159" s="44">
         <v>0</v>
@@ -16416,10 +16410,10 @@
         <v>104</v>
       </c>
       <c r="F160" s="37" t="s">
-        <v>1286</v>
+        <v>1284</v>
       </c>
       <c r="G160" s="3" t="s">
-        <v>1291</v>
+        <v>1289</v>
       </c>
       <c r="H160" s="6" t="s">
         <v>790</v>
@@ -16482,10 +16476,10 @@
         <v>104</v>
       </c>
       <c r="F161" s="37" t="s">
-        <v>1287</v>
+        <v>1285</v>
       </c>
       <c r="G161" s="3" t="s">
-        <v>1290</v>
+        <v>1288</v>
       </c>
       <c r="H161" s="6" t="s">
         <v>793</v>
@@ -16548,10 +16542,10 @@
         <v>104</v>
       </c>
       <c r="F162" s="37" t="s">
-        <v>1288</v>
+        <v>1286</v>
       </c>
       <c r="G162" s="3" t="s">
-        <v>1289</v>
+        <v>1287</v>
       </c>
       <c r="H162" s="6" t="s">
         <v>796</v>
@@ -17265,10 +17259,10 @@
         <v>3</v>
       </c>
       <c r="F173" s="7" t="s">
+        <v>1276</v>
+      </c>
+      <c r="G173" s="7" t="s">
         <v>1278</v>
-      </c>
-      <c r="G173" s="7" t="s">
-        <v>1280</v>
       </c>
       <c r="H173" s="6" t="s">
         <v>798</v>
@@ -17333,10 +17327,10 @@
         <v>3</v>
       </c>
       <c r="F174" s="7" t="s">
+        <v>1277</v>
+      </c>
+      <c r="G174" s="7" t="s">
         <v>1279</v>
-      </c>
-      <c r="G174" s="7" t="s">
-        <v>1281</v>
       </c>
       <c r="H174" s="6" t="s">
         <v>378</v>
@@ -17401,10 +17395,10 @@
         <v>3</v>
       </c>
       <c r="F175" s="36" t="s">
-        <v>1283</v>
+        <v>1281</v>
       </c>
       <c r="G175" s="6" t="s">
-        <v>1282</v>
+        <v>1280</v>
       </c>
       <c r="H175" s="6" t="s">
         <v>419</v>
@@ -18701,19 +18695,19 @@
         <v>2</v>
       </c>
       <c r="E194" s="7" t="s">
+        <v>1142</v>
+      </c>
+      <c r="F194" s="6" t="s">
+        <v>1143</v>
+      </c>
+      <c r="G194" s="6" t="s">
         <v>1144</v>
       </c>
-      <c r="F194" s="6" t="s">
+      <c r="H194" s="7" t="s">
         <v>1145</v>
       </c>
-      <c r="G194" s="6" t="s">
+      <c r="I194" s="7" t="s">
         <v>1146</v>
-      </c>
-      <c r="H194" s="7" t="s">
-        <v>1147</v>
-      </c>
-      <c r="I194" s="7" t="s">
-        <v>1148</v>
       </c>
       <c r="J194" s="6" t="s">
         <v>5</v>
@@ -18769,19 +18763,19 @@
         <v>2</v>
       </c>
       <c r="E195" s="7" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="F195" s="6" t="s">
+        <v>1147</v>
+      </c>
+      <c r="G195" s="6" t="s">
+        <v>1148</v>
+      </c>
+      <c r="H195" s="7" t="s">
         <v>1149</v>
       </c>
-      <c r="G195" s="6" t="s">
+      <c r="I195" s="46" t="s">
         <v>1150</v>
-      </c>
-      <c r="H195" s="7" t="s">
-        <v>1151</v>
-      </c>
-      <c r="I195" s="46" t="s">
-        <v>1152</v>
       </c>
       <c r="J195" s="7" t="s">
         <v>979</v>
@@ -18837,19 +18831,19 @@
         <v>2</v>
       </c>
       <c r="E196" s="7" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="F196" s="6" t="s">
+        <v>1151</v>
+      </c>
+      <c r="G196" s="6" t="s">
+        <v>1151</v>
+      </c>
+      <c r="H196" s="7" t="s">
+        <v>1152</v>
+      </c>
+      <c r="I196" s="7" t="s">
         <v>1153</v>
-      </c>
-      <c r="G196" s="6" t="s">
-        <v>1153</v>
-      </c>
-      <c r="H196" s="7" t="s">
-        <v>1154</v>
-      </c>
-      <c r="I196" s="7" t="s">
-        <v>1155</v>
       </c>
       <c r="J196" s="7" t="s">
         <v>806</v>
@@ -18870,7 +18864,7 @@
         <v>909</v>
       </c>
       <c r="Q196" s="7" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="R196" s="44">
         <v>0</v>
@@ -19399,7 +19393,7 @@
         <v>912</v>
       </c>
       <c r="G204" s="7" t="s">
-        <v>1312</v>
+        <v>1310</v>
       </c>
       <c r="H204" s="7" t="s">
         <v>913</v>
@@ -19468,7 +19462,7 @@
         <v>919</v>
       </c>
       <c r="G205" s="7" t="s">
-        <v>1313</v>
+        <v>1311</v>
       </c>
       <c r="H205" s="7" t="s">
         <v>920</v>
@@ -19537,7 +19531,7 @@
         <v>922</v>
       </c>
       <c r="G206" s="7" t="s">
-        <v>1310</v>
+        <v>1308</v>
       </c>
       <c r="H206" s="7" t="s">
         <v>923</v>
@@ -19606,7 +19600,7 @@
         <v>925</v>
       </c>
       <c r="G207" s="7" t="s">
-        <v>1311</v>
+        <v>1309</v>
       </c>
       <c r="H207" s="7" t="s">
         <v>926</v>
@@ -19746,10 +19740,10 @@
         <v>3</v>
       </c>
       <c r="F209" s="7" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="G209" s="7" t="s">
-        <v>1314</v>
+        <v>1312</v>
       </c>
       <c r="H209" s="7" t="s">
         <v>1048</v>
@@ -19814,10 +19808,10 @@
         <v>3</v>
       </c>
       <c r="F210" s="7" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="G210" s="7" t="s">
-        <v>1315</v>
+        <v>1313</v>
       </c>
       <c r="H210" s="7" t="s">
         <v>1051</v>
@@ -19882,10 +19876,10 @@
         <v>3</v>
       </c>
       <c r="F211" s="7" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="G211" s="7" t="s">
-        <v>1316</v>
+        <v>1314</v>
       </c>
       <c r="H211" s="7" t="s">
         <v>1053</v>
@@ -19950,10 +19944,10 @@
         <v>3</v>
       </c>
       <c r="F212" s="7" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="G212" s="7" t="s">
-        <v>1317</v>
+        <v>1315</v>
       </c>
       <c r="H212" s="7" t="s">
         <v>1055</v>
@@ -20018,10 +20012,10 @@
         <v>3</v>
       </c>
       <c r="F213" s="7" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="G213" s="7" t="s">
-        <v>1318</v>
+        <v>1316</v>
       </c>
       <c r="H213" s="7" t="s">
         <v>1057</v>
@@ -20086,10 +20080,10 @@
         <v>3</v>
       </c>
       <c r="F214" s="7" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="G214" s="7" t="s">
-        <v>1319</v>
+        <v>1317</v>
       </c>
       <c r="H214" s="7" t="s">
         <v>1059</v>
@@ -20154,10 +20148,10 @@
         <v>3</v>
       </c>
       <c r="F215" s="7" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="G215" s="7" t="s">
-        <v>1320</v>
+        <v>1318</v>
       </c>
       <c r="H215" s="7" t="s">
         <v>1061</v>
@@ -20222,10 +20216,10 @@
         <v>3</v>
       </c>
       <c r="F216" s="7" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="G216" s="7" t="s">
-        <v>1321</v>
+        <v>1319</v>
       </c>
       <c r="H216" s="7" t="s">
         <v>1063</v>
@@ -20290,10 +20284,10 @@
         <v>3</v>
       </c>
       <c r="F217" s="7" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
       <c r="G217" s="7" t="s">
-        <v>1322</v>
+        <v>1320</v>
       </c>
       <c r="H217" s="7" t="s">
         <v>1065</v>
@@ -20349,7 +20343,7 @@
         <v>1</v>
       </c>
       <c r="C218" s="7" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="D218" s="7" t="s">
         <v>2</v>
@@ -20376,7 +20370,7 @@
         <v>6</v>
       </c>
       <c r="L218" s="7" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="M218" s="7" t="s">
         <v>940</v>
@@ -20421,7 +20415,7 @@
         <v>1</v>
       </c>
       <c r="C219" s="7" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="D219" s="7" t="s">
         <v>2</v>
@@ -20448,7 +20442,7 @@
         <v>6</v>
       </c>
       <c r="L219" s="7" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="M219" s="7" t="s">
         <v>940</v>
@@ -20493,7 +20487,7 @@
         <v>35</v>
       </c>
       <c r="C220" s="7" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="D220" s="7" t="s">
         <v>2</v>
@@ -20502,16 +20496,16 @@
         <v>36</v>
       </c>
       <c r="F220" s="7" t="s">
+        <v>1161</v>
+      </c>
+      <c r="G220" s="7" t="s">
+        <v>1162</v>
+      </c>
+      <c r="H220" s="6" t="s">
         <v>1163</v>
       </c>
-      <c r="G220" s="7" t="s">
+      <c r="I220" s="6" t="s">
         <v>1164</v>
-      </c>
-      <c r="H220" s="6" t="s">
-        <v>1165</v>
-      </c>
-      <c r="I220" s="6" t="s">
-        <v>1166</v>
       </c>
       <c r="J220" s="6" t="s">
         <v>5</v>
@@ -20520,7 +20514,7 @@
         <v>6</v>
       </c>
       <c r="L220" s="7" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="M220" s="7" t="s">
         <v>940</v>
@@ -20564,7 +20558,7 @@
         <v>35</v>
       </c>
       <c r="C221" s="7" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="D221" s="7" t="s">
         <v>2</v>
@@ -20573,16 +20567,16 @@
         <v>41</v>
       </c>
       <c r="F221" s="7" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="G221" s="7" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
       <c r="H221" s="6" t="s">
         <v>419</v>
       </c>
       <c r="I221" s="6" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="J221" s="6" t="s">
         <v>5</v>
@@ -20591,7 +20585,7 @@
         <v>6</v>
       </c>
       <c r="L221" s="7" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="M221" s="7" t="s">
         <v>940</v>
@@ -20635,7 +20629,7 @@
         <v>35</v>
       </c>
       <c r="C222" s="7" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="D222" s="7" t="s">
         <v>2</v>
@@ -20644,16 +20638,16 @@
         <v>41</v>
       </c>
       <c r="F222" s="7" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="G222" s="7" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="H222" s="6" t="s">
         <v>378</v>
       </c>
       <c r="I222" s="6" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
       <c r="J222" s="6" t="s">
         <v>5</v>
@@ -20662,7 +20656,7 @@
         <v>6</v>
       </c>
       <c r="L222" s="7" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="M222" s="7" t="s">
         <v>940</v>
@@ -20706,7 +20700,7 @@
         <v>35</v>
       </c>
       <c r="C223" s="7" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="D223" s="7" t="s">
         <v>2</v>
@@ -20715,16 +20709,16 @@
         <v>41</v>
       </c>
       <c r="F223" s="7" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="G223" s="7" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
       <c r="H223" s="6" t="s">
         <v>304</v>
       </c>
       <c r="I223" s="6" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="J223" s="6" t="s">
         <v>5</v>
@@ -20733,7 +20727,7 @@
         <v>6</v>
       </c>
       <c r="L223" s="7" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="M223" s="7" t="s">
         <v>940</v>
@@ -20777,7 +20771,7 @@
         <v>35</v>
       </c>
       <c r="C224" s="7" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="D224" s="7" t="s">
         <v>2</v>
@@ -20786,16 +20780,16 @@
         <v>41</v>
       </c>
       <c r="F224" s="7" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="G224" s="7" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="H224" s="6" t="s">
         <v>420</v>
       </c>
       <c r="I224" s="6" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="J224" s="6" t="s">
         <v>5</v>
@@ -20804,7 +20798,7 @@
         <v>6</v>
       </c>
       <c r="L224" s="7" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="M224" s="7" t="s">
         <v>940</v>
@@ -20854,7 +20848,7 @@
         <v>35</v>
       </c>
       <c r="C225" s="7" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="D225" s="7" t="s">
         <v>2</v>
@@ -20863,16 +20857,16 @@
         <v>46</v>
       </c>
       <c r="F225" s="7" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
       <c r="G225" s="7" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
       <c r="H225" s="6" t="s">
         <v>421</v>
       </c>
       <c r="I225" s="27" t="s">
-        <v>1181</v>
+        <v>1179</v>
       </c>
       <c r="J225" s="6" t="s">
         <v>5</v>
@@ -20881,7 +20875,7 @@
         <v>6</v>
       </c>
       <c r="L225" s="7" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="M225" s="7" t="s">
         <v>940</v>
@@ -20931,7 +20925,7 @@
         <v>35</v>
       </c>
       <c r="C226" s="7" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="D226" s="7" t="s">
         <v>2</v>
@@ -20940,16 +20934,16 @@
         <v>47</v>
       </c>
       <c r="F226" s="6" t="s">
-        <v>1182</v>
+        <v>1180</v>
       </c>
       <c r="G226" s="7" t="s">
-        <v>1183</v>
+        <v>1181</v>
       </c>
       <c r="H226" s="6" t="s">
         <v>641</v>
       </c>
       <c r="I226" s="27" t="s">
-        <v>1184</v>
+        <v>1182</v>
       </c>
       <c r="J226" s="6" t="s">
         <v>5</v>
@@ -20958,7 +20952,7 @@
         <v>6</v>
       </c>
       <c r="L226" s="7" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="M226" s="7" t="s">
         <v>940</v>
@@ -21008,7 +21002,7 @@
         <v>35</v>
       </c>
       <c r="C227" s="7" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="D227" s="7" t="s">
         <v>2</v>
@@ -21017,16 +21011,16 @@
         <v>47</v>
       </c>
       <c r="F227" s="7" t="s">
-        <v>1185</v>
+        <v>1183</v>
       </c>
       <c r="G227" s="7" t="s">
-        <v>1186</v>
+        <v>1184</v>
       </c>
       <c r="H227" s="6" t="s">
         <v>379</v>
       </c>
       <c r="I227" s="6" t="s">
-        <v>1187</v>
+        <v>1185</v>
       </c>
       <c r="J227" s="6" t="s">
         <v>5</v>
@@ -21035,7 +21029,7 @@
         <v>6</v>
       </c>
       <c r="L227" s="7" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="M227" s="7" t="s">
         <v>940</v>
@@ -21085,7 +21079,7 @@
         <v>52</v>
       </c>
       <c r="C228" s="7" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="D228" s="7" t="s">
         <v>2</v>
@@ -21112,7 +21106,7 @@
         <v>6</v>
       </c>
       <c r="L228" s="7" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="M228" s="7" t="s">
         <v>940</v>
@@ -21159,7 +21153,7 @@
         <v>52</v>
       </c>
       <c r="C229" s="7" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="D229" s="7" t="s">
         <v>2</v>
@@ -21171,13 +21165,13 @@
         <v>996</v>
       </c>
       <c r="G229" s="7" t="s">
-        <v>1325</v>
+        <v>1323</v>
       </c>
       <c r="H229" s="6" t="s">
         <v>714</v>
       </c>
       <c r="I229" s="6" t="s">
-        <v>1307</v>
+        <v>1305</v>
       </c>
       <c r="J229" s="6" t="s">
         <v>5</v>
@@ -21186,7 +21180,7 @@
         <v>6</v>
       </c>
       <c r="L229" s="7" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="M229" s="7" t="s">
         <v>940</v>
@@ -21236,7 +21230,7 @@
         <v>52</v>
       </c>
       <c r="C230" s="7" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="D230" s="7" t="s">
         <v>2</v>
@@ -21248,7 +21242,7 @@
         <v>997</v>
       </c>
       <c r="G230" s="7" t="s">
-        <v>1326</v>
+        <v>1324</v>
       </c>
       <c r="H230" s="6" t="s">
         <v>384</v>
@@ -21263,7 +21257,7 @@
         <v>6</v>
       </c>
       <c r="L230" s="7" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="M230" s="7" t="s">
         <v>940</v>
@@ -21313,7 +21307,7 @@
         <v>52</v>
       </c>
       <c r="C231" s="7" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="D231" s="7" t="s">
         <v>2</v>
@@ -21325,13 +21319,13 @@
         <v>999</v>
       </c>
       <c r="G231" s="7" t="s">
-        <v>1327</v>
+        <v>1325</v>
       </c>
       <c r="H231" s="6" t="s">
         <v>714</v>
       </c>
       <c r="I231" s="6" t="s">
-        <v>1308</v>
+        <v>1306</v>
       </c>
       <c r="J231" s="6" t="s">
         <v>5</v>
@@ -21340,7 +21334,7 @@
         <v>6</v>
       </c>
       <c r="L231" s="7" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="M231" s="7" t="s">
         <v>940</v>
@@ -21390,7 +21384,7 @@
         <v>70</v>
       </c>
       <c r="C232" s="7" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="D232" s="7" t="s">
         <v>2</v>
@@ -21417,7 +21411,7 @@
         <v>6</v>
       </c>
       <c r="L232" s="7" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="M232" s="7" t="s">
         <v>940</v>
@@ -21467,7 +21461,7 @@
         <v>1000</v>
       </c>
       <c r="C233" s="7" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="D233" s="7" t="s">
         <v>2</v>
@@ -21482,7 +21476,7 @@
         <v>1074</v>
       </c>
       <c r="H233" s="7" t="s">
-        <v>1292</v>
+        <v>1290</v>
       </c>
       <c r="I233" s="6" t="s">
         <v>1075</v>
@@ -21494,7 +21488,7 @@
         <v>6</v>
       </c>
       <c r="L233" s="7" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="M233" s="7" t="s">
         <v>940</v>
@@ -21535,7 +21529,7 @@
         <v>1000</v>
       </c>
       <c r="C234" s="7" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="D234" s="7" t="s">
         <v>2</v>
@@ -21550,7 +21544,7 @@
         <v>1076</v>
       </c>
       <c r="H234" s="7" t="s">
-        <v>1304</v>
+        <v>1302</v>
       </c>
       <c r="I234" s="6" t="s">
         <v>1078</v>
@@ -21562,7 +21556,7 @@
         <v>6</v>
       </c>
       <c r="L234" s="7" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="M234" s="7" t="s">
         <v>940</v>
@@ -21603,7 +21597,7 @@
         <v>1000</v>
       </c>
       <c r="C235" s="7" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="D235" s="7" t="s">
         <v>2</v>
@@ -21630,7 +21624,7 @@
         <v>6</v>
       </c>
       <c r="L235" s="7" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="M235" s="7" t="s">
         <v>940</v>
@@ -21671,7 +21665,7 @@
         <v>1000</v>
       </c>
       <c r="C236" s="7" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="D236" s="7" t="s">
         <v>2</v>
@@ -21686,7 +21680,7 @@
         <v>1081</v>
       </c>
       <c r="H236" s="7" t="s">
-        <v>1293</v>
+        <v>1291</v>
       </c>
       <c r="I236" s="6" t="s">
         <v>1082</v>
@@ -21698,7 +21692,7 @@
         <v>6</v>
       </c>
       <c r="L236" s="7" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="M236" s="7" t="s">
         <v>940</v>
@@ -21739,7 +21733,7 @@
         <v>1000</v>
       </c>
       <c r="C237" s="7" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="D237" s="7" t="s">
         <v>2</v>
@@ -21754,7 +21748,7 @@
         <v>1083</v>
       </c>
       <c r="H237" s="7" t="s">
-        <v>1295</v>
+        <v>1293</v>
       </c>
       <c r="I237" s="6" t="s">
         <v>1084</v>
@@ -21766,7 +21760,7 @@
         <v>6</v>
       </c>
       <c r="L237" s="7" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="M237" s="7" t="s">
         <v>940</v>
@@ -21807,7 +21801,7 @@
         <v>1000</v>
       </c>
       <c r="C238" s="7" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="D238" s="7" t="s">
         <v>2</v>
@@ -21819,10 +21813,10 @@
         <v>1085</v>
       </c>
       <c r="G238" s="7" t="s">
-        <v>1323</v>
+        <v>1321</v>
       </c>
       <c r="H238" s="6" t="s">
-        <v>1296</v>
+        <v>1294</v>
       </c>
       <c r="I238" s="6" t="s">
         <v>1086</v>
@@ -21834,7 +21828,7 @@
         <v>6</v>
       </c>
       <c r="L238" s="7" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="M238" s="7" t="s">
         <v>940</v>
@@ -22094,16 +22088,16 @@
         <v>47</v>
       </c>
       <c r="F242" s="41" t="s">
+        <v>1155</v>
+      </c>
+      <c r="G242" s="41" t="s">
+        <v>1156</v>
+      </c>
+      <c r="H242" s="40" t="s">
         <v>1157</v>
       </c>
-      <c r="G242" s="41" t="s">
+      <c r="I242" s="41" t="s">
         <v>1158</v>
-      </c>
-      <c r="H242" s="40" t="s">
-        <v>1159</v>
-      </c>
-      <c r="I242" s="41" t="s">
-        <v>1160</v>
       </c>
       <c r="J242" s="40" t="s">
         <v>5</v>
@@ -22118,10 +22112,10 @@
         <v>8</v>
       </c>
       <c r="N242" s="41" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="O242" s="40" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="P242" s="40"/>
       <c r="Q242" s="40" t="s">
@@ -22390,7 +22384,7 @@
         <v>1072</v>
       </c>
       <c r="H246" s="42" t="s">
-        <v>1335</v>
+        <v>1333</v>
       </c>
       <c r="I246" s="42" t="s">
         <v>1073</v>
@@ -22445,25 +22439,25 @@
         <v>884</v>
       </c>
       <c r="D247" s="40" t="s">
+        <v>1186</v>
+      </c>
+      <c r="E247" s="40" t="s">
+        <v>1186</v>
+      </c>
+      <c r="F247" s="7" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G247" s="6" t="s">
+        <v>1187</v>
+      </c>
+      <c r="H247" s="6" t="s">
         <v>1188</v>
       </c>
-      <c r="E247" s="40" t="s">
-        <v>1188</v>
-      </c>
-      <c r="F247" s="7" t="s">
+      <c r="I247" s="6" t="s">
         <v>1189</v>
       </c>
-      <c r="G247" s="6" t="s">
-        <v>1189</v>
-      </c>
-      <c r="H247" s="6" t="s">
+      <c r="J247" s="6" t="s">
         <v>1190</v>
-      </c>
-      <c r="I247" s="6" t="s">
-        <v>1191</v>
-      </c>
-      <c r="J247" s="6" t="s">
-        <v>1192</v>
       </c>
       <c r="K247" s="6" t="s">
         <v>6</v>
@@ -22512,22 +22506,22 @@
         <v>911</v>
       </c>
       <c r="D248" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="E248" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="F248" s="7" t="s">
+        <v>1191</v>
+      </c>
+      <c r="G248" s="7" t="s">
+        <v>1192</v>
+      </c>
+      <c r="H248" s="7" t="s">
         <v>1193</v>
       </c>
-      <c r="G248" s="7" t="s">
+      <c r="I248" s="7" t="s">
         <v>1194</v>
-      </c>
-      <c r="H248" s="7" t="s">
-        <v>1195</v>
-      </c>
-      <c r="I248" s="7" t="s">
-        <v>1196</v>
       </c>
       <c r="J248" s="7" t="s">
         <v>5</v>
@@ -22548,7 +22542,7 @@
         <v>917</v>
       </c>
       <c r="Q248" s="7" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="R248" s="7">
         <v>0</v>
@@ -22578,22 +22572,22 @@
         <v>911</v>
       </c>
       <c r="D249" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="E249" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="F249" s="7" t="s">
+        <v>1196</v>
+      </c>
+      <c r="G249" s="7" t="s">
+        <v>1197</v>
+      </c>
+      <c r="H249" s="7" t="s">
         <v>1198</v>
       </c>
-      <c r="G249" s="7" t="s">
+      <c r="I249" s="7" t="s">
         <v>1199</v>
-      </c>
-      <c r="H249" s="7" t="s">
-        <v>1200</v>
-      </c>
-      <c r="I249" s="7" t="s">
-        <v>1201</v>
       </c>
       <c r="J249" s="7" t="s">
         <v>5</v>
@@ -22614,7 +22608,7 @@
         <v>917</v>
       </c>
       <c r="Q249" s="7" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="R249" s="7">
         <v>0</v>
@@ -22644,22 +22638,22 @@
         <v>911</v>
       </c>
       <c r="D250" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="E250" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="F250" s="7" t="s">
+        <v>1200</v>
+      </c>
+      <c r="G250" s="7" t="s">
+        <v>1201</v>
+      </c>
+      <c r="H250" s="7" t="s">
         <v>1202</v>
       </c>
-      <c r="G250" s="7" t="s">
+      <c r="I250" s="7" t="s">
         <v>1203</v>
-      </c>
-      <c r="H250" s="7" t="s">
-        <v>1204</v>
-      </c>
-      <c r="I250" s="7" t="s">
-        <v>1205</v>
       </c>
       <c r="J250" s="7" t="s">
         <v>5</v>
@@ -22680,7 +22674,7 @@
         <v>917</v>
       </c>
       <c r="Q250" s="7" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="R250" s="7">
         <v>0</v>
@@ -22710,22 +22704,22 @@
         <v>911</v>
       </c>
       <c r="D251" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="E251" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="F251" s="7" t="s">
+        <v>1204</v>
+      </c>
+      <c r="G251" s="7" t="s">
+        <v>1205</v>
+      </c>
+      <c r="H251" s="7" t="s">
         <v>1206</v>
       </c>
-      <c r="G251" s="7" t="s">
+      <c r="I251" s="7" t="s">
         <v>1207</v>
-      </c>
-      <c r="H251" s="7" t="s">
-        <v>1208</v>
-      </c>
-      <c r="I251" s="7" t="s">
-        <v>1209</v>
       </c>
       <c r="J251" s="7" t="s">
         <v>5</v>
@@ -22746,7 +22740,7 @@
         <v>917</v>
       </c>
       <c r="Q251" s="7" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="R251" s="7">
         <v>0</v>
@@ -22777,22 +22771,22 @@
         <v>911</v>
       </c>
       <c r="D252" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="E252" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="F252" s="7" t="s">
+        <v>1208</v>
+      </c>
+      <c r="G252" s="7" t="s">
+        <v>1209</v>
+      </c>
+      <c r="H252" s="7" t="s">
         <v>1210</v>
       </c>
-      <c r="G252" s="7" t="s">
+      <c r="I252" s="7" t="s">
         <v>1211</v>
-      </c>
-      <c r="H252" s="7" t="s">
-        <v>1212</v>
-      </c>
-      <c r="I252" s="7" t="s">
-        <v>1213</v>
       </c>
       <c r="J252" s="7" t="s">
         <v>5</v>
@@ -22814,7 +22808,7 @@
       </c>
       <c r="P252" s="7"/>
       <c r="Q252" s="7" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="R252" s="7">
         <v>0</v>
@@ -22849,22 +22843,22 @@
         <v>911</v>
       </c>
       <c r="D253" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="E253" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="F253" s="7" t="s">
+        <v>1212</v>
+      </c>
+      <c r="G253" s="7" t="s">
+        <v>1213</v>
+      </c>
+      <c r="H253" s="7" t="s">
         <v>1214</v>
       </c>
-      <c r="G253" s="7" t="s">
+      <c r="I253" s="7" t="s">
         <v>1215</v>
-      </c>
-      <c r="H253" s="7" t="s">
-        <v>1216</v>
-      </c>
-      <c r="I253" s="7" t="s">
-        <v>1217</v>
       </c>
       <c r="J253" s="7" t="s">
         <v>5</v>
@@ -22885,7 +22879,7 @@
         <v>917</v>
       </c>
       <c r="Q253" s="7" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="R253" s="7">
         <v>0</v>
@@ -22922,22 +22916,22 @@
         <v>911</v>
       </c>
       <c r="D254" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="E254" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="F254" s="7" t="s">
+        <v>1216</v>
+      </c>
+      <c r="G254" s="7" t="s">
+        <v>1217</v>
+      </c>
+      <c r="H254" s="7" t="s">
         <v>1218</v>
       </c>
-      <c r="G254" s="7" t="s">
+      <c r="I254" s="7" t="s">
         <v>1219</v>
-      </c>
-      <c r="H254" s="7" t="s">
-        <v>1220</v>
-      </c>
-      <c r="I254" s="7" t="s">
-        <v>1221</v>
       </c>
       <c r="J254" s="7" t="s">
         <v>5</v>
@@ -22958,7 +22952,7 @@
         <v>917</v>
       </c>
       <c r="Q254" s="7" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="R254" s="7">
         <v>0</v>
@@ -22996,22 +22990,22 @@
         <v>911</v>
       </c>
       <c r="D255" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="E255" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="F255" s="7" t="s">
+        <v>1220</v>
+      </c>
+      <c r="G255" s="7" t="s">
+        <v>1221</v>
+      </c>
+      <c r="H255" s="7" t="s">
         <v>1222</v>
       </c>
-      <c r="G255" s="7" t="s">
+      <c r="I255" s="7" t="s">
         <v>1223</v>
-      </c>
-      <c r="H255" s="7" t="s">
-        <v>1224</v>
-      </c>
-      <c r="I255" s="7" t="s">
-        <v>1225</v>
       </c>
       <c r="J255" s="7" t="s">
         <v>5</v>
@@ -23033,7 +23027,7 @@
       </c>
       <c r="P255" s="7"/>
       <c r="Q255" s="7" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="R255" s="7">
         <v>0</v>
@@ -23070,22 +23064,22 @@
         <v>911</v>
       </c>
       <c r="D256" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="E256" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="F256" s="7" t="s">
+        <v>1224</v>
+      </c>
+      <c r="G256" s="7" t="s">
+        <v>1225</v>
+      </c>
+      <c r="H256" s="7" t="s">
         <v>1226</v>
       </c>
-      <c r="G256" s="7" t="s">
+      <c r="I256" s="7" t="s">
         <v>1227</v>
-      </c>
-      <c r="H256" s="7" t="s">
-        <v>1228</v>
-      </c>
-      <c r="I256" s="7" t="s">
-        <v>1229</v>
       </c>
       <c r="J256" s="7" t="s">
         <v>5</v>
@@ -23107,7 +23101,7 @@
       </c>
       <c r="P256" s="7"/>
       <c r="Q256" s="7" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="R256" s="7">
         <v>0</v>
@@ -23144,22 +23138,22 @@
         <v>911</v>
       </c>
       <c r="D257" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="E257" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="F257" s="7" t="s">
+        <v>1228</v>
+      </c>
+      <c r="G257" s="7" t="s">
+        <v>1229</v>
+      </c>
+      <c r="H257" s="7" t="s">
         <v>1230</v>
       </c>
-      <c r="G257" s="7" t="s">
+      <c r="I257" s="7" t="s">
         <v>1231</v>
-      </c>
-      <c r="H257" s="7" t="s">
-        <v>1232</v>
-      </c>
-      <c r="I257" s="7" t="s">
-        <v>1233</v>
       </c>
       <c r="J257" s="7" t="s">
         <v>5</v>
@@ -23181,7 +23175,7 @@
       </c>
       <c r="P257" s="7"/>
       <c r="Q257" s="7" t="s">
-        <v>1197</v>
+        <v>1195</v>
       </c>
       <c r="R257" s="7">
         <v>0</v>
@@ -23218,22 +23212,22 @@
         <v>911</v>
       </c>
       <c r="D258" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="E258" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="F258" s="7" t="s">
+        <v>1232</v>
+      </c>
+      <c r="G258" s="7" t="s">
+        <v>1232</v>
+      </c>
+      <c r="H258" s="7" t="s">
+        <v>1233</v>
+      </c>
+      <c r="I258" s="45" t="s">
         <v>1234</v>
-      </c>
-      <c r="G258" s="7" t="s">
-        <v>1234</v>
-      </c>
-      <c r="H258" s="7" t="s">
-        <v>1235</v>
-      </c>
-      <c r="I258" s="45" t="s">
-        <v>1236</v>
       </c>
       <c r="J258" s="7" t="s">
         <v>979</v>
@@ -23292,22 +23286,22 @@
         <v>911</v>
       </c>
       <c r="D259" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="E259" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="F259" s="7" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="G259" s="7" t="s">
-        <v>1237</v>
+        <v>1235</v>
       </c>
       <c r="H259" s="7" t="s">
-        <v>1238</v>
+        <v>1236</v>
       </c>
       <c r="I259" s="45" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="J259" s="7" t="s">
         <v>979</v>
@@ -23366,22 +23360,22 @@
         <v>911</v>
       </c>
       <c r="D260" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="E260" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="F260" s="7" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="G260" s="7" t="s">
-        <v>1239</v>
+        <v>1237</v>
       </c>
       <c r="H260" s="7" t="s">
-        <v>1240</v>
+        <v>1238</v>
       </c>
       <c r="I260" s="45" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="J260" s="7" t="s">
         <v>979</v>
@@ -23440,22 +23434,22 @@
         <v>911</v>
       </c>
       <c r="D261" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="E261" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="F261" s="7" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="G261" s="7" t="s">
-        <v>1241</v>
+        <v>1239</v>
       </c>
       <c r="H261" s="7" t="s">
-        <v>1242</v>
+        <v>1240</v>
       </c>
       <c r="I261" s="45" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="J261" s="7" t="s">
         <v>979</v>
@@ -23514,22 +23508,22 @@
         <v>911</v>
       </c>
       <c r="D262" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="E262" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="F262" s="7" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="G262" s="7" t="s">
-        <v>1243</v>
+        <v>1241</v>
       </c>
       <c r="H262" s="7" t="s">
-        <v>1244</v>
+        <v>1242</v>
       </c>
       <c r="I262" s="45" t="s">
-        <v>1236</v>
+        <v>1234</v>
       </c>
       <c r="J262" s="7" t="s">
         <v>979</v>
@@ -23585,25 +23579,25 @@
       </c>
       <c r="B263" s="7"/>
       <c r="C263" s="7" t="s">
-        <v>1332</v>
+        <v>1330</v>
       </c>
       <c r="D263" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="E263" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="F263" s="7" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="G263" s="7" t="s">
-        <v>1324</v>
+        <v>1322</v>
       </c>
       <c r="H263" s="7" t="s">
-        <v>1275</v>
+        <v>1273</v>
       </c>
       <c r="I263" s="6" t="s">
-        <v>1276</v>
+        <v>1274</v>
       </c>
       <c r="J263" s="7" t="s">
         <v>979</v>
@@ -23612,7 +23606,7 @@
         <v>6</v>
       </c>
       <c r="L263" s="7" t="s">
-        <v>1336</v>
+        <v>1334</v>
       </c>
       <c r="M263" s="6" t="s">
         <v>8</v>
@@ -23656,22 +23650,22 @@
         <v>875</v>
       </c>
       <c r="D264" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="E264" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="F264" s="40" t="s">
+        <v>1243</v>
+      </c>
+      <c r="G264" s="41" t="s">
+        <v>1244</v>
+      </c>
+      <c r="H264" s="40" t="s">
         <v>1245</v>
       </c>
-      <c r="G264" s="41" t="s">
+      <c r="I264" s="41" t="s">
         <v>1246</v>
-      </c>
-      <c r="H264" s="40" t="s">
-        <v>1247</v>
-      </c>
-      <c r="I264" s="41" t="s">
-        <v>1248</v>
       </c>
       <c r="J264" s="40" t="s">
         <v>806</v>
@@ -23680,16 +23674,16 @@
         <v>231</v>
       </c>
       <c r="L264" s="40" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="M264" s="40" t="s">
         <v>8</v>
       </c>
       <c r="N264" s="41" t="s">
-        <v>1250</v>
+        <v>1248</v>
       </c>
       <c r="O264" s="40" t="s">
-        <v>1251</v>
+        <v>1249</v>
       </c>
       <c r="P264" s="40"/>
       <c r="Q264" s="40" t="s">
@@ -23730,22 +23724,22 @@
         <v>875</v>
       </c>
       <c r="D265" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="E265" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="F265" s="41" t="s">
+        <v>1250</v>
+      </c>
+      <c r="G265" s="41" t="s">
+        <v>1250</v>
+      </c>
+      <c r="H265" s="47" t="s">
+        <v>1251</v>
+      </c>
+      <c r="I265" s="41" t="s">
         <v>1252</v>
-      </c>
-      <c r="G265" s="41" t="s">
-        <v>1252</v>
-      </c>
-      <c r="H265" s="47" t="s">
-        <v>1253</v>
-      </c>
-      <c r="I265" s="41" t="s">
-        <v>1254</v>
       </c>
       <c r="J265" s="41" t="s">
         <v>1050</v>
@@ -23754,16 +23748,16 @@
         <v>231</v>
       </c>
       <c r="L265" s="40" t="s">
-        <v>1249</v>
+        <v>1247</v>
       </c>
       <c r="M265" s="40" t="s">
         <v>8</v>
       </c>
       <c r="N265" s="41" t="s">
-        <v>1255</v>
+        <v>1253</v>
       </c>
       <c r="O265" s="40" t="s">
-        <v>1256</v>
+        <v>1254</v>
       </c>
       <c r="P265" s="40"/>
       <c r="Q265" s="40" t="s">
@@ -23804,22 +23798,22 @@
         <v>875</v>
       </c>
       <c r="D266" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="E266" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="F266" s="40" t="s">
+        <v>1255</v>
+      </c>
+      <c r="G266" s="41" t="s">
+        <v>1256</v>
+      </c>
+      <c r="H266" s="47" t="s">
         <v>1257</v>
       </c>
-      <c r="G266" s="41" t="s">
+      <c r="I266" s="41" t="s">
         <v>1258</v>
-      </c>
-      <c r="H266" s="47" t="s">
-        <v>1259</v>
-      </c>
-      <c r="I266" s="41" t="s">
-        <v>1260</v>
       </c>
       <c r="J266" s="40" t="s">
         <v>806</v>
@@ -23834,10 +23828,10 @@
         <v>8</v>
       </c>
       <c r="N266" s="41" t="s">
-        <v>1261</v>
+        <v>1259</v>
       </c>
       <c r="O266" s="40" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="P266" s="40"/>
       <c r="Q266" s="40" t="s">
@@ -23878,22 +23872,22 @@
         <v>875</v>
       </c>
       <c r="D267" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="E267" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="F267" s="41" t="s">
+        <v>1261</v>
+      </c>
+      <c r="G267" s="41" t="s">
+        <v>1261</v>
+      </c>
+      <c r="H267" s="47" t="s">
+        <v>1262</v>
+      </c>
+      <c r="I267" s="41" t="s">
         <v>1263</v>
-      </c>
-      <c r="G267" s="41" t="s">
-        <v>1263</v>
-      </c>
-      <c r="H267" s="47" t="s">
-        <v>1264</v>
-      </c>
-      <c r="I267" s="41" t="s">
-        <v>1265</v>
       </c>
       <c r="J267" s="40" t="s">
         <v>979</v>
@@ -23908,10 +23902,10 @@
         <v>8</v>
       </c>
       <c r="N267" s="40" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="O267" s="40" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="P267" s="40"/>
       <c r="Q267" s="40" t="s">
@@ -23952,22 +23946,22 @@
         <v>875</v>
       </c>
       <c r="D268" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="E268" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="F268" s="40" t="s">
+        <v>1264</v>
+      </c>
+      <c r="G268" s="41" t="s">
+        <v>1265</v>
+      </c>
+      <c r="H268" s="47" t="s">
         <v>1266</v>
       </c>
-      <c r="G268" s="41" t="s">
+      <c r="I268" s="41" t="s">
         <v>1267</v>
-      </c>
-      <c r="H268" s="47" t="s">
-        <v>1268</v>
-      </c>
-      <c r="I268" s="41" t="s">
-        <v>1269</v>
       </c>
       <c r="J268" s="40" t="s">
         <v>806</v>
@@ -23982,14 +23976,14 @@
         <v>8</v>
       </c>
       <c r="N268" s="41" t="s">
-        <v>1270</v>
+        <v>1268</v>
       </c>
       <c r="O268" s="40" t="s">
-        <v>1271</v>
+        <v>1269</v>
       </c>
       <c r="P268" s="40"/>
       <c r="Q268" s="40" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="R268" s="7">
         <v>0</v>
@@ -24026,22 +24020,22 @@
         <v>875</v>
       </c>
       <c r="D269" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="E269" s="40" t="s">
-        <v>1188</v>
+        <v>1186</v>
       </c>
       <c r="F269" s="41" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="G269" s="41" t="s">
-        <v>1273</v>
+        <v>1271</v>
       </c>
       <c r="H269" s="47" t="s">
-        <v>1264</v>
+        <v>1262</v>
       </c>
       <c r="I269" s="41" t="s">
-        <v>1274</v>
+        <v>1272</v>
       </c>
       <c r="J269" s="40" t="s">
         <v>979</v>
@@ -24056,14 +24050,14 @@
         <v>8</v>
       </c>
       <c r="N269" s="40" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="O269" s="40" t="s">
-        <v>1262</v>
+        <v>1260</v>
       </c>
       <c r="P269" s="40"/>
       <c r="Q269" s="40" t="s">
-        <v>1272</v>
+        <v>1270</v>
       </c>
       <c r="R269" s="7">
         <v>0</v>
@@ -24133,7 +24127,7 @@
         <v>333</v>
       </c>
       <c r="B2" s="53" t="s">
-        <v>1333</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="17.25" customHeight="1">
@@ -24149,7 +24143,7 @@
         <v>732</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1328</v>
+        <v>1326</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1">
@@ -24165,7 +24159,7 @@
         <v>336</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1331</v>
+        <v>1329</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" customHeight="1">
@@ -24173,7 +24167,7 @@
         <v>337</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1330</v>
+        <v>1328</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="17.25" customHeight="1">
@@ -24245,7 +24239,7 @@
         <v>346</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1334</v>
+        <v>1332</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="17.25" customHeight="1">
@@ -24298,10 +24292,10 @@
     </row>
     <row r="23" spans="1:2" ht="17.25" customHeight="1">
       <c r="A23" s="13" t="s">
-        <v>1309</v>
+        <v>1307</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>1329</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="17.25" customHeight="1">

</xml_diff>

<commit_message>
Act salud ech 2020 y 2021
</commit_message>
<xml_diff>
--- a/Data/Base_fichas_indicadores.xlsx
+++ b/Data/Base_fichas_indicadores.xlsx
@@ -4659,10 +4659,10 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AK269"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A136" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="J1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E111" sqref="E111"/>
-      <selection pane="bottomLeft" activeCell="Q159" sqref="Q159"/>
+      <selection pane="bottomLeft" activeCell="O112" sqref="O112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -11986,16 +11986,16 @@
         <v>6</v>
       </c>
       <c r="L100" s="6" t="s">
-        <v>7</v>
+        <v>966</v>
       </c>
       <c r="M100" s="6" t="s">
         <v>8</v>
       </c>
       <c r="N100" s="6" t="s">
-        <v>9</v>
+        <v>1335</v>
       </c>
       <c r="O100" s="6" t="s">
-        <v>187</v>
+        <v>1336</v>
       </c>
       <c r="P100" s="6"/>
       <c r="Q100" s="6" t="s">

</xml_diff>

<commit_message>
Act ss nna ech 2020 2021
</commit_message>
<xml_diff>
--- a/Data/Base_fichas_indicadores.xlsx
+++ b/Data/Base_fichas_indicadores.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3908" uniqueCount="1341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3916" uniqueCount="1342">
   <si>
     <t>id</t>
   </si>
@@ -4079,6 +4079,9 @@
   </si>
   <si>
     <t>El indicador mide el porcentaje de ocupados que trabajan más de 40 horas semanales y perciben un salario inferior a la línea de pobreza individual.</t>
+  </si>
+  <si>
+    <t>NNA</t>
   </si>
 </sst>
 </file>
@@ -4659,10 +4662,10 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AK269"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="J1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A94" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="K1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E111" sqref="E111"/>
-      <selection pane="bottomLeft" activeCell="O112" sqref="O112"/>
+      <selection pane="bottomLeft" activeCell="N82" sqref="N82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -9583,7 +9586,9 @@
       <c r="B69" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C69" s="18"/>
+      <c r="C69" s="18" t="s">
+        <v>1341</v>
+      </c>
       <c r="D69" s="18" t="s">
         <v>2</v>
       </c>
@@ -9664,7 +9669,9 @@
       <c r="B70" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C70" s="18"/>
+      <c r="C70" s="18" t="s">
+        <v>1341</v>
+      </c>
       <c r="D70" s="18" t="s">
         <v>2</v>
       </c>
@@ -9690,16 +9697,16 @@
         <v>6</v>
       </c>
       <c r="L70" s="7" t="s">
-        <v>39</v>
+        <v>1275</v>
       </c>
       <c r="M70" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="N70" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="O70" s="7" t="s">
-        <v>187</v>
+      <c r="N70" s="6" t="s">
+        <v>1335</v>
+      </c>
+      <c r="O70" s="6" t="s">
+        <v>1336</v>
       </c>
       <c r="P70" s="7"/>
       <c r="Q70" s="7" t="s">
@@ -9745,7 +9752,9 @@
       <c r="B71" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C71" s="18"/>
+      <c r="C71" s="18" t="s">
+        <v>1341</v>
+      </c>
       <c r="D71" s="18" t="s">
         <v>2</v>
       </c>
@@ -9771,16 +9780,16 @@
         <v>6</v>
       </c>
       <c r="L71" s="7" t="s">
-        <v>225</v>
+        <v>321</v>
       </c>
       <c r="M71" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="N71" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="O71" s="7" t="s">
-        <v>187</v>
+      <c r="N71" s="6" t="s">
+        <v>1335</v>
+      </c>
+      <c r="O71" s="6" t="s">
+        <v>1336</v>
       </c>
       <c r="P71" s="7"/>
       <c r="Q71" s="7" t="s">
@@ -9825,7 +9834,9 @@
       <c r="B72" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C72" s="18"/>
+      <c r="C72" s="18" t="s">
+        <v>1341</v>
+      </c>
       <c r="D72" s="18" t="s">
         <v>2</v>
       </c>
@@ -9851,16 +9862,16 @@
         <v>6</v>
       </c>
       <c r="L72" s="7" t="s">
-        <v>225</v>
+        <v>321</v>
       </c>
       <c r="M72" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="N72" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="O72" s="7" t="s">
-        <v>187</v>
+      <c r="N72" s="6" t="s">
+        <v>1335</v>
+      </c>
+      <c r="O72" s="6" t="s">
+        <v>1336</v>
       </c>
       <c r="P72" s="7"/>
       <c r="Q72" s="7" t="s">
@@ -9906,7 +9917,9 @@
       <c r="B73" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C73" s="18"/>
+      <c r="C73" s="18" t="s">
+        <v>1341</v>
+      </c>
       <c r="D73" s="18" t="s">
         <v>2</v>
       </c>
@@ -9932,16 +9945,16 @@
         <v>6</v>
       </c>
       <c r="L73" s="7" t="s">
-        <v>225</v>
+        <v>321</v>
       </c>
       <c r="M73" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="N73" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="O73" s="7" t="s">
-        <v>187</v>
+      <c r="N73" s="6" t="s">
+        <v>1335</v>
+      </c>
+      <c r="O73" s="6" t="s">
+        <v>1336</v>
       </c>
       <c r="P73" s="7"/>
       <c r="Q73" s="7" t="s">
@@ -9987,7 +10000,9 @@
       <c r="B74" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C74" s="18"/>
+      <c r="C74" s="18" t="s">
+        <v>1341</v>
+      </c>
       <c r="D74" s="18" t="s">
         <v>2</v>
       </c>
@@ -10013,16 +10028,16 @@
         <v>6</v>
       </c>
       <c r="L74" s="7" t="s">
-        <v>225</v>
+        <v>321</v>
       </c>
       <c r="M74" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="N74" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="O74" s="7" t="s">
-        <v>187</v>
+      <c r="N74" s="6" t="s">
+        <v>1335</v>
+      </c>
+      <c r="O74" s="6" t="s">
+        <v>1336</v>
       </c>
       <c r="P74" s="7"/>
       <c r="Q74" s="7" t="s">
@@ -10068,7 +10083,9 @@
       <c r="B75" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C75" s="18"/>
+      <c r="C75" s="18" t="s">
+        <v>1341</v>
+      </c>
       <c r="D75" s="18" t="s">
         <v>2</v>
       </c>
@@ -10094,16 +10111,16 @@
         <v>6</v>
       </c>
       <c r="L75" s="7" t="s">
-        <v>7</v>
+        <v>966</v>
       </c>
       <c r="M75" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="N75" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="O75" s="7" t="s">
-        <v>187</v>
+      <c r="N75" s="6" t="s">
+        <v>1335</v>
+      </c>
+      <c r="O75" s="6" t="s">
+        <v>1336</v>
       </c>
       <c r="P75" s="7"/>
       <c r="Q75" s="7" t="s">
@@ -10149,7 +10166,9 @@
       <c r="B76" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="C76" s="18"/>
+      <c r="C76" s="18" t="s">
+        <v>1341</v>
+      </c>
       <c r="D76" s="18" t="s">
         <v>2</v>
       </c>
@@ -10175,16 +10194,16 @@
         <v>6</v>
       </c>
       <c r="L76" s="7" t="s">
-        <v>7</v>
+        <v>966</v>
       </c>
       <c r="M76" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="N76" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="O76" s="7" t="s">
-        <v>187</v>
+      <c r="N76" s="6" t="s">
+        <v>1335</v>
+      </c>
+      <c r="O76" s="6" t="s">
+        <v>1336</v>
       </c>
       <c r="P76" s="7"/>
       <c r="Q76" s="7" t="s">
@@ -10254,17 +10273,17 @@
       <c r="K77" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L77" s="6" t="s">
-        <v>7</v>
+      <c r="L77" s="7" t="s">
+        <v>966</v>
       </c>
       <c r="M77" s="6" t="s">
         <v>8</v>
       </c>
       <c r="N77" s="6" t="s">
-        <v>9</v>
+        <v>1335</v>
       </c>
       <c r="O77" s="6" t="s">
-        <v>187</v>
+        <v>1336</v>
       </c>
       <c r="P77" s="6" t="s">
         <v>54</v>

</xml_diff>

<commit_message>
Scripts R ECH 2020 y 2021
</commit_message>
<xml_diff>
--- a/Data/Base_fichas_indicadores.xlsx
+++ b/Data/Base_fichas_indicadores.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4187" uniqueCount="1349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4187" uniqueCount="1348">
   <si>
     <t>id</t>
   </si>
@@ -4090,19 +4090,23 @@
     <t>OBSERVACIONES</t>
   </si>
   <si>
-    <t>Desde marzo de 2020 hasta junio de 2021 se interrumpió el relevamiento presencial y se aplicó de manera telefónica un cuestionario restringido con el objetivo de continuar publicando los indicadores de ingresos y mercado de trabajo. En ese período la encuesta pasó a ser de paneles rotativos elegidos al azar a partir de los casos respondentes del año anterior. En julio de 2021 el INE retomó la realización de encuestas presenciales, pero introdujo un cambio metodológico, ya que la ECH pasa a ser una encuesta de panel rotativo con periodicidad mensual compuesta por seis paneles o grupos de rotación, cada uno de los cuales es una muestra representativa de la población. Con esta nueva metodología, cada hogar seleccionado participa durante seis meses de la ECH. Para 2021 este indicador se calcula a partir de la encuesta telefónica del primer semestre de 2021 y el formulario presencial de implantación del panel del segundo semestre de 2021.</t>
-  </si>
-  <si>
-    <t>Desde marzo de 2020 hasta junio de 2021 se interrumpió el relevamiento presencial y se aplicó de manera telefónica un cuestionario restringido con el objetivo de continuar publicando los indicadores de ingresos y mercado de trabajo. En ese período la encuesta pasó a ser de paneles rotativos elegidos al azar a partir de los casos respondentes del año anterior. En julio de 2021 el INE retomó la realización de encuestas presenciales, pero introdujo un cambio metodológico, ya que la ECH pasa a ser una encuesta de panel rotativo con periodicidad mensual compuesta por seis paneles o grupos de rotación, cada uno de los cuales es una muestra representativa de la población. Con esta nueva metodología, cada hogar seleccionado participa durante seis meses de la ECH. Para 2021, este indicador se calcula a partir de la encuesta telefónica del primer semestre de 2021 y el formulario de implantación de modalidad panel del segundo semestre de 2021.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Desde marzo de 2020 hasta junio de 2021 se interrumpió el relevamiento presencial y se aplicó de manera telefónica un cuestionario restringido con el objetivo de continuar publicando los indicadores de ingresos y mercado de trabajo. En ese período la encuesta pasó a ser de paneles rotativos elegidos al azar a partir de los casos respondentes del año anterior. En julio de 2021 el INE retomó la realización de encuestas presenciales, pero introdujo un cambio metodológico, ya que la ECH pasa a ser una encuesta de panel rotativo con periodicidad mensual compuesta por seis paneles o grupos de rotación, cada uno de los cuales es una muestra representativa de la población. Con esta nueva metodología, cada hogar seleccionado participa durante seis meses de la ECH. A partir de 2020 cambia el modo de relevar cobertura de salud. Antes de esta fecha se les consultaba a los/as encuestados por cobertura en cada uno de los prestadores posibles. Durante el 2020 y el primer semestre de 2021, se relevó únicamente el principal prestador de salud. En el segundo semestre de 2021 se relevó el prestador principal y secundario, hecho que habilita reconstruir un indicador más próximo al calculado antes de 2019. Para 2021, este indicador se calcula únicamente a partir de la implantación de modalidad panel del segundo semestre de 2021. Dados los cambios metodológicos en la formulación de las preguntas,no se incopora a la serie el año 2020 y tampoco se considera la información del primer semestre de 2021. </t>
-  </si>
-  <si>
     <t>Observaciones del indicador</t>
   </si>
   <si>
-    <t>Desde marzo de 2020 hasta junio de 2021 se interrumpió el relevamiento presencial y se aplicó de manera telefónica un cuestionario restringido con el objetivo de continuar publicando los indicadores de ingresos y mercado de trabajo. En ese período la encuesta pasó a ser de paneles rotativos elegidos al azar a partir de los casos respondentes del año anterior. En julio de 2021 el INE retomó la realización de encuestas presenciales, pero introdujo un cambio metodológico, ya que la ECH pasa a ser una encuesta de panel rotativo con periodicidad mensual compuesta por seis paneles o grupos de rotación, cada uno de los cuales es una muestra representativa de la población. Con esta nueva metodología, cada hogar seleccionado participa durante seis meses de la ECH. Este indicador se calcula a partir de la encuesta telefónica del primer semestre de 2021 y el formulario telefónico de modalidad panel del segundo semestre de 2021. En el segundo semestre, el quintil de ingresos del hogar corresponde a los ingresos declarados durante la implantación del panel en la encuesta presencial.</t>
+    <t>Desde marzo de 2020 hasta junio de 2021 se interrumpió el relevamiento presencial y se aplicó de manera telefónica un cuestionario restringido con el objetivo de continuar publicando los indicadores de ingresos y mercado de trabajo. En ese período la encuesta pasó a ser de paneles rotativos elegidos al azar a partir de los casos respondentes del año anterior. 
+En julio de 2021 el INE retomó la realización de encuestas presenciales, pero introdujo un cambio metodológico, ya que la ECH pasa a ser una encuesta de panel rotativo con periodicidad mensual compuesta por seis paneles o grupos de rotación, cada uno de los cuales es una muestra representativa de la población. Con esta nueva metodología, cada hogar seleccionado participa durante seis meses de la ECH.  
+Para 2020, este indicador se construye con la encuesta presencial hasta marzo de 2020 y, posteriormente, con la encuesta telefónica panel. Para 2021, este indicador se calcula a partir de la encuesta telefónica del primer semestre de 2021 y el formulario telefónico de modalidad panel del segundo semestre de 2021.</t>
+  </si>
+  <si>
+    <t>Desde marzo de 2020 hasta junio de 2021 se interrumpió el relevamiento presencial y se aplicó de manera telefónica un cuestionario restringido con el objetivo de continuar publicando los indicadores de ingresos y mercado de trabajo. En ese período la encuesta pasó a ser de paneles rotativos elegidos al azar a partir de los casos respondentes del año anterior. 
+En julio de 2021 el INE retomó la realización de encuestas presenciales, pero introdujo un cambio metodológico, ya que la ECH pasa a ser una encuesta de panel rotativo con periodicidad mensual compuesta por seis paneles o grupos de rotación, cada uno de los cuales es una muestra representativa de la población. Con esta nueva metodología, cada hogar seleccionado participa durante seis meses de la ECH.  
+Para 2020, este indicador se construye con la encuesta presencial hasta marzo de 2020 y, posteriormente, con la encuesta telefónica panel. Para 2021, este indicador se calcula a partir de la encuesta telefónica del primer semestre de 2021 y el formulario telefónico de modalidad panel del segundo semestre de 2021. En el segundo semestre, el quintil de ingresos del hogar corresponde a los ingresos declarados durante la implantación del panel en la encuesta presencial.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Desde marzo de 2020 hasta junio de 2021 se interrumpió el relevamiento presencial y se aplicó de manera telefónica un cuestionario restringido con el objetivo de continuar publicando los indicadores de ingresos y mercado de trabajo. En ese período la encuesta pasó a ser de paneles rotativos elegidos al azar a partir de los casos respondentes del año anterior. 
+En julio de 2021 el INE retomó la realización de encuestas presenciales, pero introdujo un cambio metodológico, ya que la ECH pasa a ser una encuesta de panel rotativo con periodicidad mensual compuesta por seis paneles o grupos de rotación, cada uno de los cuales es una muestra representativa de la población. Con esta nueva metodología, cada hogar seleccionado participa durante seis meses de la ECH.  
+A partir de 2020 cambia el modo de relevar cobertura de salud. Antes de esta fecha se les consultaba a los/as encuestados por cobertura en cada uno de los prestadores posibles. Durante el 2020 y el primer semestre de 2021, se relevó únicamente el principal prestador de salud. En el segundo semestre de 2021 se relevó el prestador principal y secundario, hecho que habilita reconstruir un indicador más próximo al calculado antes de 2019. 
+Para 2021, este indicador se calcula únicamente a partir de la implantación de modalidad panel del segundo semestre de 2021. Dados los cambios metodológicos en la formulación de las preguntas, no se incorpora a la serie el año 2020 y tampoco se considera la información del primer semestre de 2021. </t>
   </si>
 </sst>
 </file>
@@ -4366,9 +4370,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Normal" xfId="3"/>
@@ -4689,10 +4691,10 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AL274"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="Q1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="R1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E111" sqref="E111"/>
-      <selection pane="bottomLeft" activeCell="R143" sqref="R143:R155"/>
+      <selection pane="bottomLeft" activeCell="R143" sqref="R143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4778,7 +4780,7 @@
       <c r="Q1" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="56" t="s">
         <v>1343</v>
       </c>
       <c r="S1" s="26" t="s">
@@ -7297,8 +7299,8 @@
       <c r="Q35" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R35" s="6" t="s">
-        <v>1342</v>
+      <c r="R35" s="54" t="s">
+        <v>1345</v>
       </c>
       <c r="S35" s="6">
         <v>1</v>
@@ -9430,8 +9432,8 @@
       <c r="Q63" s="13" t="s">
         <v>475</v>
       </c>
-      <c r="R63" s="6" t="s">
-        <v>1342</v>
+      <c r="R63" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S63" s="6">
         <v>1</v>
@@ -9502,8 +9504,8 @@
       <c r="Q64" s="13" t="s">
         <v>475</v>
       </c>
-      <c r="R64" s="6" t="s">
-        <v>1342</v>
+      <c r="R64" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S64" s="6">
         <v>0</v>
@@ -9574,8 +9576,8 @@
       <c r="Q65" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R65" s="6" t="s">
-        <v>1342</v>
+      <c r="R65" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S65" s="6">
         <v>0</v>
@@ -9645,8 +9647,8 @@
       <c r="Q66" s="13" t="s">
         <v>475</v>
       </c>
-      <c r="R66" s="6" t="s">
-        <v>1342</v>
+      <c r="R66" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S66" s="6">
         <v>0</v>
@@ -9716,8 +9718,8 @@
       <c r="Q67" s="13" t="s">
         <v>475</v>
       </c>
-      <c r="R67" s="6" t="s">
-        <v>1342</v>
+      <c r="R67" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S67" s="6">
         <v>1</v>
@@ -9787,8 +9789,8 @@
       <c r="Q68" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R68" s="56" t="s">
-        <v>1344</v>
+      <c r="R68" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S68" s="6">
         <v>0</v>
@@ -9859,8 +9861,8 @@
       <c r="Q69" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R69" s="6" t="s">
-        <v>1342</v>
+      <c r="R69" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S69" s="6">
         <v>1</v>
@@ -9932,8 +9934,8 @@
       <c r="Q70" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R70" s="56" t="s">
-        <v>1345</v>
+      <c r="R70" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S70" s="6">
         <v>0</v>
@@ -10018,8 +10020,8 @@
       <c r="Q71" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R71" s="56" t="s">
-        <v>1345</v>
+      <c r="R71" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S71" s="6">
         <v>0</v>
@@ -10104,8 +10106,8 @@
       <c r="Q72" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R72" s="56" t="s">
-        <v>1345</v>
+      <c r="R72" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S72" s="6">
         <v>0</v>
@@ -10189,8 +10191,8 @@
       <c r="Q73" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R73" s="56" t="s">
-        <v>1345</v>
+      <c r="R73" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S73" s="6">
         <v>0</v>
@@ -10275,8 +10277,8 @@
       <c r="Q74" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R74" s="56" t="s">
-        <v>1345</v>
+      <c r="R74" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S74" s="6">
         <v>0</v>
@@ -10361,8 +10363,8 @@
       <c r="Q75" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R75" s="56" t="s">
-        <v>1345</v>
+      <c r="R75" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S75" s="6">
         <v>1</v>
@@ -10447,8 +10449,8 @@
       <c r="Q76" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R76" s="56" t="s">
-        <v>1345</v>
+      <c r="R76" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S76" s="6">
         <v>0</v>
@@ -10533,8 +10535,8 @@
       <c r="Q77" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R77" s="56" t="s">
-        <v>1345</v>
+      <c r="R77" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S77" s="6">
         <v>0</v>
@@ -10618,8 +10620,8 @@
       <c r="Q78" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R78" s="6" t="s">
-        <v>1342</v>
+      <c r="R78" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S78" s="6">
         <v>0</v>
@@ -10690,8 +10692,8 @@
       <c r="Q79" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R79" s="6" t="s">
-        <v>1342</v>
+      <c r="R79" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S79" s="6">
         <v>0</v>
@@ -10762,8 +10764,8 @@
       <c r="Q80" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R80" s="6" t="s">
-        <v>1342</v>
+      <c r="R80" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S80" s="6">
         <v>0</v>
@@ -10834,8 +10836,8 @@
       <c r="Q81" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R81" s="6" t="s">
-        <v>1342</v>
+      <c r="R81" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S81" s="6">
         <v>0</v>
@@ -10906,8 +10908,8 @@
       <c r="Q82" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R82" s="6" t="s">
-        <v>1342</v>
+      <c r="R82" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S82" s="6">
         <v>1</v>
@@ -10978,8 +10980,8 @@
       <c r="Q83" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R83" s="6" t="s">
-        <v>1342</v>
+      <c r="R83" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S83" s="6">
         <v>0</v>
@@ -11051,8 +11053,8 @@
       <c r="Q84" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R84" s="6" t="s">
-        <v>1342</v>
+      <c r="R84" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S84" s="6">
         <v>0</v>
@@ -11136,8 +11138,8 @@
       <c r="Q85" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R85" s="6" t="s">
-        <v>1342</v>
+      <c r="R85" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S85" s="6">
         <v>0</v>
@@ -11220,8 +11222,8 @@
       <c r="Q86" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R86" s="6" t="s">
-        <v>1342</v>
+      <c r="R86" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S86" s="6">
         <v>0</v>
@@ -11293,8 +11295,8 @@
       <c r="Q87" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R87" s="6" t="s">
-        <v>1342</v>
+      <c r="R87" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S87" s="6">
         <v>0</v>
@@ -11377,8 +11379,8 @@
       <c r="Q88" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R88" s="6" t="s">
-        <v>1342</v>
+      <c r="R88" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S88" s="6">
         <v>0</v>
@@ -11449,8 +11451,8 @@
       <c r="Q89" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R89" s="6" t="s">
-        <v>1342</v>
+      <c r="R89" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S89" s="6">
         <v>0</v>
@@ -11522,8 +11524,8 @@
       <c r="Q90" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R90" s="6" t="s">
-        <v>1342</v>
+      <c r="R90" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S90" s="6">
         <v>0</v>
@@ -12344,8 +12346,8 @@
       <c r="Q100" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="R100" s="56" t="s">
-        <v>1346</v>
+      <c r="R100" s="54" t="s">
+        <v>1347</v>
       </c>
       <c r="S100" s="6">
         <v>1</v>
@@ -15792,8 +15794,8 @@
       <c r="Q143" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="R143" s="6" t="s">
-        <v>1348</v>
+      <c r="R143" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S143" s="44">
         <v>0</v>
@@ -15861,8 +15863,8 @@
       <c r="Q144" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="R144" s="6" t="s">
-        <v>1348</v>
+      <c r="R144" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S144" s="44">
         <v>0</v>
@@ -15930,8 +15932,8 @@
       <c r="Q145" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="R145" s="6" t="s">
-        <v>1348</v>
+      <c r="R145" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S145" s="44">
         <v>0</v>
@@ -15999,8 +16001,8 @@
       <c r="Q146" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="R146" s="6" t="s">
-        <v>1348</v>
+      <c r="R146" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S146" s="44">
         <v>0</v>
@@ -16067,8 +16069,8 @@
       <c r="Q147" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="R147" s="6" t="s">
-        <v>1348</v>
+      <c r="R147" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S147" s="44">
         <v>0</v>
@@ -16138,8 +16140,8 @@
       <c r="Q148" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="R148" s="6" t="s">
-        <v>1348</v>
+      <c r="R148" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S148" s="44">
         <v>0</v>
@@ -16206,8 +16208,8 @@
       <c r="Q149" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="R149" s="6" t="s">
-        <v>1348</v>
+      <c r="R149" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S149" s="44">
         <v>0</v>
@@ -16274,8 +16276,8 @@
       <c r="Q150" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="R150" s="6" t="s">
-        <v>1348</v>
+      <c r="R150" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S150" s="44">
         <v>0</v>
@@ -16342,8 +16344,8 @@
       <c r="Q151" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="R151" s="6" t="s">
-        <v>1348</v>
+      <c r="R151" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S151" s="44">
         <v>0</v>
@@ -16413,8 +16415,8 @@
       <c r="Q152" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="R152" s="6" t="s">
-        <v>1348</v>
+      <c r="R152" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S152" s="44">
         <v>0</v>
@@ -16484,8 +16486,8 @@
       <c r="Q153" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="R153" s="6" t="s">
-        <v>1348</v>
+      <c r="R153" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S153" s="44">
         <v>0</v>
@@ -16552,8 +16554,8 @@
       <c r="Q154" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="R154" s="6" t="s">
-        <v>1348</v>
+      <c r="R154" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S154" s="44">
         <v>0</v>
@@ -16623,8 +16625,8 @@
       <c r="Q155" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="R155" s="6" t="s">
-        <v>1348</v>
+      <c r="R155" s="54" t="s">
+        <v>1346</v>
       </c>
       <c r="S155" s="54">
         <v>0</v>
@@ -25116,7 +25118,7 @@
         <v>1343</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>1347</v>
+        <v>1344</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="17.25" customHeight="1">

</xml_diff>

<commit_message>
Act Observaciones SS, Trabajo y PPL
</commit_message>
<xml_diff>
--- a/Data/Base_fichas_indicadores.xlsx
+++ b/Data/Base_fichas_indicadores.xlsx
@@ -16,14 +16,14 @@
     <sheet name="REF_COLUMNAS" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BASE_FICHAS!$A$1:$AL$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BASE_FICHAS!$A$1:$AL$269</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4187" uniqueCount="1348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4187" uniqueCount="1357">
   <si>
     <t>id</t>
   </si>
@@ -4098,15 +4098,73 @@
 Para 2020, este indicador se construye con la encuesta presencial hasta marzo de 2020 y, posteriormente, con la encuesta telefónica panel. Para 2021, este indicador se calcula a partir de la encuesta telefónica del primer semestre de 2021 y el formulario telefónico de modalidad panel del segundo semestre de 2021.</t>
   </si>
   <si>
-    <t>Desde marzo de 2020 hasta junio de 2021 se interrumpió el relevamiento presencial y se aplicó de manera telefónica un cuestionario restringido con el objetivo de continuar publicando los indicadores de ingresos y mercado de trabajo. En ese período la encuesta pasó a ser de paneles rotativos elegidos al azar a partir de los casos respondentes del año anterior. 
-En julio de 2021 el INE retomó la realización de encuestas presenciales, pero introdujo un cambio metodológico, ya que la ECH pasa a ser una encuesta de panel rotativo con periodicidad mensual compuesta por seis paneles o grupos de rotación, cada uno de los cuales es una muestra representativa de la población. Con esta nueva metodología, cada hogar seleccionado participa durante seis meses de la ECH.  
-Para 2020, este indicador se construye con la encuesta presencial hasta marzo de 2020 y, posteriormente, con la encuesta telefónica panel. Para 2021, este indicador se calcula a partir de la encuesta telefónica del primer semestre de 2021 y el formulario telefónico de modalidad panel del segundo semestre de 2021. En el segundo semestre, el quintil de ingresos del hogar corresponde a los ingresos declarados durante la implantación del panel en la encuesta presencial.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Desde marzo de 2020 hasta junio de 2021 se interrumpió el relevamiento presencial y se aplicó de manera telefónica un cuestionario restringido con el objetivo de continuar publicando los indicadores de ingresos y mercado de trabajo. En ese período la encuesta pasó a ser de paneles rotativos elegidos al azar a partir de los casos respondentes del año anterior. 
 En julio de 2021 el INE retomó la realización de encuestas presenciales, pero introdujo un cambio metodológico, ya que la ECH pasa a ser una encuesta de panel rotativo con periodicidad mensual compuesta por seis paneles o grupos de rotación, cada uno de los cuales es una muestra representativa de la población. Con esta nueva metodología, cada hogar seleccionado participa durante seis meses de la ECH.  
 A partir de 2020 cambia el modo de relevar cobertura de salud. Antes de esta fecha se les consultaba a los/as encuestados por cobertura en cada uno de los prestadores posibles. Durante el 2020 y el primer semestre de 2021, se relevó únicamente el principal prestador de salud. En el segundo semestre de 2021 se relevó el prestador principal y secundario, hecho que habilita reconstruir un indicador más próximo al calculado antes de 2019. 
 Para 2021, este indicador se calcula únicamente a partir de la implantación de modalidad panel del segundo semestre de 2021. Dados los cambios metodológicos en la formulación de las preguntas, no se incorpora a la serie el año 2020 y tampoco se considera la información del primer semestre de 2021. </t>
+  </si>
+  <si>
+    <t>Desde marzo de 2020 hasta junio de 2021 se interrumpió el relevamiento presencial y se aplicó de manera telefónica un cuestionario restringido con el objetivo de continuar publicando los indicadores de ingresos y mercado de trabajo. En ese período la encuesta pasó a ser de paneles rotativos elegidos al azar a partir de los casos respondentes del año anterior. 
+En julio de 2021 el INE retomó la realización de encuestas presenciales, pero introdujo un cambio metodológico, ya que la ECH pasa a ser una encuesta de panel rotativo con periodicidad mensual compuesta por seis paneles o grupos de rotación, cada uno de los cuales es una muestra representativa de la población. Con esta nueva metodología, cada hogar seleccionado participa durante seis meses de la ECH.  
+Los indicadores de trabajo y seguridad social del año 2020 se construyen con la encuesta presencial realizada hasta marzo de 2020 y posteriormente con la encuesta telefónica panel (siempre que la información haya sido incluida en el formulario). Para el 2021, se calculan a partir de la encuesta telefónica del primer semestre de 2021 y el formulario telefónico de modalidad panel del segundo semestre de 2021. En el segundo semestre de 2021 el quintil de ingresos del hogar corresponde a los ingresos declarados durante la implantación del panel en la encuesta presencial.</t>
+  </si>
+  <si>
+    <t>Los datos de 2016 corresponden al mes de octubre.
+Los datos de 2017 corresponden al promedio del tercer trimestre.
+Los datos de 2018 corresponden al promedio de marzo a diciembre.
+Los datos de 2019 corresponden al promedio de marzo a noviembre.
+Los datos de 2020 corresponden al mes de diciembre.
+Los datos de 2021 corresponden al mes de noviembre.</t>
+  </si>
+  <si>
+    <t>Los datos de 2016 corresponden al mes de noviembre.
+Los datos de 2017 corresponden al promedio de los meses de enero, agosto y diciembre.
+Los datos de 2021 corresponden al promedio de los meses de enero a noviembre.</t>
+  </si>
+  <si>
+    <t>Los datos de 2015 corresponden al promedio mayo-diciembre.</t>
+  </si>
+  <si>
+    <t>Los datos de 2010 corresponden a diciembre.
+Los datos de 2011 corresponden a diciembre.
+Los datos de 2012 corresponden a diciembre.
+Los datos de 2013 corresponden a diciembre.
+Los datos de 2014 corresponden a diciembre.
+Los datos de 2015 corresponden a diciembre.</t>
+  </si>
+  <si>
+    <t>Los datos de 2016 corresponden al promedio anual.
+Los datos de 2017 corresponden al promedio anual.
+Los datos de 2018 corresponden al promedio anual.
+Los datos de 2019 corresponden al promedio anual.
+Los datos de 2020 corresponden al promedio anual.
+Los datos de 2021 corresponden al promedio anual.</t>
+  </si>
+  <si>
+    <t>Los datos de 2015 corresponden al promedio mayo - diciembre.
+Para los años 2018 y 2019 desde el CPP se corrigieron las cifras para mejorar la comparabilidad bajo el concepto de plaza habilitada. La corrección refiere a las nuevas plazas de la PPP. En los informes 2018 y 2019 se utilizó la cifra total de lugares nuevos (1960), pero lo cierto es que se fue poblando muy lentamente en la medida en que la unidad se fue dotando gradualmente de personal para hacerla operativa. Se estima un poblamiento de 2/3 de las plazas habilitadas en cada mes, hasta junio de 2019. A partir de Julio de 2019 se toma la capacidad máxima 1860, más las 100 del Centro de Ingreso. El informe 2020 del CPP se hizo en base a la cifra 10.241 que era la revisión de las nuevas autoridades del ministerio de ese entonces. En el 2021 se hizo una nueva revisión que la corrige. Teniendo en cuenta que no hubo cierres ni nuevas plazas que justifiquen un cambio tan abrupto, una posible alternativa es estimar una cifra intermedia entre 2019 y 2021.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Las personas pueden tener actividades en más de un cupo. No hay datos de cantidad de personas con educación no formal.
+Los datos de 2017 corresponden al promedio del tercer trimestre.
+Los datos de 2018 corresponden al promedio de marzo a diciembre.
+Los datos de 2019 corresponden al promedio de marzo a noviembre.
+Los datos de 2020 corresponden al mes de diciembre.
+Los datos de 2021 corresponden al mes de noviembre.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Procesados sin condena incluye procesados bajo CPP 1980 (procesados) y bajo CPP 2017 (preventivas).
+Los datos de 2015 corresponden al promedio mayo a diciembre.
+El 2019 presentó numerosas anomalías (variaciones de un mes a otro) en los reportes mensuales.
+En relación al informe del CPP de 2020 se corrigió error enero-marzo de procesamiento del Ministerio del Interior de procesados en Soriano y Río Negro en Ene-Feb-Mar.
+</t>
+  </si>
+  <si>
+    <t>Procesados sin condena incluye procesados bajo CPP 1980 (procesados) y bajo CPP 2017 (preventivas).
+Los datos de 2015 corresponden al promedio mayo a diciembre.
+El 2019 presentó numerosas anomalías (variaciones de un mes a otro) en los reportes mensuales.
+En relación al informe del CPP de 2020 se corrigió error enero-marzo de procesamiento del Ministerio del Interior de procesados en Soriano y Río Negro en Ene-Feb-Mar.</t>
   </si>
 </sst>
 </file>
@@ -4223,7 +4281,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4358,9 +4416,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -4371,6 +4426,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Excel Built-in Normal" xfId="3"/>
@@ -4691,10 +4750,10 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AL274"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="R1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E111" sqref="E111"/>
-      <selection pane="bottomLeft" activeCell="R143" sqref="R143"/>
+      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4705,17 +4764,18 @@
     <col min="4" max="4" width="36.7109375" style="13" customWidth="1"/>
     <col min="5" max="5" width="37.7109375" style="13" customWidth="1"/>
     <col min="6" max="6" width="94.7109375" style="13" customWidth="1"/>
-    <col min="7" max="7" width="157.28515625" style="13" customWidth="1"/>
-    <col min="8" max="8" width="255.7109375" style="13" customWidth="1"/>
-    <col min="9" max="9" width="181.140625" style="13" customWidth="1"/>
-    <col min="10" max="10" width="59.42578125" style="13" customWidth="1"/>
-    <col min="11" max="11" width="16.140625" style="13" customWidth="1"/>
-    <col min="12" max="12" width="20.42578125" style="13" customWidth="1"/>
-    <col min="13" max="13" width="20.5703125" style="13" customWidth="1"/>
-    <col min="14" max="14" width="57.85546875" style="13" customWidth="1"/>
-    <col min="15" max="15" width="130.42578125" style="13" customWidth="1"/>
-    <col min="16" max="16" width="230.140625" style="13" customWidth="1"/>
-    <col min="17" max="18" width="98.7109375" style="13" customWidth="1"/>
+    <col min="7" max="7" width="157.28515625" style="13" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="255.7109375" style="13" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="181.140625" style="13" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="59.42578125" style="13" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="16.140625" style="13" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="20.42578125" style="13" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="20.5703125" style="13" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="57.85546875" style="13" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="130.42578125" style="13" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="230.140625" style="13" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="98.7109375" style="13" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="98.7109375" style="13" customWidth="1"/>
     <col min="19" max="19" width="15.85546875" style="13" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16.5703125" style="13" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15.85546875" style="13" bestFit="1" customWidth="1"/>
@@ -4780,7 +4840,7 @@
       <c r="Q1" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="R1" s="56" t="s">
+      <c r="R1" s="55" t="s">
         <v>1343</v>
       </c>
       <c r="S1" s="26" t="s">
@@ -7299,7 +7359,7 @@
       <c r="Q35" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R35" s="54" t="s">
+      <c r="R35" s="53" t="s">
         <v>1345</v>
       </c>
       <c r="S35" s="6">
@@ -9396,7 +9456,7 @@
       <c r="E63" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F63" s="30" t="s">
+      <c r="F63" s="56" t="s">
         <v>728</v>
       </c>
       <c r="G63" s="6" t="s">
@@ -9432,8 +9492,8 @@
       <c r="Q63" s="13" t="s">
         <v>475</v>
       </c>
-      <c r="R63" s="54" t="s">
-        <v>1346</v>
+      <c r="R63" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S63" s="6">
         <v>1</v>
@@ -9504,8 +9564,8 @@
       <c r="Q64" s="13" t="s">
         <v>475</v>
       </c>
-      <c r="R64" s="54" t="s">
-        <v>1346</v>
+      <c r="R64" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S64" s="6">
         <v>0</v>
@@ -9576,8 +9636,8 @@
       <c r="Q65" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R65" s="54" t="s">
-        <v>1346</v>
+      <c r="R65" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S65" s="6">
         <v>0</v>
@@ -9647,8 +9707,8 @@
       <c r="Q66" s="13" t="s">
         <v>475</v>
       </c>
-      <c r="R66" s="54" t="s">
-        <v>1346</v>
+      <c r="R66" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S66" s="6">
         <v>0</v>
@@ -9718,8 +9778,8 @@
       <c r="Q67" s="13" t="s">
         <v>475</v>
       </c>
-      <c r="R67" s="54" t="s">
-        <v>1346</v>
+      <c r="R67" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S67" s="6">
         <v>1</v>
@@ -9789,8 +9849,8 @@
       <c r="Q68" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R68" s="54" t="s">
-        <v>1346</v>
+      <c r="R68" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S68" s="6">
         <v>0</v>
@@ -9861,8 +9921,8 @@
       <c r="Q69" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R69" s="54" t="s">
-        <v>1346</v>
+      <c r="R69" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S69" s="6">
         <v>1</v>
@@ -9934,8 +9994,8 @@
       <c r="Q70" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R70" s="54" t="s">
-        <v>1346</v>
+      <c r="R70" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S70" s="6">
         <v>0</v>
@@ -10020,8 +10080,8 @@
       <c r="Q71" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R71" s="54" t="s">
-        <v>1346</v>
+      <c r="R71" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S71" s="6">
         <v>0</v>
@@ -10106,8 +10166,8 @@
       <c r="Q72" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R72" s="54" t="s">
-        <v>1346</v>
+      <c r="R72" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S72" s="6">
         <v>0</v>
@@ -10191,8 +10251,8 @@
       <c r="Q73" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R73" s="54" t="s">
-        <v>1346</v>
+      <c r="R73" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S73" s="6">
         <v>0</v>
@@ -10277,8 +10337,8 @@
       <c r="Q74" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R74" s="54" t="s">
-        <v>1346</v>
+      <c r="R74" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S74" s="6">
         <v>0</v>
@@ -10363,8 +10423,8 @@
       <c r="Q75" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R75" s="54" t="s">
-        <v>1346</v>
+      <c r="R75" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S75" s="6">
         <v>1</v>
@@ -10449,8 +10509,8 @@
       <c r="Q76" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R76" s="54" t="s">
-        <v>1346</v>
+      <c r="R76" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S76" s="6">
         <v>0</v>
@@ -10535,8 +10595,8 @@
       <c r="Q77" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R77" s="54" t="s">
-        <v>1346</v>
+      <c r="R77" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S77" s="6">
         <v>0</v>
@@ -10620,8 +10680,8 @@
       <c r="Q78" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R78" s="54" t="s">
-        <v>1346</v>
+      <c r="R78" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S78" s="6">
         <v>0</v>
@@ -10692,8 +10752,8 @@
       <c r="Q79" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R79" s="54" t="s">
-        <v>1346</v>
+      <c r="R79" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S79" s="6">
         <v>0</v>
@@ -10764,8 +10824,8 @@
       <c r="Q80" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R80" s="54" t="s">
-        <v>1346</v>
+      <c r="R80" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S80" s="6">
         <v>0</v>
@@ -10836,8 +10896,8 @@
       <c r="Q81" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R81" s="54" t="s">
-        <v>1346</v>
+      <c r="R81" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S81" s="6">
         <v>0</v>
@@ -10908,8 +10968,8 @@
       <c r="Q82" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R82" s="54" t="s">
-        <v>1346</v>
+      <c r="R82" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S82" s="6">
         <v>1</v>
@@ -10980,8 +11040,8 @@
       <c r="Q83" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R83" s="54" t="s">
-        <v>1346</v>
+      <c r="R83" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S83" s="6">
         <v>0</v>
@@ -11053,8 +11113,8 @@
       <c r="Q84" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R84" s="54" t="s">
-        <v>1346</v>
+      <c r="R84" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S84" s="6">
         <v>0</v>
@@ -11138,8 +11198,8 @@
       <c r="Q85" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R85" s="54" t="s">
-        <v>1346</v>
+      <c r="R85" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S85" s="6">
         <v>0</v>
@@ -11222,8 +11282,8 @@
       <c r="Q86" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R86" s="54" t="s">
-        <v>1346</v>
+      <c r="R86" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S86" s="6">
         <v>0</v>
@@ -11295,8 +11355,8 @@
       <c r="Q87" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R87" s="54" t="s">
-        <v>1346</v>
+      <c r="R87" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S87" s="6">
         <v>0</v>
@@ -11379,8 +11439,8 @@
       <c r="Q88" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R88" s="54" t="s">
-        <v>1346</v>
+      <c r="R88" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S88" s="6">
         <v>0</v>
@@ -11451,8 +11511,8 @@
       <c r="Q89" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R89" s="54" t="s">
-        <v>1346</v>
+      <c r="R89" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S89" s="6">
         <v>0</v>
@@ -11524,8 +11584,8 @@
       <c r="Q90" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R90" s="54" t="s">
-        <v>1346</v>
+      <c r="R90" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S90" s="6">
         <v>0</v>
@@ -12346,8 +12406,8 @@
       <c r="Q100" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="R100" s="54" t="s">
-        <v>1347</v>
+      <c r="R100" s="53" t="s">
+        <v>1346</v>
       </c>
       <c r="S100" s="6">
         <v>1</v>
@@ -15767,7 +15827,7 @@
       <c r="G143" s="7" t="s">
         <v>1098</v>
       </c>
-      <c r="H143" s="52" t="s">
+      <c r="H143" s="7" t="s">
         <v>1290</v>
       </c>
       <c r="I143" s="6" t="s">
@@ -15794,8 +15854,8 @@
       <c r="Q143" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="R143" s="54" t="s">
-        <v>1346</v>
+      <c r="R143" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S143" s="44">
         <v>0</v>
@@ -15863,8 +15923,8 @@
       <c r="Q144" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="R144" s="54" t="s">
-        <v>1346</v>
+      <c r="R144" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S144" s="44">
         <v>0</v>
@@ -15932,8 +15992,8 @@
       <c r="Q145" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="R145" s="54" t="s">
-        <v>1346</v>
+      <c r="R145" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S145" s="44">
         <v>0</v>
@@ -16001,8 +16061,8 @@
       <c r="Q146" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="R146" s="54" t="s">
-        <v>1346</v>
+      <c r="R146" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S146" s="44">
         <v>0</v>
@@ -16069,8 +16129,8 @@
       <c r="Q147" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="R147" s="54" t="s">
-        <v>1346</v>
+      <c r="R147" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S147" s="44">
         <v>0</v>
@@ -16140,8 +16200,8 @@
       <c r="Q148" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="R148" s="54" t="s">
-        <v>1346</v>
+      <c r="R148" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S148" s="44">
         <v>0</v>
@@ -16208,8 +16268,8 @@
       <c r="Q149" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="R149" s="54" t="s">
-        <v>1346</v>
+      <c r="R149" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S149" s="44">
         <v>0</v>
@@ -16276,8 +16336,8 @@
       <c r="Q150" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="R150" s="54" t="s">
-        <v>1346</v>
+      <c r="R150" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S150" s="44">
         <v>0</v>
@@ -16344,8 +16404,8 @@
       <c r="Q151" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="R151" s="54" t="s">
-        <v>1346</v>
+      <c r="R151" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S151" s="44">
         <v>0</v>
@@ -16415,8 +16475,8 @@
       <c r="Q152" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="R152" s="54" t="s">
-        <v>1346</v>
+      <c r="R152" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S152" s="44">
         <v>0</v>
@@ -16486,8 +16546,8 @@
       <c r="Q153" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="R153" s="54" t="s">
-        <v>1346</v>
+      <c r="R153" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S153" s="44">
         <v>0</v>
@@ -16554,8 +16614,8 @@
       <c r="Q154" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="R154" s="54" t="s">
-        <v>1346</v>
+      <c r="R154" s="57" t="s">
+        <v>1347</v>
       </c>
       <c r="S154" s="44">
         <v>0</v>
@@ -16576,8 +16636,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:24" s="54" customFormat="1">
-      <c r="A155" s="54">
+    <row r="155" spans="1:24" s="53" customFormat="1">
+      <c r="A155" s="53">
         <v>530209</v>
       </c>
       <c r="B155" s="44" t="s">
@@ -16586,10 +16646,10 @@
       <c r="D155" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="E155" s="54" t="s">
+      <c r="E155" s="53" t="s">
         <v>15</v>
       </c>
-      <c r="F155" s="54" t="s">
+      <c r="F155" s="53" t="s">
         <v>1114</v>
       </c>
       <c r="G155" s="44" t="s">
@@ -16625,25 +16685,25 @@
       <c r="Q155" s="6" t="s">
         <v>475</v>
       </c>
-      <c r="R155" s="54" t="s">
-        <v>1346</v>
-      </c>
-      <c r="S155" s="54">
-        <v>0</v>
-      </c>
-      <c r="T155" s="54">
-        <v>0</v>
-      </c>
-      <c r="U155" s="54">
-        <v>0</v>
-      </c>
-      <c r="V155" s="54">
-        <v>0</v>
-      </c>
-      <c r="W155" s="54">
-        <v>0</v>
-      </c>
-      <c r="X155" s="54">
+      <c r="R155" s="57" t="s">
+        <v>1347</v>
+      </c>
+      <c r="S155" s="53">
+        <v>0</v>
+      </c>
+      <c r="T155" s="53">
+        <v>0</v>
+      </c>
+      <c r="U155" s="53">
+        <v>0</v>
+      </c>
+      <c r="V155" s="53">
+        <v>0</v>
+      </c>
+      <c r="W155" s="53">
+        <v>0</v>
+      </c>
+      <c r="X155" s="53">
         <v>0</v>
       </c>
     </row>
@@ -22675,7 +22735,7 @@
         <v>17</v>
       </c>
       <c r="R239" s="6" t="s">
-        <v>1342</v>
+        <v>1354</v>
       </c>
       <c r="S239" s="44">
         <v>0</v>
@@ -22747,7 +22807,7 @@
         <v>17</v>
       </c>
       <c r="R240" s="6" t="s">
-        <v>1342</v>
+        <v>1348</v>
       </c>
       <c r="S240" s="44">
         <v>0</v>
@@ -22820,7 +22880,7 @@
         <v>17</v>
       </c>
       <c r="R241" s="6" t="s">
-        <v>1342</v>
+        <v>1348</v>
       </c>
       <c r="S241" s="44">
         <v>0</v>
@@ -22893,7 +22953,7 @@
         <v>17</v>
       </c>
       <c r="R242" s="6" t="s">
-        <v>1342</v>
+        <v>1353</v>
       </c>
       <c r="S242" s="44">
         <v>0</v>
@@ -23122,7 +23182,7 @@
         <v>17</v>
       </c>
       <c r="R245" s="6" t="s">
-        <v>1342</v>
+        <v>1349</v>
       </c>
       <c r="S245" s="44">
         <v>0</v>
@@ -23195,7 +23255,7 @@
         <v>17</v>
       </c>
       <c r="R246" s="6" t="s">
-        <v>1342</v>
+        <v>1349</v>
       </c>
       <c r="S246" s="44">
         <v>0</v>
@@ -24527,7 +24587,7 @@
         <v>17</v>
       </c>
       <c r="R264" s="6" t="s">
-        <v>1342</v>
+        <v>1350</v>
       </c>
       <c r="S264" s="7">
         <v>0</v>
@@ -24604,7 +24664,7 @@
         <v>17</v>
       </c>
       <c r="R265" s="6" t="s">
-        <v>1342</v>
+        <v>1350</v>
       </c>
       <c r="S265" s="7">
         <v>0</v>
@@ -24681,7 +24741,7 @@
         <v>208</v>
       </c>
       <c r="R266" s="6" t="s">
-        <v>1342</v>
+        <v>1351</v>
       </c>
       <c r="S266" s="7">
         <v>0</v>
@@ -24758,7 +24818,7 @@
         <v>208</v>
       </c>
       <c r="R267" s="6" t="s">
-        <v>1342</v>
+        <v>1352</v>
       </c>
       <c r="S267" s="7">
         <v>0</v>
@@ -24835,7 +24895,7 @@
         <v>1270</v>
       </c>
       <c r="R268" s="6" t="s">
-        <v>1342</v>
+        <v>1355</v>
       </c>
       <c r="S268" s="7">
         <v>0</v>
@@ -24912,7 +24972,7 @@
         <v>1270</v>
       </c>
       <c r="R269" s="6" t="s">
-        <v>1342</v>
+        <v>1356</v>
       </c>
       <c r="S269" s="7">
         <v>0</v>
@@ -24941,8 +25001,8 @@
       <c r="AL269" s="13"/>
     </row>
     <row r="273" spans="6:7">
-      <c r="F273" s="55"/>
-      <c r="G273" s="55"/>
+      <c r="F273" s="54"/>
+      <c r="G273" s="54"/>
     </row>
     <row r="274" spans="6:7">
       <c r="F274" s="7"/>
@@ -24950,11 +25010,7 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <autoFilter ref="A1:AL1">
-    <sortState ref="A2:AK269">
-      <sortCondition ref="A1"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:AL269"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -24989,7 +25045,7 @@
       <c r="A2" s="26" t="s">
         <v>333</v>
       </c>
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="52" t="s">
         <v>1331</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Rev ind ambiente Add ícono conindicador
</commit_message>
<xml_diff>
--- a/Data/Base_fichas_indicadores.xlsx
+++ b/Data/Base_fichas_indicadores.xlsx
@@ -4738,10 +4738,10 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AL274"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="K1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E111" sqref="E111"/>
-      <selection pane="bottomLeft" activeCell="N41" sqref="N41:N43"/>
+      <selection pane="bottomLeft" activeCell="A162" sqref="A162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Corr ind PPL Mod Tablas: 1er condicional fecha_cat (en t y ss add | lista_serie_cat)
</commit_message>
<xml_diff>
--- a/Data/Base_fichas_indicadores.xlsx
+++ b/Data/Base_fichas_indicadores.xlsx
@@ -4093,11 +4093,6 @@
 Los datos de 2021 corresponden al mes de noviembre.</t>
   </si>
   <si>
-    <t>Los datos de 2016 corresponden al mes de noviembre.
-Los datos de 2017 corresponden al promedio de los meses de enero, agosto y diciembre.
-Los datos de 2021 corresponden al promedio de los meses de enero a noviembre.</t>
-  </si>
-  <si>
     <t>Los datos de 2015 corresponden al promedio mayo-diciembre.</t>
   </si>
   <si>
@@ -4153,6 +4148,12 @@
   </si>
   <si>
     <t>UMAD con base en Memoria Anual Ministerio de Vivienda 2019</t>
+  </si>
+  <si>
+    <t>Los datos de 2016 corresponden al mes de noviembre.
+Los datos de 2017 corresponden al promedio de los meses de enero, agosto y diciembre.
+Los datos de 2019 corresponden al promedio de los meses de enero a noviembre.
+Los datos de 2021 corresponden al promedio de los meses de enero a noviembre.</t>
   </si>
 </sst>
 </file>
@@ -4269,7 +4270,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4417,6 +4418,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -4738,10 +4743,10 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AL274"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="R1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A136" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E111" sqref="E111"/>
-      <selection pane="bottomLeft" activeCell="A162" sqref="A162"/>
+      <selection pane="bottomLeft" activeCell="R159" sqref="A159:XFD159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4751,7 +4756,7 @@
     <col min="3" max="3" width="41.85546875" style="13" customWidth="1"/>
     <col min="4" max="4" width="36.7109375" style="13" customWidth="1"/>
     <col min="5" max="5" width="37.7109375" style="13" customWidth="1"/>
-    <col min="6" max="6" width="94.7109375" style="13" customWidth="1"/>
+    <col min="6" max="6" width="126.5703125" style="13" customWidth="1"/>
     <col min="7" max="7" width="157.28515625" style="13" customWidth="1"/>
     <col min="8" max="8" width="255.7109375" style="13" customWidth="1"/>
     <col min="9" max="9" width="181.140625" style="13" customWidth="1"/>
@@ -7757,7 +7762,7 @@
         <v>311</v>
       </c>
       <c r="O41" s="6" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="P41" s="6"/>
       <c r="Q41" s="6" t="s">
@@ -7840,7 +7845,7 @@
         <v>311</v>
       </c>
       <c r="O42" s="6" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="P42" s="25"/>
       <c r="Q42" s="6" t="s">
@@ -7923,7 +7928,7 @@
         <v>311</v>
       </c>
       <c r="O43" s="6" t="s">
-        <v>1352</v>
+        <v>1351</v>
       </c>
       <c r="P43" s="25"/>
       <c r="Q43" s="6" t="s">
@@ -10211,7 +10216,7 @@
         <v>658</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>1350</v>
+        <v>1349</v>
       </c>
       <c r="I73" s="7" t="s">
         <v>690</v>
@@ -10383,7 +10388,7 @@
         <v>662</v>
       </c>
       <c r="H75" s="6" t="s">
-        <v>1351</v>
+        <v>1350</v>
       </c>
       <c r="I75" s="7" t="s">
         <v>692</v>
@@ -20244,7 +20249,7 @@
         <v>1300</v>
       </c>
       <c r="H206" s="7" t="s">
-        <v>1349</v>
+        <v>1348</v>
       </c>
       <c r="I206" s="7" t="s">
         <v>916</v>
@@ -22722,7 +22727,7 @@
         <v>17</v>
       </c>
       <c r="R239" s="6" t="s">
-        <v>1346</v>
+        <v>1345</v>
       </c>
       <c r="S239" s="44">
         <v>0</v>
@@ -22940,7 +22945,7 @@
         <v>17</v>
       </c>
       <c r="R242" s="6" t="s">
-        <v>1345</v>
+        <v>1344</v>
       </c>
       <c r="S242" s="44">
         <v>0</v>
@@ -23122,54 +23127,54 @@
       <c r="A245" s="50">
         <v>94530116</v>
       </c>
-      <c r="B245" s="40" t="s">
+      <c r="B245" s="58" t="s">
         <v>992</v>
       </c>
-      <c r="C245" s="40" t="s">
+      <c r="C245" s="58" t="s">
         <v>868</v>
       </c>
-      <c r="D245" s="40" t="s">
+      <c r="D245" s="58" t="s">
         <v>2</v>
       </c>
       <c r="E245" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F245" s="41" t="s">
+      <c r="F245" s="11" t="s">
         <v>1059</v>
       </c>
-      <c r="G245" s="42" t="s">
+      <c r="G245" s="59" t="s">
         <v>1060</v>
       </c>
-      <c r="H245" s="42" t="s">
+      <c r="H245" s="59" t="s">
         <v>1061</v>
       </c>
-      <c r="I245" s="42" t="s">
+      <c r="I245" s="59" t="s">
         <v>1062</v>
       </c>
-      <c r="J245" s="40" t="s">
+      <c r="J245" s="58" t="s">
         <v>799</v>
       </c>
-      <c r="K245" s="40" t="s">
+      <c r="K245" s="58" t="s">
         <v>231</v>
       </c>
-      <c r="L245" s="40" t="s">
+      <c r="L245" s="58" t="s">
         <v>924</v>
       </c>
-      <c r="M245" s="40" t="s">
+      <c r="M245" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="N245" s="40" t="s">
+      <c r="N245" s="58" t="s">
         <v>875</v>
       </c>
-      <c r="O245" s="40" t="s">
+      <c r="O245" s="58" t="s">
         <v>876</v>
       </c>
-      <c r="P245" s="40"/>
-      <c r="Q245" s="40" t="s">
+      <c r="P245" s="58"/>
+      <c r="Q245" s="58" t="s">
         <v>17</v>
       </c>
       <c r="R245" s="6" t="s">
-        <v>1341</v>
+        <v>1352</v>
       </c>
       <c r="S245" s="44">
         <v>0</v>
@@ -23195,54 +23200,54 @@
       <c r="A246" s="50">
         <v>94530117</v>
       </c>
-      <c r="B246" s="40" t="s">
+      <c r="B246" s="58" t="s">
         <v>992</v>
       </c>
-      <c r="C246" s="40" t="s">
+      <c r="C246" s="58" t="s">
         <v>868</v>
       </c>
-      <c r="D246" s="40" t="s">
+      <c r="D246" s="58" t="s">
         <v>2</v>
       </c>
       <c r="E246" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F246" s="41" t="s">
+      <c r="F246" s="11" t="s">
         <v>1063</v>
       </c>
-      <c r="G246" s="42" t="s">
+      <c r="G246" s="59" t="s">
         <v>1064</v>
       </c>
-      <c r="H246" s="42" t="s">
+      <c r="H246" s="59" t="s">
         <v>1325</v>
       </c>
-      <c r="I246" s="42" t="s">
+      <c r="I246" s="59" t="s">
         <v>1065</v>
       </c>
-      <c r="J246" s="40" t="s">
+      <c r="J246" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="K246" s="40" t="s">
+      <c r="K246" s="58" t="s">
         <v>231</v>
       </c>
-      <c r="L246" s="40" t="s">
+      <c r="L246" s="58" t="s">
         <v>924</v>
       </c>
-      <c r="M246" s="40" t="s">
+      <c r="M246" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="N246" s="40" t="s">
+      <c r="N246" s="58" t="s">
         <v>875</v>
       </c>
-      <c r="O246" s="40" t="s">
+      <c r="O246" s="58" t="s">
         <v>876</v>
       </c>
-      <c r="P246" s="40"/>
-      <c r="Q246" s="40" t="s">
+      <c r="P246" s="58"/>
+      <c r="Q246" s="58" t="s">
         <v>17</v>
       </c>
       <c r="R246" s="6" t="s">
-        <v>1341</v>
+        <v>1352</v>
       </c>
       <c r="S246" s="44">
         <v>0</v>
@@ -24574,7 +24579,7 @@
         <v>17</v>
       </c>
       <c r="R264" s="6" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="S264" s="7">
         <v>0</v>
@@ -24651,7 +24656,7 @@
         <v>17</v>
       </c>
       <c r="R265" s="6" t="s">
-        <v>1342</v>
+        <v>1341</v>
       </c>
       <c r="S265" s="7">
         <v>0</v>
@@ -24728,7 +24733,7 @@
         <v>208</v>
       </c>
       <c r="R266" s="6" t="s">
-        <v>1343</v>
+        <v>1342</v>
       </c>
       <c r="S266" s="7">
         <v>0</v>
@@ -24805,7 +24810,7 @@
         <v>208</v>
       </c>
       <c r="R267" s="6" t="s">
-        <v>1344</v>
+        <v>1343</v>
       </c>
       <c r="S267" s="7">
         <v>0</v>
@@ -24882,7 +24887,7 @@
         <v>1262</v>
       </c>
       <c r="R268" s="6" t="s">
-        <v>1347</v>
+        <v>1346</v>
       </c>
       <c r="S268" s="7">
         <v>0</v>
@@ -24959,7 +24964,7 @@
         <v>1262</v>
       </c>
       <c r="R269" s="6" t="s">
-        <v>1348</v>
+        <v>1347</v>
       </c>
       <c r="S269" s="7">
         <v>0</v>

</xml_diff>

<commit_message>
Mod color shiny + Add ind (consultoría SURGE)
</commit_message>
<xml_diff>
--- a/Data/Base_fichas_indicadores.xlsx
+++ b/Data/Base_fichas_indicadores.xlsx
@@ -16,14 +16,14 @@
     <sheet name="REF_COLUMNAS" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BASE_FICHAS!$A$1:$AN$269</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BASE_FICHAS!$A$1:$AN$271</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4187" uniqueCount="1353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4218" uniqueCount="1366">
   <si>
     <t>id</t>
   </si>
@@ -4154,6 +4154,45 @@
   </si>
   <si>
     <t>(Personas LGBTI) Cantidad de personas trans</t>
+  </si>
+  <si>
+    <t>Para una descripición metodológica completa y mayor información visitar el Observatorio Ambiental Nacional (MA) https://www.ambiente.gub.uy/oan/</t>
+  </si>
+  <si>
+    <t>Afrodescendientes</t>
+  </si>
+  <si>
+    <t>Cantidad anual de becas educativas otorgadas a personas afrodescendientes</t>
+  </si>
+  <si>
+    <t>Para cada año calcular: Cantidad de becas educativas otorgadas a personas afrodescendientes.</t>
+  </si>
+  <si>
+    <t>OPP  2019 "Acciones afirmativas para personas afrodescendientes"</t>
+  </si>
+  <si>
+    <t>Consultoría Proyecto SURGE (ACNUDH - Uruguay) con base en OPP  2019 "Acciones afirmativas para personas afrodescendientes"</t>
+  </si>
+  <si>
+    <t>Oficina Nacional de Servicio Civil</t>
+  </si>
+  <si>
+    <t>El indicador mide el porcentaje de personas que ingresaron al estado en el marco de la Ley 19.122 en relación al total de ingresos.</t>
+  </si>
+  <si>
+    <t>Para cada año calcular: (Cantidad de ingresos de personas afrodescendientes a cargos públicos en el marco de la Ley 19.122 / Cantidad de ingresos de personas a cargos públicos en el marco de la Ley 19.122)*100</t>
+  </si>
+  <si>
+    <t>Consultoría Proyecto SURGE (ACNUDH - Uruguay) con base en Oficina Nacional del Servcio Civil</t>
+  </si>
+  <si>
+    <t>Porcentaje de ingresos de afrodescendientes a cargos públicos (Ley 19.122)</t>
+  </si>
+  <si>
+    <t>Cumplimiento de la couta de ingresos de afrodescendientes a cargos públicos (Ley 19.122)</t>
+  </si>
+  <si>
+    <t>El indicador mide la cantidad anual de becas educativas otorgadas a personas afrodescendientes.</t>
   </si>
 </sst>
 </file>
@@ -4270,7 +4309,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4411,9 +4450,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -4422,6 +4458,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -4740,13 +4783,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:AL272"/>
+  <sheetPr codeName="Hoja1" filterMode="1"/>
+  <dimension ref="A1:AL271"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A242" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E111" sqref="E111"/>
-      <selection pane="bottomLeft" activeCell="F285" sqref="F285"/>
+      <selection pane="bottomLeft" activeCell="E278" sqref="E278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4832,7 +4875,7 @@
       <c r="Q1" s="1" t="s">
         <v>342</v>
       </c>
-      <c r="R1" s="55" t="s">
+      <c r="R1" s="54" t="s">
         <v>1299</v>
       </c>
       <c r="S1" s="26" t="s">
@@ -5954,7 +5997,7 @@
       </c>
       <c r="AL17" s="6"/>
     </row>
-    <row r="18" spans="1:38">
+    <row r="18" spans="1:38" hidden="1">
       <c r="A18" s="13">
         <v>130101</v>
       </c>
@@ -6025,7 +6068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:38">
+    <row r="19" spans="1:38" hidden="1">
       <c r="A19" s="13">
         <v>130102</v>
       </c>
@@ -6096,7 +6139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:38">
+    <row r="20" spans="1:38" hidden="1">
       <c r="A20" s="13">
         <v>130103</v>
       </c>
@@ -6167,7 +6210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:38" s="6" customFormat="1">
+    <row r="21" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A21" s="14">
         <v>130104</v>
       </c>
@@ -6252,7 +6295,7 @@
       <c r="AJ21" s="13"/>
       <c r="AK21" s="13"/>
     </row>
-    <row r="22" spans="1:38" s="6" customFormat="1">
+    <row r="22" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A22" s="14">
         <v>130105</v>
       </c>
@@ -6337,7 +6380,7 @@
       <c r="AJ22" s="13"/>
       <c r="AK22" s="13"/>
     </row>
-    <row r="23" spans="1:38">
+    <row r="23" spans="1:38" hidden="1">
       <c r="A23" s="14">
         <v>130106</v>
       </c>
@@ -6409,7 +6452,7 @@
       </c>
       <c r="AL23" s="6"/>
     </row>
-    <row r="24" spans="1:38">
+    <row r="24" spans="1:38" hidden="1">
       <c r="A24" s="15">
         <v>130107</v>
       </c>
@@ -6495,7 +6538,7 @@
       <c r="AK24" s="15"/>
       <c r="AL24" s="6"/>
     </row>
-    <row r="25" spans="1:38">
+    <row r="25" spans="1:38" hidden="1">
       <c r="A25" s="15">
         <v>130108</v>
       </c>
@@ -6581,7 +6624,7 @@
       <c r="AK25" s="15"/>
       <c r="AL25" s="6"/>
     </row>
-    <row r="26" spans="1:38" s="6" customFormat="1">
+    <row r="26" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A26" s="6">
         <v>130201</v>
       </c>
@@ -6652,7 +6695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:38">
+    <row r="27" spans="1:38" hidden="1">
       <c r="A27" s="6">
         <v>130202</v>
       </c>
@@ -6737,7 +6780,7 @@
       <c r="AJ27" s="6"/>
       <c r="AK27" s="6"/>
     </row>
-    <row r="28" spans="1:38">
+    <row r="28" spans="1:38" hidden="1">
       <c r="A28" s="6">
         <v>130203</v>
       </c>
@@ -6822,7 +6865,7 @@
       <c r="AJ28" s="6"/>
       <c r="AK28" s="6"/>
     </row>
-    <row r="29" spans="1:38">
+    <row r="29" spans="1:38" hidden="1">
       <c r="A29" s="6">
         <v>130204</v>
       </c>
@@ -6893,7 +6936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:38" s="15" customFormat="1">
+    <row r="30" spans="1:38" s="15" customFormat="1" hidden="1">
       <c r="A30" s="6">
         <v>130205</v>
       </c>
@@ -6979,7 +7022,7 @@
       <c r="AK30" s="13"/>
       <c r="AL30" s="13"/>
     </row>
-    <row r="31" spans="1:38" s="15" customFormat="1">
+    <row r="31" spans="1:38" s="15" customFormat="1" hidden="1">
       <c r="A31" s="6">
         <v>130301</v>
       </c>
@@ -7063,7 +7106,7 @@
       <c r="AK31" s="13"/>
       <c r="AL31" s="6"/>
     </row>
-    <row r="32" spans="1:38" s="6" customFormat="1">
+    <row r="32" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A32" s="6">
         <v>130302</v>
       </c>
@@ -7146,7 +7189,7 @@
       <c r="AJ32" s="13"/>
       <c r="AK32" s="13"/>
     </row>
-    <row r="33" spans="1:38">
+    <row r="33" spans="1:38" hidden="1">
       <c r="A33" s="6">
         <v>130303</v>
       </c>
@@ -7216,7 +7259,7 @@
       </c>
       <c r="AL33" s="6"/>
     </row>
-    <row r="34" spans="1:38">
+    <row r="34" spans="1:38" hidden="1">
       <c r="A34" s="6">
         <v>130304</v>
       </c>
@@ -7302,7 +7345,7 @@
       <c r="AK34" s="6"/>
       <c r="AL34" s="6"/>
     </row>
-    <row r="35" spans="1:38" s="6" customFormat="1">
+    <row r="35" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A35" s="6">
         <v>130305</v>
       </c>
@@ -7373,7 +7416,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:38">
+    <row r="36" spans="1:38" hidden="1">
       <c r="A36" s="6">
         <v>130306</v>
       </c>
@@ -7445,7 +7488,7 @@
       </c>
       <c r="AL36" s="6"/>
     </row>
-    <row r="37" spans="1:38" s="6" customFormat="1">
+    <row r="37" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A37" s="6">
         <v>220101</v>
       </c>
@@ -7514,7 +7557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:38" s="6" customFormat="1">
+    <row r="38" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A38" s="6">
         <v>220102</v>
       </c>
@@ -7583,7 +7626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:38" s="6" customFormat="1">
+    <row r="39" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A39" s="6">
         <v>220103</v>
       </c>
@@ -7652,7 +7695,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:38" s="6" customFormat="1">
+    <row r="40" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A40" s="6">
         <v>220104</v>
       </c>
@@ -7721,7 +7764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:38">
+    <row r="41" spans="1:38" hidden="1">
       <c r="A41" s="6">
         <v>220105</v>
       </c>
@@ -7804,7 +7847,7 @@
       <c r="AK41" s="6"/>
       <c r="AL41" s="6"/>
     </row>
-    <row r="42" spans="1:38">
+    <row r="42" spans="1:38" hidden="1">
       <c r="A42" s="6">
         <v>220106</v>
       </c>
@@ -7887,7 +7930,7 @@
       <c r="AK42" s="25"/>
       <c r="AL42" s="6"/>
     </row>
-    <row r="43" spans="1:38">
+    <row r="43" spans="1:38" hidden="1">
       <c r="A43" s="6">
         <v>220107</v>
       </c>
@@ -7970,7 +8013,7 @@
       <c r="AK43" s="25"/>
       <c r="AL43" s="6"/>
     </row>
-    <row r="44" spans="1:38" s="6" customFormat="1">
+    <row r="44" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A44" s="17">
         <v>230101</v>
       </c>
@@ -8055,7 +8098,7 @@
       <c r="AJ44" s="13"/>
       <c r="AK44" s="13"/>
     </row>
-    <row r="45" spans="1:38" s="6" customFormat="1" ht="16.5" customHeight="1">
+    <row r="45" spans="1:38" s="6" customFormat="1" ht="16.5" hidden="1" customHeight="1">
       <c r="A45" s="17">
         <v>230201</v>
       </c>
@@ -8140,7 +8183,7 @@
       <c r="AJ45" s="13"/>
       <c r="AK45" s="13"/>
     </row>
-    <row r="46" spans="1:38" s="6" customFormat="1">
+    <row r="46" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A46" s="17">
         <v>230202</v>
       </c>
@@ -8225,7 +8268,7 @@
       <c r="AJ46" s="13"/>
       <c r="AK46" s="13"/>
     </row>
-    <row r="47" spans="1:38" s="6" customFormat="1">
+    <row r="47" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A47" s="10">
         <v>230203</v>
       </c>
@@ -8296,7 +8339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:38" s="6" customFormat="1">
+    <row r="48" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A48" s="10">
         <v>230204</v>
       </c>
@@ -8367,7 +8410,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:38" s="6" customFormat="1">
+    <row r="49" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A49" s="6">
         <v>230301</v>
       </c>
@@ -8438,7 +8481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:38">
+    <row r="50" spans="1:38" hidden="1">
       <c r="A50" s="6">
         <v>230302</v>
       </c>
@@ -8524,7 +8567,7 @@
       <c r="AK50" s="6"/>
       <c r="AL50" s="6"/>
     </row>
-    <row r="51" spans="1:38">
+    <row r="51" spans="1:38" hidden="1">
       <c r="A51" s="6">
         <v>230303</v>
       </c>
@@ -8610,7 +8653,7 @@
       <c r="AK51" s="6"/>
       <c r="AL51" s="6"/>
     </row>
-    <row r="52" spans="1:38">
+    <row r="52" spans="1:38" hidden="1">
       <c r="A52" s="6">
         <v>230304</v>
       </c>
@@ -8696,7 +8739,7 @@
       <c r="AK52" s="6"/>
       <c r="AL52" s="6"/>
     </row>
-    <row r="53" spans="1:38">
+    <row r="53" spans="1:38" hidden="1">
       <c r="A53" s="6">
         <v>230401</v>
       </c>
@@ -8782,7 +8825,7 @@
       <c r="AK53" s="6"/>
       <c r="AL53" s="6"/>
     </row>
-    <row r="54" spans="1:38" s="6" customFormat="1">
+    <row r="54" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A54" s="17">
         <v>230402</v>
       </c>
@@ -8867,7 +8910,7 @@
       <c r="AJ54" s="13"/>
       <c r="AK54" s="13"/>
     </row>
-    <row r="55" spans="1:38" s="6" customFormat="1">
+    <row r="55" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A55" s="17">
         <v>230501</v>
       </c>
@@ -8950,7 +8993,7 @@
       <c r="AJ55" s="13"/>
       <c r="AK55" s="13"/>
     </row>
-    <row r="56" spans="1:38" s="6" customFormat="1">
+    <row r="56" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A56" s="6">
         <v>320101</v>
       </c>
@@ -9019,7 +9062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:38" s="6" customFormat="1">
+    <row r="57" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A57" s="6">
         <v>320102</v>
       </c>
@@ -9088,7 +9131,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:38" s="6" customFormat="1">
+    <row r="58" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A58" s="6">
         <v>320103</v>
       </c>
@@ -9157,7 +9200,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:38" s="6" customFormat="1">
+    <row r="59" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A59" s="6">
         <v>320104</v>
       </c>
@@ -9226,7 +9269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:38" s="6" customFormat="1">
+    <row r="60" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A60" s="6">
         <v>320105</v>
       </c>
@@ -9295,7 +9338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:38" s="6" customFormat="1">
+    <row r="61" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A61" s="6">
         <v>320106</v>
       </c>
@@ -9365,7 +9408,7 @@
       </c>
       <c r="AL61" s="7"/>
     </row>
-    <row r="62" spans="1:38" s="6" customFormat="1">
+    <row r="62" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A62" s="6">
         <v>320107</v>
       </c>
@@ -9435,7 +9478,7 @@
       </c>
       <c r="AL62" s="7"/>
     </row>
-    <row r="63" spans="1:38" s="6" customFormat="1">
+    <row r="63" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A63" s="10">
         <v>330101</v>
       </c>
@@ -9448,7 +9491,7 @@
       <c r="E63" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F63" s="56" t="s">
+      <c r="F63" s="55" t="s">
         <v>718</v>
       </c>
       <c r="G63" s="6" t="s">
@@ -9484,7 +9527,7 @@
       <c r="Q63" s="13" t="s">
         <v>467</v>
       </c>
-      <c r="R63" s="57" t="s">
+      <c r="R63" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S63" s="6">
@@ -9507,7 +9550,7 @@
       </c>
       <c r="AL63" s="11"/>
     </row>
-    <row r="64" spans="1:38" s="6" customFormat="1">
+    <row r="64" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A64" s="10">
         <v>330102</v>
       </c>
@@ -9556,7 +9599,7 @@
       <c r="Q64" s="13" t="s">
         <v>467</v>
       </c>
-      <c r="R64" s="57" t="s">
+      <c r="R64" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S64" s="6">
@@ -9579,7 +9622,7 @@
       </c>
       <c r="AL64" s="7"/>
     </row>
-    <row r="65" spans="1:38" s="6" customFormat="1">
+    <row r="65" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A65" s="10">
         <v>330103</v>
       </c>
@@ -9628,7 +9671,7 @@
       <c r="Q65" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R65" s="57" t="s">
+      <c r="R65" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S65" s="6">
@@ -9650,7 +9693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:38" s="6" customFormat="1">
+    <row r="66" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A66" s="10">
         <v>330104</v>
       </c>
@@ -9699,7 +9742,7 @@
       <c r="Q66" s="13" t="s">
         <v>467</v>
       </c>
-      <c r="R66" s="57" t="s">
+      <c r="R66" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S66" s="6">
@@ -9721,7 +9764,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:38" s="6" customFormat="1">
+    <row r="67" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A67" s="10">
         <v>330105</v>
       </c>
@@ -9770,7 +9813,7 @@
       <c r="Q67" s="13" t="s">
         <v>467</v>
       </c>
-      <c r="R67" s="57" t="s">
+      <c r="R67" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S67" s="6">
@@ -9792,7 +9835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:38" s="6" customFormat="1">
+    <row r="68" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A68" s="10">
         <v>330106</v>
       </c>
@@ -9841,7 +9884,7 @@
       <c r="Q68" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R68" s="57" t="s">
+      <c r="R68" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S68" s="6">
@@ -9864,7 +9907,7 @@
       </c>
       <c r="AL68" s="11"/>
     </row>
-    <row r="69" spans="1:38" s="6" customFormat="1">
+    <row r="69" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A69" s="10">
         <v>330107</v>
       </c>
@@ -9913,7 +9956,7 @@
       <c r="Q69" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R69" s="57" t="s">
+      <c r="R69" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S69" s="6">
@@ -9936,7 +9979,7 @@
       </c>
       <c r="AL69" s="11"/>
     </row>
-    <row r="70" spans="1:38" s="6" customFormat="1">
+    <row r="70" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A70" s="10">
         <v>330108</v>
       </c>
@@ -9986,7 +10029,7 @@
       <c r="Q70" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R70" s="57" t="s">
+      <c r="R70" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S70" s="6">
@@ -10022,7 +10065,7 @@
       <c r="AK70" s="23"/>
       <c r="AL70" s="7"/>
     </row>
-    <row r="71" spans="1:38" s="6" customFormat="1">
+    <row r="71" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A71" s="10">
         <v>330109</v>
       </c>
@@ -10072,7 +10115,7 @@
       <c r="Q71" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R71" s="57" t="s">
+      <c r="R71" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S71" s="6">
@@ -10108,7 +10151,7 @@
       <c r="AK71" s="23"/>
       <c r="AL71" s="11"/>
     </row>
-    <row r="72" spans="1:38" s="6" customFormat="1">
+    <row r="72" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A72" s="10">
         <v>330110</v>
       </c>
@@ -10158,7 +10201,7 @@
       <c r="Q72" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R72" s="57" t="s">
+      <c r="R72" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S72" s="6">
@@ -10193,7 +10236,7 @@
       <c r="AJ72" s="23"/>
       <c r="AK72" s="23"/>
     </row>
-    <row r="73" spans="1:38" s="6" customFormat="1">
+    <row r="73" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A73" s="10">
         <v>330111</v>
       </c>
@@ -10243,7 +10286,7 @@
       <c r="Q73" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R73" s="57" t="s">
+      <c r="R73" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S73" s="6">
@@ -10279,7 +10322,7 @@
       <c r="AK73" s="23"/>
       <c r="AL73" s="11"/>
     </row>
-    <row r="74" spans="1:38" s="6" customFormat="1">
+    <row r="74" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A74" s="10">
         <v>330112</v>
       </c>
@@ -10329,7 +10372,7 @@
       <c r="Q74" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R74" s="57" t="s">
+      <c r="R74" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S74" s="6">
@@ -10365,7 +10408,7 @@
       <c r="AK74" s="23"/>
       <c r="AL74" s="11"/>
     </row>
-    <row r="75" spans="1:38" s="6" customFormat="1">
+    <row r="75" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A75" s="10">
         <v>330113</v>
       </c>
@@ -10415,7 +10458,7 @@
       <c r="Q75" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R75" s="57" t="s">
+      <c r="R75" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S75" s="6">
@@ -10451,7 +10494,7 @@
       <c r="AK75" s="23"/>
       <c r="AL75" s="11"/>
     </row>
-    <row r="76" spans="1:38" s="6" customFormat="1">
+    <row r="76" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A76" s="10">
         <v>330114</v>
       </c>
@@ -10501,7 +10544,7 @@
       <c r="Q76" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R76" s="57" t="s">
+      <c r="R76" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S76" s="6">
@@ -10537,7 +10580,7 @@
       <c r="AK76" s="23"/>
       <c r="AL76" s="11"/>
     </row>
-    <row r="77" spans="1:38" s="6" customFormat="1">
+    <row r="77" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A77" s="10">
         <v>330115</v>
       </c>
@@ -10587,7 +10630,7 @@
       <c r="Q77" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R77" s="57" t="s">
+      <c r="R77" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S77" s="6">
@@ -10623,7 +10666,7 @@
       <c r="AK77" s="23"/>
       <c r="AL77" s="11"/>
     </row>
-    <row r="78" spans="1:38" s="6" customFormat="1">
+    <row r="78" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A78" s="10">
         <v>330201</v>
       </c>
@@ -10672,7 +10715,7 @@
       <c r="Q78" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R78" s="57" t="s">
+      <c r="R78" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S78" s="6">
@@ -10695,7 +10738,7 @@
       </c>
       <c r="AL78" s="11"/>
     </row>
-    <row r="79" spans="1:38" s="6" customFormat="1">
+    <row r="79" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A79" s="10">
         <v>330202</v>
       </c>
@@ -10744,7 +10787,7 @@
       <c r="Q79" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R79" s="57" t="s">
+      <c r="R79" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S79" s="6">
@@ -10767,7 +10810,7 @@
       </c>
       <c r="AL79" s="11"/>
     </row>
-    <row r="80" spans="1:38" s="6" customFormat="1">
+    <row r="80" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A80" s="10">
         <v>330203</v>
       </c>
@@ -10816,7 +10859,7 @@
       <c r="Q80" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R80" s="57" t="s">
+      <c r="R80" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S80" s="6">
@@ -10839,7 +10882,7 @@
       </c>
       <c r="AL80" s="7"/>
     </row>
-    <row r="81" spans="1:38" s="6" customFormat="1">
+    <row r="81" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A81" s="10">
         <v>330204</v>
       </c>
@@ -10888,7 +10931,7 @@
       <c r="Q81" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R81" s="57" t="s">
+      <c r="R81" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S81" s="6">
@@ -10911,7 +10954,7 @@
       </c>
       <c r="AL81" s="7"/>
     </row>
-    <row r="82" spans="1:38" s="6" customFormat="1">
+    <row r="82" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A82" s="10">
         <v>330205</v>
       </c>
@@ -10960,7 +11003,7 @@
       <c r="Q82" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R82" s="57" t="s">
+      <c r="R82" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S82" s="6">
@@ -10983,7 +11026,7 @@
       </c>
       <c r="AL82" s="7"/>
     </row>
-    <row r="83" spans="1:38" s="6" customFormat="1">
+    <row r="83" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A83" s="10">
         <v>330206</v>
       </c>
@@ -11032,7 +11075,7 @@
       <c r="Q83" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R83" s="57" t="s">
+      <c r="R83" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S83" s="6">
@@ -11055,7 +11098,7 @@
       </c>
       <c r="AL83" s="7"/>
     </row>
-    <row r="84" spans="1:38" s="7" customFormat="1">
+    <row r="84" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A84" s="10">
         <v>330207</v>
       </c>
@@ -11105,7 +11148,7 @@
       <c r="Q84" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R84" s="57" t="s">
+      <c r="R84" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S84" s="6">
@@ -11140,7 +11183,7 @@
       <c r="AJ84" s="6"/>
       <c r="AK84" s="6"/>
     </row>
-    <row r="85" spans="1:38" s="7" customFormat="1">
+    <row r="85" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A85" s="10">
         <v>330208</v>
       </c>
@@ -11190,7 +11233,7 @@
       <c r="Q85" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R85" s="57" t="s">
+      <c r="R85" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S85" s="6">
@@ -11225,7 +11268,7 @@
       <c r="AJ85" s="6"/>
       <c r="AK85" s="6"/>
     </row>
-    <row r="86" spans="1:38" s="6" customFormat="1">
+    <row r="86" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A86" s="10">
         <v>330209</v>
       </c>
@@ -11274,7 +11317,7 @@
       <c r="Q86" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R86" s="57" t="s">
+      <c r="R86" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S86" s="6">
@@ -11297,7 +11340,7 @@
       </c>
       <c r="AL86" s="23"/>
     </row>
-    <row r="87" spans="1:38" s="7" customFormat="1">
+    <row r="87" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A87" s="10">
         <v>330210</v>
       </c>
@@ -11347,7 +11390,7 @@
       <c r="Q87" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R87" s="57" t="s">
+      <c r="R87" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S87" s="6">
@@ -11382,7 +11425,7 @@
       <c r="AJ87" s="6"/>
       <c r="AK87" s="6"/>
     </row>
-    <row r="88" spans="1:38" s="6" customFormat="1">
+    <row r="88" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A88" s="10">
         <v>330211</v>
       </c>
@@ -11431,7 +11474,7 @@
       <c r="Q88" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R88" s="57" t="s">
+      <c r="R88" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S88" s="6">
@@ -11454,7 +11497,7 @@
       </c>
       <c r="AL88" s="23"/>
     </row>
-    <row r="89" spans="1:38" s="6" customFormat="1">
+    <row r="89" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A89" s="10">
         <v>330212</v>
       </c>
@@ -11503,7 +11546,7 @@
       <c r="Q89" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R89" s="57" t="s">
+      <c r="R89" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S89" s="6">
@@ -11526,7 +11569,7 @@
       </c>
       <c r="AL89" s="7"/>
     </row>
-    <row r="90" spans="1:38" s="11" customFormat="1">
+    <row r="90" spans="1:38" s="11" customFormat="1" hidden="1">
       <c r="A90" s="10">
         <v>330213</v>
       </c>
@@ -11576,7 +11619,7 @@
       <c r="Q90" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R90" s="57" t="s">
+      <c r="R90" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S90" s="6">
@@ -11612,7 +11655,7 @@
       <c r="AK90" s="6"/>
       <c r="AL90" s="7"/>
     </row>
-    <row r="91" spans="1:38" s="11" customFormat="1">
+    <row r="91" spans="1:38" s="11" customFormat="1" hidden="1">
       <c r="A91" s="6">
         <v>420101</v>
       </c>
@@ -11696,7 +11739,7 @@
       <c r="AK91" s="6"/>
       <c r="AL91" s="7"/>
     </row>
-    <row r="92" spans="1:38" s="7" customFormat="1">
+    <row r="92" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A92" s="6">
         <v>420102</v>
       </c>
@@ -11779,7 +11822,7 @@
       <c r="AJ92" s="6"/>
       <c r="AK92" s="6"/>
     </row>
-    <row r="93" spans="1:38" s="11" customFormat="1">
+    <row r="93" spans="1:38" s="11" customFormat="1" hidden="1">
       <c r="A93" s="6">
         <v>420103</v>
       </c>
@@ -11863,7 +11906,7 @@
       <c r="AK93" s="6"/>
       <c r="AL93" s="23"/>
     </row>
-    <row r="94" spans="1:38" s="6" customFormat="1">
+    <row r="94" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A94" s="6">
         <v>420104</v>
       </c>
@@ -11933,7 +11976,7 @@
       </c>
       <c r="AL94" s="25"/>
     </row>
-    <row r="95" spans="1:38" s="11" customFormat="1">
+    <row r="95" spans="1:38" s="11" customFormat="1" hidden="1">
       <c r="A95" s="6">
         <v>420105</v>
       </c>
@@ -12016,7 +12059,7 @@
       <c r="AJ95" s="6"/>
       <c r="AK95" s="6"/>
     </row>
-    <row r="96" spans="1:38" s="11" customFormat="1">
+    <row r="96" spans="1:38" s="11" customFormat="1" hidden="1">
       <c r="A96" s="6">
         <v>420106</v>
       </c>
@@ -12099,7 +12142,7 @@
       <c r="AJ96" s="6"/>
       <c r="AK96" s="6"/>
     </row>
-    <row r="97" spans="1:38" s="11" customFormat="1">
+    <row r="97" spans="1:38" s="11" customFormat="1" hidden="1">
       <c r="A97" s="6">
         <v>420107</v>
       </c>
@@ -12182,7 +12225,7 @@
       <c r="AJ97" s="7"/>
       <c r="AK97" s="7"/>
     </row>
-    <row r="98" spans="1:38" s="11" customFormat="1">
+    <row r="98" spans="1:38" s="11" customFormat="1" hidden="1">
       <c r="A98" s="6">
         <v>420108</v>
       </c>
@@ -12266,7 +12309,7 @@
       <c r="AK98" s="7"/>
       <c r="AL98" s="23"/>
     </row>
-    <row r="99" spans="1:38" s="11" customFormat="1">
+    <row r="99" spans="1:38" s="11" customFormat="1" hidden="1">
       <c r="A99" s="6">
         <v>420109</v>
       </c>
@@ -12350,7 +12393,7 @@
       <c r="AK99" s="7"/>
       <c r="AL99" s="23"/>
     </row>
-    <row r="100" spans="1:38" s="11" customFormat="1">
+    <row r="100" spans="1:38" s="11" customFormat="1" hidden="1">
       <c r="A100" s="6">
         <v>430101</v>
       </c>
@@ -12434,7 +12477,7 @@
       <c r="AK100" s="6"/>
       <c r="AL100" s="23"/>
     </row>
-    <row r="101" spans="1:38" s="11" customFormat="1">
+    <row r="101" spans="1:38" s="11" customFormat="1" hidden="1">
       <c r="A101" s="6">
         <v>430102</v>
       </c>
@@ -12518,7 +12561,7 @@
       <c r="AK101" s="6"/>
       <c r="AL101" s="23"/>
     </row>
-    <row r="102" spans="1:38" s="11" customFormat="1">
+    <row r="102" spans="1:38" s="11" customFormat="1" hidden="1">
       <c r="A102" s="6">
         <v>430103</v>
       </c>
@@ -12587,7 +12630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:38" s="7" customFormat="1">
+    <row r="103" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A103" s="6">
         <v>430104</v>
       </c>
@@ -12670,7 +12713,7 @@
       <c r="AK103" s="11"/>
       <c r="AL103" s="11"/>
     </row>
-    <row r="104" spans="1:38" s="7" customFormat="1">
+    <row r="104" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A104" s="6">
         <v>430105</v>
       </c>
@@ -12752,7 +12795,7 @@
       <c r="AJ104" s="11"/>
       <c r="AK104" s="11"/>
     </row>
-    <row r="105" spans="1:38" s="7" customFormat="1">
+    <row r="105" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A105" s="6">
         <v>430106</v>
       </c>
@@ -12835,7 +12878,7 @@
       <c r="AK105" s="11"/>
       <c r="AL105" s="13"/>
     </row>
-    <row r="106" spans="1:38" s="7" customFormat="1">
+    <row r="106" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A106" s="6">
         <v>430107</v>
       </c>
@@ -12918,7 +12961,7 @@
       <c r="AK106" s="11"/>
       <c r="AL106" s="13"/>
     </row>
-    <row r="107" spans="1:38" s="7" customFormat="1">
+    <row r="107" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A107" s="6">
         <v>430108</v>
       </c>
@@ -13001,7 +13044,7 @@
       <c r="AK107" s="11"/>
       <c r="AL107" s="13"/>
     </row>
-    <row r="108" spans="1:38" s="7" customFormat="1">
+    <row r="108" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A108" s="6">
         <v>430109</v>
       </c>
@@ -13084,7 +13127,7 @@
       <c r="AK108" s="11"/>
       <c r="AL108" s="13"/>
     </row>
-    <row r="109" spans="1:38" s="23" customFormat="1">
+    <row r="109" spans="1:38" s="23" customFormat="1" hidden="1">
       <c r="A109" s="6">
         <v>430110</v>
       </c>
@@ -13168,7 +13211,7 @@
       <c r="AK109" s="11"/>
       <c r="AL109" s="13"/>
     </row>
-    <row r="110" spans="1:38" s="7" customFormat="1">
+    <row r="110" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A110" s="6">
         <v>430111</v>
       </c>
@@ -13251,7 +13294,7 @@
       <c r="AK110" s="11"/>
       <c r="AL110" s="13"/>
     </row>
-    <row r="111" spans="1:38" s="23" customFormat="1">
+    <row r="111" spans="1:38" s="23" customFormat="1" hidden="1">
       <c r="A111" s="6">
         <v>430112</v>
       </c>
@@ -13335,7 +13378,7 @@
       <c r="AK111" s="11"/>
       <c r="AL111" s="13"/>
     </row>
-    <row r="112" spans="1:38" s="7" customFormat="1">
+    <row r="112" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A112" s="6">
         <v>430113</v>
       </c>
@@ -13418,7 +13461,7 @@
       <c r="AK112" s="11"/>
       <c r="AL112" s="13"/>
     </row>
-    <row r="113" spans="1:38" s="7" customFormat="1">
+    <row r="113" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A113" s="6">
         <v>430114</v>
       </c>
@@ -13501,7 +13544,7 @@
       <c r="AK113" s="11"/>
       <c r="AL113" s="13"/>
     </row>
-    <row r="114" spans="1:38" s="7" customFormat="1">
+    <row r="114" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A114" s="6">
         <v>430201</v>
       </c>
@@ -13570,7 +13613,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:38" s="7" customFormat="1">
+    <row r="115" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A115" s="6">
         <v>430202</v>
       </c>
@@ -13639,7 +13682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:38" s="23" customFormat="1">
+    <row r="116" spans="1:38" s="23" customFormat="1" hidden="1">
       <c r="A116" s="6">
         <v>430203</v>
       </c>
@@ -13723,7 +13766,7 @@
       <c r="AK116" s="7"/>
       <c r="AL116" s="7"/>
     </row>
-    <row r="117" spans="1:38" s="25" customFormat="1">
+    <row r="117" spans="1:38" s="25" customFormat="1" hidden="1">
       <c r="A117" s="6">
         <v>430204</v>
       </c>
@@ -13807,7 +13850,7 @@
       <c r="AK117" s="7"/>
       <c r="AL117" s="7"/>
     </row>
-    <row r="118" spans="1:38" s="11" customFormat="1">
+    <row r="118" spans="1:38" s="11" customFormat="1" hidden="1">
       <c r="A118" s="6">
         <v>430205</v>
       </c>
@@ -13891,7 +13934,7 @@
       <c r="AK118" s="7"/>
       <c r="AL118" s="7"/>
     </row>
-    <row r="119" spans="1:38" s="11" customFormat="1">
+    <row r="119" spans="1:38" s="11" customFormat="1" hidden="1">
       <c r="A119" s="6">
         <v>430206</v>
       </c>
@@ -13975,7 +14018,7 @@
       <c r="AK119" s="7"/>
       <c r="AL119" s="7"/>
     </row>
-    <row r="120" spans="1:38" s="11" customFormat="1">
+    <row r="120" spans="1:38" s="11" customFormat="1" hidden="1">
       <c r="A120" s="6">
         <v>430207</v>
       </c>
@@ -14059,7 +14102,7 @@
       <c r="AK120" s="7"/>
       <c r="AL120" s="7"/>
     </row>
-    <row r="121" spans="1:38" s="23" customFormat="1">
+    <row r="121" spans="1:38" s="23" customFormat="1" hidden="1">
       <c r="A121" s="6">
         <v>430208</v>
       </c>
@@ -14143,7 +14186,7 @@
       <c r="AK121" s="7"/>
       <c r="AL121" s="7"/>
     </row>
-    <row r="122" spans="1:38" s="23" customFormat="1">
+    <row r="122" spans="1:38" s="23" customFormat="1" hidden="1">
       <c r="A122" s="6">
         <v>430209</v>
       </c>
@@ -14227,7 +14270,7 @@
       <c r="AK122" s="7"/>
       <c r="AL122" s="7"/>
     </row>
-    <row r="123" spans="1:38" s="23" customFormat="1">
+    <row r="123" spans="1:38" s="23" customFormat="1" hidden="1">
       <c r="A123" s="29">
         <v>430301</v>
       </c>
@@ -14311,7 +14354,7 @@
       <c r="AK123" s="7"/>
       <c r="AL123" s="7"/>
     </row>
-    <row r="124" spans="1:38" s="23" customFormat="1">
+    <row r="124" spans="1:38" s="23" customFormat="1" hidden="1">
       <c r="A124" s="29">
         <v>430302</v>
       </c>
@@ -14395,7 +14438,7 @@
       <c r="AK124" s="7"/>
       <c r="AL124" s="7"/>
     </row>
-    <row r="125" spans="1:38" s="11" customFormat="1">
+    <row r="125" spans="1:38" s="11" customFormat="1" hidden="1">
       <c r="A125" s="29">
         <v>430303</v>
       </c>
@@ -14465,7 +14508,7 @@
       </c>
       <c r="AL125" s="7"/>
     </row>
-    <row r="126" spans="1:38" s="11" customFormat="1">
+    <row r="126" spans="1:38" s="11" customFormat="1" hidden="1">
       <c r="A126" s="29">
         <v>430304</v>
       </c>
@@ -14535,7 +14578,7 @@
       </c>
       <c r="AL126" s="7"/>
     </row>
-    <row r="127" spans="1:38" s="7" customFormat="1">
+    <row r="127" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A127" s="29">
         <v>430305</v>
       </c>
@@ -14617,7 +14660,7 @@
       <c r="AJ127" s="11"/>
       <c r="AK127" s="11"/>
     </row>
-    <row r="128" spans="1:38">
+    <row r="128" spans="1:38" hidden="1">
       <c r="A128" s="29">
         <v>430306</v>
       </c>
@@ -14701,7 +14744,7 @@
       <c r="AK128" s="11"/>
       <c r="AL128" s="7"/>
     </row>
-    <row r="129" spans="1:38">
+    <row r="129" spans="1:38" hidden="1">
       <c r="A129" s="29">
         <v>430307</v>
       </c>
@@ -14785,7 +14828,7 @@
       <c r="AK129" s="7"/>
       <c r="AL129" s="7"/>
     </row>
-    <row r="130" spans="1:38">
+    <row r="130" spans="1:38" hidden="1">
       <c r="A130" s="7">
         <v>430401</v>
       </c>
@@ -14867,7 +14910,7 @@
       <c r="AK130" s="23"/>
       <c r="AL130" s="7"/>
     </row>
-    <row r="131" spans="1:38">
+    <row r="131" spans="1:38" hidden="1">
       <c r="A131" s="7">
         <v>430402</v>
       </c>
@@ -14949,7 +14992,7 @@
       <c r="AK131" s="23"/>
       <c r="AL131" s="7"/>
     </row>
-    <row r="132" spans="1:38">
+    <row r="132" spans="1:38" hidden="1">
       <c r="A132" s="7">
         <v>430403</v>
       </c>
@@ -15031,7 +15074,7 @@
       <c r="AK132" s="23"/>
       <c r="AL132" s="7"/>
     </row>
-    <row r="133" spans="1:38">
+    <row r="133" spans="1:38" hidden="1">
       <c r="A133" s="7">
         <v>430404</v>
       </c>
@@ -15113,7 +15156,7 @@
       <c r="AK133" s="23"/>
       <c r="AL133" s="7"/>
     </row>
-    <row r="134" spans="1:38">
+    <row r="134" spans="1:38" hidden="1">
       <c r="A134" s="7">
         <v>430405</v>
       </c>
@@ -15195,7 +15238,7 @@
       <c r="AK134" s="23"/>
       <c r="AL134" s="7"/>
     </row>
-    <row r="135" spans="1:38">
+    <row r="135" spans="1:38" hidden="1">
       <c r="A135" s="7">
         <v>430406</v>
       </c>
@@ -15277,7 +15320,7 @@
       <c r="AK135" s="23"/>
       <c r="AL135" s="7"/>
     </row>
-    <row r="136" spans="1:38">
+    <row r="136" spans="1:38" hidden="1">
       <c r="A136" s="7">
         <v>430407</v>
       </c>
@@ -15799,7 +15842,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:38" s="7" customFormat="1">
+    <row r="143" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A143" s="10">
         <v>530101</v>
       </c>
@@ -15846,7 +15889,7 @@
       <c r="Q143" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="R143" s="57" t="s">
+      <c r="R143" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S143" s="44">
@@ -15868,7 +15911,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:38" s="7" customFormat="1">
+    <row r="144" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A144" s="10">
         <v>530102</v>
       </c>
@@ -15915,7 +15958,7 @@
       <c r="Q144" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="R144" s="57" t="s">
+      <c r="R144" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S144" s="44">
@@ -15937,7 +15980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:24" s="7" customFormat="1">
+    <row r="145" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A145" s="10">
         <v>530103</v>
       </c>
@@ -15984,7 +16027,7 @@
       <c r="Q145" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="R145" s="57" t="s">
+      <c r="R145" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S145" s="44">
@@ -16006,7 +16049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:24" s="7" customFormat="1">
+    <row r="146" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A146" s="10">
         <v>530104</v>
       </c>
@@ -16053,7 +16096,7 @@
       <c r="Q146" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="R146" s="57" t="s">
+      <c r="R146" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S146" s="44">
@@ -16075,7 +16118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:24" s="7" customFormat="1">
+    <row r="147" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A147" s="10">
         <v>530201</v>
       </c>
@@ -16121,7 +16164,7 @@
       <c r="Q147" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="R147" s="57" t="s">
+      <c r="R147" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S147" s="44">
@@ -16143,7 +16186,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:24" s="7" customFormat="1">
+    <row r="148" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A148" s="10">
         <v>530202</v>
       </c>
@@ -16192,7 +16235,7 @@
       <c r="Q148" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="R148" s="57" t="s">
+      <c r="R148" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S148" s="44">
@@ -16214,7 +16257,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:24" s="7" customFormat="1">
+    <row r="149" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A149" s="10">
         <v>530203</v>
       </c>
@@ -16260,7 +16303,7 @@
       <c r="Q149" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="R149" s="57" t="s">
+      <c r="R149" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S149" s="44">
@@ -16282,7 +16325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:24" s="7" customFormat="1">
+    <row r="150" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A150" s="10">
         <v>530204</v>
       </c>
@@ -16328,7 +16371,7 @@
       <c r="Q150" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="R150" s="57" t="s">
+      <c r="R150" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S150" s="44">
@@ -16350,7 +16393,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:24" s="7" customFormat="1">
+    <row r="151" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A151" s="10">
         <v>530205</v>
       </c>
@@ -16396,7 +16439,7 @@
       <c r="Q151" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="R151" s="57" t="s">
+      <c r="R151" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S151" s="44">
@@ -16418,7 +16461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:24" s="7" customFormat="1" ht="16.5" customHeight="1">
+    <row r="152" spans="1:24" s="7" customFormat="1" ht="16.5" hidden="1" customHeight="1">
       <c r="A152" s="10">
         <v>530206</v>
       </c>
@@ -16467,7 +16510,7 @@
       <c r="Q152" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="R152" s="57" t="s">
+      <c r="R152" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S152" s="44">
@@ -16489,7 +16532,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:24" s="7" customFormat="1">
+    <row r="153" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A153" s="10">
         <v>530207</v>
       </c>
@@ -16538,7 +16581,7 @@
       <c r="Q153" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="R153" s="57" t="s">
+      <c r="R153" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S153" s="44">
@@ -16560,7 +16603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:24" s="7" customFormat="1">
+    <row r="154" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A154" s="10">
         <v>530208</v>
       </c>
@@ -16606,7 +16649,7 @@
       <c r="Q154" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="R154" s="57" t="s">
+      <c r="R154" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S154" s="44">
@@ -16628,7 +16671,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:24" s="53" customFormat="1">
+    <row r="155" spans="1:24" s="53" customFormat="1" hidden="1">
       <c r="A155" s="53">
         <v>530209</v>
       </c>
@@ -16677,7 +16720,7 @@
       <c r="Q155" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="R155" s="57" t="s">
+      <c r="R155" s="56" t="s">
         <v>1303</v>
       </c>
       <c r="S155" s="53">
@@ -16699,7 +16742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:24" s="7" customFormat="1">
+    <row r="156" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A156" s="10">
         <v>530210</v>
       </c>
@@ -16767,7 +16810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:24" s="7" customFormat="1">
+    <row r="157" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A157" s="10">
         <v>530211</v>
       </c>
@@ -16835,7 +16878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:24" s="7" customFormat="1">
+    <row r="158" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A158" s="10">
         <v>530212</v>
       </c>
@@ -16903,7 +16946,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:24" s="7" customFormat="1">
+    <row r="159" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A159" s="10">
         <v>530213</v>
       </c>
@@ -16973,7 +17016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:24" s="7" customFormat="1">
+    <row r="160" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A160" s="6">
         <v>620101</v>
       </c>
@@ -17042,7 +17085,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:24" s="7" customFormat="1">
+    <row r="161" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A161" s="6">
         <v>620102</v>
       </c>
@@ -17111,7 +17154,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:24" s="7" customFormat="1">
+    <row r="162" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A162" s="6">
         <v>620103</v>
       </c>
@@ -17180,7 +17223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:24" s="7" customFormat="1">
+    <row r="163" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A163" s="6">
         <v>620104</v>
       </c>
@@ -17248,7 +17291,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:24" s="7" customFormat="1">
+    <row r="164" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A164" s="6">
         <v>620105</v>
       </c>
@@ -17295,7 +17338,7 @@
         <v>730</v>
       </c>
       <c r="R164" s="6" t="s">
-        <v>1298</v>
+        <v>1353</v>
       </c>
       <c r="S164" s="44">
         <v>0</v>
@@ -17316,7 +17359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:24" s="7" customFormat="1">
+    <row r="165" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A165" s="6">
         <v>620106</v>
       </c>
@@ -17363,7 +17406,7 @@
         <v>730</v>
       </c>
       <c r="R165" s="6" t="s">
-        <v>1298</v>
+        <v>1353</v>
       </c>
       <c r="S165" s="44">
         <v>0</v>
@@ -17384,7 +17427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:24" s="7" customFormat="1">
+    <row r="166" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A166" s="6">
         <v>620107</v>
       </c>
@@ -17431,7 +17474,7 @@
         <v>17</v>
       </c>
       <c r="R166" s="6" t="s">
-        <v>1298</v>
+        <v>1353</v>
       </c>
       <c r="S166" s="44">
         <v>0</v>
@@ -17452,7 +17495,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:24" s="7" customFormat="1">
+    <row r="167" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A167" s="6">
         <v>620108</v>
       </c>
@@ -17499,7 +17542,7 @@
         <v>17</v>
       </c>
       <c r="R167" s="6" t="s">
-        <v>1298</v>
+        <v>1353</v>
       </c>
       <c r="S167" s="44">
         <v>0</v>
@@ -17520,7 +17563,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:24" s="7" customFormat="1">
+    <row r="168" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A168" s="6">
         <v>620109</v>
       </c>
@@ -17567,7 +17610,7 @@
         <v>17</v>
       </c>
       <c r="R168" s="6" t="s">
-        <v>1298</v>
+        <v>1353</v>
       </c>
       <c r="S168" s="44">
         <v>0</v>
@@ -17588,7 +17631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:24" s="7" customFormat="1">
+    <row r="169" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A169" s="6">
         <v>620110</v>
       </c>
@@ -17636,7 +17679,7 @@
         <v>17</v>
       </c>
       <c r="R169" s="6" t="s">
-        <v>1298</v>
+        <v>1353</v>
       </c>
       <c r="S169" s="44">
         <v>0</v>
@@ -17657,7 +17700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:24" s="7" customFormat="1">
+    <row r="170" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A170" s="6">
         <v>620111</v>
       </c>
@@ -17725,7 +17768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:24" s="7" customFormat="1">
+    <row r="171" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A171" s="6">
         <v>620112</v>
       </c>
@@ -17793,7 +17836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:24" s="7" customFormat="1">
+    <row r="172" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A172" s="6">
         <v>620113</v>
       </c>
@@ -17861,7 +17904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:24" s="7" customFormat="1">
+    <row r="173" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A173" s="7">
         <v>630101</v>
       </c>
@@ -17932,7 +17975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:24" s="7" customFormat="1">
+    <row r="174" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A174" s="7">
         <v>630102</v>
       </c>
@@ -18003,7 +18046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:24" s="7" customFormat="1">
+    <row r="175" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A175" s="7">
         <v>630103</v>
       </c>
@@ -18074,7 +18117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:24" s="7" customFormat="1">
+    <row r="176" spans="1:24" s="7" customFormat="1" hidden="1">
       <c r="A176" s="7">
         <v>630201</v>
       </c>
@@ -18124,7 +18167,7 @@
         <v>799</v>
       </c>
       <c r="R176" s="6" t="s">
-        <v>1298</v>
+        <v>1353</v>
       </c>
       <c r="S176" s="44">
         <v>0</v>
@@ -18145,7 +18188,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:38" s="7" customFormat="1">
+    <row r="177" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A177" s="7">
         <v>630202</v>
       </c>
@@ -18195,7 +18238,7 @@
         <v>799</v>
       </c>
       <c r="R177" s="6" t="s">
-        <v>1298</v>
+        <v>1353</v>
       </c>
       <c r="S177" s="44">
         <v>0</v>
@@ -18216,7 +18259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:38" s="7" customFormat="1">
+    <row r="178" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A178" s="7">
         <v>630203</v>
       </c>
@@ -18266,7 +18309,7 @@
         <v>799</v>
       </c>
       <c r="R178" s="6" t="s">
-        <v>1298</v>
+        <v>1353</v>
       </c>
       <c r="S178" s="44">
         <v>0</v>
@@ -18287,7 +18330,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:38" s="7" customFormat="1">
+    <row r="179" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A179" s="7">
         <v>630204</v>
       </c>
@@ -18337,7 +18380,7 @@
         <v>799</v>
       </c>
       <c r="R179" s="6" t="s">
-        <v>1298</v>
+        <v>1353</v>
       </c>
       <c r="S179" s="44">
         <v>0</v>
@@ -18358,7 +18401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:38" s="7" customFormat="1">
+    <row r="180" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A180" s="7">
         <v>630205</v>
       </c>
@@ -18408,7 +18451,7 @@
         <v>799</v>
       </c>
       <c r="R180" s="6" t="s">
-        <v>1298</v>
+        <v>1353</v>
       </c>
       <c r="S180" s="44">
         <v>0</v>
@@ -18429,7 +18472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:38" s="7" customFormat="1">
+    <row r="181" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A181" s="7">
         <v>630206</v>
       </c>
@@ -18479,7 +18522,7 @@
         <v>17</v>
       </c>
       <c r="R181" s="6" t="s">
-        <v>1298</v>
+        <v>1353</v>
       </c>
       <c r="S181" s="44">
         <v>0</v>
@@ -18500,7 +18543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:38" s="7" customFormat="1">
+    <row r="182" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A182" s="7">
         <v>630207</v>
       </c>
@@ -18550,7 +18593,7 @@
         <v>834</v>
       </c>
       <c r="R182" s="6" t="s">
-        <v>1298</v>
+        <v>1353</v>
       </c>
       <c r="S182" s="44">
         <v>0</v>
@@ -18571,7 +18614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:38" s="7" customFormat="1">
+    <row r="183" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A183" s="7">
         <v>630208</v>
       </c>
@@ -18621,7 +18664,7 @@
         <v>834</v>
       </c>
       <c r="R183" s="6" t="s">
-        <v>1298</v>
+        <v>1353</v>
       </c>
       <c r="S183" s="44">
         <v>0</v>
@@ -18642,7 +18685,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:38" s="7" customFormat="1">
+    <row r="184" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A184" s="7">
         <v>630209</v>
       </c>
@@ -18692,7 +18735,7 @@
         <v>843</v>
       </c>
       <c r="R184" s="6" t="s">
-        <v>1298</v>
+        <v>1353</v>
       </c>
       <c r="S184" s="44">
         <v>0</v>
@@ -18713,7 +18756,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:38" s="7" customFormat="1">
+    <row r="185" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A185" s="7">
         <v>630210</v>
       </c>
@@ -18763,7 +18806,7 @@
         <v>843</v>
       </c>
       <c r="R185" s="6" t="s">
-        <v>1298</v>
+        <v>1353</v>
       </c>
       <c r="S185" s="44">
         <v>0</v>
@@ -18784,7 +18827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:38" s="7" customFormat="1">
+    <row r="186" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A186" s="7">
         <v>630211</v>
       </c>
@@ -18834,7 +18877,7 @@
         <v>843</v>
       </c>
       <c r="R186" s="6" t="s">
-        <v>1298</v>
+        <v>1353</v>
       </c>
       <c r="S186" s="44">
         <v>0</v>
@@ -18855,7 +18898,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:38" s="7" customFormat="1">
+    <row r="187" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A187" s="7">
         <v>630212</v>
       </c>
@@ -18905,7 +18948,7 @@
         <v>843</v>
       </c>
       <c r="R187" s="6" t="s">
-        <v>1298</v>
+        <v>1353</v>
       </c>
       <c r="S187" s="44">
         <v>0</v>
@@ -18926,7 +18969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:38" s="7" customFormat="1">
+    <row r="188" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A188" s="7">
         <v>630213</v>
       </c>
@@ -18976,7 +19019,7 @@
         <v>843</v>
       </c>
       <c r="R188" s="6" t="s">
-        <v>1298</v>
+        <v>1353</v>
       </c>
       <c r="S188" s="44">
         <v>0</v>
@@ -18997,7 +19040,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:38" s="7" customFormat="1">
+    <row r="189" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A189" s="48">
         <v>91130110</v>
       </c>
@@ -19069,7 +19112,7 @@
       </c>
       <c r="AL189" s="44"/>
     </row>
-    <row r="190" spans="1:38" s="7" customFormat="1">
+    <row r="190" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A190" s="49">
         <v>91130206</v>
       </c>
@@ -19142,7 +19185,7 @@
       </c>
       <c r="AL190" s="44"/>
     </row>
-    <row r="191" spans="1:38" s="7" customFormat="1">
+    <row r="191" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A191" s="49">
         <v>91130207</v>
       </c>
@@ -19215,7 +19258,7 @@
       </c>
       <c r="AL191" s="44"/>
     </row>
-    <row r="192" spans="1:38" s="7" customFormat="1">
+    <row r="192" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A192" s="49">
         <v>91130208</v>
       </c>
@@ -19288,7 +19331,7 @@
       </c>
       <c r="AL192" s="44"/>
     </row>
-    <row r="193" spans="1:38" s="7" customFormat="1">
+    <row r="193" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A193" s="49">
         <v>91130209</v>
       </c>
@@ -19360,7 +19403,7 @@
       </c>
       <c r="AL193" s="44"/>
     </row>
-    <row r="194" spans="1:38" s="7" customFormat="1">
+    <row r="194" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A194" s="50">
         <v>91230601</v>
       </c>
@@ -19431,7 +19474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:38" s="7" customFormat="1">
+    <row r="195" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A195" s="50">
         <v>91230602</v>
       </c>
@@ -19502,7 +19545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:38" s="7" customFormat="1">
+    <row r="196" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A196" s="50">
         <v>91230603</v>
       </c>
@@ -19573,7 +19616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:38" s="7" customFormat="1">
+    <row r="197" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A197" s="50">
         <v>91330116</v>
       </c>
@@ -19650,7 +19693,7 @@
       <c r="AC197" s="44"/>
       <c r="AD197" s="44"/>
     </row>
-    <row r="198" spans="1:38" s="7" customFormat="1">
+    <row r="198" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A198" s="50">
         <v>91430115</v>
       </c>
@@ -19727,7 +19770,7 @@
       <c r="AC198" s="44"/>
       <c r="AD198" s="44"/>
     </row>
-    <row r="199" spans="1:38" s="7" customFormat="1">
+    <row r="199" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A199" s="50">
         <v>91430308</v>
       </c>
@@ -19798,7 +19841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:38" s="7" customFormat="1">
+    <row r="200" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A200" s="50">
         <v>91430309</v>
       </c>
@@ -19869,7 +19912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:38" s="7" customFormat="1">
+    <row r="201" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A201" s="50">
         <v>91430310</v>
       </c>
@@ -19940,7 +19983,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:38" s="7" customFormat="1">
+    <row r="202" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A202" s="50">
         <v>91530105</v>
       </c>
@@ -20011,7 +20054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:38" s="7" customFormat="1">
+    <row r="203" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A203" s="50">
         <v>91530106</v>
       </c>
@@ -20082,7 +20125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:38" s="7" customFormat="1">
+    <row r="204" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A204" s="50">
         <v>92130111</v>
       </c>
@@ -20154,7 +20197,7 @@
       </c>
       <c r="AL204" s="44"/>
     </row>
-    <row r="205" spans="1:38" s="7" customFormat="1">
+    <row r="205" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A205" s="50">
         <v>92130112</v>
       </c>
@@ -20226,7 +20269,7 @@
       </c>
       <c r="AL205" s="44"/>
     </row>
-    <row r="206" spans="1:38" s="7" customFormat="1">
+    <row r="206" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A206" s="50">
         <v>92130113</v>
       </c>
@@ -20298,7 +20341,7 @@
       </c>
       <c r="AL206" s="44"/>
     </row>
-    <row r="207" spans="1:38" s="7" customFormat="1">
+    <row r="207" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A207" s="50">
         <v>92130114</v>
       </c>
@@ -20370,7 +20413,7 @@
       </c>
       <c r="AL207" s="44"/>
     </row>
-    <row r="208" spans="1:38" s="7" customFormat="1">
+    <row r="208" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A208" s="50">
         <v>92330117</v>
       </c>
@@ -20447,7 +20490,7 @@
       <c r="AC208" s="44"/>
       <c r="AD208" s="44"/>
     </row>
-    <row r="209" spans="1:38" s="7" customFormat="1">
+    <row r="209" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A209" s="50">
         <v>92530107</v>
       </c>
@@ -20518,7 +20561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:38" s="7" customFormat="1">
+    <row r="210" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A210" s="50">
         <v>92530108</v>
       </c>
@@ -20589,7 +20632,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:38" s="7" customFormat="1">
+    <row r="211" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A211" s="50">
         <v>92530109</v>
       </c>
@@ -20660,7 +20703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:38" s="7" customFormat="1">
+    <row r="212" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A212" s="50">
         <v>92530110</v>
       </c>
@@ -20731,7 +20774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:38" s="7" customFormat="1">
+    <row r="213" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A213" s="50">
         <v>92530111</v>
       </c>
@@ -20802,7 +20845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:38" s="7" customFormat="1">
+    <row r="214" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A214" s="50">
         <v>92530112</v>
       </c>
@@ -20873,7 +20916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:38" s="7" customFormat="1">
+    <row r="215" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A215" s="50">
         <v>92530113</v>
       </c>
@@ -20944,7 +20987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:38" s="7" customFormat="1">
+    <row r="216" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A216" s="50">
         <v>92530114</v>
       </c>
@@ -21015,7 +21058,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:38" s="7" customFormat="1">
+    <row r="217" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A217" s="50">
         <v>92530115</v>
       </c>
@@ -21086,7 +21129,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:38" s="7" customFormat="1">
+    <row r="218" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A218" s="50">
         <v>93130117</v>
       </c>
@@ -21161,7 +21204,7 @@
       </c>
       <c r="AL218" s="44"/>
     </row>
-    <row r="219" spans="1:38" s="7" customFormat="1">
+    <row r="219" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A219" s="50">
         <v>93130118</v>
       </c>
@@ -21236,7 +21279,7 @@
       </c>
       <c r="AL219" s="44"/>
     </row>
-    <row r="220" spans="1:38" s="7" customFormat="1">
+    <row r="220" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A220" s="50">
         <v>93230102</v>
       </c>
@@ -21310,7 +21353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:38" s="7" customFormat="1">
+    <row r="221" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A221" s="50">
         <v>93230205</v>
       </c>
@@ -21384,7 +21427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:38" s="7" customFormat="1">
+    <row r="222" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A222" s="50">
         <v>93230206</v>
       </c>
@@ -21458,7 +21501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:38" s="7" customFormat="1">
+    <row r="223" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A223" s="50">
         <v>93230207</v>
       </c>
@@ -21532,7 +21575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:38" s="7" customFormat="1">
+    <row r="224" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A224" s="50">
         <v>93230208</v>
       </c>
@@ -21612,7 +21655,7 @@
       <c r="AC224" s="6"/>
       <c r="AD224" s="6"/>
     </row>
-    <row r="225" spans="1:38" s="7" customFormat="1">
+    <row r="225" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A225" s="50">
         <v>93230305</v>
       </c>
@@ -21692,7 +21735,7 @@
       <c r="AC225" s="6"/>
       <c r="AD225" s="6"/>
     </row>
-    <row r="226" spans="1:38" s="7" customFormat="1">
+    <row r="226" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A226" s="50">
         <v>93230404</v>
       </c>
@@ -21772,7 +21815,7 @@
       <c r="AC226" s="6"/>
       <c r="AD226" s="6"/>
     </row>
-    <row r="227" spans="1:38" s="7" customFormat="1">
+    <row r="227" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A227" s="50">
         <v>93230405</v>
       </c>
@@ -21852,7 +21895,7 @@
       <c r="AC227" s="6"/>
       <c r="AD227" s="6"/>
     </row>
-    <row r="228" spans="1:38" s="7" customFormat="1">
+    <row r="228" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A228" s="50">
         <v>93330118</v>
       </c>
@@ -21929,7 +21972,7 @@
       <c r="AC228" s="44"/>
       <c r="AD228" s="44"/>
     </row>
-    <row r="229" spans="1:38" s="7" customFormat="1">
+    <row r="229" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A229" s="50">
         <v>93330119</v>
       </c>
@@ -22009,7 +22052,7 @@
       <c r="AC229" s="44"/>
       <c r="AD229" s="44"/>
     </row>
-    <row r="230" spans="1:38" s="7" customFormat="1">
+    <row r="230" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A230" s="50">
         <v>93330120</v>
       </c>
@@ -22089,7 +22132,7 @@
       <c r="AC230" s="44"/>
       <c r="AD230" s="44"/>
     </row>
-    <row r="231" spans="1:38" s="7" customFormat="1">
+    <row r="231" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A231" s="50">
         <v>93330121</v>
       </c>
@@ -22169,7 +22212,7 @@
       <c r="AC231" s="44"/>
       <c r="AD231" s="44"/>
     </row>
-    <row r="232" spans="1:38" s="7" customFormat="1">
+    <row r="232" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A232" s="50">
         <v>93430118</v>
       </c>
@@ -22249,7 +22292,7 @@
       <c r="AC232" s="44"/>
       <c r="AD232" s="44"/>
     </row>
-    <row r="233" spans="1:38" s="7" customFormat="1">
+    <row r="233" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A233" s="50">
         <v>93530118</v>
       </c>
@@ -22320,7 +22363,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:38" s="7" customFormat="1">
+    <row r="234" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A234" s="50">
         <v>93530119</v>
       </c>
@@ -22391,7 +22434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:38" s="7" customFormat="1">
+    <row r="235" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A235" s="50">
         <v>93530120</v>
       </c>
@@ -22462,7 +22505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:38" s="7" customFormat="1">
+    <row r="236" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A236" s="50">
         <v>93530121</v>
       </c>
@@ -22533,7 +22576,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:38" s="7" customFormat="1">
+    <row r="237" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A237" s="50">
         <v>93530122</v>
       </c>
@@ -22604,7 +22647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:38" s="7" customFormat="1">
+    <row r="238" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A238" s="50">
         <v>93530123</v>
       </c>
@@ -22748,7 +22791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:38" s="7" customFormat="1">
+    <row r="240" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A240" s="50">
         <v>94130115</v>
       </c>
@@ -22821,7 +22864,7 @@
       </c>
       <c r="AL240" s="44"/>
     </row>
-    <row r="241" spans="1:38" s="7" customFormat="1">
+    <row r="241" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A241" s="48">
         <v>94130116</v>
       </c>
@@ -22894,7 +22937,7 @@
       </c>
       <c r="AL241" s="44"/>
     </row>
-    <row r="242" spans="1:38" s="7" customFormat="1">
+    <row r="242" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A242" s="50">
         <v>94230403</v>
       </c>
@@ -22967,7 +23010,7 @@
       </c>
       <c r="AL242" s="6"/>
     </row>
-    <row r="243" spans="1:38" s="7" customFormat="1">
+    <row r="243" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A243" s="50">
         <v>94430116</v>
       </c>
@@ -23045,7 +23088,7 @@
       <c r="AC243" s="44"/>
       <c r="AD243" s="44"/>
     </row>
-    <row r="244" spans="1:38" s="7" customFormat="1">
+    <row r="244" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A244" s="50">
         <v>94430117</v>
       </c>
@@ -23123,17 +23166,17 @@
       <c r="AC244" s="44"/>
       <c r="AD244" s="44"/>
     </row>
-    <row r="245" spans="1:38" s="7" customFormat="1">
+    <row r="245" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A245" s="50">
         <v>94530116</v>
       </c>
-      <c r="B245" s="58" t="s">
+      <c r="B245" s="57" t="s">
         <v>968</v>
       </c>
-      <c r="C245" s="58" t="s">
+      <c r="C245" s="57" t="s">
         <v>865</v>
       </c>
-      <c r="D245" s="58" t="s">
+      <c r="D245" s="57" t="s">
         <v>2</v>
       </c>
       <c r="E245" s="6" t="s">
@@ -23142,35 +23185,35 @@
       <c r="F245" s="11" t="s">
         <v>1031</v>
       </c>
-      <c r="G245" s="59" t="s">
+      <c r="G245" s="58" t="s">
         <v>1032</v>
       </c>
-      <c r="H245" s="59" t="s">
+      <c r="H245" s="58" t="s">
         <v>1033</v>
       </c>
-      <c r="I245" s="59" t="s">
+      <c r="I245" s="58" t="s">
         <v>1034</v>
       </c>
-      <c r="J245" s="58" t="s">
+      <c r="J245" s="57" t="s">
         <v>796</v>
       </c>
-      <c r="K245" s="58" t="s">
+      <c r="K245" s="57" t="s">
         <v>231</v>
       </c>
-      <c r="L245" s="58" t="s">
+      <c r="L245" s="57" t="s">
         <v>910</v>
       </c>
-      <c r="M245" s="58" t="s">
+      <c r="M245" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="N245" s="58" t="s">
+      <c r="N245" s="57" t="s">
         <v>872</v>
       </c>
-      <c r="O245" s="58" t="s">
+      <c r="O245" s="57" t="s">
         <v>873</v>
       </c>
-      <c r="P245" s="58"/>
-      <c r="Q245" s="58" t="s">
+      <c r="P245" s="57"/>
+      <c r="Q245" s="57" t="s">
         <v>17</v>
       </c>
       <c r="R245" s="6" t="s">
@@ -23196,17 +23239,17 @@
       </c>
       <c r="AL245" s="44"/>
     </row>
-    <row r="246" spans="1:38" s="7" customFormat="1">
+    <row r="246" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A246" s="50">
         <v>94530117</v>
       </c>
-      <c r="B246" s="58" t="s">
+      <c r="B246" s="57" t="s">
         <v>968</v>
       </c>
-      <c r="C246" s="58" t="s">
+      <c r="C246" s="57" t="s">
         <v>865</v>
       </c>
-      <c r="D246" s="58" t="s">
+      <c r="D246" s="57" t="s">
         <v>2</v>
       </c>
       <c r="E246" s="6" t="s">
@@ -23215,35 +23258,35 @@
       <c r="F246" s="11" t="s">
         <v>1035</v>
       </c>
-      <c r="G246" s="59" t="s">
+      <c r="G246" s="58" t="s">
         <v>1036</v>
       </c>
-      <c r="H246" s="59" t="s">
+      <c r="H246" s="58" t="s">
         <v>1290</v>
       </c>
-      <c r="I246" s="59" t="s">
+      <c r="I246" s="58" t="s">
         <v>1037</v>
       </c>
-      <c r="J246" s="58" t="s">
+      <c r="J246" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="K246" s="58" t="s">
+      <c r="K246" s="57" t="s">
         <v>231</v>
       </c>
-      <c r="L246" s="58" t="s">
+      <c r="L246" s="57" t="s">
         <v>910</v>
       </c>
-      <c r="M246" s="58" t="s">
+      <c r="M246" s="57" t="s">
         <v>8</v>
       </c>
-      <c r="N246" s="58" t="s">
+      <c r="N246" s="57" t="s">
         <v>872</v>
       </c>
-      <c r="O246" s="58" t="s">
+      <c r="O246" s="57" t="s">
         <v>873</v>
       </c>
-      <c r="P246" s="58"/>
-      <c r="Q246" s="58" t="s">
+      <c r="P246" s="57"/>
+      <c r="Q246" s="57" t="s">
         <v>17</v>
       </c>
       <c r="R246" s="6" t="s">
@@ -23269,7 +23312,7 @@
       </c>
       <c r="AL246" s="44"/>
     </row>
-    <row r="247" spans="1:38" s="7" customFormat="1">
+    <row r="247" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A247" s="48">
         <v>910199999</v>
       </c>
@@ -23339,7 +23382,7 @@
       </c>
       <c r="AL247" s="6"/>
     </row>
-    <row r="248" spans="1:38" s="7" customFormat="1">
+    <row r="248" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A248" s="50">
         <v>920199999</v>
       </c>
@@ -23408,7 +23451,7 @@
       </c>
       <c r="AL248" s="6"/>
     </row>
-    <row r="249" spans="1:38" s="7" customFormat="1">
+    <row r="249" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A249" s="50">
         <v>920299999</v>
       </c>
@@ -23477,7 +23520,7 @@
       </c>
       <c r="AL249" s="6"/>
     </row>
-    <row r="250" spans="1:38" s="7" customFormat="1">
+    <row r="250" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A250" s="50">
         <v>920399999</v>
       </c>
@@ -23546,7 +23589,7 @@
       </c>
       <c r="AL250" s="6"/>
     </row>
-    <row r="251" spans="1:38" s="7" customFormat="1">
+    <row r="251" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A251" s="50">
         <v>920499999</v>
       </c>
@@ -23615,7 +23658,7 @@
       </c>
       <c r="AL251" s="6"/>
     </row>
-    <row r="252" spans="1:38" s="6" customFormat="1">
+    <row r="252" spans="1:38" s="6" customFormat="1" hidden="1">
       <c r="A252" s="50">
         <v>920599999</v>
       </c>
@@ -23691,7 +23734,7 @@
       <c r="AC252" s="7"/>
       <c r="AD252" s="7"/>
     </row>
-    <row r="253" spans="1:38" s="7" customFormat="1">
+    <row r="253" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A253" s="50">
         <v>920699999</v>
       </c>
@@ -23767,7 +23810,7 @@
       <c r="AK253" s="6"/>
       <c r="AL253" s="6"/>
     </row>
-    <row r="254" spans="1:38" s="7" customFormat="1">
+    <row r="254" spans="1:38" s="7" customFormat="1" hidden="1">
       <c r="A254" s="50">
         <v>920799999</v>
       </c>
@@ -23843,7 +23886,7 @@
       <c r="AK254" s="6"/>
       <c r="AL254" s="6"/>
     </row>
-    <row r="255" spans="1:38" s="44" customFormat="1">
+    <row r="255" spans="1:38" s="44" customFormat="1" hidden="1">
       <c r="A255" s="50">
         <v>920899999</v>
       </c>
@@ -23920,7 +23963,7 @@
       <c r="AD255" s="7"/>
       <c r="AL255" s="6"/>
     </row>
-    <row r="256" spans="1:38" s="44" customFormat="1">
+    <row r="256" spans="1:38" s="44" customFormat="1" hidden="1">
       <c r="A256" s="50">
         <v>920999999</v>
       </c>
@@ -23997,7 +24040,7 @@
       <c r="AD256" s="7"/>
       <c r="AL256" s="6"/>
     </row>
-    <row r="257" spans="1:38" s="44" customFormat="1">
+    <row r="257" spans="1:38" s="44" customFormat="1" hidden="1">
       <c r="A257" s="50">
         <v>921099999</v>
       </c>
@@ -24074,7 +24117,7 @@
       <c r="AD257" s="7"/>
       <c r="AL257" s="6"/>
     </row>
-    <row r="258" spans="1:38" s="44" customFormat="1">
+    <row r="258" spans="1:38" s="44" customFormat="1" hidden="1">
       <c r="A258" s="50">
         <v>921199999</v>
       </c>
@@ -24151,7 +24194,7 @@
       <c r="AD258" s="7"/>
       <c r="AL258" s="6"/>
     </row>
-    <row r="259" spans="1:38" s="44" customFormat="1">
+    <row r="259" spans="1:38" s="44" customFormat="1" hidden="1">
       <c r="A259" s="50">
         <v>921299999</v>
       </c>
@@ -24228,7 +24271,7 @@
       <c r="AD259" s="7"/>
       <c r="AL259" s="6"/>
     </row>
-    <row r="260" spans="1:38" s="44" customFormat="1">
+    <row r="260" spans="1:38" s="44" customFormat="1" hidden="1">
       <c r="A260" s="50">
         <v>921399999</v>
       </c>
@@ -24305,7 +24348,7 @@
       <c r="AD260" s="7"/>
       <c r="AL260" s="7"/>
     </row>
-    <row r="261" spans="1:38" s="44" customFormat="1">
+    <row r="261" spans="1:38" s="44" customFormat="1" hidden="1">
       <c r="A261" s="50">
         <v>921499999</v>
       </c>
@@ -24382,7 +24425,7 @@
       <c r="AD261" s="7"/>
       <c r="AL261" s="7"/>
     </row>
-    <row r="262" spans="1:38" s="44" customFormat="1">
+    <row r="262" spans="1:38" s="44" customFormat="1" hidden="1">
       <c r="A262" s="50">
         <v>921599999</v>
       </c>
@@ -24459,7 +24502,7 @@
       <c r="AD262" s="7"/>
       <c r="AL262" s="7"/>
     </row>
-    <row r="263" spans="1:38" s="44" customFormat="1">
+    <row r="263" spans="1:38" s="44" customFormat="1" hidden="1">
       <c r="A263" s="50">
         <v>930199999</v>
       </c>
@@ -24530,7 +24573,7 @@
       </c>
       <c r="AL263" s="13"/>
     </row>
-    <row r="264" spans="1:38" s="44" customFormat="1">
+    <row r="264" spans="1:38" s="44" customFormat="1" hidden="1">
       <c r="A264" s="50">
         <v>940199999</v>
       </c>
@@ -24607,7 +24650,7 @@
       <c r="AD264" s="7"/>
       <c r="AL264" s="13"/>
     </row>
-    <row r="265" spans="1:38" s="44" customFormat="1">
+    <row r="265" spans="1:38" s="44" customFormat="1" hidden="1">
       <c r="A265" s="50">
         <v>940499999</v>
       </c>
@@ -24684,7 +24727,7 @@
       <c r="AD265" s="7"/>
       <c r="AL265" s="13"/>
     </row>
-    <row r="266" spans="1:38" s="44" customFormat="1">
+    <row r="266" spans="1:38" s="44" customFormat="1" hidden="1">
       <c r="A266" s="50">
         <v>940299999</v>
       </c>
@@ -24761,7 +24804,7 @@
       <c r="AD266" s="7"/>
       <c r="AL266" s="6"/>
     </row>
-    <row r="267" spans="1:38" s="44" customFormat="1">
+    <row r="267" spans="1:38" s="44" customFormat="1" hidden="1">
       <c r="A267" s="50">
         <v>940599999</v>
       </c>
@@ -24838,7 +24881,7 @@
       <c r="AD267" s="7"/>
       <c r="AL267" s="6"/>
     </row>
-    <row r="268" spans="1:38" s="44" customFormat="1">
+    <row r="268" spans="1:38" s="44" customFormat="1" hidden="1">
       <c r="A268" s="50">
         <v>940399999</v>
       </c>
@@ -24915,7 +24958,7 @@
       <c r="AD268" s="7"/>
       <c r="AL268" s="13"/>
     </row>
-    <row r="269" spans="1:38" s="44" customFormat="1">
+    <row r="269" spans="1:38" s="44" customFormat="1" hidden="1">
       <c r="A269" s="50">
         <v>940699999</v>
       </c>
@@ -24992,16 +25035,160 @@
       <c r="AD269" s="7"/>
       <c r="AL269" s="13"/>
     </row>
-    <row r="271" spans="1:38">
-      <c r="F271" s="54"/>
-      <c r="G271" s="54"/>
-    </row>
-    <row r="272" spans="1:38">
-      <c r="F272" s="7"/>
-      <c r="G272" s="7"/>
+    <row r="270" spans="1:38">
+      <c r="A270" s="49">
+        <v>95120118</v>
+      </c>
+      <c r="B270" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C270" s="13" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D270" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="E270" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="F270" s="59" t="s">
+        <v>496</v>
+      </c>
+      <c r="G270" s="59" t="s">
+        <v>1355</v>
+      </c>
+      <c r="H270" s="60" t="s">
+        <v>1365</v>
+      </c>
+      <c r="I270" s="60" t="s">
+        <v>1356</v>
+      </c>
+      <c r="J270" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="K270" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="L270" s="60" t="s">
+        <v>95</v>
+      </c>
+      <c r="M270" s="60" t="s">
+        <v>289</v>
+      </c>
+      <c r="N270" s="59" t="s">
+        <v>1357</v>
+      </c>
+      <c r="O270" s="59" t="s">
+        <v>1358</v>
+      </c>
+      <c r="Q270" s="60" t="s">
+        <v>96</v>
+      </c>
+      <c r="R270" s="60" t="s">
+        <v>1298</v>
+      </c>
+      <c r="S270" s="44">
+        <v>0</v>
+      </c>
+      <c r="T270" s="44">
+        <v>0</v>
+      </c>
+      <c r="U270" s="44">
+        <v>0</v>
+      </c>
+      <c r="V270" s="44">
+        <v>0</v>
+      </c>
+      <c r="W270" s="44">
+        <v>0</v>
+      </c>
+      <c r="X270" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="1:38" s="60" customFormat="1">
+      <c r="A271" s="49">
+        <v>95520111</v>
+      </c>
+      <c r="B271" s="13" t="s">
+        <v>968</v>
+      </c>
+      <c r="C271" s="13" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D271" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="E271" s="40" t="s">
+        <v>104</v>
+      </c>
+      <c r="F271" s="60" t="s">
+        <v>1364</v>
+      </c>
+      <c r="G271" s="60" t="s">
+        <v>1363</v>
+      </c>
+      <c r="H271" s="60" t="s">
+        <v>1360</v>
+      </c>
+      <c r="I271" s="60" t="s">
+        <v>1361</v>
+      </c>
+      <c r="J271" s="60" t="s">
+        <v>5</v>
+      </c>
+      <c r="K271" s="60" t="s">
+        <v>6</v>
+      </c>
+      <c r="L271" s="60" t="s">
+        <v>234</v>
+      </c>
+      <c r="M271" s="60" t="s">
+        <v>8</v>
+      </c>
+      <c r="N271" s="60" t="s">
+        <v>1359</v>
+      </c>
+      <c r="O271" s="24" t="s">
+        <v>1362</v>
+      </c>
+      <c r="R271" s="61" t="s">
+        <v>1298</v>
+      </c>
+      <c r="S271" s="44">
+        <v>0</v>
+      </c>
+      <c r="T271" s="44">
+        <v>0</v>
+      </c>
+      <c r="U271" s="44">
+        <v>0</v>
+      </c>
+      <c r="V271" s="44">
+        <v>0</v>
+      </c>
+      <c r="W271" s="44">
+        <v>0</v>
+      </c>
+      <c r="X271" s="6">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <autoFilter ref="A1:AN271">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Educación"/>
+        <filter val="Trabajo"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="3">
+      <filters>
+        <filter val="Políticas Públicas y Esfuerzo Económico"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
@@ -25014,7 +25201,7 @@
   <dimension ref="A1:B27"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="17.25" customHeight="1"/>

</xml_diff>

<commit_message>
Add data proyecto SURGE (prueba)
</commit_message>
<xml_diff>
--- a/Data/Base_fichas_indicadores.xlsx
+++ b/Data/Base_fichas_indicadores.xlsx
@@ -16,14 +16,14 @@
     <sheet name="REF_COLUMNAS" sheetId="5" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BASE_FICHAS!$A$1:$AN$271</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BASE_FICHAS!$A$1:$AN$269</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4218" uniqueCount="1366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4316" uniqueCount="1383">
   <si>
     <t>id</t>
   </si>
@@ -4162,37 +4162,89 @@
     <t>Afrodescendientes</t>
   </si>
   <si>
-    <t>Cantidad anual de becas educativas otorgadas a personas afrodescendientes</t>
-  </si>
-  <si>
     <t>Para cada año calcular: Cantidad de becas educativas otorgadas a personas afrodescendientes.</t>
   </si>
   <si>
     <t>OPP  2019 "Acciones afirmativas para personas afrodescendientes"</t>
   </si>
   <si>
-    <t>Consultoría Proyecto SURGE (ACNUDH - Uruguay) con base en OPP  2019 "Acciones afirmativas para personas afrodescendientes"</t>
-  </si>
-  <si>
-    <t>Oficina Nacional de Servicio Civil</t>
-  </si>
-  <si>
     <t>El indicador mide el porcentaje de personas que ingresaron al estado en el marco de la Ley 19.122 en relación al total de ingresos.</t>
   </si>
   <si>
     <t>Para cada año calcular: (Cantidad de ingresos de personas afrodescendientes a cargos públicos en el marco de la Ley 19.122 / Cantidad de ingresos de personas a cargos públicos en el marco de la Ley 19.122)*100</t>
   </si>
   <si>
-    <t>Consultoría Proyecto SURGE (ACNUDH - Uruguay) con base en Oficina Nacional del Servcio Civil</t>
-  </si>
-  <si>
-    <t>Porcentaje de ingresos de afrodescendientes a cargos públicos (Ley 19.122)</t>
-  </si>
-  <si>
-    <t>Cumplimiento de la couta de ingresos de afrodescendientes a cargos públicos (Ley 19.122)</t>
-  </si>
-  <si>
     <t>El indicador mide la cantidad anual de becas educativas otorgadas a personas afrodescendientes.</t>
+  </si>
+  <si>
+    <t>Proyecto SURGE</t>
+  </si>
+  <si>
+    <t>(Proyecto SURGE) Becas educativas</t>
+  </si>
+  <si>
+    <t>(Proyecto SURGE) Cantidad anual de becas educativas otorgadas a personas afrodescendientes</t>
+  </si>
+  <si>
+    <t>Consultoría Proyecto SURGE (OACNUDH - Uruguay) con base en OPP  2019 "Acciones afirmativas para personas afrodescendientes"</t>
+  </si>
+  <si>
+    <t>Datos elaborados en el marco de una consultoría del Proyecto SURGE de OACNUDH-Uruguay.</t>
+  </si>
+  <si>
+    <t>(Proyecto SURGE) Cumplimiento de la couta de ingresos de afrodescendientes a cargos públicos (Ley 19.122)</t>
+  </si>
+  <si>
+    <t>(Proyecto SURGE) Porcentaje de ingresos de afrodescendientes a cargos públicos (Ley 19.122)</t>
+  </si>
+  <si>
+    <t>Oficina Nacional del Servicio Civil</t>
+  </si>
+  <si>
+    <t>Consultoría Proyecto SURGE (OACNUDH - Uruguay) con base en Oficina Nacional del Servcio Civil</t>
+  </si>
+  <si>
+    <t>(Proyecto SURGE) Tenencia insegura de la vivienda</t>
+  </si>
+  <si>
+    <t>(Proyecto SURGE) Porcentaje de personas en hogares con tenencia insegura</t>
+  </si>
+  <si>
+    <t>El indicador mide el porcentaje de personas residiendo en viviendas con tenencia insegura. Esta situación es aquella en que las personas residen en viviendas de las cuales son propietarios del inmueble (ya pago o en proceso) pero no del terreno; son ocupantes gratuitos (en préstamo), en relación de dependencia o sin permiso del propietario.</t>
+  </si>
+  <si>
+    <t>ECH-INE</t>
+  </si>
+  <si>
+    <t>Consultoría Proyecto SURGE (OACNUDH - Uruguay) con base en ECH-INE</t>
+  </si>
+  <si>
+    <t>Ascendencia étnico-racial, región</t>
+  </si>
+  <si>
+    <t>(Proyecto SURGE) Asentamientos</t>
+  </si>
+  <si>
+    <t>(Proyecto SURGE) Porcentaje de personas que viven en asentamientos</t>
+  </si>
+  <si>
+    <t>(Proyecto SURGE) Tasa de actividad</t>
+  </si>
+  <si>
+    <t>Ascendencia étnico-racial, sexo</t>
+  </si>
+  <si>
+    <t>Datos elaborados en el marco de una consultoría del Proyecto SURGE de OACNUDH-Uruguay. Desde marzo de 2020 hasta junio de 2021 se interrumpió el relevamiento presencial y se aplicó de manera telefónica un cuestionario restringido con el objetivo de continuar publicando los indicadores de ingresos y mercado de trabajo. En ese período la encuesta pasó a ser de paneles rotativos elegidos al azar a partir de los casos respondentes del año anterior. 
+Los indicadores de trabajo del año 2020 se construyen con la encuesta presencial realizada hasta marzo de 2020 y posteriormente con la encuesta telefónica panel (siempre que la información haya sido incluida en el formulario).</t>
+  </si>
+  <si>
+    <t>(Proyecto SURGE) Tasa de desempleo</t>
+  </si>
+  <si>
+    <t>(Proyecto SURGE) Tasa de empleo</t>
+  </si>
+  <si>
+    <t>(Proyecto SURGE) Tasa de subempleo</t>
   </si>
 </sst>
 </file>
@@ -4203,7 +4255,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.000&quot;&quot;;\-#,##0.000&quot;&quot;"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -4285,6 +4337,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -4309,7 +4367,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4459,11 +4517,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -4784,12 +4858,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1" filterMode="1"/>
-  <dimension ref="A1:AL271"/>
+  <dimension ref="A1:AL277"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="D1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E111" sqref="E111"/>
-      <selection pane="bottomLeft" activeCell="E278" sqref="E278"/>
+      <selection pane="bottomLeft" activeCell="D270" sqref="A270:XFD271"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -25035,148 +25109,580 @@
       <c r="AD269" s="7"/>
       <c r="AL269" s="13"/>
     </row>
-    <row r="270" spans="1:38">
-      <c r="A270" s="49">
+    <row r="270" spans="1:38" s="16" customFormat="1">
+      <c r="A270" s="59">
         <v>95120118</v>
       </c>
-      <c r="B270" s="13" t="s">
+      <c r="B270" s="16" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C270" s="16" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D270" s="60" t="s">
+        <v>104</v>
+      </c>
+      <c r="E270" s="60" t="s">
+        <v>104</v>
+      </c>
+      <c r="F270" s="60" t="s">
+        <v>1361</v>
+      </c>
+      <c r="G270" s="16" t="s">
+        <v>1362</v>
+      </c>
+      <c r="H270" s="61" t="s">
+        <v>1359</v>
+      </c>
+      <c r="I270" s="61" t="s">
+        <v>1355</v>
+      </c>
+      <c r="J270" s="61" t="s">
+        <v>29</v>
+      </c>
+      <c r="K270" s="61" t="s">
+        <v>6</v>
+      </c>
+      <c r="L270" s="61" t="s">
+        <v>95</v>
+      </c>
+      <c r="M270" s="61" t="s">
+        <v>289</v>
+      </c>
+      <c r="N270" s="62" t="s">
+        <v>1356</v>
+      </c>
+      <c r="O270" s="62" t="s">
+        <v>1363</v>
+      </c>
+      <c r="Q270" s="61" t="s">
+        <v>96</v>
+      </c>
+      <c r="R270" s="61" t="s">
+        <v>1364</v>
+      </c>
+      <c r="S270" s="63">
+        <v>0</v>
+      </c>
+      <c r="T270" s="63">
+        <v>0</v>
+      </c>
+      <c r="U270" s="63">
+        <v>0</v>
+      </c>
+      <c r="V270" s="63">
+        <v>0</v>
+      </c>
+      <c r="W270" s="63">
+        <v>0</v>
+      </c>
+      <c r="X270" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="271" spans="1:38" s="61" customFormat="1">
+      <c r="A271" s="59">
+        <v>95520111</v>
+      </c>
+      <c r="B271" s="16" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C271" s="16" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D271" s="60" t="s">
+        <v>104</v>
+      </c>
+      <c r="E271" s="60" t="s">
+        <v>104</v>
+      </c>
+      <c r="F271" s="60" t="s">
+        <v>1365</v>
+      </c>
+      <c r="G271" s="16" t="s">
+        <v>1366</v>
+      </c>
+      <c r="H271" s="61" t="s">
+        <v>1357</v>
+      </c>
+      <c r="I271" s="61" t="s">
+        <v>1358</v>
+      </c>
+      <c r="J271" s="61" t="s">
+        <v>5</v>
+      </c>
+      <c r="K271" s="61" t="s">
+        <v>6</v>
+      </c>
+      <c r="L271" s="61" t="s">
+        <v>234</v>
+      </c>
+      <c r="M271" s="61" t="s">
+        <v>8</v>
+      </c>
+      <c r="N271" s="61" t="s">
+        <v>1367</v>
+      </c>
+      <c r="O271" s="64" t="s">
+        <v>1368</v>
+      </c>
+      <c r="Q271" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="R271" s="61" t="s">
+        <v>1364</v>
+      </c>
+      <c r="S271" s="63">
+        <v>0</v>
+      </c>
+      <c r="T271" s="63">
+        <v>0</v>
+      </c>
+      <c r="U271" s="63">
+        <v>0</v>
+      </c>
+      <c r="V271" s="63">
+        <v>0</v>
+      </c>
+      <c r="W271" s="63">
+        <v>0</v>
+      </c>
+      <c r="X271" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272" spans="1:38" s="16" customFormat="1">
+      <c r="A272" s="65">
+        <v>95230101</v>
+      </c>
+      <c r="B272" s="16" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C272" s="16" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D272" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E272" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F272" s="60" t="s">
+        <v>1369</v>
+      </c>
+      <c r="G272" s="16" t="s">
+        <v>1370</v>
+      </c>
+      <c r="H272" s="16" t="s">
+        <v>1371</v>
+      </c>
+      <c r="I272" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="J272" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="K272" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="L272" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="M272" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="N272" s="16" t="s">
+        <v>1372</v>
+      </c>
+      <c r="O272" s="66" t="s">
+        <v>1373</v>
+      </c>
+      <c r="P272" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q272" s="16" t="s">
+        <v>1374</v>
+      </c>
+      <c r="R272" s="61" t="s">
+        <v>1364</v>
+      </c>
+      <c r="S272" s="16">
         <v>1</v>
       </c>
-      <c r="C270" s="13" t="s">
+      <c r="T272" s="16">
+        <v>0</v>
+      </c>
+      <c r="U272" s="16">
+        <v>0</v>
+      </c>
+      <c r="V272" s="16">
+        <v>0</v>
+      </c>
+      <c r="W272" s="16">
+        <v>0</v>
+      </c>
+      <c r="X272" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273" spans="1:24" s="16" customFormat="1">
+      <c r="A273" s="65">
+        <v>95230501</v>
+      </c>
+      <c r="B273" s="16" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C273" s="16" t="s">
         <v>1354</v>
       </c>
-      <c r="D270" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="E270" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="F270" s="59" t="s">
-        <v>496</v>
-      </c>
-      <c r="G270" s="59" t="s">
-        <v>1355</v>
-      </c>
-      <c r="H270" s="60" t="s">
-        <v>1365</v>
-      </c>
-      <c r="I270" s="60" t="s">
-        <v>1356</v>
-      </c>
-      <c r="J270" s="60" t="s">
-        <v>29</v>
-      </c>
-      <c r="K270" s="60" t="s">
+      <c r="D273" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E273" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="F273" s="60" t="s">
+        <v>1375</v>
+      </c>
+      <c r="G273" s="16" t="s">
+        <v>1376</v>
+      </c>
+      <c r="H273" s="16" t="s">
+        <v>375</v>
+      </c>
+      <c r="I273" s="16" t="s">
+        <v>154</v>
+      </c>
+      <c r="J273" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="K273" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="L270" s="60" t="s">
-        <v>95</v>
-      </c>
-      <c r="M270" s="60" t="s">
-        <v>289</v>
-      </c>
-      <c r="N270" s="59" t="s">
-        <v>1357</v>
-      </c>
-      <c r="O270" s="59" t="s">
-        <v>1358</v>
-      </c>
-      <c r="Q270" s="60" t="s">
-        <v>96</v>
-      </c>
-      <c r="R270" s="60" t="s">
-        <v>1298</v>
-      </c>
-      <c r="S270" s="44">
-        <v>0</v>
-      </c>
-      <c r="T270" s="44">
-        <v>0</v>
-      </c>
-      <c r="U270" s="44">
-        <v>0</v>
-      </c>
-      <c r="V270" s="44">
-        <v>0</v>
-      </c>
-      <c r="W270" s="44">
-        <v>0</v>
-      </c>
-      <c r="X270" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="271" spans="1:38" s="60" customFormat="1">
-      <c r="A271" s="49">
-        <v>95520111</v>
-      </c>
-      <c r="B271" s="13" t="s">
-        <v>968</v>
-      </c>
-      <c r="C271" s="13" t="s">
+      <c r="L273" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="M273" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="N273" s="16" t="s">
+        <v>1372</v>
+      </c>
+      <c r="O273" s="66" t="s">
+        <v>1373</v>
+      </c>
+      <c r="Q273" s="16" t="s">
+        <v>1374</v>
+      </c>
+      <c r="R273" s="61" t="s">
+        <v>1364</v>
+      </c>
+      <c r="S273" s="16">
+        <v>1</v>
+      </c>
+      <c r="T273" s="16">
+        <v>1</v>
+      </c>
+      <c r="U273" s="16">
+        <v>1</v>
+      </c>
+      <c r="V273" s="16">
+        <v>1</v>
+      </c>
+      <c r="W273" s="16">
+        <v>1</v>
+      </c>
+      <c r="X273" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274" spans="1:24" s="67" customFormat="1">
+      <c r="A274" s="65">
+        <v>95530101</v>
+      </c>
+      <c r="B274" s="16" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C274" s="16" t="s">
         <v>1354</v>
       </c>
-      <c r="D271" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="E271" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="F271" s="60" t="s">
-        <v>1364</v>
-      </c>
-      <c r="G271" s="60" t="s">
-        <v>1363</v>
-      </c>
-      <c r="H271" s="60" t="s">
+      <c r="D274" s="67" t="s">
+        <v>2</v>
+      </c>
+      <c r="E274" s="67" t="s">
+        <v>3</v>
+      </c>
+      <c r="F274" s="60" t="s">
+        <v>1377</v>
+      </c>
+      <c r="G274" s="16" t="s">
+        <v>1377</v>
+      </c>
+      <c r="H274" s="67" t="s">
+        <v>1248</v>
+      </c>
+      <c r="I274" s="16" t="s">
+        <v>1063</v>
+      </c>
+      <c r="J274" s="16" t="s">
+        <v>1014</v>
+      </c>
+      <c r="K274" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="L274" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="M274" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="N274" s="16" t="s">
+        <v>1372</v>
+      </c>
+      <c r="O274" s="16" t="s">
+        <v>1373</v>
+      </c>
+      <c r="Q274" s="16" t="s">
+        <v>1378</v>
+      </c>
+      <c r="R274" s="63" t="s">
+        <v>1379</v>
+      </c>
+      <c r="S274" s="63">
+        <v>0</v>
+      </c>
+      <c r="T274" s="63">
+        <v>0</v>
+      </c>
+      <c r="U274" s="63">
+        <v>0</v>
+      </c>
+      <c r="V274" s="63">
+        <v>0</v>
+      </c>
+      <c r="W274" s="63">
+        <v>0</v>
+      </c>
+      <c r="X274" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275" spans="1:24" s="67" customFormat="1">
+      <c r="A275" s="65">
+        <v>95530102</v>
+      </c>
+      <c r="B275" s="16" t="s">
         <v>1360</v>
       </c>
-      <c r="I271" s="60" t="s">
-        <v>1361</v>
-      </c>
-      <c r="J271" s="60" t="s">
-        <v>5</v>
-      </c>
-      <c r="K271" s="60" t="s">
+      <c r="C275" s="16" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D275" s="67" t="s">
+        <v>2</v>
+      </c>
+      <c r="E275" s="67" t="s">
+        <v>3</v>
+      </c>
+      <c r="F275" s="60" t="s">
+        <v>1380</v>
+      </c>
+      <c r="G275" s="16" t="s">
+        <v>1380</v>
+      </c>
+      <c r="H275" s="67" t="s">
+        <v>1041</v>
+      </c>
+      <c r="I275" s="16" t="s">
+        <v>1065</v>
+      </c>
+      <c r="J275" s="16" t="s">
+        <v>1014</v>
+      </c>
+      <c r="K275" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="L271" s="60" t="s">
-        <v>234</v>
-      </c>
-      <c r="M271" s="60" t="s">
+      <c r="L275" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="M275" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="N271" s="60" t="s">
-        <v>1359</v>
-      </c>
-      <c r="O271" s="24" t="s">
-        <v>1362</v>
-      </c>
-      <c r="R271" s="61" t="s">
-        <v>1298</v>
-      </c>
-      <c r="S271" s="44">
-        <v>0</v>
-      </c>
-      <c r="T271" s="44">
-        <v>0</v>
-      </c>
-      <c r="U271" s="44">
-        <v>0</v>
-      </c>
-      <c r="V271" s="44">
-        <v>0</v>
-      </c>
-      <c r="W271" s="44">
-        <v>0</v>
-      </c>
-      <c r="X271" s="6">
+      <c r="N275" s="16" t="s">
+        <v>1372</v>
+      </c>
+      <c r="O275" s="66" t="s">
+        <v>1373</v>
+      </c>
+      <c r="Q275" s="16" t="s">
+        <v>1378</v>
+      </c>
+      <c r="R275" s="63" t="s">
+        <v>1379</v>
+      </c>
+      <c r="S275" s="63">
+        <v>0</v>
+      </c>
+      <c r="T275" s="63">
+        <v>0</v>
+      </c>
+      <c r="U275" s="63">
+        <v>0</v>
+      </c>
+      <c r="V275" s="63">
+        <v>0</v>
+      </c>
+      <c r="W275" s="63">
+        <v>0</v>
+      </c>
+      <c r="X275" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276" spans="1:24" s="67" customFormat="1">
+      <c r="A276" s="65">
+        <v>95530103</v>
+      </c>
+      <c r="B276" s="16" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C276" s="16" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D276" s="67" t="s">
+        <v>2</v>
+      </c>
+      <c r="E276" s="67" t="s">
+        <v>3</v>
+      </c>
+      <c r="F276" s="60" t="s">
+        <v>1381</v>
+      </c>
+      <c r="G276" s="16" t="s">
+        <v>1381</v>
+      </c>
+      <c r="H276" s="67" t="s">
+        <v>1015</v>
+      </c>
+      <c r="I276" s="16" t="s">
+        <v>1067</v>
+      </c>
+      <c r="J276" s="16" t="s">
+        <v>1014</v>
+      </c>
+      <c r="K276" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="L276" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="M276" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="N276" s="16" t="s">
+        <v>1372</v>
+      </c>
+      <c r="O276" s="66" t="s">
+        <v>1373</v>
+      </c>
+      <c r="Q276" s="16" t="s">
+        <v>1378</v>
+      </c>
+      <c r="R276" s="63" t="s">
+        <v>1379</v>
+      </c>
+      <c r="S276" s="63">
+        <v>0</v>
+      </c>
+      <c r="T276" s="63">
+        <v>0</v>
+      </c>
+      <c r="U276" s="63">
+        <v>0</v>
+      </c>
+      <c r="V276" s="63">
+        <v>0</v>
+      </c>
+      <c r="W276" s="63">
+        <v>0</v>
+      </c>
+      <c r="X276" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277" spans="1:24" s="67" customFormat="1">
+      <c r="A277" s="65">
+        <v>95530104</v>
+      </c>
+      <c r="B277" s="16" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C277" s="16" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D277" s="67" t="s">
+        <v>2</v>
+      </c>
+      <c r="E277" s="67" t="s">
+        <v>3</v>
+      </c>
+      <c r="F277" s="60" t="s">
+        <v>1382</v>
+      </c>
+      <c r="G277" s="16" t="s">
+        <v>1382</v>
+      </c>
+      <c r="H277" s="67" t="s">
+        <v>1249</v>
+      </c>
+      <c r="I277" s="16" t="s">
+        <v>1069</v>
+      </c>
+      <c r="J277" s="16" t="s">
+        <v>1014</v>
+      </c>
+      <c r="K277" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="L277" s="16" t="s">
+        <v>306</v>
+      </c>
+      <c r="M277" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="N277" s="16" t="s">
+        <v>1372</v>
+      </c>
+      <c r="O277" s="66" t="s">
+        <v>1373</v>
+      </c>
+      <c r="Q277" s="16" t="s">
+        <v>1378</v>
+      </c>
+      <c r="R277" s="63" t="s">
+        <v>1379</v>
+      </c>
+      <c r="S277" s="63">
+        <v>0</v>
+      </c>
+      <c r="T277" s="63">
+        <v>0</v>
+      </c>
+      <c r="U277" s="63">
+        <v>0</v>
+      </c>
+      <c r="V277" s="63">
+        <v>0</v>
+      </c>
+      <c r="W277" s="63">
+        <v>0</v>
+      </c>
+      <c r="X277" s="16">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
-  <autoFilter ref="A1:AN271">
+  <autoFilter ref="A1:AN269">
     <filterColumn colId="1">
       <filters>
         <filter val="Educación"/>

</xml_diff>

<commit_message>
Add ind Proyecto SURGE
</commit_message>
<xml_diff>
--- a/Data/Base_fichas_indicadores.xlsx
+++ b/Data/Base_fichas_indicadores.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="606"/>
+    <workbookView minimized="1" xWindow="-21720" yWindow="-120" windowWidth="21840" windowHeight="13140" tabRatio="606"/>
   </bookViews>
   <sheets>
     <sheet name="BASE_FICHAS" sheetId="4" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4316" uniqueCount="1383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4333" uniqueCount="1386">
   <si>
     <t>id</t>
   </si>
@@ -4213,12 +4213,6 @@
     <t>El indicador mide el porcentaje de personas residiendo en viviendas con tenencia insegura. Esta situación es aquella en que las personas residen en viviendas de las cuales son propietarios del inmueble (ya pago o en proceso) pero no del terreno; son ocupantes gratuitos (en préstamo), en relación de dependencia o sin permiso del propietario.</t>
   </si>
   <si>
-    <t>ECH-INE</t>
-  </si>
-  <si>
-    <t>Consultoría Proyecto SURGE (OACNUDH - Uruguay) con base en ECH-INE</t>
-  </si>
-  <si>
     <t>Ascendencia étnico-racial, región</t>
   </si>
   <si>
@@ -4245,6 +4239,21 @@
   </si>
   <si>
     <t>(Proyecto SURGE) Tasa de subempleo</t>
+  </si>
+  <si>
+    <t>No poseer cobertura de la seguridad social</t>
+  </si>
+  <si>
+    <t>(Proyecto SURGE) Porcentaje de ocupados que no aporta a la seguridad social</t>
+  </si>
+  <si>
+    <t>(Proyecto SURGE) Porcentaje de ocupados sin aporte a la seguridad social</t>
+  </si>
+  <si>
+    <t>Encuesta Continua de Hogares INE</t>
+  </si>
+  <si>
+    <t>Consultoría Proyecto SURGE (OACNUDH - Uruguay) con base en Encuesta Continua de Hogares (INE)</t>
   </si>
 </sst>
 </file>
@@ -4367,7 +4376,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4508,7 +4517,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -4520,8 +4528,6 @@
     <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -4538,6 +4544,12 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -4858,12 +4870,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1" filterMode="1"/>
-  <dimension ref="A1:AL277"/>
+  <dimension ref="A1:AL278"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="D1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="F1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A271" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E111" sqref="E111"/>
-      <selection pane="bottomLeft" activeCell="D270" sqref="A270:XFD271"/>
+      <selection pane="bottomLeft" activeCell="G278" sqref="G278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -4913,43 +4925,43 @@
       <c r="E1" s="26" t="s">
         <v>343</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="65" t="s">
         <v>483</v>
       </c>
       <c r="G1" s="26" t="s">
         <v>332</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="66" t="s">
         <v>333</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="66" t="s">
         <v>334</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="66" t="s">
         <v>335</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="66" t="s">
         <v>336</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="66" t="s">
         <v>337</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="66" t="s">
         <v>338</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="N1" s="66" t="s">
         <v>339</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="66" t="s">
         <v>340</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="P1" s="66" t="s">
         <v>341</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="Q1" s="66" t="s">
         <v>342</v>
       </c>
-      <c r="R1" s="54" t="s">
+      <c r="R1" s="66" t="s">
         <v>1299</v>
       </c>
       <c r="S1" s="26" t="s">
@@ -4984,7 +4996,7 @@
       <c r="E2" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="F2" s="30" t="s">
+      <c r="F2" s="65" t="s">
         <v>484</v>
       </c>
       <c r="G2" s="31" t="s">
@@ -5053,7 +5065,7 @@
       <c r="E3" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="F3" s="30" t="s">
+      <c r="F3" s="65" t="s">
         <v>485</v>
       </c>
       <c r="G3" s="31" t="s">
@@ -5121,7 +5133,7 @@
       <c r="E4" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="F4" s="30" t="s">
+      <c r="F4" s="65" t="s">
         <v>486</v>
       </c>
       <c r="G4" s="31" t="s">
@@ -5190,7 +5202,7 @@
       <c r="E5" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="F5" s="65" t="s">
         <v>487</v>
       </c>
       <c r="G5" s="6" t="s">
@@ -5259,7 +5271,7 @@
       <c r="E6" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="F6" s="30" t="s">
+      <c r="F6" s="65" t="s">
         <v>488</v>
       </c>
       <c r="G6" s="3" t="s">
@@ -5328,7 +5340,7 @@
       <c r="E7" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="65" t="s">
         <v>489</v>
       </c>
       <c r="G7" s="3" t="s">
@@ -5397,7 +5409,7 @@
       <c r="E8" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="65" t="s">
         <v>490</v>
       </c>
       <c r="G8" s="3" t="s">
@@ -5466,7 +5478,7 @@
       <c r="E9" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="F9" s="30" t="s">
+      <c r="F9" s="65" t="s">
         <v>491</v>
       </c>
       <c r="G9" s="6" t="s">
@@ -5534,7 +5546,7 @@
       <c r="E10" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="F10" s="30" t="s">
+      <c r="F10" s="65" t="s">
         <v>492</v>
       </c>
       <c r="G10" s="6" t="s">
@@ -5603,7 +5615,7 @@
       <c r="E11" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="F11" s="30" t="s">
+      <c r="F11" s="65" t="s">
         <v>493</v>
       </c>
       <c r="G11" s="6" t="s">
@@ -5672,7 +5684,7 @@
       <c r="E12" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="F12" s="30" t="s">
+      <c r="F12" s="65" t="s">
         <v>494</v>
       </c>
       <c r="G12" s="6" t="s">
@@ -5740,7 +5752,7 @@
       <c r="E13" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="F13" s="30" t="s">
+      <c r="F13" s="65" t="s">
         <v>495</v>
       </c>
       <c r="G13" s="3" t="s">
@@ -5809,7 +5821,7 @@
       <c r="E14" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="F14" s="30" t="s">
+      <c r="F14" s="65" t="s">
         <v>496</v>
       </c>
       <c r="G14" s="6" t="s">
@@ -5877,7 +5889,7 @@
       <c r="E15" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="F15" s="30" t="s">
+      <c r="F15" s="65" t="s">
         <v>497</v>
       </c>
       <c r="G15" s="2" t="s">
@@ -5946,7 +5958,7 @@
       <c r="E16" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="F16" s="30" t="s">
+      <c r="F16" s="65" t="s">
         <v>498</v>
       </c>
       <c r="G16" s="2" t="s">
@@ -6015,7 +6027,7 @@
       <c r="E17" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="F17" s="30" t="s">
+      <c r="F17" s="65" t="s">
         <v>499</v>
       </c>
       <c r="G17" s="2" t="s">
@@ -9565,7 +9577,7 @@
       <c r="E63" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F63" s="55" t="s">
+      <c r="F63" s="54" t="s">
         <v>718</v>
       </c>
       <c r="G63" s="6" t="s">
@@ -9601,7 +9613,7 @@
       <c r="Q63" s="13" t="s">
         <v>467</v>
       </c>
-      <c r="R63" s="56" t="s">
+      <c r="R63" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S63" s="6">
@@ -9673,7 +9685,7 @@
       <c r="Q64" s="13" t="s">
         <v>467</v>
       </c>
-      <c r="R64" s="56" t="s">
+      <c r="R64" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S64" s="6">
@@ -9745,7 +9757,7 @@
       <c r="Q65" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R65" s="56" t="s">
+      <c r="R65" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S65" s="6">
@@ -9816,7 +9828,7 @@
       <c r="Q66" s="13" t="s">
         <v>467</v>
       </c>
-      <c r="R66" s="56" t="s">
+      <c r="R66" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S66" s="6">
@@ -9887,7 +9899,7 @@
       <c r="Q67" s="13" t="s">
         <v>467</v>
       </c>
-      <c r="R67" s="56" t="s">
+      <c r="R67" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S67" s="6">
@@ -9958,7 +9970,7 @@
       <c r="Q68" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R68" s="56" t="s">
+      <c r="R68" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S68" s="6">
@@ -10030,7 +10042,7 @@
       <c r="Q69" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R69" s="56" t="s">
+      <c r="R69" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S69" s="6">
@@ -10103,7 +10115,7 @@
       <c r="Q70" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R70" s="56" t="s">
+      <c r="R70" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S70" s="6">
@@ -10189,7 +10201,7 @@
       <c r="Q71" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R71" s="56" t="s">
+      <c r="R71" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S71" s="6">
@@ -10275,7 +10287,7 @@
       <c r="Q72" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R72" s="56" t="s">
+      <c r="R72" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S72" s="6">
@@ -10360,7 +10372,7 @@
       <c r="Q73" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R73" s="56" t="s">
+      <c r="R73" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S73" s="6">
@@ -10446,7 +10458,7 @@
       <c r="Q74" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R74" s="56" t="s">
+      <c r="R74" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S74" s="6">
@@ -10532,7 +10544,7 @@
       <c r="Q75" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R75" s="56" t="s">
+      <c r="R75" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S75" s="6">
@@ -10618,7 +10630,7 @@
       <c r="Q76" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R76" s="56" t="s">
+      <c r="R76" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S76" s="6">
@@ -10704,7 +10716,7 @@
       <c r="Q77" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="R77" s="56" t="s">
+      <c r="R77" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S77" s="6">
@@ -10789,7 +10801,7 @@
       <c r="Q78" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R78" s="56" t="s">
+      <c r="R78" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S78" s="6">
@@ -10861,7 +10873,7 @@
       <c r="Q79" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R79" s="56" t="s">
+      <c r="R79" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S79" s="6">
@@ -10933,7 +10945,7 @@
       <c r="Q80" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R80" s="56" t="s">
+      <c r="R80" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S80" s="6">
@@ -11005,7 +11017,7 @@
       <c r="Q81" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R81" s="56" t="s">
+      <c r="R81" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S81" s="6">
@@ -11077,7 +11089,7 @@
       <c r="Q82" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R82" s="56" t="s">
+      <c r="R82" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S82" s="6">
@@ -11149,7 +11161,7 @@
       <c r="Q83" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R83" s="56" t="s">
+      <c r="R83" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S83" s="6">
@@ -11222,7 +11234,7 @@
       <c r="Q84" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R84" s="56" t="s">
+      <c r="R84" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S84" s="6">
@@ -11307,7 +11319,7 @@
       <c r="Q85" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R85" s="56" t="s">
+      <c r="R85" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S85" s="6">
@@ -11391,7 +11403,7 @@
       <c r="Q86" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R86" s="56" t="s">
+      <c r="R86" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S86" s="6">
@@ -11464,7 +11476,7 @@
       <c r="Q87" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R87" s="56" t="s">
+      <c r="R87" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S87" s="6">
@@ -11548,7 +11560,7 @@
       <c r="Q88" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R88" s="56" t="s">
+      <c r="R88" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S88" s="6">
@@ -11620,7 +11632,7 @@
       <c r="Q89" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R89" s="56" t="s">
+      <c r="R89" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S89" s="6">
@@ -11693,7 +11705,7 @@
       <c r="Q90" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="R90" s="56" t="s">
+      <c r="R90" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S90" s="6">
@@ -15963,7 +15975,7 @@
       <c r="Q143" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="R143" s="56" t="s">
+      <c r="R143" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S143" s="44">
@@ -16032,7 +16044,7 @@
       <c r="Q144" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="R144" s="56" t="s">
+      <c r="R144" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S144" s="44">
@@ -16101,7 +16113,7 @@
       <c r="Q145" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="R145" s="56" t="s">
+      <c r="R145" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S145" s="44">
@@ -16170,7 +16182,7 @@
       <c r="Q146" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="R146" s="56" t="s">
+      <c r="R146" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S146" s="44">
@@ -16238,7 +16250,7 @@
       <c r="Q147" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="R147" s="56" t="s">
+      <c r="R147" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S147" s="44">
@@ -16309,7 +16321,7 @@
       <c r="Q148" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="R148" s="56" t="s">
+      <c r="R148" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S148" s="44">
@@ -16377,7 +16389,7 @@
       <c r="Q149" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="R149" s="56" t="s">
+      <c r="R149" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S149" s="44">
@@ -16445,7 +16457,7 @@
       <c r="Q150" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="R150" s="56" t="s">
+      <c r="R150" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S150" s="44">
@@ -16513,7 +16525,7 @@
       <c r="Q151" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="R151" s="56" t="s">
+      <c r="R151" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S151" s="44">
@@ -16584,7 +16596,7 @@
       <c r="Q152" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="R152" s="56" t="s">
+      <c r="R152" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S152" s="44">
@@ -16655,7 +16667,7 @@
       <c r="Q153" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="R153" s="56" t="s">
+      <c r="R153" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S153" s="44">
@@ -16723,7 +16735,7 @@
       <c r="Q154" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="R154" s="56" t="s">
+      <c r="R154" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S154" s="44">
@@ -16794,7 +16806,7 @@
       <c r="Q155" s="6" t="s">
         <v>467</v>
       </c>
-      <c r="R155" s="56" t="s">
+      <c r="R155" s="55" t="s">
         <v>1303</v>
       </c>
       <c r="S155" s="53">
@@ -22797,16 +22809,16 @@
       <c r="A239" s="49">
         <v>94120117</v>
       </c>
-      <c r="B239" s="40" t="s">
+      <c r="B239" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C239" s="40" t="s">
+      <c r="C239" s="41" t="s">
         <v>865</v>
       </c>
-      <c r="D239" s="40" t="s">
+      <c r="D239" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="E239" s="40" t="s">
+      <c r="E239" s="41" t="s">
         <v>104</v>
       </c>
       <c r="F239" s="41" t="s">
@@ -22821,26 +22833,26 @@
       <c r="I239" s="42" t="s">
         <v>869</v>
       </c>
-      <c r="J239" s="40" t="s">
+      <c r="J239" s="41" t="s">
         <v>870</v>
       </c>
-      <c r="K239" s="40" t="s">
+      <c r="K239" s="41" t="s">
         <v>231</v>
       </c>
-      <c r="L239" s="40" t="s">
+      <c r="L239" s="41" t="s">
         <v>871</v>
       </c>
-      <c r="M239" s="40" t="s">
+      <c r="M239" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="N239" s="40" t="s">
+      <c r="N239" s="41" t="s">
         <v>872</v>
       </c>
-      <c r="O239" s="40" t="s">
+      <c r="O239" s="41" t="s">
         <v>873</v>
       </c>
-      <c r="P239" s="40"/>
-      <c r="Q239" s="40" t="s">
+      <c r="P239" s="41"/>
+      <c r="Q239" s="41" t="s">
         <v>17</v>
       </c>
       <c r="R239" s="6" t="s">
@@ -23244,13 +23256,13 @@
       <c r="A245" s="50">
         <v>94530116</v>
       </c>
-      <c r="B245" s="57" t="s">
+      <c r="B245" s="56" t="s">
         <v>968</v>
       </c>
-      <c r="C245" s="57" t="s">
+      <c r="C245" s="56" t="s">
         <v>865</v>
       </c>
-      <c r="D245" s="57" t="s">
+      <c r="D245" s="56" t="s">
         <v>2</v>
       </c>
       <c r="E245" s="6" t="s">
@@ -23259,35 +23271,35 @@
       <c r="F245" s="11" t="s">
         <v>1031</v>
       </c>
-      <c r="G245" s="58" t="s">
+      <c r="G245" s="57" t="s">
         <v>1032</v>
       </c>
-      <c r="H245" s="58" t="s">
+      <c r="H245" s="57" t="s">
         <v>1033</v>
       </c>
-      <c r="I245" s="58" t="s">
+      <c r="I245" s="57" t="s">
         <v>1034</v>
       </c>
-      <c r="J245" s="57" t="s">
+      <c r="J245" s="56" t="s">
         <v>796</v>
       </c>
-      <c r="K245" s="57" t="s">
+      <c r="K245" s="56" t="s">
         <v>231</v>
       </c>
-      <c r="L245" s="57" t="s">
+      <c r="L245" s="56" t="s">
         <v>910</v>
       </c>
-      <c r="M245" s="57" t="s">
+      <c r="M245" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="N245" s="57" t="s">
+      <c r="N245" s="56" t="s">
         <v>872</v>
       </c>
-      <c r="O245" s="57" t="s">
+      <c r="O245" s="56" t="s">
         <v>873</v>
       </c>
-      <c r="P245" s="57"/>
-      <c r="Q245" s="57" t="s">
+      <c r="P245" s="56"/>
+      <c r="Q245" s="56" t="s">
         <v>17</v>
       </c>
       <c r="R245" s="6" t="s">
@@ -23317,13 +23329,13 @@
       <c r="A246" s="50">
         <v>94530117</v>
       </c>
-      <c r="B246" s="57" t="s">
+      <c r="B246" s="56" t="s">
         <v>968</v>
       </c>
-      <c r="C246" s="57" t="s">
+      <c r="C246" s="56" t="s">
         <v>865</v>
       </c>
-      <c r="D246" s="57" t="s">
+      <c r="D246" s="56" t="s">
         <v>2</v>
       </c>
       <c r="E246" s="6" t="s">
@@ -23332,35 +23344,35 @@
       <c r="F246" s="11" t="s">
         <v>1035</v>
       </c>
-      <c r="G246" s="58" t="s">
+      <c r="G246" s="57" t="s">
         <v>1036</v>
       </c>
-      <c r="H246" s="58" t="s">
+      <c r="H246" s="57" t="s">
         <v>1290</v>
       </c>
-      <c r="I246" s="58" t="s">
+      <c r="I246" s="57" t="s">
         <v>1037</v>
       </c>
-      <c r="J246" s="57" t="s">
+      <c r="J246" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="K246" s="57" t="s">
+      <c r="K246" s="56" t="s">
         <v>231</v>
       </c>
-      <c r="L246" s="57" t="s">
+      <c r="L246" s="56" t="s">
         <v>910</v>
       </c>
-      <c r="M246" s="57" t="s">
+      <c r="M246" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="N246" s="57" t="s">
+      <c r="N246" s="56" t="s">
         <v>872</v>
       </c>
-      <c r="O246" s="57" t="s">
+      <c r="O246" s="56" t="s">
         <v>873</v>
       </c>
-      <c r="P246" s="57"/>
-      <c r="Q246" s="57" t="s">
+      <c r="P246" s="56"/>
+      <c r="Q246" s="56" t="s">
         <v>17</v>
       </c>
       <c r="R246" s="6" t="s">
@@ -25110,7 +25122,7 @@
       <c r="AL269" s="13"/>
     </row>
     <row r="270" spans="1:38" s="16" customFormat="1">
-      <c r="A270" s="59">
+      <c r="A270" s="58">
         <v>95120118</v>
       </c>
       <c r="B270" s="16" t="s">
@@ -25119,69 +25131,69 @@
       <c r="C270" s="16" t="s">
         <v>1354</v>
       </c>
-      <c r="D270" s="60" t="s">
+      <c r="D270" s="61" t="s">
         <v>104</v>
       </c>
-      <c r="E270" s="60" t="s">
+      <c r="E270" s="61" t="s">
         <v>104</v>
       </c>
-      <c r="F270" s="60" t="s">
+      <c r="F270" s="61" t="s">
         <v>1361</v>
       </c>
       <c r="G270" s="16" t="s">
         <v>1362</v>
       </c>
-      <c r="H270" s="61" t="s">
+      <c r="H270" s="59" t="s">
         <v>1359</v>
       </c>
-      <c r="I270" s="61" t="s">
+      <c r="I270" s="59" t="s">
         <v>1355</v>
       </c>
-      <c r="J270" s="61" t="s">
+      <c r="J270" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="K270" s="61" t="s">
+      <c r="K270" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="L270" s="61" t="s">
+      <c r="L270" s="59" t="s">
         <v>95</v>
       </c>
-      <c r="M270" s="61" t="s">
+      <c r="M270" s="59" t="s">
         <v>289</v>
       </c>
-      <c r="N270" s="62" t="s">
+      <c r="N270" s="59" t="s">
         <v>1356</v>
       </c>
-      <c r="O270" s="62" t="s">
+      <c r="O270" s="59" t="s">
         <v>1363</v>
       </c>
-      <c r="Q270" s="61" t="s">
+      <c r="Q270" s="59" t="s">
         <v>96</v>
       </c>
-      <c r="R270" s="61" t="s">
+      <c r="R270" s="59" t="s">
         <v>1364</v>
       </c>
-      <c r="S270" s="63">
-        <v>0</v>
-      </c>
-      <c r="T270" s="63">
-        <v>0</v>
-      </c>
-      <c r="U270" s="63">
-        <v>0</v>
-      </c>
-      <c r="V270" s="63">
-        <v>0</v>
-      </c>
-      <c r="W270" s="63">
+      <c r="S270" s="60">
+        <v>0</v>
+      </c>
+      <c r="T270" s="60">
+        <v>0</v>
+      </c>
+      <c r="U270" s="60">
+        <v>0</v>
+      </c>
+      <c r="V270" s="60">
+        <v>0</v>
+      </c>
+      <c r="W270" s="60">
         <v>0</v>
       </c>
       <c r="X270" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:38" s="61" customFormat="1">
-      <c r="A271" s="59">
+    <row r="271" spans="1:38" s="59" customFormat="1">
+      <c r="A271" s="58">
         <v>95520111</v>
       </c>
       <c r="B271" s="16" t="s">
@@ -25190,61 +25202,61 @@
       <c r="C271" s="16" t="s">
         <v>1354</v>
       </c>
-      <c r="D271" s="60" t="s">
+      <c r="D271" s="61" t="s">
         <v>104</v>
       </c>
-      <c r="E271" s="60" t="s">
+      <c r="E271" s="61" t="s">
         <v>104</v>
       </c>
-      <c r="F271" s="60" t="s">
+      <c r="F271" s="61" t="s">
         <v>1365</v>
       </c>
       <c r="G271" s="16" t="s">
         <v>1366</v>
       </c>
-      <c r="H271" s="61" t="s">
+      <c r="H271" s="59" t="s">
         <v>1357</v>
       </c>
-      <c r="I271" s="61" t="s">
+      <c r="I271" s="59" t="s">
         <v>1358</v>
       </c>
-      <c r="J271" s="61" t="s">
+      <c r="J271" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="K271" s="61" t="s">
+      <c r="K271" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="L271" s="61" t="s">
+      <c r="L271" s="59" t="s">
         <v>234</v>
       </c>
-      <c r="M271" s="61" t="s">
+      <c r="M271" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="N271" s="61" t="s">
+      <c r="N271" s="59" t="s">
         <v>1367</v>
       </c>
-      <c r="O271" s="64" t="s">
+      <c r="O271" s="61" t="s">
         <v>1368</v>
       </c>
-      <c r="Q271" s="60" t="s">
+      <c r="Q271" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="R271" s="61" t="s">
+      <c r="R271" s="59" t="s">
         <v>1364</v>
       </c>
-      <c r="S271" s="63">
-        <v>0</v>
-      </c>
-      <c r="T271" s="63">
-        <v>0</v>
-      </c>
-      <c r="U271" s="63">
-        <v>0</v>
-      </c>
-      <c r="V271" s="63">
-        <v>0</v>
-      </c>
-      <c r="W271" s="63">
+      <c r="S271" s="60">
+        <v>0</v>
+      </c>
+      <c r="T271" s="60">
+        <v>0</v>
+      </c>
+      <c r="U271" s="60">
+        <v>0</v>
+      </c>
+      <c r="V271" s="60">
+        <v>0</v>
+      </c>
+      <c r="W271" s="60">
         <v>0</v>
       </c>
       <c r="X271" s="16">
@@ -25252,7 +25264,7 @@
       </c>
     </row>
     <row r="272" spans="1:38" s="16" customFormat="1">
-      <c r="A272" s="65">
+      <c r="A272" s="62">
         <v>95230101</v>
       </c>
       <c r="B272" s="16" t="s">
@@ -25267,7 +25279,7 @@
       <c r="E272" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="F272" s="60" t="s">
+      <c r="F272" s="61" t="s">
         <v>1369</v>
       </c>
       <c r="G272" s="16" t="s">
@@ -25291,19 +25303,19 @@
       <c r="M272" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="N272" s="16" t="s">
-        <v>1372</v>
-      </c>
-      <c r="O272" s="66" t="s">
-        <v>1373</v>
+      <c r="N272" s="61" t="s">
+        <v>1384</v>
+      </c>
+      <c r="O272" s="63" t="s">
+        <v>1385</v>
       </c>
       <c r="P272" s="16" t="s">
         <v>40</v>
       </c>
       <c r="Q272" s="16" t="s">
-        <v>1374</v>
-      </c>
-      <c r="R272" s="61" t="s">
+        <v>1372</v>
+      </c>
+      <c r="R272" s="59" t="s">
         <v>1364</v>
       </c>
       <c r="S272" s="16">
@@ -25326,7 +25338,7 @@
       </c>
     </row>
     <row r="273" spans="1:24" s="16" customFormat="1">
-      <c r="A273" s="65">
+      <c r="A273" s="62">
         <v>95230501</v>
       </c>
       <c r="B273" s="16" t="s">
@@ -25341,11 +25353,11 @@
       <c r="E273" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="F273" s="60" t="s">
-        <v>1375</v>
+      <c r="F273" s="61" t="s">
+        <v>1373</v>
       </c>
       <c r="G273" s="16" t="s">
-        <v>1376</v>
+        <v>1374</v>
       </c>
       <c r="H273" s="16" t="s">
         <v>375</v>
@@ -25365,16 +25377,16 @@
       <c r="M273" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="N273" s="16" t="s">
+      <c r="N273" s="61" t="s">
+        <v>1384</v>
+      </c>
+      <c r="O273" s="63" t="s">
+        <v>1385</v>
+      </c>
+      <c r="Q273" s="16" t="s">
         <v>1372</v>
       </c>
-      <c r="O273" s="66" t="s">
-        <v>1373</v>
-      </c>
-      <c r="Q273" s="16" t="s">
-        <v>1374</v>
-      </c>
-      <c r="R273" s="61" t="s">
+      <c r="R273" s="59" t="s">
         <v>1364</v>
       </c>
       <c r="S273" s="16">
@@ -25396,8 +25408,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="274" spans="1:24" s="67" customFormat="1">
-      <c r="A274" s="65">
+    <row r="274" spans="1:24" s="64" customFormat="1">
+      <c r="A274" s="62">
         <v>95530101</v>
       </c>
       <c r="B274" s="16" t="s">
@@ -25406,19 +25418,19 @@
       <c r="C274" s="16" t="s">
         <v>1354</v>
       </c>
-      <c r="D274" s="67" t="s">
+      <c r="D274" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="E274" s="67" t="s">
+      <c r="E274" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="F274" s="60" t="s">
-        <v>1377</v>
+      <c r="F274" s="61" t="s">
+        <v>1375</v>
       </c>
       <c r="G274" s="16" t="s">
-        <v>1377</v>
-      </c>
-      <c r="H274" s="67" t="s">
+        <v>1375</v>
+      </c>
+      <c r="H274" s="64" t="s">
         <v>1248</v>
       </c>
       <c r="I274" s="16" t="s">
@@ -25436,39 +25448,39 @@
       <c r="M274" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="N274" s="16" t="s">
-        <v>1372</v>
-      </c>
-      <c r="O274" s="16" t="s">
-        <v>1373</v>
+      <c r="N274" s="61" t="s">
+        <v>1384</v>
+      </c>
+      <c r="O274" s="63" t="s">
+        <v>1385</v>
       </c>
       <c r="Q274" s="16" t="s">
-        <v>1378</v>
-      </c>
-      <c r="R274" s="63" t="s">
-        <v>1379</v>
-      </c>
-      <c r="S274" s="63">
-        <v>0</v>
-      </c>
-      <c r="T274" s="63">
-        <v>0</v>
-      </c>
-      <c r="U274" s="63">
-        <v>0</v>
-      </c>
-      <c r="V274" s="63">
-        <v>0</v>
-      </c>
-      <c r="W274" s="63">
+        <v>1376</v>
+      </c>
+      <c r="R274" s="60" t="s">
+        <v>1377</v>
+      </c>
+      <c r="S274" s="60">
+        <v>0</v>
+      </c>
+      <c r="T274" s="60">
+        <v>0</v>
+      </c>
+      <c r="U274" s="60">
+        <v>0</v>
+      </c>
+      <c r="V274" s="60">
+        <v>0</v>
+      </c>
+      <c r="W274" s="60">
         <v>0</v>
       </c>
       <c r="X274" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="275" spans="1:24" s="67" customFormat="1">
-      <c r="A275" s="65">
+    <row r="275" spans="1:24" s="64" customFormat="1">
+      <c r="A275" s="62">
         <v>95530102</v>
       </c>
       <c r="B275" s="16" t="s">
@@ -25477,19 +25489,19 @@
       <c r="C275" s="16" t="s">
         <v>1354</v>
       </c>
-      <c r="D275" s="67" t="s">
+      <c r="D275" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="E275" s="67" t="s">
+      <c r="E275" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="F275" s="60" t="s">
-        <v>1380</v>
+      <c r="F275" s="61" t="s">
+        <v>1378</v>
       </c>
       <c r="G275" s="16" t="s">
-        <v>1380</v>
-      </c>
-      <c r="H275" s="67" t="s">
+        <v>1378</v>
+      </c>
+      <c r="H275" s="64" t="s">
         <v>1041</v>
       </c>
       <c r="I275" s="16" t="s">
@@ -25507,39 +25519,39 @@
       <c r="M275" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="N275" s="16" t="s">
-        <v>1372</v>
-      </c>
-      <c r="O275" s="66" t="s">
-        <v>1373</v>
+      <c r="N275" s="61" t="s">
+        <v>1384</v>
+      </c>
+      <c r="O275" s="63" t="s">
+        <v>1385</v>
       </c>
       <c r="Q275" s="16" t="s">
-        <v>1378</v>
-      </c>
-      <c r="R275" s="63" t="s">
-        <v>1379</v>
-      </c>
-      <c r="S275" s="63">
-        <v>0</v>
-      </c>
-      <c r="T275" s="63">
-        <v>0</v>
-      </c>
-      <c r="U275" s="63">
-        <v>0</v>
-      </c>
-      <c r="V275" s="63">
-        <v>0</v>
-      </c>
-      <c r="W275" s="63">
+        <v>1376</v>
+      </c>
+      <c r="R275" s="60" t="s">
+        <v>1377</v>
+      </c>
+      <c r="S275" s="60">
+        <v>0</v>
+      </c>
+      <c r="T275" s="60">
+        <v>0</v>
+      </c>
+      <c r="U275" s="60">
+        <v>0</v>
+      </c>
+      <c r="V275" s="60">
+        <v>0</v>
+      </c>
+      <c r="W275" s="60">
         <v>0</v>
       </c>
       <c r="X275" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="276" spans="1:24" s="67" customFormat="1">
-      <c r="A276" s="65">
+    <row r="276" spans="1:24" s="64" customFormat="1">
+      <c r="A276" s="62">
         <v>95530103</v>
       </c>
       <c r="B276" s="16" t="s">
@@ -25548,19 +25560,19 @@
       <c r="C276" s="16" t="s">
         <v>1354</v>
       </c>
-      <c r="D276" s="67" t="s">
+      <c r="D276" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="E276" s="67" t="s">
+      <c r="E276" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="F276" s="60" t="s">
-        <v>1381</v>
+      <c r="F276" s="61" t="s">
+        <v>1379</v>
       </c>
       <c r="G276" s="16" t="s">
-        <v>1381</v>
-      </c>
-      <c r="H276" s="67" t="s">
+        <v>1379</v>
+      </c>
+      <c r="H276" s="64" t="s">
         <v>1015</v>
       </c>
       <c r="I276" s="16" t="s">
@@ -25578,39 +25590,39 @@
       <c r="M276" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="N276" s="16" t="s">
-        <v>1372</v>
-      </c>
-      <c r="O276" s="66" t="s">
-        <v>1373</v>
+      <c r="N276" s="61" t="s">
+        <v>1384</v>
+      </c>
+      <c r="O276" s="63" t="s">
+        <v>1385</v>
       </c>
       <c r="Q276" s="16" t="s">
-        <v>1378</v>
-      </c>
-      <c r="R276" s="63" t="s">
-        <v>1379</v>
-      </c>
-      <c r="S276" s="63">
-        <v>0</v>
-      </c>
-      <c r="T276" s="63">
-        <v>0</v>
-      </c>
-      <c r="U276" s="63">
-        <v>0</v>
-      </c>
-      <c r="V276" s="63">
-        <v>0</v>
-      </c>
-      <c r="W276" s="63">
+        <v>1376</v>
+      </c>
+      <c r="R276" s="60" t="s">
+        <v>1377</v>
+      </c>
+      <c r="S276" s="60">
+        <v>0</v>
+      </c>
+      <c r="T276" s="60">
+        <v>0</v>
+      </c>
+      <c r="U276" s="60">
+        <v>0</v>
+      </c>
+      <c r="V276" s="60">
+        <v>0</v>
+      </c>
+      <c r="W276" s="60">
         <v>0</v>
       </c>
       <c r="X276" s="16">
         <v>0</v>
       </c>
     </row>
-    <row r="277" spans="1:24" s="67" customFormat="1">
-      <c r="A277" s="65">
+    <row r="277" spans="1:24" s="64" customFormat="1">
+      <c r="A277" s="62">
         <v>95530104</v>
       </c>
       <c r="B277" s="16" t="s">
@@ -25619,19 +25631,19 @@
       <c r="C277" s="16" t="s">
         <v>1354</v>
       </c>
-      <c r="D277" s="67" t="s">
+      <c r="D277" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="E277" s="67" t="s">
+      <c r="E277" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="F277" s="60" t="s">
-        <v>1382</v>
+      <c r="F277" s="61" t="s">
+        <v>1380</v>
       </c>
       <c r="G277" s="16" t="s">
-        <v>1382</v>
-      </c>
-      <c r="H277" s="67" t="s">
+        <v>1380</v>
+      </c>
+      <c r="H277" s="64" t="s">
         <v>1249</v>
       </c>
       <c r="I277" s="16" t="s">
@@ -25649,34 +25661,108 @@
       <c r="M277" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="N277" s="16" t="s">
-        <v>1372</v>
-      </c>
-      <c r="O277" s="66" t="s">
-        <v>1373</v>
+      <c r="N277" s="61" t="s">
+        <v>1384</v>
+      </c>
+      <c r="O277" s="63" t="s">
+        <v>1385</v>
       </c>
       <c r="Q277" s="16" t="s">
-        <v>1378</v>
-      </c>
-      <c r="R277" s="63" t="s">
-        <v>1379</v>
-      </c>
-      <c r="S277" s="63">
-        <v>0</v>
-      </c>
-      <c r="T277" s="63">
-        <v>0</v>
-      </c>
-      <c r="U277" s="63">
-        <v>0</v>
-      </c>
-      <c r="V277" s="63">
-        <v>0</v>
-      </c>
-      <c r="W277" s="63">
+        <v>1376</v>
+      </c>
+      <c r="R277" s="60" t="s">
+        <v>1377</v>
+      </c>
+      <c r="S277" s="60">
+        <v>0</v>
+      </c>
+      <c r="T277" s="60">
+        <v>0</v>
+      </c>
+      <c r="U277" s="60">
+        <v>0</v>
+      </c>
+      <c r="V277" s="60">
+        <v>0</v>
+      </c>
+      <c r="W277" s="60">
         <v>0</v>
       </c>
       <c r="X277" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="278" spans="1:24" s="61" customFormat="1">
+      <c r="A278" s="61">
+        <v>95530202</v>
+      </c>
+      <c r="B278" s="16" t="s">
+        <v>1360</v>
+      </c>
+      <c r="C278" s="16" t="s">
+        <v>1354</v>
+      </c>
+      <c r="D278" s="64" t="s">
+        <v>2</v>
+      </c>
+      <c r="E278" s="61" t="s">
+        <v>15</v>
+      </c>
+      <c r="F278" s="61" t="s">
+        <v>1382</v>
+      </c>
+      <c r="G278" s="61" t="s">
+        <v>1383</v>
+      </c>
+      <c r="H278" s="61" t="s">
+        <v>1253</v>
+      </c>
+      <c r="I278" s="61" t="s">
+        <v>1055</v>
+      </c>
+      <c r="J278" s="61" t="s">
+        <v>5</v>
+      </c>
+      <c r="K278" s="61" t="s">
+        <v>6</v>
+      </c>
+      <c r="L278" s="61" t="s">
+        <v>306</v>
+      </c>
+      <c r="M278" s="61" t="s">
+        <v>8</v>
+      </c>
+      <c r="N278" s="61" t="s">
+        <v>1384</v>
+      </c>
+      <c r="O278" s="63" t="s">
+        <v>1385</v>
+      </c>
+      <c r="P278" s="61" t="s">
+        <v>1381</v>
+      </c>
+      <c r="Q278" s="16" t="s">
+        <v>1376</v>
+      </c>
+      <c r="R278" s="60" t="s">
+        <v>1377</v>
+      </c>
+      <c r="S278" s="61">
+        <v>0</v>
+      </c>
+      <c r="T278" s="61">
+        <v>0</v>
+      </c>
+      <c r="U278" s="61">
+        <v>0</v>
+      </c>
+      <c r="V278" s="61">
+        <v>0</v>
+      </c>
+      <c r="W278" s="61">
+        <v>0</v>
+      </c>
+      <c r="X278" s="61">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corr gasto edu obligatoria
</commit_message>
<xml_diff>
--- a/Data/Base_fichas_indicadores.xlsx
+++ b/Data/Base_fichas_indicadores.xlsx
@@ -5829,10 +5829,10 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:AN335"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E111" sqref="E111"/>
-      <selection pane="bottomLeft" activeCell="G239" sqref="G239"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="15.6" customHeight="1"/>

</xml_diff>

<commit_message>
Act edu no ech
</commit_message>
<xml_diff>
--- a/Data/Base_fichas_indicadores.xlsx
+++ b/Data/Base_fichas_indicadores.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5456" uniqueCount="1704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10876" uniqueCount="1709">
   <si>
     <t>id</t>
   </si>
@@ -5237,6 +5237,21 @@
   </si>
   <si>
     <t>Región, nivel socioeconómico, sexo, edad</t>
+  </si>
+  <si>
+    <t>2010-2022</t>
+  </si>
+  <si>
+    <t>La interrupción en la serie se debe a los años en los que afectó la pandemia de COVID19.</t>
+  </si>
+  <si>
+    <t>Observatorio de la Educación - ANEP / A partir de 2022 Monitor Educativo DGEIP</t>
+  </si>
+  <si>
+    <t>UMAD con base en Observatorio de la Educación - ANEP / A partir de 2022 Monitor Educativo DGEIP</t>
+  </si>
+  <si>
+    <t>La interrupción en la serie se debe a la pandemia de COVID19.</t>
   </si>
 </sst>
 </file>
@@ -5340,7 +5355,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5508,6 +5523,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Excel Built-in Normal" xfId="3"/>
@@ -5826,13 +5844,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr codeName="Hoja1"/>
+  <sheetPr codeName="Hoja1" filterMode="1"/>
   <dimension ref="A1:AN335"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="Q1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E111" sqref="E111"/>
-      <selection pane="bottomLeft" activeCell="B1" sqref="A1:XFD1"/>
+      <selection pane="bottomLeft" activeCell="S13" sqref="S13:S28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="15.6" customHeight="1"/>
@@ -5854,7 +5872,7 @@
     <col min="15" max="16" width="130.44140625" style="12" customWidth="1"/>
     <col min="17" max="17" width="48.6640625" style="12" customWidth="1"/>
     <col min="18" max="19" width="98.6640625" style="12" customWidth="1"/>
-    <col min="20" max="20" width="17.77734375" style="12" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.77734375" style="63" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15.88671875" style="12" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="16.5546875" style="12" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="15.88671875" style="12" bestFit="1" customWidth="1"/>
@@ -5926,7 +5944,7 @@
       <c r="S1" s="12" t="s">
         <v>1269</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="T1" s="63" t="s">
         <v>1683</v>
       </c>
       <c r="U1" s="22" t="s">
@@ -5954,7 +5972,7 @@
         <v>1623</v>
       </c>
     </row>
-    <row r="2" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="2" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A2" s="5">
         <v>120101</v>
       </c>
@@ -6029,7 +6047,7 @@
       </c>
       <c r="AN2" s="12"/>
     </row>
-    <row r="3" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="3" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A3" s="5">
         <v>120102</v>
       </c>
@@ -6103,7 +6121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="4" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A4" s="5">
         <v>120103</v>
       </c>
@@ -6178,7 +6196,7 @@
       </c>
       <c r="AN4" s="12"/>
     </row>
-    <row r="5" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="5" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A5" s="5">
         <v>120104</v>
       </c>
@@ -6253,7 +6271,7 @@
       </c>
       <c r="AN5" s="12"/>
     </row>
-    <row r="6" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="6" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A6" s="5">
         <v>120105</v>
       </c>
@@ -6328,7 +6346,7 @@
       </c>
       <c r="AN6" s="12"/>
     </row>
-    <row r="7" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="7" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A7" s="5">
         <v>120106</v>
       </c>
@@ -6403,7 +6421,7 @@
       </c>
       <c r="AN7" s="14"/>
     </row>
-    <row r="8" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="8" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A8" s="5">
         <v>120107</v>
       </c>
@@ -6478,7 +6496,7 @@
       </c>
       <c r="AN8" s="14"/>
     </row>
-    <row r="9" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="9" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A9" s="5">
         <v>120108</v>
       </c>
@@ -6549,7 +6567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="10" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A10" s="5">
         <v>120109</v>
       </c>
@@ -6621,7 +6639,7 @@
       </c>
       <c r="AN10" s="12"/>
     </row>
-    <row r="11" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="11" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A11" s="5">
         <v>120110</v>
       </c>
@@ -6693,7 +6711,7 @@
       </c>
       <c r="AN11" s="12"/>
     </row>
-    <row r="12" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="12" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A12" s="5">
         <v>120111</v>
       </c>
@@ -6799,7 +6817,7 @@
         <v>6</v>
       </c>
       <c r="L13" s="5" t="s">
-        <v>958</v>
+        <v>1704</v>
       </c>
       <c r="M13" s="5" t="s">
         <v>8</v>
@@ -6814,7 +6832,10 @@
         <v>24</v>
       </c>
       <c r="S13" s="5" t="s">
-        <v>1268</v>
+        <v>1708</v>
+      </c>
+      <c r="T13" s="42" t="s">
+        <v>1684</v>
       </c>
       <c r="U13" s="5">
         <v>0</v>
@@ -6839,7 +6860,7 @@
       </c>
       <c r="AN13" s="12"/>
     </row>
-    <row r="14" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="14" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A14" s="5">
         <v>120113</v>
       </c>
@@ -6913,7 +6934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="15" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A15" s="5">
         <v>120114</v>
       </c>
@@ -6988,7 +7009,7 @@
       </c>
       <c r="AN15" s="5"/>
     </row>
-    <row r="16" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="16" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A16" s="5">
         <v>120115</v>
       </c>
@@ -7063,7 +7084,7 @@
       </c>
       <c r="AN16" s="5"/>
     </row>
-    <row r="17" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="17" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A17" s="5">
         <v>120116</v>
       </c>
@@ -7138,7 +7159,7 @@
       </c>
       <c r="AN17" s="5"/>
     </row>
-    <row r="18" spans="1:40" ht="15.6" customHeight="1">
+    <row r="18" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A18" s="12">
         <v>130101</v>
       </c>
@@ -7218,7 +7239,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:40" ht="15.6" customHeight="1">
+    <row r="19" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A19" s="12">
         <v>130102</v>
       </c>
@@ -7298,7 +7319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:40" ht="15.6" customHeight="1">
+    <row r="20" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A20" s="12">
         <v>130103</v>
       </c>
@@ -7378,7 +7399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="21" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A21" s="13">
         <v>130104</v>
       </c>
@@ -7471,7 +7492,7 @@
       <c r="AL21" s="12"/>
       <c r="AM21" s="12"/>
     </row>
-    <row r="22" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="22" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A22" s="13">
         <v>130105</v>
       </c>
@@ -7564,7 +7585,7 @@
       <c r="AL22" s="12"/>
       <c r="AM22" s="12"/>
     </row>
-    <row r="23" spans="1:40" ht="15.6" customHeight="1">
+    <row r="23" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A23" s="13">
         <v>130106</v>
       </c>
@@ -7645,7 +7666,7 @@
       </c>
       <c r="AN23" s="5"/>
     </row>
-    <row r="24" spans="1:40" ht="15.6" customHeight="1">
+    <row r="24" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A24" s="14">
         <v>130107</v>
       </c>
@@ -7739,7 +7760,7 @@
       <c r="AM24" s="14"/>
       <c r="AN24" s="5"/>
     </row>
-    <row r="25" spans="1:40" ht="15.6" customHeight="1">
+    <row r="25" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A25" s="14">
         <v>130108</v>
       </c>
@@ -7865,16 +7886,16 @@
         <v>6</v>
       </c>
       <c r="L26" s="5" t="s">
-        <v>7</v>
+        <v>1665</v>
       </c>
       <c r="M26" s="5" t="s">
         <v>8</v>
       </c>
       <c r="N26" s="5" t="s">
-        <v>458</v>
+        <v>1706</v>
       </c>
       <c r="O26" s="5" t="s">
-        <v>460</v>
+        <v>1707</v>
       </c>
       <c r="Q26" s="5" t="s">
         <v>14</v>
@@ -7883,7 +7904,10 @@
         <v>594</v>
       </c>
       <c r="S26" s="5" t="s">
-        <v>1268</v>
+        <v>1708</v>
+      </c>
+      <c r="T26" s="42" t="s">
+        <v>1684</v>
       </c>
       <c r="U26" s="5">
         <v>0</v>
@@ -7940,16 +7964,16 @@
         <v>6</v>
       </c>
       <c r="L27" s="5" t="s">
-        <v>7</v>
+        <v>1665</v>
       </c>
       <c r="M27" s="5" t="s">
         <v>8</v>
       </c>
       <c r="N27" s="5" t="s">
-        <v>458</v>
+        <v>1706</v>
       </c>
       <c r="O27" s="5" t="s">
-        <v>460</v>
+        <v>1707</v>
       </c>
       <c r="P27" s="5"/>
       <c r="Q27" s="5" t="s">
@@ -7959,9 +7983,11 @@
         <v>594</v>
       </c>
       <c r="S27" s="5" t="s">
-        <v>1268</v>
-      </c>
-      <c r="T27" s="5"/>
+        <v>1708</v>
+      </c>
+      <c r="T27" s="42" t="s">
+        <v>1684</v>
+      </c>
       <c r="U27" s="5">
         <v>0</v>
       </c>
@@ -8029,16 +8055,16 @@
         <v>6</v>
       </c>
       <c r="L28" s="5" t="s">
-        <v>7</v>
+        <v>1665</v>
       </c>
       <c r="M28" s="5" t="s">
         <v>8</v>
       </c>
       <c r="N28" s="5" t="s">
-        <v>458</v>
+        <v>1706</v>
       </c>
       <c r="O28" s="5" t="s">
-        <v>460</v>
+        <v>1707</v>
       </c>
       <c r="P28" s="5"/>
       <c r="Q28" s="5" t="s">
@@ -8048,9 +8074,11 @@
         <v>455</v>
       </c>
       <c r="S28" s="5" t="s">
-        <v>1268</v>
-      </c>
-      <c r="T28" s="5"/>
+        <v>1708</v>
+      </c>
+      <c r="T28" s="42" t="s">
+        <v>1684</v>
+      </c>
       <c r="U28" s="5">
         <v>0</v>
       </c>
@@ -8085,7 +8113,7 @@
       <c r="AL28" s="5"/>
       <c r="AM28" s="5"/>
     </row>
-    <row r="29" spans="1:40" ht="15.6" customHeight="1">
+    <row r="29" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A29" s="5">
         <v>130204</v>
       </c>
@@ -8162,7 +8190,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:40" s="14" customFormat="1" ht="15.6" customHeight="1">
+    <row r="30" spans="1:40" s="14" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A30" s="5">
         <v>130205</v>
       </c>
@@ -8306,7 +8334,9 @@
       <c r="S31" s="5" t="s">
         <v>1268</v>
       </c>
-      <c r="T31" s="5"/>
+      <c r="T31" s="42" t="s">
+        <v>1684</v>
+      </c>
       <c r="U31" s="5">
         <v>0</v>
       </c>
@@ -8393,6 +8423,9 @@
       <c r="S32" s="5" t="s">
         <v>1268</v>
       </c>
+      <c r="T32" s="42" t="s">
+        <v>1684</v>
+      </c>
       <c r="U32" s="5">
         <v>0</v>
       </c>
@@ -8478,7 +8511,9 @@
       <c r="S33" s="5" t="s">
         <v>1268</v>
       </c>
-      <c r="T33" s="5"/>
+      <c r="T33" s="42" t="s">
+        <v>1684</v>
+      </c>
       <c r="U33" s="5">
         <v>0</v>
       </c>
@@ -8556,7 +8591,9 @@
       <c r="S34" s="5" t="s">
         <v>1268</v>
       </c>
-      <c r="T34" s="5"/>
+      <c r="T34" s="42" t="s">
+        <v>1684</v>
+      </c>
       <c r="U34" s="5">
         <v>0</v>
       </c>
@@ -8592,7 +8629,7 @@
       <c r="AM34" s="5"/>
       <c r="AN34" s="5"/>
     </row>
-    <row r="35" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="35" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A35" s="5">
         <v>130305</v>
       </c>
@@ -8672,7 +8709,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:40" ht="15.6" customHeight="1">
+    <row r="36" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A36" s="5">
         <v>130306</v>
       </c>
@@ -8753,7 +8790,7 @@
       </c>
       <c r="AN36" s="5"/>
     </row>
-    <row r="37" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="37" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A37" s="5">
         <v>220101</v>
       </c>
@@ -8828,7 +8865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="38" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A38" s="5">
         <v>220102</v>
       </c>
@@ -8903,7 +8940,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="39" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A39" s="5">
         <v>220103</v>
       </c>
@@ -8978,7 +9015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="40" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A40" s="5">
         <v>220104</v>
       </c>
@@ -9053,7 +9090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:40" ht="15.6" customHeight="1">
+    <row r="41" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A41" s="5">
         <v>220105</v>
       </c>
@@ -9140,7 +9177,7 @@
       <c r="AM41" s="5"/>
       <c r="AN41" s="5"/>
     </row>
-    <row r="42" spans="1:40" ht="15.6" customHeight="1">
+    <row r="42" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A42" s="5">
         <v>220106</v>
       </c>
@@ -9227,7 +9264,7 @@
       <c r="AM42" s="40"/>
       <c r="AN42" s="5"/>
     </row>
-    <row r="43" spans="1:40" ht="15.6" customHeight="1">
+    <row r="43" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A43" s="5">
         <v>220107</v>
       </c>
@@ -9314,7 +9351,7 @@
       <c r="AM43" s="40"/>
       <c r="AN43" s="5"/>
     </row>
-    <row r="44" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="44" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A44" s="44">
         <v>230101</v>
       </c>
@@ -9407,7 +9444,7 @@
       <c r="AL44" s="12"/>
       <c r="AM44" s="12"/>
     </row>
-    <row r="45" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="45" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A45" s="44">
         <v>230201</v>
       </c>
@@ -9500,7 +9537,7 @@
       <c r="AL45" s="12"/>
       <c r="AM45" s="12"/>
     </row>
-    <row r="46" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="46" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A46" s="44">
         <v>230202</v>
       </c>
@@ -9593,7 +9630,7 @@
       <c r="AL46" s="12"/>
       <c r="AM46" s="12"/>
     </row>
-    <row r="47" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="47" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A47" s="9">
         <v>230203</v>
       </c>
@@ -9673,7 +9710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="48" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A48" s="9">
         <v>230204</v>
       </c>
@@ -9753,7 +9790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="49" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A49" s="5">
         <v>230301</v>
       </c>
@@ -9833,7 +9870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:40" ht="15.6" customHeight="1">
+    <row r="50" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A50" s="5">
         <v>230302</v>
       </c>
@@ -9927,7 +9964,7 @@
       <c r="AM50" s="5"/>
       <c r="AN50" s="5"/>
     </row>
-    <row r="51" spans="1:40" ht="15.6" customHeight="1">
+    <row r="51" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A51" s="5">
         <v>230303</v>
       </c>
@@ -10021,7 +10058,7 @@
       <c r="AM51" s="5"/>
       <c r="AN51" s="5"/>
     </row>
-    <row r="52" spans="1:40" ht="15.6" customHeight="1">
+    <row r="52" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A52" s="5">
         <v>230304</v>
       </c>
@@ -10115,7 +10152,7 @@
       <c r="AM52" s="5"/>
       <c r="AN52" s="5"/>
     </row>
-    <row r="53" spans="1:40" ht="15.6" customHeight="1">
+    <row r="53" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A53" s="5">
         <v>230401</v>
       </c>
@@ -10209,7 +10246,7 @@
       <c r="AM53" s="5"/>
       <c r="AN53" s="5"/>
     </row>
-    <row r="54" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="54" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A54" s="44">
         <v>230402</v>
       </c>
@@ -10302,7 +10339,7 @@
       <c r="AL54" s="12"/>
       <c r="AM54" s="12"/>
     </row>
-    <row r="55" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="55" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A55" s="44">
         <v>230501</v>
       </c>
@@ -10393,7 +10430,7 @@
       <c r="AL55" s="12"/>
       <c r="AM55" s="12"/>
     </row>
-    <row r="56" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="56" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A56" s="5">
         <v>320101</v>
       </c>
@@ -10468,7 +10505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="57" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A57" s="5">
         <v>320102</v>
       </c>
@@ -10543,7 +10580,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="58" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A58" s="5">
         <v>320103</v>
       </c>
@@ -10618,7 +10655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="59" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A59" s="5">
         <v>320104</v>
       </c>
@@ -10693,7 +10730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="60" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A60" s="5">
         <v>320105</v>
       </c>
@@ -10765,7 +10802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="61" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A61" s="5">
         <v>320106</v>
       </c>
@@ -10838,7 +10875,7 @@
       </c>
       <c r="AN61" s="6"/>
     </row>
-    <row r="62" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="62" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A62" s="5">
         <v>320107</v>
       </c>
@@ -10911,7 +10948,7 @@
       </c>
       <c r="AN62" s="6"/>
     </row>
-    <row r="63" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="63" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A63" s="9">
         <v>330101</v>
       </c>
@@ -10992,7 +11029,7 @@
       </c>
       <c r="AN63" s="10"/>
     </row>
-    <row r="64" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="64" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A64" s="9">
         <v>330102</v>
       </c>
@@ -11073,7 +11110,7 @@
       </c>
       <c r="AN64" s="6"/>
     </row>
-    <row r="65" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="65" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A65" s="9">
         <v>330103</v>
       </c>
@@ -11153,7 +11190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="66" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A66" s="9">
         <v>330104</v>
       </c>
@@ -11233,7 +11270,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="67" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A67" s="9">
         <v>330105</v>
       </c>
@@ -11313,7 +11350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="68" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A68" s="9">
         <v>330106</v>
       </c>
@@ -11394,7 +11431,7 @@
       </c>
       <c r="AN68" s="10"/>
     </row>
-    <row r="69" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="69" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A69" s="9">
         <v>330107</v>
       </c>
@@ -11475,7 +11512,7 @@
       </c>
       <c r="AN69" s="10"/>
     </row>
-    <row r="70" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="70" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A70" s="9">
         <v>330108</v>
       </c>
@@ -11569,7 +11606,7 @@
       <c r="AM70" s="21"/>
       <c r="AN70" s="6"/>
     </row>
-    <row r="71" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="71" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A71" s="9">
         <v>330109</v>
       </c>
@@ -11663,7 +11700,7 @@
       <c r="AM71" s="21"/>
       <c r="AN71" s="10"/>
     </row>
-    <row r="72" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="72" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A72" s="9">
         <v>330110</v>
       </c>
@@ -11756,7 +11793,7 @@
       <c r="AL72" s="21"/>
       <c r="AM72" s="21"/>
     </row>
-    <row r="73" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="73" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A73" s="9">
         <v>330111</v>
       </c>
@@ -11850,7 +11887,7 @@
       <c r="AM73" s="21"/>
       <c r="AN73" s="10"/>
     </row>
-    <row r="74" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="74" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A74" s="9">
         <v>330112</v>
       </c>
@@ -11944,7 +11981,7 @@
       <c r="AM74" s="21"/>
       <c r="AN74" s="10"/>
     </row>
-    <row r="75" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="75" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A75" s="9">
         <v>330113</v>
       </c>
@@ -12038,7 +12075,7 @@
       <c r="AM75" s="21"/>
       <c r="AN75" s="10"/>
     </row>
-    <row r="76" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="76" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A76" s="9">
         <v>330114</v>
       </c>
@@ -12132,7 +12169,7 @@
       <c r="AM76" s="21"/>
       <c r="AN76" s="10"/>
     </row>
-    <row r="77" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="77" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A77" s="9">
         <v>330115</v>
       </c>
@@ -12224,7 +12261,7 @@
       <c r="AM77" s="21"/>
       <c r="AN77" s="10"/>
     </row>
-    <row r="78" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="78" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A78" s="9">
         <v>330201</v>
       </c>
@@ -12305,7 +12342,7 @@
       </c>
       <c r="AN78" s="10"/>
     </row>
-    <row r="79" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="79" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A79" s="9">
         <v>330202</v>
       </c>
@@ -12386,7 +12423,7 @@
       </c>
       <c r="AN79" s="10"/>
     </row>
-    <row r="80" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="80" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A80" s="9">
         <v>330203</v>
       </c>
@@ -12467,7 +12504,7 @@
       </c>
       <c r="AN80" s="6"/>
     </row>
-    <row r="81" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="81" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A81" s="9">
         <v>330204</v>
       </c>
@@ -12548,7 +12585,7 @@
       </c>
       <c r="AN81" s="6"/>
     </row>
-    <row r="82" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="82" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A82" s="9">
         <v>330205</v>
       </c>
@@ -12629,7 +12666,7 @@
       </c>
       <c r="AN82" s="6"/>
     </row>
-    <row r="83" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="83" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A83" s="9">
         <v>330206</v>
       </c>
@@ -12710,7 +12747,7 @@
       </c>
       <c r="AN83" s="6"/>
     </row>
-    <row r="84" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="84" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A84" s="9">
         <v>330207</v>
       </c>
@@ -12803,7 +12840,7 @@
       <c r="AL84" s="5"/>
       <c r="AM84" s="5"/>
     </row>
-    <row r="85" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="85" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A85" s="9">
         <v>330208</v>
       </c>
@@ -12896,7 +12933,7 @@
       <c r="AL85" s="5"/>
       <c r="AM85" s="5"/>
     </row>
-    <row r="86" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="86" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A86" s="9">
         <v>330209</v>
       </c>
@@ -12977,7 +13014,7 @@
       </c>
       <c r="AN86" s="21"/>
     </row>
-    <row r="87" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="87" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A87" s="9">
         <v>330210</v>
       </c>
@@ -13070,7 +13107,7 @@
       <c r="AL87" s="5"/>
       <c r="AM87" s="5"/>
     </row>
-    <row r="88" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="88" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A88" s="9">
         <v>330211</v>
       </c>
@@ -13151,7 +13188,7 @@
       </c>
       <c r="AN88" s="21"/>
     </row>
-    <row r="89" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="89" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A89" s="9">
         <v>330212</v>
       </c>
@@ -13232,7 +13269,7 @@
       </c>
       <c r="AN89" s="6"/>
     </row>
-    <row r="90" spans="1:40" s="10" customFormat="1" ht="15.6" customHeight="1">
+    <row r="90" spans="1:40" s="10" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A90" s="9">
         <v>330213</v>
       </c>
@@ -13326,7 +13363,7 @@
       <c r="AM90" s="5"/>
       <c r="AN90" s="6"/>
     </row>
-    <row r="91" spans="1:40" s="10" customFormat="1" ht="15.6" customHeight="1">
+    <row r="91" spans="1:40" s="10" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A91" s="5">
         <v>420101</v>
       </c>
@@ -13416,7 +13453,7 @@
       <c r="AM91" s="5"/>
       <c r="AN91" s="6"/>
     </row>
-    <row r="92" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="92" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A92" s="5">
         <v>420102</v>
       </c>
@@ -13505,7 +13542,7 @@
       <c r="AL92" s="5"/>
       <c r="AM92" s="5"/>
     </row>
-    <row r="93" spans="1:40" s="10" customFormat="1" ht="15.6" customHeight="1">
+    <row r="93" spans="1:40" s="10" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A93" s="5">
         <v>420103</v>
       </c>
@@ -13595,7 +13632,7 @@
       <c r="AM93" s="5"/>
       <c r="AN93" s="21"/>
     </row>
-    <row r="94" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="94" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A94" s="5">
         <v>420104</v>
       </c>
@@ -13671,7 +13708,7 @@
       </c>
       <c r="AN94" s="40"/>
     </row>
-    <row r="95" spans="1:40" s="10" customFormat="1" ht="15.6" customHeight="1">
+    <row r="95" spans="1:40" s="10" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A95" s="5">
         <v>420105</v>
       </c>
@@ -13758,7 +13795,7 @@
       <c r="AL95" s="5"/>
       <c r="AM95" s="5"/>
     </row>
-    <row r="96" spans="1:40" s="10" customFormat="1" ht="15.6" customHeight="1">
+    <row r="96" spans="1:40" s="10" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A96" s="5">
         <v>420106</v>
       </c>
@@ -13845,7 +13882,7 @@
       <c r="AL96" s="5"/>
       <c r="AM96" s="5"/>
     </row>
-    <row r="97" spans="1:40" s="10" customFormat="1" ht="15.6" customHeight="1">
+    <row r="97" spans="1:40" s="10" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A97" s="5">
         <v>420107</v>
       </c>
@@ -13932,7 +13969,7 @@
       <c r="AL97" s="6"/>
       <c r="AM97" s="6"/>
     </row>
-    <row r="98" spans="1:40" s="10" customFormat="1" ht="15.6" customHeight="1">
+    <row r="98" spans="1:40" s="10" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A98" s="5">
         <v>420108</v>
       </c>
@@ -14020,7 +14057,7 @@
       <c r="AM98" s="6"/>
       <c r="AN98" s="21"/>
     </row>
-    <row r="99" spans="1:40" s="10" customFormat="1" ht="15.6" customHeight="1">
+    <row r="99" spans="1:40" s="10" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A99" s="5">
         <v>420109</v>
       </c>
@@ -14108,7 +14145,7 @@
       <c r="AM99" s="6"/>
       <c r="AN99" s="21"/>
     </row>
-    <row r="100" spans="1:40" s="10" customFormat="1" ht="15.6" customHeight="1">
+    <row r="100" spans="1:40" s="10" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A100" s="5">
         <v>430101</v>
       </c>
@@ -14200,7 +14237,7 @@
       <c r="AM100" s="5"/>
       <c r="AN100" s="21"/>
     </row>
-    <row r="101" spans="1:40" s="10" customFormat="1" ht="15.6" customHeight="1">
+    <row r="101" spans="1:40" s="10" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A101" s="5">
         <v>430102</v>
       </c>
@@ -14288,7 +14325,7 @@
       <c r="AM101" s="5"/>
       <c r="AN101" s="21"/>
     </row>
-    <row r="102" spans="1:40" s="10" customFormat="1" ht="15.6" customHeight="1">
+    <row r="102" spans="1:40" s="10" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A102" s="5">
         <v>430103</v>
       </c>
@@ -14361,7 +14398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="103" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A103" s="5">
         <v>430104</v>
       </c>
@@ -14448,7 +14485,7 @@
       <c r="AM103" s="10"/>
       <c r="AN103" s="10"/>
     </row>
-    <row r="104" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="104" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A104" s="5">
         <v>430105</v>
       </c>
@@ -14534,7 +14571,7 @@
       <c r="AL104" s="10"/>
       <c r="AM104" s="10"/>
     </row>
-    <row r="105" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="105" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A105" s="5">
         <v>430106</v>
       </c>
@@ -14621,7 +14658,7 @@
       <c r="AM105" s="10"/>
       <c r="AN105" s="12"/>
     </row>
-    <row r="106" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="106" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A106" s="5">
         <v>430107</v>
       </c>
@@ -14708,7 +14745,7 @@
       <c r="AM106" s="10"/>
       <c r="AN106" s="12"/>
     </row>
-    <row r="107" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="107" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A107" s="5">
         <v>430108</v>
       </c>
@@ -14795,7 +14832,7 @@
       <c r="AM107" s="10"/>
       <c r="AN107" s="12"/>
     </row>
-    <row r="108" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="108" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A108" s="5">
         <v>430109</v>
       </c>
@@ -14882,7 +14919,7 @@
       <c r="AM108" s="10"/>
       <c r="AN108" s="12"/>
     </row>
-    <row r="109" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="109" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A109" s="5">
         <v>430110</v>
       </c>
@@ -14970,7 +15007,7 @@
       <c r="AM109" s="10"/>
       <c r="AN109" s="12"/>
     </row>
-    <row r="110" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="110" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A110" s="5">
         <v>430111</v>
       </c>
@@ -15057,7 +15094,7 @@
       <c r="AM110" s="10"/>
       <c r="AN110" s="12"/>
     </row>
-    <row r="111" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="111" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A111" s="5">
         <v>430112</v>
       </c>
@@ -15145,7 +15182,7 @@
       <c r="AM111" s="10"/>
       <c r="AN111" s="12"/>
     </row>
-    <row r="112" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="112" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A112" s="5">
         <v>430113</v>
       </c>
@@ -15232,7 +15269,7 @@
       <c r="AM112" s="10"/>
       <c r="AN112" s="12"/>
     </row>
-    <row r="113" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="113" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A113" s="5">
         <v>430114</v>
       </c>
@@ -15319,7 +15356,7 @@
       <c r="AM113" s="10"/>
       <c r="AN113" s="12"/>
     </row>
-    <row r="114" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="114" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A114" s="5">
         <v>430201</v>
       </c>
@@ -15392,7 +15429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="115" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A115" s="5">
         <v>430202</v>
       </c>
@@ -15465,7 +15502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="116" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A116" s="5">
         <v>430203</v>
       </c>
@@ -15553,7 +15590,7 @@
       <c r="AM116" s="6"/>
       <c r="AN116" s="6"/>
     </row>
-    <row r="117" spans="1:40" s="40" customFormat="1" ht="15.6" customHeight="1">
+    <row r="117" spans="1:40" s="40" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A117" s="5">
         <v>430204</v>
       </c>
@@ -15641,7 +15678,7 @@
       <c r="AM117" s="6"/>
       <c r="AN117" s="6"/>
     </row>
-    <row r="118" spans="1:40" s="10" customFormat="1" ht="15.6" customHeight="1">
+    <row r="118" spans="1:40" s="10" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A118" s="5">
         <v>430205</v>
       </c>
@@ -15729,7 +15766,7 @@
       <c r="AM118" s="6"/>
       <c r="AN118" s="6"/>
     </row>
-    <row r="119" spans="1:40" s="10" customFormat="1" ht="15.6" customHeight="1">
+    <row r="119" spans="1:40" s="10" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A119" s="5">
         <v>430206</v>
       </c>
@@ -15817,7 +15854,7 @@
       <c r="AM119" s="6"/>
       <c r="AN119" s="6"/>
     </row>
-    <row r="120" spans="1:40" s="10" customFormat="1" ht="15.6" customHeight="1">
+    <row r="120" spans="1:40" s="10" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A120" s="5">
         <v>430207</v>
       </c>
@@ -15905,7 +15942,7 @@
       <c r="AM120" s="6"/>
       <c r="AN120" s="6"/>
     </row>
-    <row r="121" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="121" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A121" s="5">
         <v>430208</v>
       </c>
@@ -15993,7 +16030,7 @@
       <c r="AM121" s="6"/>
       <c r="AN121" s="6"/>
     </row>
-    <row r="122" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="122" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A122" s="5">
         <v>430209</v>
       </c>
@@ -16081,7 +16118,7 @@
       <c r="AM122" s="6"/>
       <c r="AN122" s="6"/>
     </row>
-    <row r="123" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="123" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A123" s="25">
         <v>430301</v>
       </c>
@@ -16169,7 +16206,7 @@
       <c r="AM123" s="6"/>
       <c r="AN123" s="6"/>
     </row>
-    <row r="124" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="124" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A124" s="25">
         <v>430302</v>
       </c>
@@ -16257,7 +16294,7 @@
       <c r="AM124" s="6"/>
       <c r="AN124" s="6"/>
     </row>
-    <row r="125" spans="1:40" s="10" customFormat="1" ht="15.6" customHeight="1">
+    <row r="125" spans="1:40" s="10" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A125" s="25">
         <v>430303</v>
       </c>
@@ -16331,7 +16368,7 @@
       </c>
       <c r="AN125" s="6"/>
     </row>
-    <row r="126" spans="1:40" s="10" customFormat="1" ht="15.6" customHeight="1">
+    <row r="126" spans="1:40" s="10" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A126" s="25">
         <v>430304</v>
       </c>
@@ -16405,7 +16442,7 @@
       </c>
       <c r="AN126" s="6"/>
     </row>
-    <row r="127" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="127" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A127" s="25">
         <v>430305</v>
       </c>
@@ -16491,7 +16528,7 @@
       <c r="AL127" s="10"/>
       <c r="AM127" s="10"/>
     </row>
-    <row r="128" spans="1:40" ht="15.6" customHeight="1">
+    <row r="128" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A128" s="25">
         <v>430306</v>
       </c>
@@ -16579,7 +16616,7 @@
       <c r="AM128" s="10"/>
       <c r="AN128" s="6"/>
     </row>
-    <row r="129" spans="1:40" ht="15.6" customHeight="1">
+    <row r="129" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A129" s="25">
         <v>430307</v>
       </c>
@@ -16667,7 +16704,7 @@
       <c r="AM129" s="6"/>
       <c r="AN129" s="6"/>
     </row>
-    <row r="130" spans="1:40" ht="15.6" customHeight="1">
+    <row r="130" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A130" s="6">
         <v>430401</v>
       </c>
@@ -16753,7 +16790,7 @@
       <c r="AM130" s="21"/>
       <c r="AN130" s="6"/>
     </row>
-    <row r="131" spans="1:40" ht="15.6" customHeight="1">
+    <row r="131" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A131" s="6">
         <v>430402</v>
       </c>
@@ -16839,7 +16876,7 @@
       <c r="AM131" s="21"/>
       <c r="AN131" s="6"/>
     </row>
-    <row r="132" spans="1:40" ht="15.6" customHeight="1">
+    <row r="132" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A132" s="6">
         <v>430403</v>
       </c>
@@ -16925,7 +16962,7 @@
       <c r="AM132" s="21"/>
       <c r="AN132" s="6"/>
     </row>
-    <row r="133" spans="1:40" ht="15.6" customHeight="1">
+    <row r="133" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A133" s="6">
         <v>430404</v>
       </c>
@@ -17011,7 +17048,7 @@
       <c r="AM133" s="21"/>
       <c r="AN133" s="6"/>
     </row>
-    <row r="134" spans="1:40" ht="15.6" customHeight="1">
+    <row r="134" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A134" s="6">
         <v>430405</v>
       </c>
@@ -17097,7 +17134,7 @@
       <c r="AM134" s="21"/>
       <c r="AN134" s="6"/>
     </row>
-    <row r="135" spans="1:40" ht="15.6" customHeight="1">
+    <row r="135" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A135" s="6">
         <v>430406</v>
       </c>
@@ -17183,7 +17220,7 @@
       <c r="AM135" s="21"/>
       <c r="AN135" s="6"/>
     </row>
-    <row r="136" spans="1:40" ht="15.6" customHeight="1">
+    <row r="136" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A136" s="6">
         <v>430407</v>
       </c>
@@ -17271,7 +17308,7 @@
       <c r="AM136" s="21"/>
       <c r="AN136" s="6"/>
     </row>
-    <row r="137" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="137" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A137" s="5">
         <v>520105</v>
       </c>
@@ -17349,7 +17386,7 @@
       <c r="AE137" s="21"/>
       <c r="AF137" s="21"/>
     </row>
-    <row r="138" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="138" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A138" s="5">
         <v>520106</v>
       </c>
@@ -17427,7 +17464,7 @@
       <c r="AE138" s="21"/>
       <c r="AF138" s="21"/>
     </row>
-    <row r="139" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="139" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A139" s="5">
         <v>520107</v>
       </c>
@@ -17505,7 +17542,7 @@
       <c r="AE139" s="21"/>
       <c r="AF139" s="21"/>
     </row>
-    <row r="140" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="140" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A140" s="5">
         <v>520108</v>
       </c>
@@ -17578,7 +17615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="141" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A141" s="5">
         <v>520109</v>
       </c>
@@ -17656,7 +17693,7 @@
       <c r="AE141" s="21"/>
       <c r="AF141" s="21"/>
     </row>
-    <row r="142" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="142" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A142" s="5">
         <v>520110</v>
       </c>
@@ -17729,7 +17766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="143" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A143" s="9">
         <v>530101</v>
       </c>
@@ -17805,7 +17842,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="144" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A144" s="9">
         <v>530102</v>
       </c>
@@ -17881,7 +17918,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="145" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A145" s="9">
         <v>530103</v>
       </c>
@@ -17957,7 +17994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="146" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A146" s="9">
         <v>530104</v>
       </c>
@@ -18033,7 +18070,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="147" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A147" s="9">
         <v>530201</v>
       </c>
@@ -18110,7 +18147,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="148" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A148" s="9">
         <v>530202</v>
       </c>
@@ -18190,7 +18227,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="149" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A149" s="9">
         <v>530203</v>
       </c>
@@ -18267,7 +18304,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="150" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A150" s="9">
         <v>530204</v>
       </c>
@@ -18344,7 +18381,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="151" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A151" s="9">
         <v>530205</v>
       </c>
@@ -18421,7 +18458,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="152" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A152" s="9">
         <v>530206</v>
       </c>
@@ -18501,7 +18538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="153" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A153" s="9">
         <v>530207</v>
       </c>
@@ -18581,7 +18618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="154" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A154" s="9">
         <v>530208</v>
       </c>
@@ -18658,7 +18695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:27" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="155" spans="1:27" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A155" s="21">
         <v>530209</v>
       </c>
@@ -18738,7 +18775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="156" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A156" s="9">
         <v>530210</v>
       </c>
@@ -18810,7 +18847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="157" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A157" s="9">
         <v>530211</v>
       </c>
@@ -18882,7 +18919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="158" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A158" s="9">
         <v>530212</v>
       </c>
@@ -18954,7 +18991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="159" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A159" s="9">
         <v>530213</v>
       </c>
@@ -19029,7 +19066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="160" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A160" s="5">
         <v>620101</v>
       </c>
@@ -19105,7 +19142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="161" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A161" s="5">
         <v>620102</v>
       </c>
@@ -19181,7 +19218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="162" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A162" s="5">
         <v>620103</v>
       </c>
@@ -19257,7 +19294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="163" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A163" s="5">
         <v>620104</v>
       </c>
@@ -19331,7 +19368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="164" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A164" s="5">
         <v>620105</v>
       </c>
@@ -19404,7 +19441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="165" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A165" s="5">
         <v>620106</v>
       </c>
@@ -19477,7 +19514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="166" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A166" s="5">
         <v>620107</v>
       </c>
@@ -19550,7 +19587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="167" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A167" s="5">
         <v>620108</v>
       </c>
@@ -19623,7 +19660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="168" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A168" s="5">
         <v>620109</v>
       </c>
@@ -19696,7 +19733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="169" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A169" s="5">
         <v>620110</v>
       </c>
@@ -19770,7 +19807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="170" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A170" s="5">
         <v>620111</v>
       </c>
@@ -19842,7 +19879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="171" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A171" s="5">
         <v>620112</v>
       </c>
@@ -19914,7 +19951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="172" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A172" s="5">
         <v>620113</v>
       </c>
@@ -19986,7 +20023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="173" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A173" s="6">
         <v>630101</v>
       </c>
@@ -20064,7 +20101,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="174" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="174" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A174" s="6">
         <v>630102</v>
       </c>
@@ -20142,7 +20179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="175" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="175" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A175" s="6">
         <v>630103</v>
       </c>
@@ -20220,7 +20257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:27" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="176" spans="1:27" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A176" s="6">
         <v>630201</v>
       </c>
@@ -20296,7 +20333,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="177" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A177" s="6">
         <v>630202</v>
       </c>
@@ -20372,7 +20409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="178" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A178" s="6">
         <v>630203</v>
       </c>
@@ -20448,7 +20485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="179" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A179" s="6">
         <v>630204</v>
       </c>
@@ -20524,7 +20561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="180" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A180" s="6">
         <v>630205</v>
       </c>
@@ -20600,7 +20637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="181" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A181" s="6">
         <v>630206</v>
       </c>
@@ -20676,7 +20713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="182" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A182" s="6">
         <v>630207</v>
       </c>
@@ -20752,7 +20789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="183" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A183" s="6">
         <v>630208</v>
       </c>
@@ -20828,7 +20865,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="184" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A184" s="6">
         <v>630209</v>
       </c>
@@ -20904,7 +20941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="185" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A185" s="6">
         <v>630210</v>
       </c>
@@ -20980,7 +21017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="186" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A186" s="6">
         <v>630211</v>
       </c>
@@ -21056,7 +21093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="187" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A187" s="6">
         <v>630212</v>
       </c>
@@ -21132,7 +21169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="188" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A188" s="6">
         <v>630213</v>
       </c>
@@ -21208,7 +21245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="189" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A189" s="21">
         <v>730101</v>
       </c>
@@ -21300,7 +21337,7 @@
       <c r="AM189" s="12"/>
       <c r="AN189" s="12"/>
     </row>
-    <row r="190" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="190" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A190" s="21">
         <v>730102</v>
       </c>
@@ -21392,7 +21429,7 @@
       <c r="AM190" s="12"/>
       <c r="AN190" s="12"/>
     </row>
-    <row r="191" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="191" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A191" s="21">
         <v>730103</v>
       </c>
@@ -21484,7 +21521,7 @@
       <c r="AM191" s="12"/>
       <c r="AN191" s="12"/>
     </row>
-    <row r="192" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="192" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A192" s="21">
         <v>730104</v>
       </c>
@@ -21576,7 +21613,7 @@
       <c r="AM192" s="12"/>
       <c r="AN192" s="12"/>
     </row>
-    <row r="193" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="193" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A193" s="21">
         <v>730201</v>
       </c>
@@ -21670,7 +21707,7 @@
       <c r="AM193" s="12"/>
       <c r="AN193" s="12"/>
     </row>
-    <row r="194" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="194" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A194" s="21">
         <v>730202</v>
       </c>
@@ -21764,7 +21801,7 @@
       <c r="AM194" s="12"/>
       <c r="AN194" s="12"/>
     </row>
-    <row r="195" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="195" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A195" s="21">
         <v>730203</v>
       </c>
@@ -21858,7 +21895,7 @@
       <c r="AM195" s="12"/>
       <c r="AN195" s="12"/>
     </row>
-    <row r="196" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="196" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A196" s="21">
         <v>730204</v>
       </c>
@@ -21952,7 +21989,7 @@
       <c r="AM196" s="12"/>
       <c r="AN196" s="12"/>
     </row>
-    <row r="197" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="197" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A197" s="21">
         <v>730205</v>
       </c>
@@ -22046,7 +22083,7 @@
       <c r="AM197" s="12"/>
       <c r="AN197" s="12"/>
     </row>
-    <row r="198" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="198" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A198" s="21">
         <v>730206</v>
       </c>
@@ -22138,7 +22175,7 @@
       <c r="AM198" s="12"/>
       <c r="AN198" s="12"/>
     </row>
-    <row r="199" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="199" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A199" s="21">
         <v>730207</v>
       </c>
@@ -22230,7 +22267,7 @@
       <c r="AM199" s="12"/>
       <c r="AN199" s="12"/>
     </row>
-    <row r="200" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="200" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A200" s="21">
         <v>730208</v>
       </c>
@@ -22322,7 +22359,7 @@
       <c r="AM200" s="12"/>
       <c r="AN200" s="12"/>
     </row>
-    <row r="201" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="201" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A201" s="21">
         <v>730209</v>
       </c>
@@ -22414,7 +22451,7 @@
       <c r="AM201" s="12"/>
       <c r="AN201" s="12"/>
     </row>
-    <row r="202" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="202" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A202" s="21">
         <v>730210</v>
       </c>
@@ -22504,7 +22541,7 @@
       <c r="AM202" s="12"/>
       <c r="AN202" s="12"/>
     </row>
-    <row r="203" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="203" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A203" s="21">
         <v>730211</v>
       </c>
@@ -22594,7 +22631,7 @@
       <c r="AM203" s="12"/>
       <c r="AN203" s="12"/>
     </row>
-    <row r="204" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="204" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A204" s="34">
         <v>8100101</v>
       </c>
@@ -22680,7 +22717,7 @@
       <c r="AM204" s="21"/>
       <c r="AN204" s="12"/>
     </row>
-    <row r="205" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="205" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A205" s="34">
         <v>8100201</v>
       </c>
@@ -22766,7 +22803,7 @@
       <c r="AM205" s="21"/>
       <c r="AN205" s="12"/>
     </row>
-    <row r="206" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="206" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A206" s="34">
         <v>8100202</v>
       </c>
@@ -22852,7 +22889,7 @@
       <c r="AM206" s="21"/>
       <c r="AN206" s="12"/>
     </row>
-    <row r="207" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="207" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A207" s="34">
         <v>8100203</v>
       </c>
@@ -22938,7 +22975,7 @@
       <c r="AM207" s="21"/>
       <c r="AN207" s="12"/>
     </row>
-    <row r="208" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="208" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A208" s="34">
         <v>8100204</v>
       </c>
@@ -23024,7 +23061,7 @@
       <c r="AM208" s="21"/>
       <c r="AN208" s="12"/>
     </row>
-    <row r="209" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="209" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A209" s="34">
         <v>8100205</v>
       </c>
@@ -23110,7 +23147,7 @@
       <c r="AM209" s="21"/>
       <c r="AN209" s="12"/>
     </row>
-    <row r="210" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="210" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A210" s="34">
         <v>8100206</v>
       </c>
@@ -23196,7 +23233,7 @@
       <c r="AM210" s="21"/>
       <c r="AN210" s="12"/>
     </row>
-    <row r="211" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="211" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A211" s="34">
         <v>8100207</v>
       </c>
@@ -23282,7 +23319,7 @@
       <c r="AM211" s="21"/>
       <c r="AN211" s="12"/>
     </row>
-    <row r="212" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="212" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A212" s="34">
         <v>8100208</v>
       </c>
@@ -23368,7 +23405,7 @@
       <c r="AM212" s="21"/>
       <c r="AN212" s="12"/>
     </row>
-    <row r="213" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="213" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A213" s="34">
         <v>8100209</v>
       </c>
@@ -23454,7 +23491,7 @@
       <c r="AM213" s="21"/>
       <c r="AN213" s="12"/>
     </row>
-    <row r="214" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="214" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A214" s="34">
         <v>8100210</v>
       </c>
@@ -23540,7 +23577,7 @@
       <c r="AM214" s="21"/>
       <c r="AN214" s="12"/>
     </row>
-    <row r="215" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="215" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A215" s="34">
         <v>8100211</v>
       </c>
@@ -23626,7 +23663,7 @@
       <c r="AM215" s="21"/>
       <c r="AN215" s="12"/>
     </row>
-    <row r="216" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="216" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A216" s="34">
         <v>8100212</v>
       </c>
@@ -23712,7 +23749,7 @@
       <c r="AM216" s="21"/>
       <c r="AN216" s="12"/>
     </row>
-    <row r="217" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="217" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A217" s="34">
         <v>8100213</v>
       </c>
@@ -23800,7 +23837,7 @@
       <c r="AM217" s="21"/>
       <c r="AN217" s="12"/>
     </row>
-    <row r="218" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="218" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A218" s="34">
         <v>8100214</v>
       </c>
@@ -23888,7 +23925,7 @@
       <c r="AM218" s="21"/>
       <c r="AN218" s="12"/>
     </row>
-    <row r="219" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="219" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A219" s="34">
         <v>8100215</v>
       </c>
@@ -23976,7 +24013,7 @@
       <c r="AM219" s="21"/>
       <c r="AN219" s="12"/>
     </row>
-    <row r="220" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="220" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A220" s="34">
         <v>8100216</v>
       </c>
@@ -24064,7 +24101,7 @@
       <c r="AM220" s="21"/>
       <c r="AN220" s="12"/>
     </row>
-    <row r="221" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="221" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A221" s="34">
         <v>8100217</v>
       </c>
@@ -24152,7 +24189,7 @@
       <c r="AM221" s="21"/>
       <c r="AN221" s="12"/>
     </row>
-    <row r="222" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="222" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A222" s="34">
         <v>8100218</v>
       </c>
@@ -24240,7 +24277,7 @@
       <c r="AM222" s="21"/>
       <c r="AN222" s="12"/>
     </row>
-    <row r="223" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="223" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A223" s="34">
         <v>8100219</v>
       </c>
@@ -24328,7 +24365,7 @@
       <c r="AM223" s="21"/>
       <c r="AN223" s="12"/>
     </row>
-    <row r="224" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="224" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A224" s="34">
         <v>8200101</v>
       </c>
@@ -24416,7 +24453,7 @@
       <c r="AM224" s="21"/>
       <c r="AN224" s="12"/>
     </row>
-    <row r="225" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="225" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A225" s="34">
         <v>8200102</v>
       </c>
@@ -24504,7 +24541,7 @@
       <c r="AM225" s="21"/>
       <c r="AN225" s="12"/>
     </row>
-    <row r="226" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="226" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A226" s="34">
         <v>8200103</v>
       </c>
@@ -24592,7 +24629,7 @@
       <c r="AM226" s="21"/>
       <c r="AN226" s="12"/>
     </row>
-    <row r="227" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="227" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A227" s="34">
         <v>8200104</v>
       </c>
@@ -24680,7 +24717,7 @@
       <c r="AM227" s="21"/>
       <c r="AN227" s="12"/>
     </row>
-    <row r="228" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="228" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A228" s="34">
         <v>8200105</v>
       </c>
@@ -24772,7 +24809,7 @@
       <c r="AM228" s="21"/>
       <c r="AN228" s="12"/>
     </row>
-    <row r="229" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="229" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A229" s="34">
         <v>8300101</v>
       </c>
@@ -24860,7 +24897,7 @@
       <c r="AM229" s="21"/>
       <c r="AN229" s="12"/>
     </row>
-    <row r="230" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="230" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A230" s="34">
         <v>8300102</v>
       </c>
@@ -24948,7 +24985,7 @@
       <c r="AM230" s="21"/>
       <c r="AN230" s="12"/>
     </row>
-    <row r="231" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="231" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A231" s="34">
         <v>8300103</v>
       </c>
@@ -25036,7 +25073,7 @@
       <c r="AM231" s="21"/>
       <c r="AN231" s="12"/>
     </row>
-    <row r="232" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="232" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A232" s="34">
         <v>8300104</v>
       </c>
@@ -25124,7 +25161,7 @@
       <c r="AM232" s="21"/>
       <c r="AN232" s="12"/>
     </row>
-    <row r="233" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="233" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A233" s="34">
         <v>8300105</v>
       </c>
@@ -25212,7 +25249,7 @@
       <c r="AM233" s="21"/>
       <c r="AN233" s="12"/>
     </row>
-    <row r="234" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="234" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A234" s="34">
         <v>8300106</v>
       </c>
@@ -25300,7 +25337,7 @@
       <c r="AM234" s="21"/>
       <c r="AN234" s="12"/>
     </row>
-    <row r="235" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="235" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A235" s="34">
         <v>8300107</v>
       </c>
@@ -25388,7 +25425,7 @@
       <c r="AM235" s="21"/>
       <c r="AN235" s="12"/>
     </row>
-    <row r="236" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="236" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A236" s="34">
         <v>8300108</v>
       </c>
@@ -25476,7 +25513,7 @@
       <c r="AM236" s="21"/>
       <c r="AN236" s="12"/>
     </row>
-    <row r="237" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="237" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A237" s="34">
         <v>8300109</v>
       </c>
@@ -25568,7 +25605,7 @@
       <c r="AM237" s="21"/>
       <c r="AN237" s="12"/>
     </row>
-    <row r="238" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="238" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A238" s="34">
         <v>8300110</v>
       </c>
@@ -25660,7 +25697,7 @@
       <c r="AM238" s="21"/>
       <c r="AN238" s="12"/>
     </row>
-    <row r="239" spans="1:40" s="62" customFormat="1" ht="14.4">
+    <row r="239" spans="1:40" s="62" customFormat="1" ht="14.4" hidden="1">
       <c r="A239" s="53">
         <v>8300111</v>
       </c>
@@ -25756,7 +25793,7 @@
       <c r="AM239" s="60"/>
       <c r="AN239" s="61"/>
     </row>
-    <row r="240" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="240" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A240" s="34">
         <v>8300112</v>
       </c>
@@ -25844,7 +25881,7 @@
       <c r="AM240" s="21"/>
       <c r="AN240" s="12"/>
     </row>
-    <row r="241" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="241" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A241" s="34">
         <v>8300113</v>
       </c>
@@ -25932,7 +25969,7 @@
       <c r="AM241" s="21"/>
       <c r="AN241" s="12"/>
     </row>
-    <row r="242" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="242" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A242" s="34">
         <v>8300114</v>
       </c>
@@ -26020,7 +26057,7 @@
       <c r="AM242" s="21"/>
       <c r="AN242" s="12"/>
     </row>
-    <row r="243" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="243" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A243" s="34">
         <v>8300115</v>
       </c>
@@ -26108,7 +26145,7 @@
       <c r="AM243" s="21"/>
       <c r="AN243" s="12"/>
     </row>
-    <row r="244" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="244" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A244" s="34">
         <v>8300116</v>
       </c>
@@ -26196,7 +26233,7 @@
       <c r="AM244" s="21"/>
       <c r="AN244" s="12"/>
     </row>
-    <row r="245" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="245" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A245" s="34">
         <v>8300201</v>
       </c>
@@ -26288,7 +26325,7 @@
       <c r="AM245" s="21"/>
       <c r="AN245" s="12"/>
     </row>
-    <row r="246" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="246" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A246" s="32">
         <v>91130110</v>
       </c>
@@ -26367,7 +26404,7 @@
       </c>
       <c r="AN246" s="21"/>
     </row>
-    <row r="247" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="247" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A247" s="33">
         <v>91130206</v>
       </c>
@@ -26447,7 +26484,7 @@
       </c>
       <c r="AN247" s="21"/>
     </row>
-    <row r="248" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="248" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A248" s="33">
         <v>91130207</v>
       </c>
@@ -26527,7 +26564,7 @@
       </c>
       <c r="AN248" s="21"/>
     </row>
-    <row r="249" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="249" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A249" s="33">
         <v>91130208</v>
       </c>
@@ -26607,7 +26644,7 @@
       </c>
       <c r="AN249" s="21"/>
     </row>
-    <row r="250" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="250" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A250" s="33">
         <v>91130209</v>
       </c>
@@ -26686,7 +26723,7 @@
       </c>
       <c r="AN250" s="21"/>
     </row>
-    <row r="251" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="251" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A251" s="34">
         <v>91230601</v>
       </c>
@@ -26762,7 +26799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:40" s="5" customFormat="1" ht="15.6" customHeight="1">
+    <row r="252" spans="1:40" s="5" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A252" s="34">
         <v>91230602</v>
       </c>
@@ -26850,7 +26887,7 @@
       <c r="AM252" s="6"/>
       <c r="AN252" s="6"/>
     </row>
-    <row r="253" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="253" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A253" s="34">
         <v>91230603</v>
       </c>
@@ -26926,7 +26963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:40" s="6" customFormat="1" ht="15.6" customHeight="1">
+    <row r="254" spans="1:40" s="6" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A254" s="34">
         <v>91330116</v>
       </c>
@@ -27007,7 +27044,7 @@
       <c r="AE254" s="21"/>
       <c r="AF254" s="21"/>
     </row>
-    <row r="255" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="255" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A255" s="34">
         <v>91430115</v>
       </c>
@@ -27092,7 +27129,7 @@
       <c r="AM255" s="6"/>
       <c r="AN255" s="6"/>
     </row>
-    <row r="256" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="256" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A256" s="34">
         <v>91430308</v>
       </c>
@@ -27182,7 +27219,7 @@
       <c r="AM256" s="6"/>
       <c r="AN256" s="6"/>
     </row>
-    <row r="257" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="257" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A257" s="34">
         <v>91430309</v>
       </c>
@@ -27272,7 +27309,7 @@
       <c r="AM257" s="6"/>
       <c r="AN257" s="6"/>
     </row>
-    <row r="258" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="258" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A258" s="34">
         <v>91430310</v>
       </c>
@@ -27362,7 +27399,7 @@
       <c r="AM258" s="6"/>
       <c r="AN258" s="6"/>
     </row>
-    <row r="259" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="259" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A259" s="34">
         <v>91530105</v>
       </c>
@@ -27452,7 +27489,7 @@
       <c r="AM259" s="6"/>
       <c r="AN259" s="6"/>
     </row>
-    <row r="260" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="260" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A260" s="34">
         <v>91530106</v>
       </c>
@@ -27542,7 +27579,7 @@
       <c r="AM260" s="6"/>
       <c r="AN260" s="6"/>
     </row>
-    <row r="261" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="261" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A261" s="34">
         <v>92130111</v>
       </c>
@@ -27633,7 +27670,7 @@
       <c r="AL261" s="6"/>
       <c r="AM261" s="6"/>
     </row>
-    <row r="262" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="262" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A262" s="34">
         <v>92130112</v>
       </c>
@@ -27724,7 +27761,7 @@
       <c r="AL262" s="6"/>
       <c r="AM262" s="6"/>
     </row>
-    <row r="263" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="263" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A263" s="34">
         <v>92130113</v>
       </c>
@@ -27815,7 +27852,7 @@
       <c r="AL263" s="6"/>
       <c r="AM263" s="6"/>
     </row>
-    <row r="264" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="264" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A264" s="34">
         <v>92130114</v>
       </c>
@@ -27906,7 +27943,7 @@
       <c r="AL264" s="6"/>
       <c r="AM264" s="6"/>
     </row>
-    <row r="265" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="265" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A265" s="34">
         <v>92330117</v>
       </c>
@@ -27991,7 +28028,7 @@
       <c r="AM265" s="6"/>
       <c r="AN265" s="6"/>
     </row>
-    <row r="266" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="266" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A266" s="34">
         <v>92530107</v>
       </c>
@@ -28081,7 +28118,7 @@
       <c r="AM266" s="6"/>
       <c r="AN266" s="6"/>
     </row>
-    <row r="267" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="267" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A267" s="34">
         <v>92530108</v>
       </c>
@@ -28171,7 +28208,7 @@
       <c r="AM267" s="6"/>
       <c r="AN267" s="6"/>
     </row>
-    <row r="268" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="268" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A268" s="34">
         <v>92530109</v>
       </c>
@@ -28261,7 +28298,7 @@
       <c r="AM268" s="6"/>
       <c r="AN268" s="6"/>
     </row>
-    <row r="269" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="269" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A269" s="34">
         <v>92530110</v>
       </c>
@@ -28351,7 +28388,7 @@
       <c r="AM269" s="6"/>
       <c r="AN269" s="6"/>
     </row>
-    <row r="270" spans="1:40" s="15" customFormat="1" ht="15.6" customHeight="1">
+    <row r="270" spans="1:40" s="15" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A270" s="34">
         <v>92530111</v>
       </c>
@@ -28441,7 +28478,7 @@
       <c r="AM270" s="6"/>
       <c r="AN270" s="6"/>
     </row>
-    <row r="271" spans="1:40" s="39" customFormat="1" ht="15.6" customHeight="1">
+    <row r="271" spans="1:40" s="39" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A271" s="34">
         <v>92530112</v>
       </c>
@@ -28531,7 +28568,7 @@
       <c r="AM271" s="6"/>
       <c r="AN271" s="6"/>
     </row>
-    <row r="272" spans="1:40" s="15" customFormat="1" ht="15.6" customHeight="1">
+    <row r="272" spans="1:40" s="15" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A272" s="34">
         <v>92530113</v>
       </c>
@@ -28621,7 +28658,7 @@
       <c r="AM272" s="6"/>
       <c r="AN272" s="6"/>
     </row>
-    <row r="273" spans="1:40" s="15" customFormat="1" ht="15.6" customHeight="1">
+    <row r="273" spans="1:40" s="15" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A273" s="34">
         <v>92530114</v>
       </c>
@@ -28711,7 +28748,7 @@
       <c r="AM273" s="6"/>
       <c r="AN273" s="6"/>
     </row>
-    <row r="274" spans="1:40" s="39" customFormat="1" ht="15.6" customHeight="1">
+    <row r="274" spans="1:40" s="39" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A274" s="34">
         <v>92530115</v>
       </c>
@@ -28801,7 +28838,7 @@
       <c r="AM274" s="6"/>
       <c r="AN274" s="6"/>
     </row>
-    <row r="275" spans="1:40" s="39" customFormat="1" ht="15.6" customHeight="1">
+    <row r="275" spans="1:40" s="39" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A275" s="34">
         <v>93130117</v>
       </c>
@@ -28895,7 +28932,7 @@
       <c r="AM275" s="6"/>
       <c r="AN275" s="21"/>
     </row>
-    <row r="276" spans="1:40" s="39" customFormat="1" ht="15.6" customHeight="1">
+    <row r="276" spans="1:40" s="39" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A276" s="34">
         <v>93130118</v>
       </c>
@@ -28989,7 +29026,7 @@
       <c r="AM276" s="6"/>
       <c r="AN276" s="21"/>
     </row>
-    <row r="277" spans="1:40" s="39" customFormat="1" ht="15.6" customHeight="1">
+    <row r="277" spans="1:40" s="39" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A277" s="34">
         <v>93230102</v>
       </c>
@@ -29083,7 +29120,7 @@
       <c r="AM277" s="6"/>
       <c r="AN277" s="6"/>
     </row>
-    <row r="278" spans="1:40" s="39" customFormat="1" ht="15.6" customHeight="1">
+    <row r="278" spans="1:40" s="39" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A278" s="34">
         <v>93230205</v>
       </c>
@@ -29177,7 +29214,7 @@
       <c r="AM278" s="6"/>
       <c r="AN278" s="6"/>
     </row>
-    <row r="279" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="279" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A279" s="34">
         <v>93230206</v>
       </c>
@@ -29271,7 +29308,7 @@
       <c r="AM279" s="6"/>
       <c r="AN279" s="6"/>
     </row>
-    <row r="280" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="280" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A280" s="34">
         <v>93230207</v>
       </c>
@@ -29365,7 +29402,7 @@
       <c r="AM280" s="6"/>
       <c r="AN280" s="6"/>
     </row>
-    <row r="281" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="281" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A281" s="34">
         <v>93230208</v>
       </c>
@@ -29459,7 +29496,7 @@
       <c r="AM281" s="6"/>
       <c r="AN281" s="6"/>
     </row>
-    <row r="282" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="282" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A282" s="34">
         <v>93230305</v>
       </c>
@@ -29553,7 +29590,7 @@
       <c r="AM282" s="6"/>
       <c r="AN282" s="6"/>
     </row>
-    <row r="283" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="283" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A283" s="34">
         <v>93230404</v>
       </c>
@@ -29647,7 +29684,7 @@
       <c r="AM283" s="6"/>
       <c r="AN283" s="6"/>
     </row>
-    <row r="284" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="284" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A284" s="34">
         <v>93230405</v>
       </c>
@@ -29741,7 +29778,7 @@
       <c r="AM284" s="6"/>
       <c r="AN284" s="6"/>
     </row>
-    <row r="285" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="285" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A285" s="34">
         <v>93330118</v>
       </c>
@@ -29828,7 +29865,7 @@
       <c r="AM285" s="6"/>
       <c r="AN285" s="6"/>
     </row>
-    <row r="286" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="286" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A286" s="34">
         <v>93330119</v>
       </c>
@@ -29917,7 +29954,7 @@
       <c r="AM286" s="6"/>
       <c r="AN286" s="6"/>
     </row>
-    <row r="287" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="287" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A287" s="34">
         <v>93330120</v>
       </c>
@@ -30006,7 +30043,7 @@
       <c r="AM287" s="6"/>
       <c r="AN287" s="6"/>
     </row>
-    <row r="288" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="288" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A288" s="34">
         <v>93330121</v>
       </c>
@@ -30095,7 +30132,7 @@
       <c r="AM288" s="6"/>
       <c r="AN288" s="6"/>
     </row>
-    <row r="289" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="289" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A289" s="34">
         <v>93430118</v>
       </c>
@@ -30184,7 +30221,7 @@
       <c r="AM289" s="6"/>
       <c r="AN289" s="6"/>
     </row>
-    <row r="290" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="290" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A290" s="34">
         <v>93530118</v>
       </c>
@@ -30276,7 +30313,7 @@
       <c r="AM290" s="6"/>
       <c r="AN290" s="6"/>
     </row>
-    <row r="291" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="291" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A291" s="34">
         <v>93530119</v>
       </c>
@@ -30368,7 +30405,7 @@
       <c r="AM291" s="6"/>
       <c r="AN291" s="6"/>
     </row>
-    <row r="292" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="292" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A292" s="34">
         <v>93530120</v>
       </c>
@@ -30460,7 +30497,7 @@
       <c r="AM292" s="6"/>
       <c r="AN292" s="6"/>
     </row>
-    <row r="293" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="293" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A293" s="34">
         <v>93530121</v>
       </c>
@@ -30552,7 +30589,7 @@
       <c r="AM293" s="6"/>
       <c r="AN293" s="6"/>
     </row>
-    <row r="294" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="294" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A294" s="34">
         <v>93530122</v>
       </c>
@@ -30644,7 +30681,7 @@
       <c r="AM294" s="6"/>
       <c r="AN294" s="6"/>
     </row>
-    <row r="295" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="295" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A295" s="34">
         <v>93530123</v>
       </c>
@@ -30736,7 +30773,7 @@
       <c r="AM295" s="6"/>
       <c r="AN295" s="6"/>
     </row>
-    <row r="296" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="296" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A296" s="33">
         <v>94120117</v>
       </c>
@@ -30826,7 +30863,7 @@
       <c r="AM296" s="6"/>
       <c r="AN296" s="6"/>
     </row>
-    <row r="297" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="297" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A297" s="34">
         <v>94130115</v>
       </c>
@@ -30915,7 +30952,7 @@
       <c r="AL297" s="6"/>
       <c r="AM297" s="6"/>
     </row>
-    <row r="298" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="298" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A298" s="32">
         <v>94130116</v>
       </c>
@@ -31004,7 +31041,7 @@
       <c r="AL298" s="6"/>
       <c r="AM298" s="6"/>
     </row>
-    <row r="299" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="299" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A299" s="34">
         <v>94230403</v>
       </c>
@@ -31094,7 +31131,7 @@
       <c r="AM299" s="6"/>
       <c r="AN299" s="5"/>
     </row>
-    <row r="300" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="300" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A300" s="34">
         <v>94430116</v>
       </c>
@@ -31179,7 +31216,7 @@
       <c r="AM300" s="6"/>
       <c r="AN300" s="6"/>
     </row>
-    <row r="301" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="301" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A301" s="34">
         <v>94430117</v>
       </c>
@@ -31264,7 +31301,7 @@
       <c r="AM301" s="6"/>
       <c r="AN301" s="6"/>
     </row>
-    <row r="302" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="302" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A302" s="34">
         <v>94530116</v>
       </c>
@@ -31353,7 +31390,7 @@
       <c r="AL302" s="6"/>
       <c r="AM302" s="6"/>
     </row>
-    <row r="303" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="303" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A303" s="34">
         <v>94530117</v>
       </c>
@@ -31442,7 +31479,7 @@
       <c r="AL303" s="6"/>
       <c r="AM303" s="6"/>
     </row>
-    <row r="304" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="304" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A304" s="37">
         <v>95120118</v>
       </c>
@@ -31532,7 +31569,7 @@
       <c r="AM304" s="15"/>
       <c r="AN304" s="15"/>
     </row>
-    <row r="305" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="305" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A305" s="38">
         <v>95230101</v>
       </c>
@@ -31624,7 +31661,7 @@
       <c r="AM305" s="15"/>
       <c r="AN305" s="15"/>
     </row>
-    <row r="306" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="306" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A306" s="38">
         <v>95230501</v>
       </c>
@@ -31716,7 +31753,7 @@
       <c r="AM306" s="15"/>
       <c r="AN306" s="15"/>
     </row>
-    <row r="307" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="307" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A307" s="37">
         <v>95520111</v>
       </c>
@@ -31806,7 +31843,7 @@
       <c r="AM307" s="39"/>
       <c r="AN307" s="39"/>
     </row>
-    <row r="308" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="308" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A308" s="38">
         <v>95530101</v>
       </c>
@@ -31898,7 +31935,7 @@
       <c r="AM308" s="39"/>
       <c r="AN308" s="39"/>
     </row>
-    <row r="309" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="309" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A309" s="38">
         <v>95530102</v>
       </c>
@@ -31990,7 +32027,7 @@
       <c r="AM309" s="39"/>
       <c r="AN309" s="39"/>
     </row>
-    <row r="310" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="310" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A310" s="38">
         <v>95530103</v>
       </c>
@@ -32082,7 +32119,7 @@
       <c r="AM310" s="39"/>
       <c r="AN310" s="39"/>
     </row>
-    <row r="311" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="311" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A311" s="38">
         <v>95530104</v>
       </c>
@@ -32174,7 +32211,7 @@
       <c r="AM311" s="39"/>
       <c r="AN311" s="39"/>
     </row>
-    <row r="312" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="312" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A312" s="39">
         <v>95530202</v>
       </c>
@@ -32268,7 +32305,7 @@
       <c r="AM312" s="39"/>
       <c r="AN312" s="39"/>
     </row>
-    <row r="313" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="313" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A313" s="32">
         <v>910199999</v>
       </c>
@@ -32356,7 +32393,7 @@
       <c r="AM313" s="6"/>
       <c r="AN313" s="5"/>
     </row>
-    <row r="314" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="314" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A314" s="34">
         <v>920199999</v>
       </c>
@@ -32444,7 +32481,7 @@
       <c r="AM314" s="6"/>
       <c r="AN314" s="5"/>
     </row>
-    <row r="315" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="315" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A315" s="34">
         <v>920299999</v>
       </c>
@@ -32532,7 +32569,7 @@
       <c r="AM315" s="6"/>
       <c r="AN315" s="5"/>
     </row>
-    <row r="316" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="316" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A316" s="34">
         <v>920399999</v>
       </c>
@@ -32620,7 +32657,7 @@
       <c r="AM316" s="6"/>
       <c r="AN316" s="5"/>
     </row>
-    <row r="317" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="317" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A317" s="34">
         <v>920499999</v>
       </c>
@@ -32708,7 +32745,7 @@
       <c r="AM317" s="6"/>
       <c r="AN317" s="5"/>
     </row>
-    <row r="318" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="318" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A318" s="34">
         <v>920599999</v>
       </c>
@@ -32796,7 +32833,7 @@
       <c r="AM318" s="5"/>
       <c r="AN318" s="5"/>
     </row>
-    <row r="319" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="319" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A319" s="34">
         <v>920699999</v>
       </c>
@@ -32884,7 +32921,7 @@
       <c r="AM319" s="5"/>
       <c r="AN319" s="5"/>
     </row>
-    <row r="320" spans="1:40" s="21" customFormat="1" ht="15.6" customHeight="1">
+    <row r="320" spans="1:40" s="21" customFormat="1" ht="15.6" hidden="1" customHeight="1">
       <c r="A320" s="34">
         <v>920799999</v>
       </c>
@@ -32972,7 +33009,7 @@
       <c r="AM320" s="5"/>
       <c r="AN320" s="5"/>
     </row>
-    <row r="321" spans="1:40" ht="15.6" customHeight="1">
+    <row r="321" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A321" s="34">
         <v>920899999</v>
       </c>
@@ -33060,7 +33097,7 @@
       <c r="AM321" s="21"/>
       <c r="AN321" s="5"/>
     </row>
-    <row r="322" spans="1:40" ht="15.6" customHeight="1">
+    <row r="322" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A322" s="34">
         <v>920999999</v>
       </c>
@@ -33148,7 +33185,7 @@
       <c r="AM322" s="21"/>
       <c r="AN322" s="5"/>
     </row>
-    <row r="323" spans="1:40" ht="15.6" customHeight="1">
+    <row r="323" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A323" s="34">
         <v>921099999</v>
       </c>
@@ -33236,7 +33273,7 @@
       <c r="AM323" s="21"/>
       <c r="AN323" s="5"/>
     </row>
-    <row r="324" spans="1:40" ht="15.6" customHeight="1">
+    <row r="324" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A324" s="34">
         <v>921199999</v>
       </c>
@@ -33324,7 +33361,7 @@
       <c r="AM324" s="21"/>
       <c r="AN324" s="5"/>
     </row>
-    <row r="325" spans="1:40" ht="15.6" customHeight="1">
+    <row r="325" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A325" s="34">
         <v>921299999</v>
       </c>
@@ -33412,7 +33449,7 @@
       <c r="AM325" s="21"/>
       <c r="AN325" s="5"/>
     </row>
-    <row r="326" spans="1:40" ht="15.6" customHeight="1">
+    <row r="326" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A326" s="34">
         <v>921399999</v>
       </c>
@@ -33500,7 +33537,7 @@
       <c r="AM326" s="21"/>
       <c r="AN326" s="6"/>
     </row>
-    <row r="327" spans="1:40" ht="15.6" customHeight="1">
+    <row r="327" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A327" s="34">
         <v>921499999</v>
       </c>
@@ -33588,7 +33625,7 @@
       <c r="AM327" s="21"/>
       <c r="AN327" s="6"/>
     </row>
-    <row r="328" spans="1:40" ht="15.6" customHeight="1">
+    <row r="328" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A328" s="34">
         <v>921599999</v>
       </c>
@@ -33676,7 +33713,7 @@
       <c r="AM328" s="21"/>
       <c r="AN328" s="6"/>
     </row>
-    <row r="329" spans="1:40" ht="15.6" customHeight="1">
+    <row r="329" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A329" s="34">
         <v>930199999</v>
       </c>
@@ -33765,7 +33802,7 @@
       <c r="AL329" s="21"/>
       <c r="AM329" s="21"/>
     </row>
-    <row r="330" spans="1:40" ht="15.6" customHeight="1">
+    <row r="330" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A330" s="34">
         <v>940199999</v>
       </c>
@@ -33852,7 +33889,7 @@
       <c r="AL330" s="21"/>
       <c r="AM330" s="21"/>
     </row>
-    <row r="331" spans="1:40" ht="15.6" customHeight="1">
+    <row r="331" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A331" s="34">
         <v>940299999</v>
       </c>
@@ -33940,7 +33977,7 @@
       <c r="AM331" s="21"/>
       <c r="AN331" s="5"/>
     </row>
-    <row r="332" spans="1:40" ht="15.6" customHeight="1">
+    <row r="332" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A332" s="34">
         <v>940399999</v>
       </c>
@@ -34027,7 +34064,7 @@
       <c r="AL332" s="21"/>
       <c r="AM332" s="21"/>
     </row>
-    <row r="333" spans="1:40" ht="15.6" customHeight="1">
+    <row r="333" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A333" s="34">
         <v>940499999</v>
       </c>
@@ -34114,7 +34151,7 @@
       <c r="AL333" s="21"/>
       <c r="AM333" s="21"/>
     </row>
-    <row r="334" spans="1:40" ht="15.6" customHeight="1">
+    <row r="334" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A334" s="34">
         <v>940599999</v>
       </c>
@@ -34202,7 +34239,7 @@
       <c r="AM334" s="21"/>
       <c r="AN334" s="5"/>
     </row>
-    <row r="335" spans="1:40" ht="15.6" customHeight="1">
+    <row r="335" spans="1:40" ht="15.6" hidden="1" customHeight="1">
       <c r="A335" s="34">
         <v>940699999</v>
       </c>
@@ -34291,6 +34328,13 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <autoFilter ref="A1:AN335">
+    <filterColumn colId="13">
+      <filters>
+        <filter val="Observatorio de la Educación - ANEP"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
act tablas web jul25
</commit_message>
<xml_diff>
--- a/Data/Base_fichas_indicadores.xlsx
+++ b/Data/Base_fichas_indicadores.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5494" uniqueCount="1720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5494" uniqueCount="1721">
   <si>
     <t>id</t>
   </si>
@@ -5283,6 +5283,9 @@
   </si>
   <si>
     <t>2008-2022</t>
+  </si>
+  <si>
+    <t>Frecuentemente, en las actualizaciones anuales de CEPAL STATS se modifica ligeramente toda la serie.</t>
   </si>
 </sst>
 </file>
@@ -5889,9 +5892,9 @@
   <dimension ref="A1:AN335"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="E111" sqref="E111"/>
-      <selection pane="bottomLeft" activeCell="U2" sqref="U2:Y335"/>
+      <selection pane="bottomLeft" activeCell="S163" sqref="S163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="15.6" customHeight="1"/>
@@ -6284,7 +6287,7 @@
         <v>17</v>
       </c>
       <c r="S5" s="5" t="s">
-        <v>1260</v>
+        <v>1720</v>
       </c>
       <c r="T5" s="42" t="s">
         <v>1696</v>
@@ -9104,7 +9107,7 @@
         <v>17</v>
       </c>
       <c r="S40" s="5" t="s">
-        <v>1260</v>
+        <v>1720</v>
       </c>
       <c r="T40" s="42" t="s">
         <v>1696</v>
@@ -10744,7 +10747,7 @@
         <v>17</v>
       </c>
       <c r="S59" s="5" t="s">
-        <v>1260</v>
+        <v>1720</v>
       </c>
       <c r="T59" s="42" t="s">
         <v>1696</v>
@@ -13723,7 +13726,7 @@
         <v>17</v>
       </c>
       <c r="S94" s="5" t="s">
-        <v>1260</v>
+        <v>1720</v>
       </c>
       <c r="T94" s="42" t="s">
         <v>1696</v>
@@ -19392,7 +19395,7 @@
         <v>17</v>
       </c>
       <c r="S163" s="5" t="s">
-        <v>1260</v>
+        <v>1720</v>
       </c>
       <c r="T163" s="42" t="s">
         <v>1696</v>

</xml_diff>